<commit_message>
Fixing loadUp of parameters to match correct Excel cells
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CISNET\HHCoM\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1532,17 +1529,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1553,25 +1598,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1580,12 +1606,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1596,48 +1616,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5827,369 +5824,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Targets"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="U2" t="str">
-            <v>Population Size</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="M3" t="str">
-            <v>Total Population</v>
-          </cell>
-          <cell r="T3">
-            <v>1985</v>
-          </cell>
-          <cell r="U3">
-            <v>5420315</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="L4">
-            <v>1985</v>
-          </cell>
-          <cell r="M4">
-            <v>5420315</v>
-          </cell>
-          <cell r="N4">
-            <v>1107298</v>
-          </cell>
-          <cell r="O4">
-            <v>1108238</v>
-          </cell>
-          <cell r="P4">
-            <v>1549446</v>
-          </cell>
-          <cell r="Q4">
-            <v>1655333</v>
-          </cell>
-          <cell r="T4">
-            <v>1996</v>
-          </cell>
-          <cell r="U4">
-            <v>8068284</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="L5">
-            <v>1996</v>
-          </cell>
-          <cell r="M5">
-            <v>8068284</v>
-          </cell>
-          <cell r="N5">
-            <v>1526597</v>
-          </cell>
-          <cell r="O5">
-            <v>1537145</v>
-          </cell>
-          <cell r="P5">
-            <v>2292625</v>
-          </cell>
-          <cell r="Q5">
-            <v>2711917</v>
-          </cell>
-          <cell r="T5">
-            <v>2001</v>
-          </cell>
-          <cell r="U5">
-            <v>9138179</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="L6">
-            <v>2001</v>
-          </cell>
-          <cell r="M6">
-            <v>9138179</v>
-          </cell>
-          <cell r="N6">
-            <v>1669704</v>
-          </cell>
-          <cell r="O6">
-            <v>1675104</v>
-          </cell>
-          <cell r="P6">
-            <v>2659850</v>
-          </cell>
-          <cell r="Q6">
-            <v>3133521</v>
-          </cell>
-          <cell r="T6">
-            <v>2011</v>
-          </cell>
-          <cell r="U6">
-            <v>10267300</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="L7">
-            <v>2011</v>
-          </cell>
-          <cell r="M7">
-            <v>9759249</v>
-          </cell>
-          <cell r="N7">
-            <v>1658047</v>
-          </cell>
-          <cell r="O7">
-            <v>1621472</v>
-          </cell>
-          <cell r="P7">
-            <v>3046456</v>
-          </cell>
-          <cell r="Q7">
-            <v>3433274</v>
-          </cell>
-          <cell r="T7">
-            <v>2013</v>
-          </cell>
-          <cell r="U7">
-            <v>10456909</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="T8">
-            <v>2014</v>
-          </cell>
-          <cell r="U8">
-            <v>10571313</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="T9">
-            <v>2015</v>
-          </cell>
-          <cell r="U9">
-            <v>10688168</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="T10">
-            <v>2016</v>
-          </cell>
-          <cell r="U10">
-            <v>10806536</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="T11">
-            <v>2017</v>
-          </cell>
-          <cell r="U11">
-            <v>10924776</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="T12">
-            <v>2018</v>
-          </cell>
-          <cell r="U12">
-            <v>11039740</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="T13">
-            <v>2019</v>
-          </cell>
-          <cell r="U13">
-            <v>11155657</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21" t="str">
-            <v>Prevalence</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>1990</v>
-          </cell>
-          <cell r="B22">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>1991</v>
-          </cell>
-          <cell r="B23">
-            <v>1.0999999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>1992</v>
-          </cell>
-          <cell r="B24">
-            <v>1.4999999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>1993</v>
-          </cell>
-          <cell r="B25">
-            <v>2.7E-2</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>1994</v>
-          </cell>
-          <cell r="B26">
-            <v>5.0999999999999997E-2</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>1995</v>
-          </cell>
-          <cell r="B27">
-            <v>6.9000000000000006E-2</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>1996</v>
-          </cell>
-          <cell r="B28">
-            <v>9.5000000000000001E-2</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>1997</v>
-          </cell>
-          <cell r="B29">
-            <v>0.113</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>1998</v>
-          </cell>
-          <cell r="B30">
-            <v>0.152</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>1999</v>
-          </cell>
-          <cell r="B31">
-            <v>0.14899999999999999</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>2000</v>
-          </cell>
-          <cell r="B32">
-            <v>0.16300000000000001</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>2001</v>
-          </cell>
-          <cell r="B33">
-            <v>0.223</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>2002</v>
-          </cell>
-          <cell r="B34">
-            <v>0.24299999999999999</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35">
-            <v>2003</v>
-          </cell>
-          <cell r="B35">
-            <v>0.25</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36">
-            <v>2004</v>
-          </cell>
-          <cell r="B36">
-            <v>0.27100000000000002</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37">
-            <v>2005</v>
-          </cell>
-          <cell r="B37">
-            <v>0.26100000000000001</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38">
-            <v>2006</v>
-          </cell>
-          <cell r="B38">
-            <v>0.26100000000000001</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39">
-            <v>2007</v>
-          </cell>
-          <cell r="B39">
-            <v>0.25800000000000001</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40">
-            <v>2008</v>
-          </cell>
-          <cell r="B40">
-            <v>0.25800000000000001</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41">
-            <v>2009</v>
-          </cell>
-          <cell r="B41">
-            <v>0.26300000000000001</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42">
-            <v>2010</v>
-          </cell>
-          <cell r="B42">
-            <v>0.26300000000000001</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43">
-            <v>2012</v>
-          </cell>
-          <cell r="B43">
-            <v>0.318</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6454,144 +6088,144 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AF241"/>
+  <dimension ref="A1:AF239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F236" sqref="F236"/>
+    <sheetView tabSelected="1" topLeftCell="A220" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B241" sqref="B241"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25" customWidth="1"/>
-    <col min="16" max="16" width="17.7265625" customWidth="1"/>
-    <col min="17" max="17" width="19.81640625" customWidth="1"/>
-    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.81640625" customWidth="1"/>
-    <col min="21" max="21" width="15.453125" customWidth="1"/>
-    <col min="22" max="22" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.1796875" customWidth="1"/>
-    <col min="26" max="26" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.26953125" customWidth="1"/>
-    <col min="28" max="29" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.81640625" customWidth="1"/>
-    <col min="31" max="31" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.1796875" customWidth="1"/>
-    <col min="33" max="33" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.81640625" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" customWidth="1"/>
+    <col min="26" max="26" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" customWidth="1"/>
+    <col min="28" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.85546875" customWidth="1"/>
+    <col min="31" max="31" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.140625" customWidth="1"/>
+    <col min="33" max="33" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
-      <c r="S1" s="64"/>
-      <c r="T1" s="64"/>
-      <c r="U1" s="64"/>
-      <c r="V1" s="64"/>
-      <c r="W1" s="64"/>
-      <c r="X1" s="64"/>
-      <c r="Y1" s="64"/>
-    </row>
-    <row r="2" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+    </row>
+    <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="64"/>
-    </row>
-    <row r="3" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="65" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="57"/>
+      <c r="X2" s="57"/>
+      <c r="Y2" s="57"/>
+    </row>
+    <row r="3" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
-    </row>
-    <row r="4" spans="1:25" s="66" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="57"/>
+    </row>
+    <row r="4" spans="1:25" s="59" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="67"/>
-    </row>
-    <row r="5" spans="1:25" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="69"/>
+      <c r="C4" s="97"/>
+    </row>
+    <row r="5" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="60"/>
       <c r="B5" s="54" t="s">
         <v>0</v>
       </c>
@@ -6599,7 +6233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -6610,7 +6244,7 @@
         <v>417311</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="33.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:25" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -6621,7 +6255,7 @@
         <v>361594</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -6632,7 +6266,7 @@
         <v>329333</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -6643,7 +6277,7 @@
         <v>296947</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
@@ -6654,7 +6288,7 @@
         <v>273204</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
@@ -6665,7 +6299,7 @@
         <v>249396</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -6676,7 +6310,7 @@
         <v>211839</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
@@ -6687,7 +6321,7 @@
         <v>176470</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -6698,7 +6332,7 @@
         <v>143351</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -6709,7 +6343,7 @@
         <v>123441</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -6720,7 +6354,7 @@
         <v>98355</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>27</v>
       </c>
@@ -6731,7 +6365,7 @@
         <v>82330</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>49</v>
       </c>
@@ -6744,7 +6378,7 @@
         <v>57671.85534591195</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>50</v>
       </c>
@@ -6757,7 +6391,7 @@
         <v>44482.861635220121</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>51</v>
       </c>
@@ -6770,7 +6404,7 @@
         <v>33878.773584905655</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>52</v>
       </c>
@@ -6783,7 +6417,7 @@
         <v>22783.176100628931</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>28</v>
       </c>
@@ -6801,11 +6435,11 @@
       </c>
       <c r="X22" s="17"/>
     </row>
-    <row r="23" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
     </row>
-    <row r="24" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>59</v>
       </c>
@@ -6818,19 +6452,19 @@
         <v>6.3660571774707435</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F26" s="43"/>
     </row>
-    <row r="27" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="71" t="s">
+      <c r="B27" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="72"/>
-    </row>
-    <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.35">
+      <c r="C27" s="98"/>
+    </row>
+    <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="52" t="s">
         <v>0</v>
@@ -6840,7 +6474,7 @@
       </c>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>11</v>
       </c>
@@ -6852,7 +6486,7 @@
         <v>417311</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>14</v>
       </c>
@@ -6863,7 +6497,7 @@
         <v>361594</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>17</v>
       </c>
@@ -6875,7 +6509,7 @@
       </c>
       <c r="L31" s="11"/>
     </row>
-    <row r="32" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>18</v>
       </c>
@@ -6886,7 +6520,7 @@
         <v>296947</v>
       </c>
     </row>
-    <row r="33" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>19</v>
       </c>
@@ -6897,7 +6531,7 @@
         <v>273204</v>
       </c>
     </row>
-    <row r="34" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>20</v>
       </c>
@@ -6908,7 +6542,7 @@
         <v>249396</v>
       </c>
     </row>
-    <row r="35" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>21</v>
       </c>
@@ -6919,7 +6553,7 @@
         <v>211839</v>
       </c>
     </row>
-    <row r="36" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>22</v>
       </c>
@@ -6939,7 +6573,7 @@
       <c r="AE36" s="9"/>
       <c r="AF36" s="17"/>
     </row>
-    <row r="37" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>24</v>
       </c>
@@ -6958,7 +6592,7 @@
       <c r="AD37" s="18"/>
       <c r="AE37" s="18"/>
     </row>
-    <row r="38" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>25</v>
       </c>
@@ -6977,7 +6611,7 @@
       <c r="AD38" s="34"/>
       <c r="AE38" s="34"/>
     </row>
-    <row r="39" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>26</v>
       </c>
@@ -6996,7 +6630,7 @@
       <c r="AD39" s="35"/>
       <c r="AE39" s="35"/>
     </row>
-    <row r="40" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>27</v>
       </c>
@@ -7015,14 +6649,14 @@
       <c r="AD40" s="35"/>
       <c r="AE40" s="35"/>
     </row>
-    <row r="41" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="70">
+      <c r="B41" s="61">
         <v>-50094.736842105267</v>
       </c>
-      <c r="C41" s="70">
+      <c r="C41" s="61">
         <f>366793/6.36</f>
         <v>57671.85534591195</v>
       </c>
@@ -7035,14 +6669,14 @@
       <c r="AD41" s="35"/>
       <c r="AE41" s="35"/>
     </row>
-    <row r="42" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="70">
+      <c r="B42" s="61">
         <v>-35803.827751196171</v>
       </c>
-      <c r="C42" s="70">
+      <c r="C42" s="61">
         <f>282911/6.36</f>
         <v>44482.861635220121</v>
       </c>
@@ -7055,14 +6689,14 @@
       <c r="AD42" s="36"/>
       <c r="AE42" s="36"/>
     </row>
-    <row r="43" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="70">
+      <c r="B43" s="61">
         <v>-24102.551834130783</v>
       </c>
-      <c r="C43" s="70">
+      <c r="C43" s="61">
         <f>215469/6.36</f>
         <v>33878.773584905655</v>
       </c>
@@ -7075,14 +6709,14 @@
       <c r="AD43" s="36"/>
       <c r="AE43" s="36"/>
     </row>
-    <row r="44" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="70">
+      <c r="B44" s="61">
         <v>-14240.510366826158</v>
       </c>
-      <c r="C44" s="70">
+      <c r="C44" s="61">
         <f>144901/6.36</f>
         <v>22783.176100628931</v>
       </c>
@@ -7095,7 +6729,7 @@
       <c r="AD44" s="36"/>
       <c r="AE44" s="36"/>
     </row>
-    <row r="45" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="X45" s="36"/>
       <c r="Y45" s="36"/>
       <c r="Z45" s="36"/>
@@ -7105,7 +6739,7 @@
       <c r="AD45" s="36"/>
       <c r="AE45" s="36"/>
     </row>
-    <row r="46" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="X46" s="36"/>
       <c r="Y46" s="36"/>
       <c r="Z46" s="36"/>
@@ -7115,7 +6749,7 @@
       <c r="AD46" s="36"/>
       <c r="AE46" s="36"/>
     </row>
-    <row r="47" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="X47" s="36"/>
       <c r="Y47" s="36"/>
       <c r="Z47" s="36"/>
@@ -7125,7 +6759,7 @@
       <c r="AD47" s="36"/>
       <c r="AE47" s="36"/>
     </row>
-    <row r="48" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="X48" s="36"/>
       <c r="Y48" s="36"/>
       <c r="Z48" s="36"/>
@@ -7135,7 +6769,7 @@
       <c r="AD48" s="36"/>
       <c r="AE48" s="36"/>
     </row>
-    <row r="49" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="X49" s="36"/>
       <c r="Y49" s="36"/>
       <c r="Z49" s="36"/>
@@ -7145,32 +6779,32 @@
       <c r="AD49" s="36"/>
       <c r="AE49" s="36"/>
     </row>
-    <row r="50" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="63" t="s">
+    <row r="50" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="64"/>
-      <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="64"/>
-      <c r="H50" s="64"/>
-      <c r="I50" s="64"/>
-      <c r="J50" s="64"/>
-      <c r="K50" s="64"/>
-      <c r="L50" s="64"/>
-      <c r="M50" s="64"/>
-      <c r="N50" s="64"/>
-      <c r="O50" s="64"/>
-      <c r="P50" s="64"/>
-      <c r="Q50" s="64"/>
-      <c r="R50" s="64"/>
-      <c r="S50" s="64"/>
-      <c r="T50" s="64"/>
-      <c r="U50" s="64"/>
-      <c r="V50" s="64"/>
-      <c r="W50" s="64"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
+      <c r="L50" s="57"/>
+      <c r="M50" s="57"/>
+      <c r="N50" s="57"/>
+      <c r="O50" s="57"/>
+      <c r="P50" s="57"/>
+      <c r="Q50" s="57"/>
+      <c r="R50" s="57"/>
+      <c r="S50" s="57"/>
+      <c r="T50" s="57"/>
+      <c r="U50" s="57"/>
+      <c r="V50" s="57"/>
+      <c r="W50" s="57"/>
       <c r="X50" s="36"/>
       <c r="Y50" s="36"/>
       <c r="Z50" s="36"/>
@@ -7180,32 +6814,32 @@
       <c r="AD50" s="36"/>
       <c r="AE50" s="36"/>
     </row>
-    <row r="51" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="65" t="s">
+    <row r="51" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="64"/>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="64"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="64"/>
-      <c r="J51" s="64"/>
-      <c r="K51" s="64"/>
-      <c r="L51" s="64"/>
-      <c r="M51" s="64"/>
-      <c r="N51" s="64"/>
-      <c r="O51" s="64"/>
-      <c r="P51" s="64"/>
-      <c r="Q51" s="64"/>
-      <c r="R51" s="64"/>
-      <c r="S51" s="64"/>
-      <c r="T51" s="64"/>
-      <c r="U51" s="64"/>
-      <c r="V51" s="64"/>
-      <c r="W51" s="64"/>
+      <c r="B51" s="57"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57"/>
+      <c r="L51" s="57"/>
+      <c r="M51" s="57"/>
+      <c r="N51" s="57"/>
+      <c r="O51" s="57"/>
+      <c r="P51" s="57"/>
+      <c r="Q51" s="57"/>
+      <c r="R51" s="57"/>
+      <c r="S51" s="57"/>
+      <c r="T51" s="57"/>
+      <c r="U51" s="57"/>
+      <c r="V51" s="57"/>
+      <c r="W51" s="57"/>
       <c r="X51" s="36"/>
       <c r="Y51" s="36"/>
       <c r="Z51" s="36"/>
@@ -7215,20 +6849,20 @@
       <c r="AD51" s="36"/>
       <c r="AE51" s="36"/>
     </row>
-    <row r="52" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="58" t="s">
+    <row r="52" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="58" t="s">
+      <c r="B52" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="58" t="s">
+      <c r="C52" s="102"/>
+      <c r="D52" s="102"/>
+      <c r="E52" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="58"/>
-      <c r="G52" s="58"/>
+      <c r="F52" s="102"/>
+      <c r="G52" s="102"/>
       <c r="X52" s="34"/>
       <c r="Y52" s="34"/>
       <c r="Z52" s="34"/>
@@ -7238,8 +6872,8 @@
       <c r="AD52" s="34"/>
       <c r="AE52" s="34"/>
     </row>
-    <row r="53" spans="1:31" ht="30" x14ac:dyDescent="0.35">
-      <c r="A53" s="58"/>
+    <row r="53" spans="1:31" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="102"/>
       <c r="B53" s="52" t="s">
         <v>6</v>
       </c>
@@ -7267,7 +6901,7 @@
       <c r="AD53" s="37"/>
       <c r="AE53" s="37"/>
     </row>
-    <row r="54" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>11</v>
       </c>
@@ -7291,7 +6925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>14</v>
       </c>
@@ -7315,7 +6949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>17</v>
       </c>
@@ -7340,7 +6974,7 @@
         <v>5.0000000000000183E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>18</v>
       </c>
@@ -7363,7 +6997,7 @@
         <v>2.4213075060532689E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>19</v>
       </c>
@@ -7386,7 +7020,7 @@
         <v>1.6393442622950817E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:31" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>20</v>
       </c>
@@ -7410,7 +7044,7 @@
       </c>
       <c r="O59" s="16"/>
     </row>
-    <row r="60" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>23</v>
       </c>
@@ -7434,7 +7068,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>22</v>
       </c>
@@ -7457,7 +7091,7 @@
         <v>1.1547344110854503E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>24</v>
       </c>
@@ -7482,7 +7116,7 @@
         <v>9.9999999999988987E-5</v>
       </c>
     </row>
-    <row r="63" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>25</v>
       </c>
@@ -7506,7 +7140,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>26</v>
       </c>
@@ -7530,7 +7164,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>27</v>
       </c>
@@ -7554,7 +7188,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
         <v>49</v>
       </c>
@@ -7578,7 +7212,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
         <v>50</v>
       </c>
@@ -7602,7 +7236,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
         <v>51</v>
       </c>
@@ -7626,7 +7260,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
         <v>52</v>
       </c>
@@ -7650,7 +7284,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="43" t="s">
         <v>60</v>
       </c>
@@ -7679,7 +7313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="43" t="s">
         <v>61</v>
       </c>
@@ -7688,112 +7322,112 @@
         <v>0.83084071366534329</v>
       </c>
     </row>
-    <row r="78" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A78" s="63" t="s">
+    <row r="78" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="B78" s="64"/>
-      <c r="C78" s="64"/>
-      <c r="D78" s="64"/>
-      <c r="E78" s="64"/>
-      <c r="F78" s="64"/>
-      <c r="G78" s="64"/>
-      <c r="H78" s="64"/>
-      <c r="I78" s="64"/>
-      <c r="J78" s="64"/>
-      <c r="K78" s="64"/>
-      <c r="L78" s="64"/>
-      <c r="M78" s="64"/>
-      <c r="N78" s="64"/>
-      <c r="O78" s="64"/>
-      <c r="P78" s="64"/>
-      <c r="Q78" s="64"/>
-      <c r="R78" s="64"/>
-      <c r="S78" s="64"/>
-      <c r="T78" s="64"/>
-      <c r="U78" s="64"/>
-      <c r="V78" s="64"/>
-      <c r="W78" s="64"/>
-      <c r="X78" s="64"/>
-    </row>
-    <row r="79" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A79" s="65" t="s">
+      <c r="B78" s="57"/>
+      <c r="C78" s="57"/>
+      <c r="D78" s="57"/>
+      <c r="E78" s="57"/>
+      <c r="F78" s="57"/>
+      <c r="G78" s="57"/>
+      <c r="H78" s="57"/>
+      <c r="I78" s="57"/>
+      <c r="J78" s="57"/>
+      <c r="K78" s="57"/>
+      <c r="L78" s="57"/>
+      <c r="M78" s="57"/>
+      <c r="N78" s="57"/>
+      <c r="O78" s="57"/>
+      <c r="P78" s="57"/>
+      <c r="Q78" s="57"/>
+      <c r="R78" s="57"/>
+      <c r="S78" s="57"/>
+      <c r="T78" s="57"/>
+      <c r="U78" s="57"/>
+      <c r="V78" s="57"/>
+      <c r="W78" s="57"/>
+      <c r="X78" s="57"/>
+    </row>
+    <row r="79" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="B79" s="64"/>
-      <c r="C79" s="64"/>
-      <c r="D79" s="64"/>
-      <c r="E79" s="64"/>
-      <c r="F79" s="64"/>
-      <c r="G79" s="64"/>
-      <c r="H79" s="64"/>
-      <c r="I79" s="64"/>
-      <c r="J79" s="64"/>
-      <c r="K79" s="64"/>
-      <c r="L79" s="64"/>
-      <c r="M79" s="64"/>
-      <c r="N79" s="64"/>
-      <c r="O79" s="64"/>
-      <c r="P79" s="64"/>
-      <c r="Q79" s="64"/>
-      <c r="R79" s="64"/>
-      <c r="S79" s="64"/>
-      <c r="T79" s="64"/>
-      <c r="U79" s="64"/>
-      <c r="V79" s="64"/>
-      <c r="W79" s="64"/>
-      <c r="X79" s="64"/>
-    </row>
-    <row r="80" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="65" t="s">
+      <c r="B79" s="57"/>
+      <c r="C79" s="57"/>
+      <c r="D79" s="57"/>
+      <c r="E79" s="57"/>
+      <c r="F79" s="57"/>
+      <c r="G79" s="57"/>
+      <c r="H79" s="57"/>
+      <c r="I79" s="57"/>
+      <c r="J79" s="57"/>
+      <c r="K79" s="57"/>
+      <c r="L79" s="57"/>
+      <c r="M79" s="57"/>
+      <c r="N79" s="57"/>
+      <c r="O79" s="57"/>
+      <c r="P79" s="57"/>
+      <c r="Q79" s="57"/>
+      <c r="R79" s="57"/>
+      <c r="S79" s="57"/>
+      <c r="T79" s="57"/>
+      <c r="U79" s="57"/>
+      <c r="V79" s="57"/>
+      <c r="W79" s="57"/>
+      <c r="X79" s="57"/>
+    </row>
+    <row r="80" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="B80" s="64"/>
-      <c r="C80" s="64"/>
-      <c r="D80" s="64"/>
-      <c r="E80" s="64"/>
-      <c r="F80" s="64"/>
-      <c r="G80" s="64"/>
-      <c r="H80" s="64"/>
-      <c r="I80" s="64"/>
-      <c r="J80" s="64"/>
-      <c r="K80" s="64"/>
-      <c r="L80" s="64"/>
-      <c r="M80" s="64"/>
-      <c r="N80" s="64"/>
-      <c r="O80" s="64"/>
-      <c r="P80" s="64"/>
-      <c r="Q80" s="64"/>
-      <c r="R80" s="64"/>
-      <c r="S80" s="64"/>
-      <c r="T80" s="64"/>
-      <c r="U80" s="64"/>
-      <c r="V80" s="64"/>
-      <c r="W80" s="64"/>
-      <c r="X80" s="64"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="59" t="s">
+      <c r="B80" s="57"/>
+      <c r="C80" s="57"/>
+      <c r="D80" s="57"/>
+      <c r="E80" s="57"/>
+      <c r="F80" s="57"/>
+      <c r="G80" s="57"/>
+      <c r="H80" s="57"/>
+      <c r="I80" s="57"/>
+      <c r="J80" s="57"/>
+      <c r="K80" s="57"/>
+      <c r="L80" s="57"/>
+      <c r="M80" s="57"/>
+      <c r="N80" s="57"/>
+      <c r="O80" s="57"/>
+      <c r="P80" s="57"/>
+      <c r="Q80" s="57"/>
+      <c r="R80" s="57"/>
+      <c r="S80" s="57"/>
+      <c r="T80" s="57"/>
+      <c r="U80" s="57"/>
+      <c r="V80" s="57"/>
+      <c r="W80" s="57"/>
+      <c r="X80" s="57"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="55" t="s">
+      <c r="B81" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="55" t="s">
+      <c r="C81" s="99" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="60"/>
-      <c r="B82" s="57"/>
-      <c r="C82" s="57"/>
-    </row>
-    <row r="83" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="61"/>
-      <c r="B83" s="56"/>
-      <c r="C83" s="56"/>
-    </row>
-    <row r="84" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="88"/>
+      <c r="B82" s="100"/>
+      <c r="C82" s="100"/>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="89"/>
+      <c r="B83" s="101"/>
+      <c r="C83" s="101"/>
+    </row>
+    <row r="84" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>11</v>
       </c>
@@ -7804,7 +7438,7 @@
         <v>8.8057230624727749E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>14</v>
       </c>
@@ -7815,7 +7449,7 @@
         <v>5.2457282047517039E-4</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>17</v>
       </c>
@@ -7826,7 +7460,7 @@
         <v>4.8877879149405545E-4</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>18</v>
       </c>
@@ -7837,7 +7471,7 @@
         <v>9.035280767087482E-4</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>19</v>
       </c>
@@ -7848,7 +7482,7 @@
         <v>1.6915946235478447E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>20</v>
       </c>
@@ -7859,7 +7493,7 @@
         <v>2.0719480819543991E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>23</v>
       </c>
@@ -7870,7 +7504,7 @@
         <v>2.4601074470881829E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>22</v>
       </c>
@@ -7881,7 +7515,7 @@
         <v>2.9925533571735037E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>24</v>
       </c>
@@ -7892,7 +7526,7 @@
         <v>3.9413474052092329E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>25</v>
       </c>
@@ -7903,7 +7537,7 @@
         <v>5.3575989334735206E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>26</v>
       </c>
@@ -7914,7 +7548,7 @@
         <v>7.5410818923787939E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>27</v>
       </c>
@@ -7925,7 +7559,7 @@
         <v>1.0540154917424747E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="21" t="s">
         <v>49</v>
       </c>
@@ -7936,7 +7570,7 @@
         <v>1.5759592316689931E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="21" t="s">
         <v>50</v>
       </c>
@@ -7947,7 +7581,7 @@
         <v>2.2837523063216215E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="21" t="s">
         <v>51</v>
       </c>
@@ -7958,7 +7592,7 @@
         <v>3.3336893194863555E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="21" t="s">
         <v>52</v>
       </c>
@@ -7969,133 +7603,133 @@
         <v>6.1722846856347699E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A105" s="63" t="s">
+    <row r="105" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="B105" s="64"/>
-      <c r="C105" s="64"/>
-      <c r="D105" s="64"/>
-      <c r="E105" s="64"/>
-      <c r="F105" s="64"/>
-      <c r="G105" s="64"/>
-      <c r="H105" s="64"/>
-      <c r="I105" s="64"/>
-      <c r="J105" s="64"/>
-      <c r="K105" s="64"/>
-      <c r="L105" s="64"/>
-      <c r="M105" s="64"/>
-      <c r="N105" s="64"/>
-      <c r="O105" s="64"/>
-      <c r="P105" s="64"/>
-      <c r="Q105" s="64"/>
-      <c r="R105" s="64"/>
-      <c r="S105" s="64"/>
-      <c r="T105" s="64"/>
-      <c r="U105" s="64"/>
-      <c r="V105" s="64"/>
-      <c r="W105" s="64"/>
-      <c r="X105" s="64"/>
-    </row>
-    <row r="106" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A106" s="65" t="s">
+      <c r="B105" s="57"/>
+      <c r="C105" s="57"/>
+      <c r="D105" s="57"/>
+      <c r="E105" s="57"/>
+      <c r="F105" s="57"/>
+      <c r="G105" s="57"/>
+      <c r="H105" s="57"/>
+      <c r="I105" s="57"/>
+      <c r="J105" s="57"/>
+      <c r="K105" s="57"/>
+      <c r="L105" s="57"/>
+      <c r="M105" s="57"/>
+      <c r="N105" s="57"/>
+      <c r="O105" s="57"/>
+      <c r="P105" s="57"/>
+      <c r="Q105" s="57"/>
+      <c r="R105" s="57"/>
+      <c r="S105" s="57"/>
+      <c r="T105" s="57"/>
+      <c r="U105" s="57"/>
+      <c r="V105" s="57"/>
+      <c r="W105" s="57"/>
+      <c r="X105" s="57"/>
+    </row>
+    <row r="106" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="B106" s="64"/>
-      <c r="C106" s="64"/>
-      <c r="D106" s="64"/>
-      <c r="E106" s="64"/>
-      <c r="F106" s="64"/>
-      <c r="G106" s="64"/>
-      <c r="H106" s="64"/>
-      <c r="I106" s="64"/>
-      <c r="J106" s="64"/>
-      <c r="K106" s="64"/>
-      <c r="L106" s="64"/>
-      <c r="M106" s="64"/>
-      <c r="N106" s="64"/>
-      <c r="O106" s="64"/>
-      <c r="P106" s="64"/>
-      <c r="Q106" s="64"/>
-      <c r="R106" s="64"/>
-      <c r="S106" s="64"/>
-      <c r="T106" s="64"/>
-      <c r="U106" s="64"/>
-      <c r="V106" s="64"/>
-      <c r="W106" s="64"/>
-      <c r="X106" s="64"/>
-    </row>
-    <row r="107" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A107" s="65" t="s">
+      <c r="B106" s="57"/>
+      <c r="C106" s="57"/>
+      <c r="D106" s="57"/>
+      <c r="E106" s="57"/>
+      <c r="F106" s="57"/>
+      <c r="G106" s="57"/>
+      <c r="H106" s="57"/>
+      <c r="I106" s="57"/>
+      <c r="J106" s="57"/>
+      <c r="K106" s="57"/>
+      <c r="L106" s="57"/>
+      <c r="M106" s="57"/>
+      <c r="N106" s="57"/>
+      <c r="O106" s="57"/>
+      <c r="P106" s="57"/>
+      <c r="Q106" s="57"/>
+      <c r="R106" s="57"/>
+      <c r="S106" s="57"/>
+      <c r="T106" s="57"/>
+      <c r="U106" s="57"/>
+      <c r="V106" s="57"/>
+      <c r="W106" s="57"/>
+      <c r="X106" s="57"/>
+    </row>
+    <row r="107" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A107" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="B107" s="64"/>
-      <c r="C107" s="64"/>
-      <c r="D107" s="64"/>
-      <c r="E107" s="64"/>
-      <c r="F107" s="64"/>
-      <c r="G107" s="64"/>
-      <c r="H107" s="64"/>
-      <c r="I107" s="64"/>
-      <c r="J107" s="64"/>
-      <c r="K107" s="64"/>
-      <c r="L107" s="64"/>
-      <c r="M107" s="64"/>
-      <c r="N107" s="64"/>
-      <c r="O107" s="64"/>
-      <c r="P107" s="64"/>
-      <c r="Q107" s="64"/>
-      <c r="R107" s="64"/>
-      <c r="S107" s="64"/>
-      <c r="T107" s="64"/>
-      <c r="U107" s="64"/>
-      <c r="V107" s="64"/>
-      <c r="W107" s="64"/>
-      <c r="X107" s="64"/>
-    </row>
-    <row r="108" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="63" t="s">
+      <c r="B107" s="57"/>
+      <c r="C107" s="57"/>
+      <c r="D107" s="57"/>
+      <c r="E107" s="57"/>
+      <c r="F107" s="57"/>
+      <c r="G107" s="57"/>
+      <c r="H107" s="57"/>
+      <c r="I107" s="57"/>
+      <c r="J107" s="57"/>
+      <c r="K107" s="57"/>
+      <c r="L107" s="57"/>
+      <c r="M107" s="57"/>
+      <c r="N107" s="57"/>
+      <c r="O107" s="57"/>
+      <c r="P107" s="57"/>
+      <c r="Q107" s="57"/>
+      <c r="R107" s="57"/>
+      <c r="S107" s="57"/>
+      <c r="T107" s="57"/>
+      <c r="U107" s="57"/>
+      <c r="V107" s="57"/>
+      <c r="W107" s="57"/>
+      <c r="X107" s="57"/>
+    </row>
+    <row r="108" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="B108" s="64"/>
-      <c r="C108" s="64"/>
-      <c r="D108" s="64"/>
-      <c r="E108" s="64"/>
-      <c r="F108" s="64"/>
-      <c r="G108" s="64"/>
-      <c r="H108" s="64"/>
-      <c r="I108" s="64"/>
-      <c r="J108" s="64"/>
-      <c r="K108" s="64"/>
-      <c r="L108" s="64"/>
-      <c r="M108" s="64"/>
-      <c r="N108" s="64"/>
-      <c r="O108" s="64"/>
-      <c r="P108" s="64"/>
-      <c r="Q108" s="64"/>
-      <c r="R108" s="64"/>
-      <c r="S108" s="64"/>
-      <c r="T108" s="64"/>
-      <c r="U108" s="64"/>
-      <c r="V108" s="64"/>
-      <c r="W108" s="64"/>
-      <c r="X108" s="64"/>
-    </row>
-    <row r="109" spans="1:24" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="59" t="s">
+      <c r="B108" s="57"/>
+      <c r="C108" s="57"/>
+      <c r="D108" s="57"/>
+      <c r="E108" s="57"/>
+      <c r="F108" s="57"/>
+      <c r="G108" s="57"/>
+      <c r="H108" s="57"/>
+      <c r="I108" s="57"/>
+      <c r="J108" s="57"/>
+      <c r="K108" s="57"/>
+      <c r="L108" s="57"/>
+      <c r="M108" s="57"/>
+      <c r="N108" s="57"/>
+      <c r="O108" s="57"/>
+      <c r="P108" s="57"/>
+      <c r="Q108" s="57"/>
+      <c r="R108" s="57"/>
+      <c r="S108" s="57"/>
+      <c r="T108" s="57"/>
+      <c r="U108" s="57"/>
+      <c r="V108" s="57"/>
+      <c r="W108" s="57"/>
+      <c r="X108" s="57"/>
+    </row>
+    <row r="109" spans="1:24" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="B109" s="73" t="s">
+      <c r="B109" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="C109" s="74"/>
-      <c r="D109" s="74"/>
-      <c r="E109" s="74"/>
-      <c r="F109" s="74"/>
-      <c r="G109" s="75"/>
-    </row>
-    <row r="110" spans="1:24" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="60"/>
+      <c r="C109" s="91"/>
+      <c r="D109" s="91"/>
+      <c r="E109" s="91"/>
+      <c r="F109" s="91"/>
+      <c r="G109" s="92"/>
+    </row>
+    <row r="110" spans="1:24" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="88"/>
       <c r="B110" s="51" t="s">
         <v>83</v>
       </c>
@@ -8115,8 +7749,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="111" spans="1:24" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="61"/>
+    <row r="111" spans="1:24" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="89"/>
       <c r="B111" s="53" t="s">
         <v>76</v>
       </c>
@@ -8136,7 +7770,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="112" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>11</v>
       </c>
@@ -8159,7 +7793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
         <v>14</v>
       </c>
@@ -8182,7 +7816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
         <v>17</v>
       </c>
@@ -8204,7 +7838,7 @@
       <c r="G114" s="13">
         <v>0</v>
       </c>
-      <c r="I114" s="100"/>
+      <c r="I114" s="75"/>
       <c r="J114" s="18" t="s">
         <v>33</v>
       </c>
@@ -8221,7 +7855,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
         <v>18</v>
       </c>
@@ -8246,28 +7880,28 @@
       <c r="I115" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J115" s="99">
+      <c r="J115" s="74">
         <f>C115/$B$115</f>
         <v>1</v>
       </c>
-      <c r="K115" s="99">
+      <c r="K115" s="74">
         <f>D115/$B$115</f>
         <v>1</v>
       </c>
-      <c r="L115" s="99">
+      <c r="L115" s="74">
         <f>E115/$B$115</f>
         <v>0.58000000000000007</v>
       </c>
-      <c r="M115" s="99">
+      <c r="M115" s="74">
         <f>F115/$B$115</f>
         <v>0.58000000000000007</v>
       </c>
-      <c r="N115" s="99">
+      <c r="N115" s="74">
         <f>G115/$B$115</f>
         <v>0.41000000000000003</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
         <v>19</v>
       </c>
@@ -8290,7 +7924,7 @@
         <v>0.11398000000000003</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
         <v>20</v>
       </c>
@@ -8313,7 +7947,7 @@
         <v>0.11627600000000002</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
         <v>23</v>
       </c>
@@ -8336,7 +7970,7 @@
         <v>8.6592000000000002E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
         <v>22</v>
       </c>
@@ -8359,7 +7993,7 @@
         <v>5.5268000000000005E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
         <v>24</v>
       </c>
@@ -8382,7 +8016,7 @@
         <v>2.2222000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
         <v>25</v>
       </c>
@@ -8405,7 +8039,7 @@
         <v>7.2160000000000011E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
         <v>26</v>
       </c>
@@ -8428,7 +8062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
         <v>27</v>
       </c>
@@ -8451,7 +8085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="21" t="s">
         <v>49</v>
       </c>
@@ -8474,7 +8108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="21" t="s">
         <v>50</v>
       </c>
@@ -8497,7 +8131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="21" t="s">
         <v>51</v>
       </c>
@@ -8520,7 +8154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="21" t="s">
         <v>52</v>
       </c>
@@ -8543,48 +8177,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B128">
-        <f>5*SUM(B115:B121)</f>
+        <f t="shared" ref="B128:G128" si="3">5*SUM(B115:B121)</f>
         <v>5.604000000000001</v>
       </c>
       <c r="C128">
-        <f>5*SUM(C115:C121)</f>
+        <f t="shared" si="3"/>
         <v>5.604000000000001</v>
       </c>
       <c r="D128">
-        <f>5*SUM(D115:D121)</f>
+        <f t="shared" si="3"/>
         <v>5.604000000000001</v>
       </c>
       <c r="E128">
-        <f>5*SUM(E115:E121)</f>
+        <f t="shared" si="3"/>
         <v>3.2503200000000003</v>
       </c>
       <c r="F128">
-        <f>5*SUM(F115:F121)</f>
+        <f t="shared" si="3"/>
         <v>3.2503200000000003</v>
       </c>
       <c r="G128">
-        <f>5*SUM(G115:G121)</f>
+        <f t="shared" si="3"/>
         <v>2.2976400000000003</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="130" spans="1:7" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="78" t="s">
+    <row r="129" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="B130" s="73" t="s">
+      <c r="B130" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="C130" s="74"/>
-      <c r="D130" s="74"/>
-      <c r="E130" s="74"/>
-      <c r="F130" s="74"/>
-      <c r="G130" s="75"/>
-    </row>
-    <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="79"/>
+      <c r="C130" s="91"/>
+      <c r="D130" s="91"/>
+      <c r="E130" s="91"/>
+      <c r="F130" s="91"/>
+      <c r="G130" s="92"/>
+    </row>
+    <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="94"/>
       <c r="B131" s="38" t="s">
         <v>86</v>
       </c>
@@ -8604,15 +8238,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="80"/>
-      <c r="B132" s="76" t="s">
+    <row r="132" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="95"/>
+      <c r="B132" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="C132" s="77" t="s">
+      <c r="C132" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="D132" s="77" t="s">
+      <c r="D132" s="63" t="s">
         <v>80</v>
       </c>
       <c r="E132" s="42" t="s">
@@ -8625,7 +8259,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
         <v>11</v>
       </c>
@@ -8648,7 +8282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>14</v>
       </c>
@@ -8671,7 +8305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
         <v>17</v>
       </c>
@@ -8694,7 +8328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
         <v>18</v>
       </c>
@@ -8717,7 +8351,7 @@
         <v>2.8987000000000002E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
         <v>19</v>
       </c>
@@ -8740,7 +8374,7 @@
         <v>5.6990000000000013E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
         <v>20</v>
       </c>
@@ -8763,7 +8397,7 @@
         <v>5.8138000000000009E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="4" t="s">
         <v>23</v>
       </c>
@@ -8786,7 +8420,7 @@
         <v>4.3296000000000001E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="4" t="s">
         <v>22</v>
       </c>
@@ -8809,7 +8443,7 @@
         <v>2.7634000000000002E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="4" t="s">
         <v>24</v>
       </c>
@@ -8832,7 +8466,7 @@
         <v>1.1111000000000001E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
         <v>25</v>
       </c>
@@ -8855,7 +8489,7 @@
         <v>3.6080000000000005E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="4" t="s">
         <v>26</v>
       </c>
@@ -8878,7 +8512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
         <v>27</v>
       </c>
@@ -8901,7 +8535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="21" t="s">
         <v>49</v>
       </c>
@@ -8924,7 +8558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="21" t="s">
         <v>50</v>
       </c>
@@ -8947,7 +8581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="21" t="s">
         <v>51</v>
       </c>
@@ -8970,7 +8604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="21" t="s">
         <v>52</v>
       </c>
@@ -8993,114 +8627,114 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B149">
-        <f>5*SUM(B133:B148)</f>
+        <f t="shared" ref="B149:G149" si="4">5*SUM(B133:B148)</f>
         <v>2.8020000000000005</v>
       </c>
       <c r="C149">
-        <f>5*SUM(C133:C148)</f>
+        <f t="shared" si="4"/>
         <v>2.8020000000000005</v>
       </c>
       <c r="D149">
-        <f>5*SUM(D133:D148)</f>
+        <f t="shared" si="4"/>
         <v>2.8020000000000005</v>
       </c>
       <c r="E149">
-        <f>5*SUM(E133:E148)</f>
+        <f t="shared" si="4"/>
         <v>1.6251600000000002</v>
       </c>
       <c r="F149">
-        <f>5*SUM(F133:F148)</f>
+        <f t="shared" si="4"/>
         <v>1.6251600000000002</v>
       </c>
       <c r="G149">
-        <f>5*SUM(G133:G148)</f>
+        <f t="shared" si="4"/>
         <v>1.1488200000000002</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A155" s="63" t="s">
+    <row r="155" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A155" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="B155" s="64"/>
-      <c r="C155" s="64"/>
-      <c r="D155" s="64"/>
-      <c r="E155" s="64"/>
-      <c r="F155" s="64"/>
-      <c r="G155" s="64"/>
-      <c r="H155" s="64"/>
-      <c r="I155" s="64"/>
-      <c r="J155" s="64"/>
-      <c r="K155" s="64"/>
-      <c r="L155" s="64"/>
-      <c r="M155" s="64"/>
-      <c r="N155" s="64"/>
-      <c r="O155" s="64"/>
-      <c r="P155" s="64"/>
-      <c r="Q155" s="64"/>
-      <c r="R155" s="64"/>
-      <c r="S155" s="64"/>
-      <c r="T155" s="64"/>
-      <c r="U155" s="64"/>
-      <c r="V155" s="64"/>
-      <c r="W155" s="64"/>
-    </row>
-    <row r="156" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A156" s="65" t="s">
+      <c r="B155" s="57"/>
+      <c r="C155" s="57"/>
+      <c r="D155" s="57"/>
+      <c r="E155" s="57"/>
+      <c r="F155" s="57"/>
+      <c r="G155" s="57"/>
+      <c r="H155" s="57"/>
+      <c r="I155" s="57"/>
+      <c r="J155" s="57"/>
+      <c r="K155" s="57"/>
+      <c r="L155" s="57"/>
+      <c r="M155" s="57"/>
+      <c r="N155" s="57"/>
+      <c r="O155" s="57"/>
+      <c r="P155" s="57"/>
+      <c r="Q155" s="57"/>
+      <c r="R155" s="57"/>
+      <c r="S155" s="57"/>
+      <c r="T155" s="57"/>
+      <c r="U155" s="57"/>
+      <c r="V155" s="57"/>
+      <c r="W155" s="57"/>
+    </row>
+    <row r="156" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A156" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B156" s="64"/>
-      <c r="C156" s="64"/>
-      <c r="D156" s="64"/>
-      <c r="E156" s="64"/>
-      <c r="F156" s="64"/>
-      <c r="G156" s="64"/>
-      <c r="H156" s="64"/>
-      <c r="I156" s="64"/>
-      <c r="J156" s="64"/>
-      <c r="K156" s="64"/>
-      <c r="L156" s="64"/>
-      <c r="M156" s="64"/>
-      <c r="N156" s="64"/>
-      <c r="O156" s="64"/>
-      <c r="P156" s="64"/>
-      <c r="Q156" s="64"/>
-      <c r="R156" s="64"/>
-      <c r="S156" s="64"/>
-      <c r="T156" s="64"/>
-      <c r="U156" s="64"/>
-      <c r="V156" s="64"/>
-      <c r="W156" s="64"/>
-    </row>
-    <row r="157" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A157" s="63" t="s">
+      <c r="B156" s="57"/>
+      <c r="C156" s="57"/>
+      <c r="D156" s="57"/>
+      <c r="E156" s="57"/>
+      <c r="F156" s="57"/>
+      <c r="G156" s="57"/>
+      <c r="H156" s="57"/>
+      <c r="I156" s="57"/>
+      <c r="J156" s="57"/>
+      <c r="K156" s="57"/>
+      <c r="L156" s="57"/>
+      <c r="M156" s="57"/>
+      <c r="N156" s="57"/>
+      <c r="O156" s="57"/>
+      <c r="P156" s="57"/>
+      <c r="Q156" s="57"/>
+      <c r="R156" s="57"/>
+      <c r="S156" s="57"/>
+      <c r="T156" s="57"/>
+      <c r="U156" s="57"/>
+      <c r="V156" s="57"/>
+      <c r="W156" s="57"/>
+    </row>
+    <row r="157" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="B157" s="64"/>
-      <c r="C157" s="64"/>
-      <c r="D157" s="64"/>
-      <c r="E157" s="64"/>
-      <c r="F157" s="64"/>
-      <c r="G157" s="64"/>
-      <c r="H157" s="64"/>
-      <c r="I157" s="64"/>
-      <c r="J157" s="64"/>
-      <c r="K157" s="64"/>
-      <c r="L157" s="64"/>
-      <c r="M157" s="64"/>
-      <c r="N157" s="64"/>
-      <c r="O157" s="64"/>
-      <c r="P157" s="64"/>
-      <c r="Q157" s="64"/>
-      <c r="R157" s="64"/>
-      <c r="S157" s="64"/>
-      <c r="T157" s="64"/>
-      <c r="U157" s="64"/>
-      <c r="V157" s="64"/>
-      <c r="W157" s="64"/>
-    </row>
-    <row r="158" spans="1:23" ht="31" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B157" s="57"/>
+      <c r="C157" s="57"/>
+      <c r="D157" s="57"/>
+      <c r="E157" s="57"/>
+      <c r="F157" s="57"/>
+      <c r="G157" s="57"/>
+      <c r="H157" s="57"/>
+      <c r="I157" s="57"/>
+      <c r="J157" s="57"/>
+      <c r="K157" s="57"/>
+      <c r="L157" s="57"/>
+      <c r="M157" s="57"/>
+      <c r="N157" s="57"/>
+      <c r="O157" s="57"/>
+      <c r="P157" s="57"/>
+      <c r="Q157" s="57"/>
+      <c r="R157" s="57"/>
+      <c r="S157" s="57"/>
+      <c r="T157" s="57"/>
+      <c r="U157" s="57"/>
+      <c r="V157" s="57"/>
+      <c r="W157" s="57"/>
+    </row>
+    <row r="158" spans="1:23" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
         <v>5</v>
       </c>
@@ -9115,7 +8749,7 @@
       <c r="F158" s="82"/>
       <c r="G158" s="83"/>
     </row>
-    <row r="159" spans="1:23" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:23" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6"/>
       <c r="B159" s="7" t="s">
         <v>6</v>
@@ -9136,20 +8770,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B160" s="44">
-        <f t="shared" ref="B160:G161" si="3">10^-5</f>
+        <f t="shared" ref="B160:G161" si="5">10^-5</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C160" s="44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D160" s="44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E160" s="44">
@@ -9157,44 +8791,44 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F160" s="44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="G160" s="44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B161" s="44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C161" s="44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D161" s="44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E161" s="44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F161" s="44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="G161" s="44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="4" t="s">
         <v>17</v>
       </c>
@@ -9217,7 +8851,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
         <v>18</v>
       </c>
@@ -9240,7 +8874,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="4" t="s">
         <v>19</v>
       </c>
@@ -9263,7 +8897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="4" t="s">
         <v>20</v>
       </c>
@@ -9286,7 +8920,7 @@
         <v>5.333333333333333</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="4" t="s">
         <v>23</v>
       </c>
@@ -9309,7 +8943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
         <v>22</v>
       </c>
@@ -9332,7 +8966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
         <v>24</v>
       </c>
@@ -9355,7 +8989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
         <v>25</v>
       </c>
@@ -9378,7 +9012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="4" t="s">
         <v>26</v>
       </c>
@@ -9401,7 +9035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="4" t="s">
         <v>27</v>
       </c>
@@ -9424,7 +9058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="21" t="s">
         <v>49</v>
       </c>
@@ -9447,7 +9081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="21" t="s">
         <v>50</v>
       </c>
@@ -9470,7 +9104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="21" t="s">
         <v>51</v>
       </c>
@@ -9493,7 +9127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="21" t="s">
         <v>52</v>
       </c>
@@ -9516,49 +9150,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="10"/>
     </row>
-    <row r="182" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A182" s="63" t="s">
+    <row r="182" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A182" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="B182" s="64"/>
-      <c r="C182" s="64"/>
-      <c r="D182" s="64"/>
-      <c r="E182" s="64"/>
-      <c r="F182" s="64"/>
-      <c r="G182" s="64"/>
-      <c r="H182" s="64"/>
-      <c r="I182" s="64"/>
-      <c r="J182" s="64"/>
-      <c r="K182" s="64"/>
-      <c r="L182" s="64"/>
-      <c r="M182" s="64"/>
-      <c r="N182" s="64"/>
-      <c r="O182" s="64"/>
-      <c r="P182" s="64"/>
-      <c r="Q182" s="64"/>
-      <c r="R182" s="64"/>
-      <c r="S182" s="64"/>
-      <c r="T182" s="64"/>
-      <c r="U182" s="64"/>
-      <c r="V182" s="64"/>
-      <c r="W182" s="64"/>
-    </row>
-    <row r="183" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A183" s="85" t="s">
+      <c r="B182" s="57"/>
+      <c r="C182" s="57"/>
+      <c r="D182" s="57"/>
+      <c r="E182" s="57"/>
+      <c r="F182" s="57"/>
+      <c r="G182" s="57"/>
+      <c r="H182" s="57"/>
+      <c r="I182" s="57"/>
+      <c r="J182" s="57"/>
+      <c r="K182" s="57"/>
+      <c r="L182" s="57"/>
+      <c r="M182" s="57"/>
+      <c r="N182" s="57"/>
+      <c r="O182" s="57"/>
+      <c r="P182" s="57"/>
+      <c r="Q182" s="57"/>
+      <c r="R182" s="57"/>
+      <c r="S182" s="57"/>
+      <c r="T182" s="57"/>
+      <c r="U182" s="57"/>
+      <c r="V182" s="57"/>
+      <c r="W182" s="57"/>
+    </row>
+    <row r="183" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="B183" s="85"/>
-      <c r="C183" s="85"/>
-    </row>
-    <row r="184" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B183" s="84"/>
+      <c r="C183" s="84"/>
+    </row>
+    <row r="184" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>29</v>
       </c>
@@ -9569,7 +9203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="15">
         <v>1985</v>
       </c>
@@ -9580,7 +9214,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="186" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="15">
         <v>1990</v>
       </c>
@@ -9591,7 +9225,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="15">
         <v>2000</v>
       </c>
@@ -9602,941 +9236,917 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="194" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A194" s="63" t="s">
+    <row r="194" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A194" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="B194" s="64"/>
-      <c r="C194" s="64"/>
-      <c r="D194" s="64"/>
-      <c r="E194" s="64"/>
-      <c r="F194" s="64"/>
-      <c r="G194" s="64"/>
-      <c r="H194" s="64"/>
-      <c r="I194" s="64"/>
-      <c r="J194" s="64"/>
-      <c r="K194" s="64"/>
-      <c r="L194" s="64"/>
-      <c r="M194" s="64"/>
-      <c r="N194" s="64"/>
-      <c r="O194" s="64"/>
-      <c r="P194" s="64"/>
-      <c r="Q194" s="64"/>
-      <c r="R194" s="64"/>
-      <c r="S194" s="64"/>
-      <c r="T194" s="64"/>
-      <c r="U194" s="64"/>
-      <c r="V194" s="64"/>
-      <c r="W194" s="64"/>
-    </row>
-    <row r="195" spans="1:23" s="66" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A195" s="71" t="s">
+      <c r="B194" s="57"/>
+      <c r="C194" s="57"/>
+      <c r="D194" s="57"/>
+      <c r="E194" s="57"/>
+      <c r="F194" s="57"/>
+      <c r="G194" s="57"/>
+      <c r="H194" s="57"/>
+      <c r="I194" s="57"/>
+      <c r="J194" s="57"/>
+      <c r="K194" s="57"/>
+      <c r="L194" s="57"/>
+      <c r="M194" s="57"/>
+      <c r="N194" s="57"/>
+      <c r="O194" s="57"/>
+      <c r="P194" s="57"/>
+      <c r="Q194" s="57"/>
+      <c r="R194" s="57"/>
+      <c r="S194" s="57"/>
+      <c r="T194" s="57"/>
+      <c r="U194" s="57"/>
+      <c r="V194" s="57"/>
+      <c r="W194" s="57"/>
+    </row>
+    <row r="195" spans="1:23" s="59" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A195" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="B195" s="71"/>
-      <c r="C195" s="71"/>
-      <c r="D195" s="71"/>
-      <c r="E195" s="71"/>
-      <c r="F195" s="71"/>
-    </row>
-    <row r="196" spans="1:23" s="66" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A196" s="87" t="s">
+      <c r="B195" s="85"/>
+      <c r="C195" s="85"/>
+      <c r="D195" s="85"/>
+      <c r="E195" s="85"/>
+      <c r="F195" s="85"/>
+    </row>
+    <row r="196" spans="1:23" s="59" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A196" s="86" t="s">
         <v>94</v>
       </c>
-      <c r="B196" s="87"/>
-      <c r="C196" s="87"/>
-      <c r="D196" s="87"/>
-      <c r="E196" s="87"/>
-      <c r="F196" s="87"/>
-    </row>
-    <row r="197" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A197" s="88" t="s">
+      <c r="B196" s="86"/>
+      <c r="C196" s="86"/>
+      <c r="D196" s="86"/>
+      <c r="E196" s="86"/>
+      <c r="F196" s="86"/>
+    </row>
+    <row r="197" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A197" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="B197" s="89"/>
-      <c r="C197" s="89"/>
-      <c r="D197" s="88" t="s">
+      <c r="B197" s="66"/>
+      <c r="C197" s="66"/>
+      <c r="D197" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="E197" s="88"/>
-      <c r="F197" s="88"/>
-    </row>
-    <row r="198" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A198" s="88"/>
-      <c r="B198" s="89"/>
-      <c r="C198" s="90" t="s">
+      <c r="E197" s="78"/>
+      <c r="F197" s="78"/>
+    </row>
+    <row r="198" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A198" s="78"/>
+      <c r="B198" s="66"/>
+      <c r="C198" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="D198" s="90" t="s">
+      <c r="D198" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="E198" s="90" t="s">
+      <c r="E198" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="F198" s="90" t="s">
+      <c r="F198" s="67" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="199" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A199" s="91" t="s">
+    <row r="199" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A199" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="B199" s="89"/>
-      <c r="C199" s="89"/>
-      <c r="D199" s="92">
-        <v>0</v>
-      </c>
-      <c r="E199" s="92">
-        <v>0</v>
-      </c>
-      <c r="F199" s="92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A200" s="91" t="s">
+      <c r="B199" s="66"/>
+      <c r="C199" s="66"/>
+      <c r="D199" s="69">
+        <v>0</v>
+      </c>
+      <c r="E199" s="69">
+        <v>0</v>
+      </c>
+      <c r="F199" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A200" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="B200" s="89"/>
-      <c r="C200" s="89"/>
-      <c r="D200" s="92">
-        <v>0</v>
-      </c>
-      <c r="E200" s="92">
-        <v>0</v>
-      </c>
-      <c r="F200" s="92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A201" s="91" t="s">
+      <c r="B200" s="66"/>
+      <c r="C200" s="66"/>
+      <c r="D200" s="69">
+        <v>0</v>
+      </c>
+      <c r="E200" s="69">
+        <v>0</v>
+      </c>
+      <c r="F200" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A201" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="B201" s="89"/>
-      <c r="C201" s="89">
+      <c r="B201" s="66"/>
+      <c r="C201" s="66">
         <v>0.05</v>
       </c>
-      <c r="D201" s="93">
+      <c r="D201" s="70">
         <f>C201*D203</f>
         <v>3.1200000000000006</v>
       </c>
-      <c r="E201" s="93">
+      <c r="E201" s="70">
         <f>E203*$C$201</f>
         <v>1.8719999999999999</v>
       </c>
-      <c r="F201" s="93">
+      <c r="F201" s="70">
         <f>F203*$C$201</f>
         <v>1.1232</v>
       </c>
     </row>
-    <row r="202" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A202" s="91" t="s">
+    <row r="202" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A202" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="B202" s="89"/>
-      <c r="C202" s="89">
+      <c r="B202" s="66"/>
+      <c r="C202" s="66">
         <v>0.1</v>
       </c>
-      <c r="D202" s="93">
+      <c r="D202" s="70">
         <f>D204*$C$202</f>
         <v>15.600000000000001</v>
       </c>
-      <c r="E202" s="93">
+      <c r="E202" s="70">
         <f>E204*$C$202</f>
         <v>9.36</v>
       </c>
-      <c r="F202" s="93">
+      <c r="F202" s="70">
         <f>F204*$C$202</f>
         <v>5.6159999999999997</v>
       </c>
     </row>
-    <row r="203" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A203" s="91" t="s">
+    <row r="203" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A203" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="B203" s="94">
+      <c r="B203" s="71">
         <v>1</v>
       </c>
-      <c r="C203" s="89">
+      <c r="C203" s="66">
         <v>0.4</v>
       </c>
-      <c r="D203" s="92">
+      <c r="D203" s="69">
         <f>D204*$C$203</f>
         <v>62.400000000000006</v>
       </c>
-      <c r="E203" s="92">
+      <c r="E203" s="69">
         <f>E204*$C$203</f>
         <v>37.44</v>
       </c>
-      <c r="F203" s="92">
+      <c r="F203" s="69">
         <f>F204*$C$203</f>
         <v>22.463999999999999</v>
       </c>
     </row>
-    <row r="204" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A204" s="91" t="s">
+    <row r="204" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A204" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="B204" s="94">
+      <c r="B204" s="71">
         <v>5</v>
       </c>
-      <c r="C204" s="95"/>
-      <c r="D204" s="93">
-        <f>B240</f>
+      <c r="C204" s="72"/>
+      <c r="D204" s="70">
+        <f>B238</f>
         <v>156</v>
       </c>
-      <c r="E204" s="93">
-        <f>C240</f>
+      <c r="E204" s="70">
+        <f>C238</f>
         <v>93.6</v>
       </c>
-      <c r="F204" s="93">
-        <f>D240</f>
+      <c r="F204" s="70">
+        <f>D238</f>
         <v>56.16</v>
       </c>
     </row>
-    <row r="205" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A205" s="91" t="s">
+    <row r="205" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A205" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="B205" s="94">
+      <c r="B205" s="71">
         <v>10</v>
       </c>
-      <c r="C205" s="89">
-        <f t="shared" ref="C205:C215" si="4">EXP(LN(0.5)*B204/10)</f>
+      <c r="C205" s="66">
+        <f t="shared" ref="C205:C214" si="6">EXP(LN(0.5)*B204/10)</f>
         <v>0.70710678118654757</v>
       </c>
-      <c r="D205" s="93">
-        <f>$D$204*C205</f>
+      <c r="D205" s="70">
+        <f t="shared" ref="D205:D210" si="7">$D$204*C205</f>
         <v>110.30865786510142</v>
       </c>
-      <c r="E205" s="93">
-        <f>$E$204*C205</f>
+      <c r="E205" s="70">
+        <f t="shared" ref="E205:E210" si="8">$E$204*C205</f>
         <v>66.185194719060846</v>
       </c>
-      <c r="F205" s="93">
-        <f>$F$204*C205</f>
+      <c r="F205" s="70">
+        <f t="shared" ref="F205:F210" si="9">$F$204*C205</f>
         <v>39.711116831436506</v>
       </c>
-      <c r="M205" s="66"/>
-    </row>
-    <row r="206" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A206" s="91" t="s">
+      <c r="M205" s="59"/>
+    </row>
+    <row r="206" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A206" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="B206" s="94">
+      <c r="B206" s="71">
         <v>15</v>
       </c>
-      <c r="C206" s="89">
-        <f t="shared" si="4"/>
+      <c r="C206" s="66">
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
-      <c r="D206" s="93">
-        <f>$D$204*C206</f>
+      <c r="D206" s="70">
+        <f t="shared" si="7"/>
         <v>78</v>
       </c>
-      <c r="E206" s="93">
-        <f>$E$204*C206</f>
+      <c r="E206" s="70">
+        <f t="shared" si="8"/>
         <v>46.8</v>
       </c>
-      <c r="F206" s="93">
-        <f>$F$204*C206</f>
+      <c r="F206" s="70">
+        <f t="shared" si="9"/>
         <v>28.08</v>
       </c>
-      <c r="N206" s="66"/>
-      <c r="O206" s="66"/>
-      <c r="P206" s="66"/>
-    </row>
-    <row r="207" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A207" s="91" t="s">
+      <c r="N206" s="59"/>
+      <c r="O206" s="59"/>
+      <c r="P206" s="59"/>
+    </row>
+    <row r="207" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A207" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="B207" s="94">
+      <c r="B207" s="71">
         <v>20</v>
       </c>
-      <c r="C207" s="89">
-        <f t="shared" si="4"/>
+      <c r="C207" s="66">
+        <f t="shared" si="6"/>
         <v>0.35355339059327379</v>
       </c>
-      <c r="D207" s="93">
-        <f>$D$204*C207</f>
+      <c r="D207" s="70">
+        <f t="shared" si="7"/>
         <v>55.154328932550712</v>
       </c>
-      <c r="E207" s="93">
-        <f>$E$204*C207</f>
+      <c r="E207" s="70">
+        <f t="shared" si="8"/>
         <v>33.092597359530423</v>
       </c>
-      <c r="F207" s="93">
-        <f>$F$204*C207</f>
+      <c r="F207" s="70">
+        <f t="shared" si="9"/>
         <v>19.855558415718253</v>
       </c>
     </row>
-    <row r="208" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A208" s="91" t="s">
+    <row r="208" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A208" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="B208" s="94">
+      <c r="B208" s="71">
         <v>25</v>
       </c>
-      <c r="C208" s="89">
-        <f t="shared" si="4"/>
+      <c r="C208" s="66">
+        <f t="shared" si="6"/>
         <v>0.25</v>
       </c>
-      <c r="D208" s="93">
-        <f>$D$204*C208</f>
+      <c r="D208" s="70">
+        <f t="shared" si="7"/>
         <v>39</v>
       </c>
-      <c r="E208" s="93">
-        <f>$E$204*C208</f>
+      <c r="E208" s="70">
+        <f t="shared" si="8"/>
         <v>23.4</v>
       </c>
-      <c r="F208" s="93">
-        <f>$F$204*C208</f>
+      <c r="F208" s="70">
+        <f t="shared" si="9"/>
         <v>14.04</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A209" s="91" t="s">
+    <row r="209" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A209" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B209" s="94">
+      <c r="B209" s="71">
         <v>30</v>
       </c>
-      <c r="C209" s="89">
-        <f t="shared" si="4"/>
+      <c r="C209" s="66">
+        <f t="shared" si="6"/>
         <v>0.17677669529663689</v>
       </c>
-      <c r="D209" s="93">
-        <f>$D$204*C209</f>
+      <c r="D209" s="70">
+        <f t="shared" si="7"/>
         <v>27.577164466275356</v>
       </c>
-      <c r="E209" s="93">
-        <f>$E$204*C209</f>
+      <c r="E209" s="70">
+        <f t="shared" si="8"/>
         <v>16.546298679765211</v>
       </c>
-      <c r="F209" s="93">
-        <f>$F$204*C209</f>
+      <c r="F209" s="70">
+        <f t="shared" si="9"/>
         <v>9.9277792078591265</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A210" s="91" t="s">
+    <row r="210" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A210" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="B210" s="94">
+      <c r="B210" s="71">
         <v>35</v>
       </c>
-      <c r="C210" s="89">
-        <f t="shared" si="4"/>
+      <c r="C210" s="66">
+        <f t="shared" si="6"/>
         <v>0.12500000000000003</v>
       </c>
-      <c r="D210" s="93">
-        <f>$D$204*C210</f>
+      <c r="D210" s="70">
+        <f t="shared" si="7"/>
         <v>19.500000000000004</v>
       </c>
-      <c r="E210" s="93">
-        <f>$E$204*C210</f>
+      <c r="E210" s="70">
+        <f t="shared" si="8"/>
         <v>11.700000000000001</v>
       </c>
-      <c r="F210" s="93">
-        <f>$F$204*C210</f>
+      <c r="F210" s="70">
+        <f t="shared" si="9"/>
         <v>7.0200000000000014</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A211" s="91"/>
-      <c r="B211" s="94"/>
-      <c r="C211" s="89"/>
-      <c r="D211" s="93"/>
-      <c r="E211" s="93"/>
-      <c r="F211" s="93"/>
-    </row>
-    <row r="212" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A212" s="91" t="s">
+    <row r="211" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A211" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="B212" s="94">
+      <c r="B211" s="71">
         <v>40</v>
       </c>
-      <c r="C212" s="89">
+      <c r="C211" s="66">
         <f>EXP(LN(0.5)*B210/10)</f>
         <v>8.8388347648318447E-2</v>
       </c>
-      <c r="D212" s="93">
+      <c r="D211" s="70">
+        <f>$D$204*C211</f>
+        <v>13.788582233137678</v>
+      </c>
+      <c r="E211" s="70">
+        <f>$E$204*C211</f>
+        <v>8.2731493398826057</v>
+      </c>
+      <c r="F211" s="70">
+        <f>$F$204*C211</f>
+        <v>4.9638896039295632</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A212" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="B212" s="71">
+        <v>45</v>
+      </c>
+      <c r="C212" s="66">
+        <f t="shared" si="6"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="D212" s="70">
         <f>$D$204*C212</f>
+        <v>9.75</v>
+      </c>
+      <c r="E212" s="70">
+        <f>$E$204*C212</f>
+        <v>5.85</v>
+      </c>
+      <c r="F212" s="70">
+        <f>$F$204*C212</f>
+        <v>3.51</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A213" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="B213" s="71">
+        <v>50</v>
+      </c>
+      <c r="C213" s="66">
+        <f t="shared" si="6"/>
+        <v>4.4194173824159223E-2</v>
+      </c>
+      <c r="D213" s="70">
+        <f>$D$204*C213</f>
+        <v>6.894291116568839</v>
+      </c>
+      <c r="E213" s="70">
+        <f>$E$204*C213</f>
+        <v>4.1365746699413029</v>
+      </c>
+      <c r="F213" s="70">
+        <f>$F$204*C213</f>
+        <v>2.4819448019647816</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A214" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="B214" s="71">
+        <v>55</v>
+      </c>
+      <c r="C214" s="66">
+        <f t="shared" si="6"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="D214" s="70">
+        <f>$D$204*C214</f>
+        <v>4.875</v>
+      </c>
+      <c r="E214" s="70">
+        <f>$E$204*C214</f>
+        <v>2.9249999999999998</v>
+      </c>
+      <c r="F214" s="70">
+        <f>$F$204*C214</f>
+        <v>1.7549999999999999</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A215" s="66"/>
+      <c r="B215" s="71"/>
+      <c r="C215" s="66"/>
+      <c r="D215" s="73"/>
+      <c r="E215" s="73"/>
+      <c r="F215" s="73"/>
+    </row>
+    <row r="216" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A216" s="79" t="s">
+        <v>95</v>
+      </c>
+      <c r="B216" s="79"/>
+      <c r="C216" s="79"/>
+      <c r="D216" s="79"/>
+      <c r="E216" s="79"/>
+      <c r="F216" s="79"/>
+    </row>
+    <row r="217" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A217" s="80" t="s">
+        <v>2</v>
+      </c>
+      <c r="B217" s="66"/>
+      <c r="C217" s="66"/>
+      <c r="D217" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="E217" s="78"/>
+      <c r="F217" s="78"/>
+    </row>
+    <row r="218" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A218" s="80"/>
+      <c r="B218" s="66"/>
+      <c r="C218" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="D218" s="67" t="s">
+        <v>55</v>
+      </c>
+      <c r="E218" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="F218" s="67" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A219" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="B219" s="66"/>
+      <c r="C219" s="66"/>
+      <c r="D219" s="69">
+        <v>0</v>
+      </c>
+      <c r="E219" s="69">
+        <v>0</v>
+      </c>
+      <c r="F219" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A220" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B220" s="66"/>
+      <c r="C220" s="66"/>
+      <c r="D220" s="69">
+        <v>0</v>
+      </c>
+      <c r="E220" s="69">
+        <v>0</v>
+      </c>
+      <c r="F220" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A221" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="B221" s="66"/>
+      <c r="C221" s="66">
+        <v>0.05</v>
+      </c>
+      <c r="D221" s="69">
+        <f>$C$221*D224</f>
+        <v>7.8000000000000007</v>
+      </c>
+      <c r="E221" s="69">
+        <f>$C$221*E224</f>
+        <v>4.68</v>
+      </c>
+      <c r="F221" s="69">
+        <f>$C$221*F224</f>
+        <v>2.8079999999999998</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A222" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="B222" s="66"/>
+      <c r="C222" s="66">
+        <v>0.1</v>
+      </c>
+      <c r="D222" s="70">
+        <f>D224*$C$222</f>
+        <v>15.600000000000001</v>
+      </c>
+      <c r="E222" s="70">
+        <f>E224*$C$222</f>
+        <v>9.36</v>
+      </c>
+      <c r="F222" s="70">
+        <f>F224*$C$222</f>
+        <v>5.6159999999999997</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A223" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B223" s="71">
+        <v>1</v>
+      </c>
+      <c r="C223" s="66">
+        <v>0.4</v>
+      </c>
+      <c r="D223" s="69">
+        <f>D224*$C$223</f>
+        <v>62.400000000000006</v>
+      </c>
+      <c r="E223" s="69">
+        <f>E224*$C$223</f>
+        <v>37.44</v>
+      </c>
+      <c r="F223" s="69">
+        <f>F224*$C$223</f>
+        <v>22.463999999999999</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A224" s="68" t="s">
+        <v>42</v>
+      </c>
+      <c r="B224" s="71">
+        <v>5</v>
+      </c>
+      <c r="C224" s="72"/>
+      <c r="D224" s="69">
+        <f>B239</f>
+        <v>156</v>
+      </c>
+      <c r="E224" s="69">
+        <f>C239</f>
+        <v>93.6</v>
+      </c>
+      <c r="F224" s="69">
+        <f>D239</f>
+        <v>56.16</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A225" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="B225" s="71">
+        <v>10</v>
+      </c>
+      <c r="C225" s="66">
+        <f t="shared" ref="C225:C234" si="10">EXP(LN(0.5)*B224/10)</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="D225" s="69">
+        <f>D$224*$C$225</f>
+        <v>110.30865786510142</v>
+      </c>
+      <c r="E225" s="69">
+        <f>E$224*$C$225</f>
+        <v>66.185194719060846</v>
+      </c>
+      <c r="F225" s="69">
+        <f>F$224*$C$225</f>
+        <v>39.711116831436506</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A226" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="B226" s="71">
+        <v>15</v>
+      </c>
+      <c r="C226" s="66">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="D226" s="69">
+        <f t="shared" ref="D226:D232" si="11">$D$224*C226</f>
+        <v>78</v>
+      </c>
+      <c r="E226" s="69">
+        <f t="shared" ref="E226:E232" si="12">$E$224*C226</f>
+        <v>46.8</v>
+      </c>
+      <c r="F226" s="69">
+        <f t="shared" ref="F226:F232" si="13">$F$224*C226</f>
+        <v>28.08</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A227" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="B227" s="71">
+        <v>20</v>
+      </c>
+      <c r="C227" s="66">
+        <f t="shared" si="10"/>
+        <v>0.35355339059327379</v>
+      </c>
+      <c r="D227" s="69">
+        <f t="shared" si="11"/>
+        <v>55.154328932550712</v>
+      </c>
+      <c r="E227" s="69">
+        <f t="shared" si="12"/>
+        <v>33.092597359530423</v>
+      </c>
+      <c r="F227" s="69">
+        <f t="shared" si="13"/>
+        <v>19.855558415718253</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A228" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="B228" s="71">
+        <v>25</v>
+      </c>
+      <c r="C228" s="66">
+        <f t="shared" si="10"/>
+        <v>0.25</v>
+      </c>
+      <c r="D228" s="69">
+        <f t="shared" si="11"/>
+        <v>39</v>
+      </c>
+      <c r="E228" s="69">
+        <f t="shared" si="12"/>
+        <v>23.4</v>
+      </c>
+      <c r="F228" s="69">
+        <f t="shared" si="13"/>
+        <v>14.04</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A229" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="B229" s="71">
+        <v>30</v>
+      </c>
+      <c r="C229" s="66">
+        <f t="shared" si="10"/>
+        <v>0.17677669529663689</v>
+      </c>
+      <c r="D229" s="69">
+        <f t="shared" si="11"/>
+        <v>27.577164466275356</v>
+      </c>
+      <c r="E229" s="69">
+        <f t="shared" si="12"/>
+        <v>16.546298679765211</v>
+      </c>
+      <c r="F229" s="69">
+        <f t="shared" si="13"/>
+        <v>9.9277792078591265</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A230" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="B230" s="71">
+        <v>35</v>
+      </c>
+      <c r="C230" s="66">
+        <f t="shared" si="10"/>
+        <v>0.12500000000000003</v>
+      </c>
+      <c r="D230" s="69">
+        <f t="shared" si="11"/>
+        <v>19.500000000000004</v>
+      </c>
+      <c r="E230" s="69">
+        <f t="shared" si="12"/>
+        <v>11.700000000000001</v>
+      </c>
+      <c r="F230" s="69">
+        <f t="shared" si="13"/>
+        <v>7.0200000000000014</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A231" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="B231" s="71">
+        <v>40</v>
+      </c>
+      <c r="C231" s="66">
+        <f t="shared" si="10"/>
+        <v>8.8388347648318447E-2</v>
+      </c>
+      <c r="D231" s="69">
+        <f t="shared" si="11"/>
         <v>13.788582233137678</v>
       </c>
-      <c r="E212" s="93">
-        <f>$E$204*C212</f>
+      <c r="E231" s="69">
+        <f t="shared" si="12"/>
         <v>8.2731493398826057</v>
       </c>
-      <c r="F212" s="93">
-        <f>$F$204*C212</f>
+      <c r="F231" s="69">
+        <f t="shared" si="13"/>
         <v>4.9638896039295632</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A213" s="91" t="s">
+    <row r="232" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A232" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="B213" s="94">
+      <c r="B232" s="71">
         <v>45</v>
       </c>
-      <c r="C213" s="89">
-        <f t="shared" si="4"/>
+      <c r="C232" s="66">
+        <f t="shared" si="10"/>
         <v>6.25E-2</v>
       </c>
-      <c r="D213" s="93">
-        <f>$D$204*C213</f>
+      <c r="D232" s="69">
+        <f t="shared" si="11"/>
         <v>9.75</v>
       </c>
-      <c r="E213" s="93">
-        <f>$E$204*C213</f>
+      <c r="E232" s="69">
+        <f t="shared" si="12"/>
         <v>5.85</v>
       </c>
-      <c r="F213" s="93">
-        <f>$F$204*C213</f>
+      <c r="F232" s="69">
+        <f t="shared" si="13"/>
         <v>3.51</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A214" s="91" t="s">
+    <row r="233" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A233" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="B214" s="94">
+      <c r="B233" s="71">
         <v>50</v>
       </c>
-      <c r="C214" s="89">
-        <f t="shared" si="4"/>
+      <c r="C233" s="66">
+        <f>EXP(LN(0.5)*B232/10)</f>
         <v>4.4194173824159223E-2</v>
       </c>
-      <c r="D214" s="93">
-        <f>$D$204*C214</f>
+      <c r="D233" s="69">
+        <f>$D$224*C233</f>
         <v>6.894291116568839</v>
       </c>
-      <c r="E214" s="93">
-        <f>$E$204*C214</f>
+      <c r="E233" s="69">
+        <f>$E$224*C233</f>
         <v>4.1365746699413029</v>
       </c>
-      <c r="F214" s="93">
-        <f>$F$204*C214</f>
+      <c r="F233" s="69">
+        <f>$F$224*C233</f>
         <v>2.4819448019647816</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A215" s="91" t="s">
+    <row r="234" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A234" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="B215" s="94">
+      <c r="B234" s="71">
         <v>55</v>
       </c>
-      <c r="C215" s="89">
-        <f t="shared" si="4"/>
+      <c r="C234" s="66">
+        <f t="shared" si="10"/>
         <v>3.125E-2</v>
       </c>
-      <c r="D215" s="93">
-        <f>$D$204*C215</f>
+      <c r="D234" s="69">
+        <f>$D$224*C234</f>
         <v>4.875</v>
       </c>
-      <c r="E215" s="93">
-        <f>$E$204*C215</f>
+      <c r="E234" s="69">
+        <f>$E$224*C234</f>
         <v>2.9249999999999998</v>
       </c>
-      <c r="F215" s="93">
-        <f>$F$204*C215</f>
+      <c r="F234" s="69">
+        <f>$F$224*C234</f>
         <v>1.7549999999999999</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A216" s="89"/>
-      <c r="B216" s="94"/>
-      <c r="C216" s="89"/>
-      <c r="D216" s="96"/>
-      <c r="E216" s="96"/>
-      <c r="F216" s="96"/>
-    </row>
-    <row r="217" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A217" s="97" t="s">
-        <v>95</v>
-      </c>
-      <c r="B217" s="97"/>
-      <c r="C217" s="97"/>
-      <c r="D217" s="97"/>
-      <c r="E217" s="97"/>
-      <c r="F217" s="97"/>
-    </row>
-    <row r="218" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A218" s="98" t="s">
-        <v>2</v>
-      </c>
-      <c r="B218" s="89"/>
-      <c r="C218" s="89"/>
-      <c r="D218" s="88" t="s">
-        <v>58</v>
-      </c>
-      <c r="E218" s="88"/>
-      <c r="F218" s="88"/>
-    </row>
-    <row r="219" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A219" s="98"/>
-      <c r="B219" s="89"/>
-      <c r="C219" s="90" t="s">
-        <v>54</v>
-      </c>
-      <c r="D219" s="90" t="s">
-        <v>55</v>
-      </c>
-      <c r="E219" s="90" t="s">
-        <v>56</v>
-      </c>
-      <c r="F219" s="90" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A220" s="91" t="s">
-        <v>31</v>
-      </c>
-      <c r="B220" s="89"/>
-      <c r="C220" s="89"/>
-      <c r="D220" s="92">
-        <v>0</v>
-      </c>
-      <c r="E220" s="92">
-        <v>0</v>
-      </c>
-      <c r="F220" s="92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A221" s="91" t="s">
-        <v>30</v>
-      </c>
-      <c r="B221" s="89"/>
-      <c r="C221" s="89"/>
-      <c r="D221" s="92">
-        <v>0</v>
-      </c>
-      <c r="E221" s="92">
-        <v>0</v>
-      </c>
-      <c r="F221" s="92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A222" s="91" t="s">
-        <v>39</v>
-      </c>
-      <c r="B222" s="89"/>
-      <c r="C222" s="89">
-        <v>0.05</v>
-      </c>
-      <c r="D222" s="92">
-        <f>$C$222*D225</f>
-        <v>7.8000000000000007</v>
-      </c>
-      <c r="E222" s="92">
-        <f>$C$222*E225</f>
-        <v>4.68</v>
-      </c>
-      <c r="F222" s="92">
-        <f>$C$222*F225</f>
-        <v>2.8079999999999998</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A223" s="91" t="s">
-        <v>40</v>
-      </c>
-      <c r="B223" s="89"/>
-      <c r="C223" s="89">
-        <v>0.1</v>
-      </c>
-      <c r="D223" s="93">
-        <f>D225*$C$223</f>
-        <v>15.600000000000001</v>
-      </c>
-      <c r="E223" s="93">
-        <f>E225*$C$223</f>
-        <v>9.36</v>
-      </c>
-      <c r="F223" s="93">
-        <f>F225*$C$223</f>
-        <v>5.6159999999999997</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A224" s="91" t="s">
-        <v>41</v>
-      </c>
-      <c r="B224" s="94">
-        <v>1</v>
-      </c>
-      <c r="C224" s="89">
-        <v>0.4</v>
-      </c>
-      <c r="D224" s="92">
-        <f>D225*$C$224</f>
-        <v>62.400000000000006</v>
-      </c>
-      <c r="E224" s="92">
-        <f>E225*$C$224</f>
-        <v>37.44</v>
-      </c>
-      <c r="F224" s="92">
-        <f>F225*$C$224</f>
-        <v>22.463999999999999</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A225" s="91" t="s">
-        <v>42</v>
-      </c>
-      <c r="B225" s="94">
-        <v>5</v>
-      </c>
-      <c r="C225" s="95"/>
-      <c r="D225" s="92">
-        <f>B241</f>
-        <v>156</v>
-      </c>
-      <c r="E225" s="92">
-        <f>C241</f>
-        <v>93.6</v>
-      </c>
-      <c r="F225" s="92">
-        <f>D241</f>
-        <v>56.16</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A226" s="91" t="s">
-        <v>43</v>
-      </c>
-      <c r="B226" s="94">
-        <v>10</v>
-      </c>
-      <c r="C226" s="89">
-        <f t="shared" ref="C226:C236" si="5">EXP(LN(0.5)*B225/10)</f>
-        <v>0.70710678118654757</v>
-      </c>
-      <c r="D226" s="92">
-        <f>D$225*$C$226</f>
-        <v>110.30865786510142</v>
-      </c>
-      <c r="E226" s="92">
-        <f>E$225*$C$226</f>
-        <v>66.185194719060846</v>
-      </c>
-      <c r="F226" s="92">
-        <f>F$225*$C$226</f>
-        <v>39.711116831436506</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A227" s="91" t="s">
-        <v>44</v>
-      </c>
-      <c r="B227" s="94">
-        <v>15</v>
-      </c>
-      <c r="C227" s="89">
-        <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="D227" s="92">
-        <f>$D$225*C227</f>
-        <v>78</v>
-      </c>
-      <c r="E227" s="92">
-        <f>$E$225*C227</f>
-        <v>46.8</v>
-      </c>
-      <c r="F227" s="92">
-        <f>$F$225*C227</f>
-        <v>28.08</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A228" s="91" t="s">
-        <v>45</v>
-      </c>
-      <c r="B228" s="94">
-        <v>20</v>
-      </c>
-      <c r="C228" s="89">
-        <f t="shared" si="5"/>
-        <v>0.35355339059327379</v>
-      </c>
-      <c r="D228" s="92">
-        <f>$D$225*C228</f>
-        <v>55.154328932550712</v>
-      </c>
-      <c r="E228" s="92">
-        <f>$E$225*C228</f>
-        <v>33.092597359530423</v>
-      </c>
-      <c r="F228" s="92">
-        <f>$F$225*C228</f>
-        <v>19.855558415718253</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A229" s="91" t="s">
-        <v>46</v>
-      </c>
-      <c r="B229" s="94">
-        <v>25</v>
-      </c>
-      <c r="C229" s="89">
-        <f t="shared" si="5"/>
-        <v>0.25</v>
-      </c>
-      <c r="D229" s="92">
-        <f>$D$225*C229</f>
-        <v>39</v>
-      </c>
-      <c r="E229" s="92">
-        <f>$E$225*C229</f>
-        <v>23.4</v>
-      </c>
-      <c r="F229" s="92">
-        <f>$F$225*C229</f>
-        <v>14.04</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A230" s="91" t="s">
-        <v>47</v>
-      </c>
-      <c r="B230" s="94">
-        <v>30</v>
-      </c>
-      <c r="C230" s="89">
-        <f t="shared" si="5"/>
-        <v>0.17677669529663689</v>
-      </c>
-      <c r="D230" s="92">
-        <f>$D$225*C230</f>
-        <v>27.577164466275356</v>
-      </c>
-      <c r="E230" s="92">
-        <f>$E$225*C230</f>
-        <v>16.546298679765211</v>
-      </c>
-      <c r="F230" s="92">
-        <f>$F$225*C230</f>
-        <v>9.9277792078591265</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A231" s="91" t="s">
-        <v>48</v>
-      </c>
-      <c r="B231" s="94">
-        <v>35</v>
-      </c>
-      <c r="C231" s="89">
-        <f t="shared" si="5"/>
-        <v>0.12500000000000003</v>
-      </c>
-      <c r="D231" s="92">
-        <f>$D$225*C231</f>
-        <v>19.500000000000004</v>
-      </c>
-      <c r="E231" s="92">
-        <f>$E$225*C231</f>
-        <v>11.700000000000001</v>
-      </c>
-      <c r="F231" s="92">
-        <f>$F$225*C231</f>
-        <v>7.0200000000000014</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A232" s="91" t="s">
-        <v>49</v>
-      </c>
-      <c r="B232" s="94">
-        <v>40</v>
-      </c>
-      <c r="C232" s="89">
-        <f t="shared" si="5"/>
-        <v>8.8388347648318447E-2</v>
-      </c>
-      <c r="D232" s="92">
-        <f>$D$225*C232</f>
-        <v>13.788582233137678</v>
-      </c>
-      <c r="E232" s="92">
-        <f>$E$225*C232</f>
-        <v>8.2731493398826057</v>
-      </c>
-      <c r="F232" s="92">
-        <f>$F$225*C232</f>
-        <v>4.9638896039295632</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A233" s="91" t="s">
-        <v>50</v>
-      </c>
-      <c r="B233" s="94">
-        <v>45</v>
-      </c>
-      <c r="C233" s="89">
-        <f t="shared" si="5"/>
-        <v>6.25E-2</v>
-      </c>
-      <c r="D233" s="92">
-        <f>$D$225*C233</f>
-        <v>9.75</v>
-      </c>
-      <c r="E233" s="92">
-        <f>$E$225*C233</f>
-        <v>5.85</v>
-      </c>
-      <c r="F233" s="92">
-        <f>$F$225*C233</f>
-        <v>3.51</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A234" s="91"/>
-      <c r="B234" s="94"/>
-      <c r="C234" s="89"/>
-      <c r="D234" s="92"/>
-      <c r="E234" s="92"/>
-      <c r="F234" s="92"/>
-    </row>
-    <row r="235" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A235" s="91" t="s">
-        <v>51</v>
-      </c>
-      <c r="B235" s="94">
-        <v>50</v>
-      </c>
-      <c r="C235" s="89">
-        <f>EXP(LN(0.5)*B233/10)</f>
-        <v>4.4194173824159223E-2</v>
-      </c>
-      <c r="D235" s="92">
-        <f>$D$225*C235</f>
-        <v>6.894291116568839</v>
-      </c>
-      <c r="E235" s="92">
-        <f>$E$225*C235</f>
-        <v>4.1365746699413029</v>
-      </c>
-      <c r="F235" s="92">
-        <f>$F$225*C235</f>
-        <v>2.4819448019647816</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A236" s="91" t="s">
-        <v>52</v>
-      </c>
-      <c r="B236" s="94">
-        <v>55</v>
-      </c>
-      <c r="C236" s="89">
-        <f t="shared" si="5"/>
-        <v>3.125E-2</v>
-      </c>
-      <c r="D236" s="92">
-        <f>$D$225*C236</f>
-        <v>4.875</v>
-      </c>
-      <c r="E236" s="92">
-        <f>$E$225*C236</f>
-        <v>2.9249999999999998</v>
-      </c>
-      <c r="F236" s="92">
-        <f>$F$225*C236</f>
-        <v>1.7549999999999999</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A237" s="62"/>
-      <c r="B237" s="62"/>
-      <c r="C237" s="86"/>
-      <c r="D237" s="62"/>
-      <c r="E237" s="62"/>
-      <c r="F237" s="62"/>
-    </row>
-    <row r="238" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A238" s="84" t="s">
+    <row r="235" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A235" s="55"/>
+      <c r="B235" s="55"/>
+      <c r="C235" s="65"/>
+      <c r="D235" s="55"/>
+      <c r="E235" s="55"/>
+      <c r="F235" s="55"/>
+    </row>
+    <row r="236" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A236" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="B238" s="66"/>
-      <c r="C238" s="66"/>
-      <c r="D238" s="66"/>
-      <c r="E238" s="62"/>
-      <c r="F238" s="62"/>
-    </row>
-    <row r="239" spans="1:6" ht="31" x14ac:dyDescent="0.35">
-      <c r="A239" s="101" t="s">
+      <c r="B236" s="59"/>
+      <c r="C236" s="59"/>
+      <c r="D236" s="59"/>
+      <c r="E236" s="55"/>
+      <c r="F236" s="55"/>
+    </row>
+    <row r="237" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A237" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="B239" s="102" t="s">
+      <c r="B237" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C239" s="102" t="s">
+      <c r="C237" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="D239" s="102" t="s">
+      <c r="D237" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="E239" s="62"/>
-      <c r="F239" s="62"/>
-    </row>
-    <row r="240" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A240" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B240" s="94">
+      <c r="E237" s="55"/>
+      <c r="F237" s="55"/>
+    </row>
+    <row r="238" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A238" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B238" s="71">
         <f>52*3</f>
         <v>156</v>
       </c>
-      <c r="C240" s="94">
-        <f>B240*0.6</f>
+      <c r="C238" s="71">
+        <f>B238*0.6</f>
         <v>93.6</v>
       </c>
-      <c r="D240" s="94">
-        <f>C240*0.6</f>
+      <c r="D238" s="71">
+        <f>C238*0.6</f>
         <v>56.16</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A241" s="26" t="s">
+    <row r="239" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A239" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B241" s="94">
+      <c r="B239" s="71">
         <f>52*3</f>
         <v>156</v>
       </c>
-      <c r="C241" s="94">
-        <f>B241*0.6</f>
+      <c r="C239" s="71">
+        <f>B239*0.6</f>
         <v>93.6</v>
       </c>
-      <c r="D241" s="94">
-        <f>C241*0.6</f>
+      <c r="D239" s="71">
+        <f>C239*0.6</f>
         <v>56.16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="A217:F217"/>
-    <mergeCell ref="A218:A219"/>
-    <mergeCell ref="B158:D158"/>
-    <mergeCell ref="E158:G158"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A195:F195"/>
-    <mergeCell ref="A196:F196"/>
     <mergeCell ref="A109:A111"/>
     <mergeCell ref="B109:G109"/>
     <mergeCell ref="B130:G130"/>
@@ -10549,8 +10159,16 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="B81:B83"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="A216:F216"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="B158:D158"/>
+    <mergeCell ref="E158:G158"/>
+    <mergeCell ref="A183:C183"/>
+    <mergeCell ref="A195:F195"/>
+    <mergeCell ref="A196:F196"/>
     <mergeCell ref="D197:F197"/>
-    <mergeCell ref="D218:F218"/>
+    <mergeCell ref="D217:F217"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added hpvImmVaxd2 to calcInds.m. Load in to script via Params/mixInfectIndices2.mat.
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15840" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -1562,33 +1562,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1622,6 +1595,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1636,6 +1612,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -6090,8 +6090,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B241" sqref="B241"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6103,7 +6103,7 @@
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25" customWidth="1"/>
@@ -6219,10 +6219,10 @@
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="97"/>
+      <c r="C4" s="88"/>
     </row>
     <row r="5" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="60"/>
@@ -6459,10 +6459,10 @@
       <c r="A27" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="85" t="s">
+      <c r="B27" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="98"/>
+      <c r="C27" s="90"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
@@ -6850,19 +6850,19 @@
       <c r="AE51" s="36"/>
     </row>
     <row r="52" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="102" t="s">
+      <c r="A52" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="102" t="s">
+      <c r="B52" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="102"/>
-      <c r="D52" s="102"/>
-      <c r="E52" s="102" t="s">
+      <c r="C52" s="94"/>
+      <c r="D52" s="94"/>
+      <c r="E52" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="102"/>
-      <c r="G52" s="102"/>
+      <c r="F52" s="94"/>
+      <c r="G52" s="94"/>
       <c r="X52" s="34"/>
       <c r="Y52" s="34"/>
       <c r="Z52" s="34"/>
@@ -6873,7 +6873,7 @@
       <c r="AE52" s="34"/>
     </row>
     <row r="53" spans="1:31" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="102"/>
+      <c r="A53" s="94"/>
       <c r="B53" s="52" t="s">
         <v>6</v>
       </c>
@@ -7407,25 +7407,25 @@
       <c r="X80" s="57"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="87" t="s">
+      <c r="A81" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="99" t="s">
+      <c r="B81" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="99" t="s">
+      <c r="C81" s="91" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="88"/>
-      <c r="B82" s="100"/>
-      <c r="C82" s="100"/>
+      <c r="A82" s="79"/>
+      <c r="B82" s="92"/>
+      <c r="C82" s="92"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="89"/>
-      <c r="B83" s="101"/>
-      <c r="C83" s="101"/>
+      <c r="A83" s="80"/>
+      <c r="B83" s="93"/>
+      <c r="C83" s="93"/>
     </row>
     <row r="84" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
@@ -7716,20 +7716,20 @@
       <c r="X108" s="57"/>
     </row>
     <row r="109" spans="1:24" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="87" t="s">
+      <c r="A109" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B109" s="90" t="s">
+      <c r="B109" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="C109" s="91"/>
-      <c r="D109" s="91"/>
-      <c r="E109" s="91"/>
-      <c r="F109" s="91"/>
-      <c r="G109" s="92"/>
+      <c r="C109" s="82"/>
+      <c r="D109" s="82"/>
+      <c r="E109" s="82"/>
+      <c r="F109" s="82"/>
+      <c r="G109" s="83"/>
     </row>
     <row r="110" spans="1:24" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="88"/>
+      <c r="A110" s="79"/>
       <c r="B110" s="51" t="s">
         <v>83</v>
       </c>
@@ -7750,7 +7750,7 @@
       </c>
     </row>
     <row r="111" spans="1:24" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="89"/>
+      <c r="A111" s="80"/>
       <c r="B111" s="53" t="s">
         <v>76</v>
       </c>
@@ -8205,20 +8205,20 @@
     </row>
     <row r="129" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="93" t="s">
+      <c r="A130" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="B130" s="90" t="s">
+      <c r="B130" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="C130" s="91"/>
-      <c r="D130" s="91"/>
-      <c r="E130" s="91"/>
-      <c r="F130" s="91"/>
-      <c r="G130" s="92"/>
+      <c r="C130" s="82"/>
+      <c r="D130" s="82"/>
+      <c r="E130" s="82"/>
+      <c r="F130" s="82"/>
+      <c r="G130" s="83"/>
     </row>
     <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="94"/>
+      <c r="A131" s="85"/>
       <c r="B131" s="38" t="s">
         <v>86</v>
       </c>
@@ -8239,7 +8239,7 @@
       </c>
     </row>
     <row r="132" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="95"/>
+      <c r="A132" s="86"/>
       <c r="B132" s="62" t="s">
         <v>76</v>
       </c>
@@ -8738,16 +8738,16 @@
       <c r="A158" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B158" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="C158" s="82"/>
-      <c r="D158" s="83"/>
-      <c r="E158" s="81" t="s">
+      <c r="B158" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" s="99"/>
+      <c r="D158" s="100"/>
+      <c r="E158" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="F158" s="82"/>
-      <c r="G158" s="83"/>
+      <c r="F158" s="99"/>
+      <c r="G158" s="100"/>
     </row>
     <row r="159" spans="1:23" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6"/>
@@ -8798,8 +8798,20 @@
         <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J160">
+        <f>B160*B54</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K160">
+        <f t="shared" ref="K160:L175" si="6">C160*C54</f>
+        <v>0</v>
+      </c>
+      <c r="L160">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="4" t="s">
         <v>14</v>
       </c>
@@ -8827,8 +8839,20 @@
         <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J161">
+        <f t="shared" ref="J161:J175" si="7">B161*B55</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K161">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L161">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="4" t="s">
         <v>17</v>
       </c>
@@ -8850,8 +8874,28 @@
       <c r="G162" s="46">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J162">
+        <f t="shared" si="7"/>
+        <v>1.176E-2</v>
+      </c>
+      <c r="K162">
+        <f t="shared" si="6"/>
+        <v>1.8E-3</v>
+      </c>
+      <c r="L162">
+        <f t="shared" si="6"/>
+        <v>6.0000000000000218E-3</v>
+      </c>
+      <c r="M162">
+        <f>SUM(J162:L162)</f>
+        <v>1.9560000000000022E-2</v>
+      </c>
+      <c r="N162">
+        <f>1/M162</f>
+        <v>51.124744376278059</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
         <v>18</v>
       </c>
@@ -8873,8 +8917,28 @@
       <c r="G163" s="47">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J163">
+        <f t="shared" si="7"/>
+        <v>0.33787878787878783</v>
+      </c>
+      <c r="K163">
+        <f t="shared" si="6"/>
+        <v>1.040909090909091</v>
+      </c>
+      <c r="L163">
+        <f t="shared" si="6"/>
+        <v>0.58030303030303021</v>
+      </c>
+      <c r="M163">
+        <f t="shared" ref="M163:M175" si="8">SUM(J163:L163)</f>
+        <v>1.959090909090909</v>
+      </c>
+      <c r="N163">
+        <f t="shared" ref="N163:N175" si="9">1/M163</f>
+        <v>0.51044083526682138</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="4" t="s">
         <v>19</v>
       </c>
@@ -8896,8 +8960,28 @@
       <c r="G164" s="47">
         <v>10</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J164">
+        <f t="shared" si="7"/>
+        <v>0.33193277310924363</v>
+      </c>
+      <c r="K164">
+        <f t="shared" si="6"/>
+        <v>1.1274509803921566</v>
+      </c>
+      <c r="L164">
+        <f t="shared" si="6"/>
+        <v>0.65546218487394958</v>
+      </c>
+      <c r="M164">
+        <f t="shared" si="8"/>
+        <v>2.1148459383753497</v>
+      </c>
+      <c r="N164">
+        <f t="shared" si="9"/>
+        <v>0.47284768211920541</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="4" t="s">
         <v>20</v>
       </c>
@@ -8919,8 +9003,28 @@
       <c r="G165" s="47">
         <v>5.333333333333333</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J165">
+        <f t="shared" si="7"/>
+        <v>0.39310344827586208</v>
+      </c>
+      <c r="K165">
+        <f t="shared" si="6"/>
+        <v>1.0551724137931036</v>
+      </c>
+      <c r="L165">
+        <f t="shared" si="6"/>
+        <v>0.54482758620689653</v>
+      </c>
+      <c r="M165">
+        <f t="shared" si="8"/>
+        <v>1.9931034482758623</v>
+      </c>
+      <c r="N165">
+        <f t="shared" si="9"/>
+        <v>0.50173010380622829</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="4" t="s">
         <v>23</v>
       </c>
@@ -8942,8 +9046,28 @@
       <c r="G166" s="47">
         <v>1</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J166">
+        <f t="shared" si="7"/>
+        <v>0.46610169491525422</v>
+      </c>
+      <c r="K166">
+        <f t="shared" si="6"/>
+        <v>0.84745762711864414</v>
+      </c>
+      <c r="L166">
+        <f t="shared" si="6"/>
+        <v>0.3135593220338983</v>
+      </c>
+      <c r="M166">
+        <f t="shared" si="8"/>
+        <v>1.6271186440677967</v>
+      </c>
+      <c r="N166">
+        <f t="shared" si="9"/>
+        <v>0.61458333333333326</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
         <v>22</v>
       </c>
@@ -8965,8 +9089,28 @@
       <c r="G167" s="47">
         <v>9</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J167">
+        <f t="shared" si="7"/>
+        <v>0.59655172413793101</v>
+      </c>
+      <c r="K167">
+        <f t="shared" si="6"/>
+        <v>0.48965517241379303</v>
+      </c>
+      <c r="L167">
+        <f t="shared" si="6"/>
+        <v>0.19310344827586207</v>
+      </c>
+      <c r="M167">
+        <f t="shared" si="8"/>
+        <v>1.279310344827586</v>
+      </c>
+      <c r="N167">
+        <f t="shared" si="9"/>
+        <v>0.78167115902964968</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
         <v>24</v>
       </c>
@@ -8988,8 +9132,28 @@
       <c r="G168" s="47">
         <v>1</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J168">
+        <f t="shared" si="7"/>
+        <v>0.68881118881118875</v>
+      </c>
+      <c r="K168">
+        <f t="shared" si="6"/>
+        <v>0.40559440559440557</v>
+      </c>
+      <c r="L168">
+        <f t="shared" si="6"/>
+        <v>0.10839160839160839</v>
+      </c>
+      <c r="M168">
+        <f t="shared" si="8"/>
+        <v>1.2027972027972027</v>
+      </c>
+      <c r="N168">
+        <f t="shared" si="9"/>
+        <v>0.83139534883720934</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
         <v>25</v>
       </c>
@@ -9011,8 +9175,28 @@
       <c r="G169" s="47">
         <v>1</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J169">
+        <f t="shared" si="7"/>
+        <v>0.61194029850746268</v>
+      </c>
+      <c r="K169">
+        <f t="shared" si="6"/>
+        <v>0.34468992537313536</v>
+      </c>
+      <c r="L169">
+        <f t="shared" si="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="M169">
+        <f t="shared" si="8"/>
+        <v>0.95763022388059804</v>
+      </c>
+      <c r="N169">
+        <f t="shared" si="9"/>
+        <v>1.0442444015057371</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="4" t="s">
         <v>26</v>
       </c>
@@ -9034,8 +9218,28 @@
       <c r="G170" s="47">
         <v>1</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J170">
+        <f t="shared" si="7"/>
+        <v>0.61194029850746268</v>
+      </c>
+      <c r="K170">
+        <f t="shared" si="6"/>
+        <v>0.34468992537313536</v>
+      </c>
+      <c r="L170">
+        <f t="shared" si="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="M170">
+        <f t="shared" si="8"/>
+        <v>0.95763022388059804</v>
+      </c>
+      <c r="N170">
+        <f t="shared" si="9"/>
+        <v>1.0442444015057371</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="4" t="s">
         <v>27</v>
       </c>
@@ -9057,8 +9261,28 @@
       <c r="G171" s="47">
         <v>1</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J171">
+        <f t="shared" si="7"/>
+        <v>0.61194029850746268</v>
+      </c>
+      <c r="K171">
+        <f t="shared" si="6"/>
+        <v>0.34468992537313536</v>
+      </c>
+      <c r="L171">
+        <f t="shared" si="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="M171">
+        <f t="shared" si="8"/>
+        <v>0.95763022388059804</v>
+      </c>
+      <c r="N171">
+        <f t="shared" si="9"/>
+        <v>1.0442444015057371</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="21" t="s">
         <v>49</v>
       </c>
@@ -9080,8 +9304,28 @@
       <c r="G172" s="50">
         <v>1</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J172">
+        <f t="shared" si="7"/>
+        <v>0.61194029850746268</v>
+      </c>
+      <c r="K172">
+        <f t="shared" si="6"/>
+        <v>0.34468992537313536</v>
+      </c>
+      <c r="L172">
+        <f t="shared" si="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="M172">
+        <f t="shared" si="8"/>
+        <v>0.95763022388059804</v>
+      </c>
+      <c r="N172">
+        <f t="shared" si="9"/>
+        <v>1.0442444015057371</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="21" t="s">
         <v>50</v>
       </c>
@@ -9103,8 +9347,28 @@
       <c r="G173" s="50">
         <v>1</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J173">
+        <f t="shared" si="7"/>
+        <v>0.61194029850746268</v>
+      </c>
+      <c r="K173">
+        <f t="shared" si="6"/>
+        <v>0.34468992537313536</v>
+      </c>
+      <c r="L173">
+        <f t="shared" si="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="M173">
+        <f t="shared" si="8"/>
+        <v>0.95763022388059804</v>
+      </c>
+      <c r="N173">
+        <f t="shared" si="9"/>
+        <v>1.0442444015057371</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="21" t="s">
         <v>51</v>
       </c>
@@ -9126,8 +9390,28 @@
       <c r="G174" s="50">
         <v>1</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J174">
+        <f t="shared" si="7"/>
+        <v>0.61194029850746268</v>
+      </c>
+      <c r="K174">
+        <f t="shared" si="6"/>
+        <v>0.34468992537313536</v>
+      </c>
+      <c r="L174">
+        <f t="shared" si="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="M174">
+        <f t="shared" si="8"/>
+        <v>0.95763022388059804</v>
+      </c>
+      <c r="N174">
+        <f t="shared" si="9"/>
+        <v>1.0442444015057371</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="21" t="s">
         <v>52</v>
       </c>
@@ -9149,10 +9433,38 @@
       <c r="G175" s="50">
         <v>1</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H175">
+        <f>SUM(B160:D175)/(3*16)</f>
+        <v>1.8866801277495602</v>
+      </c>
+      <c r="J175">
+        <f t="shared" si="7"/>
+        <v>0.61194029850746268</v>
+      </c>
+      <c r="K175">
+        <f t="shared" si="6"/>
+        <v>0.34468992537313536</v>
+      </c>
+      <c r="L175">
+        <f t="shared" si="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="M175">
+        <f t="shared" si="8"/>
+        <v>0.95763022388059804</v>
+      </c>
+      <c r="N175">
+        <f t="shared" si="9"/>
+        <v>1.0442444015057371</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>37</v>
+      </c>
+      <c r="N176">
+        <f>AVERAGE(N162:N175)</f>
+        <v>4.4390802606579047</v>
       </c>
     </row>
     <row r="180" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
@@ -9186,11 +9498,11 @@
       <c r="W182" s="57"/>
     </row>
     <row r="183" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="84" t="s">
+      <c r="A183" s="101" t="s">
         <v>92</v>
       </c>
-      <c r="B183" s="84"/>
-      <c r="C183" s="84"/>
+      <c r="B183" s="101"/>
+      <c r="C183" s="101"/>
     </row>
     <row r="184" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
@@ -9264,39 +9576,39 @@
       <c r="W194" s="57"/>
     </row>
     <row r="195" spans="1:23" s="59" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A195" s="85" t="s">
+      <c r="A195" s="89" t="s">
         <v>93</v>
       </c>
-      <c r="B195" s="85"/>
-      <c r="C195" s="85"/>
-      <c r="D195" s="85"/>
-      <c r="E195" s="85"/>
-      <c r="F195" s="85"/>
+      <c r="B195" s="89"/>
+      <c r="C195" s="89"/>
+      <c r="D195" s="89"/>
+      <c r="E195" s="89"/>
+      <c r="F195" s="89"/>
     </row>
     <row r="196" spans="1:23" s="59" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A196" s="86" t="s">
+      <c r="A196" s="102" t="s">
         <v>94</v>
       </c>
-      <c r="B196" s="86"/>
-      <c r="C196" s="86"/>
-      <c r="D196" s="86"/>
-      <c r="E196" s="86"/>
-      <c r="F196" s="86"/>
+      <c r="B196" s="102"/>
+      <c r="C196" s="102"/>
+      <c r="D196" s="102"/>
+      <c r="E196" s="102"/>
+      <c r="F196" s="102"/>
     </row>
     <row r="197" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A197" s="78" t="s">
+      <c r="A197" s="95" t="s">
         <v>53</v>
       </c>
       <c r="B197" s="66"/>
       <c r="C197" s="66"/>
-      <c r="D197" s="78" t="s">
+      <c r="D197" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="E197" s="78"/>
-      <c r="F197" s="78"/>
+      <c r="E197" s="95"/>
+      <c r="F197" s="95"/>
     </row>
     <row r="198" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="78"/>
+      <c r="A198" s="95"/>
       <c r="B198" s="66"/>
       <c r="C198" s="67" t="s">
         <v>54</v>
@@ -9310,6 +9622,10 @@
       <c r="F198" s="67" t="s">
         <v>57</v>
       </c>
+      <c r="H198">
+        <f>(365.25/7)*2.4</f>
+        <v>125.22857142857143</v>
+      </c>
     </row>
     <row r="199" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A199" s="68" t="s">
@@ -9326,6 +9642,18 @@
       <c r="F199" s="69">
         <v>0</v>
       </c>
+      <c r="H199">
+        <f>D199*B54</f>
+        <v>0</v>
+      </c>
+      <c r="I199">
+        <f t="shared" ref="I199:J214" si="10">E199*C54</f>
+        <v>0</v>
+      </c>
+      <c r="J199">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="200" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A200" s="68" t="s">
@@ -9342,6 +9670,18 @@
       <c r="F200" s="69">
         <v>0</v>
       </c>
+      <c r="H200">
+        <f t="shared" ref="H200:H214" si="11">D200*B55</f>
+        <v>0</v>
+      </c>
+      <c r="I200">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="J200">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="201" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="68" t="s">
@@ -9363,6 +9703,22 @@
         <f>F203*$C$201</f>
         <v>1.1232</v>
       </c>
+      <c r="H201">
+        <f t="shared" si="11"/>
+        <v>3.0576000000000003</v>
+      </c>
+      <c r="I201">
+        <f t="shared" si="10"/>
+        <v>2.8079999999999997E-2</v>
+      </c>
+      <c r="J201">
+        <f t="shared" si="10"/>
+        <v>5.6160000000000203E-3</v>
+      </c>
+      <c r="K201">
+        <f>SUM(H201:J201)</f>
+        <v>3.0912960000000003</v>
+      </c>
     </row>
     <row r="202" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A202" s="68" t="s">
@@ -9384,6 +9740,22 @@
         <f>F204*$C$202</f>
         <v>5.6159999999999997</v>
       </c>
+      <c r="H202">
+        <f t="shared" si="11"/>
+        <v>7.9418181818181814</v>
+      </c>
+      <c r="I202">
+        <f t="shared" si="10"/>
+        <v>3.814909090909091</v>
+      </c>
+      <c r="J202">
+        <f t="shared" si="10"/>
+        <v>0.46799999999999986</v>
+      </c>
+      <c r="K202">
+        <f t="shared" ref="K202:K214" si="12">SUM(H202:J202)</f>
+        <v>12.224727272727272</v>
+      </c>
     </row>
     <row r="203" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="68" t="s">
@@ -9406,6 +9778,22 @@
       <c r="F203" s="69">
         <f>F204*$C$203</f>
         <v>22.463999999999999</v>
+      </c>
+      <c r="H203">
+        <f t="shared" si="11"/>
+        <v>29.452100840336133</v>
+      </c>
+      <c r="I203">
+        <f t="shared" si="10"/>
+        <v>16.570084033613444</v>
+      </c>
+      <c r="J203">
+        <f t="shared" si="10"/>
+        <v>1.9191932773109244</v>
+      </c>
+      <c r="K203">
+        <f t="shared" si="12"/>
+        <v>47.941378151260501</v>
       </c>
     </row>
     <row r="204" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
@@ -9428,6 +9816,22 @@
         <f>D238</f>
         <v>56.16</v>
       </c>
+      <c r="H204">
+        <f t="shared" si="11"/>
+        <v>79.613793103448273</v>
+      </c>
+      <c r="I204">
+        <f t="shared" si="10"/>
+        <v>38.515862068965518</v>
+      </c>
+      <c r="J204">
+        <f t="shared" si="10"/>
+        <v>4.38951724137931</v>
+      </c>
+      <c r="K204">
+        <f t="shared" si="12"/>
+        <v>122.5191724137931</v>
+      </c>
     </row>
     <row r="205" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205" s="68" t="s">
@@ -9437,20 +9841,36 @@
         <v>10</v>
       </c>
       <c r="C205" s="66">
-        <f t="shared" ref="C205:C214" si="6">EXP(LN(0.5)*B204/10)</f>
+        <f t="shared" ref="C205:C214" si="13">EXP(LN(0.5)*B204/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D205" s="70">
-        <f t="shared" ref="D205:D210" si="7">$D$204*C205</f>
+        <f t="shared" ref="D205:D210" si="14">$D$204*C205</f>
         <v>110.30865786510142</v>
       </c>
       <c r="E205" s="70">
-        <f t="shared" ref="E205:E210" si="8">$E$204*C205</f>
+        <f t="shared" ref="E205:E210" si="15">$E$204*C205</f>
         <v>66.185194719060846</v>
       </c>
       <c r="F205" s="70">
-        <f t="shared" ref="F205:F210" si="9">$F$204*C205</f>
+        <f t="shared" ref="F205:F210" si="16">$F$204*C205</f>
         <v>39.711116831436506</v>
+      </c>
+      <c r="H205">
+        <f t="shared" si="11"/>
+        <v>66.683764924100856</v>
+      </c>
+      <c r="I205">
+        <f t="shared" si="10"/>
+        <v>22.62262305369029</v>
+      </c>
+      <c r="J205">
+        <f t="shared" si="10"/>
+        <v>2.1313876265460272</v>
+      </c>
+      <c r="K205">
+        <f t="shared" si="12"/>
+        <v>91.437775604337176</v>
       </c>
       <c r="M205" s="59"/>
     </row>
@@ -9462,20 +9882,36 @@
         <v>15</v>
       </c>
       <c r="C206" s="66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
       <c r="D206" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>78</v>
       </c>
       <c r="E206" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>46.8</v>
       </c>
       <c r="F206" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>28.08</v>
+      </c>
+      <c r="H206">
+        <f t="shared" si="11"/>
+        <v>59.710344827586205</v>
+      </c>
+      <c r="I206">
+        <f t="shared" si="10"/>
+        <v>9.5213793103448268</v>
+      </c>
+      <c r="J206">
+        <f t="shared" si="10"/>
+        <v>0.87144827586206886</v>
+      </c>
+      <c r="K206">
+        <f t="shared" si="12"/>
+        <v>70.103172413793089</v>
       </c>
       <c r="N206" s="59"/>
       <c r="O206" s="59"/>
@@ -9489,20 +9925,36 @@
         <v>20</v>
       </c>
       <c r="C207" s="66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0.35355339059327379</v>
       </c>
       <c r="D207" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>55.154328932550712</v>
       </c>
       <c r="E207" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>33.092597359530423</v>
       </c>
       <c r="F207" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>19.855558415718253</v>
+      </c>
+      <c r="H207">
+        <f t="shared" si="11"/>
+        <v>45.126269126632394</v>
+      </c>
+      <c r="I207">
+        <f t="shared" si="10"/>
+        <v>5.5540023540470642</v>
+      </c>
+      <c r="J207">
+        <f t="shared" si="10"/>
+        <v>0.2777001177023532</v>
+      </c>
+      <c r="K207">
+        <f t="shared" si="12"/>
+        <v>50.95797159838181</v>
       </c>
     </row>
     <row r="208" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
@@ -9513,23 +9965,39 @@
         <v>25</v>
       </c>
       <c r="C208" s="66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0.25</v>
       </c>
       <c r="D208" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>39</v>
       </c>
       <c r="E208" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>23.4</v>
       </c>
       <c r="F208" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>14.04</v>
       </c>
-    </row>
-    <row r="209" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H208">
+        <f t="shared" si="11"/>
+        <v>33.179104477611936</v>
+      </c>
+      <c r="I208">
+        <f t="shared" si="10"/>
+        <v>3.4691373134328458</v>
+      </c>
+      <c r="J208">
+        <f t="shared" si="10"/>
+        <v>1.4039999999999999E-2</v>
+      </c>
+      <c r="K208">
+        <f t="shared" si="12"/>
+        <v>36.662281791044784</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="68" t="s">
         <v>47</v>
       </c>
@@ -9537,23 +10005,39 @@
         <v>30</v>
       </c>
       <c r="C209" s="66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0.17677669529663689</v>
       </c>
       <c r="D209" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>27.577164466275356</v>
       </c>
       <c r="E209" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>16.546298679765211</v>
       </c>
       <c r="F209" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>9.9277792078591265</v>
       </c>
-    </row>
-    <row r="210" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H209">
+        <f t="shared" si="11"/>
+        <v>23.461169769816344</v>
+      </c>
+      <c r="I209">
+        <f t="shared" si="10"/>
+        <v>2.4530505191956467</v>
+      </c>
+      <c r="J209">
+        <f t="shared" si="10"/>
+        <v>9.9277792078591269E-3</v>
+      </c>
+      <c r="K209">
+        <f t="shared" si="12"/>
+        <v>25.92414806821985</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210" s="68" t="s">
         <v>48</v>
       </c>
@@ -9561,23 +10045,39 @@
         <v>35</v>
       </c>
       <c r="C210" s="66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>0.12500000000000003</v>
       </c>
       <c r="D210" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>19.500000000000004</v>
       </c>
       <c r="E210" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>11.700000000000001</v>
       </c>
       <c r="F210" s="70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>7.0200000000000014</v>
       </c>
-    </row>
-    <row r="211" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H210">
+        <f t="shared" si="11"/>
+        <v>16.589552238805972</v>
+      </c>
+      <c r="I210">
+        <f t="shared" si="10"/>
+        <v>1.7345686567164231</v>
+      </c>
+      <c r="J210">
+        <f t="shared" si="10"/>
+        <v>7.0200000000000011E-3</v>
+      </c>
+      <c r="K210">
+        <f t="shared" si="12"/>
+        <v>18.331140895522395</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A211" s="68" t="s">
         <v>49</v>
       </c>
@@ -9600,8 +10100,24 @@
         <f>$F$204*C211</f>
         <v>4.9638896039295632</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H211">
+        <f t="shared" si="11"/>
+        <v>11.730584884908172</v>
+      </c>
+      <c r="I211">
+        <f t="shared" si="10"/>
+        <v>1.2265252595978233</v>
+      </c>
+      <c r="J211">
+        <f t="shared" si="10"/>
+        <v>4.9638896039295635E-3</v>
+      </c>
+      <c r="K211">
+        <f t="shared" si="12"/>
+        <v>12.962074034109925</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A212" s="68" t="s">
         <v>50</v>
       </c>
@@ -9609,7 +10125,7 @@
         <v>45</v>
       </c>
       <c r="C212" s="66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>6.25E-2</v>
       </c>
       <c r="D212" s="70">
@@ -9624,8 +10140,24 @@
         <f>$F$204*C212</f>
         <v>3.51</v>
       </c>
-    </row>
-    <row r="213" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H212">
+        <f t="shared" si="11"/>
+        <v>8.2947761194029841</v>
+      </c>
+      <c r="I212">
+        <f t="shared" si="10"/>
+        <v>0.86728432835821145</v>
+      </c>
+      <c r="J212">
+        <f t="shared" si="10"/>
+        <v>3.5099999999999997E-3</v>
+      </c>
+      <c r="K212">
+        <f t="shared" si="12"/>
+        <v>9.1655704477611959</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A213" s="68" t="s">
         <v>51</v>
       </c>
@@ -9633,7 +10165,7 @@
         <v>50</v>
       </c>
       <c r="C213" s="66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>4.4194173824159223E-2</v>
       </c>
       <c r="D213" s="70">
@@ -9648,8 +10180,24 @@
         <f>$F$204*C213</f>
         <v>2.4819448019647816</v>
       </c>
-    </row>
-    <row r="214" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H213">
+        <f t="shared" si="11"/>
+        <v>5.865292442454086</v>
+      </c>
+      <c r="I213">
+        <f t="shared" si="10"/>
+        <v>0.61326262979891166</v>
+      </c>
+      <c r="J213">
+        <f t="shared" si="10"/>
+        <v>2.4819448019647817E-3</v>
+      </c>
+      <c r="K213">
+        <f t="shared" si="12"/>
+        <v>6.4810370170549625</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A214" s="68" t="s">
         <v>52</v>
       </c>
@@ -9657,7 +10205,7 @@
         <v>55</v>
       </c>
       <c r="C214" s="66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>3.125E-2</v>
       </c>
       <c r="D214" s="70">
@@ -9672,39 +10220,63 @@
         <f>$F$204*C214</f>
         <v>1.7549999999999999</v>
       </c>
-    </row>
-    <row r="215" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H214">
+        <f t="shared" si="11"/>
+        <v>4.147388059701492</v>
+      </c>
+      <c r="I214">
+        <f t="shared" si="10"/>
+        <v>0.43364216417910573</v>
+      </c>
+      <c r="J214">
+        <f t="shared" si="10"/>
+        <v>1.7549999999999998E-3</v>
+      </c>
+      <c r="K214">
+        <f t="shared" si="12"/>
+        <v>4.5827852238805979</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A215" s="66"/>
       <c r="B215" s="71"/>
       <c r="C215" s="66"/>
       <c r="D215" s="73"/>
       <c r="E215" s="73"/>
       <c r="F215" s="73"/>
-    </row>
-    <row r="216" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A216" s="79" t="s">
+      <c r="K215">
+        <f>AVERAGE(K201:K214)</f>
+        <v>36.59889506656333</v>
+      </c>
+      <c r="L215">
+        <f>K215/(365.25/7)</f>
+        <v>0.7014161956630891</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A216" s="96" t="s">
         <v>95</v>
       </c>
-      <c r="B216" s="79"/>
-      <c r="C216" s="79"/>
-      <c r="D216" s="79"/>
-      <c r="E216" s="79"/>
-      <c r="F216" s="79"/>
-    </row>
-    <row r="217" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A217" s="80" t="s">
+      <c r="B216" s="96"/>
+      <c r="C216" s="96"/>
+      <c r="D216" s="96"/>
+      <c r="E216" s="96"/>
+      <c r="F216" s="96"/>
+    </row>
+    <row r="217" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A217" s="97" t="s">
         <v>2</v>
       </c>
       <c r="B217" s="66"/>
       <c r="C217" s="66"/>
-      <c r="D217" s="78" t="s">
+      <c r="D217" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="E217" s="78"/>
-      <c r="F217" s="78"/>
-    </row>
-    <row r="218" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A218" s="80"/>
+      <c r="E217" s="95"/>
+      <c r="F217" s="95"/>
+    </row>
+    <row r="218" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A218" s="97"/>
       <c r="B218" s="66"/>
       <c r="C218" s="67" t="s">
         <v>54</v>
@@ -9719,7 +10291,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A219" s="68" t="s">
         <v>31</v>
       </c>
@@ -9735,7 +10307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220" s="68" t="s">
         <v>30</v>
       </c>
@@ -9751,7 +10323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A221" s="68" t="s">
         <v>39</v>
       </c>
@@ -9772,7 +10344,7 @@
         <v>2.8079999999999998</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A222" s="68" t="s">
         <v>40</v>
       </c>
@@ -9793,7 +10365,7 @@
         <v>5.6159999999999997</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="68" t="s">
         <v>41</v>
       </c>
@@ -9816,7 +10388,7 @@
         <v>22.463999999999999</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A224" s="68" t="s">
         <v>42</v>
       </c>
@@ -9845,7 +10417,7 @@
         <v>10</v>
       </c>
       <c r="C225" s="66">
-        <f t="shared" ref="C225:C234" si="10">EXP(LN(0.5)*B224/10)</f>
+        <f t="shared" ref="C225:C234" si="17">EXP(LN(0.5)*B224/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D225" s="69">
@@ -9869,19 +10441,19 @@
         <v>15</v>
       </c>
       <c r="C226" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
       <c r="D226" s="69">
-        <f t="shared" ref="D226:D232" si="11">$D$224*C226</f>
+        <f t="shared" ref="D226:D232" si="18">$D$224*C226</f>
         <v>78</v>
       </c>
       <c r="E226" s="69">
-        <f t="shared" ref="E226:E232" si="12">$E$224*C226</f>
+        <f t="shared" ref="E226:E232" si="19">$E$224*C226</f>
         <v>46.8</v>
       </c>
       <c r="F226" s="69">
-        <f t="shared" ref="F226:F232" si="13">$F$224*C226</f>
+        <f t="shared" ref="F226:F232" si="20">$F$224*C226</f>
         <v>28.08</v>
       </c>
     </row>
@@ -9893,19 +10465,19 @@
         <v>20</v>
       </c>
       <c r="C227" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.35355339059327379</v>
       </c>
       <c r="D227" s="69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>55.154328932550712</v>
       </c>
       <c r="E227" s="69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>33.092597359530423</v>
       </c>
       <c r="F227" s="69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>19.855558415718253</v>
       </c>
     </row>
@@ -9917,19 +10489,19 @@
         <v>25</v>
       </c>
       <c r="C228" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.25</v>
       </c>
       <c r="D228" s="69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>39</v>
       </c>
       <c r="E228" s="69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>23.4</v>
       </c>
       <c r="F228" s="69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>14.04</v>
       </c>
     </row>
@@ -9941,19 +10513,19 @@
         <v>30</v>
       </c>
       <c r="C229" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.17677669529663689</v>
       </c>
       <c r="D229" s="69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>27.577164466275356</v>
       </c>
       <c r="E229" s="69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>16.546298679765211</v>
       </c>
       <c r="F229" s="69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>9.9277792078591265</v>
       </c>
     </row>
@@ -9965,19 +10537,19 @@
         <v>35</v>
       </c>
       <c r="C230" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>0.12500000000000003</v>
       </c>
       <c r="D230" s="69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>19.500000000000004</v>
       </c>
       <c r="E230" s="69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>11.700000000000001</v>
       </c>
       <c r="F230" s="69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>7.0200000000000014</v>
       </c>
     </row>
@@ -9989,19 +10561,19 @@
         <v>40</v>
       </c>
       <c r="C231" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>8.8388347648318447E-2</v>
       </c>
       <c r="D231" s="69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>13.788582233137678</v>
       </c>
       <c r="E231" s="69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>8.2731493398826057</v>
       </c>
       <c r="F231" s="69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>4.9638896039295632</v>
       </c>
     </row>
@@ -10013,19 +10585,19 @@
         <v>45</v>
       </c>
       <c r="C232" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>6.25E-2</v>
       </c>
       <c r="D232" s="69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>9.75</v>
       </c>
       <c r="E232" s="69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>5.85</v>
       </c>
       <c r="F232" s="69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>3.51</v>
       </c>
     </row>
@@ -10061,7 +10633,7 @@
         <v>55</v>
       </c>
       <c r="C234" s="66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>3.125E-2</v>
       </c>
       <c r="D234" s="69">
@@ -10147,6 +10719,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="A216:F216"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="B158:D158"/>
+    <mergeCell ref="E158:G158"/>
+    <mergeCell ref="A183:C183"/>
+    <mergeCell ref="A195:F195"/>
+    <mergeCell ref="A196:F196"/>
+    <mergeCell ref="D197:F197"/>
+    <mergeCell ref="D217:F217"/>
     <mergeCell ref="A109:A111"/>
     <mergeCell ref="B109:G109"/>
     <mergeCell ref="B130:G130"/>
@@ -10159,16 +10741,6 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="B81:B83"/>
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="A216:F216"/>
-    <mergeCell ref="A217:A218"/>
-    <mergeCell ref="B158:D158"/>
-    <mergeCell ref="E158:G158"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A195:F195"/>
-    <mergeCell ref="A196:F196"/>
-    <mergeCell ref="D197:F197"/>
-    <mergeCell ref="D217:F217"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changing baseline vaccination of 9 year-olds to vaccinate the whole age group vs. 1/5th (*0.20). This gives the correct coverage at transition to 10-14 age group, and isn't effected by prevalent HPV because 9 year-olds (group 2: 5-9) are not sexually active. Also added a script to save VCLIR results into Excel files.
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -748,7 +748,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -764,12 +764,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1337,42 +1331,42 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1387,7 +1381,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1442,24 +1436,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1469,9 +1456,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1510,13 +1494,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1562,6 +1539,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1595,9 +1599,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1613,30 +1614,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -6090,8 +6068,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6129,107 +6107,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="57"/>
-      <c r="X2" s="57"/>
-      <c r="Y2" s="57"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
     </row>
     <row r="3" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="57"/>
-      <c r="U3" s="57"/>
-      <c r="V3" s="57"/>
-      <c r="W3" s="57"/>
-      <c r="X3" s="57"/>
-      <c r="Y3" s="57"/>
-    </row>
-    <row r="4" spans="1:25" s="59" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
+    </row>
+    <row r="4" spans="1:25" s="52" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="88"/>
+      <c r="C4" s="90"/>
     </row>
     <row r="5" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="60"/>
-      <c r="B5" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="54" t="s">
+      <c r="A5" s="53"/>
+      <c r="B5" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="47" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6355,13 +6333,13 @@
       </c>
     </row>
     <row r="17" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <v>70487</v>
       </c>
-      <c r="C17" s="24">
+      <c r="C17" s="23">
         <v>82330</v>
       </c>
     </row>
@@ -6369,11 +6347,11 @@
       <c r="A18" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="96">
         <f>314094/6.27</f>
         <v>50094.736842105267</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="96">
         <f>366793/6.36</f>
         <v>57671.85534591195</v>
       </c>
@@ -6382,11 +6360,11 @@
       <c r="A19" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="96">
         <f>224490/6.27</f>
         <v>35803.827751196171</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="96">
         <f>282911/6.36</f>
         <v>44482.861635220121</v>
       </c>
@@ -6395,11 +6373,11 @@
       <c r="A20" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20" s="96">
         <f>151123/6.27</f>
         <v>24102.551834130783</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="96">
         <f>215469/6.36</f>
         <v>33878.773584905655</v>
       </c>
@@ -6408,17 +6386,17 @@
       <c r="A21" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="96">
         <f>89288/6.27</f>
         <v>14240.510366826158</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="96">
         <f>144901/6.36</f>
         <v>22783.176100628931</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="24" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="12">
@@ -6440,7 +6418,7 @@
       <c r="B23" s="9"/>
     </row>
     <row r="24" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="25" t="s">
         <v>59</v>
       </c>
       <c r="B24">
@@ -6453,23 +6431,23 @@
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F26" s="43"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="89" t="s">
+      <c r="B27" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="90"/>
+      <c r="C27" s="91"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
-      <c r="B28" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="52" t="s">
+      <c r="B28" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="45" t="s">
         <v>1</v>
       </c>
       <c r="F28" s="20"/>
@@ -6478,11 +6456,11 @@
       <c r="A29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="26">
+      <c r="B29" s="24">
         <f t="array" ref="B29:B44">-1*B6:B22</f>
         <v>-418189</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="24">
         <v>417311</v>
       </c>
     </row>
@@ -6490,10 +6468,10 @@
       <c r="A30" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="26">
+      <c r="B30" s="24">
         <v>-361938</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="24">
         <v>361594</v>
       </c>
     </row>
@@ -6501,10 +6479,10 @@
       <c r="A31" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="26">
+      <c r="B31" s="24">
         <v>-327171</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="24">
         <v>329333</v>
       </c>
       <c r="L31" s="11"/>
@@ -6513,10 +6491,10 @@
       <c r="A32" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="26">
+      <c r="B32" s="24">
         <v>-289627</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="24">
         <v>296947</v>
       </c>
     </row>
@@ -6524,10 +6502,10 @@
       <c r="A33" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="26">
+      <c r="B33" s="24">
         <v>-262704</v>
       </c>
-      <c r="C33" s="26">
+      <c r="C33" s="24">
         <v>273204</v>
       </c>
     </row>
@@ -6535,10 +6513,10 @@
       <c r="A34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="26">
+      <c r="B34" s="24">
         <v>-235673</v>
       </c>
-      <c r="C34" s="26">
+      <c r="C34" s="24">
         <v>249396</v>
       </c>
     </row>
@@ -6546,10 +6524,10 @@
       <c r="A35" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="26">
+      <c r="B35" s="24">
         <v>-197816</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="24">
         <v>211839</v>
       </c>
     </row>
@@ -6557,10 +6535,10 @@
       <c r="A36" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="26">
+      <c r="B36" s="24">
         <v>-160952</v>
       </c>
-      <c r="C36" s="26">
+      <c r="C36" s="24">
         <v>176470</v>
       </c>
       <c r="X36" s="17"/>
@@ -6577,10 +6555,10 @@
       <c r="A37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="26">
+      <c r="B37" s="24">
         <v>-132311</v>
       </c>
-      <c r="C37" s="26">
+      <c r="C37" s="24">
         <v>143351</v>
       </c>
       <c r="X37" s="18"/>
@@ -6596,310 +6574,310 @@
       <c r="A38" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="26">
+      <c r="B38" s="24">
         <v>-110849</v>
       </c>
-      <c r="C38" s="26">
+      <c r="C38" s="24">
         <v>123441</v>
       </c>
-      <c r="X38" s="34"/>
-      <c r="Y38" s="34"/>
-      <c r="Z38" s="34"/>
-      <c r="AA38" s="34"/>
-      <c r="AB38" s="34"/>
-      <c r="AC38" s="34"/>
-      <c r="AD38" s="34"/>
-      <c r="AE38" s="34"/>
+      <c r="X38" s="30"/>
+      <c r="Y38" s="30"/>
+      <c r="Z38" s="30"/>
+      <c r="AA38" s="30"/>
+      <c r="AB38" s="30"/>
+      <c r="AC38" s="30"/>
+      <c r="AD38" s="30"/>
+      <c r="AE38" s="30"/>
     </row>
     <row r="39" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="26">
+      <c r="B39" s="24">
         <v>-89027</v>
       </c>
-      <c r="C39" s="26">
+      <c r="C39" s="24">
         <v>98355</v>
       </c>
-      <c r="X39" s="35"/>
-      <c r="Y39" s="35"/>
-      <c r="Z39" s="35"/>
-      <c r="AA39" s="35"/>
-      <c r="AB39" s="35"/>
-      <c r="AC39" s="35"/>
-      <c r="AD39" s="35"/>
-      <c r="AE39" s="35"/>
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="31"/>
+      <c r="AC39" s="31"/>
+      <c r="AD39" s="31"/>
+      <c r="AE39" s="31"/>
     </row>
     <row r="40" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="26">
+      <c r="B40" s="24">
         <v>-70487</v>
       </c>
-      <c r="C40" s="26">
+      <c r="C40" s="24">
         <v>82330</v>
       </c>
-      <c r="X40" s="35"/>
-      <c r="Y40" s="35"/>
-      <c r="Z40" s="35"/>
-      <c r="AA40" s="35"/>
-      <c r="AB40" s="35"/>
-      <c r="AC40" s="35"/>
-      <c r="AD40" s="35"/>
-      <c r="AE40" s="35"/>
+      <c r="X40" s="31"/>
+      <c r="Y40" s="31"/>
+      <c r="Z40" s="31"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="31"/>
+      <c r="AC40" s="31"/>
+      <c r="AD40" s="31"/>
+      <c r="AE40" s="31"/>
     </row>
     <row r="41" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="61">
+      <c r="B41" s="54">
         <v>-50094.736842105267</v>
       </c>
-      <c r="C41" s="61">
+      <c r="C41" s="54">
         <f>366793/6.36</f>
         <v>57671.85534591195</v>
       </c>
-      <c r="X41" s="35"/>
-      <c r="Y41" s="35"/>
-      <c r="Z41" s="35"/>
-      <c r="AA41" s="35"/>
-      <c r="AB41" s="35"/>
-      <c r="AC41" s="35"/>
-      <c r="AD41" s="35"/>
-      <c r="AE41" s="35"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
     </row>
     <row r="42" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="61">
+      <c r="B42" s="54">
         <v>-35803.827751196171</v>
       </c>
-      <c r="C42" s="61">
+      <c r="C42" s="54">
         <f>282911/6.36</f>
         <v>44482.861635220121</v>
       </c>
-      <c r="X42" s="36"/>
-      <c r="Y42" s="36"/>
-      <c r="Z42" s="36"/>
-      <c r="AA42" s="36"/>
-      <c r="AB42" s="36"/>
-      <c r="AC42" s="36"/>
-      <c r="AD42" s="36"/>
-      <c r="AE42" s="36"/>
+      <c r="X42" s="32"/>
+      <c r="Y42" s="32"/>
+      <c r="Z42" s="32"/>
+      <c r="AA42" s="32"/>
+      <c r="AB42" s="32"/>
+      <c r="AC42" s="32"/>
+      <c r="AD42" s="32"/>
+      <c r="AE42" s="32"/>
     </row>
     <row r="43" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="61">
+      <c r="B43" s="54">
         <v>-24102.551834130783</v>
       </c>
-      <c r="C43" s="61">
+      <c r="C43" s="54">
         <f>215469/6.36</f>
         <v>33878.773584905655</v>
       </c>
-      <c r="X43" s="36"/>
-      <c r="Y43" s="36"/>
-      <c r="Z43" s="36"/>
-      <c r="AA43" s="36"/>
-      <c r="AB43" s="36"/>
-      <c r="AC43" s="36"/>
-      <c r="AD43" s="36"/>
-      <c r="AE43" s="36"/>
+      <c r="X43" s="32"/>
+      <c r="Y43" s="32"/>
+      <c r="Z43" s="32"/>
+      <c r="AA43" s="32"/>
+      <c r="AB43" s="32"/>
+      <c r="AC43" s="32"/>
+      <c r="AD43" s="32"/>
+      <c r="AE43" s="32"/>
     </row>
     <row r="44" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="61">
+      <c r="B44" s="54">
         <v>-14240.510366826158</v>
       </c>
-      <c r="C44" s="61">
+      <c r="C44" s="54">
         <f>144901/6.36</f>
         <v>22783.176100628931</v>
       </c>
-      <c r="X44" s="36"/>
-      <c r="Y44" s="36"/>
-      <c r="Z44" s="36"/>
-      <c r="AA44" s="36"/>
-      <c r="AB44" s="36"/>
-      <c r="AC44" s="36"/>
-      <c r="AD44" s="36"/>
-      <c r="AE44" s="36"/>
+      <c r="X44" s="32"/>
+      <c r="Y44" s="32"/>
+      <c r="Z44" s="32"/>
+      <c r="AA44" s="32"/>
+      <c r="AB44" s="32"/>
+      <c r="AC44" s="32"/>
+      <c r="AD44" s="32"/>
+      <c r="AE44" s="32"/>
     </row>
     <row r="45" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="X45" s="36"/>
-      <c r="Y45" s="36"/>
-      <c r="Z45" s="36"/>
-      <c r="AA45" s="36"/>
-      <c r="AB45" s="36"/>
-      <c r="AC45" s="36"/>
-      <c r="AD45" s="36"/>
-      <c r="AE45" s="36"/>
+      <c r="X45" s="32"/>
+      <c r="Y45" s="32"/>
+      <c r="Z45" s="32"/>
+      <c r="AA45" s="32"/>
+      <c r="AB45" s="32"/>
+      <c r="AC45" s="32"/>
+      <c r="AD45" s="32"/>
+      <c r="AE45" s="32"/>
     </row>
     <row r="46" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="X46" s="36"/>
-      <c r="Y46" s="36"/>
-      <c r="Z46" s="36"/>
-      <c r="AA46" s="36"/>
-      <c r="AB46" s="36"/>
-      <c r="AC46" s="36"/>
-      <c r="AD46" s="36"/>
-      <c r="AE46" s="36"/>
+      <c r="X46" s="32"/>
+      <c r="Y46" s="32"/>
+      <c r="Z46" s="32"/>
+      <c r="AA46" s="32"/>
+      <c r="AB46" s="32"/>
+      <c r="AC46" s="32"/>
+      <c r="AD46" s="32"/>
+      <c r="AE46" s="32"/>
     </row>
     <row r="47" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="X47" s="36"/>
-      <c r="Y47" s="36"/>
-      <c r="Z47" s="36"/>
-      <c r="AA47" s="36"/>
-      <c r="AB47" s="36"/>
-      <c r="AC47" s="36"/>
-      <c r="AD47" s="36"/>
-      <c r="AE47" s="36"/>
+      <c r="X47" s="32"/>
+      <c r="Y47" s="32"/>
+      <c r="Z47" s="32"/>
+      <c r="AA47" s="32"/>
+      <c r="AB47" s="32"/>
+      <c r="AC47" s="32"/>
+      <c r="AD47" s="32"/>
+      <c r="AE47" s="32"/>
     </row>
     <row r="48" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="X48" s="36"/>
-      <c r="Y48" s="36"/>
-      <c r="Z48" s="36"/>
-      <c r="AA48" s="36"/>
-      <c r="AB48" s="36"/>
-      <c r="AC48" s="36"/>
-      <c r="AD48" s="36"/>
-      <c r="AE48" s="36"/>
+      <c r="X48" s="32"/>
+      <c r="Y48" s="32"/>
+      <c r="Z48" s="32"/>
+      <c r="AA48" s="32"/>
+      <c r="AB48" s="32"/>
+      <c r="AC48" s="32"/>
+      <c r="AD48" s="32"/>
+      <c r="AE48" s="32"/>
     </row>
     <row r="49" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="X49" s="36"/>
-      <c r="Y49" s="36"/>
-      <c r="Z49" s="36"/>
-      <c r="AA49" s="36"/>
-      <c r="AB49" s="36"/>
-      <c r="AC49" s="36"/>
-      <c r="AD49" s="36"/>
-      <c r="AE49" s="36"/>
+      <c r="X49" s="32"/>
+      <c r="Y49" s="32"/>
+      <c r="Z49" s="32"/>
+      <c r="AA49" s="32"/>
+      <c r="AB49" s="32"/>
+      <c r="AC49" s="32"/>
+      <c r="AD49" s="32"/>
+      <c r="AE49" s="32"/>
     </row>
     <row r="50" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="56" t="s">
+      <c r="A50" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="57"/>
-      <c r="C50" s="57"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
-      <c r="L50" s="57"/>
-      <c r="M50" s="57"/>
-      <c r="N50" s="57"/>
-      <c r="O50" s="57"/>
-      <c r="P50" s="57"/>
-      <c r="Q50" s="57"/>
-      <c r="R50" s="57"/>
-      <c r="S50" s="57"/>
-      <c r="T50" s="57"/>
-      <c r="U50" s="57"/>
-      <c r="V50" s="57"/>
-      <c r="W50" s="57"/>
-      <c r="X50" s="36"/>
-      <c r="Y50" s="36"/>
-      <c r="Z50" s="36"/>
-      <c r="AA50" s="36"/>
-      <c r="AB50" s="36"/>
-      <c r="AC50" s="36"/>
-      <c r="AD50" s="36"/>
-      <c r="AE50" s="36"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="50"/>
+      <c r="J50" s="50"/>
+      <c r="K50" s="50"/>
+      <c r="L50" s="50"/>
+      <c r="M50" s="50"/>
+      <c r="N50" s="50"/>
+      <c r="O50" s="50"/>
+      <c r="P50" s="50"/>
+      <c r="Q50" s="50"/>
+      <c r="R50" s="50"/>
+      <c r="S50" s="50"/>
+      <c r="T50" s="50"/>
+      <c r="U50" s="50"/>
+      <c r="V50" s="50"/>
+      <c r="W50" s="50"/>
+      <c r="X50" s="32"/>
+      <c r="Y50" s="32"/>
+      <c r="Z50" s="32"/>
+      <c r="AA50" s="32"/>
+      <c r="AB50" s="32"/>
+      <c r="AC50" s="32"/>
+      <c r="AD50" s="32"/>
+      <c r="AE50" s="32"/>
     </row>
     <row r="51" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="58" t="s">
+      <c r="A51" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="57"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
-      <c r="J51" s="57"/>
-      <c r="K51" s="57"/>
-      <c r="L51" s="57"/>
-      <c r="M51" s="57"/>
-      <c r="N51" s="57"/>
-      <c r="O51" s="57"/>
-      <c r="P51" s="57"/>
-      <c r="Q51" s="57"/>
-      <c r="R51" s="57"/>
-      <c r="S51" s="57"/>
-      <c r="T51" s="57"/>
-      <c r="U51" s="57"/>
-      <c r="V51" s="57"/>
-      <c r="W51" s="57"/>
-      <c r="X51" s="36"/>
-      <c r="Y51" s="36"/>
-      <c r="Z51" s="36"/>
-      <c r="AA51" s="36"/>
-      <c r="AB51" s="36"/>
-      <c r="AC51" s="36"/>
-      <c r="AD51" s="36"/>
-      <c r="AE51" s="36"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="50"/>
+      <c r="M51" s="50"/>
+      <c r="N51" s="50"/>
+      <c r="O51" s="50"/>
+      <c r="P51" s="50"/>
+      <c r="Q51" s="50"/>
+      <c r="R51" s="50"/>
+      <c r="S51" s="50"/>
+      <c r="T51" s="50"/>
+      <c r="U51" s="50"/>
+      <c r="V51" s="50"/>
+      <c r="W51" s="50"/>
+      <c r="X51" s="32"/>
+      <c r="Y51" s="32"/>
+      <c r="Z51" s="32"/>
+      <c r="AA51" s="32"/>
+      <c r="AB51" s="32"/>
+      <c r="AC51" s="32"/>
+      <c r="AD51" s="32"/>
+      <c r="AE51" s="32"/>
     </row>
     <row r="52" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="94" t="s">
+      <c r="A52" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="94" t="s">
+      <c r="B52" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="94"/>
-      <c r="D52" s="94"/>
-      <c r="E52" s="94" t="s">
+      <c r="C52" s="95"/>
+      <c r="D52" s="95"/>
+      <c r="E52" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="94"/>
-      <c r="G52" s="94"/>
-      <c r="X52" s="34"/>
-      <c r="Y52" s="34"/>
-      <c r="Z52" s="34"/>
-      <c r="AA52" s="34"/>
-      <c r="AB52" s="34"/>
-      <c r="AC52" s="34"/>
-      <c r="AD52" s="34"/>
-      <c r="AE52" s="34"/>
+      <c r="F52" s="95"/>
+      <c r="G52" s="95"/>
+      <c r="X52" s="30"/>
+      <c r="Y52" s="30"/>
+      <c r="Z52" s="30"/>
+      <c r="AA52" s="30"/>
+      <c r="AB52" s="30"/>
+      <c r="AC52" s="30"/>
+      <c r="AD52" s="30"/>
+      <c r="AE52" s="30"/>
     </row>
     <row r="53" spans="1:31" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="94"/>
-      <c r="B53" s="52" t="s">
+      <c r="A53" s="95"/>
+      <c r="B53" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="52" t="s">
+      <c r="C53" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D53" s="52" t="s">
+      <c r="D53" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="52" t="s">
+      <c r="E53" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F53" s="52" t="s">
+      <c r="F53" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="G53" s="52" t="s">
+      <c r="G53" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="X53" s="32"/>
-      <c r="Y53" s="32"/>
-      <c r="Z53" s="31"/>
-      <c r="AA53" s="37"/>
-      <c r="AB53" s="37"/>
-      <c r="AC53" s="37"/>
-      <c r="AD53" s="37"/>
-      <c r="AE53" s="37"/>
+      <c r="X53" s="29"/>
+      <c r="Y53" s="29"/>
+      <c r="Z53" s="28"/>
+      <c r="AA53" s="33"/>
+      <c r="AB53" s="33"/>
+      <c r="AC53" s="33"/>
+      <c r="AD53" s="33"/>
+      <c r="AE53" s="33"/>
     </row>
     <row r="54" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
@@ -7192,23 +7170,23 @@
       <c r="A66" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B66" s="22">
+      <c r="B66" s="27">
         <v>0.85074626865671632</v>
       </c>
-      <c r="C66" s="22">
+      <c r="C66" s="27">
         <f t="shared" si="1"/>
         <v>0.14825373134328401</v>
       </c>
-      <c r="D66" s="22">
+      <c r="D66" s="27">
         <v>1E-3</v>
       </c>
-      <c r="E66" s="22">
+      <c r="E66" s="27">
         <v>0.99568965517241381</v>
       </c>
-      <c r="F66" s="22">
+      <c r="F66" s="27">
         <v>2.8735632183908046E-3</v>
       </c>
-      <c r="G66" s="22">
+      <c r="G66" s="27">
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
@@ -7216,23 +7194,23 @@
       <c r="A67" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B67" s="22">
+      <c r="B67" s="27">
         <v>0.85074626865671632</v>
       </c>
-      <c r="C67" s="22">
+      <c r="C67" s="27">
         <f t="shared" si="1"/>
         <v>0.14825373134328401</v>
       </c>
-      <c r="D67" s="22">
+      <c r="D67" s="27">
         <v>1E-3</v>
       </c>
-      <c r="E67" s="22">
+      <c r="E67" s="27">
         <v>0.99568965517241381</v>
       </c>
-      <c r="F67" s="22">
+      <c r="F67" s="27">
         <v>2.8735632183908046E-3</v>
       </c>
-      <c r="G67" s="22">
+      <c r="G67" s="27">
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
@@ -7240,23 +7218,23 @@
       <c r="A68" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B68" s="22">
+      <c r="B68" s="27">
         <v>0.85074626865671632</v>
       </c>
-      <c r="C68" s="22">
+      <c r="C68" s="27">
         <f t="shared" si="1"/>
         <v>0.14825373134328401</v>
       </c>
-      <c r="D68" s="22">
+      <c r="D68" s="27">
         <v>1E-3</v>
       </c>
-      <c r="E68" s="22">
+      <c r="E68" s="27">
         <v>0.99568965517241381</v>
       </c>
-      <c r="F68" s="22">
+      <c r="F68" s="27">
         <v>2.8735632183908046E-3</v>
       </c>
-      <c r="G68" s="22">
+      <c r="G68" s="27">
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
@@ -7264,28 +7242,28 @@
       <c r="A69" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B69" s="22">
+      <c r="B69" s="27">
         <v>0.85074626865671632</v>
       </c>
-      <c r="C69" s="22">
+      <c r="C69" s="27">
         <f t="shared" si="1"/>
         <v>0.14825373134328401</v>
       </c>
-      <c r="D69" s="22">
+      <c r="D69" s="27">
         <v>1E-3</v>
       </c>
-      <c r="E69" s="22">
+      <c r="E69" s="27">
         <v>0.99568965517241381</v>
       </c>
-      <c r="F69" s="22">
+      <c r="F69" s="27">
         <v>2.8735632183908046E-3</v>
       </c>
-      <c r="G69" s="22">
+      <c r="G69" s="27">
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A71" s="43" t="s">
+      <c r="A71" s="39" t="s">
         <v>60</v>
       </c>
       <c r="B71">
@@ -7314,7 +7292,7 @@
       </c>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A72" s="43" t="s">
+      <c r="A72" s="39" t="s">
         <v>61</v>
       </c>
       <c r="B72">
@@ -7323,109 +7301,109 @@
       </c>
     </row>
     <row r="78" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="56" t="s">
+      <c r="A78" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="B78" s="57"/>
-      <c r="C78" s="57"/>
-      <c r="D78" s="57"/>
-      <c r="E78" s="57"/>
-      <c r="F78" s="57"/>
-      <c r="G78" s="57"/>
-      <c r="H78" s="57"/>
-      <c r="I78" s="57"/>
-      <c r="J78" s="57"/>
-      <c r="K78" s="57"/>
-      <c r="L78" s="57"/>
-      <c r="M78" s="57"/>
-      <c r="N78" s="57"/>
-      <c r="O78" s="57"/>
-      <c r="P78" s="57"/>
-      <c r="Q78" s="57"/>
-      <c r="R78" s="57"/>
-      <c r="S78" s="57"/>
-      <c r="T78" s="57"/>
-      <c r="U78" s="57"/>
-      <c r="V78" s="57"/>
-      <c r="W78" s="57"/>
-      <c r="X78" s="57"/>
+      <c r="B78" s="50"/>
+      <c r="C78" s="50"/>
+      <c r="D78" s="50"/>
+      <c r="E78" s="50"/>
+      <c r="F78" s="50"/>
+      <c r="G78" s="50"/>
+      <c r="H78" s="50"/>
+      <c r="I78" s="50"/>
+      <c r="J78" s="50"/>
+      <c r="K78" s="50"/>
+      <c r="L78" s="50"/>
+      <c r="M78" s="50"/>
+      <c r="N78" s="50"/>
+      <c r="O78" s="50"/>
+      <c r="P78" s="50"/>
+      <c r="Q78" s="50"/>
+      <c r="R78" s="50"/>
+      <c r="S78" s="50"/>
+      <c r="T78" s="50"/>
+      <c r="U78" s="50"/>
+      <c r="V78" s="50"/>
+      <c r="W78" s="50"/>
+      <c r="X78" s="50"/>
     </row>
     <row r="79" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="58" t="s">
+      <c r="A79" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="B79" s="57"/>
-      <c r="C79" s="57"/>
-      <c r="D79" s="57"/>
-      <c r="E79" s="57"/>
-      <c r="F79" s="57"/>
-      <c r="G79" s="57"/>
-      <c r="H79" s="57"/>
-      <c r="I79" s="57"/>
-      <c r="J79" s="57"/>
-      <c r="K79" s="57"/>
-      <c r="L79" s="57"/>
-      <c r="M79" s="57"/>
-      <c r="N79" s="57"/>
-      <c r="O79" s="57"/>
-      <c r="P79" s="57"/>
-      <c r="Q79" s="57"/>
-      <c r="R79" s="57"/>
-      <c r="S79" s="57"/>
-      <c r="T79" s="57"/>
-      <c r="U79" s="57"/>
-      <c r="V79" s="57"/>
-      <c r="W79" s="57"/>
-      <c r="X79" s="57"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="50"/>
+      <c r="D79" s="50"/>
+      <c r="E79" s="50"/>
+      <c r="F79" s="50"/>
+      <c r="G79" s="50"/>
+      <c r="H79" s="50"/>
+      <c r="I79" s="50"/>
+      <c r="J79" s="50"/>
+      <c r="K79" s="50"/>
+      <c r="L79" s="50"/>
+      <c r="M79" s="50"/>
+      <c r="N79" s="50"/>
+      <c r="O79" s="50"/>
+      <c r="P79" s="50"/>
+      <c r="Q79" s="50"/>
+      <c r="R79" s="50"/>
+      <c r="S79" s="50"/>
+      <c r="T79" s="50"/>
+      <c r="U79" s="50"/>
+      <c r="V79" s="50"/>
+      <c r="W79" s="50"/>
+      <c r="X79" s="50"/>
     </row>
     <row r="80" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="58" t="s">
+      <c r="A80" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="B80" s="57"/>
-      <c r="C80" s="57"/>
-      <c r="D80" s="57"/>
-      <c r="E80" s="57"/>
-      <c r="F80" s="57"/>
-      <c r="G80" s="57"/>
-      <c r="H80" s="57"/>
-      <c r="I80" s="57"/>
-      <c r="J80" s="57"/>
-      <c r="K80" s="57"/>
-      <c r="L80" s="57"/>
-      <c r="M80" s="57"/>
-      <c r="N80" s="57"/>
-      <c r="O80" s="57"/>
-      <c r="P80" s="57"/>
-      <c r="Q80" s="57"/>
-      <c r="R80" s="57"/>
-      <c r="S80" s="57"/>
-      <c r="T80" s="57"/>
-      <c r="U80" s="57"/>
-      <c r="V80" s="57"/>
-      <c r="W80" s="57"/>
-      <c r="X80" s="57"/>
+      <c r="B80" s="50"/>
+      <c r="C80" s="50"/>
+      <c r="D80" s="50"/>
+      <c r="E80" s="50"/>
+      <c r="F80" s="50"/>
+      <c r="G80" s="50"/>
+      <c r="H80" s="50"/>
+      <c r="I80" s="50"/>
+      <c r="J80" s="50"/>
+      <c r="K80" s="50"/>
+      <c r="L80" s="50"/>
+      <c r="M80" s="50"/>
+      <c r="N80" s="50"/>
+      <c r="O80" s="50"/>
+      <c r="P80" s="50"/>
+      <c r="Q80" s="50"/>
+      <c r="R80" s="50"/>
+      <c r="S80" s="50"/>
+      <c r="T80" s="50"/>
+      <c r="U80" s="50"/>
+      <c r="V80" s="50"/>
+      <c r="W80" s="50"/>
+      <c r="X80" s="50"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="78" t="s">
+      <c r="A81" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="91" t="s">
+      <c r="B81" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="91" t="s">
+      <c r="C81" s="92" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="79"/>
-      <c r="B82" s="92"/>
-      <c r="C82" s="92"/>
+      <c r="A82" s="81"/>
+      <c r="B82" s="93"/>
+      <c r="C82" s="93"/>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="80"/>
-      <c r="B83" s="93"/>
-      <c r="C83" s="93"/>
+      <c r="A83" s="82"/>
+      <c r="B83" s="94"/>
+      <c r="C83" s="94"/>
     </row>
     <row r="84" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
@@ -7563,10 +7541,10 @@
       <c r="A96" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B96" s="28">
+      <c r="B96" s="13">
         <v>2.6650488106048104E-2</v>
       </c>
-      <c r="C96" s="28">
+      <c r="C96" s="13">
         <v>1.5759592316689931E-2</v>
       </c>
     </row>
@@ -7574,10 +7552,10 @@
       <c r="A97" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B97" s="28">
+      <c r="B97" s="13">
         <v>3.6763608595780588E-2</v>
       </c>
-      <c r="C97" s="28">
+      <c r="C97" s="13">
         <v>2.2837523063216215E-2</v>
       </c>
     </row>
@@ -7585,10 +7563,10 @@
       <c r="A98" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B98" s="28">
+      <c r="B98" s="13">
         <v>5.1790400883394136E-2</v>
       </c>
-      <c r="C98" s="28">
+      <c r="C98" s="13">
         <v>3.3336893194863555E-2</v>
       </c>
     </row>
@@ -7596,147 +7574,147 @@
       <c r="A99" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B99" s="28">
+      <c r="B99" s="13">
         <v>8.3577387695122712E-2</v>
       </c>
-      <c r="C99" s="28">
+      <c r="C99" s="13">
         <v>6.1722846856347699E-2</v>
       </c>
     </row>
     <row r="105" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A105" s="56" t="s">
+      <c r="A105" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="B105" s="57"/>
-      <c r="C105" s="57"/>
-      <c r="D105" s="57"/>
-      <c r="E105" s="57"/>
-      <c r="F105" s="57"/>
-      <c r="G105" s="57"/>
-      <c r="H105" s="57"/>
-      <c r="I105" s="57"/>
-      <c r="J105" s="57"/>
-      <c r="K105" s="57"/>
-      <c r="L105" s="57"/>
-      <c r="M105" s="57"/>
-      <c r="N105" s="57"/>
-      <c r="O105" s="57"/>
-      <c r="P105" s="57"/>
-      <c r="Q105" s="57"/>
-      <c r="R105" s="57"/>
-      <c r="S105" s="57"/>
-      <c r="T105" s="57"/>
-      <c r="U105" s="57"/>
-      <c r="V105" s="57"/>
-      <c r="W105" s="57"/>
-      <c r="X105" s="57"/>
+      <c r="B105" s="50"/>
+      <c r="C105" s="50"/>
+      <c r="D105" s="50"/>
+      <c r="E105" s="50"/>
+      <c r="F105" s="50"/>
+      <c r="G105" s="50"/>
+      <c r="H105" s="50"/>
+      <c r="I105" s="50"/>
+      <c r="J105" s="50"/>
+      <c r="K105" s="50"/>
+      <c r="L105" s="50"/>
+      <c r="M105" s="50"/>
+      <c r="N105" s="50"/>
+      <c r="O105" s="50"/>
+      <c r="P105" s="50"/>
+      <c r="Q105" s="50"/>
+      <c r="R105" s="50"/>
+      <c r="S105" s="50"/>
+      <c r="T105" s="50"/>
+      <c r="U105" s="50"/>
+      <c r="V105" s="50"/>
+      <c r="W105" s="50"/>
+      <c r="X105" s="50"/>
     </row>
     <row r="106" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="58" t="s">
+      <c r="A106" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="B106" s="57"/>
-      <c r="C106" s="57"/>
-      <c r="D106" s="57"/>
-      <c r="E106" s="57"/>
-      <c r="F106" s="57"/>
-      <c r="G106" s="57"/>
-      <c r="H106" s="57"/>
-      <c r="I106" s="57"/>
-      <c r="J106" s="57"/>
-      <c r="K106" s="57"/>
-      <c r="L106" s="57"/>
-      <c r="M106" s="57"/>
-      <c r="N106" s="57"/>
-      <c r="O106" s="57"/>
-      <c r="P106" s="57"/>
-      <c r="Q106" s="57"/>
-      <c r="R106" s="57"/>
-      <c r="S106" s="57"/>
-      <c r="T106" s="57"/>
-      <c r="U106" s="57"/>
-      <c r="V106" s="57"/>
-      <c r="W106" s="57"/>
-      <c r="X106" s="57"/>
+      <c r="B106" s="50"/>
+      <c r="C106" s="50"/>
+      <c r="D106" s="50"/>
+      <c r="E106" s="50"/>
+      <c r="F106" s="50"/>
+      <c r="G106" s="50"/>
+      <c r="H106" s="50"/>
+      <c r="I106" s="50"/>
+      <c r="J106" s="50"/>
+      <c r="K106" s="50"/>
+      <c r="L106" s="50"/>
+      <c r="M106" s="50"/>
+      <c r="N106" s="50"/>
+      <c r="O106" s="50"/>
+      <c r="P106" s="50"/>
+      <c r="Q106" s="50"/>
+      <c r="R106" s="50"/>
+      <c r="S106" s="50"/>
+      <c r="T106" s="50"/>
+      <c r="U106" s="50"/>
+      <c r="V106" s="50"/>
+      <c r="W106" s="50"/>
+      <c r="X106" s="50"/>
     </row>
     <row r="107" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A107" s="58" t="s">
+      <c r="A107" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="B107" s="57"/>
-      <c r="C107" s="57"/>
-      <c r="D107" s="57"/>
-      <c r="E107" s="57"/>
-      <c r="F107" s="57"/>
-      <c r="G107" s="57"/>
-      <c r="H107" s="57"/>
-      <c r="I107" s="57"/>
-      <c r="J107" s="57"/>
-      <c r="K107" s="57"/>
-      <c r="L107" s="57"/>
-      <c r="M107" s="57"/>
-      <c r="N107" s="57"/>
-      <c r="O107" s="57"/>
-      <c r="P107" s="57"/>
-      <c r="Q107" s="57"/>
-      <c r="R107" s="57"/>
-      <c r="S107" s="57"/>
-      <c r="T107" s="57"/>
-      <c r="U107" s="57"/>
-      <c r="V107" s="57"/>
-      <c r="W107" s="57"/>
-      <c r="X107" s="57"/>
+      <c r="B107" s="50"/>
+      <c r="C107" s="50"/>
+      <c r="D107" s="50"/>
+      <c r="E107" s="50"/>
+      <c r="F107" s="50"/>
+      <c r="G107" s="50"/>
+      <c r="H107" s="50"/>
+      <c r="I107" s="50"/>
+      <c r="J107" s="50"/>
+      <c r="K107" s="50"/>
+      <c r="L107" s="50"/>
+      <c r="M107" s="50"/>
+      <c r="N107" s="50"/>
+      <c r="O107" s="50"/>
+      <c r="P107" s="50"/>
+      <c r="Q107" s="50"/>
+      <c r="R107" s="50"/>
+      <c r="S107" s="50"/>
+      <c r="T107" s="50"/>
+      <c r="U107" s="50"/>
+      <c r="V107" s="50"/>
+      <c r="W107" s="50"/>
+      <c r="X107" s="50"/>
     </row>
     <row r="108" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="56" t="s">
+      <c r="A108" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="B108" s="57"/>
-      <c r="C108" s="57"/>
-      <c r="D108" s="57"/>
-      <c r="E108" s="57"/>
-      <c r="F108" s="57"/>
-      <c r="G108" s="57"/>
-      <c r="H108" s="57"/>
-      <c r="I108" s="57"/>
-      <c r="J108" s="57"/>
-      <c r="K108" s="57"/>
-      <c r="L108" s="57"/>
-      <c r="M108" s="57"/>
-      <c r="N108" s="57"/>
-      <c r="O108" s="57"/>
-      <c r="P108" s="57"/>
-      <c r="Q108" s="57"/>
-      <c r="R108" s="57"/>
-      <c r="S108" s="57"/>
-      <c r="T108" s="57"/>
-      <c r="U108" s="57"/>
-      <c r="V108" s="57"/>
-      <c r="W108" s="57"/>
-      <c r="X108" s="57"/>
+      <c r="B108" s="50"/>
+      <c r="C108" s="50"/>
+      <c r="D108" s="50"/>
+      <c r="E108" s="50"/>
+      <c r="F108" s="50"/>
+      <c r="G108" s="50"/>
+      <c r="H108" s="50"/>
+      <c r="I108" s="50"/>
+      <c r="J108" s="50"/>
+      <c r="K108" s="50"/>
+      <c r="L108" s="50"/>
+      <c r="M108" s="50"/>
+      <c r="N108" s="50"/>
+      <c r="O108" s="50"/>
+      <c r="P108" s="50"/>
+      <c r="Q108" s="50"/>
+      <c r="R108" s="50"/>
+      <c r="S108" s="50"/>
+      <c r="T108" s="50"/>
+      <c r="U108" s="50"/>
+      <c r="V108" s="50"/>
+      <c r="W108" s="50"/>
+      <c r="X108" s="50"/>
     </row>
     <row r="109" spans="1:24" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="78" t="s">
+      <c r="A109" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B109" s="81" t="s">
+      <c r="B109" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="C109" s="82"/>
-      <c r="D109" s="82"/>
-      <c r="E109" s="82"/>
-      <c r="F109" s="82"/>
-      <c r="G109" s="83"/>
+      <c r="C109" s="84"/>
+      <c r="D109" s="84"/>
+      <c r="E109" s="84"/>
+      <c r="F109" s="84"/>
+      <c r="G109" s="85"/>
     </row>
     <row r="110" spans="1:24" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="79"/>
-      <c r="B110" s="51" t="s">
+      <c r="A110" s="81"/>
+      <c r="B110" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="C110" s="51" t="s">
+      <c r="C110" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="D110" s="51" t="s">
+      <c r="D110" s="44" t="s">
         <v>79</v>
       </c>
       <c r="E110" s="5" t="s">
@@ -7750,14 +7728,14 @@
       </c>
     </row>
     <row r="111" spans="1:24" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="80"/>
-      <c r="B111" s="53" t="s">
+      <c r="A111" s="82"/>
+      <c r="B111" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="C111" s="53" t="s">
+      <c r="C111" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="D111" s="53" t="s">
+      <c r="D111" s="46" t="s">
         <v>80</v>
       </c>
       <c r="E111" s="7" t="s">
@@ -7766,7 +7744,7 @@
       <c r="F111" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G111" s="53" t="s">
+      <c r="G111" s="46" t="s">
         <v>82</v>
       </c>
     </row>
@@ -7838,7 +7816,7 @@
       <c r="G114" s="13">
         <v>0</v>
       </c>
-      <c r="I114" s="75"/>
+      <c r="I114" s="68"/>
       <c r="J114" s="18" t="s">
         <v>33</v>
       </c>
@@ -7880,23 +7858,23 @@
       <c r="I115" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J115" s="74">
+      <c r="J115" s="67">
         <f>C115/$B$115</f>
         <v>1</v>
       </c>
-      <c r="K115" s="74">
+      <c r="K115" s="67">
         <f>D115/$B$115</f>
         <v>1</v>
       </c>
-      <c r="L115" s="74">
+      <c r="L115" s="67">
         <f>E115/$B$115</f>
         <v>0.58000000000000007</v>
       </c>
-      <c r="M115" s="74">
+      <c r="M115" s="67">
         <f>F115/$B$115</f>
         <v>0.58000000000000007</v>
       </c>
-      <c r="N115" s="74">
+      <c r="N115" s="67">
         <f>G115/$B$115</f>
         <v>0.41000000000000003</v>
       </c>
@@ -8089,22 +8067,22 @@
       <c r="A124" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B124" s="28">
-        <v>0</v>
-      </c>
-      <c r="C124" s="28">
-        <v>0</v>
-      </c>
-      <c r="D124" s="28">
-        <v>0</v>
-      </c>
-      <c r="E124" s="28">
-        <v>0</v>
-      </c>
-      <c r="F124" s="28">
-        <v>0</v>
-      </c>
-      <c r="G124" s="28">
+      <c r="B124" s="13">
+        <v>0</v>
+      </c>
+      <c r="C124" s="13">
+        <v>0</v>
+      </c>
+      <c r="D124" s="13">
+        <v>0</v>
+      </c>
+      <c r="E124" s="13">
+        <v>0</v>
+      </c>
+      <c r="F124" s="13">
+        <v>0</v>
+      </c>
+      <c r="G124" s="13">
         <v>0</v>
       </c>
     </row>
@@ -8112,22 +8090,22 @@
       <c r="A125" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B125" s="28">
-        <v>0</v>
-      </c>
-      <c r="C125" s="28">
-        <v>0</v>
-      </c>
-      <c r="D125" s="28">
-        <v>0</v>
-      </c>
-      <c r="E125" s="28">
-        <v>0</v>
-      </c>
-      <c r="F125" s="28">
-        <v>0</v>
-      </c>
-      <c r="G125" s="28">
+      <c r="B125" s="13">
+        <v>0</v>
+      </c>
+      <c r="C125" s="13">
+        <v>0</v>
+      </c>
+      <c r="D125" s="13">
+        <v>0</v>
+      </c>
+      <c r="E125" s="13">
+        <v>0</v>
+      </c>
+      <c r="F125" s="13">
+        <v>0</v>
+      </c>
+      <c r="G125" s="13">
         <v>0</v>
       </c>
     </row>
@@ -8135,22 +8113,22 @@
       <c r="A126" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B126" s="28">
-        <v>0</v>
-      </c>
-      <c r="C126" s="28">
-        <v>0</v>
-      </c>
-      <c r="D126" s="28">
-        <v>0</v>
-      </c>
-      <c r="E126" s="28">
-        <v>0</v>
-      </c>
-      <c r="F126" s="28">
-        <v>0</v>
-      </c>
-      <c r="G126" s="28">
+      <c r="B126" s="13">
+        <v>0</v>
+      </c>
+      <c r="C126" s="13">
+        <v>0</v>
+      </c>
+      <c r="D126" s="13">
+        <v>0</v>
+      </c>
+      <c r="E126" s="13">
+        <v>0</v>
+      </c>
+      <c r="F126" s="13">
+        <v>0</v>
+      </c>
+      <c r="G126" s="13">
         <v>0</v>
       </c>
     </row>
@@ -8158,22 +8136,22 @@
       <c r="A127" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B127" s="28">
-        <v>0</v>
-      </c>
-      <c r="C127" s="28">
-        <v>0</v>
-      </c>
-      <c r="D127" s="28">
-        <v>0</v>
-      </c>
-      <c r="E127" s="28">
-        <v>0</v>
-      </c>
-      <c r="F127" s="28">
-        <v>0</v>
-      </c>
-      <c r="G127" s="28">
+      <c r="B127" s="13">
+        <v>0</v>
+      </c>
+      <c r="C127" s="13">
+        <v>0</v>
+      </c>
+      <c r="D127" s="13">
+        <v>0</v>
+      </c>
+      <c r="E127" s="13">
+        <v>0</v>
+      </c>
+      <c r="F127" s="13">
+        <v>0</v>
+      </c>
+      <c r="G127" s="13">
         <v>0</v>
       </c>
     </row>
@@ -8205,57 +8183,57 @@
     </row>
     <row r="129" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="84" t="s">
+      <c r="A130" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B130" s="81" t="s">
+      <c r="B130" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="C130" s="82"/>
-      <c r="D130" s="82"/>
-      <c r="E130" s="82"/>
-      <c r="F130" s="82"/>
-      <c r="G130" s="83"/>
+      <c r="C130" s="84"/>
+      <c r="D130" s="84"/>
+      <c r="E130" s="84"/>
+      <c r="F130" s="84"/>
+      <c r="G130" s="85"/>
     </row>
     <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="85"/>
-      <c r="B131" s="38" t="s">
+      <c r="A131" s="87"/>
+      <c r="B131" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="C131" s="39" t="s">
+      <c r="C131" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="D131" s="39" t="s">
+      <c r="D131" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="E131" s="40" t="s">
+      <c r="E131" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F131" s="40" t="s">
+      <c r="F131" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="G131" s="41" t="s">
+      <c r="G131" s="37" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="86"/>
-      <c r="B132" s="62" t="s">
+      <c r="A132" s="88"/>
+      <c r="B132" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="C132" s="63" t="s">
+      <c r="C132" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="D132" s="63" t="s">
+      <c r="D132" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="E132" s="42" t="s">
+      <c r="E132" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F132" s="42" t="s">
+      <c r="F132" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G132" s="53" t="s">
+      <c r="G132" s="46" t="s">
         <v>82</v>
       </c>
     </row>
@@ -8263,22 +8241,22 @@
       <c r="A133" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B133" s="30">
-        <v>0</v>
-      </c>
-      <c r="C133" s="30">
-        <v>0</v>
-      </c>
-      <c r="D133" s="30">
-        <v>0</v>
-      </c>
-      <c r="E133" s="30">
-        <v>0</v>
-      </c>
-      <c r="F133" s="30">
-        <v>0</v>
-      </c>
-      <c r="G133" s="30">
+      <c r="B133" s="27">
+        <v>0</v>
+      </c>
+      <c r="C133" s="27">
+        <v>0</v>
+      </c>
+      <c r="D133" s="27">
+        <v>0</v>
+      </c>
+      <c r="E133" s="27">
+        <v>0</v>
+      </c>
+      <c r="F133" s="27">
+        <v>0</v>
+      </c>
+      <c r="G133" s="27">
         <v>0</v>
       </c>
     </row>
@@ -8286,22 +8264,22 @@
       <c r="A134" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B134" s="30">
-        <v>0</v>
-      </c>
-      <c r="C134" s="30">
-        <v>0</v>
-      </c>
-      <c r="D134" s="30">
-        <v>0</v>
-      </c>
-      <c r="E134" s="30">
-        <v>0</v>
-      </c>
-      <c r="F134" s="30">
-        <v>0</v>
-      </c>
-      <c r="G134" s="30">
+      <c r="B134" s="27">
+        <v>0</v>
+      </c>
+      <c r="C134" s="27">
+        <v>0</v>
+      </c>
+      <c r="D134" s="27">
+        <v>0</v>
+      </c>
+      <c r="E134" s="27">
+        <v>0</v>
+      </c>
+      <c r="F134" s="27">
+        <v>0</v>
+      </c>
+      <c r="G134" s="27">
         <v>0</v>
       </c>
     </row>
@@ -8309,22 +8287,22 @@
       <c r="A135" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B135" s="30">
-        <v>0</v>
-      </c>
-      <c r="C135" s="30">
-        <v>0</v>
-      </c>
-      <c r="D135" s="30">
-        <v>0</v>
-      </c>
-      <c r="E135" s="30">
-        <v>0</v>
-      </c>
-      <c r="F135" s="30">
-        <v>0</v>
-      </c>
-      <c r="G135" s="30">
+      <c r="B135" s="27">
+        <v>0</v>
+      </c>
+      <c r="C135" s="27">
+        <v>0</v>
+      </c>
+      <c r="D135" s="27">
+        <v>0</v>
+      </c>
+      <c r="E135" s="27">
+        <v>0</v>
+      </c>
+      <c r="F135" s="27">
+        <v>0</v>
+      </c>
+      <c r="G135" s="27">
         <v>0</v>
       </c>
     </row>
@@ -8332,22 +8310,22 @@
       <c r="A136" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B136" s="30">
+      <c r="B136" s="27">
         <v>7.0699999999999999E-2</v>
       </c>
-      <c r="C136" s="30">
+      <c r="C136" s="27">
         <v>7.0699999999999999E-2</v>
       </c>
-      <c r="D136" s="30">
+      <c r="D136" s="27">
         <v>7.0699999999999999E-2</v>
       </c>
-      <c r="E136" s="30">
+      <c r="E136" s="27">
         <v>4.1006000000000008E-2</v>
       </c>
-      <c r="F136" s="30">
+      <c r="F136" s="27">
         <v>4.1006000000000008E-2</v>
       </c>
-      <c r="G136" s="30">
+      <c r="G136" s="27">
         <v>2.8987000000000002E-2</v>
       </c>
     </row>
@@ -8355,22 +8333,22 @@
       <c r="A137" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B137" s="30">
+      <c r="B137" s="27">
         <v>0.13900000000000001</v>
       </c>
-      <c r="C137" s="30">
+      <c r="C137" s="27">
         <v>0.13900000000000001</v>
       </c>
-      <c r="D137" s="30">
+      <c r="D137" s="27">
         <v>0.13900000000000001</v>
       </c>
-      <c r="E137" s="30">
+      <c r="E137" s="27">
         <v>8.0620000000000011E-2</v>
       </c>
-      <c r="F137" s="30">
+      <c r="F137" s="27">
         <v>8.0620000000000011E-2</v>
       </c>
-      <c r="G137" s="30">
+      <c r="G137" s="27">
         <v>5.6990000000000013E-2</v>
       </c>
     </row>
@@ -8378,22 +8356,22 @@
       <c r="A138" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B138" s="30">
+      <c r="B138" s="27">
         <v>0.14180000000000001</v>
       </c>
-      <c r="C138" s="30">
+      <c r="C138" s="27">
         <v>0.14180000000000001</v>
       </c>
-      <c r="D138" s="30">
+      <c r="D138" s="27">
         <v>0.14180000000000001</v>
       </c>
-      <c r="E138" s="30">
+      <c r="E138" s="27">
         <v>8.2244000000000012E-2</v>
       </c>
-      <c r="F138" s="30">
+      <c r="F138" s="27">
         <v>8.2244000000000012E-2</v>
       </c>
-      <c r="G138" s="30">
+      <c r="G138" s="27">
         <v>5.8138000000000009E-2</v>
       </c>
     </row>
@@ -8401,22 +8379,22 @@
       <c r="A139" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B139" s="30">
+      <c r="B139" s="27">
         <v>0.1056</v>
       </c>
-      <c r="C139" s="30">
+      <c r="C139" s="27">
         <v>0.1056</v>
       </c>
-      <c r="D139" s="30">
+      <c r="D139" s="27">
         <v>0.1056</v>
       </c>
-      <c r="E139" s="30">
+      <c r="E139" s="27">
         <v>6.1248000000000004E-2</v>
       </c>
-      <c r="F139" s="30">
+      <c r="F139" s="27">
         <v>6.1248000000000004E-2</v>
       </c>
-      <c r="G139" s="30">
+      <c r="G139" s="27">
         <v>4.3296000000000001E-2</v>
       </c>
     </row>
@@ -8424,22 +8402,22 @@
       <c r="A140" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B140" s="30">
+      <c r="B140" s="27">
         <v>6.7400000000000002E-2</v>
       </c>
-      <c r="C140" s="30">
+      <c r="C140" s="27">
         <v>6.7400000000000002E-2</v>
       </c>
-      <c r="D140" s="30">
+      <c r="D140" s="27">
         <v>6.7400000000000002E-2</v>
       </c>
-      <c r="E140" s="30">
+      <c r="E140" s="27">
         <v>3.9092000000000009E-2</v>
       </c>
-      <c r="F140" s="30">
+      <c r="F140" s="27">
         <v>3.9092000000000009E-2</v>
       </c>
-      <c r="G140" s="30">
+      <c r="G140" s="27">
         <v>2.7634000000000002E-2</v>
       </c>
     </row>
@@ -8447,22 +8425,22 @@
       <c r="A141" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B141" s="30">
+      <c r="B141" s="27">
         <v>2.7100000000000003E-2</v>
       </c>
-      <c r="C141" s="30">
+      <c r="C141" s="27">
         <v>2.7100000000000003E-2</v>
       </c>
-      <c r="D141" s="30">
+      <c r="D141" s="27">
         <v>2.7100000000000003E-2</v>
       </c>
-      <c r="E141" s="30">
+      <c r="E141" s="27">
         <v>1.5718000000000003E-2</v>
       </c>
-      <c r="F141" s="30">
+      <c r="F141" s="27">
         <v>1.5718000000000003E-2</v>
       </c>
-      <c r="G141" s="30">
+      <c r="G141" s="27">
         <v>1.1111000000000001E-2</v>
       </c>
     </row>
@@ -8470,22 +8448,22 @@
       <c r="A142" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B142" s="30">
+      <c r="B142" s="27">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="C142" s="30">
+      <c r="C142" s="27">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="D142" s="30">
+      <c r="D142" s="27">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="E142" s="30">
+      <c r="E142" s="27">
         <v>5.1040000000000009E-3</v>
       </c>
-      <c r="F142" s="30">
+      <c r="F142" s="27">
         <v>5.1040000000000009E-3</v>
       </c>
-      <c r="G142" s="30">
+      <c r="G142" s="27">
         <v>3.6080000000000005E-3</v>
       </c>
     </row>
@@ -8493,22 +8471,22 @@
       <c r="A143" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B143" s="30">
-        <v>0</v>
-      </c>
-      <c r="C143" s="30">
-        <v>0</v>
-      </c>
-      <c r="D143" s="30">
-        <v>0</v>
-      </c>
-      <c r="E143" s="30">
-        <v>0</v>
-      </c>
-      <c r="F143" s="30">
-        <v>0</v>
-      </c>
-      <c r="G143" s="30">
+      <c r="B143" s="27">
+        <v>0</v>
+      </c>
+      <c r="C143" s="27">
+        <v>0</v>
+      </c>
+      <c r="D143" s="27">
+        <v>0</v>
+      </c>
+      <c r="E143" s="27">
+        <v>0</v>
+      </c>
+      <c r="F143" s="27">
+        <v>0</v>
+      </c>
+      <c r="G143" s="27">
         <v>0</v>
       </c>
     </row>
@@ -8516,22 +8494,22 @@
       <c r="A144" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B144" s="30">
-        <v>0</v>
-      </c>
-      <c r="C144" s="30">
-        <v>0</v>
-      </c>
-      <c r="D144" s="30">
-        <v>0</v>
-      </c>
-      <c r="E144" s="30">
-        <v>0</v>
-      </c>
-      <c r="F144" s="30">
-        <v>0</v>
-      </c>
-      <c r="G144" s="30">
+      <c r="B144" s="27">
+        <v>0</v>
+      </c>
+      <c r="C144" s="27">
+        <v>0</v>
+      </c>
+      <c r="D144" s="27">
+        <v>0</v>
+      </c>
+      <c r="E144" s="27">
+        <v>0</v>
+      </c>
+      <c r="F144" s="27">
+        <v>0</v>
+      </c>
+      <c r="G144" s="27">
         <v>0</v>
       </c>
     </row>
@@ -8539,22 +8517,22 @@
       <c r="A145" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B145" s="33">
-        <v>0</v>
-      </c>
-      <c r="C145" s="33">
-        <v>0</v>
-      </c>
-      <c r="D145" s="33">
-        <v>0</v>
-      </c>
-      <c r="E145" s="33">
-        <v>0</v>
-      </c>
-      <c r="F145" s="33">
-        <v>0</v>
-      </c>
-      <c r="G145" s="33">
+      <c r="B145" s="27">
+        <v>0</v>
+      </c>
+      <c r="C145" s="27">
+        <v>0</v>
+      </c>
+      <c r="D145" s="27">
+        <v>0</v>
+      </c>
+      <c r="E145" s="27">
+        <v>0</v>
+      </c>
+      <c r="F145" s="27">
+        <v>0</v>
+      </c>
+      <c r="G145" s="27">
         <v>0</v>
       </c>
     </row>
@@ -8562,22 +8540,22 @@
       <c r="A146" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B146" s="33">
-        <v>0</v>
-      </c>
-      <c r="C146" s="33">
-        <v>0</v>
-      </c>
-      <c r="D146" s="33">
-        <v>0</v>
-      </c>
-      <c r="E146" s="33">
-        <v>0</v>
-      </c>
-      <c r="F146" s="33">
-        <v>0</v>
-      </c>
-      <c r="G146" s="33">
+      <c r="B146" s="27">
+        <v>0</v>
+      </c>
+      <c r="C146" s="27">
+        <v>0</v>
+      </c>
+      <c r="D146" s="27">
+        <v>0</v>
+      </c>
+      <c r="E146" s="27">
+        <v>0</v>
+      </c>
+      <c r="F146" s="27">
+        <v>0</v>
+      </c>
+      <c r="G146" s="27">
         <v>0</v>
       </c>
     </row>
@@ -8585,22 +8563,22 @@
       <c r="A147" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B147" s="33">
-        <v>0</v>
-      </c>
-      <c r="C147" s="33">
-        <v>0</v>
-      </c>
-      <c r="D147" s="33">
-        <v>0</v>
-      </c>
-      <c r="E147" s="33">
-        <v>0</v>
-      </c>
-      <c r="F147" s="33">
-        <v>0</v>
-      </c>
-      <c r="G147" s="33">
+      <c r="B147" s="27">
+        <v>0</v>
+      </c>
+      <c r="C147" s="27">
+        <v>0</v>
+      </c>
+      <c r="D147" s="27">
+        <v>0</v>
+      </c>
+      <c r="E147" s="27">
+        <v>0</v>
+      </c>
+      <c r="F147" s="27">
+        <v>0</v>
+      </c>
+      <c r="G147" s="27">
         <v>0</v>
       </c>
     </row>
@@ -8608,22 +8586,22 @@
       <c r="A148" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B148" s="33">
-        <v>0</v>
-      </c>
-      <c r="C148" s="33">
-        <v>0</v>
-      </c>
-      <c r="D148" s="33">
-        <v>0</v>
-      </c>
-      <c r="E148" s="33">
-        <v>0</v>
-      </c>
-      <c r="F148" s="33">
-        <v>0</v>
-      </c>
-      <c r="G148" s="33">
+      <c r="B148" s="27">
+        <v>0</v>
+      </c>
+      <c r="C148" s="27">
+        <v>0</v>
+      </c>
+      <c r="D148" s="27">
+        <v>0</v>
+      </c>
+      <c r="E148" s="27">
+        <v>0</v>
+      </c>
+      <c r="F148" s="27">
+        <v>0</v>
+      </c>
+      <c r="G148" s="27">
         <v>0</v>
       </c>
     </row>
@@ -8654,100 +8632,100 @@
       </c>
     </row>
     <row r="155" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="56" t="s">
+      <c r="A155" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="B155" s="57"/>
-      <c r="C155" s="57"/>
-      <c r="D155" s="57"/>
-      <c r="E155" s="57"/>
-      <c r="F155" s="57"/>
-      <c r="G155" s="57"/>
-      <c r="H155" s="57"/>
-      <c r="I155" s="57"/>
-      <c r="J155" s="57"/>
-      <c r="K155" s="57"/>
-      <c r="L155" s="57"/>
-      <c r="M155" s="57"/>
-      <c r="N155" s="57"/>
-      <c r="O155" s="57"/>
-      <c r="P155" s="57"/>
-      <c r="Q155" s="57"/>
-      <c r="R155" s="57"/>
-      <c r="S155" s="57"/>
-      <c r="T155" s="57"/>
-      <c r="U155" s="57"/>
-      <c r="V155" s="57"/>
-      <c r="W155" s="57"/>
+      <c r="B155" s="50"/>
+      <c r="C155" s="50"/>
+      <c r="D155" s="50"/>
+      <c r="E155" s="50"/>
+      <c r="F155" s="50"/>
+      <c r="G155" s="50"/>
+      <c r="H155" s="50"/>
+      <c r="I155" s="50"/>
+      <c r="J155" s="50"/>
+      <c r="K155" s="50"/>
+      <c r="L155" s="50"/>
+      <c r="M155" s="50"/>
+      <c r="N155" s="50"/>
+      <c r="O155" s="50"/>
+      <c r="P155" s="50"/>
+      <c r="Q155" s="50"/>
+      <c r="R155" s="50"/>
+      <c r="S155" s="50"/>
+      <c r="T155" s="50"/>
+      <c r="U155" s="50"/>
+      <c r="V155" s="50"/>
+      <c r="W155" s="50"/>
     </row>
     <row r="156" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="58" t="s">
+      <c r="A156" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="B156" s="57"/>
-      <c r="C156" s="57"/>
-      <c r="D156" s="57"/>
-      <c r="E156" s="57"/>
-      <c r="F156" s="57"/>
-      <c r="G156" s="57"/>
-      <c r="H156" s="57"/>
-      <c r="I156" s="57"/>
-      <c r="J156" s="57"/>
-      <c r="K156" s="57"/>
-      <c r="L156" s="57"/>
-      <c r="M156" s="57"/>
-      <c r="N156" s="57"/>
-      <c r="O156" s="57"/>
-      <c r="P156" s="57"/>
-      <c r="Q156" s="57"/>
-      <c r="R156" s="57"/>
-      <c r="S156" s="57"/>
-      <c r="T156" s="57"/>
-      <c r="U156" s="57"/>
-      <c r="V156" s="57"/>
-      <c r="W156" s="57"/>
+      <c r="B156" s="50"/>
+      <c r="C156" s="50"/>
+      <c r="D156" s="50"/>
+      <c r="E156" s="50"/>
+      <c r="F156" s="50"/>
+      <c r="G156" s="50"/>
+      <c r="H156" s="50"/>
+      <c r="I156" s="50"/>
+      <c r="J156" s="50"/>
+      <c r="K156" s="50"/>
+      <c r="L156" s="50"/>
+      <c r="M156" s="50"/>
+      <c r="N156" s="50"/>
+      <c r="O156" s="50"/>
+      <c r="P156" s="50"/>
+      <c r="Q156" s="50"/>
+      <c r="R156" s="50"/>
+      <c r="S156" s="50"/>
+      <c r="T156" s="50"/>
+      <c r="U156" s="50"/>
+      <c r="V156" s="50"/>
+      <c r="W156" s="50"/>
     </row>
     <row r="157" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="56" t="s">
+      <c r="A157" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="B157" s="57"/>
-      <c r="C157" s="57"/>
-      <c r="D157" s="57"/>
-      <c r="E157" s="57"/>
-      <c r="F157" s="57"/>
-      <c r="G157" s="57"/>
-      <c r="H157" s="57"/>
-      <c r="I157" s="57"/>
-      <c r="J157" s="57"/>
-      <c r="K157" s="57"/>
-      <c r="L157" s="57"/>
-      <c r="M157" s="57"/>
-      <c r="N157" s="57"/>
-      <c r="O157" s="57"/>
-      <c r="P157" s="57"/>
-      <c r="Q157" s="57"/>
-      <c r="R157" s="57"/>
-      <c r="S157" s="57"/>
-      <c r="T157" s="57"/>
-      <c r="U157" s="57"/>
-      <c r="V157" s="57"/>
-      <c r="W157" s="57"/>
+      <c r="B157" s="50"/>
+      <c r="C157" s="50"/>
+      <c r="D157" s="50"/>
+      <c r="E157" s="50"/>
+      <c r="F157" s="50"/>
+      <c r="G157" s="50"/>
+      <c r="H157" s="50"/>
+      <c r="I157" s="50"/>
+      <c r="J157" s="50"/>
+      <c r="K157" s="50"/>
+      <c r="L157" s="50"/>
+      <c r="M157" s="50"/>
+      <c r="N157" s="50"/>
+      <c r="O157" s="50"/>
+      <c r="P157" s="50"/>
+      <c r="Q157" s="50"/>
+      <c r="R157" s="50"/>
+      <c r="S157" s="50"/>
+      <c r="T157" s="50"/>
+      <c r="U157" s="50"/>
+      <c r="V157" s="50"/>
+      <c r="W157" s="50"/>
     </row>
     <row r="158" spans="1:23" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B158" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="C158" s="99"/>
-      <c r="D158" s="100"/>
-      <c r="E158" s="98" t="s">
+      <c r="B158" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" s="75"/>
+      <c r="D158" s="76"/>
+      <c r="E158" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="F158" s="99"/>
-      <c r="G158" s="100"/>
+      <c r="F158" s="75"/>
+      <c r="G158" s="76"/>
     </row>
     <row r="159" spans="1:23" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="6"/>
@@ -8774,27 +8752,27 @@
       <c r="A160" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B160" s="44">
+      <c r="B160" s="40">
         <f t="shared" ref="B160:G161" si="5">10^-5</f>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="C160" s="44">
+      <c r="C160" s="40">
         <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D160" s="44">
+      <c r="D160" s="40">
         <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E160" s="44">
+      <c r="E160" s="40">
         <f>10^-5</f>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="F160" s="44">
+      <c r="F160" s="40">
         <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G160" s="44">
+      <c r="G160" s="40">
         <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
@@ -8815,27 +8793,27 @@
       <c r="A161" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B161" s="44">
+      <c r="B161" s="40">
         <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="C161" s="44">
+      <c r="C161" s="40">
         <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="D161" s="44">
+      <c r="D161" s="40">
         <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="E161" s="44">
+      <c r="E161" s="40">
         <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="F161" s="44">
+      <c r="F161" s="40">
         <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G161" s="44">
+      <c r="G161" s="40">
         <f t="shared" si="5"/>
         <v>1.0000000000000001E-5</v>
       </c>
@@ -8856,22 +8834,22 @@
       <c r="A162" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B162" s="44">
+      <c r="B162" s="40">
         <v>1.2E-2</v>
       </c>
-      <c r="C162" s="44">
+      <c r="C162" s="40">
         <v>0.12</v>
       </c>
-      <c r="D162" s="44">
+      <c r="D162" s="40">
         <v>1.2</v>
       </c>
-      <c r="E162" s="44">
+      <c r="E162" s="40">
         <v>1.2E-2</v>
       </c>
-      <c r="F162" s="45">
+      <c r="F162" s="41">
         <v>0.12</v>
       </c>
-      <c r="G162" s="46">
+      <c r="G162" s="42">
         <v>1.2</v>
       </c>
       <c r="J162">
@@ -8899,22 +8877,22 @@
       <c r="A163" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B163" s="44">
+      <c r="B163" s="40">
         <v>0.66369047619047616</v>
       </c>
-      <c r="C163" s="44">
+      <c r="C163" s="40">
         <v>2.553903345724907</v>
       </c>
-      <c r="D163" s="44">
+      <c r="D163" s="40">
         <v>6.9636363636363638</v>
       </c>
-      <c r="E163" s="44">
+      <c r="E163" s="40">
         <v>0.66959798994974873</v>
       </c>
-      <c r="F163" s="45">
+      <c r="F163" s="41">
         <v>2.2142857142857144</v>
       </c>
-      <c r="G163" s="47">
+      <c r="G163" s="43">
         <v>6.5</v>
       </c>
       <c r="J163">
@@ -8942,22 +8920,22 @@
       <c r="A164" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B164" s="44">
+      <c r="B164" s="40">
         <v>0.70326409495548958</v>
       </c>
-      <c r="C164" s="44">
+      <c r="C164" s="40">
         <v>2.5474683544303796</v>
       </c>
-      <c r="D164" s="44">
+      <c r="D164" s="40">
         <v>7.6721311475409832</v>
       </c>
-      <c r="E164" s="44">
+      <c r="E164" s="40">
         <v>0.79487179487179482</v>
       </c>
-      <c r="F164" s="45">
+      <c r="F164" s="41">
         <v>2.25</v>
       </c>
-      <c r="G164" s="47">
+      <c r="G164" s="43">
         <v>10</v>
       </c>
       <c r="J164">
@@ -8985,22 +8963,22 @@
       <c r="A165" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B165" s="44">
+      <c r="B165" s="40">
         <v>0.77027027027027029</v>
       </c>
-      <c r="C165" s="44">
+      <c r="C165" s="40">
         <v>2.564245810055866</v>
       </c>
-      <c r="D165" s="44">
+      <c r="D165" s="40">
         <v>6.9705882352941178</v>
       </c>
-      <c r="E165" s="44">
+      <c r="E165" s="40">
         <v>0.80509304603330067</v>
       </c>
-      <c r="F165" s="45">
+      <c r="F165" s="41">
         <v>2.2666666666666666</v>
       </c>
-      <c r="G165" s="47">
+      <c r="G165" s="43">
         <v>5.333333333333333</v>
       </c>
       <c r="J165">
@@ -9028,22 +9006,22 @@
       <c r="A166" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B166" s="44">
+      <c r="B166" s="40">
         <v>0.7710280373831776</v>
       </c>
-      <c r="C166" s="44">
+      <c r="C166" s="40">
         <v>2.4793388429752068</v>
       </c>
-      <c r="D166" s="44">
+      <c r="D166" s="40">
         <v>5.8421052631578947</v>
       </c>
-      <c r="E166" s="44">
+      <c r="E166" s="40">
         <v>0.75512405609492983</v>
       </c>
-      <c r="F166" s="45">
+      <c r="F166" s="41">
         <v>2.0625</v>
       </c>
-      <c r="G166" s="47">
+      <c r="G166" s="43">
         <v>1</v>
       </c>
       <c r="J166">
@@ -9071,22 +9049,22 @@
       <c r="A167" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B167" s="44">
+      <c r="B167" s="40">
         <v>0.77927927927927931</v>
       </c>
-      <c r="C167" s="44">
+      <c r="C167" s="40">
         <v>2.406779661016949</v>
       </c>
-      <c r="D167" s="44">
+      <c r="D167" s="40">
         <v>6.2222222222222223</v>
       </c>
-      <c r="E167" s="44">
+      <c r="E167" s="40">
         <v>0.75529411764705878</v>
       </c>
-      <c r="F167" s="45">
+      <c r="F167" s="41">
         <v>2.2666666666666666</v>
       </c>
-      <c r="G167" s="47">
+      <c r="G167" s="43">
         <v>9</v>
       </c>
       <c r="J167">
@@ -9114,22 +9092,22 @@
       <c r="A168" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B168" s="44">
+      <c r="B168" s="40">
         <v>0.84188034188034189</v>
       </c>
-      <c r="C168" s="44">
+      <c r="C168" s="40">
         <v>2.4166666666666665</v>
       </c>
-      <c r="D168" s="44">
+      <c r="D168" s="40">
         <v>7.75</v>
       </c>
-      <c r="E168" s="44">
+      <c r="E168" s="40">
         <v>0.68708971553610498</v>
       </c>
-      <c r="F168" s="45">
+      <c r="F168" s="41">
         <v>2.2666666666666666</v>
       </c>
-      <c r="G168" s="47">
+      <c r="G168" s="43">
         <v>1</v>
       </c>
       <c r="J168">
@@ -9157,22 +9135,22 @@
       <c r="A169" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B169" s="44">
+      <c r="B169" s="40">
         <v>0.7192982456140351</v>
       </c>
-      <c r="C169" s="44">
+      <c r="C169" s="40">
         <v>2.3250000000000002</v>
       </c>
-      <c r="D169" s="44">
+      <c r="D169" s="40">
         <v>1</v>
       </c>
-      <c r="E169" s="44">
+      <c r="E169" s="40">
         <v>0.68708971553610498</v>
       </c>
-      <c r="F169" s="45">
+      <c r="F169" s="41">
         <v>2.2666666666666666</v>
       </c>
-      <c r="G169" s="47">
+      <c r="G169" s="43">
         <v>1</v>
       </c>
       <c r="J169">
@@ -9200,22 +9178,22 @@
       <c r="A170" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B170" s="44">
+      <c r="B170" s="40">
         <v>0.7192982456140351</v>
       </c>
-      <c r="C170" s="44">
+      <c r="C170" s="40">
         <v>2.3250000000000002</v>
       </c>
-      <c r="D170" s="44">
+      <c r="D170" s="40">
         <v>1</v>
       </c>
-      <c r="E170" s="44">
+      <c r="E170" s="40">
         <v>0.68708971553610498</v>
       </c>
-      <c r="F170" s="45">
+      <c r="F170" s="41">
         <v>2.2666666666666666</v>
       </c>
-      <c r="G170" s="47">
+      <c r="G170" s="43">
         <v>1</v>
       </c>
       <c r="J170">
@@ -9243,22 +9221,22 @@
       <c r="A171" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B171" s="44">
+      <c r="B171" s="40">
         <v>0.7192982456140351</v>
       </c>
-      <c r="C171" s="44">
+      <c r="C171" s="40">
         <v>2.3250000000000002</v>
       </c>
-      <c r="D171" s="44">
+      <c r="D171" s="40">
         <v>1</v>
       </c>
-      <c r="E171" s="44">
+      <c r="E171" s="40">
         <v>0.68708971553610498</v>
       </c>
-      <c r="F171" s="45">
+      <c r="F171" s="41">
         <v>2.2666666666666666</v>
       </c>
-      <c r="G171" s="47">
+      <c r="G171" s="43">
         <v>1</v>
       </c>
       <c r="J171">
@@ -9286,22 +9264,22 @@
       <c r="A172" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B172" s="48">
+      <c r="B172" s="40">
         <v>0.7192982456140351</v>
       </c>
-      <c r="C172" s="48">
+      <c r="C172" s="40">
         <v>2.3250000000000002</v>
       </c>
-      <c r="D172" s="48">
+      <c r="D172" s="40">
         <v>1</v>
       </c>
-      <c r="E172" s="48">
+      <c r="E172" s="40">
         <v>0.68708971553610498</v>
       </c>
-      <c r="F172" s="49">
+      <c r="F172" s="41">
         <v>2.2666666666666666</v>
       </c>
-      <c r="G172" s="50">
+      <c r="G172" s="43">
         <v>1</v>
       </c>
       <c r="J172">
@@ -9329,22 +9307,22 @@
       <c r="A173" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B173" s="48">
+      <c r="B173" s="40">
         <v>0.7192982456140351</v>
       </c>
-      <c r="C173" s="48">
+      <c r="C173" s="40">
         <v>2.3250000000000002</v>
       </c>
-      <c r="D173" s="48">
+      <c r="D173" s="40">
         <v>1</v>
       </c>
-      <c r="E173" s="48">
+      <c r="E173" s="40">
         <v>0.68708971553610498</v>
       </c>
-      <c r="F173" s="49">
+      <c r="F173" s="41">
         <v>2.2666666666666666</v>
       </c>
-      <c r="G173" s="50">
+      <c r="G173" s="43">
         <v>1</v>
       </c>
       <c r="J173">
@@ -9372,22 +9350,22 @@
       <c r="A174" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B174" s="48">
+      <c r="B174" s="40">
         <v>0.7192982456140351</v>
       </c>
-      <c r="C174" s="48">
+      <c r="C174" s="40">
         <v>2.3250000000000002</v>
       </c>
-      <c r="D174" s="48">
+      <c r="D174" s="40">
         <v>1</v>
       </c>
-      <c r="E174" s="48">
+      <c r="E174" s="40">
         <v>0.68708971553610498</v>
       </c>
-      <c r="F174" s="49">
+      <c r="F174" s="41">
         <v>2.2666666666666666</v>
       </c>
-      <c r="G174" s="50">
+      <c r="G174" s="43">
         <v>1</v>
       </c>
       <c r="J174">
@@ -9415,22 +9393,22 @@
       <c r="A175" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B175" s="48">
+      <c r="B175" s="40">
         <v>0.7192982456140351</v>
       </c>
-      <c r="C175" s="48">
+      <c r="C175" s="40">
         <v>2.3250000000000002</v>
       </c>
-      <c r="D175" s="48">
+      <c r="D175" s="40">
         <v>1</v>
       </c>
-      <c r="E175" s="48">
+      <c r="E175" s="40">
         <v>0.68708971553610498</v>
       </c>
-      <c r="F175" s="49">
+      <c r="F175" s="41">
         <v>2.2666666666666666</v>
       </c>
-      <c r="G175" s="50">
+      <c r="G175" s="43">
         <v>1</v>
       </c>
       <c r="H175">
@@ -9471,38 +9449,38 @@
       <c r="A180" s="10"/>
     </row>
     <row r="182" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A182" s="56" t="s">
+      <c r="A182" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="B182" s="57"/>
-      <c r="C182" s="57"/>
-      <c r="D182" s="57"/>
-      <c r="E182" s="57"/>
-      <c r="F182" s="57"/>
-      <c r="G182" s="57"/>
-      <c r="H182" s="57"/>
-      <c r="I182" s="57"/>
-      <c r="J182" s="57"/>
-      <c r="K182" s="57"/>
-      <c r="L182" s="57"/>
-      <c r="M182" s="57"/>
-      <c r="N182" s="57"/>
-      <c r="O182" s="57"/>
-      <c r="P182" s="57"/>
-      <c r="Q182" s="57"/>
-      <c r="R182" s="57"/>
-      <c r="S182" s="57"/>
-      <c r="T182" s="57"/>
-      <c r="U182" s="57"/>
-      <c r="V182" s="57"/>
-      <c r="W182" s="57"/>
+      <c r="B182" s="50"/>
+      <c r="C182" s="50"/>
+      <c r="D182" s="50"/>
+      <c r="E182" s="50"/>
+      <c r="F182" s="50"/>
+      <c r="G182" s="50"/>
+      <c r="H182" s="50"/>
+      <c r="I182" s="50"/>
+      <c r="J182" s="50"/>
+      <c r="K182" s="50"/>
+      <c r="L182" s="50"/>
+      <c r="M182" s="50"/>
+      <c r="N182" s="50"/>
+      <c r="O182" s="50"/>
+      <c r="P182" s="50"/>
+      <c r="Q182" s="50"/>
+      <c r="R182" s="50"/>
+      <c r="S182" s="50"/>
+      <c r="T182" s="50"/>
+      <c r="U182" s="50"/>
+      <c r="V182" s="50"/>
+      <c r="W182" s="50"/>
     </row>
     <row r="183" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="101" t="s">
+      <c r="A183" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="B183" s="101"/>
-      <c r="C183" s="101"/>
+      <c r="B183" s="77"/>
+      <c r="C183" s="77"/>
     </row>
     <row r="184" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
@@ -9519,10 +9497,10 @@
       <c r="A185" s="15">
         <v>1985</v>
       </c>
-      <c r="B185" s="29">
+      <c r="B185" s="26">
         <v>0.3</v>
       </c>
-      <c r="C185" s="29">
+      <c r="C185" s="26">
         <v>0.3</v>
       </c>
     </row>
@@ -9530,10 +9508,10 @@
       <c r="A186" s="15">
         <v>1990</v>
       </c>
-      <c r="B186" s="29">
+      <c r="B186" s="26">
         <v>0.4</v>
       </c>
-      <c r="C186" s="29">
+      <c r="C186" s="26">
         <v>0.4</v>
       </c>
     </row>
@@ -9541,85 +9519,85 @@
       <c r="A187" s="15">
         <v>2000</v>
       </c>
-      <c r="B187" s="29">
+      <c r="B187" s="26">
         <v>0.1</v>
       </c>
-      <c r="C187" s="29">
+      <c r="C187" s="26">
         <v>0.1</v>
       </c>
     </row>
     <row r="194" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A194" s="56" t="s">
+      <c r="A194" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="B194" s="57"/>
-      <c r="C194" s="57"/>
-      <c r="D194" s="57"/>
-      <c r="E194" s="57"/>
-      <c r="F194" s="57"/>
-      <c r="G194" s="57"/>
-      <c r="H194" s="57"/>
-      <c r="I194" s="57"/>
-      <c r="J194" s="57"/>
-      <c r="K194" s="57"/>
-      <c r="L194" s="57"/>
-      <c r="M194" s="57"/>
-      <c r="N194" s="57"/>
-      <c r="O194" s="57"/>
-      <c r="P194" s="57"/>
-      <c r="Q194" s="57"/>
-      <c r="R194" s="57"/>
-      <c r="S194" s="57"/>
-      <c r="T194" s="57"/>
-      <c r="U194" s="57"/>
-      <c r="V194" s="57"/>
-      <c r="W194" s="57"/>
-    </row>
-    <row r="195" spans="1:23" s="59" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A195" s="89" t="s">
+      <c r="B194" s="50"/>
+      <c r="C194" s="50"/>
+      <c r="D194" s="50"/>
+      <c r="E194" s="50"/>
+      <c r="F194" s="50"/>
+      <c r="G194" s="50"/>
+      <c r="H194" s="50"/>
+      <c r="I194" s="50"/>
+      <c r="J194" s="50"/>
+      <c r="K194" s="50"/>
+      <c r="L194" s="50"/>
+      <c r="M194" s="50"/>
+      <c r="N194" s="50"/>
+      <c r="O194" s="50"/>
+      <c r="P194" s="50"/>
+      <c r="Q194" s="50"/>
+      <c r="R194" s="50"/>
+      <c r="S194" s="50"/>
+      <c r="T194" s="50"/>
+      <c r="U194" s="50"/>
+      <c r="V194" s="50"/>
+      <c r="W194" s="50"/>
+    </row>
+    <row r="195" spans="1:23" s="52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A195" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="B195" s="89"/>
-      <c r="C195" s="89"/>
-      <c r="D195" s="89"/>
-      <c r="E195" s="89"/>
-      <c r="F195" s="89"/>
-    </row>
-    <row r="196" spans="1:23" s="59" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A196" s="102" t="s">
+      <c r="B195" s="78"/>
+      <c r="C195" s="78"/>
+      <c r="D195" s="78"/>
+      <c r="E195" s="78"/>
+      <c r="F195" s="78"/>
+    </row>
+    <row r="196" spans="1:23" s="52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A196" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="B196" s="102"/>
-      <c r="C196" s="102"/>
-      <c r="D196" s="102"/>
-      <c r="E196" s="102"/>
-      <c r="F196" s="102"/>
+      <c r="B196" s="79"/>
+      <c r="C196" s="79"/>
+      <c r="D196" s="79"/>
+      <c r="E196" s="79"/>
+      <c r="F196" s="79"/>
     </row>
     <row r="197" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A197" s="95" t="s">
+      <c r="A197" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="B197" s="66"/>
-      <c r="C197" s="66"/>
-      <c r="D197" s="95" t="s">
+      <c r="B197" s="59"/>
+      <c r="C197" s="59"/>
+      <c r="D197" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="E197" s="95"/>
-      <c r="F197" s="95"/>
+      <c r="E197" s="71"/>
+      <c r="F197" s="71"/>
     </row>
     <row r="198" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="95"/>
-      <c r="B198" s="66"/>
-      <c r="C198" s="67" t="s">
+      <c r="A198" s="71"/>
+      <c r="B198" s="59"/>
+      <c r="C198" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="D198" s="67" t="s">
+      <c r="D198" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="E198" s="67" t="s">
+      <c r="E198" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="F198" s="67" t="s">
+      <c r="F198" s="60" t="s">
         <v>57</v>
       </c>
       <c r="H198">
@@ -9628,18 +9606,18 @@
       </c>
     </row>
     <row r="199" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="68" t="s">
+      <c r="A199" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B199" s="66"/>
-      <c r="C199" s="66"/>
-      <c r="D199" s="69">
-        <v>0</v>
-      </c>
-      <c r="E199" s="69">
-        <v>0</v>
-      </c>
-      <c r="F199" s="69">
+      <c r="B199" s="59"/>
+      <c r="C199" s="59"/>
+      <c r="D199" s="62">
+        <v>0</v>
+      </c>
+      <c r="E199" s="62">
+        <v>0</v>
+      </c>
+      <c r="F199" s="62">
         <v>0</v>
       </c>
       <c r="H199">
@@ -9656,18 +9634,18 @@
       </c>
     </row>
     <row r="200" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A200" s="68" t="s">
+      <c r="A200" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="B200" s="66"/>
-      <c r="C200" s="66"/>
-      <c r="D200" s="69">
-        <v>0</v>
-      </c>
-      <c r="E200" s="69">
-        <v>0</v>
-      </c>
-      <c r="F200" s="69">
+      <c r="B200" s="59"/>
+      <c r="C200" s="59"/>
+      <c r="D200" s="62">
+        <v>0</v>
+      </c>
+      <c r="E200" s="62">
+        <v>0</v>
+      </c>
+      <c r="F200" s="62">
         <v>0</v>
       </c>
       <c r="H200">
@@ -9684,22 +9662,22 @@
       </c>
     </row>
     <row r="201" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A201" s="68" t="s">
+      <c r="A201" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="B201" s="66"/>
-      <c r="C201" s="66">
+      <c r="B201" s="59"/>
+      <c r="C201" s="59">
         <v>0.05</v>
       </c>
-      <c r="D201" s="70">
+      <c r="D201" s="63">
         <f>C201*D203</f>
         <v>3.1200000000000006</v>
       </c>
-      <c r="E201" s="70">
+      <c r="E201" s="63">
         <f>E203*$C$201</f>
         <v>1.8719999999999999</v>
       </c>
-      <c r="F201" s="70">
+      <c r="F201" s="63">
         <f>F203*$C$201</f>
         <v>1.1232</v>
       </c>
@@ -9721,22 +9699,22 @@
       </c>
     </row>
     <row r="202" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A202" s="68" t="s">
+      <c r="A202" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="B202" s="66"/>
-      <c r="C202" s="66">
+      <c r="B202" s="59"/>
+      <c r="C202" s="59">
         <v>0.1</v>
       </c>
-      <c r="D202" s="70">
+      <c r="D202" s="63">
         <f>D204*$C$202</f>
         <v>15.600000000000001</v>
       </c>
-      <c r="E202" s="70">
+      <c r="E202" s="63">
         <f>E204*$C$202</f>
         <v>9.36</v>
       </c>
-      <c r="F202" s="70">
+      <c r="F202" s="63">
         <f>F204*$C$202</f>
         <v>5.6159999999999997</v>
       </c>
@@ -9758,24 +9736,24 @@
       </c>
     </row>
     <row r="203" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A203" s="68" t="s">
+      <c r="A203" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="B203" s="71">
+      <c r="B203" s="64">
         <v>1</v>
       </c>
-      <c r="C203" s="66">
+      <c r="C203" s="59">
         <v>0.4</v>
       </c>
-      <c r="D203" s="69">
+      <c r="D203" s="62">
         <f>D204*$C$203</f>
         <v>62.400000000000006</v>
       </c>
-      <c r="E203" s="69">
+      <c r="E203" s="62">
         <f>E204*$C$203</f>
         <v>37.44</v>
       </c>
-      <c r="F203" s="69">
+      <c r="F203" s="62">
         <f>F204*$C$203</f>
         <v>22.463999999999999</v>
       </c>
@@ -9797,22 +9775,22 @@
       </c>
     </row>
     <row r="204" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A204" s="68" t="s">
+      <c r="A204" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="B204" s="71">
+      <c r="B204" s="64">
         <v>5</v>
       </c>
-      <c r="C204" s="72"/>
-      <c r="D204" s="70">
+      <c r="C204" s="65"/>
+      <c r="D204" s="63">
         <f>B238</f>
         <v>156</v>
       </c>
-      <c r="E204" s="70">
+      <c r="E204" s="63">
         <f>C238</f>
         <v>93.6</v>
       </c>
-      <c r="F204" s="70">
+      <c r="F204" s="63">
         <f>D238</f>
         <v>56.16</v>
       </c>
@@ -9834,25 +9812,25 @@
       </c>
     </row>
     <row r="205" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A205" s="68" t="s">
+      <c r="A205" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="B205" s="71">
+      <c r="B205" s="64">
         <v>10</v>
       </c>
-      <c r="C205" s="66">
+      <c r="C205" s="59">
         <f t="shared" ref="C205:C214" si="13">EXP(LN(0.5)*B204/10)</f>
         <v>0.70710678118654757</v>
       </c>
-      <c r="D205" s="70">
+      <c r="D205" s="63">
         <f t="shared" ref="D205:D210" si="14">$D$204*C205</f>
         <v>110.30865786510142</v>
       </c>
-      <c r="E205" s="70">
+      <c r="E205" s="63">
         <f t="shared" ref="E205:E210" si="15">$E$204*C205</f>
         <v>66.185194719060846</v>
       </c>
-      <c r="F205" s="70">
+      <c r="F205" s="63">
         <f t="shared" ref="F205:F210" si="16">$F$204*C205</f>
         <v>39.711116831436506</v>
       </c>
@@ -9872,28 +9850,28 @@
         <f t="shared" si="12"/>
         <v>91.437775604337176</v>
       </c>
-      <c r="M205" s="59"/>
+      <c r="M205" s="52"/>
     </row>
     <row r="206" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A206" s="68" t="s">
+      <c r="A206" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B206" s="71">
+      <c r="B206" s="64">
         <v>15</v>
       </c>
-      <c r="C206" s="66">
+      <c r="C206" s="59">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
-      <c r="D206" s="70">
+      <c r="D206" s="63">
         <f t="shared" si="14"/>
         <v>78</v>
       </c>
-      <c r="E206" s="70">
+      <c r="E206" s="63">
         <f t="shared" si="15"/>
         <v>46.8</v>
       </c>
-      <c r="F206" s="70">
+      <c r="F206" s="63">
         <f t="shared" si="16"/>
         <v>28.08</v>
       </c>
@@ -9913,30 +9891,30 @@
         <f t="shared" si="12"/>
         <v>70.103172413793089</v>
       </c>
-      <c r="N206" s="59"/>
-      <c r="O206" s="59"/>
-      <c r="P206" s="59"/>
+      <c r="N206" s="52"/>
+      <c r="O206" s="52"/>
+      <c r="P206" s="52"/>
     </row>
     <row r="207" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A207" s="68" t="s">
+      <c r="A207" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="B207" s="71">
+      <c r="B207" s="64">
         <v>20</v>
       </c>
-      <c r="C207" s="66">
+      <c r="C207" s="59">
         <f t="shared" si="13"/>
         <v>0.35355339059327379</v>
       </c>
-      <c r="D207" s="70">
+      <c r="D207" s="63">
         <f t="shared" si="14"/>
         <v>55.154328932550712</v>
       </c>
-      <c r="E207" s="70">
+      <c r="E207" s="63">
         <f t="shared" si="15"/>
         <v>33.092597359530423</v>
       </c>
-      <c r="F207" s="70">
+      <c r="F207" s="63">
         <f t="shared" si="16"/>
         <v>19.855558415718253</v>
       </c>
@@ -9958,25 +9936,25 @@
       </c>
     </row>
     <row r="208" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A208" s="68" t="s">
+      <c r="A208" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="B208" s="71">
+      <c r="B208" s="64">
         <v>25</v>
       </c>
-      <c r="C208" s="66">
+      <c r="C208" s="59">
         <f t="shared" si="13"/>
         <v>0.25</v>
       </c>
-      <c r="D208" s="70">
+      <c r="D208" s="63">
         <f t="shared" si="14"/>
         <v>39</v>
       </c>
-      <c r="E208" s="70">
+      <c r="E208" s="63">
         <f t="shared" si="15"/>
         <v>23.4</v>
       </c>
-      <c r="F208" s="70">
+      <c r="F208" s="63">
         <f t="shared" si="16"/>
         <v>14.04</v>
       </c>
@@ -9998,25 +9976,25 @@
       </c>
     </row>
     <row r="209" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A209" s="68" t="s">
+      <c r="A209" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="B209" s="71">
+      <c r="B209" s="64">
         <v>30</v>
       </c>
-      <c r="C209" s="66">
+      <c r="C209" s="59">
         <f t="shared" si="13"/>
         <v>0.17677669529663689</v>
       </c>
-      <c r="D209" s="70">
+      <c r="D209" s="63">
         <f t="shared" si="14"/>
         <v>27.577164466275356</v>
       </c>
-      <c r="E209" s="70">
+      <c r="E209" s="63">
         <f t="shared" si="15"/>
         <v>16.546298679765211</v>
       </c>
-      <c r="F209" s="70">
+      <c r="F209" s="63">
         <f t="shared" si="16"/>
         <v>9.9277792078591265</v>
       </c>
@@ -10038,25 +10016,25 @@
       </c>
     </row>
     <row r="210" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A210" s="68" t="s">
+      <c r="A210" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="B210" s="71">
+      <c r="B210" s="64">
         <v>35</v>
       </c>
-      <c r="C210" s="66">
+      <c r="C210" s="59">
         <f t="shared" si="13"/>
         <v>0.12500000000000003</v>
       </c>
-      <c r="D210" s="70">
+      <c r="D210" s="63">
         <f t="shared" si="14"/>
         <v>19.500000000000004</v>
       </c>
-      <c r="E210" s="70">
+      <c r="E210" s="63">
         <f t="shared" si="15"/>
         <v>11.700000000000001</v>
       </c>
-      <c r="F210" s="70">
+      <c r="F210" s="63">
         <f t="shared" si="16"/>
         <v>7.0200000000000014</v>
       </c>
@@ -10078,25 +10056,25 @@
       </c>
     </row>
     <row r="211" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A211" s="68" t="s">
+      <c r="A211" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="B211" s="71">
+      <c r="B211" s="64">
         <v>40</v>
       </c>
-      <c r="C211" s="66">
+      <c r="C211" s="59">
         <f>EXP(LN(0.5)*B210/10)</f>
         <v>8.8388347648318447E-2</v>
       </c>
-      <c r="D211" s="70">
+      <c r="D211" s="63">
         <f>$D$204*C211</f>
         <v>13.788582233137678</v>
       </c>
-      <c r="E211" s="70">
+      <c r="E211" s="63">
         <f>$E$204*C211</f>
         <v>8.2731493398826057</v>
       </c>
-      <c r="F211" s="70">
+      <c r="F211" s="63">
         <f>$F$204*C211</f>
         <v>4.9638896039295632</v>
       </c>
@@ -10118,25 +10096,25 @@
       </c>
     </row>
     <row r="212" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A212" s="68" t="s">
+      <c r="A212" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B212" s="71">
+      <c r="B212" s="64">
         <v>45</v>
       </c>
-      <c r="C212" s="66">
+      <c r="C212" s="59">
         <f t="shared" si="13"/>
         <v>6.25E-2</v>
       </c>
-      <c r="D212" s="70">
+      <c r="D212" s="63">
         <f>$D$204*C212</f>
         <v>9.75</v>
       </c>
-      <c r="E212" s="70">
+      <c r="E212" s="63">
         <f>$E$204*C212</f>
         <v>5.85</v>
       </c>
-      <c r="F212" s="70">
+      <c r="F212" s="63">
         <f>$F$204*C212</f>
         <v>3.51</v>
       </c>
@@ -10158,25 +10136,25 @@
       </c>
     </row>
     <row r="213" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A213" s="68" t="s">
+      <c r="A213" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="B213" s="71">
+      <c r="B213" s="64">
         <v>50</v>
       </c>
-      <c r="C213" s="66">
+      <c r="C213" s="59">
         <f t="shared" si="13"/>
         <v>4.4194173824159223E-2</v>
       </c>
-      <c r="D213" s="70">
+      <c r="D213" s="63">
         <f>$D$204*C213</f>
         <v>6.894291116568839</v>
       </c>
-      <c r="E213" s="70">
+      <c r="E213" s="63">
         <f>$E$204*C213</f>
         <v>4.1365746699413029</v>
       </c>
-      <c r="F213" s="70">
+      <c r="F213" s="63">
         <f>$F$204*C213</f>
         <v>2.4819448019647816</v>
       </c>
@@ -10198,25 +10176,25 @@
       </c>
     </row>
     <row r="214" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A214" s="68" t="s">
+      <c r="A214" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="B214" s="71">
+      <c r="B214" s="64">
         <v>55</v>
       </c>
-      <c r="C214" s="66">
+      <c r="C214" s="59">
         <f t="shared" si="13"/>
         <v>3.125E-2</v>
       </c>
-      <c r="D214" s="70">
+      <c r="D214" s="63">
         <f>$D$204*C214</f>
         <v>4.875</v>
       </c>
-      <c r="E214" s="70">
+      <c r="E214" s="63">
         <f>$E$204*C214</f>
         <v>2.9249999999999998</v>
       </c>
-      <c r="F214" s="70">
+      <c r="F214" s="63">
         <f>$F$204*C214</f>
         <v>1.7549999999999999</v>
       </c>
@@ -10238,12 +10216,12 @@
       </c>
     </row>
     <row r="215" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A215" s="66"/>
-      <c r="B215" s="71"/>
-      <c r="C215" s="66"/>
-      <c r="D215" s="73"/>
-      <c r="E215" s="73"/>
-      <c r="F215" s="73"/>
+      <c r="A215" s="59"/>
+      <c r="B215" s="64"/>
+      <c r="C215" s="59"/>
+      <c r="D215" s="66"/>
+      <c r="E215" s="66"/>
+      <c r="F215" s="66"/>
       <c r="K215">
         <f>AVERAGE(K201:K214)</f>
         <v>36.59889506656333</v>
@@ -10254,481 +10232,471 @@
       </c>
     </row>
     <row r="216" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A216" s="96" t="s">
+      <c r="A216" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="B216" s="96"/>
-      <c r="C216" s="96"/>
-      <c r="D216" s="96"/>
-      <c r="E216" s="96"/>
-      <c r="F216" s="96"/>
+      <c r="B216" s="72"/>
+      <c r="C216" s="72"/>
+      <c r="D216" s="72"/>
+      <c r="E216" s="72"/>
+      <c r="F216" s="72"/>
     </row>
     <row r="217" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A217" s="97" t="s">
+      <c r="A217" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B217" s="66"/>
-      <c r="C217" s="66"/>
-      <c r="D217" s="95" t="s">
+      <c r="B217" s="59"/>
+      <c r="C217" s="59"/>
+      <c r="D217" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="E217" s="95"/>
-      <c r="F217" s="95"/>
+      <c r="E217" s="71"/>
+      <c r="F217" s="71"/>
     </row>
     <row r="218" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A218" s="97"/>
-      <c r="B218" s="66"/>
-      <c r="C218" s="67" t="s">
+      <c r="A218" s="73"/>
+      <c r="B218" s="59"/>
+      <c r="C218" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="D218" s="67" t="s">
+      <c r="D218" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="E218" s="67" t="s">
+      <c r="E218" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="F218" s="67" t="s">
+      <c r="F218" s="60" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="219" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="68" t="s">
+      <c r="A219" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B219" s="66"/>
-      <c r="C219" s="66"/>
-      <c r="D219" s="69">
-        <v>0</v>
-      </c>
-      <c r="E219" s="69">
-        <v>0</v>
-      </c>
-      <c r="F219" s="69">
+      <c r="B219" s="59"/>
+      <c r="C219" s="59"/>
+      <c r="D219" s="62">
+        <v>0</v>
+      </c>
+      <c r="E219" s="62">
+        <v>0</v>
+      </c>
+      <c r="F219" s="62">
         <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A220" s="68" t="s">
+      <c r="A220" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="B220" s="66"/>
-      <c r="C220" s="66"/>
-      <c r="D220" s="69">
-        <v>0</v>
-      </c>
-      <c r="E220" s="69">
-        <v>0</v>
-      </c>
-      <c r="F220" s="69">
+      <c r="B220" s="59"/>
+      <c r="C220" s="59"/>
+      <c r="D220" s="62">
+        <v>0</v>
+      </c>
+      <c r="E220" s="62">
+        <v>0</v>
+      </c>
+      <c r="F220" s="62">
         <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A221" s="68" t="s">
+      <c r="A221" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="B221" s="66"/>
-      <c r="C221" s="66">
+      <c r="B221" s="59"/>
+      <c r="C221" s="59">
         <v>0.05</v>
       </c>
-      <c r="D221" s="69">
+      <c r="D221" s="62">
         <f>$C$221*D224</f>
         <v>7.8000000000000007</v>
       </c>
-      <c r="E221" s="69">
+      <c r="E221" s="62">
         <f>$C$221*E224</f>
         <v>4.68</v>
       </c>
-      <c r="F221" s="69">
+      <c r="F221" s="62">
         <f>$C$221*F224</f>
         <v>2.8079999999999998</v>
       </c>
     </row>
     <row r="222" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A222" s="68" t="s">
+      <c r="A222" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="B222" s="66"/>
-      <c r="C222" s="66">
+      <c r="B222" s="59"/>
+      <c r="C222" s="59">
         <v>0.1</v>
       </c>
-      <c r="D222" s="70">
+      <c r="D222" s="63">
         <f>D224*$C$222</f>
         <v>15.600000000000001</v>
       </c>
-      <c r="E222" s="70">
+      <c r="E222" s="63">
         <f>E224*$C$222</f>
         <v>9.36</v>
       </c>
-      <c r="F222" s="70">
+      <c r="F222" s="63">
         <f>F224*$C$222</f>
         <v>5.6159999999999997</v>
       </c>
     </row>
     <row r="223" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A223" s="68" t="s">
+      <c r="A223" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="B223" s="71">
+      <c r="B223" s="64">
         <v>1</v>
       </c>
-      <c r="C223" s="66">
+      <c r="C223" s="59">
         <v>0.4</v>
       </c>
-      <c r="D223" s="69">
+      <c r="D223" s="62">
         <f>D224*$C$223</f>
         <v>62.400000000000006</v>
       </c>
-      <c r="E223" s="69">
+      <c r="E223" s="62">
         <f>E224*$C$223</f>
         <v>37.44</v>
       </c>
-      <c r="F223" s="69">
+      <c r="F223" s="62">
         <f>F224*$C$223</f>
         <v>22.463999999999999</v>
       </c>
     </row>
     <row r="224" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A224" s="68" t="s">
+      <c r="A224" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="B224" s="71">
+      <c r="B224" s="64">
         <v>5</v>
       </c>
-      <c r="C224" s="72"/>
-      <c r="D224" s="69">
+      <c r="C224" s="65"/>
+      <c r="D224" s="62">
         <f>B239</f>
         <v>156</v>
       </c>
-      <c r="E224" s="69">
+      <c r="E224" s="62">
         <f>C239</f>
         <v>93.6</v>
       </c>
-      <c r="F224" s="69">
+      <c r="F224" s="62">
         <f>D239</f>
         <v>56.16</v>
       </c>
     </row>
     <row r="225" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A225" s="68" t="s">
+      <c r="A225" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="B225" s="71">
+      <c r="B225" s="64">
         <v>10</v>
       </c>
-      <c r="C225" s="66">
+      <c r="C225" s="59">
         <f t="shared" ref="C225:C234" si="17">EXP(LN(0.5)*B224/10)</f>
         <v>0.70710678118654757</v>
       </c>
-      <c r="D225" s="69">
+      <c r="D225" s="62">
         <f>D$224*$C$225</f>
         <v>110.30865786510142</v>
       </c>
-      <c r="E225" s="69">
+      <c r="E225" s="62">
         <f>E$224*$C$225</f>
         <v>66.185194719060846</v>
       </c>
-      <c r="F225" s="69">
+      <c r="F225" s="62">
         <f>F$224*$C$225</f>
         <v>39.711116831436506</v>
       </c>
     </row>
     <row r="226" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A226" s="68" t="s">
+      <c r="A226" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B226" s="71">
+      <c r="B226" s="64">
         <v>15</v>
       </c>
-      <c r="C226" s="66">
+      <c r="C226" s="59">
         <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="D226" s="69">
+      <c r="D226" s="62">
         <f t="shared" ref="D226:D232" si="18">$D$224*C226</f>
         <v>78</v>
       </c>
-      <c r="E226" s="69">
+      <c r="E226" s="62">
         <f t="shared" ref="E226:E232" si="19">$E$224*C226</f>
         <v>46.8</v>
       </c>
-      <c r="F226" s="69">
+      <c r="F226" s="62">
         <f t="shared" ref="F226:F232" si="20">$F$224*C226</f>
         <v>28.08</v>
       </c>
     </row>
     <row r="227" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A227" s="68" t="s">
+      <c r="A227" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="B227" s="71">
+      <c r="B227" s="64">
         <v>20</v>
       </c>
-      <c r="C227" s="66">
+      <c r="C227" s="59">
         <f t="shared" si="17"/>
         <v>0.35355339059327379</v>
       </c>
-      <c r="D227" s="69">
+      <c r="D227" s="62">
         <f t="shared" si="18"/>
         <v>55.154328932550712</v>
       </c>
-      <c r="E227" s="69">
+      <c r="E227" s="62">
         <f t="shared" si="19"/>
         <v>33.092597359530423</v>
       </c>
-      <c r="F227" s="69">
+      <c r="F227" s="62">
         <f t="shared" si="20"/>
         <v>19.855558415718253</v>
       </c>
     </row>
     <row r="228" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A228" s="68" t="s">
+      <c r="A228" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="B228" s="71">
+      <c r="B228" s="64">
         <v>25</v>
       </c>
-      <c r="C228" s="66">
+      <c r="C228" s="59">
         <f t="shared" si="17"/>
         <v>0.25</v>
       </c>
-      <c r="D228" s="69">
+      <c r="D228" s="62">
         <f t="shared" si="18"/>
         <v>39</v>
       </c>
-      <c r="E228" s="69">
+      <c r="E228" s="62">
         <f t="shared" si="19"/>
         <v>23.4</v>
       </c>
-      <c r="F228" s="69">
+      <c r="F228" s="62">
         <f t="shared" si="20"/>
         <v>14.04</v>
       </c>
     </row>
     <row r="229" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A229" s="68" t="s">
+      <c r="A229" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="B229" s="71">
+      <c r="B229" s="64">
         <v>30</v>
       </c>
-      <c r="C229" s="66">
+      <c r="C229" s="59">
         <f t="shared" si="17"/>
         <v>0.17677669529663689</v>
       </c>
-      <c r="D229" s="69">
+      <c r="D229" s="62">
         <f t="shared" si="18"/>
         <v>27.577164466275356</v>
       </c>
-      <c r="E229" s="69">
+      <c r="E229" s="62">
         <f t="shared" si="19"/>
         <v>16.546298679765211</v>
       </c>
-      <c r="F229" s="69">
+      <c r="F229" s="62">
         <f t="shared" si="20"/>
         <v>9.9277792078591265</v>
       </c>
     </row>
     <row r="230" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A230" s="68" t="s">
+      <c r="A230" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="B230" s="71">
+      <c r="B230" s="64">
         <v>35</v>
       </c>
-      <c r="C230" s="66">
+      <c r="C230" s="59">
         <f t="shared" si="17"/>
         <v>0.12500000000000003</v>
       </c>
-      <c r="D230" s="69">
+      <c r="D230" s="62">
         <f t="shared" si="18"/>
         <v>19.500000000000004</v>
       </c>
-      <c r="E230" s="69">
+      <c r="E230" s="62">
         <f t="shared" si="19"/>
         <v>11.700000000000001</v>
       </c>
-      <c r="F230" s="69">
+      <c r="F230" s="62">
         <f t="shared" si="20"/>
         <v>7.0200000000000014</v>
       </c>
     </row>
     <row r="231" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A231" s="68" t="s">
+      <c r="A231" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="B231" s="71">
+      <c r="B231" s="64">
         <v>40</v>
       </c>
-      <c r="C231" s="66">
+      <c r="C231" s="59">
         <f t="shared" si="17"/>
         <v>8.8388347648318447E-2</v>
       </c>
-      <c r="D231" s="69">
+      <c r="D231" s="62">
         <f t="shared" si="18"/>
         <v>13.788582233137678</v>
       </c>
-      <c r="E231" s="69">
+      <c r="E231" s="62">
         <f t="shared" si="19"/>
         <v>8.2731493398826057</v>
       </c>
-      <c r="F231" s="69">
+      <c r="F231" s="62">
         <f t="shared" si="20"/>
         <v>4.9638896039295632</v>
       </c>
     </row>
     <row r="232" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A232" s="68" t="s">
+      <c r="A232" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B232" s="71">
+      <c r="B232" s="64">
         <v>45</v>
       </c>
-      <c r="C232" s="66">
+      <c r="C232" s="59">
         <f t="shared" si="17"/>
         <v>6.25E-2</v>
       </c>
-      <c r="D232" s="69">
+      <c r="D232" s="62">
         <f t="shared" si="18"/>
         <v>9.75</v>
       </c>
-      <c r="E232" s="69">
+      <c r="E232" s="62">
         <f t="shared" si="19"/>
         <v>5.85</v>
       </c>
-      <c r="F232" s="69">
+      <c r="F232" s="62">
         <f t="shared" si="20"/>
         <v>3.51</v>
       </c>
     </row>
     <row r="233" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A233" s="68" t="s">
+      <c r="A233" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="B233" s="71">
+      <c r="B233" s="64">
         <v>50</v>
       </c>
-      <c r="C233" s="66">
+      <c r="C233" s="59">
         <f>EXP(LN(0.5)*B232/10)</f>
         <v>4.4194173824159223E-2</v>
       </c>
-      <c r="D233" s="69">
+      <c r="D233" s="62">
         <f>$D$224*C233</f>
         <v>6.894291116568839</v>
       </c>
-      <c r="E233" s="69">
+      <c r="E233" s="62">
         <f>$E$224*C233</f>
         <v>4.1365746699413029</v>
       </c>
-      <c r="F233" s="69">
+      <c r="F233" s="62">
         <f>$F$224*C233</f>
         <v>2.4819448019647816</v>
       </c>
     </row>
     <row r="234" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A234" s="68" t="s">
+      <c r="A234" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="B234" s="71">
+      <c r="B234" s="64">
         <v>55</v>
       </c>
-      <c r="C234" s="66">
+      <c r="C234" s="59">
         <f t="shared" si="17"/>
         <v>3.125E-2</v>
       </c>
-      <c r="D234" s="69">
+      <c r="D234" s="62">
         <f>$D$224*C234</f>
         <v>4.875</v>
       </c>
-      <c r="E234" s="69">
+      <c r="E234" s="62">
         <f>$E$224*C234</f>
         <v>2.9249999999999998</v>
       </c>
-      <c r="F234" s="69">
+      <c r="F234" s="62">
         <f>$F$224*C234</f>
         <v>1.7549999999999999</v>
       </c>
     </row>
     <row r="235" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A235" s="55"/>
-      <c r="B235" s="55"/>
-      <c r="C235" s="65"/>
-      <c r="D235" s="55"/>
-      <c r="E235" s="55"/>
-      <c r="F235" s="55"/>
+      <c r="A235" s="48"/>
+      <c r="B235" s="48"/>
+      <c r="C235" s="58"/>
+      <c r="D235" s="48"/>
+      <c r="E235" s="48"/>
+      <c r="F235" s="48"/>
     </row>
     <row r="236" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A236" s="64" t="s">
+      <c r="A236" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="B236" s="59"/>
-      <c r="C236" s="59"/>
-      <c r="D236" s="59"/>
-      <c r="E236" s="55"/>
-      <c r="F236" s="55"/>
+      <c r="B236" s="52"/>
+      <c r="C236" s="52"/>
+      <c r="D236" s="52"/>
+      <c r="E236" s="48"/>
+      <c r="F236" s="48"/>
     </row>
     <row r="237" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A237" s="76" t="s">
+      <c r="A237" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="B237" s="77" t="s">
+      <c r="B237" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="C237" s="77" t="s">
+      <c r="C237" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="D237" s="77" t="s">
+      <c r="D237" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="E237" s="55"/>
-      <c r="F237" s="55"/>
+      <c r="E237" s="48"/>
+      <c r="F237" s="48"/>
     </row>
     <row r="238" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A238" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B238" s="71">
+      <c r="A238" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B238" s="64">
         <f>52*3</f>
         <v>156</v>
       </c>
-      <c r="C238" s="71">
+      <c r="C238" s="64">
         <f>B238*0.6</f>
         <v>93.6</v>
       </c>
-      <c r="D238" s="71">
+      <c r="D238" s="64">
         <f>C238*0.6</f>
         <v>56.16</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A239" s="26" t="s">
+      <c r="A239" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B239" s="71">
+      <c r="B239" s="64">
         <f>52*3</f>
         <v>156</v>
       </c>
-      <c r="C239" s="71">
+      <c r="C239" s="64">
         <f>B239*0.6</f>
         <v>93.6</v>
       </c>
-      <c r="D239" s="71">
+      <c r="D239" s="64">
         <f>C239*0.6</f>
         <v>56.16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="A216:F216"/>
-    <mergeCell ref="A217:A218"/>
-    <mergeCell ref="B158:D158"/>
-    <mergeCell ref="E158:G158"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A195:F195"/>
-    <mergeCell ref="A196:F196"/>
-    <mergeCell ref="D197:F197"/>
-    <mergeCell ref="D217:F217"/>
     <mergeCell ref="A109:A111"/>
     <mergeCell ref="B109:G109"/>
     <mergeCell ref="B130:G130"/>
@@ -10741,6 +10709,16 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="B81:B83"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="A216:F216"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="B158:D158"/>
+    <mergeCell ref="E158:G158"/>
+    <mergeCell ref="A183:C183"/>
+    <mergeCell ref="A195:F195"/>
+    <mergeCell ref="A196:F196"/>
+    <mergeCell ref="D197:F197"/>
+    <mergeCell ref="D217:F217"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add a third matrix for fertility by 2020 in Excel doc and update years. In loadUp2, add code to load and save matrix and set up matrices for use in bornAgeDieRisk. Update bornAgeDieRisk accordingly to scale fertility down from 1990 to 2010 and from 2010 to 2020. Update loadUp2 inputs in historicalSim, futureSim, and showResults. Update file names accordingly. In loadUp2, update transmission probability to assume persons on ART are virally suppressed. Decrease frequency of checkpointing in historicalSim.
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="99">
   <si>
     <t>Male</t>
   </si>
@@ -418,9 +418,6 @@
     <t>Note: fertility rates changed linearly from 1995 to 2005 so that the model's population growth resembles actual population growth patterns. Fertility rate for 2005 onwards is 1/2 the fertility rate before 1995.</t>
   </si>
   <si>
-    <t>Fertility Rate (per year) before 1995</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">HIV- </t>
     </r>
@@ -433,9 +430,6 @@
       </rPr>
       <t/>
     </r>
-  </si>
-  <si>
-    <t>Fertility Rate (per year) after 2005</t>
   </si>
   <si>
     <r>
@@ -531,6 +525,15 @@
   </si>
   <si>
     <t>Statistics South Africa. Primary tables KwaZulu-Natal: Census '96 and 2001 compared. . (2004). (http://www.statssa.gov.za/census/census_2011/census_products/KZN_Municipal_Report.pdf, page 120)</t>
+  </si>
+  <si>
+    <t>Fertility Rate (per year) before 1990</t>
+  </si>
+  <si>
+    <t>Fertility Rate (per year) by 2010</t>
+  </si>
+  <si>
+    <t>Fertility Rate (per year) by 2020</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1384,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1539,33 +1542,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1599,6 +1582,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1614,7 +1600,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -6068,45 +6077,46 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q142" sqref="Q142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" customWidth="1"/>
-    <col min="17" max="17" width="19.85546875" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.140625" customWidth="1"/>
-    <col min="26" max="26" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.28515625" customWidth="1"/>
-    <col min="28" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" customWidth="1"/>
-    <col min="31" max="31" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.140625" customWidth="1"/>
-    <col min="33" max="33" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.7265625" customWidth="1"/>
+    <col min="17" max="17" width="19.81640625" customWidth="1"/>
+    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.81640625" customWidth="1"/>
+    <col min="21" max="21" width="15.453125" customWidth="1"/>
+    <col min="22" max="22" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.1796875" customWidth="1"/>
+    <col min="26" max="26" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.26953125" customWidth="1"/>
+    <col min="28" max="29" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.81640625" customWidth="1"/>
+    <col min="31" max="31" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.1796875" customWidth="1"/>
+    <col min="33" max="33" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
         <v>63</v>
       </c>
@@ -6135,7 +6145,7 @@
       <c r="X1" s="50"/>
       <c r="Y1" s="50"/>
     </row>
-    <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="51" t="s">
         <v>62</v>
       </c>
@@ -6164,9 +6174,9 @@
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
     </row>
-    <row r="3" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -6193,16 +6203,16 @@
       <c r="X3" s="50"/>
       <c r="Y3" s="50"/>
     </row>
-    <row r="4" spans="1:25" s="52" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" s="52" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="90"/>
-    </row>
-    <row r="5" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="84"/>
+    </row>
+    <row r="5" spans="1:25" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="53"/>
       <c r="B5" s="47" t="s">
         <v>0</v>
@@ -6211,7 +6221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -6222,7 +6232,7 @@
         <v>417311</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="33.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -6233,7 +6243,7 @@
         <v>361594</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -6244,7 +6254,7 @@
         <v>329333</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -6255,7 +6265,7 @@
         <v>296947</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
@@ -6266,7 +6276,7 @@
         <v>273204</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
@@ -6277,7 +6287,7 @@
         <v>249396</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -6288,7 +6298,7 @@
         <v>211839</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
@@ -6299,7 +6309,7 @@
         <v>176470</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -6310,7 +6320,7 @@
         <v>143351</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -6321,7 +6331,7 @@
         <v>123441</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -6332,7 +6342,7 @@
         <v>98355</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
         <v>27</v>
       </c>
@@ -6343,59 +6353,59 @@
         <v>82330</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="96">
+      <c r="B18" s="73">
         <f>314094/6.27</f>
         <v>50094.736842105267</v>
       </c>
-      <c r="C18" s="96">
+      <c r="C18" s="73">
         <f>366793/6.36</f>
         <v>57671.85534591195</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="96">
+      <c r="B19" s="73">
         <f>224490/6.27</f>
         <v>35803.827751196171</v>
       </c>
-      <c r="C19" s="96">
+      <c r="C19" s="73">
         <f>282911/6.36</f>
         <v>44482.861635220121</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="96">
+      <c r="B20" s="73">
         <f>151123/6.27</f>
         <v>24102.551834130783</v>
       </c>
-      <c r="C20" s="96">
+      <c r="C20" s="73">
         <f>215469/6.36</f>
         <v>33878.773584905655</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="96">
+      <c r="B21" s="73">
         <f>89288/6.27</f>
         <v>14240.510366826158</v>
       </c>
-      <c r="C21" s="96">
+      <c r="C21" s="73">
         <f>144901/6.36</f>
         <v>22783.176100628931</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="24" t="s">
         <v>28</v>
       </c>
@@ -6413,11 +6423,11 @@
       </c>
       <c r="X22" s="17"/>
     </row>
-    <row r="23" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
     </row>
-    <row r="24" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
         <v>59</v>
       </c>
@@ -6430,19 +6440,19 @@
         <v>6.3660571774707435</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="F26" s="39"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="91"/>
-    </row>
-    <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C27" s="86"/>
+    </row>
+    <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="12"/>
       <c r="B28" s="45" t="s">
         <v>0</v>
@@ -6452,7 +6462,7 @@
       </c>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>11</v>
       </c>
@@ -6464,7 +6474,7 @@
         <v>417311</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
         <v>14</v>
       </c>
@@ -6475,7 +6485,7 @@
         <v>361594</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>17</v>
       </c>
@@ -6487,7 +6497,7 @@
       </c>
       <c r="L31" s="11"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
         <v>18</v>
       </c>
@@ -6498,7 +6508,7 @@
         <v>296947</v>
       </c>
     </row>
-    <row r="33" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
         <v>19</v>
       </c>
@@ -6509,7 +6519,7 @@
         <v>273204</v>
       </c>
     </row>
-    <row r="34" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
         <v>20</v>
       </c>
@@ -6520,7 +6530,7 @@
         <v>249396</v>
       </c>
     </row>
-    <row r="35" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
         <v>21</v>
       </c>
@@ -6531,7 +6541,7 @@
         <v>211839</v>
       </c>
     </row>
-    <row r="36" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
         <v>22</v>
       </c>
@@ -6551,7 +6561,7 @@
       <c r="AE36" s="9"/>
       <c r="AF36" s="17"/>
     </row>
-    <row r="37" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
         <v>24</v>
       </c>
@@ -6570,7 +6580,7 @@
       <c r="AD37" s="18"/>
       <c r="AE37" s="18"/>
     </row>
-    <row r="38" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>25</v>
       </c>
@@ -6589,7 +6599,7 @@
       <c r="AD38" s="30"/>
       <c r="AE38" s="30"/>
     </row>
-    <row r="39" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
         <v>26</v>
       </c>
@@ -6608,7 +6618,7 @@
       <c r="AD39" s="31"/>
       <c r="AE39" s="31"/>
     </row>
-    <row r="40" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
         <v>27</v>
       </c>
@@ -6627,7 +6637,7 @@
       <c r="AD40" s="31"/>
       <c r="AE40" s="31"/>
     </row>
-    <row r="41" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="21" t="s">
         <v>49</v>
       </c>
@@ -6647,7 +6657,7 @@
       <c r="AD41" s="31"/>
       <c r="AE41" s="31"/>
     </row>
-    <row r="42" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="21" t="s">
         <v>50</v>
       </c>
@@ -6667,7 +6677,7 @@
       <c r="AD42" s="32"/>
       <c r="AE42" s="32"/>
     </row>
-    <row r="43" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="21" t="s">
         <v>51</v>
       </c>
@@ -6687,7 +6697,7 @@
       <c r="AD43" s="32"/>
       <c r="AE43" s="32"/>
     </row>
-    <row r="44" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="21" t="s">
         <v>52</v>
       </c>
@@ -6707,7 +6717,7 @@
       <c r="AD44" s="32"/>
       <c r="AE44" s="32"/>
     </row>
-    <row r="45" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="X45" s="32"/>
       <c r="Y45" s="32"/>
       <c r="Z45" s="32"/>
@@ -6717,7 +6727,7 @@
       <c r="AD45" s="32"/>
       <c r="AE45" s="32"/>
     </row>
-    <row r="46" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="X46" s="32"/>
       <c r="Y46" s="32"/>
       <c r="Z46" s="32"/>
@@ -6727,7 +6737,7 @@
       <c r="AD46" s="32"/>
       <c r="AE46" s="32"/>
     </row>
-    <row r="47" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="X47" s="32"/>
       <c r="Y47" s="32"/>
       <c r="Z47" s="32"/>
@@ -6737,7 +6747,7 @@
       <c r="AD47" s="32"/>
       <c r="AE47" s="32"/>
     </row>
-    <row r="48" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
       <c r="X48" s="32"/>
       <c r="Y48" s="32"/>
       <c r="Z48" s="32"/>
@@ -6747,7 +6757,7 @@
       <c r="AD48" s="32"/>
       <c r="AE48" s="32"/>
     </row>
-    <row r="49" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="X49" s="32"/>
       <c r="Y49" s="32"/>
       <c r="Z49" s="32"/>
@@ -6757,7 +6767,7 @@
       <c r="AD49" s="32"/>
       <c r="AE49" s="32"/>
     </row>
-    <row r="50" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="49" t="s">
         <v>66</v>
       </c>
@@ -6792,7 +6802,7 @@
       <c r="AD50" s="32"/>
       <c r="AE50" s="32"/>
     </row>
-    <row r="51" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="51" t="s">
         <v>69</v>
       </c>
@@ -6827,20 +6837,20 @@
       <c r="AD51" s="32"/>
       <c r="AE51" s="32"/>
     </row>
-    <row r="52" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="95" t="s">
+    <row r="52" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="95" t="s">
+      <c r="B52" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="95"/>
-      <c r="D52" s="95"/>
-      <c r="E52" s="95" t="s">
+      <c r="C52" s="90"/>
+      <c r="D52" s="90"/>
+      <c r="E52" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="95"/>
-      <c r="G52" s="95"/>
+      <c r="F52" s="90"/>
+      <c r="G52" s="90"/>
       <c r="X52" s="30"/>
       <c r="Y52" s="30"/>
       <c r="Z52" s="30"/>
@@ -6850,8 +6860,8 @@
       <c r="AD52" s="30"/>
       <c r="AE52" s="30"/>
     </row>
-    <row r="53" spans="1:31" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="95"/>
+    <row r="53" spans="1:31" ht="30" x14ac:dyDescent="0.35">
+      <c r="A53" s="90"/>
       <c r="B53" s="45" t="s">
         <v>6</v>
       </c>
@@ -6879,7 +6889,7 @@
       <c r="AD53" s="33"/>
       <c r="AE53" s="33"/>
     </row>
-    <row r="54" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
         <v>11</v>
       </c>
@@ -6903,7 +6913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="8" t="s">
         <v>14</v>
       </c>
@@ -6927,7 +6937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="8" t="s">
         <v>17</v>
       </c>
@@ -6952,7 +6962,7 @@
         <v>5.0000000000000183E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="8" t="s">
         <v>18</v>
       </c>
@@ -6975,7 +6985,7 @@
         <v>2.4213075060532689E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="8" t="s">
         <v>19</v>
       </c>
@@ -6998,7 +7008,7 @@
         <v>1.6393442622950817E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="8" t="s">
         <v>20</v>
       </c>
@@ -7022,7 +7032,7 @@
       </c>
       <c r="O59" s="16"/>
     </row>
-    <row r="60" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="8" t="s">
         <v>23</v>
       </c>
@@ -7046,7 +7056,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="8" t="s">
         <v>22</v>
       </c>
@@ -7069,7 +7079,7 @@
         <v>1.1547344110854503E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="8" t="s">
         <v>24</v>
       </c>
@@ -7094,7 +7104,7 @@
         <v>9.9999999999988987E-5</v>
       </c>
     </row>
-    <row r="63" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="8" t="s">
         <v>25</v>
       </c>
@@ -7118,7 +7128,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64" s="8" t="s">
         <v>26</v>
       </c>
@@ -7142,7 +7152,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65" s="8" t="s">
         <v>27</v>
       </c>
@@ -7166,7 +7176,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66" s="21" t="s">
         <v>49</v>
       </c>
@@ -7190,7 +7200,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="21" t="s">
         <v>50</v>
       </c>
@@ -7214,7 +7224,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68" s="21" t="s">
         <v>51</v>
       </c>
@@ -7238,7 +7248,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69" s="21" t="s">
         <v>52</v>
       </c>
@@ -7262,7 +7272,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A71" s="39" t="s">
         <v>60</v>
       </c>
@@ -7291,7 +7301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A72" s="39" t="s">
         <v>61</v>
       </c>
@@ -7300,7 +7310,7 @@
         <v>0.83084071366534329</v>
       </c>
     </row>
-    <row r="78" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A78" s="49" t="s">
         <v>70</v>
       </c>
@@ -7328,7 +7338,7 @@
       <c r="W78" s="50"/>
       <c r="X78" s="50"/>
     </row>
-    <row r="79" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79" s="51" t="s">
         <v>71</v>
       </c>
@@ -7356,7 +7366,7 @@
       <c r="W79" s="50"/>
       <c r="X79" s="50"/>
     </row>
-    <row r="80" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="51" t="s">
         <v>72</v>
       </c>
@@ -7384,28 +7394,28 @@
       <c r="W80" s="50"/>
       <c r="X80" s="50"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="80" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="92" t="s">
+      <c r="B81" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="92" t="s">
+      <c r="C81" s="87" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="81"/>
-      <c r="B82" s="93"/>
-      <c r="C82" s="93"/>
-    </row>
-    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="82"/>
-      <c r="B83" s="94"/>
-      <c r="C83" s="94"/>
-    </row>
-    <row r="84" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="75"/>
+      <c r="B82" s="88"/>
+      <c r="C82" s="88"/>
+    </row>
+    <row r="83" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="76"/>
+      <c r="B83" s="89"/>
+      <c r="C83" s="89"/>
+    </row>
+    <row r="84" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="4" t="s">
         <v>11</v>
       </c>
@@ -7416,7 +7426,7 @@
         <v>8.8057230624727749E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="4" t="s">
         <v>14</v>
       </c>
@@ -7427,7 +7437,7 @@
         <v>5.2457282047517039E-4</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="4" t="s">
         <v>17</v>
       </c>
@@ -7438,7 +7448,7 @@
         <v>4.8877879149405545E-4</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="4" t="s">
         <v>18</v>
       </c>
@@ -7449,7 +7459,7 @@
         <v>9.035280767087482E-4</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="4" t="s">
         <v>19</v>
       </c>
@@ -7460,7 +7470,7 @@
         <v>1.6915946235478447E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="4" t="s">
         <v>20</v>
       </c>
@@ -7471,7 +7481,7 @@
         <v>2.0719480819543991E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="4" t="s">
         <v>23</v>
       </c>
@@ -7482,7 +7492,7 @@
         <v>2.4601074470881829E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="4" t="s">
         <v>22</v>
       </c>
@@ -7493,7 +7503,7 @@
         <v>2.9925533571735037E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="4" t="s">
         <v>24</v>
       </c>
@@ -7504,7 +7514,7 @@
         <v>3.9413474052092329E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="4" t="s">
         <v>25</v>
       </c>
@@ -7515,7 +7525,7 @@
         <v>5.3575989334735206E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="4" t="s">
         <v>26</v>
       </c>
@@ -7526,7 +7536,7 @@
         <v>7.5410818923787939E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="4" t="s">
         <v>27</v>
       </c>
@@ -7537,7 +7547,7 @@
         <v>1.0540154917424747E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="21" t="s">
         <v>49</v>
       </c>
@@ -7548,7 +7558,7 @@
         <v>1.5759592316689931E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="21" t="s">
         <v>50</v>
       </c>
@@ -7559,7 +7569,7 @@
         <v>2.2837523063216215E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="21" t="s">
         <v>51</v>
       </c>
@@ -7570,7 +7580,7 @@
         <v>3.3336893194863555E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="21" t="s">
         <v>52</v>
       </c>
@@ -7581,7 +7591,17 @@
         <v>6.1722846856347699E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B100">
+        <f>5*SUM(B84:B99)</f>
+        <v>1.4052970667115117</v>
+      </c>
+      <c r="C100">
+        <f>5*SUM(C84:C99)</f>
+        <v>0.90487922420259181</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A105" s="49" t="s">
         <v>73</v>
       </c>
@@ -7609,7 +7629,7 @@
       <c r="W105" s="50"/>
       <c r="X105" s="50"/>
     </row>
-    <row r="106" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A106" s="51" t="s">
         <v>74</v>
       </c>
@@ -7637,7 +7657,7 @@
       <c r="W106" s="50"/>
       <c r="X106" s="50"/>
     </row>
-    <row r="107" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A107" s="51" t="s">
         <v>75</v>
       </c>
@@ -7665,7 +7685,7 @@
       <c r="W107" s="50"/>
       <c r="X107" s="50"/>
     </row>
-    <row r="108" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="49" t="s">
         <v>84</v>
       </c>
@@ -7693,21 +7713,21 @@
       <c r="W108" s="50"/>
       <c r="X108" s="50"/>
     </row>
-    <row r="109" spans="1:24" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="80" t="s">
+    <row r="109" spans="1:24" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B109" s="83" t="s">
-        <v>85</v>
-      </c>
-      <c r="C109" s="84"/>
-      <c r="D109" s="84"/>
-      <c r="E109" s="84"/>
-      <c r="F109" s="84"/>
-      <c r="G109" s="85"/>
-    </row>
-    <row r="110" spans="1:24" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="81"/>
+      <c r="B109" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="C109" s="78"/>
+      <c r="D109" s="78"/>
+      <c r="E109" s="78"/>
+      <c r="F109" s="78"/>
+      <c r="G109" s="79"/>
+    </row>
+    <row r="110" spans="1:24" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="75"/>
       <c r="B110" s="44" t="s">
         <v>83</v>
       </c>
@@ -7727,8 +7747,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="111" spans="1:24" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="82"/>
+    <row r="111" spans="1:24" ht="47" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="76"/>
       <c r="B111" s="46" t="s">
         <v>76</v>
       </c>
@@ -7748,7 +7768,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="112" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="4" t="s">
         <v>11</v>
       </c>
@@ -7771,7 +7791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="4" t="s">
         <v>14</v>
       </c>
@@ -7794,7 +7814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="4" t="s">
         <v>17</v>
       </c>
@@ -7833,7 +7853,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="4" t="s">
         <v>18</v>
       </c>
@@ -7879,7 +7899,7 @@
         <v>0.41000000000000003</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="4" t="s">
         <v>19</v>
       </c>
@@ -7902,7 +7922,7 @@
         <v>0.11398000000000003</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A117" s="4" t="s">
         <v>20</v>
       </c>
@@ -7925,7 +7945,7 @@
         <v>0.11627600000000002</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A118" s="4" t="s">
         <v>23</v>
       </c>
@@ -7948,7 +7968,7 @@
         <v>8.6592000000000002E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A119" s="4" t="s">
         <v>22</v>
       </c>
@@ -7971,7 +7991,7 @@
         <v>5.5268000000000005E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" s="4" t="s">
         <v>24</v>
       </c>
@@ -7994,7 +8014,7 @@
         <v>2.2222000000000002E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A121" s="4" t="s">
         <v>25</v>
       </c>
@@ -8017,7 +8037,7 @@
         <v>7.2160000000000011E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A122" s="4" t="s">
         <v>26</v>
       </c>
@@ -8040,7 +8060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A123" s="4" t="s">
         <v>27</v>
       </c>
@@ -8063,7 +8083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A124" s="21" t="s">
         <v>49</v>
       </c>
@@ -8086,7 +8106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A125" s="21" t="s">
         <v>50</v>
       </c>
@@ -8109,7 +8129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A126" s="21" t="s">
         <v>51</v>
       </c>
@@ -8132,7 +8152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A127" s="21" t="s">
         <v>52</v>
       </c>
@@ -8155,7 +8175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B128">
         <f t="shared" ref="B128:G128" si="3">5*SUM(B115:B121)</f>
         <v>5.604000000000001</v>
@@ -8181,24 +8201,35 @@
         <v>2.2976400000000003</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="130" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="86" t="s">
+    <row r="129" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="130" spans="1:15" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A130" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B130" s="83" t="s">
-        <v>87</v>
-      </c>
-      <c r="C130" s="84"/>
-      <c r="D130" s="84"/>
-      <c r="E130" s="84"/>
-      <c r="F130" s="84"/>
-      <c r="G130" s="85"/>
-    </row>
-    <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="87"/>
+      <c r="B130" s="77" t="s">
+        <v>97</v>
+      </c>
+      <c r="C130" s="78"/>
+      <c r="D130" s="78"/>
+      <c r="E130" s="78"/>
+      <c r="F130" s="78"/>
+      <c r="G130" s="79"/>
+      <c r="I130" s="80" t="s">
+        <v>2</v>
+      </c>
+      <c r="J130" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="K130" s="78"/>
+      <c r="L130" s="78"/>
+      <c r="M130" s="78"/>
+      <c r="N130" s="78"/>
+      <c r="O130" s="79"/>
+    </row>
+    <row r="131" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="81"/>
       <c r="B131" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C131" s="35" t="s">
         <v>77</v>
@@ -8215,9 +8246,28 @@
       <c r="G131" s="37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="88"/>
+      <c r="I131" s="81"/>
+      <c r="J131" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="K131" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="L131" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="M131" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="N131" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="O131" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" ht="47" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A132" s="82"/>
       <c r="B132" s="55" t="s">
         <v>76</v>
       </c>
@@ -8236,8 +8286,27 @@
       <c r="G132" s="46" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I132" s="82"/>
+      <c r="J132" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="K132" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="L132" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="M132" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="N132" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="O132" s="71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A133" s="4" t="s">
         <v>11</v>
       </c>
@@ -8259,8 +8328,29 @@
       <c r="G133" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I133" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="J133" s="27">
+        <v>0</v>
+      </c>
+      <c r="K133" s="27">
+        <v>0</v>
+      </c>
+      <c r="L133" s="27">
+        <v>0</v>
+      </c>
+      <c r="M133" s="27">
+        <v>0</v>
+      </c>
+      <c r="N133" s="27">
+        <v>0</v>
+      </c>
+      <c r="O133" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A134" s="4" t="s">
         <v>14</v>
       </c>
@@ -8282,8 +8372,29 @@
       <c r="G134" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I134" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="J134" s="27">
+        <v>0</v>
+      </c>
+      <c r="K134" s="27">
+        <v>0</v>
+      </c>
+      <c r="L134" s="27">
+        <v>0</v>
+      </c>
+      <c r="M134" s="27">
+        <v>0</v>
+      </c>
+      <c r="N134" s="27">
+        <v>0</v>
+      </c>
+      <c r="O134" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A135" s="4" t="s">
         <v>17</v>
       </c>
@@ -8305,8 +8416,29 @@
       <c r="G135" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I135" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="J135" s="27">
+        <v>0</v>
+      </c>
+      <c r="K135" s="27">
+        <v>0</v>
+      </c>
+      <c r="L135" s="27">
+        <v>0</v>
+      </c>
+      <c r="M135" s="27">
+        <v>0</v>
+      </c>
+      <c r="N135" s="27">
+        <v>0</v>
+      </c>
+      <c r="O135" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A136" s="4" t="s">
         <v>18</v>
       </c>
@@ -8328,8 +8460,35 @@
       <c r="G136" s="27">
         <v>2.8987000000000002E-2</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I136" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="J136" s="27">
+        <f>B136*0.75</f>
+        <v>5.3025000000000003E-2</v>
+      </c>
+      <c r="K136" s="27">
+        <f t="shared" ref="K136:O142" si="4">C136*0.75</f>
+        <v>5.3025000000000003E-2</v>
+      </c>
+      <c r="L136" s="27">
+        <f t="shared" si="4"/>
+        <v>5.3025000000000003E-2</v>
+      </c>
+      <c r="M136" s="27">
+        <f t="shared" si="4"/>
+        <v>3.0754500000000004E-2</v>
+      </c>
+      <c r="N136" s="27">
+        <f t="shared" si="4"/>
+        <v>3.0754500000000004E-2</v>
+      </c>
+      <c r="O136" s="27">
+        <f t="shared" si="4"/>
+        <v>2.1740250000000003E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A137" s="4" t="s">
         <v>19</v>
       </c>
@@ -8351,8 +8510,35 @@
       <c r="G137" s="27">
         <v>5.6990000000000013E-2</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I137" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="J137" s="27">
+        <f t="shared" ref="J137:J142" si="5">B137*0.75</f>
+        <v>0.10425000000000001</v>
+      </c>
+      <c r="K137" s="27">
+        <f t="shared" si="4"/>
+        <v>0.10425000000000001</v>
+      </c>
+      <c r="L137" s="27">
+        <f t="shared" si="4"/>
+        <v>0.10425000000000001</v>
+      </c>
+      <c r="M137" s="27">
+        <f t="shared" si="4"/>
+        <v>6.0465000000000005E-2</v>
+      </c>
+      <c r="N137" s="27">
+        <f t="shared" si="4"/>
+        <v>6.0465000000000005E-2</v>
+      </c>
+      <c r="O137" s="27">
+        <f t="shared" si="4"/>
+        <v>4.274250000000001E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A138" s="4" t="s">
         <v>20</v>
       </c>
@@ -8374,8 +8560,35 @@
       <c r="G138" s="27">
         <v>5.8138000000000009E-2</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I138" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="J138" s="27">
+        <f t="shared" si="5"/>
+        <v>0.10635</v>
+      </c>
+      <c r="K138" s="27">
+        <f t="shared" si="4"/>
+        <v>0.10635</v>
+      </c>
+      <c r="L138" s="27">
+        <f t="shared" si="4"/>
+        <v>0.10635</v>
+      </c>
+      <c r="M138" s="27">
+        <f t="shared" si="4"/>
+        <v>6.1683000000000009E-2</v>
+      </c>
+      <c r="N138" s="27">
+        <f t="shared" si="4"/>
+        <v>6.1683000000000009E-2</v>
+      </c>
+      <c r="O138" s="27">
+        <f t="shared" si="4"/>
+        <v>4.3603500000000003E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A139" s="4" t="s">
         <v>23</v>
       </c>
@@ -8397,8 +8610,35 @@
       <c r="G139" s="27">
         <v>4.3296000000000001E-2</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I139" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="J139" s="27">
+        <f t="shared" si="5"/>
+        <v>7.9199999999999993E-2</v>
+      </c>
+      <c r="K139" s="27">
+        <f t="shared" si="4"/>
+        <v>7.9199999999999993E-2</v>
+      </c>
+      <c r="L139" s="27">
+        <f t="shared" si="4"/>
+        <v>7.9199999999999993E-2</v>
+      </c>
+      <c r="M139" s="27">
+        <f t="shared" si="4"/>
+        <v>4.5936000000000005E-2</v>
+      </c>
+      <c r="N139" s="27">
+        <f t="shared" si="4"/>
+        <v>4.5936000000000005E-2</v>
+      </c>
+      <c r="O139" s="27">
+        <f t="shared" si="4"/>
+        <v>3.2472000000000001E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A140" s="4" t="s">
         <v>22</v>
       </c>
@@ -8420,8 +8660,35 @@
       <c r="G140" s="27">
         <v>2.7634000000000002E-2</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I140" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="J140" s="27">
+        <f t="shared" si="5"/>
+        <v>5.0549999999999998E-2</v>
+      </c>
+      <c r="K140" s="27">
+        <f t="shared" si="4"/>
+        <v>5.0549999999999998E-2</v>
+      </c>
+      <c r="L140" s="27">
+        <f t="shared" si="4"/>
+        <v>5.0549999999999998E-2</v>
+      </c>
+      <c r="M140" s="27">
+        <f t="shared" si="4"/>
+        <v>2.9319000000000005E-2</v>
+      </c>
+      <c r="N140" s="27">
+        <f t="shared" si="4"/>
+        <v>2.9319000000000005E-2</v>
+      </c>
+      <c r="O140" s="27">
+        <f t="shared" si="4"/>
+        <v>2.0725500000000001E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A141" s="4" t="s">
         <v>24</v>
       </c>
@@ -8443,8 +8710,35 @@
       <c r="G141" s="27">
         <v>1.1111000000000001E-2</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I141" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="J141" s="27">
+        <f t="shared" si="5"/>
+        <v>2.0325000000000003E-2</v>
+      </c>
+      <c r="K141" s="27">
+        <f t="shared" si="4"/>
+        <v>2.0325000000000003E-2</v>
+      </c>
+      <c r="L141" s="27">
+        <f t="shared" si="4"/>
+        <v>2.0325000000000003E-2</v>
+      </c>
+      <c r="M141" s="27">
+        <f t="shared" si="4"/>
+        <v>1.1788500000000002E-2</v>
+      </c>
+      <c r="N141" s="27">
+        <f t="shared" si="4"/>
+        <v>1.1788500000000002E-2</v>
+      </c>
+      <c r="O141" s="27">
+        <f t="shared" si="4"/>
+        <v>8.3332500000000004E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A142" s="4" t="s">
         <v>25</v>
       </c>
@@ -8466,8 +8760,35 @@
       <c r="G142" s="27">
         <v>3.6080000000000005E-3</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I142" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="J142" s="27">
+        <f t="shared" si="5"/>
+        <v>6.6E-3</v>
+      </c>
+      <c r="K142" s="27">
+        <f t="shared" si="4"/>
+        <v>6.6E-3</v>
+      </c>
+      <c r="L142" s="27">
+        <f t="shared" si="4"/>
+        <v>6.6E-3</v>
+      </c>
+      <c r="M142" s="27">
+        <f t="shared" si="4"/>
+        <v>3.8280000000000007E-3</v>
+      </c>
+      <c r="N142" s="27">
+        <f t="shared" si="4"/>
+        <v>3.8280000000000007E-3</v>
+      </c>
+      <c r="O142" s="27">
+        <f t="shared" si="4"/>
+        <v>2.7060000000000005E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A143" s="4" t="s">
         <v>26</v>
       </c>
@@ -8489,8 +8810,29 @@
       <c r="G143" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I143" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="J143" s="27">
+        <v>0</v>
+      </c>
+      <c r="K143" s="27">
+        <v>0</v>
+      </c>
+      <c r="L143" s="27">
+        <v>0</v>
+      </c>
+      <c r="M143" s="27">
+        <v>0</v>
+      </c>
+      <c r="N143" s="27">
+        <v>0</v>
+      </c>
+      <c r="O143" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A144" s="4" t="s">
         <v>27</v>
       </c>
@@ -8512,8 +8854,29 @@
       <c r="G144" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I144" s="72" t="s">
+        <v>27</v>
+      </c>
+      <c r="J144" s="27">
+        <v>0</v>
+      </c>
+      <c r="K144" s="27">
+        <v>0</v>
+      </c>
+      <c r="L144" s="27">
+        <v>0</v>
+      </c>
+      <c r="M144" s="27">
+        <v>0</v>
+      </c>
+      <c r="N144" s="27">
+        <v>0</v>
+      </c>
+      <c r="O144" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A145" s="21" t="s">
         <v>49</v>
       </c>
@@ -8535,8 +8898,29 @@
       <c r="G145" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I145" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="J145" s="27">
+        <v>0</v>
+      </c>
+      <c r="K145" s="27">
+        <v>0</v>
+      </c>
+      <c r="L145" s="27">
+        <v>0</v>
+      </c>
+      <c r="M145" s="27">
+        <v>0</v>
+      </c>
+      <c r="N145" s="27">
+        <v>0</v>
+      </c>
+      <c r="O145" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A146" s="21" t="s">
         <v>50</v>
       </c>
@@ -8558,8 +8942,29 @@
       <c r="G146" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I146" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="J146" s="27">
+        <v>0</v>
+      </c>
+      <c r="K146" s="27">
+        <v>0</v>
+      </c>
+      <c r="L146" s="27">
+        <v>0</v>
+      </c>
+      <c r="M146" s="27">
+        <v>0</v>
+      </c>
+      <c r="N146" s="27">
+        <v>0</v>
+      </c>
+      <c r="O146" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A147" s="21" t="s">
         <v>51</v>
       </c>
@@ -8581,8 +8986,29 @@
       <c r="G147" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I147" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="J147" s="27">
+        <v>0</v>
+      </c>
+      <c r="K147" s="27">
+        <v>0</v>
+      </c>
+      <c r="L147" s="27">
+        <v>0</v>
+      </c>
+      <c r="M147" s="27">
+        <v>0</v>
+      </c>
+      <c r="N147" s="27">
+        <v>0</v>
+      </c>
+      <c r="O147" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A148" s="21" t="s">
         <v>52</v>
       </c>
@@ -8604,36 +9030,81 @@
       <c r="G148" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I148" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J148" s="27">
+        <v>0</v>
+      </c>
+      <c r="K148" s="27">
+        <v>0</v>
+      </c>
+      <c r="L148" s="27">
+        <v>0</v>
+      </c>
+      <c r="M148" s="27">
+        <v>0</v>
+      </c>
+      <c r="N148" s="27">
+        <v>0</v>
+      </c>
+      <c r="O148" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B149">
-        <f t="shared" ref="B149:G149" si="4">5*SUM(B133:B148)</f>
+        <f t="shared" ref="B149:G149" si="6">5*SUM(B133:B148)</f>
         <v>2.8020000000000005</v>
       </c>
       <c r="C149">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.8020000000000005</v>
       </c>
       <c r="D149">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.8020000000000005</v>
       </c>
       <c r="E149">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.6251600000000002</v>
       </c>
       <c r="F149">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.6251600000000002</v>
       </c>
       <c r="G149">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.1488200000000002</v>
       </c>
-    </row>
-    <row r="155" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J149">
+        <f t="shared" ref="J149:O149" si="7">5*SUM(J133:J148)</f>
+        <v>2.1014999999999997</v>
+      </c>
+      <c r="K149">
+        <f t="shared" si="7"/>
+        <v>2.1014999999999997</v>
+      </c>
+      <c r="L149">
+        <f t="shared" si="7"/>
+        <v>2.1014999999999997</v>
+      </c>
+      <c r="M149">
+        <f t="shared" si="7"/>
+        <v>1.2188700000000003</v>
+      </c>
+      <c r="N149">
+        <f t="shared" si="7"/>
+        <v>1.2188700000000003</v>
+      </c>
+      <c r="O149">
+        <f t="shared" si="7"/>
+        <v>0.86161500000000013</v>
+      </c>
+    </row>
+    <row r="155" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A155" s="49" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B155" s="50"/>
       <c r="C155" s="50"/>
@@ -8658,7 +9129,7 @@
       <c r="V155" s="50"/>
       <c r="W155" s="50"/>
     </row>
-    <row r="156" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A156" s="51" t="s">
         <v>69</v>
       </c>
@@ -8685,9 +9156,9 @@
       <c r="V156" s="50"/>
       <c r="W156" s="50"/>
     </row>
-    <row r="157" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A157" s="49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B157" s="50"/>
       <c r="C157" s="50"/>
@@ -8712,22 +9183,22 @@
       <c r="V157" s="50"/>
       <c r="W157" s="50"/>
     </row>
-    <row r="158" spans="1:23" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:23" ht="31" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A158" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B158" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="C158" s="75"/>
-      <c r="D158" s="76"/>
-      <c r="E158" s="74" t="s">
+      <c r="B158" s="94" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" s="95"/>
+      <c r="D158" s="96"/>
+      <c r="E158" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="F158" s="75"/>
-      <c r="G158" s="76"/>
-    </row>
-    <row r="159" spans="1:23" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F158" s="95"/>
+      <c r="G158" s="96"/>
+    </row>
+    <row r="159" spans="1:23" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A159" s="6"/>
       <c r="B159" s="7" t="s">
         <v>6</v>
@@ -8748,20 +9219,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A160" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B160" s="40">
-        <f t="shared" ref="B160:G161" si="5">10^-5</f>
+        <f t="shared" ref="B160:G161" si="8">10^-5</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C160" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D160" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E160" s="40">
@@ -8769,11 +9240,11 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F160" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="G160" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J160">
@@ -8781,56 +9252,56 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="K160">
-        <f t="shared" ref="K160:L175" si="6">C160*C54</f>
+        <f t="shared" ref="K160:L175" si="9">C160*C54</f>
         <v>0</v>
       </c>
       <c r="L160">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A161" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B161" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C161" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D161" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E161" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F161" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="G161" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J161">
-        <f t="shared" ref="J161:J175" si="7">B161*B55</f>
+        <f t="shared" ref="J161:J175" si="10">B161*B55</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="K161">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L161">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A162" s="4" t="s">
         <v>17</v>
       </c>
@@ -8853,15 +9324,15 @@
         <v>1.2</v>
       </c>
       <c r="J162">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.176E-2</v>
       </c>
       <c r="K162">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.8E-3</v>
       </c>
       <c r="L162">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>6.0000000000000218E-3</v>
       </c>
       <c r="M162">
@@ -8873,7 +9344,7 @@
         <v>51.124744376278059</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A163" s="4" t="s">
         <v>18</v>
       </c>
@@ -8896,27 +9367,27 @@
         <v>6.5</v>
       </c>
       <c r="J163">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.33787878787878783</v>
       </c>
       <c r="K163">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.040909090909091</v>
       </c>
       <c r="L163">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.58030303030303021</v>
       </c>
       <c r="M163">
-        <f t="shared" ref="M163:M175" si="8">SUM(J163:L163)</f>
+        <f t="shared" ref="M163:M175" si="11">SUM(J163:L163)</f>
         <v>1.959090909090909</v>
       </c>
       <c r="N163">
-        <f t="shared" ref="N163:N175" si="9">1/M163</f>
+        <f t="shared" ref="N163:N175" si="12">1/M163</f>
         <v>0.51044083526682138</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A164" s="4" t="s">
         <v>19</v>
       </c>
@@ -8939,27 +9410,27 @@
         <v>10</v>
       </c>
       <c r="J164">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.33193277310924363</v>
       </c>
       <c r="K164">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.1274509803921566</v>
       </c>
       <c r="L164">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.65546218487394958</v>
       </c>
       <c r="M164">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.1148459383753497</v>
       </c>
       <c r="N164">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.47284768211920541</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A165" s="4" t="s">
         <v>20</v>
       </c>
@@ -8982,27 +9453,27 @@
         <v>5.333333333333333</v>
       </c>
       <c r="J165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.39310344827586208</v>
       </c>
       <c r="K165">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.0551724137931036</v>
       </c>
       <c r="L165">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.54482758620689653</v>
       </c>
       <c r="M165">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.9931034482758623</v>
       </c>
       <c r="N165">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.50173010380622829</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A166" s="4" t="s">
         <v>23</v>
       </c>
@@ -9025,27 +9496,27 @@
         <v>1</v>
       </c>
       <c r="J166">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.46610169491525422</v>
       </c>
       <c r="K166">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.84745762711864414</v>
       </c>
       <c r="L166">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.3135593220338983</v>
       </c>
       <c r="M166">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.6271186440677967</v>
       </c>
       <c r="N166">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.61458333333333326</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A167" s="4" t="s">
         <v>22</v>
       </c>
@@ -9068,27 +9539,27 @@
         <v>9</v>
       </c>
       <c r="J167">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.59655172413793101</v>
       </c>
       <c r="K167">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.48965517241379303</v>
       </c>
       <c r="L167">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.19310344827586207</v>
       </c>
       <c r="M167">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.279310344827586</v>
       </c>
       <c r="N167">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.78167115902964968</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A168" s="4" t="s">
         <v>24</v>
       </c>
@@ -9111,27 +9582,27 @@
         <v>1</v>
       </c>
       <c r="J168">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.68881118881118875</v>
       </c>
       <c r="K168">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.40559440559440557</v>
       </c>
       <c r="L168">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.10839160839160839</v>
       </c>
       <c r="M168">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.2027972027972027</v>
       </c>
       <c r="N168">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.83139534883720934</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A169" s="4" t="s">
         <v>25</v>
       </c>
@@ -9154,27 +9625,27 @@
         <v>1</v>
       </c>
       <c r="J169">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K169">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L169">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1E-3</v>
       </c>
       <c r="M169">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A170" s="4" t="s">
         <v>26</v>
       </c>
@@ -9197,27 +9668,27 @@
         <v>1</v>
       </c>
       <c r="J170">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K170">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L170">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1E-3</v>
       </c>
       <c r="M170">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N170">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A171" s="4" t="s">
         <v>27</v>
       </c>
@@ -9240,27 +9711,27 @@
         <v>1</v>
       </c>
       <c r="J171">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K171">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L171">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1E-3</v>
       </c>
       <c r="M171">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N171">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A172" s="21" t="s">
         <v>49</v>
       </c>
@@ -9283,27 +9754,27 @@
         <v>1</v>
       </c>
       <c r="J172">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K172">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L172">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1E-3</v>
       </c>
       <c r="M172">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N172">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A173" s="21" t="s">
         <v>50</v>
       </c>
@@ -9326,27 +9797,27 @@
         <v>1</v>
       </c>
       <c r="J173">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K173">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L173">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1E-3</v>
       </c>
       <c r="M173">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N173">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A174" s="21" t="s">
         <v>51</v>
       </c>
@@ -9369,27 +9840,27 @@
         <v>1</v>
       </c>
       <c r="J174">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K174">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L174">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1E-3</v>
       </c>
       <c r="M174">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N174">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A175" s="21" t="s">
         <v>52</v>
       </c>
@@ -9416,27 +9887,27 @@
         <v>1.8866801277495602</v>
       </c>
       <c r="J175">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K175">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L175">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1E-3</v>
       </c>
       <c r="M175">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N175">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>37</v>
       </c>
@@ -9445,12 +9916,12 @@
         <v>4.4390802606579047</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A180" s="10"/>
     </row>
-    <row r="182" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A182" s="49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B182" s="50"/>
       <c r="C182" s="50"/>
@@ -9475,14 +9946,14 @@
       <c r="V182" s="50"/>
       <c r="W182" s="50"/>
     </row>
-    <row r="183" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="77" t="s">
-        <v>92</v>
-      </c>
-      <c r="B183" s="77"/>
-      <c r="C183" s="77"/>
-    </row>
-    <row r="184" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A183" s="97" t="s">
+        <v>90</v>
+      </c>
+      <c r="B183" s="97"/>
+      <c r="C183" s="97"/>
+    </row>
+    <row r="184" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A184" s="1" t="s">
         <v>29</v>
       </c>
@@ -9493,7 +9964,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A185" s="15">
         <v>1985</v>
       </c>
@@ -9504,7 +9975,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="186" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A186" s="15">
         <v>1990</v>
       </c>
@@ -9515,7 +9986,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A187" s="15">
         <v>2000</v>
       </c>
@@ -9526,9 +9997,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="194" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A194" s="49" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B194" s="50"/>
       <c r="C194" s="50"/>
@@ -9553,40 +10024,40 @@
       <c r="V194" s="50"/>
       <c r="W194" s="50"/>
     </row>
-    <row r="195" spans="1:23" s="52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A195" s="78" t="s">
-        <v>93</v>
-      </c>
-      <c r="B195" s="78"/>
-      <c r="C195" s="78"/>
-      <c r="D195" s="78"/>
-      <c r="E195" s="78"/>
-      <c r="F195" s="78"/>
-    </row>
-    <row r="196" spans="1:23" s="52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A196" s="79" t="s">
-        <v>94</v>
-      </c>
-      <c r="B196" s="79"/>
-      <c r="C196" s="79"/>
-      <c r="D196" s="79"/>
-      <c r="E196" s="79"/>
-      <c r="F196" s="79"/>
-    </row>
-    <row r="197" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A197" s="71" t="s">
+    <row r="195" spans="1:23" s="52" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A195" s="85" t="s">
+        <v>91</v>
+      </c>
+      <c r="B195" s="85"/>
+      <c r="C195" s="85"/>
+      <c r="D195" s="85"/>
+      <c r="E195" s="85"/>
+      <c r="F195" s="85"/>
+    </row>
+    <row r="196" spans="1:23" s="52" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A196" s="98" t="s">
+        <v>92</v>
+      </c>
+      <c r="B196" s="98"/>
+      <c r="C196" s="98"/>
+      <c r="D196" s="98"/>
+      <c r="E196" s="98"/>
+      <c r="F196" s="98"/>
+    </row>
+    <row r="197" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A197" s="91" t="s">
         <v>53</v>
       </c>
       <c r="B197" s="59"/>
       <c r="C197" s="59"/>
-      <c r="D197" s="71" t="s">
+      <c r="D197" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="E197" s="71"/>
-      <c r="F197" s="71"/>
-    </row>
-    <row r="198" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="71"/>
+      <c r="E197" s="91"/>
+      <c r="F197" s="91"/>
+    </row>
+    <row r="198" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A198" s="91"/>
       <c r="B198" s="59"/>
       <c r="C198" s="60" t="s">
         <v>54</v>
@@ -9605,7 +10076,7 @@
         <v>125.22857142857143</v>
       </c>
     </row>
-    <row r="199" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A199" s="61" t="s">
         <v>31</v>
       </c>
@@ -9625,15 +10096,15 @@
         <v>0</v>
       </c>
       <c r="I199">
-        <f t="shared" ref="I199:J214" si="10">E199*C54</f>
+        <f t="shared" ref="I199:J214" si="13">E199*C54</f>
         <v>0</v>
       </c>
       <c r="J199">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A200" s="61" t="s">
         <v>30</v>
       </c>
@@ -9649,19 +10120,19 @@
         <v>0</v>
       </c>
       <c r="H200">
-        <f t="shared" ref="H200:H214" si="11">D200*B55</f>
+        <f t="shared" ref="H200:H214" si="14">D200*B55</f>
         <v>0</v>
       </c>
       <c r="I200">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J200">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A201" s="61" t="s">
         <v>39</v>
       </c>
@@ -9682,15 +10153,15 @@
         <v>1.1232</v>
       </c>
       <c r="H201">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>3.0576000000000003</v>
       </c>
       <c r="I201">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2.8079999999999997E-2</v>
       </c>
       <c r="J201">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>5.6160000000000203E-3</v>
       </c>
       <c r="K201">
@@ -9698,7 +10169,7 @@
         <v>3.0912960000000003</v>
       </c>
     </row>
-    <row r="202" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A202" s="61" t="s">
         <v>40</v>
       </c>
@@ -9719,23 +10190,23 @@
         <v>5.6159999999999997</v>
       </c>
       <c r="H202">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>7.9418181818181814</v>
       </c>
       <c r="I202">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>3.814909090909091</v>
       </c>
       <c r="J202">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.46799999999999986</v>
       </c>
       <c r="K202">
-        <f t="shared" ref="K202:K214" si="12">SUM(H202:J202)</f>
+        <f t="shared" ref="K202:K214" si="15">SUM(H202:J202)</f>
         <v>12.224727272727272</v>
       </c>
     </row>
-    <row r="203" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A203" s="61" t="s">
         <v>41</v>
       </c>
@@ -9758,23 +10229,23 @@
         <v>22.463999999999999</v>
       </c>
       <c r="H203">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>29.452100840336133</v>
       </c>
       <c r="I203">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>16.570084033613444</v>
       </c>
       <c r="J203">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1.9191932773109244</v>
       </c>
       <c r="K203">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>47.941378151260501</v>
       </c>
     </row>
-    <row r="204" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A204" s="61" t="s">
         <v>42</v>
       </c>
@@ -9795,23 +10266,23 @@
         <v>56.16</v>
       </c>
       <c r="H204">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>79.613793103448273</v>
       </c>
       <c r="I204">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>38.515862068965518</v>
       </c>
       <c r="J204">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4.38951724137931</v>
       </c>
       <c r="K204">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>122.5191724137931</v>
       </c>
     </row>
-    <row r="205" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A205" s="61" t="s">
         <v>43</v>
       </c>
@@ -9819,40 +10290,40 @@
         <v>10</v>
       </c>
       <c r="C205" s="59">
-        <f t="shared" ref="C205:C214" si="13">EXP(LN(0.5)*B204/10)</f>
+        <f t="shared" ref="C205:C214" si="16">EXP(LN(0.5)*B204/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D205" s="63">
-        <f t="shared" ref="D205:D210" si="14">$D$204*C205</f>
+        <f t="shared" ref="D205:D210" si="17">$D$204*C205</f>
         <v>110.30865786510142</v>
       </c>
       <c r="E205" s="63">
-        <f t="shared" ref="E205:E210" si="15">$E$204*C205</f>
+        <f t="shared" ref="E205:E210" si="18">$E$204*C205</f>
         <v>66.185194719060846</v>
       </c>
       <c r="F205" s="63">
-        <f t="shared" ref="F205:F210" si="16">$F$204*C205</f>
+        <f t="shared" ref="F205:F210" si="19">$F$204*C205</f>
         <v>39.711116831436506</v>
       </c>
       <c r="H205">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>66.683764924100856</v>
       </c>
       <c r="I205">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>22.62262305369029</v>
       </c>
       <c r="J205">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2.1313876265460272</v>
       </c>
       <c r="K205">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>91.437775604337176</v>
       </c>
       <c r="M205" s="52"/>
     </row>
-    <row r="206" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A206" s="61" t="s">
         <v>44</v>
       </c>
@@ -9860,42 +10331,42 @@
         <v>15</v>
       </c>
       <c r="C206" s="59">
+        <f t="shared" si="16"/>
+        <v>0.5</v>
+      </c>
+      <c r="D206" s="63">
+        <f t="shared" si="17"/>
+        <v>78</v>
+      </c>
+      <c r="E206" s="63">
+        <f t="shared" si="18"/>
+        <v>46.8</v>
+      </c>
+      <c r="F206" s="63">
+        <f t="shared" si="19"/>
+        <v>28.08</v>
+      </c>
+      <c r="H206">
+        <f t="shared" si="14"/>
+        <v>59.710344827586205</v>
+      </c>
+      <c r="I206">
         <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
-      <c r="D206" s="63">
-        <f t="shared" si="14"/>
-        <v>78</v>
-      </c>
-      <c r="E206" s="63">
+        <v>9.5213793103448268</v>
+      </c>
+      <c r="J206">
+        <f t="shared" si="13"/>
+        <v>0.87144827586206886</v>
+      </c>
+      <c r="K206">
         <f t="shared" si="15"/>
-        <v>46.8</v>
-      </c>
-      <c r="F206" s="63">
-        <f t="shared" si="16"/>
-        <v>28.08</v>
-      </c>
-      <c r="H206">
-        <f t="shared" si="11"/>
-        <v>59.710344827586205</v>
-      </c>
-      <c r="I206">
-        <f t="shared" si="10"/>
-        <v>9.5213793103448268</v>
-      </c>
-      <c r="J206">
-        <f t="shared" si="10"/>
-        <v>0.87144827586206886</v>
-      </c>
-      <c r="K206">
-        <f t="shared" si="12"/>
         <v>70.103172413793089</v>
       </c>
       <c r="N206" s="52"/>
       <c r="O206" s="52"/>
       <c r="P206" s="52"/>
     </row>
-    <row r="207" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A207" s="61" t="s">
         <v>45</v>
       </c>
@@ -9903,39 +10374,39 @@
         <v>20</v>
       </c>
       <c r="C207" s="59">
+        <f t="shared" si="16"/>
+        <v>0.35355339059327379</v>
+      </c>
+      <c r="D207" s="63">
+        <f t="shared" si="17"/>
+        <v>55.154328932550712</v>
+      </c>
+      <c r="E207" s="63">
+        <f t="shared" si="18"/>
+        <v>33.092597359530423</v>
+      </c>
+      <c r="F207" s="63">
+        <f t="shared" si="19"/>
+        <v>19.855558415718253</v>
+      </c>
+      <c r="H207">
+        <f t="shared" si="14"/>
+        <v>45.126269126632394</v>
+      </c>
+      <c r="I207">
         <f t="shared" si="13"/>
-        <v>0.35355339059327379</v>
-      </c>
-      <c r="D207" s="63">
-        <f t="shared" si="14"/>
-        <v>55.154328932550712</v>
-      </c>
-      <c r="E207" s="63">
+        <v>5.5540023540470642</v>
+      </c>
+      <c r="J207">
+        <f t="shared" si="13"/>
+        <v>0.2777001177023532</v>
+      </c>
+      <c r="K207">
         <f t="shared" si="15"/>
-        <v>33.092597359530423</v>
-      </c>
-      <c r="F207" s="63">
-        <f t="shared" si="16"/>
-        <v>19.855558415718253</v>
-      </c>
-      <c r="H207">
-        <f t="shared" si="11"/>
-        <v>45.126269126632394</v>
-      </c>
-      <c r="I207">
-        <f t="shared" si="10"/>
-        <v>5.5540023540470642</v>
-      </c>
-      <c r="J207">
-        <f t="shared" si="10"/>
-        <v>0.2777001177023532</v>
-      </c>
-      <c r="K207">
-        <f t="shared" si="12"/>
         <v>50.95797159838181</v>
       </c>
     </row>
-    <row r="208" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A208" s="61" t="s">
         <v>46</v>
       </c>
@@ -9943,39 +10414,39 @@
         <v>25</v>
       </c>
       <c r="C208" s="59">
+        <f t="shared" si="16"/>
+        <v>0.25</v>
+      </c>
+      <c r="D208" s="63">
+        <f t="shared" si="17"/>
+        <v>39</v>
+      </c>
+      <c r="E208" s="63">
+        <f t="shared" si="18"/>
+        <v>23.4</v>
+      </c>
+      <c r="F208" s="63">
+        <f t="shared" si="19"/>
+        <v>14.04</v>
+      </c>
+      <c r="H208">
+        <f t="shared" si="14"/>
+        <v>33.179104477611936</v>
+      </c>
+      <c r="I208">
         <f t="shared" si="13"/>
-        <v>0.25</v>
-      </c>
-      <c r="D208" s="63">
-        <f t="shared" si="14"/>
-        <v>39</v>
-      </c>
-      <c r="E208" s="63">
+        <v>3.4691373134328458</v>
+      </c>
+      <c r="J208">
+        <f t="shared" si="13"/>
+        <v>1.4039999999999999E-2</v>
+      </c>
+      <c r="K208">
         <f t="shared" si="15"/>
-        <v>23.4</v>
-      </c>
-      <c r="F208" s="63">
-        <f t="shared" si="16"/>
-        <v>14.04</v>
-      </c>
-      <c r="H208">
-        <f t="shared" si="11"/>
-        <v>33.179104477611936</v>
-      </c>
-      <c r="I208">
-        <f t="shared" si="10"/>
-        <v>3.4691373134328458</v>
-      </c>
-      <c r="J208">
-        <f t="shared" si="10"/>
-        <v>1.4039999999999999E-2</v>
-      </c>
-      <c r="K208">
-        <f t="shared" si="12"/>
         <v>36.662281791044784</v>
       </c>
     </row>
-    <row r="209" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A209" s="61" t="s">
         <v>47</v>
       </c>
@@ -9983,39 +10454,39 @@
         <v>30</v>
       </c>
       <c r="C209" s="59">
+        <f t="shared" si="16"/>
+        <v>0.17677669529663689</v>
+      </c>
+      <c r="D209" s="63">
+        <f t="shared" si="17"/>
+        <v>27.577164466275356</v>
+      </c>
+      <c r="E209" s="63">
+        <f t="shared" si="18"/>
+        <v>16.546298679765211</v>
+      </c>
+      <c r="F209" s="63">
+        <f t="shared" si="19"/>
+        <v>9.9277792078591265</v>
+      </c>
+      <c r="H209">
+        <f t="shared" si="14"/>
+        <v>23.461169769816344</v>
+      </c>
+      <c r="I209">
         <f t="shared" si="13"/>
-        <v>0.17677669529663689</v>
-      </c>
-      <c r="D209" s="63">
-        <f t="shared" si="14"/>
-        <v>27.577164466275356</v>
-      </c>
-      <c r="E209" s="63">
+        <v>2.4530505191956467</v>
+      </c>
+      <c r="J209">
+        <f t="shared" si="13"/>
+        <v>9.9277792078591269E-3</v>
+      </c>
+      <c r="K209">
         <f t="shared" si="15"/>
-        <v>16.546298679765211</v>
-      </c>
-      <c r="F209" s="63">
-        <f t="shared" si="16"/>
-        <v>9.9277792078591265</v>
-      </c>
-      <c r="H209">
-        <f t="shared" si="11"/>
-        <v>23.461169769816344</v>
-      </c>
-      <c r="I209">
-        <f t="shared" si="10"/>
-        <v>2.4530505191956467</v>
-      </c>
-      <c r="J209">
-        <f t="shared" si="10"/>
-        <v>9.9277792078591269E-3</v>
-      </c>
-      <c r="K209">
-        <f t="shared" si="12"/>
         <v>25.92414806821985</v>
       </c>
     </row>
-    <row r="210" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A210" s="61" t="s">
         <v>48</v>
       </c>
@@ -10023,39 +10494,39 @@
         <v>35</v>
       </c>
       <c r="C210" s="59">
+        <f t="shared" si="16"/>
+        <v>0.12500000000000003</v>
+      </c>
+      <c r="D210" s="63">
+        <f t="shared" si="17"/>
+        <v>19.500000000000004</v>
+      </c>
+      <c r="E210" s="63">
+        <f t="shared" si="18"/>
+        <v>11.700000000000001</v>
+      </c>
+      <c r="F210" s="63">
+        <f t="shared" si="19"/>
+        <v>7.0200000000000014</v>
+      </c>
+      <c r="H210">
+        <f t="shared" si="14"/>
+        <v>16.589552238805972</v>
+      </c>
+      <c r="I210">
         <f t="shared" si="13"/>
-        <v>0.12500000000000003</v>
-      </c>
-      <c r="D210" s="63">
-        <f t="shared" si="14"/>
-        <v>19.500000000000004</v>
-      </c>
-      <c r="E210" s="63">
+        <v>1.7345686567164231</v>
+      </c>
+      <c r="J210">
+        <f t="shared" si="13"/>
+        <v>7.0200000000000011E-3</v>
+      </c>
+      <c r="K210">
         <f t="shared" si="15"/>
-        <v>11.700000000000001</v>
-      </c>
-      <c r="F210" s="63">
-        <f t="shared" si="16"/>
-        <v>7.0200000000000014</v>
-      </c>
-      <c r="H210">
-        <f t="shared" si="11"/>
-        <v>16.589552238805972</v>
-      </c>
-      <c r="I210">
-        <f t="shared" si="10"/>
-        <v>1.7345686567164231</v>
-      </c>
-      <c r="J210">
-        <f t="shared" si="10"/>
-        <v>7.0200000000000011E-3</v>
-      </c>
-      <c r="K210">
-        <f t="shared" si="12"/>
         <v>18.331140895522395</v>
       </c>
     </row>
-    <row r="211" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A211" s="61" t="s">
         <v>49</v>
       </c>
@@ -10079,23 +10550,23 @@
         <v>4.9638896039295632</v>
       </c>
       <c r="H211">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>11.730584884908172</v>
       </c>
       <c r="I211">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1.2265252595978233</v>
       </c>
       <c r="J211">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4.9638896039295635E-3</v>
       </c>
       <c r="K211">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>12.962074034109925</v>
       </c>
     </row>
-    <row r="212" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A212" s="61" t="s">
         <v>50</v>
       </c>
@@ -10103,7 +10574,7 @@
         <v>45</v>
       </c>
       <c r="C212" s="59">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>6.25E-2</v>
       </c>
       <c r="D212" s="63">
@@ -10119,23 +10590,23 @@
         <v>3.51</v>
       </c>
       <c r="H212">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>8.2947761194029841</v>
       </c>
       <c r="I212">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.86728432835821145</v>
       </c>
       <c r="J212">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>3.5099999999999997E-3</v>
       </c>
       <c r="K212">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>9.1655704477611959</v>
       </c>
     </row>
-    <row r="213" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A213" s="61" t="s">
         <v>51</v>
       </c>
@@ -10143,7 +10614,7 @@
         <v>50</v>
       </c>
       <c r="C213" s="59">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>4.4194173824159223E-2</v>
       </c>
       <c r="D213" s="63">
@@ -10159,23 +10630,23 @@
         <v>2.4819448019647816</v>
       </c>
       <c r="H213">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>5.865292442454086</v>
       </c>
       <c r="I213">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.61326262979891166</v>
       </c>
       <c r="J213">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2.4819448019647817E-3</v>
       </c>
       <c r="K213">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>6.4810370170549625</v>
       </c>
     </row>
-    <row r="214" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A214" s="61" t="s">
         <v>52</v>
       </c>
@@ -10183,7 +10654,7 @@
         <v>55</v>
       </c>
       <c r="C214" s="59">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>3.125E-2</v>
       </c>
       <c r="D214" s="63">
@@ -10199,23 +10670,23 @@
         <v>1.7549999999999999</v>
       </c>
       <c r="H214">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>4.147388059701492</v>
       </c>
       <c r="I214">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.43364216417910573</v>
       </c>
       <c r="J214">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1.7549999999999998E-3</v>
       </c>
       <c r="K214">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>4.5827852238805979</v>
       </c>
     </row>
-    <row r="215" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A215" s="59"/>
       <c r="B215" s="64"/>
       <c r="C215" s="59"/>
@@ -10231,30 +10702,30 @@
         <v>0.7014161956630891</v>
       </c>
     </row>
-    <row r="216" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A216" s="72" t="s">
-        <v>95</v>
-      </c>
-      <c r="B216" s="72"/>
-      <c r="C216" s="72"/>
-      <c r="D216" s="72"/>
-      <c r="E216" s="72"/>
-      <c r="F216" s="72"/>
-    </row>
-    <row r="217" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A217" s="73" t="s">
+    <row r="216" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A216" s="92" t="s">
+        <v>93</v>
+      </c>
+      <c r="B216" s="92"/>
+      <c r="C216" s="92"/>
+      <c r="D216" s="92"/>
+      <c r="E216" s="92"/>
+      <c r="F216" s="92"/>
+    </row>
+    <row r="217" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A217" s="93" t="s">
         <v>2</v>
       </c>
       <c r="B217" s="59"/>
       <c r="C217" s="59"/>
-      <c r="D217" s="71" t="s">
+      <c r="D217" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="E217" s="71"/>
-      <c r="F217" s="71"/>
-    </row>
-    <row r="218" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A218" s="73"/>
+      <c r="E217" s="91"/>
+      <c r="F217" s="91"/>
+    </row>
+    <row r="218" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A218" s="93"/>
       <c r="B218" s="59"/>
       <c r="C218" s="60" t="s">
         <v>54</v>
@@ -10269,7 +10740,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="219" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A219" s="61" t="s">
         <v>31</v>
       </c>
@@ -10285,7 +10756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A220" s="61" t="s">
         <v>30</v>
       </c>
@@ -10301,7 +10772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A221" s="61" t="s">
         <v>39</v>
       </c>
@@ -10322,7 +10793,7 @@
         <v>2.8079999999999998</v>
       </c>
     </row>
-    <row r="222" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A222" s="61" t="s">
         <v>40</v>
       </c>
@@ -10343,7 +10814,7 @@
         <v>5.6159999999999997</v>
       </c>
     </row>
-    <row r="223" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A223" s="61" t="s">
         <v>41</v>
       </c>
@@ -10366,7 +10837,7 @@
         <v>22.463999999999999</v>
       </c>
     </row>
-    <row r="224" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A224" s="61" t="s">
         <v>42</v>
       </c>
@@ -10387,7 +10858,7 @@
         <v>56.16</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A225" s="61" t="s">
         <v>43</v>
       </c>
@@ -10395,7 +10866,7 @@
         <v>10</v>
       </c>
       <c r="C225" s="59">
-        <f t="shared" ref="C225:C234" si="17">EXP(LN(0.5)*B224/10)</f>
+        <f t="shared" ref="C225:C234" si="20">EXP(LN(0.5)*B224/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D225" s="62">
@@ -10411,7 +10882,7 @@
         <v>39.711116831436506</v>
       </c>
     </row>
-    <row r="226" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A226" s="61" t="s">
         <v>44</v>
       </c>
@@ -10419,23 +10890,23 @@
         <v>15</v>
       </c>
       <c r="C226" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
       <c r="D226" s="62">
-        <f t="shared" ref="D226:D232" si="18">$D$224*C226</f>
+        <f t="shared" ref="D226:D232" si="21">$D$224*C226</f>
         <v>78</v>
       </c>
       <c r="E226" s="62">
-        <f t="shared" ref="E226:E232" si="19">$E$224*C226</f>
+        <f t="shared" ref="E226:E232" si="22">$E$224*C226</f>
         <v>46.8</v>
       </c>
       <c r="F226" s="62">
-        <f t="shared" ref="F226:F232" si="20">$F$224*C226</f>
+        <f t="shared" ref="F226:F232" si="23">$F$224*C226</f>
         <v>28.08</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A227" s="61" t="s">
         <v>45</v>
       </c>
@@ -10443,23 +10914,23 @@
         <v>20</v>
       </c>
       <c r="C227" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0.35355339059327379</v>
       </c>
       <c r="D227" s="62">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>55.154328932550712</v>
       </c>
       <c r="E227" s="62">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>33.092597359530423</v>
       </c>
       <c r="F227" s="62">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>19.855558415718253</v>
       </c>
     </row>
-    <row r="228" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A228" s="61" t="s">
         <v>46</v>
       </c>
@@ -10467,23 +10938,23 @@
         <v>25</v>
       </c>
       <c r="C228" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0.25</v>
       </c>
       <c r="D228" s="62">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>39</v>
       </c>
       <c r="E228" s="62">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>23.4</v>
       </c>
       <c r="F228" s="62">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>14.04</v>
       </c>
     </row>
-    <row r="229" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A229" s="61" t="s">
         <v>47</v>
       </c>
@@ -10491,23 +10962,23 @@
         <v>30</v>
       </c>
       <c r="C229" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0.17677669529663689</v>
       </c>
       <c r="D229" s="62">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>27.577164466275356</v>
       </c>
       <c r="E229" s="62">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>16.546298679765211</v>
       </c>
       <c r="F229" s="62">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>9.9277792078591265</v>
       </c>
     </row>
-    <row r="230" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A230" s="61" t="s">
         <v>48</v>
       </c>
@@ -10515,23 +10986,23 @@
         <v>35</v>
       </c>
       <c r="C230" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0.12500000000000003</v>
       </c>
       <c r="D230" s="62">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>19.500000000000004</v>
       </c>
       <c r="E230" s="62">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>11.700000000000001</v>
       </c>
       <c r="F230" s="62">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>7.0200000000000014</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A231" s="61" t="s">
         <v>49</v>
       </c>
@@ -10539,23 +11010,23 @@
         <v>40</v>
       </c>
       <c r="C231" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>8.8388347648318447E-2</v>
       </c>
       <c r="D231" s="62">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>13.788582233137678</v>
       </c>
       <c r="E231" s="62">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>8.2731493398826057</v>
       </c>
       <c r="F231" s="62">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>4.9638896039295632</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A232" s="61" t="s">
         <v>50</v>
       </c>
@@ -10563,23 +11034,23 @@
         <v>45</v>
       </c>
       <c r="C232" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>6.25E-2</v>
       </c>
       <c r="D232" s="62">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>9.75</v>
       </c>
       <c r="E232" s="62">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>5.85</v>
       </c>
       <c r="F232" s="62">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>3.51</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A233" s="61" t="s">
         <v>51</v>
       </c>
@@ -10603,7 +11074,7 @@
         <v>2.4819448019647816</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A234" s="61" t="s">
         <v>52</v>
       </c>
@@ -10611,7 +11082,7 @@
         <v>55</v>
       </c>
       <c r="C234" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>3.125E-2</v>
       </c>
       <c r="D234" s="62">
@@ -10627,7 +11098,7 @@
         <v>1.7549999999999999</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A235" s="48"/>
       <c r="B235" s="48"/>
       <c r="C235" s="58"/>
@@ -10635,9 +11106,9 @@
       <c r="E235" s="48"/>
       <c r="F235" s="48"/>
     </row>
-    <row r="236" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A236" s="57" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B236" s="52"/>
       <c r="C236" s="52"/>
@@ -10645,7 +11116,7 @@
       <c r="E236" s="48"/>
       <c r="F236" s="48"/>
     </row>
-    <row r="237" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A237" s="69" t="s">
         <v>38</v>
       </c>
@@ -10661,7 +11132,7 @@
       <c r="E237" s="48"/>
       <c r="F237" s="48"/>
     </row>
-    <row r="238" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A238" s="24" t="s">
         <v>0</v>
       </c>
@@ -10678,7 +11149,7 @@
         <v>56.16</v>
       </c>
     </row>
-    <row r="239" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A239" s="24" t="s">
         <v>1</v>
       </c>
@@ -10696,7 +11167,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
+    <mergeCell ref="I130:I132"/>
+    <mergeCell ref="J130:O130"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="A216:F216"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="B158:D158"/>
+    <mergeCell ref="E158:G158"/>
+    <mergeCell ref="A183:C183"/>
+    <mergeCell ref="A195:F195"/>
+    <mergeCell ref="A196:F196"/>
+    <mergeCell ref="D197:F197"/>
+    <mergeCell ref="D217:F217"/>
     <mergeCell ref="A109:A111"/>
     <mergeCell ref="B109:G109"/>
     <mergeCell ref="B130:G130"/>
@@ -10709,16 +11192,6 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="B81:B83"/>
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="A216:F216"/>
-    <mergeCell ref="A217:A218"/>
-    <mergeCell ref="B158:D158"/>
-    <mergeCell ref="E158:G158"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A195:F195"/>
-    <mergeCell ref="A196:F196"/>
-    <mergeCell ref="D197:F197"/>
-    <mergeCell ref="D217:F217"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add additional background mortality data to Excel doc.
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="105">
   <si>
     <t>Male</t>
   </si>
@@ -415,9 +415,6 @@
     <t>HIV-</t>
   </si>
   <si>
-    <t>Note: fertility rates changed linearly from 1995 to 2005 so that the model's population growth resembles actual population growth patterns. Fertility rate for 2005 onwards is 1/2 the fertility rate before 1995.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">HIV- </t>
     </r>
@@ -535,12 +532,37 @@
   <si>
     <t>Fertility Rate (per year) by 2020</t>
   </si>
+  <si>
+    <t>1985-1990</t>
+  </si>
+  <si>
+    <t>Roger Ying paper</t>
+  </si>
+  <si>
+    <t>males</t>
+  </si>
+  <si>
+    <t>females</t>
+  </si>
+  <si>
+    <t>UN World Population Prospects 2019</t>
+  </si>
+  <si>
+    <t>Note: fertility rates changed linearly from 1990 to 2010 so that the model's population growth resembles actual population growth patterns. Fertility rate for 2010 onwards is 1/2 the fertility rate before 1990.</t>
+  </si>
+  <si>
+    <t>&lt;--should use UNICEF data here instead?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="30" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="168" formatCode="0.00000;\-0.00000;0"/>
+    <numFmt numFmtId="169" formatCode="###;\-###;0"/>
+  </numFmts>
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -749,6 +771,24 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -1384,7 +1424,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1550,13 +1590,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1566,39 +1606,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1622,7 +1629,72 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -6077,8 +6149,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q142" sqref="Q142"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N101" sqref="N101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6176,7 +6248,7 @@
     </row>
     <row r="3" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="50"/>
@@ -6207,10 +6279,10 @@
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="84"/>
+      <c r="C4" s="93"/>
     </row>
     <row r="5" spans="1:25" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="53"/>
@@ -6447,10 +6519,10 @@
       <c r="A27" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="85" t="s">
+      <c r="B27" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="86"/>
+      <c r="C27" s="94"/>
     </row>
     <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="12"/>
@@ -6838,19 +6910,19 @@
       <c r="AE51" s="32"/>
     </row>
     <row r="52" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="90" t="s">
+      <c r="A52" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="90" t="s">
+      <c r="B52" s="98" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="90"/>
-      <c r="D52" s="90"/>
-      <c r="E52" s="90" t="s">
+      <c r="C52" s="98"/>
+      <c r="D52" s="98"/>
+      <c r="E52" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="90"/>
-      <c r="G52" s="90"/>
+      <c r="F52" s="98"/>
+      <c r="G52" s="98"/>
       <c r="X52" s="30"/>
       <c r="Y52" s="30"/>
       <c r="Z52" s="30"/>
@@ -6861,7 +6933,7 @@
       <c r="AE52" s="30"/>
     </row>
     <row r="53" spans="1:31" ht="30" x14ac:dyDescent="0.35">
-      <c r="A53" s="90"/>
+      <c r="A53" s="98"/>
       <c r="B53" s="45" t="s">
         <v>6</v>
       </c>
@@ -7394,28 +7466,58 @@
       <c r="W80" s="50"/>
       <c r="X80" s="50"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="74" t="s">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A81" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="87" t="s">
+      <c r="B81" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="87" t="s">
+      <c r="C81" s="95" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="75"/>
-      <c r="B82" s="88"/>
-      <c r="C82" s="88"/>
-    </row>
-    <row r="83" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="76"/>
-      <c r="B83" s="89"/>
-      <c r="C83" s="89"/>
-    </row>
-    <row r="84" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H81" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A82" s="90"/>
+      <c r="B82" s="96"/>
+      <c r="C82" s="96"/>
+      <c r="I82" s="102" t="s">
+        <v>98</v>
+      </c>
+      <c r="K82" t="s">
+        <v>100</v>
+      </c>
+      <c r="L82" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="91"/>
+      <c r="B83" s="97"/>
+      <c r="C83" s="97"/>
+      <c r="E83" t="s">
+        <v>99</v>
+      </c>
+      <c r="H83" s="100"/>
+      <c r="I83" s="104">
+        <v>0</v>
+      </c>
+      <c r="J83" s="104">
+        <v>1</v>
+      </c>
+      <c r="K83" s="110">
+        <v>5.1751479000000003E-2</v>
+      </c>
+      <c r="L83" s="110">
+        <v>4.2747080999999999E-2</v>
+      </c>
+      <c r="O83" s="105"/>
+      <c r="P83" s="105"/>
+    </row>
+    <row r="84" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="4" t="s">
         <v>11</v>
       </c>
@@ -7425,8 +7527,30 @@
       <c r="C84" s="13">
         <v>8.8057230624727749E-3</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E84">
+        <v>0.06</v>
+      </c>
+      <c r="F84">
+        <v>0.06</v>
+      </c>
+      <c r="H84" s="100"/>
+      <c r="I84" s="104">
+        <v>1</v>
+      </c>
+      <c r="J84" s="104">
+        <v>4</v>
+      </c>
+      <c r="K84" s="110">
+        <v>5.2241062999999997E-3</v>
+      </c>
+      <c r="L84" s="110">
+        <v>4.6946237E-3</v>
+      </c>
+      <c r="M84" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="4" t="s">
         <v>14</v>
       </c>
@@ -7436,8 +7560,30 @@
       <c r="C85" s="13">
         <v>5.2457282047517039E-4</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E85">
+        <v>5.2999999999999998E-4</v>
+      </c>
+      <c r="F85">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="H85" s="100"/>
+      <c r="I85" s="106">
+        <v>0</v>
+      </c>
+      <c r="J85" s="107">
+        <f>SUM(J83:J84)</f>
+        <v>5</v>
+      </c>
+      <c r="K85" s="108">
+        <f>SUM(K83:K84)</f>
+        <v>5.6975585300000006E-2</v>
+      </c>
+      <c r="L85" s="108">
+        <f>SUM(L83:L84)</f>
+        <v>4.7441704699999997E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="4" t="s">
         <v>17</v>
       </c>
@@ -7447,8 +7593,27 @@
       <c r="C86" s="13">
         <v>4.8877879149405545E-4</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E86">
+        <v>5.5999999999999995E-4</v>
+      </c>
+      <c r="F86">
+        <v>4.2999999999999999E-4</v>
+      </c>
+      <c r="H86" s="100"/>
+      <c r="I86" s="101">
+        <v>5</v>
+      </c>
+      <c r="J86" s="101">
+        <v>5</v>
+      </c>
+      <c r="K86" s="109">
+        <v>2.4750038999999998E-3</v>
+      </c>
+      <c r="L86" s="109">
+        <v>1.8590649E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="4" t="s">
         <v>18</v>
       </c>
@@ -7458,8 +7623,27 @@
       <c r="C87" s="13">
         <v>9.035280767087482E-4</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E87">
+        <v>1.83E-3</v>
+      </c>
+      <c r="F87">
+        <v>7.6000000000000004E-4</v>
+      </c>
+      <c r="H87" s="100"/>
+      <c r="I87" s="101">
+        <v>10</v>
+      </c>
+      <c r="J87" s="101">
+        <v>5</v>
+      </c>
+      <c r="K87" s="109">
+        <v>1.5814690000000001E-3</v>
+      </c>
+      <c r="L87" s="109">
+        <v>1.2227608999999999E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="4" t="s">
         <v>19</v>
       </c>
@@ -7469,8 +7653,27 @@
       <c r="C88" s="13">
         <v>1.6915946235478447E-3</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E88">
+        <v>3.98E-3</v>
+      </c>
+      <c r="F88">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="H88" s="100"/>
+      <c r="I88" s="101">
+        <v>15</v>
+      </c>
+      <c r="J88" s="101">
+        <v>5</v>
+      </c>
+      <c r="K88" s="109">
+        <v>2.5001934000000001E-3</v>
+      </c>
+      <c r="L88" s="109">
+        <v>1.6750273E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="4" t="s">
         <v>20</v>
       </c>
@@ -7480,8 +7683,27 @@
       <c r="C89" s="13">
         <v>2.0719480819543991E-3</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E89">
+        <v>5.1399999999999996E-3</v>
+      </c>
+      <c r="F89">
+        <v>1.83E-3</v>
+      </c>
+      <c r="H89" s="100"/>
+      <c r="I89" s="101">
+        <v>20</v>
+      </c>
+      <c r="J89" s="101">
+        <v>5</v>
+      </c>
+      <c r="K89" s="109">
+        <v>3.7640993E-3</v>
+      </c>
+      <c r="L89" s="109">
+        <v>2.3815536E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="4" t="s">
         <v>23</v>
       </c>
@@ -7491,8 +7713,27 @@
       <c r="C90" s="13">
         <v>2.4601074470881829E-3</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E90">
+        <v>6.0600000000000003E-3</v>
+      </c>
+      <c r="F90">
+        <v>2.5200000000000001E-3</v>
+      </c>
+      <c r="H90" s="100"/>
+      <c r="I90" s="101">
+        <v>25</v>
+      </c>
+      <c r="J90" s="101">
+        <v>5</v>
+      </c>
+      <c r="K90" s="109">
+        <v>4.3315932999999996E-3</v>
+      </c>
+      <c r="L90" s="109">
+        <v>3.1198295999999999E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="4" t="s">
         <v>22</v>
       </c>
@@ -7502,8 +7743,27 @@
       <c r="C91" s="13">
         <v>2.9925533571735037E-3</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E91">
+        <v>7.1500000000000001E-3</v>
+      </c>
+      <c r="F91">
+        <v>3.15E-3</v>
+      </c>
+      <c r="H91" s="100"/>
+      <c r="I91" s="101">
+        <v>30</v>
+      </c>
+      <c r="J91" s="101">
+        <v>5</v>
+      </c>
+      <c r="K91" s="109">
+        <v>5.1669517000000002E-3</v>
+      </c>
+      <c r="L91" s="109">
+        <v>3.7817176000000002E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="4" t="s">
         <v>24</v>
       </c>
@@ -7513,8 +7773,27 @@
       <c r="C92" s="13">
         <v>3.9413474052092329E-3</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E92">
+        <v>9.5200000000000007E-3</v>
+      </c>
+      <c r="F92">
+        <v>4.4799999999999996E-3</v>
+      </c>
+      <c r="H92" s="100"/>
+      <c r="I92" s="101">
+        <v>35</v>
+      </c>
+      <c r="J92" s="101">
+        <v>5</v>
+      </c>
+      <c r="K92" s="109">
+        <v>6.4414638999999996E-3</v>
+      </c>
+      <c r="L92" s="109">
+        <v>4.6448573999999998E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="4" t="s">
         <v>25</v>
       </c>
@@ -7524,8 +7803,27 @@
       <c r="C93" s="13">
         <v>5.3575989334735206E-3</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E93">
+        <v>1.1780000000000001E-2</v>
+      </c>
+      <c r="F93">
+        <v>5.7600000000000004E-3</v>
+      </c>
+      <c r="H93" s="100"/>
+      <c r="I93" s="101">
+        <v>40</v>
+      </c>
+      <c r="J93" s="101">
+        <v>5</v>
+      </c>
+      <c r="K93" s="109">
+        <v>8.0432449999999992E-3</v>
+      </c>
+      <c r="L93" s="109">
+        <v>5.6773359000000002E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="4" t="s">
         <v>26</v>
       </c>
@@ -7535,8 +7833,27 @@
       <c r="C94" s="13">
         <v>7.5410818923787939E-3</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E94">
+        <v>1.711E-2</v>
+      </c>
+      <c r="F94">
+        <v>9.6399999999999993E-3</v>
+      </c>
+      <c r="H94" s="100"/>
+      <c r="I94" s="101">
+        <v>45</v>
+      </c>
+      <c r="J94" s="101">
+        <v>5</v>
+      </c>
+      <c r="K94" s="109">
+        <v>1.0135829000000001E-2</v>
+      </c>
+      <c r="L94" s="109">
+        <v>6.6691631000000001E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="4" t="s">
         <v>27</v>
       </c>
@@ -7546,8 +7863,27 @@
       <c r="C95" s="13">
         <v>1.0540154917424747E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E95" s="52">
+        <v>2.0809999999999999E-2</v>
+      </c>
+      <c r="F95" s="52">
+        <v>1.393E-2</v>
+      </c>
+      <c r="H95" s="100"/>
+      <c r="I95" s="101">
+        <v>50</v>
+      </c>
+      <c r="J95" s="101">
+        <v>5</v>
+      </c>
+      <c r="K95" s="109">
+        <v>1.4004198000000001E-2</v>
+      </c>
+      <c r="L95" s="109">
+        <v>8.9763412999999993E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="21" t="s">
         <v>49</v>
       </c>
@@ -7556,6 +7892,21 @@
       </c>
       <c r="C96" s="13">
         <v>1.5759592316689931E-2</v>
+      </c>
+      <c r="E96" s="103"/>
+      <c r="F96" s="103"/>
+      <c r="H96" s="100"/>
+      <c r="I96" s="101">
+        <v>55</v>
+      </c>
+      <c r="J96" s="101">
+        <v>5</v>
+      </c>
+      <c r="K96" s="109">
+        <v>1.8576009000000001E-2</v>
+      </c>
+      <c r="L96" s="109">
+        <v>1.2049147E-2</v>
       </c>
     </row>
     <row r="97" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -7568,6 +7919,21 @@
       <c r="C97" s="13">
         <v>2.2837523063216215E-2</v>
       </c>
+      <c r="E97" s="103"/>
+      <c r="F97" s="103"/>
+      <c r="H97" s="100"/>
+      <c r="I97" s="101">
+        <v>60</v>
+      </c>
+      <c r="J97" s="101">
+        <v>5</v>
+      </c>
+      <c r="K97" s="109">
+        <v>2.7759598999999999E-2</v>
+      </c>
+      <c r="L97" s="109">
+        <v>1.8543285E-2</v>
+      </c>
     </row>
     <row r="98" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="21" t="s">
@@ -7579,6 +7945,21 @@
       <c r="C98" s="13">
         <v>3.3336893194863555E-2</v>
       </c>
+      <c r="E98" s="103"/>
+      <c r="F98" s="103"/>
+      <c r="H98" s="100"/>
+      <c r="I98" s="101">
+        <v>65</v>
+      </c>
+      <c r="J98" s="101">
+        <v>5</v>
+      </c>
+      <c r="K98" s="109">
+        <v>4.2779603999999999E-2</v>
+      </c>
+      <c r="L98" s="109">
+        <v>3.039122E-2</v>
+      </c>
     </row>
     <row r="99" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="21" t="s">
@@ -7590,16 +7971,57 @@
       <c r="C99" s="13">
         <v>6.1722846856347699E-2</v>
       </c>
+      <c r="E99" s="103"/>
+      <c r="F99" s="103"/>
+      <c r="H99" s="100"/>
+      <c r="I99" s="101">
+        <v>70</v>
+      </c>
+      <c r="J99" s="101">
+        <v>5</v>
+      </c>
+      <c r="K99" s="109">
+        <v>6.8473476000000005E-2</v>
+      </c>
+      <c r="L99" s="109">
+        <v>5.1704121999999998E-2</v>
+      </c>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="B100">
-        <f>5*SUM(B84:B99)</f>
-        <v>1.4052970667115117</v>
-      </c>
-      <c r="C100">
-        <f>5*SUM(C84:C99)</f>
-        <v>0.90487922420259181</v>
-      </c>
+      <c r="E100" s="99"/>
+      <c r="F100" s="99"/>
+      <c r="I100" s="101">
+        <v>75</v>
+      </c>
+      <c r="J100" s="101">
+        <v>5</v>
+      </c>
+      <c r="K100" s="109">
+        <v>0.11201527999999999</v>
+      </c>
+      <c r="L100" s="109">
+        <v>8.8066895000000006E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="I101" s="101"/>
+      <c r="J101" s="101"/>
+      <c r="K101" s="100"/>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="I102" s="101"/>
+      <c r="J102" s="101"/>
+      <c r="K102" s="100"/>
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="I103" s="101"/>
+      <c r="J103" s="101"/>
+      <c r="K103" s="100"/>
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="I104" s="101"/>
+      <c r="J104" s="101"/>
+      <c r="K104" s="100"/>
     </row>
     <row r="105" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A105" s="49" t="s">
@@ -7687,7 +8109,7 @@
     </row>
     <row r="108" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="49" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="B108" s="50"/>
       <c r="C108" s="50"/>
@@ -7714,11 +8136,11 @@
       <c r="X108" s="50"/>
     </row>
     <row r="109" spans="1:24" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="74" t="s">
+      <c r="A109" s="89" t="s">
         <v>2</v>
       </c>
       <c r="B109" s="77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C109" s="78"/>
       <c r="D109" s="78"/>
@@ -7727,7 +8149,7 @@
       <c r="G109" s="79"/>
     </row>
     <row r="110" spans="1:24" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="75"/>
+      <c r="A110" s="90"/>
       <c r="B110" s="44" t="s">
         <v>83</v>
       </c>
@@ -7748,7 +8170,7 @@
       </c>
     </row>
     <row r="111" spans="1:24" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="76"/>
+      <c r="A111" s="91"/>
       <c r="B111" s="46" t="s">
         <v>76</v>
       </c>
@@ -8203,22 +8625,22 @@
     </row>
     <row r="129" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="130" spans="1:15" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="80" t="s">
+      <c r="A130" s="74" t="s">
         <v>2</v>
       </c>
       <c r="B130" s="77" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C130" s="78"/>
       <c r="D130" s="78"/>
       <c r="E130" s="78"/>
       <c r="F130" s="78"/>
       <c r="G130" s="79"/>
-      <c r="I130" s="80" t="s">
+      <c r="I130" s="74" t="s">
         <v>2</v>
       </c>
       <c r="J130" s="77" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K130" s="78"/>
       <c r="L130" s="78"/>
@@ -8227,9 +8649,9 @@
       <c r="O130" s="79"/>
     </row>
     <row r="131" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="81"/>
+      <c r="A131" s="75"/>
       <c r="B131" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C131" s="35" t="s">
         <v>77</v>
@@ -8246,9 +8668,9 @@
       <c r="G131" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="I131" s="81"/>
+      <c r="I131" s="75"/>
       <c r="J131" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K131" s="35" t="s">
         <v>77</v>
@@ -8267,7 +8689,7 @@
       </c>
     </row>
     <row r="132" spans="1:15" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="82"/>
+      <c r="A132" s="76"/>
       <c r="B132" s="55" t="s">
         <v>76</v>
       </c>
@@ -8286,7 +8708,7 @@
       <c r="G132" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="I132" s="82"/>
+      <c r="I132" s="76"/>
       <c r="J132" s="55" t="s">
         <v>76</v>
       </c>
@@ -9104,7 +9526,7 @@
     </row>
     <row r="155" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A155" s="49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B155" s="50"/>
       <c r="C155" s="50"/>
@@ -9158,7 +9580,7 @@
     </row>
     <row r="157" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A157" s="49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B157" s="50"/>
       <c r="C157" s="50"/>
@@ -9187,16 +9609,16 @@
       <c r="A158" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B158" s="94" t="s">
-        <v>0</v>
-      </c>
-      <c r="C158" s="95"/>
-      <c r="D158" s="96"/>
-      <c r="E158" s="94" t="s">
+      <c r="B158" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" s="84"/>
+      <c r="D158" s="85"/>
+      <c r="E158" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="F158" s="95"/>
-      <c r="G158" s="96"/>
+      <c r="F158" s="84"/>
+      <c r="G158" s="85"/>
     </row>
     <row r="159" spans="1:23" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A159" s="6"/>
@@ -9921,7 +10343,7 @@
     </row>
     <row r="182" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A182" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B182" s="50"/>
       <c r="C182" s="50"/>
@@ -9947,11 +10369,11 @@
       <c r="W182" s="50"/>
     </row>
     <row r="183" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A183" s="97" t="s">
-        <v>90</v>
-      </c>
-      <c r="B183" s="97"/>
-      <c r="C183" s="97"/>
+      <c r="A183" s="86" t="s">
+        <v>89</v>
+      </c>
+      <c r="B183" s="86"/>
+      <c r="C183" s="86"/>
     </row>
     <row r="184" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A184" s="1" t="s">
@@ -9999,7 +10421,7 @@
     </row>
     <row r="194" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A194" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B194" s="50"/>
       <c r="C194" s="50"/>
@@ -10025,39 +10447,39 @@
       <c r="W194" s="50"/>
     </row>
     <row r="195" spans="1:23" s="52" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A195" s="85" t="s">
+      <c r="A195" s="87" t="s">
+        <v>90</v>
+      </c>
+      <c r="B195" s="87"/>
+      <c r="C195" s="87"/>
+      <c r="D195" s="87"/>
+      <c r="E195" s="87"/>
+      <c r="F195" s="87"/>
+    </row>
+    <row r="196" spans="1:23" s="52" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A196" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="B195" s="85"/>
-      <c r="C195" s="85"/>
-      <c r="D195" s="85"/>
-      <c r="E195" s="85"/>
-      <c r="F195" s="85"/>
-    </row>
-    <row r="196" spans="1:23" s="52" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A196" s="98" t="s">
-        <v>92</v>
-      </c>
-      <c r="B196" s="98"/>
-      <c r="C196" s="98"/>
-      <c r="D196" s="98"/>
-      <c r="E196" s="98"/>
-      <c r="F196" s="98"/>
+      <c r="B196" s="88"/>
+      <c r="C196" s="88"/>
+      <c r="D196" s="88"/>
+      <c r="E196" s="88"/>
+      <c r="F196" s="88"/>
     </row>
     <row r="197" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A197" s="91" t="s">
+      <c r="A197" s="80" t="s">
         <v>53</v>
       </c>
       <c r="B197" s="59"/>
       <c r="C197" s="59"/>
-      <c r="D197" s="91" t="s">
+      <c r="D197" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="E197" s="91"/>
-      <c r="F197" s="91"/>
+      <c r="E197" s="80"/>
+      <c r="F197" s="80"/>
     </row>
     <row r="198" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A198" s="91"/>
+      <c r="A198" s="80"/>
       <c r="B198" s="59"/>
       <c r="C198" s="60" t="s">
         <v>54</v>
@@ -10703,29 +11125,29 @@
       </c>
     </row>
     <row r="216" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A216" s="92" t="s">
-        <v>93</v>
-      </c>
-      <c r="B216" s="92"/>
-      <c r="C216" s="92"/>
-      <c r="D216" s="92"/>
-      <c r="E216" s="92"/>
-      <c r="F216" s="92"/>
+      <c r="A216" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="B216" s="81"/>
+      <c r="C216" s="81"/>
+      <c r="D216" s="81"/>
+      <c r="E216" s="81"/>
+      <c r="F216" s="81"/>
     </row>
     <row r="217" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A217" s="93" t="s">
+      <c r="A217" s="82" t="s">
         <v>2</v>
       </c>
       <c r="B217" s="59"/>
       <c r="C217" s="59"/>
-      <c r="D217" s="91" t="s">
+      <c r="D217" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="E217" s="91"/>
-      <c r="F217" s="91"/>
+      <c r="E217" s="80"/>
+      <c r="F217" s="80"/>
     </row>
     <row r="218" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A218" s="93"/>
+      <c r="A218" s="82"/>
       <c r="B218" s="59"/>
       <c r="C218" s="60" t="s">
         <v>54</v>
@@ -11108,7 +11530,7 @@
     </row>
     <row r="236" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A236" s="57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B236" s="52"/>
       <c r="C236" s="52"/>
@@ -11168,6 +11590,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A109:A111"/>
+    <mergeCell ref="B109:G109"/>
+    <mergeCell ref="B130:G130"/>
+    <mergeCell ref="A130:A132"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="B81:B83"/>
     <mergeCell ref="I130:I132"/>
     <mergeCell ref="J130:O130"/>
     <mergeCell ref="A197:A198"/>
@@ -11180,18 +11614,6 @@
     <mergeCell ref="A196:F196"/>
     <mergeCell ref="D197:F197"/>
     <mergeCell ref="D217:F217"/>
-    <mergeCell ref="A109:A111"/>
-    <mergeCell ref="B109:G109"/>
-    <mergeCell ref="B130:G130"/>
-    <mergeCell ref="A130:A132"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="B81:B83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change fertility2 by 2010 to be 0.65*original fertility matrix. Load from Excel doc and save in fertilityBy2010 mat file rather than loading from calibratedParams mat file. Update file names accordingly.
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -559,8 +559,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.00000;\-0.00000;0"/>
-    <numFmt numFmtId="169" formatCode="###;\-###;0"/>
+    <numFmt numFmtId="164" formatCode="0.00000;\-0.00000;0"/>
+    <numFmt numFmtId="165" formatCode="###;\-###;0"/>
   </numFmts>
   <fonts count="33" x14ac:knownFonts="1">
     <font>
@@ -1589,6 +1589,56 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1598,14 +1648,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1629,72 +1694,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -6149,8 +6149,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N101" sqref="N101"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J136" sqref="J136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6279,10 +6279,10 @@
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="93"/>
+      <c r="C4" s="96"/>
     </row>
     <row r="5" spans="1:25" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="53"/>
@@ -6519,10 +6519,10 @@
       <c r="A27" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="87" t="s">
+      <c r="B27" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="94"/>
+      <c r="C27" s="98"/>
     </row>
     <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="12"/>
@@ -6910,19 +6910,19 @@
       <c r="AE51" s="32"/>
     </row>
     <row r="52" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="98" t="s">
+      <c r="A52" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="98" t="s">
+      <c r="B52" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="98"/>
-      <c r="D52" s="98"/>
-      <c r="E52" s="98" t="s">
+      <c r="C52" s="102"/>
+      <c r="D52" s="102"/>
+      <c r="E52" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="98"/>
-      <c r="G52" s="98"/>
+      <c r="F52" s="102"/>
+      <c r="G52" s="102"/>
       <c r="X52" s="30"/>
       <c r="Y52" s="30"/>
       <c r="Z52" s="30"/>
@@ -6933,7 +6933,7 @@
       <c r="AE52" s="30"/>
     </row>
     <row r="53" spans="1:31" ht="30" x14ac:dyDescent="0.35">
-      <c r="A53" s="98"/>
+      <c r="A53" s="102"/>
       <c r="B53" s="45" t="s">
         <v>6</v>
       </c>
@@ -7467,13 +7467,13 @@
       <c r="X80" s="50"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A81" s="89" t="s">
+      <c r="A81" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="95" t="s">
+      <c r="B81" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="95" t="s">
+      <c r="C81" s="99" t="s">
         <v>4</v>
       </c>
       <c r="H81" t="s">
@@ -7481,10 +7481,10 @@
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A82" s="90"/>
-      <c r="B82" s="96"/>
-      <c r="C82" s="96"/>
-      <c r="I82" s="102" t="s">
+      <c r="A82" s="87"/>
+      <c r="B82" s="100"/>
+      <c r="C82" s="100"/>
+      <c r="I82" s="77" t="s">
         <v>98</v>
       </c>
       <c r="K82" t="s">
@@ -7495,27 +7495,27 @@
       </c>
     </row>
     <row r="83" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="91"/>
-      <c r="B83" s="97"/>
-      <c r="C83" s="97"/>
+      <c r="A83" s="88"/>
+      <c r="B83" s="101"/>
+      <c r="C83" s="101"/>
       <c r="E83" t="s">
         <v>99</v>
       </c>
-      <c r="H83" s="100"/>
-      <c r="I83" s="104">
-        <v>0</v>
-      </c>
-      <c r="J83" s="104">
+      <c r="H83" s="75"/>
+      <c r="I83" s="79">
+        <v>0</v>
+      </c>
+      <c r="J83" s="79">
         <v>1</v>
       </c>
-      <c r="K83" s="110">
+      <c r="K83" s="85">
         <v>5.1751479000000003E-2</v>
       </c>
-      <c r="L83" s="110">
+      <c r="L83" s="85">
         <v>4.2747080999999999E-2</v>
       </c>
-      <c r="O83" s="105"/>
-      <c r="P83" s="105"/>
+      <c r="O83" s="80"/>
+      <c r="P83" s="80"/>
     </row>
     <row r="84" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="4" t="s">
@@ -7533,17 +7533,17 @@
       <c r="F84">
         <v>0.06</v>
       </c>
-      <c r="H84" s="100"/>
-      <c r="I84" s="104">
+      <c r="H84" s="75"/>
+      <c r="I84" s="79">
         <v>1</v>
       </c>
-      <c r="J84" s="104">
+      <c r="J84" s="79">
         <v>4</v>
       </c>
-      <c r="K84" s="110">
+      <c r="K84" s="85">
         <v>5.2241062999999997E-3</v>
       </c>
-      <c r="L84" s="110">
+      <c r="L84" s="85">
         <v>4.6946237E-3</v>
       </c>
       <c r="M84" t="s">
@@ -7566,19 +7566,19 @@
       <c r="F85">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="H85" s="100"/>
-      <c r="I85" s="106">
-        <v>0</v>
-      </c>
-      <c r="J85" s="107">
+      <c r="H85" s="75"/>
+      <c r="I85" s="81">
+        <v>0</v>
+      </c>
+      <c r="J85" s="82">
         <f>SUM(J83:J84)</f>
         <v>5</v>
       </c>
-      <c r="K85" s="108">
+      <c r="K85" s="83">
         <f>SUM(K83:K84)</f>
         <v>5.6975585300000006E-2</v>
       </c>
-      <c r="L85" s="108">
+      <c r="L85" s="83">
         <f>SUM(L83:L84)</f>
         <v>4.7441704699999997E-2</v>
       </c>
@@ -7599,17 +7599,17 @@
       <c r="F86">
         <v>4.2999999999999999E-4</v>
       </c>
-      <c r="H86" s="100"/>
-      <c r="I86" s="101">
+      <c r="H86" s="75"/>
+      <c r="I86" s="76">
         <v>5</v>
       </c>
-      <c r="J86" s="101">
+      <c r="J86" s="76">
         <v>5</v>
       </c>
-      <c r="K86" s="109">
+      <c r="K86" s="84">
         <v>2.4750038999999998E-3</v>
       </c>
-      <c r="L86" s="109">
+      <c r="L86" s="84">
         <v>1.8590649E-3</v>
       </c>
     </row>
@@ -7629,17 +7629,17 @@
       <c r="F87">
         <v>7.6000000000000004E-4</v>
       </c>
-      <c r="H87" s="100"/>
-      <c r="I87" s="101">
+      <c r="H87" s="75"/>
+      <c r="I87" s="76">
         <v>10</v>
       </c>
-      <c r="J87" s="101">
+      <c r="J87" s="76">
         <v>5</v>
       </c>
-      <c r="K87" s="109">
+      <c r="K87" s="84">
         <v>1.5814690000000001E-3</v>
       </c>
-      <c r="L87" s="109">
+      <c r="L87" s="84">
         <v>1.2227608999999999E-3</v>
       </c>
     </row>
@@ -7659,17 +7659,17 @@
       <c r="F88">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="H88" s="100"/>
-      <c r="I88" s="101">
+      <c r="H88" s="75"/>
+      <c r="I88" s="76">
         <v>15</v>
       </c>
-      <c r="J88" s="101">
+      <c r="J88" s="76">
         <v>5</v>
       </c>
-      <c r="K88" s="109">
+      <c r="K88" s="84">
         <v>2.5001934000000001E-3</v>
       </c>
-      <c r="L88" s="109">
+      <c r="L88" s="84">
         <v>1.6750273E-3</v>
       </c>
     </row>
@@ -7689,17 +7689,17 @@
       <c r="F89">
         <v>1.83E-3</v>
       </c>
-      <c r="H89" s="100"/>
-      <c r="I89" s="101">
+      <c r="H89" s="75"/>
+      <c r="I89" s="76">
         <v>20</v>
       </c>
-      <c r="J89" s="101">
+      <c r="J89" s="76">
         <v>5</v>
       </c>
-      <c r="K89" s="109">
+      <c r="K89" s="84">
         <v>3.7640993E-3</v>
       </c>
-      <c r="L89" s="109">
+      <c r="L89" s="84">
         <v>2.3815536E-3</v>
       </c>
     </row>
@@ -7719,17 +7719,17 @@
       <c r="F90">
         <v>2.5200000000000001E-3</v>
       </c>
-      <c r="H90" s="100"/>
-      <c r="I90" s="101">
+      <c r="H90" s="75"/>
+      <c r="I90" s="76">
         <v>25</v>
       </c>
-      <c r="J90" s="101">
+      <c r="J90" s="76">
         <v>5</v>
       </c>
-      <c r="K90" s="109">
+      <c r="K90" s="84">
         <v>4.3315932999999996E-3</v>
       </c>
-      <c r="L90" s="109">
+      <c r="L90" s="84">
         <v>3.1198295999999999E-3</v>
       </c>
     </row>
@@ -7749,17 +7749,17 @@
       <c r="F91">
         <v>3.15E-3</v>
       </c>
-      <c r="H91" s="100"/>
-      <c r="I91" s="101">
+      <c r="H91" s="75"/>
+      <c r="I91" s="76">
         <v>30</v>
       </c>
-      <c r="J91" s="101">
+      <c r="J91" s="76">
         <v>5</v>
       </c>
-      <c r="K91" s="109">
+      <c r="K91" s="84">
         <v>5.1669517000000002E-3</v>
       </c>
-      <c r="L91" s="109">
+      <c r="L91" s="84">
         <v>3.7817176000000002E-3</v>
       </c>
     </row>
@@ -7779,17 +7779,17 @@
       <c r="F92">
         <v>4.4799999999999996E-3</v>
       </c>
-      <c r="H92" s="100"/>
-      <c r="I92" s="101">
+      <c r="H92" s="75"/>
+      <c r="I92" s="76">
         <v>35</v>
       </c>
-      <c r="J92" s="101">
+      <c r="J92" s="76">
         <v>5</v>
       </c>
-      <c r="K92" s="109">
+      <c r="K92" s="84">
         <v>6.4414638999999996E-3</v>
       </c>
-      <c r="L92" s="109">
+      <c r="L92" s="84">
         <v>4.6448573999999998E-3</v>
       </c>
     </row>
@@ -7809,17 +7809,17 @@
       <c r="F93">
         <v>5.7600000000000004E-3</v>
       </c>
-      <c r="H93" s="100"/>
-      <c r="I93" s="101">
+      <c r="H93" s="75"/>
+      <c r="I93" s="76">
         <v>40</v>
       </c>
-      <c r="J93" s="101">
+      <c r="J93" s="76">
         <v>5</v>
       </c>
-      <c r="K93" s="109">
+      <c r="K93" s="84">
         <v>8.0432449999999992E-3</v>
       </c>
-      <c r="L93" s="109">
+      <c r="L93" s="84">
         <v>5.6773359000000002E-3</v>
       </c>
     </row>
@@ -7839,17 +7839,17 @@
       <c r="F94">
         <v>9.6399999999999993E-3</v>
       </c>
-      <c r="H94" s="100"/>
-      <c r="I94" s="101">
+      <c r="H94" s="75"/>
+      <c r="I94" s="76">
         <v>45</v>
       </c>
-      <c r="J94" s="101">
+      <c r="J94" s="76">
         <v>5</v>
       </c>
-      <c r="K94" s="109">
+      <c r="K94" s="84">
         <v>1.0135829000000001E-2</v>
       </c>
-      <c r="L94" s="109">
+      <c r="L94" s="84">
         <v>6.6691631000000001E-3</v>
       </c>
     </row>
@@ -7869,17 +7869,17 @@
       <c r="F95" s="52">
         <v>1.393E-2</v>
       </c>
-      <c r="H95" s="100"/>
-      <c r="I95" s="101">
+      <c r="H95" s="75"/>
+      <c r="I95" s="76">
         <v>50</v>
       </c>
-      <c r="J95" s="101">
+      <c r="J95" s="76">
         <v>5</v>
       </c>
-      <c r="K95" s="109">
+      <c r="K95" s="84">
         <v>1.4004198000000001E-2</v>
       </c>
-      <c r="L95" s="109">
+      <c r="L95" s="84">
         <v>8.9763412999999993E-3</v>
       </c>
     </row>
@@ -7893,19 +7893,19 @@
       <c r="C96" s="13">
         <v>1.5759592316689931E-2</v>
       </c>
-      <c r="E96" s="103"/>
-      <c r="F96" s="103"/>
-      <c r="H96" s="100"/>
-      <c r="I96" s="101">
+      <c r="E96" s="78"/>
+      <c r="F96" s="78"/>
+      <c r="H96" s="75"/>
+      <c r="I96" s="76">
         <v>55</v>
       </c>
-      <c r="J96" s="101">
+      <c r="J96" s="76">
         <v>5</v>
       </c>
-      <c r="K96" s="109">
+      <c r="K96" s="84">
         <v>1.8576009000000001E-2</v>
       </c>
-      <c r="L96" s="109">
+      <c r="L96" s="84">
         <v>1.2049147E-2</v>
       </c>
     </row>
@@ -7919,19 +7919,19 @@
       <c r="C97" s="13">
         <v>2.2837523063216215E-2</v>
       </c>
-      <c r="E97" s="103"/>
-      <c r="F97" s="103"/>
-      <c r="H97" s="100"/>
-      <c r="I97" s="101">
+      <c r="E97" s="78"/>
+      <c r="F97" s="78"/>
+      <c r="H97" s="75"/>
+      <c r="I97" s="76">
         <v>60</v>
       </c>
-      <c r="J97" s="101">
+      <c r="J97" s="76">
         <v>5</v>
       </c>
-      <c r="K97" s="109">
+      <c r="K97" s="84">
         <v>2.7759598999999999E-2</v>
       </c>
-      <c r="L97" s="109">
+      <c r="L97" s="84">
         <v>1.8543285E-2</v>
       </c>
     </row>
@@ -7945,19 +7945,19 @@
       <c r="C98" s="13">
         <v>3.3336893194863555E-2</v>
       </c>
-      <c r="E98" s="103"/>
-      <c r="F98" s="103"/>
-      <c r="H98" s="100"/>
-      <c r="I98" s="101">
+      <c r="E98" s="78"/>
+      <c r="F98" s="78"/>
+      <c r="H98" s="75"/>
+      <c r="I98" s="76">
         <v>65</v>
       </c>
-      <c r="J98" s="101">
+      <c r="J98" s="76">
         <v>5</v>
       </c>
-      <c r="K98" s="109">
+      <c r="K98" s="84">
         <v>4.2779603999999999E-2</v>
       </c>
-      <c r="L98" s="109">
+      <c r="L98" s="84">
         <v>3.039122E-2</v>
       </c>
     </row>
@@ -7971,57 +7971,57 @@
       <c r="C99" s="13">
         <v>6.1722846856347699E-2</v>
       </c>
-      <c r="E99" s="103"/>
-      <c r="F99" s="103"/>
-      <c r="H99" s="100"/>
-      <c r="I99" s="101">
+      <c r="E99" s="78"/>
+      <c r="F99" s="78"/>
+      <c r="H99" s="75"/>
+      <c r="I99" s="76">
         <v>70</v>
       </c>
-      <c r="J99" s="101">
+      <c r="J99" s="76">
         <v>5</v>
       </c>
-      <c r="K99" s="109">
+      <c r="K99" s="84">
         <v>6.8473476000000005E-2</v>
       </c>
-      <c r="L99" s="109">
+      <c r="L99" s="84">
         <v>5.1704121999999998E-2</v>
       </c>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="E100" s="99"/>
-      <c r="F100" s="99"/>
-      <c r="I100" s="101">
+      <c r="E100" s="74"/>
+      <c r="F100" s="74"/>
+      <c r="I100" s="76">
         <v>75</v>
       </c>
-      <c r="J100" s="101">
+      <c r="J100" s="76">
         <v>5</v>
       </c>
-      <c r="K100" s="109">
+      <c r="K100" s="84">
         <v>0.11201527999999999</v>
       </c>
-      <c r="L100" s="109">
+      <c r="L100" s="84">
         <v>8.8066895000000006E-2</v>
       </c>
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="I101" s="101"/>
-      <c r="J101" s="101"/>
-      <c r="K101" s="100"/>
+      <c r="I101" s="76"/>
+      <c r="J101" s="76"/>
+      <c r="K101" s="75"/>
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="I102" s="101"/>
-      <c r="J102" s="101"/>
-      <c r="K102" s="100"/>
+      <c r="I102" s="76"/>
+      <c r="J102" s="76"/>
+      <c r="K102" s="75"/>
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="I103" s="101"/>
-      <c r="J103" s="101"/>
-      <c r="K103" s="100"/>
+      <c r="I103" s="76"/>
+      <c r="J103" s="76"/>
+      <c r="K103" s="75"/>
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="I104" s="101"/>
-      <c r="J104" s="101"/>
-      <c r="K104" s="100"/>
+      <c r="I104" s="76"/>
+      <c r="J104" s="76"/>
+      <c r="K104" s="75"/>
     </row>
     <row r="105" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A105" s="49" t="s">
@@ -8136,20 +8136,20 @@
       <c r="X108" s="50"/>
     </row>
     <row r="109" spans="1:24" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="89" t="s">
+      <c r="A109" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B109" s="77" t="s">
+      <c r="B109" s="89" t="s">
         <v>95</v>
       </c>
-      <c r="C109" s="78"/>
-      <c r="D109" s="78"/>
-      <c r="E109" s="78"/>
-      <c r="F109" s="78"/>
-      <c r="G109" s="79"/>
+      <c r="C109" s="90"/>
+      <c r="D109" s="90"/>
+      <c r="E109" s="90"/>
+      <c r="F109" s="90"/>
+      <c r="G109" s="91"/>
     </row>
     <row r="110" spans="1:24" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="90"/>
+      <c r="A110" s="87"/>
       <c r="B110" s="44" t="s">
         <v>83</v>
       </c>
@@ -8170,7 +8170,7 @@
       </c>
     </row>
     <row r="111" spans="1:24" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="91"/>
+      <c r="A111" s="88"/>
       <c r="B111" s="46" t="s">
         <v>76</v>
       </c>
@@ -8625,31 +8625,31 @@
     </row>
     <row r="129" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="130" spans="1:15" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="74" t="s">
+      <c r="A130" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="B130" s="77" t="s">
+      <c r="B130" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="C130" s="78"/>
-      <c r="D130" s="78"/>
-      <c r="E130" s="78"/>
-      <c r="F130" s="78"/>
-      <c r="G130" s="79"/>
-      <c r="I130" s="74" t="s">
+      <c r="C130" s="90"/>
+      <c r="D130" s="90"/>
+      <c r="E130" s="90"/>
+      <c r="F130" s="90"/>
+      <c r="G130" s="91"/>
+      <c r="I130" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="J130" s="77" t="s">
+      <c r="J130" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="K130" s="78"/>
-      <c r="L130" s="78"/>
-      <c r="M130" s="78"/>
-      <c r="N130" s="78"/>
-      <c r="O130" s="79"/>
+      <c r="K130" s="90"/>
+      <c r="L130" s="90"/>
+      <c r="M130" s="90"/>
+      <c r="N130" s="90"/>
+      <c r="O130" s="91"/>
     </row>
     <row r="131" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="75"/>
+      <c r="A131" s="93"/>
       <c r="B131" s="34" t="s">
         <v>84</v>
       </c>
@@ -8668,7 +8668,7 @@
       <c r="G131" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="I131" s="75"/>
+      <c r="I131" s="93"/>
       <c r="J131" s="34" t="s">
         <v>84</v>
       </c>
@@ -8689,7 +8689,7 @@
       </c>
     </row>
     <row r="132" spans="1:15" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="76"/>
+      <c r="A132" s="94"/>
       <c r="B132" s="55" t="s">
         <v>76</v>
       </c>
@@ -8708,7 +8708,7 @@
       <c r="G132" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="I132" s="76"/>
+      <c r="I132" s="94"/>
       <c r="J132" s="55" t="s">
         <v>76</v>
       </c>
@@ -8865,49 +8865,55 @@
         <v>18</v>
       </c>
       <c r="B136" s="27">
-        <v>7.0699999999999999E-2</v>
+        <f>B115*0.65</f>
+        <v>9.1910000000000006E-2</v>
       </c>
       <c r="C136" s="27">
-        <v>7.0699999999999999E-2</v>
+        <f t="shared" ref="C136:G136" si="4">C115*0.65</f>
+        <v>9.1910000000000006E-2</v>
       </c>
       <c r="D136" s="27">
-        <v>7.0699999999999999E-2</v>
+        <f t="shared" si="4"/>
+        <v>9.1910000000000006E-2</v>
       </c>
       <c r="E136" s="27">
-        <v>4.1006000000000008E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.3307800000000009E-2</v>
       </c>
       <c r="F136" s="27">
-        <v>4.1006000000000008E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.3307800000000009E-2</v>
       </c>
       <c r="G136" s="27">
-        <v>2.8987000000000002E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.7683100000000004E-2</v>
       </c>
       <c r="I136" s="72" t="s">
         <v>18</v>
       </c>
       <c r="J136" s="27">
         <f>B136*0.75</f>
-        <v>5.3025000000000003E-2</v>
+        <v>6.8932500000000008E-2</v>
       </c>
       <c r="K136" s="27">
-        <f t="shared" ref="K136:O142" si="4">C136*0.75</f>
-        <v>5.3025000000000003E-2</v>
+        <f t="shared" ref="K136:O142" si="5">C136*0.75</f>
+        <v>6.8932500000000008E-2</v>
       </c>
       <c r="L136" s="27">
-        <f t="shared" si="4"/>
-        <v>5.3025000000000003E-2</v>
+        <f t="shared" si="5"/>
+        <v>6.8932500000000008E-2</v>
       </c>
       <c r="M136" s="27">
-        <f t="shared" si="4"/>
-        <v>3.0754500000000004E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.9980850000000005E-2</v>
       </c>
       <c r="N136" s="27">
-        <f t="shared" si="4"/>
-        <v>3.0754500000000004E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.9980850000000005E-2</v>
       </c>
       <c r="O136" s="27">
-        <f t="shared" si="4"/>
-        <v>2.1740250000000003E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.8262325000000005E-2</v>
       </c>
     </row>
     <row r="137" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -8915,49 +8921,55 @@
         <v>19</v>
       </c>
       <c r="B137" s="27">
-        <v>0.13900000000000001</v>
+        <f t="shared" ref="B137:G142" si="6">B116*0.65</f>
+        <v>0.18070000000000003</v>
       </c>
       <c r="C137" s="27">
-        <v>0.13900000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0.18070000000000003</v>
       </c>
       <c r="D137" s="27">
-        <v>0.13900000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0.18070000000000003</v>
       </c>
       <c r="E137" s="27">
-        <v>8.0620000000000011E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.10480600000000002</v>
       </c>
       <c r="F137" s="27">
-        <v>8.0620000000000011E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.10480600000000002</v>
       </c>
       <c r="G137" s="27">
-        <v>5.6990000000000013E-2</v>
+        <f t="shared" si="6"/>
+        <v>7.4087000000000014E-2</v>
       </c>
       <c r="I137" s="72" t="s">
         <v>19</v>
       </c>
       <c r="J137" s="27">
-        <f t="shared" ref="J137:J142" si="5">B137*0.75</f>
-        <v>0.10425000000000001</v>
+        <f t="shared" ref="J137:J142" si="7">B137*0.75</f>
+        <v>0.13552500000000001</v>
       </c>
       <c r="K137" s="27">
-        <f t="shared" si="4"/>
-        <v>0.10425000000000001</v>
+        <f t="shared" si="5"/>
+        <v>0.13552500000000001</v>
       </c>
       <c r="L137" s="27">
-        <f t="shared" si="4"/>
-        <v>0.10425000000000001</v>
+        <f t="shared" si="5"/>
+        <v>0.13552500000000001</v>
       </c>
       <c r="M137" s="27">
-        <f t="shared" si="4"/>
-        <v>6.0465000000000005E-2</v>
+        <f t="shared" si="5"/>
+        <v>7.8604500000000022E-2</v>
       </c>
       <c r="N137" s="27">
-        <f t="shared" si="4"/>
-        <v>6.0465000000000005E-2</v>
+        <f t="shared" si="5"/>
+        <v>7.8604500000000022E-2</v>
       </c>
       <c r="O137" s="27">
-        <f t="shared" si="4"/>
-        <v>4.274250000000001E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.556525000000001E-2</v>
       </c>
     </row>
     <row r="138" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -8965,49 +8977,55 @@
         <v>20</v>
       </c>
       <c r="B138" s="27">
-        <v>0.14180000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0.18434000000000003</v>
       </c>
       <c r="C138" s="27">
-        <v>0.14180000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0.18434000000000003</v>
       </c>
       <c r="D138" s="27">
-        <v>0.14180000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0.18434000000000003</v>
       </c>
       <c r="E138" s="27">
-        <v>8.2244000000000012E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.10691720000000002</v>
       </c>
       <c r="F138" s="27">
-        <v>8.2244000000000012E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.10691720000000002</v>
       </c>
       <c r="G138" s="27">
-        <v>5.8138000000000009E-2</v>
+        <f t="shared" si="6"/>
+        <v>7.5579400000000019E-2</v>
       </c>
       <c r="I138" s="72" t="s">
         <v>20</v>
       </c>
       <c r="J138" s="27">
+        <f t="shared" si="7"/>
+        <v>0.13825500000000002</v>
+      </c>
+      <c r="K138" s="27">
         <f t="shared" si="5"/>
-        <v>0.10635</v>
-      </c>
-      <c r="K138" s="27">
-        <f t="shared" si="4"/>
-        <v>0.10635</v>
+        <v>0.13825500000000002</v>
       </c>
       <c r="L138" s="27">
-        <f t="shared" si="4"/>
-        <v>0.10635</v>
+        <f t="shared" si="5"/>
+        <v>0.13825500000000002</v>
       </c>
       <c r="M138" s="27">
-        <f t="shared" si="4"/>
-        <v>6.1683000000000009E-2</v>
+        <f t="shared" si="5"/>
+        <v>8.0187900000000006E-2</v>
       </c>
       <c r="N138" s="27">
-        <f t="shared" si="4"/>
-        <v>6.1683000000000009E-2</v>
+        <f t="shared" si="5"/>
+        <v>8.0187900000000006E-2</v>
       </c>
       <c r="O138" s="27">
-        <f t="shared" si="4"/>
-        <v>4.3603500000000003E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.6684550000000014E-2</v>
       </c>
     </row>
     <row r="139" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9015,49 +9033,55 @@
         <v>23</v>
       </c>
       <c r="B139" s="27">
-        <v>0.1056</v>
+        <f t="shared" si="6"/>
+        <v>0.13728000000000001</v>
       </c>
       <c r="C139" s="27">
-        <v>0.1056</v>
+        <f t="shared" si="6"/>
+        <v>0.13728000000000001</v>
       </c>
       <c r="D139" s="27">
-        <v>0.1056</v>
+        <f t="shared" si="6"/>
+        <v>0.13728000000000001</v>
       </c>
       <c r="E139" s="27">
-        <v>6.1248000000000004E-2</v>
+        <f t="shared" si="6"/>
+        <v>7.962240000000001E-2</v>
       </c>
       <c r="F139" s="27">
-        <v>6.1248000000000004E-2</v>
+        <f t="shared" si="6"/>
+        <v>7.962240000000001E-2</v>
       </c>
       <c r="G139" s="27">
-        <v>4.3296000000000001E-2</v>
+        <f t="shared" si="6"/>
+        <v>5.6284800000000003E-2</v>
       </c>
       <c r="I139" s="72" t="s">
         <v>23</v>
       </c>
       <c r="J139" s="27">
+        <f t="shared" si="7"/>
+        <v>0.10296000000000001</v>
+      </c>
+      <c r="K139" s="27">
         <f t="shared" si="5"/>
-        <v>7.9199999999999993E-2</v>
-      </c>
-      <c r="K139" s="27">
-        <f t="shared" si="4"/>
-        <v>7.9199999999999993E-2</v>
+        <v>0.10296000000000001</v>
       </c>
       <c r="L139" s="27">
-        <f t="shared" si="4"/>
-        <v>7.9199999999999993E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.10296000000000001</v>
       </c>
       <c r="M139" s="27">
-        <f t="shared" si="4"/>
-        <v>4.5936000000000005E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.9716800000000007E-2</v>
       </c>
       <c r="N139" s="27">
-        <f t="shared" si="4"/>
-        <v>4.5936000000000005E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.9716800000000007E-2</v>
       </c>
       <c r="O139" s="27">
-        <f t="shared" si="4"/>
-        <v>3.2472000000000001E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.2213600000000004E-2</v>
       </c>
     </row>
     <row r="140" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9065,49 +9089,55 @@
         <v>22</v>
       </c>
       <c r="B140" s="27">
-        <v>6.7400000000000002E-2</v>
+        <f t="shared" si="6"/>
+        <v>8.7620000000000003E-2</v>
       </c>
       <c r="C140" s="27">
-        <v>6.7400000000000002E-2</v>
+        <f t="shared" si="6"/>
+        <v>8.7620000000000003E-2</v>
       </c>
       <c r="D140" s="27">
-        <v>6.7400000000000002E-2</v>
+        <f t="shared" si="6"/>
+        <v>8.7620000000000003E-2</v>
       </c>
       <c r="E140" s="27">
-        <v>3.9092000000000009E-2</v>
+        <f t="shared" si="6"/>
+        <v>5.0819600000000013E-2</v>
       </c>
       <c r="F140" s="27">
-        <v>3.9092000000000009E-2</v>
+        <f t="shared" si="6"/>
+        <v>5.0819600000000013E-2</v>
       </c>
       <c r="G140" s="27">
-        <v>2.7634000000000002E-2</v>
+        <f t="shared" si="6"/>
+        <v>3.5924200000000003E-2</v>
       </c>
       <c r="I140" s="72" t="s">
         <v>22</v>
       </c>
       <c r="J140" s="27">
+        <f t="shared" si="7"/>
+        <v>6.5714999999999996E-2</v>
+      </c>
+      <c r="K140" s="27">
         <f t="shared" si="5"/>
-        <v>5.0549999999999998E-2</v>
-      </c>
-      <c r="K140" s="27">
-        <f t="shared" si="4"/>
-        <v>5.0549999999999998E-2</v>
+        <v>6.5714999999999996E-2</v>
       </c>
       <c r="L140" s="27">
-        <f t="shared" si="4"/>
-        <v>5.0549999999999998E-2</v>
+        <f t="shared" si="5"/>
+        <v>6.5714999999999996E-2</v>
       </c>
       <c r="M140" s="27">
-        <f t="shared" si="4"/>
-        <v>2.9319000000000005E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.8114700000000008E-2</v>
       </c>
       <c r="N140" s="27">
-        <f t="shared" si="4"/>
-        <v>2.9319000000000005E-2</v>
+        <f t="shared" si="5"/>
+        <v>3.8114700000000008E-2</v>
       </c>
       <c r="O140" s="27">
-        <f t="shared" si="4"/>
-        <v>2.0725500000000001E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.6943150000000003E-2</v>
       </c>
     </row>
     <row r="141" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9115,49 +9145,55 @@
         <v>24</v>
       </c>
       <c r="B141" s="27">
-        <v>2.7100000000000003E-2</v>
+        <f t="shared" si="6"/>
+        <v>3.5230000000000004E-2</v>
       </c>
       <c r="C141" s="27">
-        <v>2.7100000000000003E-2</v>
+        <f t="shared" si="6"/>
+        <v>3.5230000000000004E-2</v>
       </c>
       <c r="D141" s="27">
-        <v>2.7100000000000003E-2</v>
+        <f t="shared" si="6"/>
+        <v>3.5230000000000004E-2</v>
       </c>
       <c r="E141" s="27">
-        <v>1.5718000000000003E-2</v>
+        <f t="shared" si="6"/>
+        <v>2.0433400000000004E-2</v>
       </c>
       <c r="F141" s="27">
-        <v>1.5718000000000003E-2</v>
+        <f t="shared" si="6"/>
+        <v>2.0433400000000004E-2</v>
       </c>
       <c r="G141" s="27">
-        <v>1.1111000000000001E-2</v>
+        <f t="shared" si="6"/>
+        <v>1.4444300000000002E-2</v>
       </c>
       <c r="I141" s="72" t="s">
         <v>24</v>
       </c>
       <c r="J141" s="27">
+        <f t="shared" si="7"/>
+        <v>2.6422500000000002E-2</v>
+      </c>
+      <c r="K141" s="27">
         <f t="shared" si="5"/>
-        <v>2.0325000000000003E-2</v>
-      </c>
-      <c r="K141" s="27">
-        <f t="shared" si="4"/>
-        <v>2.0325000000000003E-2</v>
+        <v>2.6422500000000002E-2</v>
       </c>
       <c r="L141" s="27">
-        <f t="shared" si="4"/>
-        <v>2.0325000000000003E-2</v>
+        <f t="shared" si="5"/>
+        <v>2.6422500000000002E-2</v>
       </c>
       <c r="M141" s="27">
-        <f t="shared" si="4"/>
-        <v>1.1788500000000002E-2</v>
+        <f t="shared" si="5"/>
+        <v>1.5325050000000003E-2</v>
       </c>
       <c r="N141" s="27">
-        <f t="shared" si="4"/>
-        <v>1.1788500000000002E-2</v>
+        <f t="shared" si="5"/>
+        <v>1.5325050000000003E-2</v>
       </c>
       <c r="O141" s="27">
-        <f t="shared" si="4"/>
-        <v>8.3332500000000004E-3</v>
+        <f t="shared" si="5"/>
+        <v>1.0833225000000002E-2</v>
       </c>
     </row>
     <row r="142" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9165,49 +9201,55 @@
         <v>25</v>
       </c>
       <c r="B142" s="27">
-        <v>8.8000000000000005E-3</v>
+        <f t="shared" si="6"/>
+        <v>1.1440000000000001E-2</v>
       </c>
       <c r="C142" s="27">
-        <v>8.8000000000000005E-3</v>
+        <f t="shared" si="6"/>
+        <v>1.1440000000000001E-2</v>
       </c>
       <c r="D142" s="27">
-        <v>8.8000000000000005E-3</v>
+        <f t="shared" si="6"/>
+        <v>1.1440000000000001E-2</v>
       </c>
       <c r="E142" s="27">
-        <v>5.1040000000000009E-3</v>
+        <f t="shared" si="6"/>
+        <v>6.6352000000000017E-3</v>
       </c>
       <c r="F142" s="27">
-        <v>5.1040000000000009E-3</v>
+        <f t="shared" si="6"/>
+        <v>6.6352000000000017E-3</v>
       </c>
       <c r="G142" s="27">
-        <v>3.6080000000000005E-3</v>
+        <f t="shared" si="6"/>
+        <v>4.6904000000000008E-3</v>
       </c>
       <c r="I142" s="72" t="s">
         <v>25</v>
       </c>
       <c r="J142" s="27">
+        <f t="shared" si="7"/>
+        <v>8.5800000000000008E-3</v>
+      </c>
+      <c r="K142" s="27">
         <f t="shared" si="5"/>
-        <v>6.6E-3</v>
-      </c>
-      <c r="K142" s="27">
-        <f t="shared" si="4"/>
-        <v>6.6E-3</v>
+        <v>8.5800000000000008E-3</v>
       </c>
       <c r="L142" s="27">
-        <f t="shared" si="4"/>
-        <v>6.6E-3</v>
+        <f t="shared" si="5"/>
+        <v>8.5800000000000008E-3</v>
       </c>
       <c r="M142" s="27">
-        <f t="shared" si="4"/>
-        <v>3.8280000000000007E-3</v>
+        <f t="shared" si="5"/>
+        <v>4.9764000000000015E-3</v>
       </c>
       <c r="N142" s="27">
-        <f t="shared" si="4"/>
-        <v>3.8280000000000007E-3</v>
+        <f t="shared" si="5"/>
+        <v>4.9764000000000015E-3</v>
       </c>
       <c r="O142" s="27">
-        <f t="shared" si="4"/>
-        <v>2.7060000000000005E-3</v>
+        <f t="shared" si="5"/>
+        <v>3.5178000000000006E-3</v>
       </c>
     </row>
     <row r="143" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9476,52 +9518,52 @@
     </row>
     <row r="149" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B149">
-        <f t="shared" ref="B149:G149" si="6">5*SUM(B133:B148)</f>
-        <v>2.8020000000000005</v>
+        <f t="shared" ref="B149:G149" si="8">5*SUM(B133:B148)</f>
+        <v>3.6426000000000003</v>
       </c>
       <c r="C149">
-        <f t="shared" si="6"/>
-        <v>2.8020000000000005</v>
+        <f t="shared" si="8"/>
+        <v>3.6426000000000003</v>
       </c>
       <c r="D149">
-        <f t="shared" si="6"/>
-        <v>2.8020000000000005</v>
+        <f t="shared" si="8"/>
+        <v>3.6426000000000003</v>
       </c>
       <c r="E149">
-        <f t="shared" si="6"/>
-        <v>1.6251600000000002</v>
+        <f t="shared" si="8"/>
+        <v>2.112708</v>
       </c>
       <c r="F149">
-        <f t="shared" si="6"/>
-        <v>1.6251600000000002</v>
+        <f t="shared" si="8"/>
+        <v>2.112708</v>
       </c>
       <c r="G149">
-        <f t="shared" si="6"/>
-        <v>1.1488200000000002</v>
+        <f t="shared" si="8"/>
+        <v>1.4934660000000002</v>
       </c>
       <c r="J149">
-        <f t="shared" ref="J149:O149" si="7">5*SUM(J133:J148)</f>
-        <v>2.1014999999999997</v>
+        <f t="shared" ref="J149:O149" si="9">5*SUM(J133:J148)</f>
+        <v>2.7319500000000003</v>
       </c>
       <c r="K149">
-        <f t="shared" si="7"/>
-        <v>2.1014999999999997</v>
+        <f t="shared" si="9"/>
+        <v>2.7319500000000003</v>
       </c>
       <c r="L149">
-        <f t="shared" si="7"/>
-        <v>2.1014999999999997</v>
+        <f t="shared" si="9"/>
+        <v>2.7319500000000003</v>
       </c>
       <c r="M149">
-        <f t="shared" si="7"/>
-        <v>1.2188700000000003</v>
+        <f t="shared" si="9"/>
+        <v>1.5845310000000001</v>
       </c>
       <c r="N149">
-        <f t="shared" si="7"/>
-        <v>1.2188700000000003</v>
+        <f t="shared" si="9"/>
+        <v>1.5845310000000001</v>
       </c>
       <c r="O149">
-        <f t="shared" si="7"/>
-        <v>0.86161500000000013</v>
+        <f t="shared" si="9"/>
+        <v>1.1200995000000002</v>
       </c>
     </row>
     <row r="155" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
@@ -9609,16 +9651,16 @@
       <c r="A158" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B158" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="C158" s="84"/>
-      <c r="D158" s="85"/>
-      <c r="E158" s="83" t="s">
+      <c r="B158" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" s="107"/>
+      <c r="D158" s="108"/>
+      <c r="E158" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="F158" s="84"/>
-      <c r="G158" s="85"/>
+      <c r="F158" s="107"/>
+      <c r="G158" s="108"/>
     </row>
     <row r="159" spans="1:23" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A159" s="6"/>
@@ -9646,15 +9688,15 @@
         <v>11</v>
       </c>
       <c r="B160" s="40">
-        <f t="shared" ref="B160:G161" si="8">10^-5</f>
+        <f t="shared" ref="B160:G161" si="10">10^-5</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C160" s="40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D160" s="40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E160" s="40">
@@ -9662,11 +9704,11 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F160" s="40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="G160" s="40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J160">
@@ -9674,11 +9716,11 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="K160">
-        <f t="shared" ref="K160:L175" si="9">C160*C54</f>
+        <f t="shared" ref="K160:L175" si="11">C160*C54</f>
         <v>0</v>
       </c>
       <c r="L160">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -9687,39 +9729,39 @@
         <v>14</v>
       </c>
       <c r="B161" s="40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C161" s="40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D161" s="40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E161" s="40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F161" s="40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="G161" s="40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J161">
-        <f t="shared" ref="J161:J175" si="10">B161*B55</f>
+        <f t="shared" ref="J161:J175" si="12">B161*B55</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="K161">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L161">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -9746,15 +9788,15 @@
         <v>1.2</v>
       </c>
       <c r="J162">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.176E-2</v>
       </c>
       <c r="K162">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.8E-3</v>
       </c>
       <c r="L162">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>6.0000000000000218E-3</v>
       </c>
       <c r="M162">
@@ -9789,23 +9831,23 @@
         <v>6.5</v>
       </c>
       <c r="J163">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.33787878787878783</v>
       </c>
       <c r="K163">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.040909090909091</v>
       </c>
       <c r="L163">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.58030303030303021</v>
       </c>
       <c r="M163">
-        <f t="shared" ref="M163:M175" si="11">SUM(J163:L163)</f>
+        <f t="shared" ref="M163:M175" si="13">SUM(J163:L163)</f>
         <v>1.959090909090909</v>
       </c>
       <c r="N163">
-        <f t="shared" ref="N163:N175" si="12">1/M163</f>
+        <f t="shared" ref="N163:N175" si="14">1/M163</f>
         <v>0.51044083526682138</v>
       </c>
     </row>
@@ -9832,23 +9874,23 @@
         <v>10</v>
       </c>
       <c r="J164">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.33193277310924363</v>
       </c>
       <c r="K164">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.1274509803921566</v>
       </c>
       <c r="L164">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.65546218487394958</v>
       </c>
       <c r="M164">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.1148459383753497</v>
       </c>
       <c r="N164">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.47284768211920541</v>
       </c>
     </row>
@@ -9875,23 +9917,23 @@
         <v>5.333333333333333</v>
       </c>
       <c r="J165">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.39310344827586208</v>
       </c>
       <c r="K165">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.0551724137931036</v>
       </c>
       <c r="L165">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.54482758620689653</v>
       </c>
       <c r="M165">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.9931034482758623</v>
       </c>
       <c r="N165">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.50173010380622829</v>
       </c>
     </row>
@@ -9918,23 +9960,23 @@
         <v>1</v>
       </c>
       <c r="J166">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.46610169491525422</v>
       </c>
       <c r="K166">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.84745762711864414</v>
       </c>
       <c r="L166">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.3135593220338983</v>
       </c>
       <c r="M166">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.6271186440677967</v>
       </c>
       <c r="N166">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.61458333333333326</v>
       </c>
     </row>
@@ -9961,23 +10003,23 @@
         <v>9</v>
       </c>
       <c r="J167">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.59655172413793101</v>
       </c>
       <c r="K167">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.48965517241379303</v>
       </c>
       <c r="L167">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.19310344827586207</v>
       </c>
       <c r="M167">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.279310344827586</v>
       </c>
       <c r="N167">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.78167115902964968</v>
       </c>
     </row>
@@ -10004,23 +10046,23 @@
         <v>1</v>
       </c>
       <c r="J168">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.68881118881118875</v>
       </c>
       <c r="K168">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.40559440559440557</v>
       </c>
       <c r="L168">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.10839160839160839</v>
       </c>
       <c r="M168">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.2027972027972027</v>
       </c>
       <c r="N168">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.83139534883720934</v>
       </c>
     </row>
@@ -10047,23 +10089,23 @@
         <v>1</v>
       </c>
       <c r="J169">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1E-3</v>
       </c>
       <c r="M169">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N169">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10090,23 +10132,23 @@
         <v>1</v>
       </c>
       <c r="J170">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K170">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L170">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1E-3</v>
       </c>
       <c r="M170">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N170">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10133,23 +10175,23 @@
         <v>1</v>
       </c>
       <c r="J171">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K171">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L171">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1E-3</v>
       </c>
       <c r="M171">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N171">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10176,23 +10218,23 @@
         <v>1</v>
       </c>
       <c r="J172">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K172">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L172">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1E-3</v>
       </c>
       <c r="M172">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N172">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10219,23 +10261,23 @@
         <v>1</v>
       </c>
       <c r="J173">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K173">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L173">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1E-3</v>
       </c>
       <c r="M173">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N173">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10262,23 +10304,23 @@
         <v>1</v>
       </c>
       <c r="J174">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K174">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L174">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1E-3</v>
       </c>
       <c r="M174">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N174">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10309,23 +10351,23 @@
         <v>1.8866801277495602</v>
       </c>
       <c r="J175">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K175">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L175">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1E-3</v>
       </c>
       <c r="M175">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N175">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10369,11 +10411,11 @@
       <c r="W182" s="50"/>
     </row>
     <row r="183" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A183" s="86" t="s">
+      <c r="A183" s="109" t="s">
         <v>89</v>
       </c>
-      <c r="B183" s="86"/>
-      <c r="C183" s="86"/>
+      <c r="B183" s="109"/>
+      <c r="C183" s="109"/>
     </row>
     <row r="184" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A184" s="1" t="s">
@@ -10447,39 +10489,39 @@
       <c r="W194" s="50"/>
     </row>
     <row r="195" spans="1:23" s="52" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A195" s="87" t="s">
+      <c r="A195" s="97" t="s">
         <v>90</v>
       </c>
-      <c r="B195" s="87"/>
-      <c r="C195" s="87"/>
-      <c r="D195" s="87"/>
-      <c r="E195" s="87"/>
-      <c r="F195" s="87"/>
+      <c r="B195" s="97"/>
+      <c r="C195" s="97"/>
+      <c r="D195" s="97"/>
+      <c r="E195" s="97"/>
+      <c r="F195" s="97"/>
     </row>
     <row r="196" spans="1:23" s="52" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A196" s="88" t="s">
+      <c r="A196" s="110" t="s">
         <v>91</v>
       </c>
-      <c r="B196" s="88"/>
-      <c r="C196" s="88"/>
-      <c r="D196" s="88"/>
-      <c r="E196" s="88"/>
-      <c r="F196" s="88"/>
+      <c r="B196" s="110"/>
+      <c r="C196" s="110"/>
+      <c r="D196" s="110"/>
+      <c r="E196" s="110"/>
+      <c r="F196" s="110"/>
     </row>
     <row r="197" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A197" s="80" t="s">
+      <c r="A197" s="103" t="s">
         <v>53</v>
       </c>
       <c r="B197" s="59"/>
       <c r="C197" s="59"/>
-      <c r="D197" s="80" t="s">
+      <c r="D197" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="E197" s="80"/>
-      <c r="F197" s="80"/>
+      <c r="E197" s="103"/>
+      <c r="F197" s="103"/>
     </row>
     <row r="198" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A198" s="80"/>
+      <c r="A198" s="103"/>
       <c r="B198" s="59"/>
       <c r="C198" s="60" t="s">
         <v>54</v>
@@ -10518,11 +10560,11 @@
         <v>0</v>
       </c>
       <c r="I199">
-        <f t="shared" ref="I199:J214" si="13">E199*C54</f>
+        <f t="shared" ref="I199:J214" si="15">E199*C54</f>
         <v>0</v>
       </c>
       <c r="J199">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -10542,15 +10584,15 @@
         <v>0</v>
       </c>
       <c r="H200">
-        <f t="shared" ref="H200:H214" si="14">D200*B55</f>
+        <f t="shared" ref="H200:H214" si="16">D200*B55</f>
         <v>0</v>
       </c>
       <c r="I200">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="J200">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -10575,15 +10617,15 @@
         <v>1.1232</v>
       </c>
       <c r="H201">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>3.0576000000000003</v>
       </c>
       <c r="I201">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2.8079999999999997E-2</v>
       </c>
       <c r="J201">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>5.6160000000000203E-3</v>
       </c>
       <c r="K201">
@@ -10612,19 +10654,19 @@
         <v>5.6159999999999997</v>
       </c>
       <c r="H202">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>7.9418181818181814</v>
       </c>
       <c r="I202">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3.814909090909091</v>
       </c>
       <c r="J202">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.46799999999999986</v>
       </c>
       <c r="K202">
-        <f t="shared" ref="K202:K214" si="15">SUM(H202:J202)</f>
+        <f t="shared" ref="K202:K214" si="17">SUM(H202:J202)</f>
         <v>12.224727272727272</v>
       </c>
     </row>
@@ -10651,19 +10693,19 @@
         <v>22.463999999999999</v>
       </c>
       <c r="H203">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>29.452100840336133</v>
       </c>
       <c r="I203">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>16.570084033613444</v>
       </c>
       <c r="J203">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.9191932773109244</v>
       </c>
       <c r="K203">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>47.941378151260501</v>
       </c>
     </row>
@@ -10688,19 +10730,19 @@
         <v>56.16</v>
       </c>
       <c r="H204">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>79.613793103448273</v>
       </c>
       <c r="I204">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>38.515862068965518</v>
       </c>
       <c r="J204">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4.38951724137931</v>
       </c>
       <c r="K204">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>122.5191724137931</v>
       </c>
     </row>
@@ -10712,35 +10754,35 @@
         <v>10</v>
       </c>
       <c r="C205" s="59">
-        <f t="shared" ref="C205:C214" si="16">EXP(LN(0.5)*B204/10)</f>
+        <f t="shared" ref="C205:C214" si="18">EXP(LN(0.5)*B204/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D205" s="63">
-        <f t="shared" ref="D205:D210" si="17">$D$204*C205</f>
+        <f t="shared" ref="D205:D210" si="19">$D$204*C205</f>
         <v>110.30865786510142</v>
       </c>
       <c r="E205" s="63">
-        <f t="shared" ref="E205:E210" si="18">$E$204*C205</f>
+        <f t="shared" ref="E205:E210" si="20">$E$204*C205</f>
         <v>66.185194719060846</v>
       </c>
       <c r="F205" s="63">
-        <f t="shared" ref="F205:F210" si="19">$F$204*C205</f>
+        <f t="shared" ref="F205:F210" si="21">$F$204*C205</f>
         <v>39.711116831436506</v>
       </c>
       <c r="H205">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>66.683764924100856</v>
       </c>
       <c r="I205">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>22.62262305369029</v>
       </c>
       <c r="J205">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2.1313876265460272</v>
       </c>
       <c r="K205">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>91.437775604337176</v>
       </c>
       <c r="M205" s="52"/>
@@ -10753,35 +10795,35 @@
         <v>15</v>
       </c>
       <c r="C206" s="59">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
+      <c r="D206" s="63">
+        <f t="shared" si="19"/>
+        <v>78</v>
+      </c>
+      <c r="E206" s="63">
+        <f t="shared" si="20"/>
+        <v>46.8</v>
+      </c>
+      <c r="F206" s="63">
+        <f t="shared" si="21"/>
+        <v>28.08</v>
+      </c>
+      <c r="H206">
         <f t="shared" si="16"/>
-        <v>0.5</v>
-      </c>
-      <c r="D206" s="63">
+        <v>59.710344827586205</v>
+      </c>
+      <c r="I206">
+        <f t="shared" si="15"/>
+        <v>9.5213793103448268</v>
+      </c>
+      <c r="J206">
+        <f t="shared" si="15"/>
+        <v>0.87144827586206886</v>
+      </c>
+      <c r="K206">
         <f t="shared" si="17"/>
-        <v>78</v>
-      </c>
-      <c r="E206" s="63">
-        <f t="shared" si="18"/>
-        <v>46.8</v>
-      </c>
-      <c r="F206" s="63">
-        <f t="shared" si="19"/>
-        <v>28.08</v>
-      </c>
-      <c r="H206">
-        <f t="shared" si="14"/>
-        <v>59.710344827586205</v>
-      </c>
-      <c r="I206">
-        <f t="shared" si="13"/>
-        <v>9.5213793103448268</v>
-      </c>
-      <c r="J206">
-        <f t="shared" si="13"/>
-        <v>0.87144827586206886</v>
-      </c>
-      <c r="K206">
-        <f t="shared" si="15"/>
         <v>70.103172413793089</v>
       </c>
       <c r="N206" s="52"/>
@@ -10796,35 +10838,35 @@
         <v>20</v>
       </c>
       <c r="C207" s="59">
+        <f t="shared" si="18"/>
+        <v>0.35355339059327379</v>
+      </c>
+      <c r="D207" s="63">
+        <f t="shared" si="19"/>
+        <v>55.154328932550712</v>
+      </c>
+      <c r="E207" s="63">
+        <f t="shared" si="20"/>
+        <v>33.092597359530423</v>
+      </c>
+      <c r="F207" s="63">
+        <f t="shared" si="21"/>
+        <v>19.855558415718253</v>
+      </c>
+      <c r="H207">
         <f t="shared" si="16"/>
-        <v>0.35355339059327379</v>
-      </c>
-      <c r="D207" s="63">
+        <v>45.126269126632394</v>
+      </c>
+      <c r="I207">
+        <f t="shared" si="15"/>
+        <v>5.5540023540470642</v>
+      </c>
+      <c r="J207">
+        <f t="shared" si="15"/>
+        <v>0.2777001177023532</v>
+      </c>
+      <c r="K207">
         <f t="shared" si="17"/>
-        <v>55.154328932550712</v>
-      </c>
-      <c r="E207" s="63">
-        <f t="shared" si="18"/>
-        <v>33.092597359530423</v>
-      </c>
-      <c r="F207" s="63">
-        <f t="shared" si="19"/>
-        <v>19.855558415718253</v>
-      </c>
-      <c r="H207">
-        <f t="shared" si="14"/>
-        <v>45.126269126632394</v>
-      </c>
-      <c r="I207">
-        <f t="shared" si="13"/>
-        <v>5.5540023540470642</v>
-      </c>
-      <c r="J207">
-        <f t="shared" si="13"/>
-        <v>0.2777001177023532</v>
-      </c>
-      <c r="K207">
-        <f t="shared" si="15"/>
         <v>50.95797159838181</v>
       </c>
     </row>
@@ -10836,35 +10878,35 @@
         <v>25</v>
       </c>
       <c r="C208" s="59">
+        <f t="shared" si="18"/>
+        <v>0.25</v>
+      </c>
+      <c r="D208" s="63">
+        <f t="shared" si="19"/>
+        <v>39</v>
+      </c>
+      <c r="E208" s="63">
+        <f t="shared" si="20"/>
+        <v>23.4</v>
+      </c>
+      <c r="F208" s="63">
+        <f t="shared" si="21"/>
+        <v>14.04</v>
+      </c>
+      <c r="H208">
         <f t="shared" si="16"/>
-        <v>0.25</v>
-      </c>
-      <c r="D208" s="63">
+        <v>33.179104477611936</v>
+      </c>
+      <c r="I208">
+        <f t="shared" si="15"/>
+        <v>3.4691373134328458</v>
+      </c>
+      <c r="J208">
+        <f t="shared" si="15"/>
+        <v>1.4039999999999999E-2</v>
+      </c>
+      <c r="K208">
         <f t="shared" si="17"/>
-        <v>39</v>
-      </c>
-      <c r="E208" s="63">
-        <f t="shared" si="18"/>
-        <v>23.4</v>
-      </c>
-      <c r="F208" s="63">
-        <f t="shared" si="19"/>
-        <v>14.04</v>
-      </c>
-      <c r="H208">
-        <f t="shared" si="14"/>
-        <v>33.179104477611936</v>
-      </c>
-      <c r="I208">
-        <f t="shared" si="13"/>
-        <v>3.4691373134328458</v>
-      </c>
-      <c r="J208">
-        <f t="shared" si="13"/>
-        <v>1.4039999999999999E-2</v>
-      </c>
-      <c r="K208">
-        <f t="shared" si="15"/>
         <v>36.662281791044784</v>
       </c>
     </row>
@@ -10876,35 +10918,35 @@
         <v>30</v>
       </c>
       <c r="C209" s="59">
+        <f t="shared" si="18"/>
+        <v>0.17677669529663689</v>
+      </c>
+      <c r="D209" s="63">
+        <f t="shared" si="19"/>
+        <v>27.577164466275356</v>
+      </c>
+      <c r="E209" s="63">
+        <f t="shared" si="20"/>
+        <v>16.546298679765211</v>
+      </c>
+      <c r="F209" s="63">
+        <f t="shared" si="21"/>
+        <v>9.9277792078591265</v>
+      </c>
+      <c r="H209">
         <f t="shared" si="16"/>
-        <v>0.17677669529663689</v>
-      </c>
-      <c r="D209" s="63">
+        <v>23.461169769816344</v>
+      </c>
+      <c r="I209">
+        <f t="shared" si="15"/>
+        <v>2.4530505191956467</v>
+      </c>
+      <c r="J209">
+        <f t="shared" si="15"/>
+        <v>9.9277792078591269E-3</v>
+      </c>
+      <c r="K209">
         <f t="shared" si="17"/>
-        <v>27.577164466275356</v>
-      </c>
-      <c r="E209" s="63">
-        <f t="shared" si="18"/>
-        <v>16.546298679765211</v>
-      </c>
-      <c r="F209" s="63">
-        <f t="shared" si="19"/>
-        <v>9.9277792078591265</v>
-      </c>
-      <c r="H209">
-        <f t="shared" si="14"/>
-        <v>23.461169769816344</v>
-      </c>
-      <c r="I209">
-        <f t="shared" si="13"/>
-        <v>2.4530505191956467</v>
-      </c>
-      <c r="J209">
-        <f t="shared" si="13"/>
-        <v>9.9277792078591269E-3</v>
-      </c>
-      <c r="K209">
-        <f t="shared" si="15"/>
         <v>25.92414806821985</v>
       </c>
     </row>
@@ -10916,35 +10958,35 @@
         <v>35</v>
       </c>
       <c r="C210" s="59">
+        <f t="shared" si="18"/>
+        <v>0.12500000000000003</v>
+      </c>
+      <c r="D210" s="63">
+        <f t="shared" si="19"/>
+        <v>19.500000000000004</v>
+      </c>
+      <c r="E210" s="63">
+        <f t="shared" si="20"/>
+        <v>11.700000000000001</v>
+      </c>
+      <c r="F210" s="63">
+        <f t="shared" si="21"/>
+        <v>7.0200000000000014</v>
+      </c>
+      <c r="H210">
         <f t="shared" si="16"/>
-        <v>0.12500000000000003</v>
-      </c>
-      <c r="D210" s="63">
+        <v>16.589552238805972</v>
+      </c>
+      <c r="I210">
+        <f t="shared" si="15"/>
+        <v>1.7345686567164231</v>
+      </c>
+      <c r="J210">
+        <f t="shared" si="15"/>
+        <v>7.0200000000000011E-3</v>
+      </c>
+      <c r="K210">
         <f t="shared" si="17"/>
-        <v>19.500000000000004</v>
-      </c>
-      <c r="E210" s="63">
-        <f t="shared" si="18"/>
-        <v>11.700000000000001</v>
-      </c>
-      <c r="F210" s="63">
-        <f t="shared" si="19"/>
-        <v>7.0200000000000014</v>
-      </c>
-      <c r="H210">
-        <f t="shared" si="14"/>
-        <v>16.589552238805972</v>
-      </c>
-      <c r="I210">
-        <f t="shared" si="13"/>
-        <v>1.7345686567164231</v>
-      </c>
-      <c r="J210">
-        <f t="shared" si="13"/>
-        <v>7.0200000000000011E-3</v>
-      </c>
-      <c r="K210">
-        <f t="shared" si="15"/>
         <v>18.331140895522395</v>
       </c>
     </row>
@@ -10972,19 +11014,19 @@
         <v>4.9638896039295632</v>
       </c>
       <c r="H211">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>11.730584884908172</v>
       </c>
       <c r="I211">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.2265252595978233</v>
       </c>
       <c r="J211">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4.9638896039295635E-3</v>
       </c>
       <c r="K211">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>12.962074034109925</v>
       </c>
     </row>
@@ -10996,7 +11038,7 @@
         <v>45</v>
       </c>
       <c r="C212" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>6.25E-2</v>
       </c>
       <c r="D212" s="63">
@@ -11012,19 +11054,19 @@
         <v>3.51</v>
       </c>
       <c r="H212">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>8.2947761194029841</v>
       </c>
       <c r="I212">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.86728432835821145</v>
       </c>
       <c r="J212">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3.5099999999999997E-3</v>
       </c>
       <c r="K212">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>9.1655704477611959</v>
       </c>
     </row>
@@ -11036,7 +11078,7 @@
         <v>50</v>
       </c>
       <c r="C213" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>4.4194173824159223E-2</v>
       </c>
       <c r="D213" s="63">
@@ -11052,19 +11094,19 @@
         <v>2.4819448019647816</v>
       </c>
       <c r="H213">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>5.865292442454086</v>
       </c>
       <c r="I213">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.61326262979891166</v>
       </c>
       <c r="J213">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2.4819448019647817E-3</v>
       </c>
       <c r="K213">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6.4810370170549625</v>
       </c>
     </row>
@@ -11076,7 +11118,7 @@
         <v>55</v>
       </c>
       <c r="C214" s="59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.125E-2</v>
       </c>
       <c r="D214" s="63">
@@ -11092,19 +11134,19 @@
         <v>1.7549999999999999</v>
       </c>
       <c r="H214">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>4.147388059701492</v>
       </c>
       <c r="I214">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.43364216417910573</v>
       </c>
       <c r="J214">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.7549999999999998E-3</v>
       </c>
       <c r="K214">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4.5827852238805979</v>
       </c>
     </row>
@@ -11125,29 +11167,29 @@
       </c>
     </row>
     <row r="216" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A216" s="81" t="s">
+      <c r="A216" s="104" t="s">
         <v>92</v>
       </c>
-      <c r="B216" s="81"/>
-      <c r="C216" s="81"/>
-      <c r="D216" s="81"/>
-      <c r="E216" s="81"/>
-      <c r="F216" s="81"/>
+      <c r="B216" s="104"/>
+      <c r="C216" s="104"/>
+      <c r="D216" s="104"/>
+      <c r="E216" s="104"/>
+      <c r="F216" s="104"/>
     </row>
     <row r="217" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A217" s="82" t="s">
+      <c r="A217" s="105" t="s">
         <v>2</v>
       </c>
       <c r="B217" s="59"/>
       <c r="C217" s="59"/>
-      <c r="D217" s="80" t="s">
+      <c r="D217" s="103" t="s">
         <v>58</v>
       </c>
-      <c r="E217" s="80"/>
-      <c r="F217" s="80"/>
+      <c r="E217" s="103"/>
+      <c r="F217" s="103"/>
     </row>
     <row r="218" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A218" s="82"/>
+      <c r="A218" s="105"/>
       <c r="B218" s="59"/>
       <c r="C218" s="60" t="s">
         <v>54</v>
@@ -11288,7 +11330,7 @@
         <v>10</v>
       </c>
       <c r="C225" s="59">
-        <f t="shared" ref="C225:C234" si="20">EXP(LN(0.5)*B224/10)</f>
+        <f t="shared" ref="C225:C234" si="22">EXP(LN(0.5)*B224/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D225" s="62">
@@ -11312,19 +11354,19 @@
         <v>15</v>
       </c>
       <c r="C226" s="59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.5</v>
       </c>
       <c r="D226" s="62">
-        <f t="shared" ref="D226:D232" si="21">$D$224*C226</f>
+        <f t="shared" ref="D226:D232" si="23">$D$224*C226</f>
         <v>78</v>
       </c>
       <c r="E226" s="62">
-        <f t="shared" ref="E226:E232" si="22">$E$224*C226</f>
+        <f t="shared" ref="E226:E232" si="24">$E$224*C226</f>
         <v>46.8</v>
       </c>
       <c r="F226" s="62">
-        <f t="shared" ref="F226:F232" si="23">$F$224*C226</f>
+        <f t="shared" ref="F226:F232" si="25">$F$224*C226</f>
         <v>28.08</v>
       </c>
     </row>
@@ -11336,19 +11378,19 @@
         <v>20</v>
       </c>
       <c r="C227" s="59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.35355339059327379</v>
       </c>
       <c r="D227" s="62">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>55.154328932550712</v>
       </c>
       <c r="E227" s="62">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>33.092597359530423</v>
       </c>
       <c r="F227" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>19.855558415718253</v>
       </c>
     </row>
@@ -11360,19 +11402,19 @@
         <v>25</v>
       </c>
       <c r="C228" s="59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.25</v>
       </c>
       <c r="D228" s="62">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>39</v>
       </c>
       <c r="E228" s="62">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>23.4</v>
       </c>
       <c r="F228" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>14.04</v>
       </c>
     </row>
@@ -11384,19 +11426,19 @@
         <v>30</v>
       </c>
       <c r="C229" s="59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.17677669529663689</v>
       </c>
       <c r="D229" s="62">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>27.577164466275356</v>
       </c>
       <c r="E229" s="62">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>16.546298679765211</v>
       </c>
       <c r="F229" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>9.9277792078591265</v>
       </c>
     </row>
@@ -11408,19 +11450,19 @@
         <v>35</v>
       </c>
       <c r="C230" s="59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.12500000000000003</v>
       </c>
       <c r="D230" s="62">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>19.500000000000004</v>
       </c>
       <c r="E230" s="62">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>11.700000000000001</v>
       </c>
       <c r="F230" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>7.0200000000000014</v>
       </c>
     </row>
@@ -11432,19 +11474,19 @@
         <v>40</v>
       </c>
       <c r="C231" s="59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>8.8388347648318447E-2</v>
       </c>
       <c r="D231" s="62">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>13.788582233137678</v>
       </c>
       <c r="E231" s="62">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>8.2731493398826057</v>
       </c>
       <c r="F231" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>4.9638896039295632</v>
       </c>
     </row>
@@ -11456,19 +11498,19 @@
         <v>45</v>
       </c>
       <c r="C232" s="59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>6.25E-2</v>
       </c>
       <c r="D232" s="62">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>9.75</v>
       </c>
       <c r="E232" s="62">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>5.85</v>
       </c>
       <c r="F232" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>3.51</v>
       </c>
     </row>
@@ -11504,7 +11546,7 @@
         <v>55</v>
       </c>
       <c r="C234" s="59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>3.125E-2</v>
       </c>
       <c r="D234" s="62">
@@ -11590,6 +11632,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="I130:I132"/>
+    <mergeCell ref="J130:O130"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="A216:F216"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="B158:D158"/>
+    <mergeCell ref="E158:G158"/>
+    <mergeCell ref="A183:C183"/>
+    <mergeCell ref="A195:F195"/>
+    <mergeCell ref="A196:F196"/>
+    <mergeCell ref="D197:F197"/>
+    <mergeCell ref="D217:F217"/>
     <mergeCell ref="A109:A111"/>
     <mergeCell ref="B109:G109"/>
     <mergeCell ref="B130:G130"/>
@@ -11602,18 +11656,6 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="B81:B83"/>
-    <mergeCell ref="I130:I132"/>
-    <mergeCell ref="J130:O130"/>
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="A216:F216"/>
-    <mergeCell ref="A217:A218"/>
-    <mergeCell ref="B158:D158"/>
-    <mergeCell ref="E158:G158"/>
-    <mergeCell ref="A183:C183"/>
-    <mergeCell ref="A195:F195"/>
-    <mergeCell ref="A196:F196"/>
-    <mergeCell ref="D197:F197"/>
-    <mergeCell ref="D217:F217"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reduce fertility decrease by 2010 to 0.75*fertility matrix.
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="106">
   <si>
     <t>Male</t>
   </si>
@@ -552,6 +552,9 @@
   </si>
   <si>
     <t>&lt;--should use UNICEF data here instead?</t>
+  </si>
+  <si>
+    <t>File MORT/17-2: Abridged life tables, for males/females, 1950-2100</t>
   </si>
 </sst>
 </file>
@@ -1622,13 +1625,13 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1638,39 +1641,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1694,7 +1664,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -1806,7 +1809,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2321,7 +2323,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6150,7 +6151,7 @@
   <dimension ref="A1:AF239"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J136" sqref="J136"/>
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6279,10 +6280,10 @@
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="96"/>
+      <c r="C4" s="105"/>
     </row>
     <row r="5" spans="1:25" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="53"/>
@@ -6519,10 +6520,10 @@
       <c r="A27" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="97" t="s">
+      <c r="B27" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="98"/>
+      <c r="C27" s="106"/>
     </row>
     <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="12"/>
@@ -6910,19 +6911,19 @@
       <c r="AE51" s="32"/>
     </row>
     <row r="52" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="102" t="s">
+      <c r="A52" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="102" t="s">
+      <c r="B52" s="110" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="102"/>
-      <c r="D52" s="102"/>
-      <c r="E52" s="102" t="s">
+      <c r="C52" s="110"/>
+      <c r="D52" s="110"/>
+      <c r="E52" s="110" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="102"/>
-      <c r="G52" s="102"/>
+      <c r="F52" s="110"/>
+      <c r="G52" s="110"/>
       <c r="X52" s="30"/>
       <c r="Y52" s="30"/>
       <c r="Z52" s="30"/>
@@ -6933,7 +6934,7 @@
       <c r="AE52" s="30"/>
     </row>
     <row r="53" spans="1:31" ht="30" x14ac:dyDescent="0.35">
-      <c r="A53" s="102"/>
+      <c r="A53" s="110"/>
       <c r="B53" s="45" t="s">
         <v>6</v>
       </c>
@@ -7467,23 +7468,26 @@
       <c r="X80" s="50"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A81" s="86" t="s">
+      <c r="A81" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="99" t="s">
+      <c r="B81" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="99" t="s">
+      <c r="C81" s="107" t="s">
         <v>4</v>
       </c>
       <c r="H81" t="s">
         <v>102</v>
       </c>
+      <c r="K81" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A82" s="87"/>
-      <c r="B82" s="100"/>
-      <c r="C82" s="100"/>
+      <c r="A82" s="102"/>
+      <c r="B82" s="108"/>
+      <c r="C82" s="108"/>
       <c r="I82" s="77" t="s">
         <v>98</v>
       </c>
@@ -7495,9 +7499,9 @@
       </c>
     </row>
     <row r="83" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="88"/>
-      <c r="B83" s="101"/>
-      <c r="C83" s="101"/>
+      <c r="A83" s="103"/>
+      <c r="B83" s="109"/>
+      <c r="C83" s="109"/>
       <c r="E83" t="s">
         <v>99</v>
       </c>
@@ -8136,7 +8140,7 @@
       <c r="X108" s="50"/>
     </row>
     <row r="109" spans="1:24" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="86" t="s">
+      <c r="A109" s="101" t="s">
         <v>2</v>
       </c>
       <c r="B109" s="89" t="s">
@@ -8149,7 +8153,7 @@
       <c r="G109" s="91"/>
     </row>
     <row r="110" spans="1:24" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="87"/>
+      <c r="A110" s="102"/>
       <c r="B110" s="44" t="s">
         <v>83</v>
       </c>
@@ -8170,7 +8174,7 @@
       </c>
     </row>
     <row r="111" spans="1:24" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="88"/>
+      <c r="A111" s="103"/>
       <c r="B111" s="46" t="s">
         <v>76</v>
       </c>
@@ -8625,7 +8629,7 @@
     </row>
     <row r="129" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="130" spans="1:15" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="92" t="s">
+      <c r="A130" s="86" t="s">
         <v>2</v>
       </c>
       <c r="B130" s="89" t="s">
@@ -8636,7 +8640,7 @@
       <c r="E130" s="90"/>
       <c r="F130" s="90"/>
       <c r="G130" s="91"/>
-      <c r="I130" s="92" t="s">
+      <c r="I130" s="86" t="s">
         <v>2</v>
       </c>
       <c r="J130" s="89" t="s">
@@ -8649,7 +8653,7 @@
       <c r="O130" s="91"/>
     </row>
     <row r="131" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="93"/>
+      <c r="A131" s="87"/>
       <c r="B131" s="34" t="s">
         <v>84</v>
       </c>
@@ -8668,7 +8672,7 @@
       <c r="G131" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="I131" s="93"/>
+      <c r="I131" s="87"/>
       <c r="J131" s="34" t="s">
         <v>84</v>
       </c>
@@ -8689,7 +8693,7 @@
       </c>
     </row>
     <row r="132" spans="1:15" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="94"/>
+      <c r="A132" s="88"/>
       <c r="B132" s="55" t="s">
         <v>76</v>
       </c>
@@ -8708,7 +8712,7 @@
       <c r="G132" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="I132" s="94"/>
+      <c r="I132" s="88"/>
       <c r="J132" s="55" t="s">
         <v>76</v>
       </c>
@@ -8865,55 +8869,55 @@
         <v>18</v>
       </c>
       <c r="B136" s="27">
-        <f>B115*0.65</f>
-        <v>9.1910000000000006E-2</v>
+        <f>B115*0.75</f>
+        <v>0.10605000000000001</v>
       </c>
       <c r="C136" s="27">
-        <f t="shared" ref="C136:G136" si="4">C115*0.65</f>
-        <v>9.1910000000000006E-2</v>
+        <f t="shared" ref="C136:G136" si="4">C115*0.75</f>
+        <v>0.10605000000000001</v>
       </c>
       <c r="D136" s="27">
         <f t="shared" si="4"/>
-        <v>9.1910000000000006E-2</v>
+        <v>0.10605000000000001</v>
       </c>
       <c r="E136" s="27">
         <f t="shared" si="4"/>
-        <v>5.3307800000000009E-2</v>
+        <v>6.1509000000000008E-2</v>
       </c>
       <c r="F136" s="27">
         <f t="shared" si="4"/>
-        <v>5.3307800000000009E-2</v>
+        <v>6.1509000000000008E-2</v>
       </c>
       <c r="G136" s="27">
         <f t="shared" si="4"/>
-        <v>3.7683100000000004E-2</v>
+        <v>4.3480500000000005E-2</v>
       </c>
       <c r="I136" s="72" t="s">
         <v>18</v>
       </c>
       <c r="J136" s="27">
         <f>B136*0.75</f>
-        <v>6.8932500000000008E-2</v>
+        <v>7.9537500000000011E-2</v>
       </c>
       <c r="K136" s="27">
         <f t="shared" ref="K136:O142" si="5">C136*0.75</f>
-        <v>6.8932500000000008E-2</v>
+        <v>7.9537500000000011E-2</v>
       </c>
       <c r="L136" s="27">
         <f t="shared" si="5"/>
-        <v>6.8932500000000008E-2</v>
+        <v>7.9537500000000011E-2</v>
       </c>
       <c r="M136" s="27">
         <f t="shared" si="5"/>
-        <v>3.9980850000000005E-2</v>
+        <v>4.6131750000000006E-2</v>
       </c>
       <c r="N136" s="27">
         <f t="shared" si="5"/>
-        <v>3.9980850000000005E-2</v>
+        <v>4.6131750000000006E-2</v>
       </c>
       <c r="O136" s="27">
         <f t="shared" si="5"/>
-        <v>2.8262325000000005E-2</v>
+        <v>3.2610375000000004E-2</v>
       </c>
     </row>
     <row r="137" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -8921,55 +8925,55 @@
         <v>19</v>
       </c>
       <c r="B137" s="27">
-        <f t="shared" ref="B137:G142" si="6">B116*0.65</f>
-        <v>0.18070000000000003</v>
+        <f t="shared" ref="B137:G142" si="6">B116*0.75</f>
+        <v>0.20850000000000002</v>
       </c>
       <c r="C137" s="27">
         <f t="shared" si="6"/>
-        <v>0.18070000000000003</v>
+        <v>0.20850000000000002</v>
       </c>
       <c r="D137" s="27">
         <f t="shared" si="6"/>
-        <v>0.18070000000000003</v>
+        <v>0.20850000000000002</v>
       </c>
       <c r="E137" s="27">
         <f t="shared" si="6"/>
-        <v>0.10480600000000002</v>
+        <v>0.12093000000000001</v>
       </c>
       <c r="F137" s="27">
         <f t="shared" si="6"/>
-        <v>0.10480600000000002</v>
+        <v>0.12093000000000001</v>
       </c>
       <c r="G137" s="27">
         <f t="shared" si="6"/>
-        <v>7.4087000000000014E-2</v>
+        <v>8.5485000000000019E-2</v>
       </c>
       <c r="I137" s="72" t="s">
         <v>19</v>
       </c>
       <c r="J137" s="27">
         <f t="shared" ref="J137:J142" si="7">B137*0.75</f>
-        <v>0.13552500000000001</v>
+        <v>0.15637500000000001</v>
       </c>
       <c r="K137" s="27">
         <f t="shared" si="5"/>
-        <v>0.13552500000000001</v>
+        <v>0.15637500000000001</v>
       </c>
       <c r="L137" s="27">
         <f t="shared" si="5"/>
-        <v>0.13552500000000001</v>
+        <v>0.15637500000000001</v>
       </c>
       <c r="M137" s="27">
         <f t="shared" si="5"/>
-        <v>7.8604500000000022E-2</v>
+        <v>9.0697500000000014E-2</v>
       </c>
       <c r="N137" s="27">
         <f t="shared" si="5"/>
-        <v>7.8604500000000022E-2</v>
+        <v>9.0697500000000014E-2</v>
       </c>
       <c r="O137" s="27">
         <f t="shared" si="5"/>
-        <v>5.556525000000001E-2</v>
+        <v>6.4113750000000011E-2</v>
       </c>
     </row>
     <row r="138" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -8978,54 +8982,54 @@
       </c>
       <c r="B138" s="27">
         <f t="shared" si="6"/>
-        <v>0.18434000000000003</v>
+        <v>0.2127</v>
       </c>
       <c r="C138" s="27">
         <f t="shared" si="6"/>
-        <v>0.18434000000000003</v>
+        <v>0.2127</v>
       </c>
       <c r="D138" s="27">
         <f t="shared" si="6"/>
-        <v>0.18434000000000003</v>
+        <v>0.2127</v>
       </c>
       <c r="E138" s="27">
         <f t="shared" si="6"/>
-        <v>0.10691720000000002</v>
+        <v>0.12336600000000002</v>
       </c>
       <c r="F138" s="27">
         <f t="shared" si="6"/>
-        <v>0.10691720000000002</v>
+        <v>0.12336600000000002</v>
       </c>
       <c r="G138" s="27">
         <f t="shared" si="6"/>
-        <v>7.5579400000000019E-2</v>
+        <v>8.7207000000000007E-2</v>
       </c>
       <c r="I138" s="72" t="s">
         <v>20</v>
       </c>
       <c r="J138" s="27">
         <f t="shared" si="7"/>
-        <v>0.13825500000000002</v>
+        <v>0.159525</v>
       </c>
       <c r="K138" s="27">
         <f t="shared" si="5"/>
-        <v>0.13825500000000002</v>
+        <v>0.159525</v>
       </c>
       <c r="L138" s="27">
         <f t="shared" si="5"/>
-        <v>0.13825500000000002</v>
+        <v>0.159525</v>
       </c>
       <c r="M138" s="27">
         <f t="shared" si="5"/>
-        <v>8.0187900000000006E-2</v>
+        <v>9.252450000000001E-2</v>
       </c>
       <c r="N138" s="27">
         <f t="shared" si="5"/>
-        <v>8.0187900000000006E-2</v>
+        <v>9.252450000000001E-2</v>
       </c>
       <c r="O138" s="27">
         <f t="shared" si="5"/>
-        <v>5.6684550000000014E-2</v>
+        <v>6.5405249999999998E-2</v>
       </c>
     </row>
     <row r="139" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9034,54 +9038,54 @@
       </c>
       <c r="B139" s="27">
         <f t="shared" si="6"/>
-        <v>0.13728000000000001</v>
+        <v>0.15839999999999999</v>
       </c>
       <c r="C139" s="27">
         <f t="shared" si="6"/>
-        <v>0.13728000000000001</v>
+        <v>0.15839999999999999</v>
       </c>
       <c r="D139" s="27">
         <f t="shared" si="6"/>
-        <v>0.13728000000000001</v>
+        <v>0.15839999999999999</v>
       </c>
       <c r="E139" s="27">
         <f t="shared" si="6"/>
-        <v>7.962240000000001E-2</v>
+        <v>9.1872000000000009E-2</v>
       </c>
       <c r="F139" s="27">
         <f t="shared" si="6"/>
-        <v>7.962240000000001E-2</v>
+        <v>9.1872000000000009E-2</v>
       </c>
       <c r="G139" s="27">
         <f t="shared" si="6"/>
-        <v>5.6284800000000003E-2</v>
+        <v>6.4944000000000002E-2</v>
       </c>
       <c r="I139" s="72" t="s">
         <v>23</v>
       </c>
       <c r="J139" s="27">
         <f t="shared" si="7"/>
-        <v>0.10296000000000001</v>
+        <v>0.11879999999999999</v>
       </c>
       <c r="K139" s="27">
         <f t="shared" si="5"/>
-        <v>0.10296000000000001</v>
+        <v>0.11879999999999999</v>
       </c>
       <c r="L139" s="27">
         <f t="shared" si="5"/>
-        <v>0.10296000000000001</v>
+        <v>0.11879999999999999</v>
       </c>
       <c r="M139" s="27">
         <f t="shared" si="5"/>
-        <v>5.9716800000000007E-2</v>
+        <v>6.8904000000000007E-2</v>
       </c>
       <c r="N139" s="27">
         <f t="shared" si="5"/>
-        <v>5.9716800000000007E-2</v>
+        <v>6.8904000000000007E-2</v>
       </c>
       <c r="O139" s="27">
         <f t="shared" si="5"/>
-        <v>4.2213600000000004E-2</v>
+        <v>4.8708000000000001E-2</v>
       </c>
     </row>
     <row r="140" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9090,54 +9094,54 @@
       </c>
       <c r="B140" s="27">
         <f t="shared" si="6"/>
-        <v>8.7620000000000003E-2</v>
+        <v>0.1011</v>
       </c>
       <c r="C140" s="27">
         <f t="shared" si="6"/>
-        <v>8.7620000000000003E-2</v>
+        <v>0.1011</v>
       </c>
       <c r="D140" s="27">
         <f t="shared" si="6"/>
-        <v>8.7620000000000003E-2</v>
+        <v>0.1011</v>
       </c>
       <c r="E140" s="27">
         <f t="shared" si="6"/>
-        <v>5.0819600000000013E-2</v>
+        <v>5.863800000000001E-2</v>
       </c>
       <c r="F140" s="27">
         <f t="shared" si="6"/>
-        <v>5.0819600000000013E-2</v>
+        <v>5.863800000000001E-2</v>
       </c>
       <c r="G140" s="27">
         <f t="shared" si="6"/>
-        <v>3.5924200000000003E-2</v>
+        <v>4.1451000000000002E-2</v>
       </c>
       <c r="I140" s="72" t="s">
         <v>22</v>
       </c>
       <c r="J140" s="27">
         <f t="shared" si="7"/>
-        <v>6.5714999999999996E-2</v>
+        <v>7.5825000000000004E-2</v>
       </c>
       <c r="K140" s="27">
         <f t="shared" si="5"/>
-        <v>6.5714999999999996E-2</v>
+        <v>7.5825000000000004E-2</v>
       </c>
       <c r="L140" s="27">
         <f t="shared" si="5"/>
-        <v>6.5714999999999996E-2</v>
+        <v>7.5825000000000004E-2</v>
       </c>
       <c r="M140" s="27">
         <f t="shared" si="5"/>
-        <v>3.8114700000000008E-2</v>
+        <v>4.3978500000000004E-2</v>
       </c>
       <c r="N140" s="27">
         <f t="shared" si="5"/>
-        <v>3.8114700000000008E-2</v>
+        <v>4.3978500000000004E-2</v>
       </c>
       <c r="O140" s="27">
         <f t="shared" si="5"/>
-        <v>2.6943150000000003E-2</v>
+        <v>3.1088250000000001E-2</v>
       </c>
     </row>
     <row r="141" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9146,54 +9150,54 @@
       </c>
       <c r="B141" s="27">
         <f t="shared" si="6"/>
-        <v>3.5230000000000004E-2</v>
+        <v>4.0650000000000006E-2</v>
       </c>
       <c r="C141" s="27">
         <f t="shared" si="6"/>
-        <v>3.5230000000000004E-2</v>
+        <v>4.0650000000000006E-2</v>
       </c>
       <c r="D141" s="27">
         <f t="shared" si="6"/>
-        <v>3.5230000000000004E-2</v>
+        <v>4.0650000000000006E-2</v>
       </c>
       <c r="E141" s="27">
         <f t="shared" si="6"/>
-        <v>2.0433400000000004E-2</v>
+        <v>2.3577000000000004E-2</v>
       </c>
       <c r="F141" s="27">
         <f t="shared" si="6"/>
-        <v>2.0433400000000004E-2</v>
+        <v>2.3577000000000004E-2</v>
       </c>
       <c r="G141" s="27">
         <f t="shared" si="6"/>
-        <v>1.4444300000000002E-2</v>
+        <v>1.6666500000000001E-2</v>
       </c>
       <c r="I141" s="72" t="s">
         <v>24</v>
       </c>
       <c r="J141" s="27">
         <f t="shared" si="7"/>
-        <v>2.6422500000000002E-2</v>
+        <v>3.0487500000000004E-2</v>
       </c>
       <c r="K141" s="27">
         <f t="shared" si="5"/>
-        <v>2.6422500000000002E-2</v>
+        <v>3.0487500000000004E-2</v>
       </c>
       <c r="L141" s="27">
         <f t="shared" si="5"/>
-        <v>2.6422500000000002E-2</v>
+        <v>3.0487500000000004E-2</v>
       </c>
       <c r="M141" s="27">
         <f t="shared" si="5"/>
-        <v>1.5325050000000003E-2</v>
+        <v>1.7682750000000004E-2</v>
       </c>
       <c r="N141" s="27">
         <f t="shared" si="5"/>
-        <v>1.5325050000000003E-2</v>
+        <v>1.7682750000000004E-2</v>
       </c>
       <c r="O141" s="27">
         <f t="shared" si="5"/>
-        <v>1.0833225000000002E-2</v>
+        <v>1.2499875000000001E-2</v>
       </c>
     </row>
     <row r="142" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9202,54 +9206,54 @@
       </c>
       <c r="B142" s="27">
         <f t="shared" si="6"/>
-        <v>1.1440000000000001E-2</v>
+        <v>1.32E-2</v>
       </c>
       <c r="C142" s="27">
         <f t="shared" si="6"/>
-        <v>1.1440000000000001E-2</v>
+        <v>1.32E-2</v>
       </c>
       <c r="D142" s="27">
         <f t="shared" si="6"/>
-        <v>1.1440000000000001E-2</v>
+        <v>1.32E-2</v>
       </c>
       <c r="E142" s="27">
         <f t="shared" si="6"/>
-        <v>6.6352000000000017E-3</v>
+        <v>7.6560000000000013E-3</v>
       </c>
       <c r="F142" s="27">
         <f t="shared" si="6"/>
-        <v>6.6352000000000017E-3</v>
+        <v>7.6560000000000013E-3</v>
       </c>
       <c r="G142" s="27">
         <f t="shared" si="6"/>
-        <v>4.6904000000000008E-3</v>
+        <v>5.412000000000001E-3</v>
       </c>
       <c r="I142" s="72" t="s">
         <v>25</v>
       </c>
       <c r="J142" s="27">
         <f t="shared" si="7"/>
-        <v>8.5800000000000008E-3</v>
+        <v>9.8999999999999991E-3</v>
       </c>
       <c r="K142" s="27">
         <f t="shared" si="5"/>
-        <v>8.5800000000000008E-3</v>
+        <v>9.8999999999999991E-3</v>
       </c>
       <c r="L142" s="27">
         <f t="shared" si="5"/>
-        <v>8.5800000000000008E-3</v>
+        <v>9.8999999999999991E-3</v>
       </c>
       <c r="M142" s="27">
         <f t="shared" si="5"/>
-        <v>4.9764000000000015E-3</v>
+        <v>5.7420000000000006E-3</v>
       </c>
       <c r="N142" s="27">
         <f t="shared" si="5"/>
-        <v>4.9764000000000015E-3</v>
+        <v>5.7420000000000006E-3</v>
       </c>
       <c r="O142" s="27">
         <f t="shared" si="5"/>
-        <v>3.5178000000000006E-3</v>
+        <v>4.059000000000001E-3</v>
       </c>
     </row>
     <row r="143" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9519,51 +9523,51 @@
     <row r="149" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B149">
         <f t="shared" ref="B149:G149" si="8">5*SUM(B133:B148)</f>
-        <v>3.6426000000000003</v>
+        <v>4.2029999999999994</v>
       </c>
       <c r="C149">
         <f t="shared" si="8"/>
-        <v>3.6426000000000003</v>
+        <v>4.2029999999999994</v>
       </c>
       <c r="D149">
         <f t="shared" si="8"/>
-        <v>3.6426000000000003</v>
+        <v>4.2029999999999994</v>
       </c>
       <c r="E149">
         <f t="shared" si="8"/>
-        <v>2.112708</v>
+        <v>2.4377400000000007</v>
       </c>
       <c r="F149">
         <f t="shared" si="8"/>
-        <v>2.112708</v>
+        <v>2.4377400000000007</v>
       </c>
       <c r="G149">
         <f t="shared" si="8"/>
-        <v>1.4934660000000002</v>
+        <v>1.7232300000000003</v>
       </c>
       <c r="J149">
         <f t="shared" ref="J149:O149" si="9">5*SUM(J133:J148)</f>
-        <v>2.7319500000000003</v>
+        <v>3.1522500000000004</v>
       </c>
       <c r="K149">
         <f t="shared" si="9"/>
-        <v>2.7319500000000003</v>
+        <v>3.1522500000000004</v>
       </c>
       <c r="L149">
         <f t="shared" si="9"/>
-        <v>2.7319500000000003</v>
+        <v>3.1522500000000004</v>
       </c>
       <c r="M149">
         <f t="shared" si="9"/>
-        <v>1.5845310000000001</v>
+        <v>1.8283050000000003</v>
       </c>
       <c r="N149">
         <f t="shared" si="9"/>
-        <v>1.5845310000000001</v>
+        <v>1.8283050000000003</v>
       </c>
       <c r="O149">
         <f t="shared" si="9"/>
-        <v>1.1200995000000002</v>
+        <v>1.2924225</v>
       </c>
     </row>
     <row r="155" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
@@ -9651,16 +9655,16 @@
       <c r="A158" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B158" s="106" t="s">
-        <v>0</v>
-      </c>
-      <c r="C158" s="107"/>
-      <c r="D158" s="108"/>
-      <c r="E158" s="106" t="s">
+      <c r="B158" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" s="96"/>
+      <c r="D158" s="97"/>
+      <c r="E158" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="F158" s="107"/>
-      <c r="G158" s="108"/>
+      <c r="F158" s="96"/>
+      <c r="G158" s="97"/>
     </row>
     <row r="159" spans="1:23" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A159" s="6"/>
@@ -10411,11 +10415,11 @@
       <c r="W182" s="50"/>
     </row>
     <row r="183" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A183" s="109" t="s">
+      <c r="A183" s="98" t="s">
         <v>89</v>
       </c>
-      <c r="B183" s="109"/>
-      <c r="C183" s="109"/>
+      <c r="B183" s="98"/>
+      <c r="C183" s="98"/>
     </row>
     <row r="184" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A184" s="1" t="s">
@@ -10489,39 +10493,39 @@
       <c r="W194" s="50"/>
     </row>
     <row r="195" spans="1:23" s="52" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A195" s="97" t="s">
+      <c r="A195" s="99" t="s">
         <v>90</v>
       </c>
-      <c r="B195" s="97"/>
-      <c r="C195" s="97"/>
-      <c r="D195" s="97"/>
-      <c r="E195" s="97"/>
-      <c r="F195" s="97"/>
+      <c r="B195" s="99"/>
+      <c r="C195" s="99"/>
+      <c r="D195" s="99"/>
+      <c r="E195" s="99"/>
+      <c r="F195" s="99"/>
     </row>
     <row r="196" spans="1:23" s="52" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A196" s="110" t="s">
+      <c r="A196" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="B196" s="110"/>
-      <c r="C196" s="110"/>
-      <c r="D196" s="110"/>
-      <c r="E196" s="110"/>
-      <c r="F196" s="110"/>
+      <c r="B196" s="100"/>
+      <c r="C196" s="100"/>
+      <c r="D196" s="100"/>
+      <c r="E196" s="100"/>
+      <c r="F196" s="100"/>
     </row>
     <row r="197" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A197" s="103" t="s">
+      <c r="A197" s="92" t="s">
         <v>53</v>
       </c>
       <c r="B197" s="59"/>
       <c r="C197" s="59"/>
-      <c r="D197" s="103" t="s">
+      <c r="D197" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="E197" s="103"/>
-      <c r="F197" s="103"/>
+      <c r="E197" s="92"/>
+      <c r="F197" s="92"/>
     </row>
     <row r="198" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A198" s="103"/>
+      <c r="A198" s="92"/>
       <c r="B198" s="59"/>
       <c r="C198" s="60" t="s">
         <v>54</v>
@@ -11167,29 +11171,29 @@
       </c>
     </row>
     <row r="216" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A216" s="104" t="s">
+      <c r="A216" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="B216" s="104"/>
-      <c r="C216" s="104"/>
-      <c r="D216" s="104"/>
-      <c r="E216" s="104"/>
-      <c r="F216" s="104"/>
+      <c r="B216" s="93"/>
+      <c r="C216" s="93"/>
+      <c r="D216" s="93"/>
+      <c r="E216" s="93"/>
+      <c r="F216" s="93"/>
     </row>
     <row r="217" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A217" s="105" t="s">
+      <c r="A217" s="94" t="s">
         <v>2</v>
       </c>
       <c r="B217" s="59"/>
       <c r="C217" s="59"/>
-      <c r="D217" s="103" t="s">
+      <c r="D217" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="E217" s="103"/>
-      <c r="F217" s="103"/>
+      <c r="E217" s="92"/>
+      <c r="F217" s="92"/>
     </row>
     <row r="218" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A218" s="105"/>
+      <c r="A218" s="94"/>
       <c r="B218" s="59"/>
       <c r="C218" s="60" t="s">
         <v>54</v>
@@ -11632,6 +11636,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A109:A111"/>
+    <mergeCell ref="B109:G109"/>
+    <mergeCell ref="B130:G130"/>
+    <mergeCell ref="A130:A132"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="B81:B83"/>
     <mergeCell ref="I130:I132"/>
     <mergeCell ref="J130:O130"/>
     <mergeCell ref="A197:A198"/>
@@ -11644,18 +11660,6 @@
     <mergeCell ref="A196:F196"/>
     <mergeCell ref="D197:F197"/>
     <mergeCell ref="D217:F217"/>
-    <mergeCell ref="A109:A111"/>
-    <mergeCell ref="B109:G109"/>
-    <mergeCell ref="B130:G130"/>
-    <mergeCell ref="A130:A132"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="B81:B83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change fertility matrices back to original values: fertility2=0.5*fertility, fertility3=0.75*fertility2. Update popInit using KZN:SA population proportion and back-calculating KZN by gender assuming exponential distributions by age. Math done in excel docs, save new values in popInitProjExp mat file and re-load in loadUp2.
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -1427,7 +1427,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1624,6 +1624,8 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1809,6 +1811,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2323,6 +2326,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2445,7 +2449,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3141,7 +3144,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3269,7 +3271,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3958,7 +3959,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6150,8 +6150,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F141" sqref="F141"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6164,7 +6164,7 @@
     <col min="6" max="6" width="16.81640625" customWidth="1"/>
     <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.81640625" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25" customWidth="1"/>
@@ -6280,10 +6280,10 @@
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="105"/>
+      <c r="C4" s="107"/>
     </row>
     <row r="5" spans="1:25" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="53"/>
@@ -6304,6 +6304,20 @@
       <c r="C6" s="13">
         <v>417311</v>
       </c>
+      <c r="F6" s="86">
+        <v>116.45919703766501</v>
+      </c>
+      <c r="G6" s="87">
+        <v>156.85219677743601</v>
+      </c>
+      <c r="H6" s="52">
+        <f>F6*1000</f>
+        <v>116459.19703766501</v>
+      </c>
+      <c r="I6" s="52">
+        <f>G6*1000</f>
+        <v>156852.19677743601</v>
+      </c>
     </row>
     <row r="7" spans="1:25" ht="33.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
@@ -6315,6 +6329,20 @@
       <c r="C7" s="13">
         <v>361594</v>
       </c>
+      <c r="F7" s="86">
+        <v>76.187743222862409</v>
+      </c>
+      <c r="G7" s="87">
+        <v>102.61289100384487</v>
+      </c>
+      <c r="H7" s="52">
+        <f t="shared" ref="H7:H21" si="0">F7*1000</f>
+        <v>76187.743222862409</v>
+      </c>
+      <c r="I7" s="52">
+        <f t="shared" ref="I7:I21" si="1">G7*1000</f>
+        <v>102612.89100384487</v>
+      </c>
     </row>
     <row r="8" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
@@ -6326,6 +6354,20 @@
       <c r="C8" s="13">
         <v>329333</v>
       </c>
+      <c r="F8" s="86">
+        <v>75.385542052984889</v>
+      </c>
+      <c r="G8" s="87">
+        <v>87.786369045850634</v>
+      </c>
+      <c r="H8" s="52">
+        <f t="shared" si="0"/>
+        <v>75385.542052984893</v>
+      </c>
+      <c r="I8" s="52">
+        <f t="shared" si="1"/>
+        <v>87786.369045850632</v>
+      </c>
     </row>
     <row r="9" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
@@ -6337,6 +6379,20 @@
       <c r="C9" s="13">
         <v>296947</v>
       </c>
+      <c r="F9" s="86">
+        <v>71.896515135187158</v>
+      </c>
+      <c r="G9" s="87">
+        <v>63.757104105268432</v>
+      </c>
+      <c r="H9" s="52">
+        <f t="shared" si="0"/>
+        <v>71896.515135187161</v>
+      </c>
+      <c r="I9" s="52">
+        <f t="shared" si="1"/>
+        <v>63757.10410526843</v>
+      </c>
     </row>
     <row r="10" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
@@ -6348,6 +6404,20 @@
       <c r="C10" s="13">
         <v>273204</v>
       </c>
+      <c r="F10" s="86">
+        <v>51.997757864486189</v>
+      </c>
+      <c r="G10" s="87">
+        <v>51.450259534369195</v>
+      </c>
+      <c r="H10" s="52">
+        <f t="shared" si="0"/>
+        <v>51997.757864486186</v>
+      </c>
+      <c r="I10" s="52">
+        <f t="shared" si="1"/>
+        <v>51450.259534369194</v>
+      </c>
     </row>
     <row r="11" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
@@ -6359,6 +6429,20 @@
       <c r="C11" s="13">
         <v>249396</v>
       </c>
+      <c r="F11" s="86">
+        <v>46.60176948050119</v>
+      </c>
+      <c r="G11" s="87">
+        <v>43.513908158546549</v>
+      </c>
+      <c r="H11" s="52">
+        <f t="shared" si="0"/>
+        <v>46601.769480501192</v>
+      </c>
+      <c r="I11" s="52">
+        <f t="shared" si="1"/>
+        <v>43513.908158546546</v>
+      </c>
     </row>
     <row r="12" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
@@ -6370,6 +6454,20 @@
       <c r="C12" s="13">
         <v>211839</v>
       </c>
+      <c r="F12" s="86">
+        <v>38.908922911901001</v>
+      </c>
+      <c r="G12" s="87">
+        <v>53.232318780424968</v>
+      </c>
+      <c r="H12" s="52">
+        <f t="shared" si="0"/>
+        <v>38908.922911900998</v>
+      </c>
+      <c r="I12" s="52">
+        <f t="shared" si="1"/>
+        <v>53232.318780424968</v>
+      </c>
     </row>
     <row r="13" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
@@ -6381,6 +6479,20 @@
       <c r="C13" s="13">
         <v>176470</v>
       </c>
+      <c r="F13" s="86">
+        <v>32.485982807963815</v>
+      </c>
+      <c r="G13" s="87">
+        <v>31.805477141060052</v>
+      </c>
+      <c r="H13" s="52">
+        <f t="shared" si="0"/>
+        <v>32485.982807963814</v>
+      </c>
+      <c r="I13" s="52">
+        <f t="shared" si="1"/>
+        <v>31805.477141060052</v>
+      </c>
     </row>
     <row r="14" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
@@ -6392,6 +6504,20 @@
       <c r="C14" s="13">
         <v>143351</v>
       </c>
+      <c r="F14" s="86">
+        <v>48.105368931368112</v>
+      </c>
+      <c r="G14" s="87">
+        <v>43.876145321947618</v>
+      </c>
+      <c r="H14" s="52">
+        <f t="shared" si="0"/>
+        <v>48105.36893136811</v>
+      </c>
+      <c r="I14" s="52">
+        <f t="shared" si="1"/>
+        <v>43876.145321947617</v>
+      </c>
     </row>
     <row r="15" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
@@ -6403,6 +6529,20 @@
       <c r="C15" s="13">
         <v>123441</v>
       </c>
+      <c r="F15" s="86">
+        <v>27.123317738423211</v>
+      </c>
+      <c r="G15" s="87">
+        <v>29.945252135950131</v>
+      </c>
+      <c r="H15" s="52">
+        <f t="shared" si="0"/>
+        <v>27123.317738423211</v>
+      </c>
+      <c r="I15" s="52">
+        <f t="shared" si="1"/>
+        <v>29945.25213595013</v>
+      </c>
     </row>
     <row r="16" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
@@ -6414,6 +6554,20 @@
       <c r="C16" s="13">
         <v>98355</v>
       </c>
+      <c r="F16" s="86">
+        <v>26.837729055778073</v>
+      </c>
+      <c r="G16" s="87">
+        <v>18.123756746459325</v>
+      </c>
+      <c r="H16" s="52">
+        <f t="shared" si="0"/>
+        <v>26837.729055778073</v>
+      </c>
+      <c r="I16" s="52">
+        <f t="shared" si="1"/>
+        <v>18123.756746459323</v>
+      </c>
     </row>
     <row r="17" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
@@ -6425,6 +6579,20 @@
       <c r="C17" s="23">
         <v>82330</v>
       </c>
+      <c r="F17" s="86">
+        <v>18.123756746459325</v>
+      </c>
+      <c r="G17" s="87">
+        <v>22.803929628009573</v>
+      </c>
+      <c r="H17" s="52">
+        <f t="shared" si="0"/>
+        <v>18123.756746459323</v>
+      </c>
+      <c r="I17" s="52">
+        <f t="shared" si="1"/>
+        <v>22803.929628009573</v>
+      </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
@@ -6438,6 +6606,20 @@
         <f>366793/6.36</f>
         <v>57671.85534591195</v>
       </c>
+      <c r="F18" s="86">
+        <v>13.980530844150357</v>
+      </c>
+      <c r="G18" s="87">
+        <v>19.286357512430385</v>
+      </c>
+      <c r="H18" s="52">
+        <f t="shared" si="0"/>
+        <v>13980.530844150357</v>
+      </c>
+      <c r="I18" s="52">
+        <f t="shared" si="1"/>
+        <v>19286.357512430386</v>
+      </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
@@ -6451,6 +6633,20 @@
         <f>282911/6.36</f>
         <v>44482.861635220121</v>
       </c>
+      <c r="F19" s="86">
+        <v>8.1781693204119676</v>
+      </c>
+      <c r="G19" s="87">
+        <v>13.333477747336939</v>
+      </c>
+      <c r="H19" s="52">
+        <f t="shared" si="0"/>
+        <v>8178.1693204119674</v>
+      </c>
+      <c r="I19" s="52">
+        <f t="shared" si="1"/>
+        <v>13333.47774733694</v>
+      </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
@@ -6464,6 +6660,20 @@
         <f>215469/6.36</f>
         <v>33878.773584905655</v>
       </c>
+      <c r="F20" s="86">
+        <v>6.7562521870106114</v>
+      </c>
+      <c r="G20" s="87">
+        <v>8.591408456529452</v>
+      </c>
+      <c r="H20" s="52">
+        <f t="shared" si="0"/>
+        <v>6756.2521870106111</v>
+      </c>
+      <c r="I20" s="52">
+        <f t="shared" si="1"/>
+        <v>8591.4084565294525</v>
+      </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
@@ -6477,6 +6687,20 @@
         <f>144901/6.36</f>
         <v>22783.176100628931</v>
       </c>
+      <c r="F21" s="86">
+        <v>4.250473607017895</v>
+      </c>
+      <c r="G21" s="87">
+        <v>3.0486932223679761</v>
+      </c>
+      <c r="H21" s="52">
+        <f t="shared" si="0"/>
+        <v>4250.4736070178951</v>
+      </c>
+      <c r="I21" s="52">
+        <f t="shared" si="1"/>
+        <v>3048.693222367976</v>
+      </c>
     </row>
     <row r="22" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="24" t="s">
@@ -6494,6 +6718,10 @@
         <f>SUM(B22:C22)</f>
         <v>5703373.2934609242</v>
       </c>
+      <c r="I22">
+        <f>SUM(H6:I21)</f>
+        <v>1413298.5742620032</v>
+      </c>
       <c r="X22" s="17"/>
     </row>
     <row r="23" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
@@ -6520,10 +6748,10 @@
       <c r="A27" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="99" t="s">
+      <c r="B27" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="106"/>
+      <c r="C27" s="108"/>
     </row>
     <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="12"/>
@@ -6911,19 +7139,19 @@
       <c r="AE51" s="32"/>
     </row>
     <row r="52" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="110" t="s">
+      <c r="A52" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="110" t="s">
+      <c r="B52" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="110"/>
-      <c r="D52" s="110"/>
-      <c r="E52" s="110" t="s">
+      <c r="C52" s="112"/>
+      <c r="D52" s="112"/>
+      <c r="E52" s="112" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="110"/>
-      <c r="G52" s="110"/>
+      <c r="F52" s="112"/>
+      <c r="G52" s="112"/>
       <c r="X52" s="30"/>
       <c r="Y52" s="30"/>
       <c r="Z52" s="30"/>
@@ -6934,7 +7162,7 @@
       <c r="AE52" s="30"/>
     </row>
     <row r="53" spans="1:31" ht="30" x14ac:dyDescent="0.35">
-      <c r="A53" s="110"/>
+      <c r="A53" s="112"/>
       <c r="B53" s="45" t="s">
         <v>6</v>
       </c>
@@ -7006,7 +7234,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="14">
-        <f t="shared" ref="G55:G56" si="0">1-E55-F55</f>
+        <f t="shared" ref="G55:G56" si="2">1-E55-F55</f>
         <v>0</v>
       </c>
     </row>
@@ -7031,7 +7259,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G56" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.0000000000000183E-3</v>
       </c>
     </row>
@@ -7209,7 +7437,7 @@
         <v>0.85074626865671632</v>
       </c>
       <c r="C64" s="14">
-        <f t="shared" ref="C64:C69" si="1">0.149253731343284-0.001</f>
+        <f t="shared" ref="C64:C69" si="3">0.149253731343284-0.001</f>
         <v>0.14825373134328401</v>
       </c>
       <c r="D64" s="14">
@@ -7233,7 +7461,7 @@
         <v>0.85074626865671632</v>
       </c>
       <c r="C65" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.14825373134328401</v>
       </c>
       <c r="D65" s="14">
@@ -7257,7 +7485,7 @@
         <v>0.85074626865671632</v>
       </c>
       <c r="C66" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.14825373134328401</v>
       </c>
       <c r="D66" s="27">
@@ -7281,7 +7509,7 @@
         <v>0.85074626865671632</v>
       </c>
       <c r="C67" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.14825373134328401</v>
       </c>
       <c r="D67" s="27">
@@ -7305,7 +7533,7 @@
         <v>0.85074626865671632</v>
       </c>
       <c r="C68" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.14825373134328401</v>
       </c>
       <c r="D68" s="27">
@@ -7329,7 +7557,7 @@
         <v>0.85074626865671632</v>
       </c>
       <c r="C69" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.14825373134328401</v>
       </c>
       <c r="D69" s="27">
@@ -7354,23 +7582,23 @@
         <v>1.4676838219218388E-2</v>
       </c>
       <c r="C71">
-        <f t="shared" ref="C71:G71" si="2">PRODUCT(C54:C69)</f>
+        <f t="shared" ref="C71:G71" si="4">PRODUCT(C54:C69)</f>
         <v>0</v>
       </c>
       <c r="D71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.79671076610996394</v>
       </c>
       <c r="F71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -7468,13 +7696,13 @@
       <c r="X80" s="50"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A81" s="101" t="s">
+      <c r="A81" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="107" t="s">
+      <c r="B81" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="107" t="s">
+      <c r="C81" s="109" t="s">
         <v>4</v>
       </c>
       <c r="H81" t="s">
@@ -7485,9 +7713,9 @@
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A82" s="102"/>
-      <c r="B82" s="108"/>
-      <c r="C82" s="108"/>
+      <c r="A82" s="104"/>
+      <c r="B82" s="110"/>
+      <c r="C82" s="110"/>
       <c r="I82" s="77" t="s">
         <v>98</v>
       </c>
@@ -7499,9 +7727,9 @@
       </c>
     </row>
     <row r="83" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="103"/>
-      <c r="B83" s="109"/>
-      <c r="C83" s="109"/>
+      <c r="A83" s="105"/>
+      <c r="B83" s="111"/>
+      <c r="C83" s="111"/>
       <c r="E83" t="s">
         <v>99</v>
       </c>
@@ -8140,20 +8368,20 @@
       <c r="X108" s="50"/>
     </row>
     <row r="109" spans="1:24" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="101" t="s">
+      <c r="A109" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B109" s="89" t="s">
+      <c r="B109" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="C109" s="90"/>
-      <c r="D109" s="90"/>
-      <c r="E109" s="90"/>
-      <c r="F109" s="90"/>
-      <c r="G109" s="91"/>
+      <c r="C109" s="92"/>
+      <c r="D109" s="92"/>
+      <c r="E109" s="92"/>
+      <c r="F109" s="92"/>
+      <c r="G109" s="93"/>
     </row>
     <row r="110" spans="1:24" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="102"/>
+      <c r="A110" s="104"/>
       <c r="B110" s="44" t="s">
         <v>83</v>
       </c>
@@ -8174,7 +8402,7 @@
       </c>
     </row>
     <row r="111" spans="1:24" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="103"/>
+      <c r="A111" s="105"/>
       <c r="B111" s="46" t="s">
         <v>76</v>
       </c>
@@ -8603,57 +8831,57 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B128">
-        <f t="shared" ref="B128:G128" si="3">5*SUM(B115:B121)</f>
+        <f t="shared" ref="B128:G128" si="5">5*SUM(B115:B121)</f>
         <v>5.604000000000001</v>
       </c>
       <c r="C128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.604000000000001</v>
       </c>
       <c r="D128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.604000000000001</v>
       </c>
       <c r="E128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.2503200000000003</v>
       </c>
       <c r="F128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.2503200000000003</v>
       </c>
       <c r="G128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.2976400000000003</v>
       </c>
     </row>
     <row r="129" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="130" spans="1:15" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="86" t="s">
+      <c r="A130" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="B130" s="89" t="s">
+      <c r="B130" s="91" t="s">
         <v>96</v>
       </c>
-      <c r="C130" s="90"/>
-      <c r="D130" s="90"/>
-      <c r="E130" s="90"/>
-      <c r="F130" s="90"/>
-      <c r="G130" s="91"/>
-      <c r="I130" s="86" t="s">
+      <c r="C130" s="92"/>
+      <c r="D130" s="92"/>
+      <c r="E130" s="92"/>
+      <c r="F130" s="92"/>
+      <c r="G130" s="93"/>
+      <c r="I130" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="J130" s="89" t="s">
+      <c r="J130" s="91" t="s">
         <v>97</v>
       </c>
-      <c r="K130" s="90"/>
-      <c r="L130" s="90"/>
-      <c r="M130" s="90"/>
-      <c r="N130" s="90"/>
-      <c r="O130" s="91"/>
+      <c r="K130" s="92"/>
+      <c r="L130" s="92"/>
+      <c r="M130" s="92"/>
+      <c r="N130" s="92"/>
+      <c r="O130" s="93"/>
     </row>
     <row r="131" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="87"/>
+      <c r="A131" s="89"/>
       <c r="B131" s="34" t="s">
         <v>84</v>
       </c>
@@ -8672,7 +8900,7 @@
       <c r="G131" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="I131" s="87"/>
+      <c r="I131" s="89"/>
       <c r="J131" s="34" t="s">
         <v>84</v>
       </c>
@@ -8693,7 +8921,7 @@
       </c>
     </row>
     <row r="132" spans="1:15" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="88"/>
+      <c r="A132" s="90"/>
       <c r="B132" s="55" t="s">
         <v>76</v>
       </c>
@@ -8712,7 +8940,7 @@
       <c r="G132" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="I132" s="88"/>
+      <c r="I132" s="90"/>
       <c r="J132" s="55" t="s">
         <v>76</v>
       </c>
@@ -8869,55 +9097,55 @@
         <v>18</v>
       </c>
       <c r="B136" s="27">
-        <f>B115*0.75</f>
-        <v>0.10605000000000001</v>
+        <f>B115*0.5</f>
+        <v>7.0699999999999999E-2</v>
       </c>
       <c r="C136" s="27">
-        <f t="shared" ref="C136:G136" si="4">C115*0.75</f>
-        <v>0.10605000000000001</v>
+        <f t="shared" ref="C136:G136" si="6">C115*0.5</f>
+        <v>7.0699999999999999E-2</v>
       </c>
       <c r="D136" s="27">
-        <f t="shared" si="4"/>
-        <v>0.10605000000000001</v>
+        <f t="shared" si="6"/>
+        <v>7.0699999999999999E-2</v>
       </c>
       <c r="E136" s="27">
-        <f t="shared" si="4"/>
-        <v>6.1509000000000008E-2</v>
+        <f t="shared" si="6"/>
+        <v>4.1006000000000008E-2</v>
       </c>
       <c r="F136" s="27">
-        <f t="shared" si="4"/>
-        <v>6.1509000000000008E-2</v>
+        <f t="shared" si="6"/>
+        <v>4.1006000000000008E-2</v>
       </c>
       <c r="G136" s="27">
-        <f t="shared" si="4"/>
-        <v>4.3480500000000005E-2</v>
+        <f t="shared" si="6"/>
+        <v>2.8987000000000002E-2</v>
       </c>
       <c r="I136" s="72" t="s">
         <v>18</v>
       </c>
       <c r="J136" s="27">
         <f>B136*0.75</f>
-        <v>7.9537500000000011E-2</v>
+        <v>5.3025000000000003E-2</v>
       </c>
       <c r="K136" s="27">
-        <f t="shared" ref="K136:O142" si="5">C136*0.75</f>
-        <v>7.9537500000000011E-2</v>
+        <f t="shared" ref="K136:O142" si="7">C136*0.75</f>
+        <v>5.3025000000000003E-2</v>
       </c>
       <c r="L136" s="27">
-        <f t="shared" si="5"/>
-        <v>7.9537500000000011E-2</v>
+        <f t="shared" si="7"/>
+        <v>5.3025000000000003E-2</v>
       </c>
       <c r="M136" s="27">
-        <f t="shared" si="5"/>
-        <v>4.6131750000000006E-2</v>
+        <f t="shared" si="7"/>
+        <v>3.0754500000000004E-2</v>
       </c>
       <c r="N136" s="27">
-        <f t="shared" si="5"/>
-        <v>4.6131750000000006E-2</v>
+        <f t="shared" si="7"/>
+        <v>3.0754500000000004E-2</v>
       </c>
       <c r="O136" s="27">
-        <f t="shared" si="5"/>
-        <v>3.2610375000000004E-2</v>
+        <f t="shared" si="7"/>
+        <v>2.1740250000000003E-2</v>
       </c>
     </row>
     <row r="137" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -8925,55 +9153,55 @@
         <v>19</v>
       </c>
       <c r="B137" s="27">
-        <f t="shared" ref="B137:G142" si="6">B116*0.75</f>
-        <v>0.20850000000000002</v>
+        <f t="shared" ref="B137:G142" si="8">B116*0.5</f>
+        <v>0.13900000000000001</v>
       </c>
       <c r="C137" s="27">
-        <f t="shared" si="6"/>
-        <v>0.20850000000000002</v>
+        <f t="shared" si="8"/>
+        <v>0.13900000000000001</v>
       </c>
       <c r="D137" s="27">
-        <f t="shared" si="6"/>
-        <v>0.20850000000000002</v>
+        <f t="shared" si="8"/>
+        <v>0.13900000000000001</v>
       </c>
       <c r="E137" s="27">
-        <f t="shared" si="6"/>
-        <v>0.12093000000000001</v>
+        <f t="shared" si="8"/>
+        <v>8.0620000000000011E-2</v>
       </c>
       <c r="F137" s="27">
-        <f t="shared" si="6"/>
-        <v>0.12093000000000001</v>
+        <f t="shared" si="8"/>
+        <v>8.0620000000000011E-2</v>
       </c>
       <c r="G137" s="27">
-        <f t="shared" si="6"/>
-        <v>8.5485000000000019E-2</v>
+        <f t="shared" si="8"/>
+        <v>5.6990000000000013E-2</v>
       </c>
       <c r="I137" s="72" t="s">
         <v>19</v>
       </c>
       <c r="J137" s="27">
-        <f t="shared" ref="J137:J142" si="7">B137*0.75</f>
-        <v>0.15637500000000001</v>
+        <f t="shared" ref="J137:J142" si="9">B137*0.75</f>
+        <v>0.10425000000000001</v>
       </c>
       <c r="K137" s="27">
-        <f t="shared" si="5"/>
-        <v>0.15637500000000001</v>
+        <f t="shared" si="7"/>
+        <v>0.10425000000000001</v>
       </c>
       <c r="L137" s="27">
-        <f t="shared" si="5"/>
-        <v>0.15637500000000001</v>
+        <f t="shared" si="7"/>
+        <v>0.10425000000000001</v>
       </c>
       <c r="M137" s="27">
-        <f t="shared" si="5"/>
-        <v>9.0697500000000014E-2</v>
+        <f t="shared" si="7"/>
+        <v>6.0465000000000005E-2</v>
       </c>
       <c r="N137" s="27">
-        <f t="shared" si="5"/>
-        <v>9.0697500000000014E-2</v>
+        <f t="shared" si="7"/>
+        <v>6.0465000000000005E-2</v>
       </c>
       <c r="O137" s="27">
-        <f t="shared" si="5"/>
-        <v>6.4113750000000011E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.274250000000001E-2</v>
       </c>
     </row>
     <row r="138" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -8981,55 +9209,55 @@
         <v>20</v>
       </c>
       <c r="B138" s="27">
-        <f t="shared" si="6"/>
-        <v>0.2127</v>
+        <f t="shared" si="8"/>
+        <v>0.14180000000000001</v>
       </c>
       <c r="C138" s="27">
-        <f t="shared" si="6"/>
-        <v>0.2127</v>
+        <f t="shared" si="8"/>
+        <v>0.14180000000000001</v>
       </c>
       <c r="D138" s="27">
-        <f t="shared" si="6"/>
-        <v>0.2127</v>
+        <f t="shared" si="8"/>
+        <v>0.14180000000000001</v>
       </c>
       <c r="E138" s="27">
-        <f t="shared" si="6"/>
-        <v>0.12336600000000002</v>
+        <f t="shared" si="8"/>
+        <v>8.2244000000000012E-2</v>
       </c>
       <c r="F138" s="27">
-        <f t="shared" si="6"/>
-        <v>0.12336600000000002</v>
+        <f t="shared" si="8"/>
+        <v>8.2244000000000012E-2</v>
       </c>
       <c r="G138" s="27">
-        <f t="shared" si="6"/>
-        <v>8.7207000000000007E-2</v>
+        <f t="shared" si="8"/>
+        <v>5.8138000000000009E-2</v>
       </c>
       <c r="I138" s="72" t="s">
         <v>20</v>
       </c>
       <c r="J138" s="27">
+        <f t="shared" si="9"/>
+        <v>0.10635</v>
+      </c>
+      <c r="K138" s="27">
         <f t="shared" si="7"/>
-        <v>0.159525</v>
-      </c>
-      <c r="K138" s="27">
-        <f t="shared" si="5"/>
-        <v>0.159525</v>
+        <v>0.10635</v>
       </c>
       <c r="L138" s="27">
-        <f t="shared" si="5"/>
-        <v>0.159525</v>
+        <f t="shared" si="7"/>
+        <v>0.10635</v>
       </c>
       <c r="M138" s="27">
-        <f t="shared" si="5"/>
-        <v>9.252450000000001E-2</v>
+        <f t="shared" si="7"/>
+        <v>6.1683000000000009E-2</v>
       </c>
       <c r="N138" s="27">
-        <f t="shared" si="5"/>
-        <v>9.252450000000001E-2</v>
+        <f t="shared" si="7"/>
+        <v>6.1683000000000009E-2</v>
       </c>
       <c r="O138" s="27">
-        <f t="shared" si="5"/>
-        <v>6.5405249999999998E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.3603500000000003E-2</v>
       </c>
     </row>
     <row r="139" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9037,55 +9265,55 @@
         <v>23</v>
       </c>
       <c r="B139" s="27">
-        <f t="shared" si="6"/>
-        <v>0.15839999999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.1056</v>
       </c>
       <c r="C139" s="27">
-        <f t="shared" si="6"/>
-        <v>0.15839999999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.1056</v>
       </c>
       <c r="D139" s="27">
-        <f t="shared" si="6"/>
-        <v>0.15839999999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.1056</v>
       </c>
       <c r="E139" s="27">
-        <f t="shared" si="6"/>
-        <v>9.1872000000000009E-2</v>
+        <f t="shared" si="8"/>
+        <v>6.1248000000000004E-2</v>
       </c>
       <c r="F139" s="27">
-        <f t="shared" si="6"/>
-        <v>9.1872000000000009E-2</v>
+        <f t="shared" si="8"/>
+        <v>6.1248000000000004E-2</v>
       </c>
       <c r="G139" s="27">
-        <f t="shared" si="6"/>
-        <v>6.4944000000000002E-2</v>
+        <f t="shared" si="8"/>
+        <v>4.3296000000000001E-2</v>
       </c>
       <c r="I139" s="72" t="s">
         <v>23</v>
       </c>
       <c r="J139" s="27">
+        <f t="shared" si="9"/>
+        <v>7.9199999999999993E-2</v>
+      </c>
+      <c r="K139" s="27">
         <f t="shared" si="7"/>
-        <v>0.11879999999999999</v>
-      </c>
-      <c r="K139" s="27">
-        <f t="shared" si="5"/>
-        <v>0.11879999999999999</v>
+        <v>7.9199999999999993E-2</v>
       </c>
       <c r="L139" s="27">
-        <f t="shared" si="5"/>
-        <v>0.11879999999999999</v>
+        <f t="shared" si="7"/>
+        <v>7.9199999999999993E-2</v>
       </c>
       <c r="M139" s="27">
-        <f t="shared" si="5"/>
-        <v>6.8904000000000007E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.5936000000000005E-2</v>
       </c>
       <c r="N139" s="27">
-        <f t="shared" si="5"/>
-        <v>6.8904000000000007E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.5936000000000005E-2</v>
       </c>
       <c r="O139" s="27">
-        <f t="shared" si="5"/>
-        <v>4.8708000000000001E-2</v>
+        <f t="shared" si="7"/>
+        <v>3.2472000000000001E-2</v>
       </c>
     </row>
     <row r="140" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9093,55 +9321,55 @@
         <v>22</v>
       </c>
       <c r="B140" s="27">
-        <f t="shared" si="6"/>
-        <v>0.1011</v>
+        <f t="shared" si="8"/>
+        <v>6.7400000000000002E-2</v>
       </c>
       <c r="C140" s="27">
-        <f t="shared" si="6"/>
-        <v>0.1011</v>
+        <f t="shared" si="8"/>
+        <v>6.7400000000000002E-2</v>
       </c>
       <c r="D140" s="27">
-        <f t="shared" si="6"/>
-        <v>0.1011</v>
+        <f t="shared" si="8"/>
+        <v>6.7400000000000002E-2</v>
       </c>
       <c r="E140" s="27">
-        <f t="shared" si="6"/>
-        <v>5.863800000000001E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.9092000000000009E-2</v>
       </c>
       <c r="F140" s="27">
-        <f t="shared" si="6"/>
-        <v>5.863800000000001E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.9092000000000009E-2</v>
       </c>
       <c r="G140" s="27">
-        <f t="shared" si="6"/>
-        <v>4.1451000000000002E-2</v>
+        <f t="shared" si="8"/>
+        <v>2.7634000000000002E-2</v>
       </c>
       <c r="I140" s="72" t="s">
         <v>22</v>
       </c>
       <c r="J140" s="27">
+        <f t="shared" si="9"/>
+        <v>5.0549999999999998E-2</v>
+      </c>
+      <c r="K140" s="27">
         <f t="shared" si="7"/>
-        <v>7.5825000000000004E-2</v>
-      </c>
-      <c r="K140" s="27">
-        <f t="shared" si="5"/>
-        <v>7.5825000000000004E-2</v>
+        <v>5.0549999999999998E-2</v>
       </c>
       <c r="L140" s="27">
-        <f t="shared" si="5"/>
-        <v>7.5825000000000004E-2</v>
+        <f t="shared" si="7"/>
+        <v>5.0549999999999998E-2</v>
       </c>
       <c r="M140" s="27">
-        <f t="shared" si="5"/>
-        <v>4.3978500000000004E-2</v>
+        <f t="shared" si="7"/>
+        <v>2.9319000000000005E-2</v>
       </c>
       <c r="N140" s="27">
-        <f t="shared" si="5"/>
-        <v>4.3978500000000004E-2</v>
+        <f t="shared" si="7"/>
+        <v>2.9319000000000005E-2</v>
       </c>
       <c r="O140" s="27">
-        <f t="shared" si="5"/>
-        <v>3.1088250000000001E-2</v>
+        <f t="shared" si="7"/>
+        <v>2.0725500000000001E-2</v>
       </c>
     </row>
     <row r="141" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9149,55 +9377,55 @@
         <v>24</v>
       </c>
       <c r="B141" s="27">
-        <f t="shared" si="6"/>
-        <v>4.0650000000000006E-2</v>
+        <f t="shared" si="8"/>
+        <v>2.7100000000000003E-2</v>
       </c>
       <c r="C141" s="27">
-        <f t="shared" si="6"/>
-        <v>4.0650000000000006E-2</v>
+        <f t="shared" si="8"/>
+        <v>2.7100000000000003E-2</v>
       </c>
       <c r="D141" s="27">
-        <f t="shared" si="6"/>
-        <v>4.0650000000000006E-2</v>
+        <f t="shared" si="8"/>
+        <v>2.7100000000000003E-2</v>
       </c>
       <c r="E141" s="27">
-        <f t="shared" si="6"/>
-        <v>2.3577000000000004E-2</v>
+        <f t="shared" si="8"/>
+        <v>1.5718000000000003E-2</v>
       </c>
       <c r="F141" s="27">
-        <f t="shared" si="6"/>
-        <v>2.3577000000000004E-2</v>
+        <f t="shared" si="8"/>
+        <v>1.5718000000000003E-2</v>
       </c>
       <c r="G141" s="27">
-        <f t="shared" si="6"/>
-        <v>1.6666500000000001E-2</v>
+        <f t="shared" si="8"/>
+        <v>1.1111000000000001E-2</v>
       </c>
       <c r="I141" s="72" t="s">
         <v>24</v>
       </c>
       <c r="J141" s="27">
+        <f t="shared" si="9"/>
+        <v>2.0325000000000003E-2</v>
+      </c>
+      <c r="K141" s="27">
         <f t="shared" si="7"/>
-        <v>3.0487500000000004E-2</v>
-      </c>
-      <c r="K141" s="27">
-        <f t="shared" si="5"/>
-        <v>3.0487500000000004E-2</v>
+        <v>2.0325000000000003E-2</v>
       </c>
       <c r="L141" s="27">
-        <f t="shared" si="5"/>
-        <v>3.0487500000000004E-2</v>
+        <f t="shared" si="7"/>
+        <v>2.0325000000000003E-2</v>
       </c>
       <c r="M141" s="27">
-        <f t="shared" si="5"/>
-        <v>1.7682750000000004E-2</v>
+        <f t="shared" si="7"/>
+        <v>1.1788500000000002E-2</v>
       </c>
       <c r="N141" s="27">
-        <f t="shared" si="5"/>
-        <v>1.7682750000000004E-2</v>
+        <f t="shared" si="7"/>
+        <v>1.1788500000000002E-2</v>
       </c>
       <c r="O141" s="27">
-        <f t="shared" si="5"/>
-        <v>1.2499875000000001E-2</v>
+        <f t="shared" si="7"/>
+        <v>8.3332500000000004E-3</v>
       </c>
     </row>
     <row r="142" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9205,55 +9433,55 @@
         <v>25</v>
       </c>
       <c r="B142" s="27">
-        <f t="shared" si="6"/>
-        <v>1.32E-2</v>
+        <f t="shared" si="8"/>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="C142" s="27">
-        <f t="shared" si="6"/>
-        <v>1.32E-2</v>
+        <f t="shared" si="8"/>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="D142" s="27">
-        <f t="shared" si="6"/>
-        <v>1.32E-2</v>
+        <f t="shared" si="8"/>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="E142" s="27">
-        <f t="shared" si="6"/>
-        <v>7.6560000000000013E-3</v>
+        <f t="shared" si="8"/>
+        <v>5.1040000000000009E-3</v>
       </c>
       <c r="F142" s="27">
-        <f t="shared" si="6"/>
-        <v>7.6560000000000013E-3</v>
+        <f t="shared" si="8"/>
+        <v>5.1040000000000009E-3</v>
       </c>
       <c r="G142" s="27">
-        <f t="shared" si="6"/>
-        <v>5.412000000000001E-3</v>
+        <f t="shared" si="8"/>
+        <v>3.6080000000000005E-3</v>
       </c>
       <c r="I142" s="72" t="s">
         <v>25</v>
       </c>
       <c r="J142" s="27">
+        <f t="shared" si="9"/>
+        <v>6.6E-3</v>
+      </c>
+      <c r="K142" s="27">
         <f t="shared" si="7"/>
-        <v>9.8999999999999991E-3</v>
-      </c>
-      <c r="K142" s="27">
-        <f t="shared" si="5"/>
-        <v>9.8999999999999991E-3</v>
+        <v>6.6E-3</v>
       </c>
       <c r="L142" s="27">
-        <f t="shared" si="5"/>
-        <v>9.8999999999999991E-3</v>
+        <f t="shared" si="7"/>
+        <v>6.6E-3</v>
       </c>
       <c r="M142" s="27">
-        <f t="shared" si="5"/>
-        <v>5.7420000000000006E-3</v>
+        <f t="shared" si="7"/>
+        <v>3.8280000000000007E-3</v>
       </c>
       <c r="N142" s="27">
-        <f t="shared" si="5"/>
-        <v>5.7420000000000006E-3</v>
+        <f t="shared" si="7"/>
+        <v>3.8280000000000007E-3</v>
       </c>
       <c r="O142" s="27">
-        <f t="shared" si="5"/>
-        <v>4.059000000000001E-3</v>
+        <f t="shared" si="7"/>
+        <v>2.7060000000000005E-3</v>
       </c>
     </row>
     <row r="143" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -9522,52 +9750,52 @@
     </row>
     <row r="149" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B149">
-        <f t="shared" ref="B149:G149" si="8">5*SUM(B133:B148)</f>
-        <v>4.2029999999999994</v>
+        <f t="shared" ref="B149:G149" si="10">5*SUM(B133:B148)</f>
+        <v>2.8020000000000005</v>
       </c>
       <c r="C149">
-        <f t="shared" si="8"/>
-        <v>4.2029999999999994</v>
+        <f t="shared" si="10"/>
+        <v>2.8020000000000005</v>
       </c>
       <c r="D149">
-        <f t="shared" si="8"/>
-        <v>4.2029999999999994</v>
+        <f t="shared" si="10"/>
+        <v>2.8020000000000005</v>
       </c>
       <c r="E149">
-        <f t="shared" si="8"/>
-        <v>2.4377400000000007</v>
+        <f t="shared" si="10"/>
+        <v>1.6251600000000002</v>
       </c>
       <c r="F149">
-        <f t="shared" si="8"/>
-        <v>2.4377400000000007</v>
+        <f t="shared" si="10"/>
+        <v>1.6251600000000002</v>
       </c>
       <c r="G149">
-        <f t="shared" si="8"/>
-        <v>1.7232300000000003</v>
+        <f t="shared" si="10"/>
+        <v>1.1488200000000002</v>
       </c>
       <c r="J149">
-        <f t="shared" ref="J149:O149" si="9">5*SUM(J133:J148)</f>
-        <v>3.1522500000000004</v>
+        <f t="shared" ref="J149:O149" si="11">5*SUM(J133:J148)</f>
+        <v>2.1014999999999997</v>
       </c>
       <c r="K149">
-        <f t="shared" si="9"/>
-        <v>3.1522500000000004</v>
+        <f t="shared" si="11"/>
+        <v>2.1014999999999997</v>
       </c>
       <c r="L149">
-        <f t="shared" si="9"/>
-        <v>3.1522500000000004</v>
+        <f t="shared" si="11"/>
+        <v>2.1014999999999997</v>
       </c>
       <c r="M149">
-        <f t="shared" si="9"/>
-        <v>1.8283050000000003</v>
+        <f t="shared" si="11"/>
+        <v>1.2188700000000003</v>
       </c>
       <c r="N149">
-        <f t="shared" si="9"/>
-        <v>1.8283050000000003</v>
+        <f t="shared" si="11"/>
+        <v>1.2188700000000003</v>
       </c>
       <c r="O149">
-        <f t="shared" si="9"/>
-        <v>1.2924225</v>
+        <f t="shared" si="11"/>
+        <v>0.86161500000000013</v>
       </c>
     </row>
     <row r="155" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
@@ -9655,16 +9883,16 @@
       <c r="A158" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B158" s="95" t="s">
-        <v>0</v>
-      </c>
-      <c r="C158" s="96"/>
-      <c r="D158" s="97"/>
-      <c r="E158" s="95" t="s">
+      <c r="B158" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="C158" s="98"/>
+      <c r="D158" s="99"/>
+      <c r="E158" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="F158" s="96"/>
-      <c r="G158" s="97"/>
+      <c r="F158" s="98"/>
+      <c r="G158" s="99"/>
     </row>
     <row r="159" spans="1:23" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A159" s="6"/>
@@ -9692,15 +9920,15 @@
         <v>11</v>
       </c>
       <c r="B160" s="40">
-        <f t="shared" ref="B160:G161" si="10">10^-5</f>
+        <f t="shared" ref="B160:G161" si="12">10^-5</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C160" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D160" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E160" s="40">
@@ -9708,11 +9936,11 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F160" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="G160" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J160">
@@ -9720,11 +9948,11 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="K160">
-        <f t="shared" ref="K160:L175" si="11">C160*C54</f>
+        <f t="shared" ref="K160:L175" si="13">C160*C54</f>
         <v>0</v>
       </c>
       <c r="L160">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -9733,39 +9961,39 @@
         <v>14</v>
       </c>
       <c r="B161" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="C161" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D161" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E161" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F161" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="G161" s="40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J161">
-        <f t="shared" ref="J161:J175" si="12">B161*B55</f>
+        <f t="shared" ref="J161:J175" si="14">B161*B55</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="K161">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L161">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -9792,15 +10020,15 @@
         <v>1.2</v>
       </c>
       <c r="J162">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.176E-2</v>
       </c>
       <c r="K162">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.8E-3</v>
       </c>
       <c r="L162">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6.0000000000000218E-3</v>
       </c>
       <c r="M162">
@@ -9835,23 +10063,23 @@
         <v>6.5</v>
       </c>
       <c r="J163">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.33787878787878783</v>
       </c>
       <c r="K163">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.040909090909091</v>
       </c>
       <c r="L163">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.58030303030303021</v>
       </c>
       <c r="M163">
-        <f t="shared" ref="M163:M175" si="13">SUM(J163:L163)</f>
+        <f t="shared" ref="M163:M175" si="15">SUM(J163:L163)</f>
         <v>1.959090909090909</v>
       </c>
       <c r="N163">
-        <f t="shared" ref="N163:N175" si="14">1/M163</f>
+        <f t="shared" ref="N163:N175" si="16">1/M163</f>
         <v>0.51044083526682138</v>
       </c>
     </row>
@@ -9878,23 +10106,23 @@
         <v>10</v>
       </c>
       <c r="J164">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.33193277310924363</v>
       </c>
       <c r="K164">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.1274509803921566</v>
       </c>
       <c r="L164">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.65546218487394958</v>
       </c>
       <c r="M164">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2.1148459383753497</v>
       </c>
       <c r="N164">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.47284768211920541</v>
       </c>
     </row>
@@ -9921,23 +10149,23 @@
         <v>5.333333333333333</v>
       </c>
       <c r="J165">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.39310344827586208</v>
       </c>
       <c r="K165">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.0551724137931036</v>
       </c>
       <c r="L165">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.54482758620689653</v>
       </c>
       <c r="M165">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.9931034482758623</v>
       </c>
       <c r="N165">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.50173010380622829</v>
       </c>
     </row>
@@ -9964,23 +10192,23 @@
         <v>1</v>
       </c>
       <c r="J166">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.46610169491525422</v>
       </c>
       <c r="K166">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.84745762711864414</v>
       </c>
       <c r="L166">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.3135593220338983</v>
       </c>
       <c r="M166">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.6271186440677967</v>
       </c>
       <c r="N166">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.61458333333333326</v>
       </c>
     </row>
@@ -10007,23 +10235,23 @@
         <v>9</v>
       </c>
       <c r="J167">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.59655172413793101</v>
       </c>
       <c r="K167">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.48965517241379303</v>
       </c>
       <c r="L167">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.19310344827586207</v>
       </c>
       <c r="M167">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.279310344827586</v>
       </c>
       <c r="N167">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.78167115902964968</v>
       </c>
     </row>
@@ -10050,23 +10278,23 @@
         <v>1</v>
       </c>
       <c r="J168">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.68881118881118875</v>
       </c>
       <c r="K168">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.40559440559440557</v>
       </c>
       <c r="L168">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.10839160839160839</v>
       </c>
       <c r="M168">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.2027972027972027</v>
       </c>
       <c r="N168">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.83139534883720934</v>
       </c>
     </row>
@@ -10093,23 +10321,23 @@
         <v>1</v>
       </c>
       <c r="J169">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K169">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L169">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
       <c r="M169">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N169">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10136,23 +10364,23 @@
         <v>1</v>
       </c>
       <c r="J170">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K170">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L170">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
       <c r="M170">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N170">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10179,23 +10407,23 @@
         <v>1</v>
       </c>
       <c r="J171">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K171">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L171">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
       <c r="M171">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N171">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10222,23 +10450,23 @@
         <v>1</v>
       </c>
       <c r="J172">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K172">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L172">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
       <c r="M172">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N172">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10265,23 +10493,23 @@
         <v>1</v>
       </c>
       <c r="J173">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K173">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L173">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
       <c r="M173">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N173">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10308,23 +10536,23 @@
         <v>1</v>
       </c>
       <c r="J174">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K174">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L174">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
       <c r="M174">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N174">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10355,23 +10583,23 @@
         <v>1.8866801277495602</v>
       </c>
       <c r="J175">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.61194029850746268</v>
       </c>
       <c r="K175">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L175">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
       <c r="M175">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.95763022388059804</v>
       </c>
       <c r="N175">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -10415,11 +10643,11 @@
       <c r="W182" s="50"/>
     </row>
     <row r="183" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A183" s="98" t="s">
+      <c r="A183" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="B183" s="98"/>
-      <c r="C183" s="98"/>
+      <c r="B183" s="100"/>
+      <c r="C183" s="100"/>
     </row>
     <row r="184" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A184" s="1" t="s">
@@ -10493,39 +10721,39 @@
       <c r="W194" s="50"/>
     </row>
     <row r="195" spans="1:23" s="52" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A195" s="99" t="s">
+      <c r="A195" s="101" t="s">
         <v>90</v>
       </c>
-      <c r="B195" s="99"/>
-      <c r="C195" s="99"/>
-      <c r="D195" s="99"/>
-      <c r="E195" s="99"/>
-      <c r="F195" s="99"/>
+      <c r="B195" s="101"/>
+      <c r="C195" s="101"/>
+      <c r="D195" s="101"/>
+      <c r="E195" s="101"/>
+      <c r="F195" s="101"/>
     </row>
     <row r="196" spans="1:23" s="52" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A196" s="100" t="s">
+      <c r="A196" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="B196" s="100"/>
-      <c r="C196" s="100"/>
-      <c r="D196" s="100"/>
-      <c r="E196" s="100"/>
-      <c r="F196" s="100"/>
+      <c r="B196" s="102"/>
+      <c r="C196" s="102"/>
+      <c r="D196" s="102"/>
+      <c r="E196" s="102"/>
+      <c r="F196" s="102"/>
     </row>
     <row r="197" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A197" s="92" t="s">
+      <c r="A197" s="94" t="s">
         <v>53</v>
       </c>
       <c r="B197" s="59"/>
       <c r="C197" s="59"/>
-      <c r="D197" s="92" t="s">
+      <c r="D197" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="E197" s="92"/>
-      <c r="F197" s="92"/>
+      <c r="E197" s="94"/>
+      <c r="F197" s="94"/>
     </row>
     <row r="198" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A198" s="92"/>
+      <c r="A198" s="94"/>
       <c r="B198" s="59"/>
       <c r="C198" s="60" t="s">
         <v>54</v>
@@ -10564,11 +10792,11 @@
         <v>0</v>
       </c>
       <c r="I199">
-        <f t="shared" ref="I199:J214" si="15">E199*C54</f>
+        <f t="shared" ref="I199:J214" si="17">E199*C54</f>
         <v>0</v>
       </c>
       <c r="J199">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -10588,15 +10816,15 @@
         <v>0</v>
       </c>
       <c r="H200">
-        <f t="shared" ref="H200:H214" si="16">D200*B55</f>
+        <f t="shared" ref="H200:H214" si="18">D200*B55</f>
         <v>0</v>
       </c>
       <c r="I200">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="J200">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -10621,15 +10849,15 @@
         <v>1.1232</v>
       </c>
       <c r="H201">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.0576000000000003</v>
       </c>
       <c r="I201">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2.8079999999999997E-2</v>
       </c>
       <c r="J201">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5.6160000000000203E-3</v>
       </c>
       <c r="K201">
@@ -10658,19 +10886,19 @@
         <v>5.6159999999999997</v>
       </c>
       <c r="H202">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>7.9418181818181814</v>
       </c>
       <c r="I202">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3.814909090909091</v>
       </c>
       <c r="J202">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.46799999999999986</v>
       </c>
       <c r="K202">
-        <f t="shared" ref="K202:K214" si="17">SUM(H202:J202)</f>
+        <f t="shared" ref="K202:K214" si="19">SUM(H202:J202)</f>
         <v>12.224727272727272</v>
       </c>
     </row>
@@ -10697,19 +10925,19 @@
         <v>22.463999999999999</v>
       </c>
       <c r="H203">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>29.452100840336133</v>
       </c>
       <c r="I203">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>16.570084033613444</v>
       </c>
       <c r="J203">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.9191932773109244</v>
       </c>
       <c r="K203">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>47.941378151260501</v>
       </c>
     </row>
@@ -10734,19 +10962,19 @@
         <v>56.16</v>
       </c>
       <c r="H204">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>79.613793103448273</v>
       </c>
       <c r="I204">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>38.515862068965518</v>
       </c>
       <c r="J204">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4.38951724137931</v>
       </c>
       <c r="K204">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>122.5191724137931</v>
       </c>
     </row>
@@ -10758,35 +10986,35 @@
         <v>10</v>
       </c>
       <c r="C205" s="59">
-        <f t="shared" ref="C205:C214" si="18">EXP(LN(0.5)*B204/10)</f>
+        <f t="shared" ref="C205:C214" si="20">EXP(LN(0.5)*B204/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D205" s="63">
-        <f t="shared" ref="D205:D210" si="19">$D$204*C205</f>
+        <f t="shared" ref="D205:D210" si="21">$D$204*C205</f>
         <v>110.30865786510142</v>
       </c>
       <c r="E205" s="63">
-        <f t="shared" ref="E205:E210" si="20">$E$204*C205</f>
+        <f t="shared" ref="E205:E210" si="22">$E$204*C205</f>
         <v>66.185194719060846</v>
       </c>
       <c r="F205" s="63">
-        <f t="shared" ref="F205:F210" si="21">$F$204*C205</f>
+        <f t="shared" ref="F205:F210" si="23">$F$204*C205</f>
         <v>39.711116831436506</v>
       </c>
       <c r="H205">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>66.683764924100856</v>
       </c>
       <c r="I205">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>22.62262305369029</v>
       </c>
       <c r="J205">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2.1313876265460272</v>
       </c>
       <c r="K205">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>91.437775604337176</v>
       </c>
       <c r="M205" s="52"/>
@@ -10799,35 +11027,35 @@
         <v>15</v>
       </c>
       <c r="C206" s="59">
+        <f t="shared" si="20"/>
+        <v>0.5</v>
+      </c>
+      <c r="D206" s="63">
+        <f t="shared" si="21"/>
+        <v>78</v>
+      </c>
+      <c r="E206" s="63">
+        <f t="shared" si="22"/>
+        <v>46.8</v>
+      </c>
+      <c r="F206" s="63">
+        <f t="shared" si="23"/>
+        <v>28.08</v>
+      </c>
+      <c r="H206">
         <f t="shared" si="18"/>
-        <v>0.5</v>
-      </c>
-      <c r="D206" s="63">
+        <v>59.710344827586205</v>
+      </c>
+      <c r="I206">
+        <f t="shared" si="17"/>
+        <v>9.5213793103448268</v>
+      </c>
+      <c r="J206">
+        <f t="shared" si="17"/>
+        <v>0.87144827586206886</v>
+      </c>
+      <c r="K206">
         <f t="shared" si="19"/>
-        <v>78</v>
-      </c>
-      <c r="E206" s="63">
-        <f t="shared" si="20"/>
-        <v>46.8</v>
-      </c>
-      <c r="F206" s="63">
-        <f t="shared" si="21"/>
-        <v>28.08</v>
-      </c>
-      <c r="H206">
-        <f t="shared" si="16"/>
-        <v>59.710344827586205</v>
-      </c>
-      <c r="I206">
-        <f t="shared" si="15"/>
-        <v>9.5213793103448268</v>
-      </c>
-      <c r="J206">
-        <f t="shared" si="15"/>
-        <v>0.87144827586206886</v>
-      </c>
-      <c r="K206">
-        <f t="shared" si="17"/>
         <v>70.103172413793089</v>
       </c>
       <c r="N206" s="52"/>
@@ -10842,35 +11070,35 @@
         <v>20</v>
       </c>
       <c r="C207" s="59">
+        <f t="shared" si="20"/>
+        <v>0.35355339059327379</v>
+      </c>
+      <c r="D207" s="63">
+        <f t="shared" si="21"/>
+        <v>55.154328932550712</v>
+      </c>
+      <c r="E207" s="63">
+        <f t="shared" si="22"/>
+        <v>33.092597359530423</v>
+      </c>
+      <c r="F207" s="63">
+        <f t="shared" si="23"/>
+        <v>19.855558415718253</v>
+      </c>
+      <c r="H207">
         <f t="shared" si="18"/>
-        <v>0.35355339059327379</v>
-      </c>
-      <c r="D207" s="63">
+        <v>45.126269126632394</v>
+      </c>
+      <c r="I207">
+        <f t="shared" si="17"/>
+        <v>5.5540023540470642</v>
+      </c>
+      <c r="J207">
+        <f t="shared" si="17"/>
+        <v>0.2777001177023532</v>
+      </c>
+      <c r="K207">
         <f t="shared" si="19"/>
-        <v>55.154328932550712</v>
-      </c>
-      <c r="E207" s="63">
-        <f t="shared" si="20"/>
-        <v>33.092597359530423</v>
-      </c>
-      <c r="F207" s="63">
-        <f t="shared" si="21"/>
-        <v>19.855558415718253</v>
-      </c>
-      <c r="H207">
-        <f t="shared" si="16"/>
-        <v>45.126269126632394</v>
-      </c>
-      <c r="I207">
-        <f t="shared" si="15"/>
-        <v>5.5540023540470642</v>
-      </c>
-      <c r="J207">
-        <f t="shared" si="15"/>
-        <v>0.2777001177023532</v>
-      </c>
-      <c r="K207">
-        <f t="shared" si="17"/>
         <v>50.95797159838181</v>
       </c>
     </row>
@@ -10882,35 +11110,35 @@
         <v>25</v>
       </c>
       <c r="C208" s="59">
+        <f t="shared" si="20"/>
+        <v>0.25</v>
+      </c>
+      <c r="D208" s="63">
+        <f t="shared" si="21"/>
+        <v>39</v>
+      </c>
+      <c r="E208" s="63">
+        <f t="shared" si="22"/>
+        <v>23.4</v>
+      </c>
+      <c r="F208" s="63">
+        <f t="shared" si="23"/>
+        <v>14.04</v>
+      </c>
+      <c r="H208">
         <f t="shared" si="18"/>
-        <v>0.25</v>
-      </c>
-      <c r="D208" s="63">
+        <v>33.179104477611936</v>
+      </c>
+      <c r="I208">
+        <f t="shared" si="17"/>
+        <v>3.4691373134328458</v>
+      </c>
+      <c r="J208">
+        <f t="shared" si="17"/>
+        <v>1.4039999999999999E-2</v>
+      </c>
+      <c r="K208">
         <f t="shared" si="19"/>
-        <v>39</v>
-      </c>
-      <c r="E208" s="63">
-        <f t="shared" si="20"/>
-        <v>23.4</v>
-      </c>
-      <c r="F208" s="63">
-        <f t="shared" si="21"/>
-        <v>14.04</v>
-      </c>
-      <c r="H208">
-        <f t="shared" si="16"/>
-        <v>33.179104477611936</v>
-      </c>
-      <c r="I208">
-        <f t="shared" si="15"/>
-        <v>3.4691373134328458</v>
-      </c>
-      <c r="J208">
-        <f t="shared" si="15"/>
-        <v>1.4039999999999999E-2</v>
-      </c>
-      <c r="K208">
-        <f t="shared" si="17"/>
         <v>36.662281791044784</v>
       </c>
     </row>
@@ -10922,35 +11150,35 @@
         <v>30</v>
       </c>
       <c r="C209" s="59">
+        <f t="shared" si="20"/>
+        <v>0.17677669529663689</v>
+      </c>
+      <c r="D209" s="63">
+        <f t="shared" si="21"/>
+        <v>27.577164466275356</v>
+      </c>
+      <c r="E209" s="63">
+        <f t="shared" si="22"/>
+        <v>16.546298679765211</v>
+      </c>
+      <c r="F209" s="63">
+        <f t="shared" si="23"/>
+        <v>9.9277792078591265</v>
+      </c>
+      <c r="H209">
         <f t="shared" si="18"/>
-        <v>0.17677669529663689</v>
-      </c>
-      <c r="D209" s="63">
+        <v>23.461169769816344</v>
+      </c>
+      <c r="I209">
+        <f t="shared" si="17"/>
+        <v>2.4530505191956467</v>
+      </c>
+      <c r="J209">
+        <f t="shared" si="17"/>
+        <v>9.9277792078591269E-3</v>
+      </c>
+      <c r="K209">
         <f t="shared" si="19"/>
-        <v>27.577164466275356</v>
-      </c>
-      <c r="E209" s="63">
-        <f t="shared" si="20"/>
-        <v>16.546298679765211</v>
-      </c>
-      <c r="F209" s="63">
-        <f t="shared" si="21"/>
-        <v>9.9277792078591265</v>
-      </c>
-      <c r="H209">
-        <f t="shared" si="16"/>
-        <v>23.461169769816344</v>
-      </c>
-      <c r="I209">
-        <f t="shared" si="15"/>
-        <v>2.4530505191956467</v>
-      </c>
-      <c r="J209">
-        <f t="shared" si="15"/>
-        <v>9.9277792078591269E-3</v>
-      </c>
-      <c r="K209">
-        <f t="shared" si="17"/>
         <v>25.92414806821985</v>
       </c>
     </row>
@@ -10962,35 +11190,35 @@
         <v>35</v>
       </c>
       <c r="C210" s="59">
+        <f t="shared" si="20"/>
+        <v>0.12500000000000003</v>
+      </c>
+      <c r="D210" s="63">
+        <f t="shared" si="21"/>
+        <v>19.500000000000004</v>
+      </c>
+      <c r="E210" s="63">
+        <f t="shared" si="22"/>
+        <v>11.700000000000001</v>
+      </c>
+      <c r="F210" s="63">
+        <f t="shared" si="23"/>
+        <v>7.0200000000000014</v>
+      </c>
+      <c r="H210">
         <f t="shared" si="18"/>
-        <v>0.12500000000000003</v>
-      </c>
-      <c r="D210" s="63">
+        <v>16.589552238805972</v>
+      </c>
+      <c r="I210">
+        <f t="shared" si="17"/>
+        <v>1.7345686567164231</v>
+      </c>
+      <c r="J210">
+        <f t="shared" si="17"/>
+        <v>7.0200000000000011E-3</v>
+      </c>
+      <c r="K210">
         <f t="shared" si="19"/>
-        <v>19.500000000000004</v>
-      </c>
-      <c r="E210" s="63">
-        <f t="shared" si="20"/>
-        <v>11.700000000000001</v>
-      </c>
-      <c r="F210" s="63">
-        <f t="shared" si="21"/>
-        <v>7.0200000000000014</v>
-      </c>
-      <c r="H210">
-        <f t="shared" si="16"/>
-        <v>16.589552238805972</v>
-      </c>
-      <c r="I210">
-        <f t="shared" si="15"/>
-        <v>1.7345686567164231</v>
-      </c>
-      <c r="J210">
-        <f t="shared" si="15"/>
-        <v>7.0200000000000011E-3</v>
-      </c>
-      <c r="K210">
-        <f t="shared" si="17"/>
         <v>18.331140895522395</v>
       </c>
     </row>
@@ -11018,19 +11246,19 @@
         <v>4.9638896039295632</v>
       </c>
       <c r="H211">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>11.730584884908172</v>
       </c>
       <c r="I211">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.2265252595978233</v>
       </c>
       <c r="J211">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4.9638896039295635E-3</v>
       </c>
       <c r="K211">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>12.962074034109925</v>
       </c>
     </row>
@@ -11042,7 +11270,7 @@
         <v>45</v>
       </c>
       <c r="C212" s="59">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>6.25E-2</v>
       </c>
       <c r="D212" s="63">
@@ -11058,19 +11286,19 @@
         <v>3.51</v>
       </c>
       <c r="H212">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.2947761194029841</v>
       </c>
       <c r="I212">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.86728432835821145</v>
       </c>
       <c r="J212">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3.5099999999999997E-3</v>
       </c>
       <c r="K212">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>9.1655704477611959</v>
       </c>
     </row>
@@ -11082,7 +11310,7 @@
         <v>50</v>
       </c>
       <c r="C213" s="59">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>4.4194173824159223E-2</v>
       </c>
       <c r="D213" s="63">
@@ -11098,19 +11326,19 @@
         <v>2.4819448019647816</v>
       </c>
       <c r="H213">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5.865292442454086</v>
       </c>
       <c r="I213">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.61326262979891166</v>
       </c>
       <c r="J213">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2.4819448019647817E-3</v>
       </c>
       <c r="K213">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>6.4810370170549625</v>
       </c>
     </row>
@@ -11122,7 +11350,7 @@
         <v>55</v>
       </c>
       <c r="C214" s="59">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>3.125E-2</v>
       </c>
       <c r="D214" s="63">
@@ -11138,19 +11366,19 @@
         <v>1.7549999999999999</v>
       </c>
       <c r="H214">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>4.147388059701492</v>
       </c>
       <c r="I214">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.43364216417910573</v>
       </c>
       <c r="J214">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.7549999999999998E-3</v>
       </c>
       <c r="K214">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>4.5827852238805979</v>
       </c>
     </row>
@@ -11171,29 +11399,29 @@
       </c>
     </row>
     <row r="216" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A216" s="93" t="s">
+      <c r="A216" s="95" t="s">
         <v>92</v>
       </c>
-      <c r="B216" s="93"/>
-      <c r="C216" s="93"/>
-      <c r="D216" s="93"/>
-      <c r="E216" s="93"/>
-      <c r="F216" s="93"/>
+      <c r="B216" s="95"/>
+      <c r="C216" s="95"/>
+      <c r="D216" s="95"/>
+      <c r="E216" s="95"/>
+      <c r="F216" s="95"/>
     </row>
     <row r="217" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A217" s="94" t="s">
+      <c r="A217" s="96" t="s">
         <v>2</v>
       </c>
       <c r="B217" s="59"/>
       <c r="C217" s="59"/>
-      <c r="D217" s="92" t="s">
+      <c r="D217" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="E217" s="92"/>
-      <c r="F217" s="92"/>
+      <c r="E217" s="94"/>
+      <c r="F217" s="94"/>
     </row>
     <row r="218" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A218" s="94"/>
+      <c r="A218" s="96"/>
       <c r="B218" s="59"/>
       <c r="C218" s="60" t="s">
         <v>54</v>
@@ -11334,7 +11562,7 @@
         <v>10</v>
       </c>
       <c r="C225" s="59">
-        <f t="shared" ref="C225:C234" si="22">EXP(LN(0.5)*B224/10)</f>
+        <f t="shared" ref="C225:C234" si="24">EXP(LN(0.5)*B224/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D225" s="62">
@@ -11358,19 +11586,19 @@
         <v>15</v>
       </c>
       <c r="C226" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.5</v>
       </c>
       <c r="D226" s="62">
-        <f t="shared" ref="D226:D232" si="23">$D$224*C226</f>
+        <f t="shared" ref="D226:D232" si="25">$D$224*C226</f>
         <v>78</v>
       </c>
       <c r="E226" s="62">
-        <f t="shared" ref="E226:E232" si="24">$E$224*C226</f>
+        <f t="shared" ref="E226:E232" si="26">$E$224*C226</f>
         <v>46.8</v>
       </c>
       <c r="F226" s="62">
-        <f t="shared" ref="F226:F232" si="25">$F$224*C226</f>
+        <f t="shared" ref="F226:F232" si="27">$F$224*C226</f>
         <v>28.08</v>
       </c>
     </row>
@@ -11382,19 +11610,19 @@
         <v>20</v>
       </c>
       <c r="C227" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.35355339059327379</v>
       </c>
       <c r="D227" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>55.154328932550712</v>
       </c>
       <c r="E227" s="62">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>33.092597359530423</v>
       </c>
       <c r="F227" s="62">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>19.855558415718253</v>
       </c>
     </row>
@@ -11406,19 +11634,19 @@
         <v>25</v>
       </c>
       <c r="C228" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.25</v>
       </c>
       <c r="D228" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>39</v>
       </c>
       <c r="E228" s="62">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>23.4</v>
       </c>
       <c r="F228" s="62">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>14.04</v>
       </c>
     </row>
@@ -11430,19 +11658,19 @@
         <v>30</v>
       </c>
       <c r="C229" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.17677669529663689</v>
       </c>
       <c r="D229" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>27.577164466275356</v>
       </c>
       <c r="E229" s="62">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>16.546298679765211</v>
       </c>
       <c r="F229" s="62">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>9.9277792078591265</v>
       </c>
     </row>
@@ -11454,19 +11682,19 @@
         <v>35</v>
       </c>
       <c r="C230" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.12500000000000003</v>
       </c>
       <c r="D230" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>19.500000000000004</v>
       </c>
       <c r="E230" s="62">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>11.700000000000001</v>
       </c>
       <c r="F230" s="62">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>7.0200000000000014</v>
       </c>
     </row>
@@ -11478,19 +11706,19 @@
         <v>40</v>
       </c>
       <c r="C231" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>8.8388347648318447E-2</v>
       </c>
       <c r="D231" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>13.788582233137678</v>
       </c>
       <c r="E231" s="62">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.2731493398826057</v>
       </c>
       <c r="F231" s="62">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>4.9638896039295632</v>
       </c>
     </row>
@@ -11502,19 +11730,19 @@
         <v>45</v>
       </c>
       <c r="C232" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>6.25E-2</v>
       </c>
       <c r="D232" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>9.75</v>
       </c>
       <c r="E232" s="62">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>5.85</v>
       </c>
       <c r="F232" s="62">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>3.51</v>
       </c>
     </row>
@@ -11550,7 +11778,7 @@
         <v>55</v>
       </c>
       <c r="C234" s="59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>3.125E-2</v>
       </c>
       <c r="D234" s="62">

</xml_diff>

<commit_message>
Add notes to Population_data Excel doc on age ratios of acts per partnership per year.
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15840" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="99">
   <si>
     <t>Male</t>
   </si>
@@ -466,6 +466,12 @@
       </rPr>
       <t>Values are calibrated to fit age-specific HIV and HPV prevalence data.</t>
     </r>
+  </si>
+  <si>
+    <t>Female Age Ratios</t>
+  </si>
+  <si>
+    <t>Male Age Ratios</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1341,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1523,33 +1529,21 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1571,6 +1565,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1583,27 +1580,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -5915,8 +5925,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H252" sqref="H252"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N228" sqref="N228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6046,14 +6056,14 @@
       <c r="A4" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="85" t="s">
+      <c r="C4" s="105"/>
+      <c r="D4" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="86"/>
+      <c r="E4" s="105"/>
     </row>
     <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
@@ -6481,10 +6491,10 @@
       <c r="A27" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="85" t="s">
+      <c r="B27" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="86"/>
+      <c r="C27" s="105"/>
     </row>
     <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
@@ -6899,19 +6909,19 @@
       <c r="AE51" s="24"/>
     </row>
     <row r="52" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="103" t="s">
+      <c r="A52" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="103" t="s">
+      <c r="B52" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="103"/>
-      <c r="D52" s="103"/>
-      <c r="E52" s="103" t="s">
+      <c r="C52" s="108"/>
+      <c r="D52" s="108"/>
+      <c r="E52" s="108" t="s">
         <v>57</v>
       </c>
-      <c r="F52" s="103"/>
-      <c r="G52" s="103"/>
+      <c r="F52" s="108"/>
+      <c r="G52" s="108"/>
       <c r="X52" s="22"/>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
@@ -6922,7 +6932,7 @@
       <c r="AE52" s="22"/>
     </row>
     <row r="53" spans="1:31" ht="15" x14ac:dyDescent="0.35">
-      <c r="A53" s="103"/>
+      <c r="A53" s="108"/>
       <c r="B53" s="33" t="s">
         <v>3</v>
       </c>
@@ -7456,29 +7466,29 @@
       <c r="X80" s="37"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A81" s="100" t="s">
+      <c r="A81" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="83" t="s">
+      <c r="B81" s="106" t="s">
         <v>83</v>
       </c>
-      <c r="C81" s="83" t="s">
+      <c r="C81" s="106" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A82" s="101"/>
-      <c r="B82" s="84"/>
-      <c r="C82" s="84"/>
+      <c r="A82" s="102"/>
+      <c r="B82" s="107"/>
+      <c r="C82" s="107"/>
       <c r="E82" t="s">
         <v>85</v>
       </c>
       <c r="I82" s="55"/>
     </row>
     <row r="83" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="102"/>
-      <c r="B83" s="84"/>
-      <c r="C83" s="84"/>
+      <c r="A83" s="103"/>
+      <c r="B83" s="107"/>
+      <c r="C83" s="107"/>
       <c r="E83" s="9"/>
       <c r="F83" s="9" t="s">
         <v>74</v>
@@ -8003,7 +8013,7 @@
       <c r="X111" s="37"/>
     </row>
     <row r="112" spans="1:24" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="100" t="s">
+      <c r="A112" s="101" t="s">
         <v>2</v>
       </c>
       <c r="B112" s="96" t="s">
@@ -8016,7 +8026,7 @@
       <c r="G112" s="98"/>
     </row>
     <row r="113" spans="1:14" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="101"/>
+      <c r="A113" s="102"/>
       <c r="B113" s="32" t="s">
         <v>70</v>
       </c>
@@ -8037,7 +8047,7 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="102"/>
+      <c r="A114" s="103"/>
       <c r="B114" s="34" t="s">
         <v>63</v>
       </c>
@@ -8125,20 +8135,20 @@
       <c r="G117" s="10">
         <v>0</v>
       </c>
-      <c r="I117" s="109"/>
-      <c r="J117" s="110" t="s">
+      <c r="I117" s="87"/>
+      <c r="J117" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="K117" s="110" t="s">
+      <c r="K117" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="L117" s="110" t="s">
+      <c r="L117" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="M117" s="110" t="s">
+      <c r="M117" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="N117" s="110" t="s">
+      <c r="N117" s="88" t="s">
         <v>30</v>
       </c>
     </row>
@@ -8167,23 +8177,23 @@
       <c r="I118" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J118" s="111">
+      <c r="J118" s="89">
         <f>C118/$B$118</f>
         <v>1</v>
       </c>
-      <c r="K118" s="111">
+      <c r="K118" s="89">
         <f>D118/$B$118</f>
         <v>1</v>
       </c>
-      <c r="L118" s="111">
+      <c r="L118" s="89">
         <f>E118/$B$118</f>
         <v>0.58000000000000007</v>
       </c>
-      <c r="M118" s="111">
+      <c r="M118" s="89">
         <f>F118/$B$118</f>
         <v>0.58000000000000007</v>
       </c>
-      <c r="N118" s="111">
+      <c r="N118" s="89">
         <f>G118/$B$118</f>
         <v>0.41000000000000003</v>
       </c>
@@ -9515,22 +9525,22 @@
       <c r="W160" s="37"/>
     </row>
     <row r="161" spans="1:14" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="87" t="s">
+      <c r="A161" s="109" t="s">
         <v>94</v>
       </c>
-      <c r="B161" s="89" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="89"/>
-      <c r="D161" s="89"/>
-      <c r="E161" s="89" t="s">
+      <c r="B161" s="111" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="111"/>
+      <c r="D161" s="111"/>
+      <c r="E161" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="F161" s="89"/>
-      <c r="G161" s="89"/>
+      <c r="F161" s="111"/>
+      <c r="G161" s="111"/>
     </row>
     <row r="162" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A162" s="87"/>
+      <c r="A162" s="109"/>
       <c r="B162" s="80" t="s">
         <v>3</v>
       </c>
@@ -10296,7 +10306,7 @@
       <c r="AB184" s="20"/>
     </row>
     <row r="185" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A185" s="105"/>
+      <c r="A185" s="84"/>
       <c r="B185" s="20"/>
       <c r="C185" s="20"/>
       <c r="D185" s="20"/>
@@ -10326,9 +10336,9 @@
       <c r="AB185" s="20"/>
     </row>
     <row r="186" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A186" s="106"/>
-      <c r="B186" s="106"/>
-      <c r="C186" s="106"/>
+      <c r="A186" s="112"/>
+      <c r="B186" s="112"/>
+      <c r="C186" s="112"/>
       <c r="D186" s="20"/>
       <c r="E186" s="20"/>
       <c r="F186" s="20"/>
@@ -10356,9 +10366,9 @@
       <c r="AB186" s="20"/>
     </row>
     <row r="187" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A187" s="107"/>
-      <c r="B187" s="108"/>
-      <c r="C187" s="108"/>
+      <c r="A187" s="85"/>
+      <c r="B187" s="86"/>
+      <c r="C187" s="86"/>
       <c r="D187" s="20"/>
       <c r="E187" s="20"/>
       <c r="F187" s="20"/>
@@ -10387,8 +10397,8 @@
     </row>
     <row r="188" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A188" s="6"/>
-      <c r="B188" s="104"/>
-      <c r="C188" s="104"/>
+      <c r="B188" s="83"/>
+      <c r="C188" s="83"/>
       <c r="D188" s="20"/>
       <c r="E188" s="20"/>
       <c r="F188" s="20"/>
@@ -10417,8 +10427,8 @@
     </row>
     <row r="189" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A189" s="6"/>
-      <c r="B189" s="104"/>
-      <c r="C189" s="104"/>
+      <c r="B189" s="83"/>
+      <c r="C189" s="83"/>
       <c r="D189" s="20"/>
       <c r="E189" s="20"/>
       <c r="F189" s="20"/>
@@ -10447,8 +10457,8 @@
     </row>
     <row r="190" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A190" s="6"/>
-      <c r="B190" s="104"/>
-      <c r="C190" s="104"/>
+      <c r="B190" s="83"/>
+      <c r="C190" s="83"/>
       <c r="D190" s="20"/>
       <c r="E190" s="20"/>
       <c r="F190" s="20"/>
@@ -10503,39 +10513,39 @@
       <c r="W197" s="37"/>
     </row>
     <row r="198" spans="1:23" s="39" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A198" s="85" t="s">
+      <c r="A198" s="104" t="s">
         <v>73</v>
       </c>
-      <c r="B198" s="85"/>
-      <c r="C198" s="85"/>
-      <c r="D198" s="85"/>
-      <c r="E198" s="85"/>
-      <c r="F198" s="85"/>
+      <c r="B198" s="104"/>
+      <c r="C198" s="104"/>
+      <c r="D198" s="104"/>
+      <c r="E198" s="104"/>
+      <c r="F198" s="104"/>
     </row>
     <row r="199" spans="1:23" s="39" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A199" s="90" t="s">
+      <c r="A199" s="113" t="s">
         <v>74</v>
       </c>
-      <c r="B199" s="90"/>
-      <c r="C199" s="90"/>
-      <c r="D199" s="90"/>
-      <c r="E199" s="90"/>
-      <c r="F199" s="90"/>
+      <c r="B199" s="113"/>
+      <c r="C199" s="113"/>
+      <c r="D199" s="113"/>
+      <c r="E199" s="113"/>
+      <c r="F199" s="113"/>
     </row>
     <row r="200" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A200" s="91" t="s">
+      <c r="A200" s="99" t="s">
         <v>46</v>
       </c>
       <c r="B200" s="43"/>
       <c r="C200" s="43"/>
-      <c r="D200" s="91" t="s">
+      <c r="D200" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="E200" s="91"/>
-      <c r="F200" s="91"/>
+      <c r="E200" s="99"/>
+      <c r="F200" s="99"/>
     </row>
     <row r="201" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A201" s="91"/>
+      <c r="A201" s="99"/>
       <c r="B201" s="43"/>
       <c r="C201" s="44" t="s">
         <v>47</v>
@@ -10581,6 +10591,14 @@
         <f t="shared" ref="J202:J217" si="21">F202*D54</f>
         <v>0</v>
       </c>
+      <c r="N202" s="114" t="s">
+        <v>2</v>
+      </c>
+      <c r="O202" s="115" t="s">
+        <v>98</v>
+      </c>
+      <c r="P202" s="115"/>
+      <c r="Q202" s="115"/>
     </row>
     <row r="203" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A203" s="45" t="s">
@@ -10609,6 +10627,18 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
+      <c r="N203" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="O203" s="9">
+        <v>0</v>
+      </c>
+      <c r="P203" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q203" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="204" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A204" s="45" t="s">
@@ -10643,6 +10673,18 @@
         <f>SUM(H204:J204)</f>
         <v>3.0912959999999998</v>
       </c>
+      <c r="N204" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="O204" s="9">
+        <v>0</v>
+      </c>
+      <c r="P204" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q204" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="205" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A205" s="45" t="s">
@@ -10677,6 +10719,18 @@
         <f t="shared" ref="K205:K217" si="22">SUM(H205:J205)</f>
         <v>12.224727272727272</v>
       </c>
+      <c r="N205" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="O205" s="9">
+        <v>0</v>
+      </c>
+      <c r="P205" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q205" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="206" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A206" s="45" t="s">
@@ -10713,6 +10767,21 @@
         <f t="shared" si="22"/>
         <v>47.941378151260494</v>
       </c>
+      <c r="N206" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="O206" s="9">
+        <f>D205/D204</f>
+        <v>5</v>
+      </c>
+      <c r="P206" s="9">
+        <f>E205/E204</f>
+        <v>4.9999999999999991</v>
+      </c>
+      <c r="Q206" s="9">
+        <f>F205/F204</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="207" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A207" s="45" t="s">
@@ -10747,6 +10816,21 @@
         <f t="shared" si="22"/>
         <v>122.5191724137931</v>
       </c>
+      <c r="N207" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="O207" s="9">
+        <f>D206/D205</f>
+        <v>4</v>
+      </c>
+      <c r="P207" s="9">
+        <f>E206/E205</f>
+        <v>4</v>
+      </c>
+      <c r="Q207" s="9">
+        <f>F206/F205</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="208" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A208" s="45" t="s">
@@ -10785,8 +10869,23 @@
         <v>91.437775604336935</v>
       </c>
       <c r="M208" s="39"/>
-    </row>
-    <row r="209" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N208" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="O208" s="9">
+        <f>D207/D206</f>
+        <v>2.5</v>
+      </c>
+      <c r="P208" s="9">
+        <f>E207/E206</f>
+        <v>2.5</v>
+      </c>
+      <c r="Q208" s="9">
+        <f>F207/F206</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A209" s="45" t="s">
         <v>37</v>
       </c>
@@ -10822,11 +10921,23 @@
         <f t="shared" si="22"/>
         <v>70.103172413793089</v>
       </c>
-      <c r="N209" s="39"/>
-      <c r="O209" s="39"/>
-      <c r="P209" s="39"/>
-    </row>
-    <row r="210" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N209" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="O209" s="9">
+        <f>D208/D207</f>
+        <v>0.70710678118654491</v>
+      </c>
+      <c r="P209" s="9">
+        <f>E208/E207</f>
+        <v>0.70710678118654813</v>
+      </c>
+      <c r="Q209" s="9">
+        <f>F208/F207</f>
+        <v>0.70710678118654735</v>
+      </c>
+    </row>
+    <row r="210" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A210" s="45" t="s">
         <v>38</v>
       </c>
@@ -10862,8 +10973,23 @@
         <f t="shared" si="22"/>
         <v>50.957971598381803</v>
       </c>
-    </row>
-    <row r="211" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N210" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="O210" s="9">
+        <f>D209/D208</f>
+        <v>0.70710678118655024</v>
+      </c>
+      <c r="P210" s="9">
+        <f>E209/E208</f>
+        <v>0.70710678118654691</v>
+      </c>
+      <c r="Q210" s="9">
+        <f>F209/F208</f>
+        <v>0.70710678118654768</v>
+      </c>
+    </row>
+    <row r="211" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A211" s="45" t="s">
         <v>39</v>
       </c>
@@ -10899,8 +11025,23 @@
         <f t="shared" si="22"/>
         <v>36.662281791044784</v>
       </c>
-    </row>
-    <row r="212" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N211" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="O211" s="9">
+        <f>D210/D209</f>
+        <v>0.70710678118654735</v>
+      </c>
+      <c r="P211" s="9">
+        <f>E210/E209</f>
+        <v>0.70710678118654713</v>
+      </c>
+      <c r="Q211" s="9">
+        <f>F210/F209</f>
+        <v>0.70710678118654913</v>
+      </c>
+    </row>
+    <row r="212" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A212" s="45" t="s">
         <v>40</v>
       </c>
@@ -10936,8 +11077,23 @@
         <f t="shared" si="22"/>
         <v>25.924148068219885</v>
       </c>
-    </row>
-    <row r="213" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N212" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O212" s="9">
+        <f>D211/D210</f>
+        <v>0.70710678118654768</v>
+      </c>
+      <c r="P212" s="9">
+        <f>E211/E210</f>
+        <v>0.70710678118654802</v>
+      </c>
+      <c r="Q212" s="9">
+        <f>F211/F210</f>
+        <v>0.70710678118654591</v>
+      </c>
+    </row>
+    <row r="213" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A213" s="45" t="s">
         <v>41</v>
       </c>
@@ -10973,8 +11129,23 @@
         <f t="shared" si="22"/>
         <v>18.331140895522392</v>
       </c>
-    </row>
-    <row r="214" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N213" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="O213" s="9">
+        <f>D212/D211</f>
+        <v>0.70710678118654868</v>
+      </c>
+      <c r="P213" s="9">
+        <f>E212/E211</f>
+        <v>0.70710678118654713</v>
+      </c>
+      <c r="Q213" s="9">
+        <f>F212/F211</f>
+        <v>0.70710678118654779</v>
+      </c>
+    </row>
+    <row r="214" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A214" s="45" t="s">
         <v>42</v>
       </c>
@@ -11010,8 +11181,23 @@
         <f t="shared" si="22"/>
         <v>12.962074034109945</v>
       </c>
-    </row>
-    <row r="215" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N214" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="O214" s="9">
+        <f>D213/D212</f>
+        <v>0.70710678118654635</v>
+      </c>
+      <c r="P214" s="9">
+        <f>E213/E212</f>
+        <v>0.70710678118654802</v>
+      </c>
+      <c r="Q214" s="9">
+        <f>F213/F212</f>
+        <v>0.70710678118654724</v>
+      </c>
+    </row>
+    <row r="215" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A215" s="45" t="s">
         <v>43</v>
       </c>
@@ -11047,8 +11233,23 @@
         <f t="shared" si="22"/>
         <v>9.1655704477611959</v>
       </c>
-    </row>
-    <row r="216" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N215" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O215" s="9">
+        <f>D214/D213</f>
+        <v>0.70710678118654868</v>
+      </c>
+      <c r="P215" s="9">
+        <f>E214/E213</f>
+        <v>0.70710678118654779</v>
+      </c>
+      <c r="Q215" s="9">
+        <f>F214/F213</f>
+        <v>0.70710678118654702</v>
+      </c>
+    </row>
+    <row r="216" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A216" s="45" t="s">
         <v>44</v>
       </c>
@@ -11084,8 +11285,23 @@
         <f t="shared" si="22"/>
         <v>6.4810370170549634</v>
       </c>
-    </row>
-    <row r="217" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N216" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="O216" s="9">
+        <f>D215/D214</f>
+        <v>0.70710678118654635</v>
+      </c>
+      <c r="P216" s="9">
+        <f>E215/E214</f>
+        <v>0.70710678118654724</v>
+      </c>
+      <c r="Q216" s="9">
+        <f>F215/F214</f>
+        <v>0.70710678118654802</v>
+      </c>
+    </row>
+    <row r="217" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A217" s="45" t="s">
         <v>45</v>
       </c>
@@ -11121,8 +11337,23 @@
         <f t="shared" si="22"/>
         <v>4.5827852238805979</v>
       </c>
-    </row>
-    <row r="218" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N217" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="O217" s="9">
+        <f>D216/D215</f>
+        <v>0.70710678118654768</v>
+      </c>
+      <c r="P217" s="9">
+        <f>E216/E215</f>
+        <v>0.70710678118654713</v>
+      </c>
+      <c r="Q217" s="9">
+        <f>F216/F215</f>
+        <v>0.70710678118654702</v>
+      </c>
+    </row>
+    <row r="218" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A218" s="43"/>
       <c r="B218" s="46"/>
       <c r="C218" s="43"/>
@@ -11137,31 +11368,46 @@
         <f>K218/(365.25/7)</f>
         <v>0.70141619566308888</v>
       </c>
-    </row>
-    <row r="219" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A219" s="99" t="s">
+      <c r="N218" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="O218" s="9">
+        <f>D217/D216</f>
+        <v>0.70710678118654735</v>
+      </c>
+      <c r="P218" s="9">
+        <f>E217/E216</f>
+        <v>0.70710678118654802</v>
+      </c>
+      <c r="Q218" s="9">
+        <f>F217/F216</f>
+        <v>0.70710678118654802</v>
+      </c>
+    </row>
+    <row r="219" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A219" s="100" t="s">
         <v>75</v>
       </c>
-      <c r="B219" s="99"/>
-      <c r="C219" s="99"/>
-      <c r="D219" s="99"/>
-      <c r="E219" s="99"/>
-      <c r="F219" s="99"/>
-    </row>
-    <row r="220" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A220" s="88" t="s">
+      <c r="B219" s="100"/>
+      <c r="C219" s="100"/>
+      <c r="D219" s="100"/>
+      <c r="E219" s="100"/>
+      <c r="F219" s="100"/>
+    </row>
+    <row r="220" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A220" s="110" t="s">
         <v>2</v>
       </c>
       <c r="B220" s="43"/>
       <c r="C220" s="43"/>
-      <c r="D220" s="91" t="s">
+      <c r="D220" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="E220" s="91"/>
-      <c r="F220" s="91"/>
-    </row>
-    <row r="221" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A221" s="88"/>
+      <c r="E220" s="99"/>
+      <c r="F220" s="99"/>
+    </row>
+    <row r="221" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A221" s="110"/>
       <c r="B221" s="43"/>
       <c r="C221" s="44" t="s">
         <v>47</v>
@@ -11176,7 +11422,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A222" s="45" t="s">
         <v>25</v>
       </c>
@@ -11191,8 +11437,16 @@
       <c r="F222" s="81">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N222" s="114" t="s">
+        <v>2</v>
+      </c>
+      <c r="O222" s="115" t="s">
+        <v>97</v>
+      </c>
+      <c r="P222" s="115"/>
+      <c r="Q222" s="115"/>
+    </row>
+    <row r="223" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A223" s="45" t="s">
         <v>24</v>
       </c>
@@ -11207,8 +11461,20 @@
       <c r="F223" s="81">
         <v>0</v>
       </c>
-    </row>
-    <row r="224" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N223" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="O223" s="9">
+        <v>0</v>
+      </c>
+      <c r="P223" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q223" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A224" s="45" t="s">
         <v>32</v>
       </c>
@@ -11225,8 +11491,20 @@
       <c r="F224" s="81">
         <v>2.8079999999999998</v>
       </c>
-    </row>
-    <row r="225" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N224" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="O224" s="9">
+        <v>0</v>
+      </c>
+      <c r="P224" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q224" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A225" s="45" t="s">
         <v>33</v>
       </c>
@@ -11243,8 +11521,20 @@
       <c r="F225" s="82">
         <v>6.7392000000000003</v>
       </c>
-    </row>
-    <row r="226" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N225" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="O225" s="9">
+        <v>0</v>
+      </c>
+      <c r="P225" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q225" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A226" s="45" t="s">
         <v>34</v>
       </c>
@@ -11263,8 +11553,23 @@
       <c r="F226" s="81">
         <v>26.956800000000001</v>
       </c>
-    </row>
-    <row r="227" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N226" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="O226" s="9">
+        <f>D225/D224</f>
+        <v>2.4</v>
+      </c>
+      <c r="P226" s="9">
+        <f>E225/E224</f>
+        <v>2.4</v>
+      </c>
+      <c r="Q226" s="9">
+        <f>F225/F224</f>
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="227" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A227" s="45" t="s">
         <v>35</v>
       </c>
@@ -11281,8 +11586,23 @@
       <c r="F227" s="81">
         <v>50.543999999999997</v>
       </c>
-    </row>
-    <row r="228" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N227" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="O227" s="9">
+        <f>D226/D225</f>
+        <v>4</v>
+      </c>
+      <c r="P227" s="9">
+        <f>E226/E225</f>
+        <v>4</v>
+      </c>
+      <c r="Q227" s="9">
+        <f>F226/F225</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="228" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A228" s="45" t="s">
         <v>36</v>
       </c>
@@ -11302,8 +11622,23 @@
       <c r="F228" s="81">
         <v>35.740005148292902</v>
       </c>
-    </row>
-    <row r="229" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N228" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="O228" s="9">
+        <f>D227/D226</f>
+        <v>1.8750000000000002</v>
+      </c>
+      <c r="P228" s="9">
+        <f>E227/E226</f>
+        <v>1.875</v>
+      </c>
+      <c r="Q228" s="9">
+        <f>F227/F226</f>
+        <v>1.8749999999999998</v>
+      </c>
+    </row>
+    <row r="229" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A229" s="45" t="s">
         <v>37</v>
       </c>
@@ -11323,8 +11658,23 @@
       <c r="F229" s="81">
         <v>25.271999999999998</v>
       </c>
-    </row>
-    <row r="230" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N229" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="O229" s="9">
+        <f>D228/D227</f>
+        <v>0.70710678118654768</v>
+      </c>
+      <c r="P229" s="9">
+        <f>E228/E227</f>
+        <v>0.70710678118654802</v>
+      </c>
+      <c r="Q229" s="9">
+        <f>F228/F227</f>
+        <v>0.70710678118654846</v>
+      </c>
+    </row>
+    <row r="230" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A230" s="45" t="s">
         <v>38</v>
       </c>
@@ -11344,8 +11694,23 @@
       <c r="F230" s="81">
         <v>17.870002574146401</v>
       </c>
-    </row>
-    <row r="231" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N230" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="O230" s="9">
+        <f>D229/D228</f>
+        <v>0.70710678118654735</v>
+      </c>
+      <c r="P230" s="9">
+        <f>E229/E228</f>
+        <v>0.70710678118654702</v>
+      </c>
+      <c r="Q230" s="9">
+        <f>F229/F228</f>
+        <v>0.70710678118654657</v>
+      </c>
+    </row>
+    <row r="231" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A231" s="45" t="s">
         <v>39</v>
       </c>
@@ -11365,8 +11730,23 @@
       <c r="F231" s="81">
         <v>12.635999999999999</v>
       </c>
-    </row>
-    <row r="232" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N231" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="O231" s="9">
+        <f>D230/D229</f>
+        <v>0.70710678118654702</v>
+      </c>
+      <c r="P231" s="9">
+        <f>E230/E229</f>
+        <v>0.70710678118654802</v>
+      </c>
+      <c r="Q231" s="9">
+        <f>F230/F229</f>
+        <v>0.70710678118654646</v>
+      </c>
+    </row>
+    <row r="232" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A232" s="45" t="s">
         <v>40</v>
       </c>
@@ -11386,8 +11766,23 @@
       <c r="F232" s="81">
         <v>9.92777920785913</v>
       </c>
-    </row>
-    <row r="233" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N232" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O232" s="9">
+        <f>D231/D230</f>
+        <v>0.70710678118654802</v>
+      </c>
+      <c r="P232" s="9">
+        <f>E231/E230</f>
+        <v>0.70710678118654702</v>
+      </c>
+      <c r="Q232" s="9">
+        <f>F231/F230</f>
+        <v>0.70710678118654857</v>
+      </c>
+    </row>
+    <row r="233" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A233" s="45" t="s">
         <v>41</v>
       </c>
@@ -11407,8 +11802,23 @@
       <c r="F233" s="81">
         <v>7.02</v>
       </c>
-    </row>
-    <row r="234" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N233" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="O233" s="9">
+        <f>D232/D231</f>
+        <v>0.78567420131838739</v>
+      </c>
+      <c r="P233" s="9">
+        <f>E232/E231</f>
+        <v>0.78567420131838561</v>
+      </c>
+      <c r="Q233" s="9">
+        <f>F232/F231</f>
+        <v>0.78567420131838639</v>
+      </c>
+    </row>
+    <row r="234" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A234" s="45" t="s">
         <v>42</v>
       </c>
@@ -11428,8 +11838,23 @@
       <c r="F234" s="81">
         <v>4.9638896039295597</v>
       </c>
-    </row>
-    <row r="235" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N234" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="O234" s="9">
+        <f>D233/D232</f>
+        <v>0.70710678118654635</v>
+      </c>
+      <c r="P234" s="9">
+        <f>E233/E232</f>
+        <v>0.70710678118654802</v>
+      </c>
+      <c r="Q234" s="9">
+        <f>F233/F232</f>
+        <v>0.70710678118654724</v>
+      </c>
+    </row>
+    <row r="235" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A235" s="45" t="s">
         <v>43</v>
       </c>
@@ -11449,8 +11874,23 @@
       <c r="F235" s="81">
         <v>3.51</v>
       </c>
-    </row>
-    <row r="236" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N235" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O235" s="9">
+        <f>D234/D233</f>
+        <v>0.70710678118654868</v>
+      </c>
+      <c r="P235" s="9">
+        <f>E234/E233</f>
+        <v>0.70710678118654779</v>
+      </c>
+      <c r="Q235" s="9">
+        <f>F234/F233</f>
+        <v>0.70710678118654702</v>
+      </c>
+    </row>
+    <row r="236" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A236" s="45" t="s">
         <v>44</v>
       </c>
@@ -11470,8 +11910,23 @@
       <c r="F236" s="81">
         <v>2.4819448019647798</v>
       </c>
-    </row>
-    <row r="237" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N236" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="O236" s="9">
+        <f>D235/D234</f>
+        <v>0.70710678118654635</v>
+      </c>
+      <c r="P236" s="9">
+        <f>E235/E234</f>
+        <v>0.70710678118654724</v>
+      </c>
+      <c r="Q236" s="9">
+        <f>F235/F234</f>
+        <v>0.70710678118654802</v>
+      </c>
+    </row>
+    <row r="237" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A237" s="45" t="s">
         <v>45</v>
       </c>
@@ -11491,43 +11946,73 @@
       <c r="F237" s="81">
         <v>1.7549999999999999</v>
       </c>
-    </row>
-    <row r="238" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="N237" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="O237" s="9">
+        <f>D236/D235</f>
+        <v>0.70710678118654768</v>
+      </c>
+      <c r="P237" s="9">
+        <f>E236/E235</f>
+        <v>0.70710678118654713</v>
+      </c>
+      <c r="Q237" s="9">
+        <f>F236/F235</f>
+        <v>0.70710678118654702</v>
+      </c>
+    </row>
+    <row r="238" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A238" s="35"/>
       <c r="B238" s="35"/>
       <c r="C238" s="42"/>
       <c r="D238" s="35"/>
       <c r="E238" s="35"/>
       <c r="F238" s="35"/>
-    </row>
-    <row r="239" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A239" s="112"/>
+      <c r="N238" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="O238" s="9">
+        <f>D237/D236</f>
+        <v>0.70710678118654735</v>
+      </c>
+      <c r="P238" s="9">
+        <f>E237/E236</f>
+        <v>0.70710678118654802</v>
+      </c>
+      <c r="Q238" s="9">
+        <f>F237/F236</f>
+        <v>0.70710678118654802</v>
+      </c>
+    </row>
+    <row r="239" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A239" s="90"/>
       <c r="B239" s="20"/>
       <c r="C239" s="20"/>
       <c r="D239" s="20"/>
-      <c r="E239" s="113"/>
+      <c r="E239" s="91"/>
       <c r="F239" s="35"/>
     </row>
-    <row r="240" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A240" s="107"/>
-      <c r="B240" s="108"/>
-      <c r="C240" s="108"/>
-      <c r="D240" s="108"/>
-      <c r="E240" s="113"/>
+    <row r="240" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A240" s="85"/>
+      <c r="B240" s="86"/>
+      <c r="C240" s="86"/>
+      <c r="D240" s="86"/>
+      <c r="E240" s="91"/>
       <c r="F240" s="35"/>
     </row>
     <row r="241" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A241" s="6"/>
-      <c r="B241" s="104"/>
-      <c r="C241" s="104"/>
-      <c r="D241" s="104"/>
+      <c r="B241" s="83"/>
+      <c r="C241" s="83"/>
+      <c r="D241" s="83"/>
       <c r="E241" s="25"/>
     </row>
     <row r="242" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A242" s="6"/>
-      <c r="B242" s="104"/>
-      <c r="C242" s="104"/>
-      <c r="D242" s="104"/>
+      <c r="B242" s="83"/>
+      <c r="C242" s="83"/>
+      <c r="D242" s="83"/>
       <c r="E242" s="25"/>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.35">
@@ -11552,7 +12037,20 @@
       <c r="E245" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="29">
+    <mergeCell ref="O222:Q222"/>
+    <mergeCell ref="O202:Q202"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="E161:G161"/>
+    <mergeCell ref="A186:C186"/>
+    <mergeCell ref="A198:F198"/>
+    <mergeCell ref="A199:F199"/>
+    <mergeCell ref="D200:F200"/>
+    <mergeCell ref="D220:F220"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="I133:I135"/>
     <mergeCell ref="J133:O133"/>
@@ -11569,17 +12067,6 @@
     <mergeCell ref="B52:D52"/>
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A161:A162"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="E161:G161"/>
-    <mergeCell ref="A186:C186"/>
-    <mergeCell ref="A198:F198"/>
-    <mergeCell ref="A199:F199"/>
-    <mergeCell ref="D200:F200"/>
-    <mergeCell ref="D220:F220"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add descriptions to population data Excel sheets.
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -339,27 +339,6 @@
     <t>Initial Population Size (thousands)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Initial population size (1910).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Age distribution based on SA 1985 census and scaled to fit KZN's population growth and size profile.</t>
-    </r>
-  </si>
-  <si>
     <t>United Nations Population Division World Population Prospectus 2019</t>
   </si>
   <si>
@@ -472,6 +451,27 @@
   </si>
   <si>
     <t>Male Age Ratios</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Initial population size (1910).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Calculate backward-projected KZN population. Assume that KZN:SA proportion was decreasing from 1910-2002 according to same trend as from 2002-2019. Assume male and female populations by age follow exponential distributions. See Population_validation Excel document for more detail.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1544,6 +1544,40 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1565,9 +1599,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1580,39 +1611,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -5925,8 +5925,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N228" sqref="N228"/>
+    <sheetView tabSelected="1" topLeftCell="A244" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K222" sqref="K222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5967,7 +5967,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -5995,16 +5995,16 @@
       <c r="Y1" s="37"/>
     </row>
     <row r="2" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="92" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
+      <c r="A2" s="104" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -6025,7 +6025,7 @@
     </row>
     <row r="3" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
@@ -6056,14 +6056,14 @@
       <c r="A4" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="105"/>
-      <c r="D4" s="104" t="s">
+      <c r="C4" s="97"/>
+      <c r="D4" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="105"/>
+      <c r="E4" s="97"/>
     </row>
     <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
@@ -6491,10 +6491,10 @@
       <c r="A27" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="104" t="s">
+      <c r="B27" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="105"/>
+      <c r="C27" s="97"/>
     </row>
     <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
@@ -6840,7 +6840,7 @@
     </row>
     <row r="50" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" s="37"/>
       <c r="C50" s="37"/>
@@ -6909,19 +6909,19 @@
       <c r="AE51" s="24"/>
     </row>
     <row r="52" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="108" t="s">
+      <c r="A52" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="108" t="s">
+      <c r="B52" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="108"/>
-      <c r="D52" s="108"/>
-      <c r="E52" s="108" t="s">
+      <c r="C52" s="115"/>
+      <c r="D52" s="115"/>
+      <c r="E52" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="F52" s="108"/>
-      <c r="G52" s="108"/>
+      <c r="F52" s="115"/>
+      <c r="G52" s="115"/>
       <c r="X52" s="22"/>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
@@ -6932,7 +6932,7 @@
       <c r="AE52" s="22"/>
     </row>
     <row r="53" spans="1:31" ht="15" x14ac:dyDescent="0.35">
-      <c r="A53" s="108"/>
+      <c r="A53" s="115"/>
       <c r="B53" s="33" t="s">
         <v>3</v>
       </c>
@@ -7411,7 +7411,7 @@
     </row>
     <row r="79" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79" s="38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B79" s="37"/>
       <c r="C79" s="37"/>
@@ -7439,7 +7439,7 @@
     </row>
     <row r="80" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B80" s="37"/>
       <c r="C80" s="37"/>
@@ -7466,29 +7466,29 @@
       <c r="X80" s="37"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A81" s="101" t="s">
+      <c r="A81" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="106" t="s">
+      <c r="B81" s="94" t="s">
+        <v>82</v>
+      </c>
+      <c r="C81" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="C81" s="106" t="s">
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A82" s="113"/>
+      <c r="B82" s="95"/>
+      <c r="C82" s="95"/>
+      <c r="E82" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A82" s="102"/>
-      <c r="B82" s="107"/>
-      <c r="C82" s="107"/>
-      <c r="E82" t="s">
-        <v>85</v>
-      </c>
       <c r="I82" s="55"/>
     </row>
     <row r="83" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="103"/>
-      <c r="B83" s="107"/>
-      <c r="C83" s="107"/>
+      <c r="A83" s="114"/>
+      <c r="B83" s="95"/>
+      <c r="C83" s="95"/>
       <c r="E83" s="9"/>
       <c r="F83" s="9" t="s">
         <v>74</v>
@@ -7541,7 +7541,7 @@
         <v>1.8590649E-3</v>
       </c>
       <c r="E85" s="75" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F85" s="74">
         <v>5.2241062999999997E-3</v>
@@ -7902,7 +7902,7 @@
     </row>
     <row r="108" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A108" s="38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B108" s="37"/>
       <c r="C108" s="37"/>
@@ -7930,7 +7930,7 @@
     </row>
     <row r="109" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A109" s="38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B109" s="37"/>
       <c r="C109" s="37"/>
@@ -7958,7 +7958,7 @@
     </row>
     <row r="110" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A110" s="76" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B110" s="37"/>
       <c r="C110" s="37"/>
@@ -7986,7 +7986,7 @@
     </row>
     <row r="111" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B111" s="37"/>
       <c r="C111" s="37"/>
@@ -8013,20 +8013,20 @@
       <c r="X111" s="37"/>
     </row>
     <row r="112" spans="1:24" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="101" t="s">
+      <c r="A112" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="96" t="s">
-        <v>88</v>
-      </c>
-      <c r="C112" s="97"/>
-      <c r="D112" s="97"/>
-      <c r="E112" s="97"/>
-      <c r="F112" s="97"/>
-      <c r="G112" s="98"/>
+      <c r="B112" s="108" t="s">
+        <v>87</v>
+      </c>
+      <c r="C112" s="109"/>
+      <c r="D112" s="109"/>
+      <c r="E112" s="109"/>
+      <c r="F112" s="109"/>
+      <c r="G112" s="110"/>
     </row>
     <row r="113" spans="1:14" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="102"/>
+      <c r="A113" s="113"/>
       <c r="B113" s="32" t="s">
         <v>70</v>
       </c>
@@ -8047,7 +8047,7 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="103"/>
+      <c r="A114" s="114"/>
       <c r="B114" s="34" t="s">
         <v>63</v>
       </c>
@@ -8502,31 +8502,31 @@
     </row>
     <row r="132" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="133" spans="1:15" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A133" s="93" t="s">
+      <c r="A133" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="96" t="s">
-        <v>89</v>
-      </c>
-      <c r="C133" s="97"/>
-      <c r="D133" s="97"/>
-      <c r="E133" s="97"/>
-      <c r="F133" s="97"/>
-      <c r="G133" s="98"/>
-      <c r="I133" s="93" t="s">
+      <c r="B133" s="108" t="s">
+        <v>88</v>
+      </c>
+      <c r="C133" s="109"/>
+      <c r="D133" s="109"/>
+      <c r="E133" s="109"/>
+      <c r="F133" s="109"/>
+      <c r="G133" s="110"/>
+      <c r="I133" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="J133" s="96" t="s">
+      <c r="J133" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="K133" s="97"/>
-      <c r="L133" s="97"/>
-      <c r="M133" s="97"/>
-      <c r="N133" s="97"/>
-      <c r="O133" s="98"/>
+      <c r="K133" s="109"/>
+      <c r="L133" s="109"/>
+      <c r="M133" s="109"/>
+      <c r="N133" s="109"/>
+      <c r="O133" s="110"/>
     </row>
     <row r="134" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="94"/>
+      <c r="A134" s="106"/>
       <c r="B134" s="26" t="s">
         <v>71</v>
       </c>
@@ -8545,7 +8545,7 @@
       <c r="G134" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I134" s="94"/>
+      <c r="I134" s="106"/>
       <c r="J134" s="26" t="s">
         <v>71</v>
       </c>
@@ -8566,7 +8566,7 @@
       </c>
     </row>
     <row r="135" spans="1:15" ht="47" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A135" s="95"/>
+      <c r="A135" s="107"/>
       <c r="B135" s="40" t="s">
         <v>63</v>
       </c>
@@ -8585,7 +8585,7 @@
       <c r="G135" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I135" s="95"/>
+      <c r="I135" s="107"/>
       <c r="J135" s="40" t="s">
         <v>63</v>
       </c>
@@ -9445,7 +9445,7 @@
     </row>
     <row r="158" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A158" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B158" s="37"/>
       <c r="C158" s="37"/>
@@ -9525,22 +9525,22 @@
       <c r="W160" s="37"/>
     </row>
     <row r="161" spans="1:14" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="109" t="s">
-        <v>94</v>
-      </c>
-      <c r="B161" s="111" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="111"/>
-      <c r="D161" s="111"/>
-      <c r="E161" s="111" t="s">
+      <c r="A161" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="B161" s="100" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="100"/>
+      <c r="D161" s="100"/>
+      <c r="E161" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="F161" s="111"/>
-      <c r="G161" s="111"/>
+      <c r="F161" s="100"/>
+      <c r="G161" s="100"/>
     </row>
     <row r="162" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A162" s="109"/>
+      <c r="A162" s="98"/>
       <c r="B162" s="80" t="s">
         <v>3</v>
       </c>
@@ -10336,9 +10336,9 @@
       <c r="AB185" s="20"/>
     </row>
     <row r="186" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A186" s="112"/>
-      <c r="B186" s="112"/>
-      <c r="C186" s="112"/>
+      <c r="A186" s="101"/>
+      <c r="B186" s="101"/>
+      <c r="C186" s="101"/>
       <c r="D186" s="20"/>
       <c r="E186" s="20"/>
       <c r="F186" s="20"/>
@@ -10487,7 +10487,7 @@
     </row>
     <row r="197" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A197" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B197" s="37"/>
       <c r="C197" s="37"/>
@@ -10513,39 +10513,39 @@
       <c r="W197" s="37"/>
     </row>
     <row r="198" spans="1:23" s="39" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A198" s="104" t="s">
+      <c r="A198" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="B198" s="104"/>
-      <c r="C198" s="104"/>
-      <c r="D198" s="104"/>
-      <c r="E198" s="104"/>
-      <c r="F198" s="104"/>
+      <c r="B198" s="96"/>
+      <c r="C198" s="96"/>
+      <c r="D198" s="96"/>
+      <c r="E198" s="96"/>
+      <c r="F198" s="96"/>
     </row>
     <row r="199" spans="1:23" s="39" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A199" s="113" t="s">
+      <c r="A199" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="B199" s="113"/>
-      <c r="C199" s="113"/>
-      <c r="D199" s="113"/>
-      <c r="E199" s="113"/>
-      <c r="F199" s="113"/>
+      <c r="B199" s="102"/>
+      <c r="C199" s="102"/>
+      <c r="D199" s="102"/>
+      <c r="E199" s="102"/>
+      <c r="F199" s="102"/>
     </row>
     <row r="200" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A200" s="99" t="s">
+      <c r="A200" s="103" t="s">
         <v>46</v>
       </c>
       <c r="B200" s="43"/>
       <c r="C200" s="43"/>
-      <c r="D200" s="99" t="s">
+      <c r="D200" s="103" t="s">
         <v>51</v>
       </c>
-      <c r="E200" s="99"/>
-      <c r="F200" s="99"/>
+      <c r="E200" s="103"/>
+      <c r="F200" s="103"/>
     </row>
     <row r="201" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A201" s="99"/>
+      <c r="A201" s="103"/>
       <c r="B201" s="43"/>
       <c r="C201" s="44" t="s">
         <v>47</v>
@@ -10591,14 +10591,14 @@
         <f t="shared" ref="J202:J217" si="21">F202*D54</f>
         <v>0</v>
       </c>
-      <c r="N202" s="114" t="s">
+      <c r="N202" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="O202" s="115" t="s">
-        <v>98</v>
-      </c>
-      <c r="P202" s="115"/>
-      <c r="Q202" s="115"/>
+      <c r="O202" s="93" t="s">
+        <v>97</v>
+      </c>
+      <c r="P202" s="93"/>
+      <c r="Q202" s="93"/>
     </row>
     <row r="203" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A203" s="45" t="s">
@@ -10771,15 +10771,15 @@
         <v>33</v>
       </c>
       <c r="O206" s="9">
-        <f>D205/D204</f>
+        <f t="shared" ref="O206:O218" si="23">D205/D204</f>
         <v>5</v>
       </c>
       <c r="P206" s="9">
-        <f>E205/E204</f>
+        <f t="shared" ref="P206:P218" si="24">E205/E204</f>
         <v>4.9999999999999991</v>
       </c>
       <c r="Q206" s="9">
-        <f>F205/F204</f>
+        <f t="shared" ref="Q206:Q218" si="25">F205/F204</f>
         <v>5</v>
       </c>
     </row>
@@ -10820,15 +10820,15 @@
         <v>34</v>
       </c>
       <c r="O207" s="9">
-        <f>D206/D205</f>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="P207" s="9">
-        <f>E206/E205</f>
+        <f t="shared" si="24"/>
         <v>4</v>
       </c>
       <c r="Q207" s="9">
-        <f>F206/F205</f>
+        <f t="shared" si="25"/>
         <v>4</v>
       </c>
     </row>
@@ -10840,7 +10840,7 @@
         <v>10</v>
       </c>
       <c r="C208" s="43">
-        <f t="shared" ref="C208:C217" si="23">EXP(LN(0.5)*B207/10)</f>
+        <f t="shared" ref="C208:C217" si="26">EXP(LN(0.5)*B207/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D208" s="82">
@@ -10873,15 +10873,15 @@
         <v>35</v>
       </c>
       <c r="O208" s="9">
-        <f>D207/D206</f>
+        <f t="shared" si="23"/>
         <v>2.5</v>
       </c>
       <c r="P208" s="9">
-        <f>E207/E206</f>
+        <f t="shared" si="24"/>
         <v>2.5</v>
       </c>
       <c r="Q208" s="9">
-        <f>F207/F206</f>
+        <f t="shared" si="25"/>
         <v>2.5</v>
       </c>
     </row>
@@ -10893,7 +10893,7 @@
         <v>15</v>
       </c>
       <c r="C209" s="43">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0.5</v>
       </c>
       <c r="D209" s="82">
@@ -10925,15 +10925,15 @@
         <v>36</v>
       </c>
       <c r="O209" s="9">
-        <f>D208/D207</f>
+        <f t="shared" si="23"/>
         <v>0.70710678118654491</v>
       </c>
       <c r="P209" s="9">
-        <f>E208/E207</f>
+        <f t="shared" si="24"/>
         <v>0.70710678118654813</v>
       </c>
       <c r="Q209" s="9">
-        <f>F208/F207</f>
+        <f t="shared" si="25"/>
         <v>0.70710678118654735</v>
       </c>
     </row>
@@ -10945,7 +10945,7 @@
         <v>20</v>
       </c>
       <c r="C210" s="43">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0.35355339059327379</v>
       </c>
       <c r="D210" s="82">
@@ -10977,15 +10977,15 @@
         <v>37</v>
       </c>
       <c r="O210" s="9">
-        <f>D209/D208</f>
+        <f t="shared" si="23"/>
         <v>0.70710678118655024</v>
       </c>
       <c r="P210" s="9">
-        <f>E209/E208</f>
+        <f t="shared" si="24"/>
         <v>0.70710678118654691</v>
       </c>
       <c r="Q210" s="9">
-        <f>F209/F208</f>
+        <f t="shared" si="25"/>
         <v>0.70710678118654768</v>
       </c>
     </row>
@@ -10997,7 +10997,7 @@
         <v>25</v>
       </c>
       <c r="C211" s="43">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0.25</v>
       </c>
       <c r="D211" s="82">
@@ -11029,15 +11029,15 @@
         <v>38</v>
       </c>
       <c r="O211" s="9">
-        <f>D210/D209</f>
+        <f t="shared" si="23"/>
         <v>0.70710678118654735</v>
       </c>
       <c r="P211" s="9">
-        <f>E210/E209</f>
+        <f t="shared" si="24"/>
         <v>0.70710678118654713</v>
       </c>
       <c r="Q211" s="9">
-        <f>F210/F209</f>
+        <f t="shared" si="25"/>
         <v>0.70710678118654913</v>
       </c>
     </row>
@@ -11049,7 +11049,7 @@
         <v>30</v>
       </c>
       <c r="C212" s="43">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0.17677669529663689</v>
       </c>
       <c r="D212" s="82">
@@ -11081,15 +11081,15 @@
         <v>39</v>
       </c>
       <c r="O212" s="9">
-        <f>D211/D210</f>
+        <f t="shared" si="23"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="P212" s="9">
-        <f>E211/E210</f>
+        <f t="shared" si="24"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q212" s="9">
-        <f>F211/F210</f>
+        <f t="shared" si="25"/>
         <v>0.70710678118654591</v>
       </c>
     </row>
@@ -11101,7 +11101,7 @@
         <v>35</v>
       </c>
       <c r="C213" s="43">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>0.12500000000000003</v>
       </c>
       <c r="D213" s="82">
@@ -11133,15 +11133,15 @@
         <v>40</v>
       </c>
       <c r="O213" s="9">
-        <f>D212/D211</f>
+        <f t="shared" si="23"/>
         <v>0.70710678118654868</v>
       </c>
       <c r="P213" s="9">
-        <f>E212/E211</f>
+        <f t="shared" si="24"/>
         <v>0.70710678118654713</v>
       </c>
       <c r="Q213" s="9">
-        <f>F212/F211</f>
+        <f t="shared" si="25"/>
         <v>0.70710678118654779</v>
       </c>
     </row>
@@ -11185,15 +11185,15 @@
         <v>41</v>
       </c>
       <c r="O214" s="9">
-        <f>D213/D212</f>
+        <f t="shared" si="23"/>
         <v>0.70710678118654635</v>
       </c>
       <c r="P214" s="9">
-        <f>E213/E212</f>
+        <f t="shared" si="24"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q214" s="9">
-        <f>F213/F212</f>
+        <f t="shared" si="25"/>
         <v>0.70710678118654724</v>
       </c>
     </row>
@@ -11205,7 +11205,7 @@
         <v>45</v>
       </c>
       <c r="C215" s="43">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>6.25E-2</v>
       </c>
       <c r="D215" s="82">
@@ -11237,15 +11237,15 @@
         <v>42</v>
       </c>
       <c r="O215" s="9">
-        <f>D214/D213</f>
+        <f t="shared" si="23"/>
         <v>0.70710678118654868</v>
       </c>
       <c r="P215" s="9">
-        <f>E214/E213</f>
+        <f t="shared" si="24"/>
         <v>0.70710678118654779</v>
       </c>
       <c r="Q215" s="9">
-        <f>F214/F213</f>
+        <f t="shared" si="25"/>
         <v>0.70710678118654702</v>
       </c>
     </row>
@@ -11257,7 +11257,7 @@
         <v>50</v>
       </c>
       <c r="C216" s="43">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>4.4194173824159223E-2</v>
       </c>
       <c r="D216" s="82">
@@ -11289,15 +11289,15 @@
         <v>43</v>
       </c>
       <c r="O216" s="9">
-        <f>D215/D214</f>
+        <f t="shared" si="23"/>
         <v>0.70710678118654635</v>
       </c>
       <c r="P216" s="9">
-        <f>E215/E214</f>
+        <f t="shared" si="24"/>
         <v>0.70710678118654724</v>
       </c>
       <c r="Q216" s="9">
-        <f>F215/F214</f>
+        <f t="shared" si="25"/>
         <v>0.70710678118654802</v>
       </c>
     </row>
@@ -11309,7 +11309,7 @@
         <v>55</v>
       </c>
       <c r="C217" s="43">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>3.125E-2</v>
       </c>
       <c r="D217" s="82">
@@ -11341,15 +11341,15 @@
         <v>44</v>
       </c>
       <c r="O217" s="9">
-        <f>D216/D215</f>
+        <f t="shared" si="23"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="P217" s="9">
-        <f>E216/E215</f>
+        <f t="shared" si="24"/>
         <v>0.70710678118654713</v>
       </c>
       <c r="Q217" s="9">
-        <f>F216/F215</f>
+        <f t="shared" si="25"/>
         <v>0.70710678118654702</v>
       </c>
     </row>
@@ -11372,42 +11372,42 @@
         <v>45</v>
       </c>
       <c r="O218" s="9">
-        <f>D217/D216</f>
+        <f t="shared" si="23"/>
         <v>0.70710678118654735</v>
       </c>
       <c r="P218" s="9">
-        <f>E217/E216</f>
+        <f t="shared" si="24"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q218" s="9">
-        <f>F217/F216</f>
+        <f t="shared" si="25"/>
         <v>0.70710678118654802</v>
       </c>
     </row>
     <row r="219" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A219" s="100" t="s">
+      <c r="A219" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="B219" s="100"/>
-      <c r="C219" s="100"/>
-      <c r="D219" s="100"/>
-      <c r="E219" s="100"/>
-      <c r="F219" s="100"/>
+      <c r="B219" s="111"/>
+      <c r="C219" s="111"/>
+      <c r="D219" s="111"/>
+      <c r="E219" s="111"/>
+      <c r="F219" s="111"/>
     </row>
     <row r="220" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A220" s="110" t="s">
+      <c r="A220" s="99" t="s">
         <v>2</v>
       </c>
       <c r="B220" s="43"/>
       <c r="C220" s="43"/>
-      <c r="D220" s="99" t="s">
+      <c r="D220" s="103" t="s">
         <v>51</v>
       </c>
-      <c r="E220" s="99"/>
-      <c r="F220" s="99"/>
+      <c r="E220" s="103"/>
+      <c r="F220" s="103"/>
     </row>
     <row r="221" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A221" s="110"/>
+      <c r="A221" s="99"/>
       <c r="B221" s="43"/>
       <c r="C221" s="44" t="s">
         <v>47</v>
@@ -11437,14 +11437,14 @@
       <c r="F222" s="81">
         <v>0</v>
       </c>
-      <c r="N222" s="114" t="s">
+      <c r="N222" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="O222" s="115" t="s">
-        <v>97</v>
-      </c>
-      <c r="P222" s="115"/>
-      <c r="Q222" s="115"/>
+      <c r="O222" s="93" t="s">
+        <v>96</v>
+      </c>
+      <c r="P222" s="93"/>
+      <c r="Q222" s="93"/>
     </row>
     <row r="223" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A223" s="45" t="s">
@@ -11557,15 +11557,15 @@
         <v>33</v>
       </c>
       <c r="O226" s="9">
-        <f>D225/D224</f>
+        <f t="shared" ref="O226:O238" si="27">D225/D224</f>
         <v>2.4</v>
       </c>
       <c r="P226" s="9">
-        <f>E225/E224</f>
+        <f t="shared" ref="P226:P238" si="28">E225/E224</f>
         <v>2.4</v>
       </c>
       <c r="Q226" s="9">
-        <f>F225/F224</f>
+        <f t="shared" ref="Q226:Q238" si="29">F225/F224</f>
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -11590,15 +11590,15 @@
         <v>34</v>
       </c>
       <c r="O227" s="9">
-        <f>D226/D225</f>
+        <f t="shared" si="27"/>
         <v>4</v>
       </c>
       <c r="P227" s="9">
-        <f>E226/E225</f>
+        <f t="shared" si="28"/>
         <v>4</v>
       </c>
       <c r="Q227" s="9">
-        <f>F226/F225</f>
+        <f t="shared" si="29"/>
         <v>4</v>
       </c>
     </row>
@@ -11610,7 +11610,7 @@
         <v>10</v>
       </c>
       <c r="C228" s="43">
-        <f t="shared" ref="C228:C237" si="24">EXP(LN(0.5)*B227/10)</f>
+        <f t="shared" ref="C228:C237" si="30">EXP(LN(0.5)*B227/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D228" s="81">
@@ -11626,15 +11626,15 @@
         <v>35</v>
       </c>
       <c r="O228" s="9">
-        <f>D227/D226</f>
+        <f t="shared" si="27"/>
         <v>1.8750000000000002</v>
       </c>
       <c r="P228" s="9">
-        <f>E227/E226</f>
+        <f t="shared" si="28"/>
         <v>1.875</v>
       </c>
       <c r="Q228" s="9">
-        <f>F227/F226</f>
+        <f t="shared" si="29"/>
         <v>1.8749999999999998</v>
       </c>
     </row>
@@ -11646,7 +11646,7 @@
         <v>15</v>
       </c>
       <c r="C229" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0.5</v>
       </c>
       <c r="D229" s="81">
@@ -11662,15 +11662,15 @@
         <v>36</v>
       </c>
       <c r="O229" s="9">
-        <f>D228/D227</f>
+        <f t="shared" si="27"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="P229" s="9">
-        <f>E228/E227</f>
+        <f t="shared" si="28"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q229" s="9">
-        <f>F228/F227</f>
+        <f t="shared" si="29"/>
         <v>0.70710678118654846</v>
       </c>
     </row>
@@ -11682,7 +11682,7 @@
         <v>20</v>
       </c>
       <c r="C230" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0.35355339059327379</v>
       </c>
       <c r="D230" s="81">
@@ -11698,15 +11698,15 @@
         <v>37</v>
       </c>
       <c r="O230" s="9">
-        <f>D229/D228</f>
+        <f t="shared" si="27"/>
         <v>0.70710678118654735</v>
       </c>
       <c r="P230" s="9">
-        <f>E229/E228</f>
+        <f t="shared" si="28"/>
         <v>0.70710678118654702</v>
       </c>
       <c r="Q230" s="9">
-        <f>F229/F228</f>
+        <f t="shared" si="29"/>
         <v>0.70710678118654657</v>
       </c>
     </row>
@@ -11718,7 +11718,7 @@
         <v>25</v>
       </c>
       <c r="C231" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0.25</v>
       </c>
       <c r="D231" s="81">
@@ -11734,15 +11734,15 @@
         <v>38</v>
       </c>
       <c r="O231" s="9">
-        <f>D230/D229</f>
+        <f t="shared" si="27"/>
         <v>0.70710678118654702</v>
       </c>
       <c r="P231" s="9">
-        <f>E230/E229</f>
+        <f t="shared" si="28"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q231" s="9">
-        <f>F230/F229</f>
+        <f t="shared" si="29"/>
         <v>0.70710678118654646</v>
       </c>
     </row>
@@ -11754,7 +11754,7 @@
         <v>30</v>
       </c>
       <c r="C232" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0.17677669529663689</v>
       </c>
       <c r="D232" s="81">
@@ -11770,15 +11770,15 @@
         <v>39</v>
       </c>
       <c r="O232" s="9">
-        <f>D231/D230</f>
+        <f t="shared" si="27"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="P232" s="9">
-        <f>E231/E230</f>
+        <f t="shared" si="28"/>
         <v>0.70710678118654702</v>
       </c>
       <c r="Q232" s="9">
-        <f>F231/F230</f>
+        <f t="shared" si="29"/>
         <v>0.70710678118654857</v>
       </c>
     </row>
@@ -11790,7 +11790,7 @@
         <v>35</v>
       </c>
       <c r="C233" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0.12500000000000003</v>
       </c>
       <c r="D233" s="81">
@@ -11806,15 +11806,15 @@
         <v>40</v>
       </c>
       <c r="O233" s="9">
-        <f>D232/D231</f>
+        <f t="shared" si="27"/>
         <v>0.78567420131838739</v>
       </c>
       <c r="P233" s="9">
-        <f>E232/E231</f>
+        <f t="shared" si="28"/>
         <v>0.78567420131838561</v>
       </c>
       <c r="Q233" s="9">
-        <f>F232/F231</f>
+        <f t="shared" si="29"/>
         <v>0.78567420131838639</v>
       </c>
     </row>
@@ -11826,7 +11826,7 @@
         <v>40</v>
       </c>
       <c r="C234" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>8.8388347648318447E-2</v>
       </c>
       <c r="D234" s="81">
@@ -11842,15 +11842,15 @@
         <v>41</v>
       </c>
       <c r="O234" s="9">
-        <f>D233/D232</f>
+        <f t="shared" si="27"/>
         <v>0.70710678118654635</v>
       </c>
       <c r="P234" s="9">
-        <f>E233/E232</f>
+        <f t="shared" si="28"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q234" s="9">
-        <f>F233/F232</f>
+        <f t="shared" si="29"/>
         <v>0.70710678118654724</v>
       </c>
     </row>
@@ -11862,7 +11862,7 @@
         <v>45</v>
       </c>
       <c r="C235" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>6.25E-2</v>
       </c>
       <c r="D235" s="81">
@@ -11878,15 +11878,15 @@
         <v>42</v>
       </c>
       <c r="O235" s="9">
-        <f>D234/D233</f>
+        <f t="shared" si="27"/>
         <v>0.70710678118654868</v>
       </c>
       <c r="P235" s="9">
-        <f>E234/E233</f>
+        <f t="shared" si="28"/>
         <v>0.70710678118654779</v>
       </c>
       <c r="Q235" s="9">
-        <f>F234/F233</f>
+        <f t="shared" si="29"/>
         <v>0.70710678118654702</v>
       </c>
     </row>
@@ -11914,15 +11914,15 @@
         <v>43</v>
       </c>
       <c r="O236" s="9">
-        <f>D235/D234</f>
+        <f t="shared" si="27"/>
         <v>0.70710678118654635</v>
       </c>
       <c r="P236" s="9">
-        <f>E235/E234</f>
+        <f t="shared" si="28"/>
         <v>0.70710678118654724</v>
       </c>
       <c r="Q236" s="9">
-        <f>F235/F234</f>
+        <f t="shared" si="29"/>
         <v>0.70710678118654802</v>
       </c>
     </row>
@@ -11934,7 +11934,7 @@
         <v>55</v>
       </c>
       <c r="C237" s="43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>3.125E-2</v>
       </c>
       <c r="D237" s="81">
@@ -11950,15 +11950,15 @@
         <v>44</v>
       </c>
       <c r="O237" s="9">
-        <f>D236/D235</f>
+        <f t="shared" si="27"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="P237" s="9">
-        <f>E236/E235</f>
+        <f t="shared" si="28"/>
         <v>0.70710678118654713</v>
       </c>
       <c r="Q237" s="9">
-        <f>F236/F235</f>
+        <f t="shared" si="29"/>
         <v>0.70710678118654702</v>
       </c>
     </row>
@@ -11973,15 +11973,15 @@
         <v>45</v>
       </c>
       <c r="O238" s="9">
-        <f>D237/D236</f>
+        <f t="shared" si="27"/>
         <v>0.70710678118654735</v>
       </c>
       <c r="P238" s="9">
-        <f>E237/E236</f>
+        <f t="shared" si="28"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q238" s="9">
-        <f>F237/F236</f>
+        <f t="shared" si="29"/>
         <v>0.70710678118654802</v>
       </c>
     </row>
@@ -12038,19 +12038,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="O222:Q222"/>
-    <mergeCell ref="O202:Q202"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A161:A162"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="E161:G161"/>
-    <mergeCell ref="A186:C186"/>
-    <mergeCell ref="A198:F198"/>
-    <mergeCell ref="A199:F199"/>
-    <mergeCell ref="D200:F200"/>
-    <mergeCell ref="D220:F220"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="I133:I135"/>
     <mergeCell ref="J133:O133"/>
@@ -12067,6 +12054,19 @@
     <mergeCell ref="B52:D52"/>
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
+    <mergeCell ref="O222:Q222"/>
+    <mergeCell ref="O202:Q202"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="E161:G161"/>
+    <mergeCell ref="A186:C186"/>
+    <mergeCell ref="A198:F198"/>
+    <mergeCell ref="A199:F199"/>
+    <mergeCell ref="D200:F200"/>
+    <mergeCell ref="D220:F220"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Push forward start year to 1925
It looks like cervical cancer incidence/prevalence equilibrates within
55 years. Therefore, pushing forward the start year from 1910 to 1925.
This will make the historical part of the model run faster during
calibration.
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -447,27 +447,6 @@
     <t>Male Age Ratios</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Initial population size (1910).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Calculate backward-projected KZN population. Assume that KZN:SA proportion was decreasing from 1910-2002 according to same trend as from 2002-2019. Assume male and female populations by age follow exponential distributions. See Population_validation Excel document for more detail.</t>
-    </r>
-  </si>
-  <si>
     <t>1950-1955</t>
   </si>
   <si>
@@ -499,6 +478,27 @@
   </si>
   <si>
     <t>Note: fertility rates decline linearly from 1960 to 2000 so that the model's population growth resembles actual population growth patterns and as stated by Moultrie 2003. Fertility rates stall between 2000 and 2010 as described by Moultrie 2008. Fertility rate declines again between 2010 and 2020 as described by Moultri 2007 and seen in observed data. Increasing initial values provided by Nick and Monisha so that fertility in HIV-negative women more closely matches observed data. The exact absolute values seem to be reasonable but semi-arbitrary anyways.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Initial population size (1925).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Calculate backward-projected KZN population. Assume that KZN:SA proportion was decreasing from 1925-2002 according to same trend as from 2002-2019. Assume male and female populations by age follow exponential distributions. See Population_validation Excel document for more detail.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1619,6 +1619,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1640,9 +1691,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1655,58 +1703,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1819,6 +1819,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1977,52 +1978,52 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>-116459.19703766501</c:v>
+                  <c:v>-152100.42167838168</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-76187.743222862409</c:v>
+                  <c:v>-106612.48230402569</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-75385.542052984893</c:v>
+                  <c:v>-107405.94202558786</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-71896.515135187161</c:v>
+                  <c:v>-101517.15463011744</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-51997.757864486186</c:v>
+                  <c:v>-72544.531411124772</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-46601.769480501192</c:v>
+                  <c:v>-64144.510344209695</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-38908.922911900998</c:v>
+                  <c:v>-52521.552285925158</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-32485.982807963814</c:v>
+                  <c:v>-43004.6692962585</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-48105.36893136811</c:v>
+                  <c:v>-62733.386819434447</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-27123.317738423211</c:v>
+                  <c:v>-35212.241466369451</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-26837.729055778073</c:v>
+                  <c:v>-35474.307358708502</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-18123.756746459323</c:v>
+                  <c:v>-24318.165076374728</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-13980.530844150357</c:v>
+                  <c:v>-19243.353103262907</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-8178.1693204119674</c:v>
+                  <c:v>-11512.902075623842</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-6756.2521870106111</c:v>
+                  <c:v>-9496.9275082166223</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-4250.4736070178951</c:v>
+                  <c:v>-6028.6940611282835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2149,52 +2150,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>156852.19677743601</c:v>
+                  <c:v>203324.64541775131</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>102612.89100384487</c:v>
+                  <c:v>142517.32455685426</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87786.369045850632</c:v>
+                  <c:v>124325.88693031289</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>63757.10410526843</c:v>
+                  <c:v>90430.410916924244</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51450.259534369194</c:v>
+                  <c:v>73084.441583464475</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43513.908158546546</c:v>
+                  <c:v>61533.430640663515</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53232.318780424968</c:v>
+                  <c:v>74044.458827794922</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31805.477141060052</c:v>
+                  <c:v>43647.172872749325</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43876.145321947617</c:v>
+                  <c:v>58960.6802707362</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29945.25213595013</c:v>
+                  <c:v>40119.832401277803</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18123.756746459323</c:v>
+                  <c:v>24318.165076374728</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22803.929628009573</c:v>
+                  <c:v>30874.570169486131</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19286.357512430386</c:v>
+                  <c:v>25994.838038336002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13333.47774733694</c:v>
+                  <c:v>18188.290291429978</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8591.4084565294525</c:v>
+                  <c:v>11968.314355555985</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3048.693222367976</c:v>
+                  <c:v>4496.1121070609634</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2333,6 +2334,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3279,7 +3281,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3968,7 +3969,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8187,8 +8187,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G134" sqref="G134"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8233,7 +8233,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -8261,16 +8261,16 @@
       <c r="Y1" s="37"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="109" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -8322,14 +8322,14 @@
       <c r="A4" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="105"/>
-      <c r="D4" s="104" t="s">
+      <c r="C4" s="102"/>
+      <c r="D4" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="105"/>
+      <c r="E4" s="102"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -8353,18 +8353,18 @@
         <v>6</v>
       </c>
       <c r="B6" s="54">
-        <v>116.45919703766501</v>
+        <v>152.10042167838168</v>
       </c>
       <c r="C6" s="54">
-        <v>156.85219677743601</v>
+        <v>203.3246454177513</v>
       </c>
       <c r="D6" s="51">
         <f>B6*1000</f>
-        <v>116459.19703766501</v>
+        <v>152100.42167838168</v>
       </c>
       <c r="E6" s="51">
         <f>C6*1000</f>
-        <v>156852.19677743601</v>
+        <v>203324.64541775131</v>
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="56"/>
@@ -8376,18 +8376,18 @@
         <v>9</v>
       </c>
       <c r="B7" s="54">
-        <v>76.187743222862409</v>
+        <v>106.61248230402569</v>
       </c>
       <c r="C7" s="54">
-        <v>102.61289100384487</v>
+        <v>142.51732455685425</v>
       </c>
       <c r="D7" s="51">
         <f t="shared" ref="D7:D21" si="0">B7*1000</f>
-        <v>76187.743222862409</v>
+        <v>106612.48230402569</v>
       </c>
       <c r="E7" s="51">
         <f t="shared" ref="E7:E21" si="1">C7*1000</f>
-        <v>102612.89100384487</v>
+        <v>142517.32455685426</v>
       </c>
       <c r="F7" s="56"/>
       <c r="G7" s="56"/>
@@ -8399,18 +8399,18 @@
         <v>12</v>
       </c>
       <c r="B8" s="54">
-        <v>75.385542052984889</v>
+        <v>107.40594202558786</v>
       </c>
       <c r="C8" s="54">
-        <v>87.786369045850634</v>
+        <v>124.32588693031289</v>
       </c>
       <c r="D8" s="51">
         <f t="shared" si="0"/>
-        <v>75385.542052984893</v>
+        <v>107405.94202558786</v>
       </c>
       <c r="E8" s="51">
         <f t="shared" si="1"/>
-        <v>87786.369045850632</v>
+        <v>124325.88693031289</v>
       </c>
       <c r="F8" s="56"/>
       <c r="G8" s="56"/>
@@ -8422,18 +8422,18 @@
         <v>13</v>
       </c>
       <c r="B9" s="54">
-        <v>71.896515135187158</v>
+        <v>101.51715463011743</v>
       </c>
       <c r="C9" s="54">
-        <v>63.757104105268432</v>
+        <v>90.430410916924245</v>
       </c>
       <c r="D9" s="51">
         <f t="shared" si="0"/>
-        <v>71896.515135187161</v>
+        <v>101517.15463011744</v>
       </c>
       <c r="E9" s="51">
         <f t="shared" si="1"/>
-        <v>63757.10410526843</v>
+        <v>90430.410916924244</v>
       </c>
       <c r="F9" s="56"/>
       <c r="G9" s="56"/>
@@ -8445,18 +8445,18 @@
         <v>14</v>
       </c>
       <c r="B10" s="54">
-        <v>51.997757864486189</v>
+        <v>72.544531411124765</v>
       </c>
       <c r="C10" s="54">
-        <v>51.450259534369195</v>
+        <v>73.084441583464468</v>
       </c>
       <c r="D10" s="51">
         <f t="shared" si="0"/>
-        <v>51997.757864486186</v>
+        <v>72544.531411124772</v>
       </c>
       <c r="E10" s="51">
         <f t="shared" si="1"/>
-        <v>51450.259534369194</v>
+        <v>73084.441583464475</v>
       </c>
       <c r="F10" s="56"/>
       <c r="G10" s="56"/>
@@ -8468,18 +8468,18 @@
         <v>15</v>
       </c>
       <c r="B11" s="54">
-        <v>46.60176948050119</v>
+        <v>64.144510344209692</v>
       </c>
       <c r="C11" s="54">
-        <v>43.513908158546549</v>
+        <v>61.533430640663518</v>
       </c>
       <c r="D11" s="51">
         <f t="shared" si="0"/>
-        <v>46601.769480501192</v>
+        <v>64144.510344209695</v>
       </c>
       <c r="E11" s="51">
         <f t="shared" si="1"/>
-        <v>43513.908158546546</v>
+        <v>61533.430640663515</v>
       </c>
       <c r="F11" s="56"/>
       <c r="G11" s="56"/>
@@ -8491,18 +8491,18 @@
         <v>16</v>
       </c>
       <c r="B12" s="54">
-        <v>38.908922911901001</v>
+        <v>52.521552285925161</v>
       </c>
       <c r="C12" s="54">
-        <v>53.232318780424968</v>
+        <v>74.044458827794926</v>
       </c>
       <c r="D12" s="51">
         <f t="shared" si="0"/>
-        <v>38908.922911900998</v>
+        <v>52521.552285925158</v>
       </c>
       <c r="E12" s="51">
         <f t="shared" si="1"/>
-        <v>53232.318780424968</v>
+        <v>74044.458827794922</v>
       </c>
       <c r="F12" s="56"/>
       <c r="G12" s="56"/>
@@ -8514,18 +8514,18 @@
         <v>17</v>
       </c>
       <c r="B13" s="54">
-        <v>32.485982807963815</v>
+        <v>43.004669296258498</v>
       </c>
       <c r="C13" s="54">
-        <v>31.805477141060052</v>
+        <v>43.647172872749323</v>
       </c>
       <c r="D13" s="51">
         <f t="shared" si="0"/>
-        <v>32485.982807963814</v>
+        <v>43004.6692962585</v>
       </c>
       <c r="E13" s="51">
         <f t="shared" si="1"/>
-        <v>31805.477141060052</v>
+        <v>43647.172872749325</v>
       </c>
       <c r="F13" s="56"/>
       <c r="G13" s="56"/>
@@ -8537,18 +8537,18 @@
         <v>19</v>
       </c>
       <c r="B14" s="54">
-        <v>48.105368931368112</v>
+        <v>62.73338681943445</v>
       </c>
       <c r="C14" s="54">
-        <v>43.876145321947618</v>
+        <v>58.960680270736198</v>
       </c>
       <c r="D14" s="51">
         <f t="shared" si="0"/>
-        <v>48105.36893136811</v>
+        <v>62733.386819434447</v>
       </c>
       <c r="E14" s="51">
         <f t="shared" si="1"/>
-        <v>43876.145321947617</v>
+        <v>58960.6802707362</v>
       </c>
       <c r="F14" s="56"/>
       <c r="G14" s="56"/>
@@ -8560,18 +8560,18 @@
         <v>20</v>
       </c>
       <c r="B15" s="54">
-        <v>27.123317738423211</v>
+        <v>35.212241466369449</v>
       </c>
       <c r="C15" s="54">
-        <v>29.945252135950131</v>
+        <v>40.119832401277804</v>
       </c>
       <c r="D15" s="51">
         <f t="shared" si="0"/>
-        <v>27123.317738423211</v>
+        <v>35212.241466369451</v>
       </c>
       <c r="E15" s="51">
         <f t="shared" si="1"/>
-        <v>29945.25213595013</v>
+        <v>40119.832401277803</v>
       </c>
       <c r="F15" s="56"/>
       <c r="G15" s="56"/>
@@ -8583,18 +8583,18 @@
         <v>21</v>
       </c>
       <c r="B16" s="54">
-        <v>26.837729055778073</v>
+        <v>35.474307358708501</v>
       </c>
       <c r="C16" s="54">
-        <v>18.123756746459325</v>
+        <v>24.318165076374729</v>
       </c>
       <c r="D16" s="51">
         <f t="shared" si="0"/>
-        <v>26837.729055778073</v>
+        <v>35474.307358708502</v>
       </c>
       <c r="E16" s="51">
         <f t="shared" si="1"/>
-        <v>18123.756746459323</v>
+        <v>24318.165076374728</v>
       </c>
       <c r="F16" s="56"/>
       <c r="G16" s="56"/>
@@ -8606,18 +8606,18 @@
         <v>22</v>
       </c>
       <c r="B17" s="54">
-        <v>18.123756746459325</v>
+        <v>24.318165076374729</v>
       </c>
       <c r="C17" s="54">
-        <v>22.803929628009573</v>
+        <v>30.87457016948613</v>
       </c>
       <c r="D17" s="51">
         <f t="shared" si="0"/>
-        <v>18123.756746459323</v>
+        <v>24318.165076374728</v>
       </c>
       <c r="E17" s="51">
         <f t="shared" si="1"/>
-        <v>22803.929628009573</v>
+        <v>30874.570169486131</v>
       </c>
       <c r="F17" s="56"/>
       <c r="G17" s="56"/>
@@ -8629,18 +8629,18 @@
         <v>42</v>
       </c>
       <c r="B18" s="54">
-        <v>13.980530844150357</v>
+        <v>19.243353103262908</v>
       </c>
       <c r="C18" s="54">
-        <v>19.286357512430385</v>
+        <v>25.994838038336002</v>
       </c>
       <c r="D18" s="51">
         <f t="shared" si="0"/>
-        <v>13980.530844150357</v>
+        <v>19243.353103262907</v>
       </c>
       <c r="E18" s="51">
         <f t="shared" si="1"/>
-        <v>19286.357512430386</v>
+        <v>25994.838038336002</v>
       </c>
       <c r="F18" s="56"/>
       <c r="G18" s="56"/>
@@ -8652,18 +8652,18 @@
         <v>43</v>
       </c>
       <c r="B19" s="54">
-        <v>8.1781693204119676</v>
+        <v>11.512902075623842</v>
       </c>
       <c r="C19" s="54">
-        <v>13.333477747336939</v>
+        <v>18.188290291429979</v>
       </c>
       <c r="D19" s="51">
         <f t="shared" si="0"/>
-        <v>8178.1693204119674</v>
+        <v>11512.902075623842</v>
       </c>
       <c r="E19" s="51">
         <f t="shared" si="1"/>
-        <v>13333.47774733694</v>
+        <v>18188.290291429978</v>
       </c>
       <c r="F19" s="56"/>
       <c r="G19" s="56"/>
@@ -8675,18 +8675,18 @@
         <v>44</v>
       </c>
       <c r="B20" s="54">
-        <v>6.7562521870106114</v>
+        <v>9.496927508216622</v>
       </c>
       <c r="C20" s="54">
-        <v>8.591408456529452</v>
+        <v>11.968314355555986</v>
       </c>
       <c r="D20" s="51">
         <f t="shared" si="0"/>
-        <v>6756.2521870106111</v>
+        <v>9496.9275082166223</v>
       </c>
       <c r="E20" s="51">
         <f t="shared" si="1"/>
-        <v>8591.4084565294525</v>
+        <v>11968.314355555985</v>
       </c>
       <c r="F20" s="56"/>
       <c r="G20" s="56"/>
@@ -8698,18 +8698,18 @@
         <v>45</v>
       </c>
       <c r="B21" s="54">
-        <v>4.250473607017895</v>
+        <v>6.0286940611282835</v>
       </c>
       <c r="C21" s="54">
-        <v>3.0486932223679761</v>
+        <v>4.4961121070609638</v>
       </c>
       <c r="D21" s="51">
         <f t="shared" si="0"/>
-        <v>4250.4736070178951</v>
+        <v>6028.6940611282835</v>
       </c>
       <c r="E21" s="51">
         <f t="shared" si="1"/>
-        <v>3048.693222367976</v>
+        <v>4496.1121070609634</v>
       </c>
       <c r="F21" s="56"/>
       <c r="G21" s="56"/>
@@ -8722,23 +8722,23 @@
       </c>
       <c r="B22" s="9">
         <f>SUM(B6:B21)</f>
-        <v>663.27902894417116</v>
+        <v>903.87124144474967</v>
       </c>
       <c r="C22" s="9">
         <f>SUM(C6:C21)</f>
-        <v>750.01954531783213</v>
+        <v>1027.8285744567727</v>
       </c>
       <c r="D22" s="9">
         <f>SUM(D6:D21)</f>
-        <v>663279.02894417115</v>
+        <v>903871.24144474964</v>
       </c>
       <c r="E22" s="9">
         <f>SUM(E6:E21)</f>
-        <v>750019.54531783226</v>
+        <v>1027828.5744567729</v>
       </c>
       <c r="F22" s="57">
         <f>D22+E22</f>
-        <v>1413298.5742620034</v>
+        <v>1931699.8159015225</v>
       </c>
       <c r="G22" s="25"/>
       <c r="X22" s="13"/>
@@ -8757,10 +8757,10 @@
       <c r="A27" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="104" t="s">
+      <c r="B27" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="105"/>
+      <c r="C27" s="102"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -8778,11 +8778,11 @@
       </c>
       <c r="B29" s="58">
         <f>(-1)*D6</f>
-        <v>-116459.19703766501</v>
+        <v>-152100.42167838168</v>
       </c>
       <c r="C29" s="17">
         <f>E6</f>
-        <v>156852.19677743601</v>
+        <v>203324.64541775131</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -8791,11 +8791,11 @@
       </c>
       <c r="B30" s="58">
         <f t="shared" ref="B30:B44" si="2">(-1)*D7</f>
-        <v>-76187.743222862409</v>
+        <v>-106612.48230402569</v>
       </c>
       <c r="C30" s="17">
         <f t="shared" ref="C30:C44" si="3">E7</f>
-        <v>102612.89100384487</v>
+        <v>142517.32455685426</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -8804,11 +8804,11 @@
       </c>
       <c r="B31" s="58">
         <f t="shared" si="2"/>
-        <v>-75385.542052984893</v>
+        <v>-107405.94202558786</v>
       </c>
       <c r="C31" s="17">
         <f t="shared" si="3"/>
-        <v>87786.369045850632</v>
+        <v>124325.88693031289</v>
       </c>
       <c r="L31" s="8"/>
     </row>
@@ -8818,11 +8818,11 @@
       </c>
       <c r="B32" s="58">
         <f t="shared" si="2"/>
-        <v>-71896.515135187161</v>
+        <v>-101517.15463011744</v>
       </c>
       <c r="C32" s="17">
         <f t="shared" si="3"/>
-        <v>63757.10410526843</v>
+        <v>90430.410916924244</v>
       </c>
     </row>
     <row r="33" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
@@ -8831,11 +8831,11 @@
       </c>
       <c r="B33" s="58">
         <f t="shared" si="2"/>
-        <v>-51997.757864486186</v>
+        <v>-72544.531411124772</v>
       </c>
       <c r="C33" s="17">
         <f t="shared" si="3"/>
-        <v>51450.259534369194</v>
+        <v>73084.441583464475</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
@@ -8844,11 +8844,11 @@
       </c>
       <c r="B34" s="58">
         <f t="shared" si="2"/>
-        <v>-46601.769480501192</v>
+        <v>-64144.510344209695</v>
       </c>
       <c r="C34" s="17">
         <f t="shared" si="3"/>
-        <v>43513.908158546546</v>
+        <v>61533.430640663515</v>
       </c>
     </row>
     <row r="35" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
@@ -8857,11 +8857,11 @@
       </c>
       <c r="B35" s="58">
         <f t="shared" si="2"/>
-        <v>-38908.922911900998</v>
+        <v>-52521.552285925158</v>
       </c>
       <c r="C35" s="17">
         <f t="shared" si="3"/>
-        <v>53232.318780424968</v>
+        <v>74044.458827794922</v>
       </c>
     </row>
     <row r="36" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
@@ -8870,11 +8870,11 @@
       </c>
       <c r="B36" s="58">
         <f t="shared" si="2"/>
-        <v>-32485.982807963814</v>
+        <v>-43004.6692962585</v>
       </c>
       <c r="C36" s="17">
         <f t="shared" si="3"/>
-        <v>31805.477141060052</v>
+        <v>43647.172872749325</v>
       </c>
       <c r="X36" s="13"/>
       <c r="Y36" s="13"/>
@@ -8892,11 +8892,11 @@
       </c>
       <c r="B37" s="58">
         <f t="shared" si="2"/>
-        <v>-48105.36893136811</v>
+        <v>-62733.386819434447</v>
       </c>
       <c r="C37" s="17">
         <f t="shared" si="3"/>
-        <v>43876.145321947617</v>
+        <v>58960.6802707362</v>
       </c>
       <c r="X37" s="14"/>
       <c r="Y37" s="14"/>
@@ -8913,11 +8913,11 @@
       </c>
       <c r="B38" s="58">
         <f t="shared" si="2"/>
-        <v>-27123.317738423211</v>
+        <v>-35212.241466369451</v>
       </c>
       <c r="C38" s="17">
         <f t="shared" si="3"/>
-        <v>29945.25213595013</v>
+        <v>40119.832401277803</v>
       </c>
       <c r="X38" s="22"/>
       <c r="Y38" s="22"/>
@@ -8934,11 +8934,11 @@
       </c>
       <c r="B39" s="58">
         <f t="shared" si="2"/>
-        <v>-26837.729055778073</v>
+        <v>-35474.307358708502</v>
       </c>
       <c r="C39" s="17">
         <f t="shared" si="3"/>
-        <v>18123.756746459323</v>
+        <v>24318.165076374728</v>
       </c>
       <c r="X39" s="23"/>
       <c r="Y39" s="23"/>
@@ -8955,11 +8955,11 @@
       </c>
       <c r="B40" s="58">
         <f t="shared" si="2"/>
-        <v>-18123.756746459323</v>
+        <v>-24318.165076374728</v>
       </c>
       <c r="C40" s="17">
         <f t="shared" si="3"/>
-        <v>22803.929628009573</v>
+        <v>30874.570169486131</v>
       </c>
       <c r="X40" s="23"/>
       <c r="Y40" s="23"/>
@@ -8976,11 +8976,11 @@
       </c>
       <c r="B41" s="58">
         <f t="shared" si="2"/>
-        <v>-13980.530844150357</v>
+        <v>-19243.353103262907</v>
       </c>
       <c r="C41" s="17">
         <f t="shared" si="3"/>
-        <v>19286.357512430386</v>
+        <v>25994.838038336002</v>
       </c>
       <c r="X41" s="23"/>
       <c r="Y41" s="23"/>
@@ -8997,11 +8997,11 @@
       </c>
       <c r="B42" s="58">
         <f t="shared" si="2"/>
-        <v>-8178.1693204119674</v>
+        <v>-11512.902075623842</v>
       </c>
       <c r="C42" s="17">
         <f t="shared" si="3"/>
-        <v>13333.47774733694</v>
+        <v>18188.290291429978</v>
       </c>
       <c r="X42" s="24"/>
       <c r="Y42" s="24"/>
@@ -9018,11 +9018,11 @@
       </c>
       <c r="B43" s="58">
         <f t="shared" si="2"/>
-        <v>-6756.2521870106111</v>
+        <v>-9496.9275082166223</v>
       </c>
       <c r="C43" s="17">
         <f t="shared" si="3"/>
-        <v>8591.4084565294525</v>
+        <v>11968.314355555985</v>
       </c>
       <c r="X43" s="24"/>
       <c r="Y43" s="24"/>
@@ -9039,11 +9039,11 @@
       </c>
       <c r="B44" s="58">
         <f t="shared" si="2"/>
-        <v>-4250.4736070178951</v>
+        <v>-6028.6940611282835</v>
       </c>
       <c r="C44" s="17">
         <f t="shared" si="3"/>
-        <v>3048.693222367976</v>
+        <v>4496.1121070609634</v>
       </c>
       <c r="X44" s="24"/>
       <c r="Y44" s="24"/>
@@ -9175,19 +9175,19 @@
       <c r="AE51" s="24"/>
     </row>
     <row r="52" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="106" t="s">
+      <c r="B52" s="120" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106" t="s">
+      <c r="C52" s="120"/>
+      <c r="D52" s="120"/>
+      <c r="E52" s="120" t="s">
         <v>57</v>
       </c>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
+      <c r="F52" s="120"/>
+      <c r="G52" s="120"/>
       <c r="X52" s="22"/>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
@@ -9198,7 +9198,7 @@
       <c r="AE52" s="22"/>
     </row>
     <row r="53" spans="1:31" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="106"/>
+      <c r="A53" s="120"/>
       <c r="B53" s="33" t="s">
         <v>3</v>
       </c>
@@ -9705,7 +9705,7 @@
     </row>
     <row r="80" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B80" s="37"/>
       <c r="C80" s="37"/>
@@ -9732,158 +9732,158 @@
       <c r="X80" s="37"/>
     </row>
     <row r="81" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="107" t="s">
+      <c r="A81" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="112" t="s">
+      <c r="B81" s="93" t="s">
         <v>81</v>
       </c>
-      <c r="C81" s="112"/>
-      <c r="D81" s="112"/>
-      <c r="E81" s="112"/>
-      <c r="F81" s="112"/>
-      <c r="G81" s="112"/>
-      <c r="H81" s="112"/>
-      <c r="I81" s="112"/>
+      <c r="C81" s="93"/>
+      <c r="D81" s="93"/>
+      <c r="E81" s="93"/>
+      <c r="F81" s="93"/>
+      <c r="G81" s="93"/>
+      <c r="H81" s="93"/>
+      <c r="I81" s="93"/>
       <c r="J81" s="35"/>
-      <c r="K81" s="107" t="s">
+      <c r="K81" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="L81" s="112" t="s">
+      <c r="L81" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="M81" s="112"/>
-      <c r="N81" s="112"/>
-      <c r="O81" s="112"/>
-      <c r="P81" s="112"/>
-      <c r="Q81" s="112"/>
-      <c r="R81" s="112"/>
-      <c r="S81" s="112"/>
+      <c r="M81" s="93"/>
+      <c r="N81" s="93"/>
+      <c r="O81" s="93"/>
+      <c r="P81" s="93"/>
+      <c r="Q81" s="93"/>
+      <c r="R81" s="93"/>
+      <c r="S81" s="93"/>
       <c r="T81" s="35"/>
-      <c r="U81" s="118" t="s">
+      <c r="U81" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="V81" s="118"/>
-      <c r="W81" s="118"/>
-      <c r="X81" s="118"/>
-      <c r="Y81" s="118"/>
-      <c r="Z81" s="118"/>
-      <c r="AA81" s="118"/>
-      <c r="AB81" s="118"/>
-      <c r="AC81" s="118"/>
+      <c r="V81" s="92"/>
+      <c r="W81" s="92"/>
+      <c r="X81" s="92"/>
+      <c r="Y81" s="92"/>
+      <c r="Z81" s="92"/>
+      <c r="AA81" s="92"/>
+      <c r="AB81" s="92"/>
+      <c r="AC81" s="92"/>
     </row>
     <row r="82" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="108"/>
-      <c r="B82" s="112"/>
-      <c r="C82" s="112"/>
-      <c r="D82" s="112"/>
-      <c r="E82" s="112"/>
-      <c r="F82" s="112"/>
-      <c r="G82" s="112"/>
-      <c r="H82" s="112"/>
-      <c r="I82" s="112"/>
+      <c r="A82" s="95"/>
+      <c r="B82" s="93"/>
+      <c r="C82" s="93"/>
+      <c r="D82" s="93"/>
+      <c r="E82" s="93"/>
+      <c r="F82" s="93"/>
+      <c r="G82" s="93"/>
+      <c r="H82" s="93"/>
+      <c r="I82" s="93"/>
       <c r="J82" s="35"/>
-      <c r="K82" s="108"/>
-      <c r="L82" s="112"/>
-      <c r="M82" s="112"/>
-      <c r="N82" s="112"/>
-      <c r="O82" s="112"/>
-      <c r="P82" s="112"/>
-      <c r="Q82" s="112"/>
-      <c r="R82" s="112"/>
-      <c r="S82" s="112"/>
+      <c r="K82" s="95"/>
+      <c r="L82" s="93"/>
+      <c r="M82" s="93"/>
+      <c r="N82" s="93"/>
+      <c r="O82" s="93"/>
+      <c r="P82" s="93"/>
+      <c r="Q82" s="93"/>
+      <c r="R82" s="93"/>
+      <c r="S82" s="93"/>
       <c r="T82" s="35"/>
-      <c r="U82" s="118" t="s">
+      <c r="U82" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="V82" s="119" t="s">
+      <c r="V82" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="W82" s="120"/>
-      <c r="X82" s="120"/>
-      <c r="Y82" s="120"/>
-      <c r="Z82" s="120"/>
-      <c r="AA82" s="120"/>
-      <c r="AB82" s="120"/>
-      <c r="AC82" s="121"/>
+      <c r="W82" s="98"/>
+      <c r="X82" s="98"/>
+      <c r="Y82" s="98"/>
+      <c r="Z82" s="98"/>
+      <c r="AA82" s="98"/>
+      <c r="AB82" s="98"/>
+      <c r="AC82" s="99"/>
     </row>
     <row r="83" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="109"/>
+      <c r="A83" s="96"/>
       <c r="B83" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="C83" s="79" t="s">
+      <c r="D83" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="D83" s="79" t="s">
+      <c r="E83" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="E83" s="79" t="s">
+      <c r="F83" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="G83" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="F83" s="88" t="s">
-        <v>104</v>
-      </c>
-      <c r="G83" s="79" t="s">
+      <c r="H83" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="I83" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="H83" s="79" t="s">
+      <c r="J83" s="35"/>
+      <c r="K83" s="96"/>
+      <c r="L83" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="M83" s="79" t="s">
+        <v>97</v>
+      </c>
+      <c r="N83" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="O83" s="79" t="s">
+        <v>99</v>
+      </c>
+      <c r="P83" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="I83" s="79" t="s">
+      <c r="Q83" s="79" t="s">
+        <v>100</v>
+      </c>
+      <c r="R83" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="J83" s="35"/>
-      <c r="K83" s="109"/>
-      <c r="L83" s="79" t="s">
+      <c r="S83" s="79" t="s">
+        <v>101</v>
+      </c>
+      <c r="T83" s="35"/>
+      <c r="U83" s="92"/>
+      <c r="V83" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="W83" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="M83" s="79" t="s">
+      <c r="X83" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="N83" s="79" t="s">
+      <c r="Y83" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="O83" s="79" t="s">
+      <c r="Z83" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA83" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="P83" s="80" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q83" s="79" t="s">
+      <c r="AB83" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC83" s="79" t="s">
         <v>101</v>
-      </c>
-      <c r="R83" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="S83" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="T83" s="35"/>
-      <c r="U83" s="118"/>
-      <c r="V83" s="79" t="s">
-        <v>97</v>
-      </c>
-      <c r="W83" s="79" t="s">
-        <v>98</v>
-      </c>
-      <c r="X83" s="79" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y83" s="79" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z83" s="80" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA83" s="79" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB83" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC83" s="79" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="84" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
@@ -10196,19 +10196,19 @@
         <v>1.6750273E-3</v>
       </c>
       <c r="T87" s="35"/>
-      <c r="U87" s="118" t="s">
+      <c r="U87" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="V87" s="118" t="s">
+      <c r="V87" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="W87" s="118"/>
-      <c r="X87" s="118"/>
-      <c r="Y87" s="118"/>
-      <c r="Z87" s="118"/>
-      <c r="AA87" s="118"/>
-      <c r="AB87" s="118"/>
-      <c r="AC87" s="118"/>
+      <c r="W87" s="92"/>
+      <c r="X87" s="92"/>
+      <c r="Y87" s="92"/>
+      <c r="Z87" s="92"/>
+      <c r="AA87" s="92"/>
+      <c r="AB87" s="92"/>
+      <c r="AC87" s="92"/>
     </row>
     <row r="88" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="75" t="s">
@@ -10267,30 +10267,30 @@
         <v>2.3815536E-3</v>
       </c>
       <c r="T88" s="35"/>
-      <c r="U88" s="118"/>
+      <c r="U88" s="92"/>
       <c r="V88" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="W88" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="W88" s="79" t="s">
+      <c r="X88" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="X88" s="79" t="s">
+      <c r="Y88" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="Y88" s="79" t="s">
+      <c r="Z88" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA88" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="Z88" s="80" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA88" s="79" t="s">
+      <c r="AB88" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC88" s="79" t="s">
         <v>101</v>
-      </c>
-      <c r="AB88" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC88" s="79" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
@@ -11288,25 +11288,25 @@
       <c r="X110" s="37"/>
     </row>
     <row r="111" spans="1:29" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="117" t="s">
-        <v>107</v>
-      </c>
-      <c r="B111" s="117"/>
-      <c r="C111" s="117"/>
-      <c r="D111" s="117"/>
-      <c r="E111" s="117"/>
-      <c r="F111" s="117"/>
-      <c r="G111" s="117"/>
-      <c r="H111" s="117"/>
-      <c r="I111" s="117"/>
-      <c r="J111" s="117"/>
-      <c r="K111" s="117"/>
-      <c r="L111" s="117"/>
-      <c r="M111" s="117"/>
-      <c r="N111" s="117"/>
-      <c r="O111" s="117"/>
-      <c r="P111" s="117"/>
-      <c r="Q111" s="117"/>
+      <c r="A111" s="108" t="s">
+        <v>106</v>
+      </c>
+      <c r="B111" s="108"/>
+      <c r="C111" s="108"/>
+      <c r="D111" s="108"/>
+      <c r="E111" s="108"/>
+      <c r="F111" s="108"/>
+      <c r="G111" s="108"/>
+      <c r="H111" s="108"/>
+      <c r="I111" s="108"/>
+      <c r="J111" s="108"/>
+      <c r="K111" s="108"/>
+      <c r="L111" s="108"/>
+      <c r="M111" s="108"/>
+      <c r="N111" s="108"/>
+      <c r="O111" s="108"/>
+      <c r="P111" s="108"/>
+      <c r="Q111" s="108"/>
       <c r="R111" s="37"/>
       <c r="S111" s="37"/>
       <c r="T111" s="37"/>
@@ -11316,17 +11316,17 @@
       <c r="X111" s="37"/>
     </row>
     <row r="112" spans="1:29" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="101" t="s">
+      <c r="A112" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="96" t="s">
+      <c r="B112" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="C112" s="97"/>
-      <c r="D112" s="97"/>
-      <c r="E112" s="97"/>
-      <c r="F112" s="97"/>
-      <c r="G112" s="98"/>
+      <c r="C112" s="114"/>
+      <c r="D112" s="114"/>
+      <c r="E112" s="114"/>
+      <c r="F112" s="114"/>
+      <c r="G112" s="115"/>
       <c r="I112" s="74"/>
       <c r="J112" s="90" t="s">
         <v>27</v>
@@ -11345,7 +11345,7 @@
       </c>
     </row>
     <row r="113" spans="1:14" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="102"/>
+      <c r="A113" s="118"/>
       <c r="B113" s="32" t="s">
         <v>70</v>
       </c>
@@ -11389,7 +11389,7 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="103"/>
+      <c r="A114" s="119"/>
       <c r="B114" s="34" t="s">
         <v>63</v>
       </c>
@@ -11437,14 +11437,14 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="I115" s="110" t="s">
-        <v>106</v>
-      </c>
-      <c r="J115" s="110"/>
-      <c r="K115" s="110"/>
-      <c r="L115" s="110"/>
-      <c r="M115" s="110"/>
-      <c r="N115" s="110"/>
+      <c r="I115" s="121" t="s">
+        <v>105</v>
+      </c>
+      <c r="J115" s="121"/>
+      <c r="K115" s="121"/>
+      <c r="L115" s="121"/>
+      <c r="M115" s="121"/>
+      <c r="N115" s="121"/>
     </row>
     <row r="116" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
@@ -12197,31 +12197,31 @@
     </row>
     <row r="132" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="133" spans="1:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="93" t="s">
+      <c r="A133" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="96" t="s">
+      <c r="B133" s="113" t="s">
         <v>87</v>
       </c>
-      <c r="C133" s="97"/>
-      <c r="D133" s="97"/>
-      <c r="E133" s="97"/>
-      <c r="F133" s="97"/>
-      <c r="G133" s="98"/>
-      <c r="I133" s="93" t="s">
+      <c r="C133" s="114"/>
+      <c r="D133" s="114"/>
+      <c r="E133" s="114"/>
+      <c r="F133" s="114"/>
+      <c r="G133" s="115"/>
+      <c r="I133" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="J133" s="96" t="s">
+      <c r="J133" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="K133" s="97"/>
-      <c r="L133" s="97"/>
-      <c r="M133" s="97"/>
-      <c r="N133" s="97"/>
-      <c r="O133" s="98"/>
+      <c r="K133" s="114"/>
+      <c r="L133" s="114"/>
+      <c r="M133" s="114"/>
+      <c r="N133" s="114"/>
+      <c r="O133" s="115"/>
     </row>
     <row r="134" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="94"/>
+      <c r="A134" s="111"/>
       <c r="B134" s="26" t="s">
         <v>71</v>
       </c>
@@ -12240,7 +12240,7 @@
       <c r="G134" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I134" s="94"/>
+      <c r="I134" s="111"/>
       <c r="J134" s="26" t="s">
         <v>71</v>
       </c>
@@ -12261,7 +12261,7 @@
       </c>
     </row>
     <row r="135" spans="1:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="95"/>
+      <c r="A135" s="112"/>
       <c r="B135" s="40" t="s">
         <v>63</v>
       </c>
@@ -12280,7 +12280,7 @@
       <c r="G135" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I135" s="95"/>
+      <c r="I135" s="112"/>
       <c r="J135" s="40" t="s">
         <v>63</v>
       </c>
@@ -13220,22 +13220,22 @@
       <c r="W160" s="37"/>
     </row>
     <row r="161" spans="1:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="112" t="s">
+      <c r="A161" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="B161" s="114" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="114"/>
-      <c r="D161" s="114"/>
-      <c r="E161" s="114" t="s">
+      <c r="B161" s="104" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="104"/>
+      <c r="D161" s="104"/>
+      <c r="E161" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="F161" s="114"/>
-      <c r="G161" s="114"/>
+      <c r="F161" s="104"/>
+      <c r="G161" s="104"/>
     </row>
     <row r="162" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="112"/>
+      <c r="A162" s="93"/>
       <c r="B162" s="64" t="s">
         <v>3</v>
       </c>
@@ -14031,9 +14031,9 @@
       <c r="AB185" s="20"/>
     </row>
     <row r="186" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="115"/>
-      <c r="B186" s="115"/>
-      <c r="C186" s="115"/>
+      <c r="A186" s="105"/>
+      <c r="B186" s="105"/>
+      <c r="C186" s="105"/>
       <c r="D186" s="20"/>
       <c r="E186" s="20"/>
       <c r="F186" s="20"/>
@@ -14208,39 +14208,39 @@
       <c r="W197" s="37"/>
     </row>
     <row r="198" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="104" t="s">
+      <c r="A198" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="B198" s="104"/>
-      <c r="C198" s="104"/>
-      <c r="D198" s="104"/>
-      <c r="E198" s="104"/>
-      <c r="F198" s="104"/>
+      <c r="B198" s="101"/>
+      <c r="C198" s="101"/>
+      <c r="D198" s="101"/>
+      <c r="E198" s="101"/>
+      <c r="F198" s="101"/>
     </row>
     <row r="199" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="116" t="s">
+      <c r="A199" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="B199" s="116"/>
-      <c r="C199" s="116"/>
-      <c r="D199" s="116"/>
-      <c r="E199" s="116"/>
-      <c r="F199" s="116"/>
+      <c r="B199" s="106"/>
+      <c r="C199" s="106"/>
+      <c r="D199" s="106"/>
+      <c r="E199" s="106"/>
+      <c r="F199" s="106"/>
     </row>
     <row r="200" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A200" s="99" t="s">
+      <c r="A200" s="107" t="s">
         <v>46</v>
       </c>
       <c r="B200" s="43"/>
       <c r="C200" s="43"/>
-      <c r="D200" s="99" t="s">
+      <c r="D200" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="E200" s="99"/>
-      <c r="F200" s="99"/>
+      <c r="E200" s="107"/>
+      <c r="F200" s="107"/>
     </row>
     <row r="201" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A201" s="99"/>
+      <c r="A201" s="107"/>
       <c r="B201" s="43"/>
       <c r="C201" s="44" t="s">
         <v>47</v>
@@ -14289,11 +14289,11 @@
       <c r="N202" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="O202" s="111" t="s">
+      <c r="O202" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="P202" s="111"/>
-      <c r="Q202" s="111"/>
+      <c r="P202" s="100"/>
+      <c r="Q202" s="100"/>
     </row>
     <row r="203" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="45" t="s">
@@ -15080,29 +15080,29 @@
       </c>
     </row>
     <row r="219" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="100" t="s">
+      <c r="A219" s="116" t="s">
         <v>75</v>
       </c>
-      <c r="B219" s="100"/>
-      <c r="C219" s="100"/>
-      <c r="D219" s="100"/>
-      <c r="E219" s="100"/>
-      <c r="F219" s="100"/>
+      <c r="B219" s="116"/>
+      <c r="C219" s="116"/>
+      <c r="D219" s="116"/>
+      <c r="E219" s="116"/>
+      <c r="F219" s="116"/>
     </row>
     <row r="220" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A220" s="113" t="s">
+      <c r="A220" s="103" t="s">
         <v>2</v>
       </c>
       <c r="B220" s="43"/>
       <c r="C220" s="43"/>
-      <c r="D220" s="99" t="s">
+      <c r="D220" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="E220" s="99"/>
-      <c r="F220" s="99"/>
+      <c r="E220" s="107"/>
+      <c r="F220" s="107"/>
     </row>
     <row r="221" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A221" s="113"/>
+      <c r="A221" s="103"/>
       <c r="B221" s="43"/>
       <c r="C221" s="44" t="s">
         <v>47</v>
@@ -15135,11 +15135,11 @@
       <c r="N222" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="O222" s="111" t="s">
+      <c r="O222" s="100" t="s">
         <v>94</v>
       </c>
-      <c r="P222" s="111"/>
-      <c r="Q222" s="111"/>
+      <c r="P222" s="100"/>
+      <c r="Q222" s="100"/>
     </row>
     <row r="223" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="45" t="s">
@@ -15733,27 +15733,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="V87:AC87"/>
-    <mergeCell ref="U87:U88"/>
-    <mergeCell ref="B81:I82"/>
-    <mergeCell ref="U82:U83"/>
-    <mergeCell ref="K81:K83"/>
-    <mergeCell ref="U81:AC81"/>
-    <mergeCell ref="L81:S82"/>
-    <mergeCell ref="V82:AC82"/>
-    <mergeCell ref="O222:Q222"/>
-    <mergeCell ref="O202:Q202"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A161:A162"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="E161:G161"/>
-    <mergeCell ref="A186:C186"/>
-    <mergeCell ref="A198:F198"/>
-    <mergeCell ref="A199:F199"/>
-    <mergeCell ref="D200:F200"/>
-    <mergeCell ref="D220:F220"/>
-    <mergeCell ref="A111:Q111"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="I133:I135"/>
     <mergeCell ref="J133:O133"/>
@@ -15770,6 +15749,27 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="I115:N115"/>
+    <mergeCell ref="O222:Q222"/>
+    <mergeCell ref="O202:Q202"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="E161:G161"/>
+    <mergeCell ref="A186:C186"/>
+    <mergeCell ref="A198:F198"/>
+    <mergeCell ref="A199:F199"/>
+    <mergeCell ref="D200:F200"/>
+    <mergeCell ref="D220:F220"/>
+    <mergeCell ref="A111:Q111"/>
+    <mergeCell ref="V87:AC87"/>
+    <mergeCell ref="U87:U88"/>
+    <mergeCell ref="B81:I82"/>
+    <mergeCell ref="U82:U83"/>
+    <mergeCell ref="K81:K83"/>
+    <mergeCell ref="U81:AC81"/>
+    <mergeCell ref="L81:S82"/>
+    <mergeCell ref="V82:AC82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update description of bkgrnd mortality data
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="607"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2625" windowHeight="2385" tabRatio="607"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -345,9 +345,6 @@
     <t>Statistical Release P0302 2019 Mid-year population estimates Table 5.3</t>
   </si>
   <si>
-    <t xml:space="preserve">UN World Population Prospects 2019, File MORT/17-2: Abridged life tables, for males/females, 1950-2100. </t>
-  </si>
-  <si>
     <t>Male Background Mortality</t>
   </si>
   <si>
@@ -471,9 +468,6 @@
     <t>1970-1975</t>
   </si>
   <si>
-    <t>Used values from 1950-1990 before the widespread HIV epidemic</t>
-  </si>
-  <si>
     <t>Initial Fertility Rate (per year) from Nick and Monisha</t>
   </si>
   <si>
@@ -499,6 +493,12 @@
       </rPr>
       <t xml:space="preserve"> Calculate backward-projected KZN population. Assume that KZN:SA proportion was decreasing from 1925-2002 according to same trend as from 2002-2019. Assume male and female populations by age follow exponential distributions. See Population_validation Excel document for more detail.</t>
     </r>
+  </si>
+  <si>
+    <t>UN World Population Prospects 2019, File MORT/17-2: Abridged life tables, for males/females, 1950-2100; GHDx GBD Results Tool</t>
+  </si>
+  <si>
+    <t>Used UN values from 1950-1990 before the widespread HIV epidemic. Used the GHDx GBD Results Tool to subtract HIV-specific mortality from all-cause mortality after 1990. Smoothed over the trough in the 1990s and made the decline in under 5 mortality a little less severe. Extrapolated the trend between 2000 and 2017 to 2020.</t>
   </si>
 </sst>
 </file>
@@ -1618,93 +1618,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1727,17 +1640,104 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -8221,8 +8221,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AI245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M79" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W103" sqref="W103"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L103" sqref="L103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8266,7 +8266,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -8294,16 +8294,16 @@
       <c r="Y1" s="37"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="117" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -8355,14 +8355,14 @@
       <c r="A4" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="102"/>
-      <c r="D4" s="101" t="s">
+      <c r="C4" s="110"/>
+      <c r="D4" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="102"/>
+      <c r="E4" s="110"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -8790,10 +8790,10 @@
       <c r="A27" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="101" t="s">
+      <c r="B27" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="102"/>
+      <c r="C27" s="110"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -9139,7 +9139,7 @@
     </row>
     <row r="50" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B50" s="37"/>
       <c r="C50" s="37"/>
@@ -9208,19 +9208,19 @@
       <c r="AE51" s="24"/>
     </row>
     <row r="52" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="103" t="s">
+      <c r="A52" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="103" t="s">
+      <c r="B52" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="103"/>
-      <c r="D52" s="103"/>
-      <c r="E52" s="103" t="s">
+      <c r="C52" s="128"/>
+      <c r="D52" s="128"/>
+      <c r="E52" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="F52" s="103"/>
-      <c r="G52" s="103"/>
+      <c r="F52" s="128"/>
+      <c r="G52" s="128"/>
       <c r="X52" s="22"/>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
@@ -9231,7 +9231,7 @@
       <c r="AE52" s="22"/>
     </row>
     <row r="53" spans="1:31" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="103"/>
+      <c r="A53" s="128"/>
       <c r="B53" s="33" t="s">
         <v>3</v>
       </c>
@@ -9710,7 +9710,7 @@
     </row>
     <row r="79" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="38" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="B79" s="37"/>
       <c r="C79" s="37"/>
@@ -9738,7 +9738,7 @@
     </row>
     <row r="80" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="36" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B80" s="37"/>
       <c r="C80" s="37"/>
@@ -9765,182 +9765,182 @@
       <c r="X80" s="37"/>
     </row>
     <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="104" t="s">
+      <c r="A81" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="109" t="s">
+      <c r="B81" s="104" t="s">
+        <v>80</v>
+      </c>
+      <c r="C81" s="104"/>
+      <c r="D81" s="104"/>
+      <c r="E81" s="104"/>
+      <c r="F81" s="104"/>
+      <c r="G81" s="104"/>
+      <c r="H81" s="104"/>
+      <c r="I81" s="104"/>
+      <c r="J81" s="104"/>
+      <c r="K81" s="104"/>
+      <c r="L81" s="104"/>
+      <c r="N81" s="101" t="s">
+        <v>2</v>
+      </c>
+      <c r="O81" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="C81" s="109"/>
-      <c r="D81" s="109"/>
-      <c r="E81" s="109"/>
-      <c r="F81" s="109"/>
-      <c r="G81" s="109"/>
-      <c r="H81" s="109"/>
-      <c r="I81" s="109"/>
-      <c r="J81" s="109"/>
-      <c r="K81" s="109"/>
-      <c r="L81" s="109"/>
-      <c r="N81" s="104" t="s">
+      <c r="P81" s="104"/>
+      <c r="Q81" s="104"/>
+      <c r="R81" s="104"/>
+      <c r="S81" s="104"/>
+      <c r="T81" s="104"/>
+      <c r="U81" s="104"/>
+      <c r="V81" s="104"/>
+      <c r="W81" s="104"/>
+      <c r="X81" s="104"/>
+      <c r="Y81" s="104"/>
+      <c r="AA81" s="105" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB81" s="106"/>
+      <c r="AC81" s="106"/>
+      <c r="AD81" s="106"/>
+      <c r="AE81" s="106"/>
+      <c r="AF81" s="106"/>
+      <c r="AG81" s="106"/>
+      <c r="AH81" s="106"/>
+      <c r="AI81" s="107"/>
+    </row>
+    <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="102"/>
+      <c r="B82" s="104"/>
+      <c r="C82" s="104"/>
+      <c r="D82" s="104"/>
+      <c r="E82" s="104"/>
+      <c r="F82" s="104"/>
+      <c r="G82" s="104"/>
+      <c r="H82" s="104"/>
+      <c r="I82" s="104"/>
+      <c r="J82" s="104"/>
+      <c r="K82" s="104"/>
+      <c r="L82" s="104"/>
+      <c r="N82" s="102"/>
+      <c r="O82" s="104"/>
+      <c r="P82" s="104"/>
+      <c r="Q82" s="104"/>
+      <c r="R82" s="104"/>
+      <c r="S82" s="104"/>
+      <c r="T82" s="104"/>
+      <c r="U82" s="104"/>
+      <c r="V82" s="104"/>
+      <c r="W82" s="104"/>
+      <c r="X82" s="104"/>
+      <c r="Y82" s="104"/>
+      <c r="AA82" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="O81" s="109" t="s">
-        <v>82</v>
-      </c>
-      <c r="P81" s="109"/>
-      <c r="Q81" s="109"/>
-      <c r="R81" s="109"/>
-      <c r="S81" s="109"/>
-      <c r="T81" s="109"/>
-      <c r="U81" s="109"/>
-      <c r="V81" s="109"/>
-      <c r="W81" s="109"/>
-      <c r="X81" s="109"/>
-      <c r="Y81" s="109"/>
-      <c r="AA81" s="115" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB81" s="116"/>
-      <c r="AC81" s="116"/>
-      <c r="AD81" s="116"/>
-      <c r="AE81" s="116"/>
-      <c r="AF81" s="116"/>
-      <c r="AG81" s="116"/>
-      <c r="AH81" s="116"/>
-      <c r="AI81" s="117"/>
-    </row>
-    <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="105"/>
-      <c r="B82" s="109"/>
-      <c r="C82" s="109"/>
-      <c r="D82" s="109"/>
-      <c r="E82" s="109"/>
-      <c r="F82" s="109"/>
-      <c r="G82" s="109"/>
-      <c r="H82" s="109"/>
-      <c r="I82" s="109"/>
-      <c r="J82" s="109"/>
-      <c r="K82" s="109"/>
-      <c r="L82" s="109"/>
-      <c r="N82" s="105"/>
-      <c r="O82" s="109"/>
-      <c r="P82" s="109"/>
-      <c r="Q82" s="109"/>
-      <c r="R82" s="109"/>
-      <c r="S82" s="109"/>
-      <c r="T82" s="109"/>
-      <c r="U82" s="109"/>
-      <c r="V82" s="109"/>
-      <c r="W82" s="109"/>
-      <c r="X82" s="109"/>
-      <c r="Y82" s="109"/>
-      <c r="AA82" s="126" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB82" s="115" t="s">
+      <c r="AB82" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="AC82" s="116"/>
-      <c r="AD82" s="116"/>
-      <c r="AE82" s="116"/>
-      <c r="AF82" s="116"/>
-      <c r="AG82" s="116"/>
-      <c r="AH82" s="116"/>
-      <c r="AI82" s="117"/>
+      <c r="AC82" s="106"/>
+      <c r="AD82" s="106"/>
+      <c r="AE82" s="106"/>
+      <c r="AF82" s="106"/>
+      <c r="AG82" s="106"/>
+      <c r="AH82" s="106"/>
+      <c r="AI82" s="107"/>
     </row>
     <row r="83" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="106"/>
+      <c r="A83" s="103"/>
       <c r="B83" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="C83" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="C83" s="76" t="s">
+      <c r="D83" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="D83" s="76" t="s">
+      <c r="E83" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="E83" s="76" t="s">
+      <c r="F83" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="G83" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="F83" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="G83" s="76" t="s">
+      <c r="H83" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="I83" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="H83" s="76" t="s">
+      <c r="J83" s="93">
+        <v>2000</v>
+      </c>
+      <c r="K83" s="94">
+        <v>2017</v>
+      </c>
+      <c r="L83" s="89">
+        <v>2020</v>
+      </c>
+      <c r="N83" s="103"/>
+      <c r="O83" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="P83" s="76" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q83" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="R83" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="S83" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="I83" s="76" t="s">
+      <c r="T83" s="76" t="s">
+        <v>99</v>
+      </c>
+      <c r="U83" s="76" t="s">
         <v>101</v>
       </c>
-      <c r="J83" s="122">
+      <c r="V83" s="76" t="s">
+        <v>100</v>
+      </c>
+      <c r="W83" s="93">
         <v>2000</v>
       </c>
-      <c r="K83" s="123">
+      <c r="X83" s="94">
         <v>2017</v>
       </c>
-      <c r="L83" s="118">
+      <c r="Y83" s="89">
         <v>2020</v>
       </c>
-      <c r="N83" s="106"/>
-      <c r="O83" s="76" t="s">
+      <c r="AA83" s="100"/>
+      <c r="AB83" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC83" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="P83" s="76" t="s">
+      <c r="AD83" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="Q83" s="76" t="s">
+      <c r="AE83" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="R83" s="76" t="s">
+      <c r="AF83" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG83" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="S83" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="T83" s="76" t="s">
+      <c r="AH83" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI83" s="76" t="s">
         <v>100</v>
-      </c>
-      <c r="U83" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="V83" s="76" t="s">
-        <v>101</v>
-      </c>
-      <c r="W83" s="122">
-        <v>2000</v>
-      </c>
-      <c r="X83" s="123">
-        <v>2017</v>
-      </c>
-      <c r="Y83" s="118">
-        <v>2020</v>
-      </c>
-      <c r="AA83" s="127"/>
-      <c r="AB83" s="76" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC83" s="76" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD83" s="76" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE83" s="76" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF83" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="AG83" s="76" t="s">
-        <v>100</v>
-      </c>
-      <c r="AH83" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI83" s="76" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="84" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
@@ -9948,44 +9948,44 @@
         <v>6</v>
       </c>
       <c r="B84" s="79">
-        <f>SUM(AB84:AB85)</f>
+        <f t="shared" ref="B84:I84" si="7">SUM(AB84:AB85)</f>
         <v>0.19005920400000001</v>
       </c>
       <c r="C84" s="78">
-        <f>SUM(AC84:AC85)</f>
+        <f t="shared" si="7"/>
         <v>0.16702423499999999</v>
       </c>
       <c r="D84" s="78">
-        <f>SUM(AD84:AD85)</f>
+        <f t="shared" si="7"/>
         <v>0.15232399099999999</v>
       </c>
       <c r="E84" s="78">
-        <f>SUM(AE84:AE85)</f>
+        <f t="shared" si="7"/>
         <v>0.137224824</v>
       </c>
       <c r="F84" s="78">
-        <f>SUM(AF84:AF85)</f>
+        <f t="shared" si="7"/>
         <v>0.115676261</v>
       </c>
       <c r="G84" s="78">
-        <f>SUM(AG84:AG85)</f>
+        <f t="shared" si="7"/>
         <v>9.0002309699999991E-2</v>
       </c>
       <c r="H84" s="78">
-        <f>SUM(AH84:AH85)</f>
+        <f t="shared" si="7"/>
         <v>7.0407469099999995E-2</v>
       </c>
-      <c r="I84" s="119">
-        <f>SUM(AI84:AI85)</f>
+      <c r="I84" s="90">
+        <f t="shared" si="7"/>
         <v>5.6975585300000006E-2</v>
       </c>
-      <c r="J84" s="128">
+      <c r="J84" s="97">
         <v>1.2464773E-2</v>
       </c>
-      <c r="K84" s="124">
+      <c r="K84" s="95">
         <v>5.892614E-3</v>
       </c>
-      <c r="L84" s="121">
+      <c r="L84" s="92">
         <f>K84+($L$83-$K$83)*M84</f>
         <v>4.7328212352941174E-3</v>
       </c>
@@ -9997,44 +9997,44 @@
         <v>6</v>
       </c>
       <c r="O84" s="79">
-        <f>SUM(AB89:AB90)</f>
+        <f t="shared" ref="O84:V84" si="8">SUM(AB89:AB90)</f>
         <v>0.16283755500000002</v>
       </c>
       <c r="P84" s="78">
-        <f>SUM(AC89:AC90)</f>
+        <f t="shared" si="8"/>
         <v>0.143554814</v>
       </c>
       <c r="Q84" s="78">
-        <f>SUM(AD89:AD90)</f>
+        <f t="shared" si="8"/>
         <v>0.131042716</v>
       </c>
       <c r="R84" s="78">
-        <f>SUM(AE89:AE90)</f>
+        <f t="shared" si="8"/>
         <v>0.11815073600000001</v>
       </c>
       <c r="S84" s="78">
-        <f>SUM(AF89:AF90)</f>
+        <f t="shared" si="8"/>
         <v>9.9835274000000002E-2</v>
       </c>
       <c r="T84" s="78">
-        <f>SUM(AG89:AG90)</f>
+        <f t="shared" si="8"/>
         <v>7.7719069000000002E-2</v>
       </c>
       <c r="U84" s="78">
-        <f>SUM(AH89:AH90)</f>
+        <f t="shared" si="8"/>
         <v>5.96665085E-2</v>
       </c>
-      <c r="V84" s="119">
-        <f>SUM(AI89:AI90)</f>
+      <c r="V84" s="90">
+        <f t="shared" si="8"/>
         <v>4.7441704699999997E-2</v>
       </c>
-      <c r="W84" s="128">
+      <c r="W84" s="97">
         <v>1.0375972000000001E-2</v>
       </c>
-      <c r="X84" s="124">
+      <c r="X84" s="95">
         <v>4.9718649999999998E-3</v>
       </c>
-      <c r="Y84" s="121">
+      <c r="Y84" s="92">
         <f>X84+($Y$83-$X$83)*Z84</f>
         <v>4.0181990588235295E-3</v>
       </c>
@@ -10095,21 +10095,21 @@
       <c r="H85" s="81">
         <v>3.0634688E-3</v>
       </c>
-      <c r="I85" s="120">
+      <c r="I85" s="91">
         <v>2.4750038999999998E-3</v>
       </c>
-      <c r="J85" s="128">
+      <c r="J85" s="97">
         <v>1.2523619999999999E-3</v>
       </c>
-      <c r="K85" s="125">
+      <c r="K85" s="96">
         <v>4.3800000000000002E-4</v>
       </c>
-      <c r="L85" s="121">
-        <f t="shared" ref="L85:L99" si="7">K85+($L$83-$K$83)*M85</f>
+      <c r="L85" s="92">
+        <f t="shared" ref="L85:L99" si="9">K85+($L$83-$K$83)*M85</f>
         <v>2.9428905882352948E-4</v>
       </c>
       <c r="M85">
-        <f t="shared" ref="M85:M99" si="8">(K85-J85)/($K$83-$J$83)</f>
+        <f t="shared" ref="M85:M99" si="10">(K85-J85)/($K$83-$J$83)</f>
         <v>-4.7903647058823526E-5</v>
       </c>
       <c r="N85" s="88" t="s">
@@ -10136,25 +10136,25 @@
       <c r="U85" s="81">
         <v>2.3506893000000001E-3</v>
       </c>
-      <c r="V85" s="120">
+      <c r="V85" s="91">
         <v>1.8590649E-3</v>
       </c>
-      <c r="W85" s="129">
+      <c r="W85" s="98">
         <v>9.1699999999999995E-4</v>
       </c>
-      <c r="X85" s="125">
+      <c r="X85" s="96">
         <v>3.0899999999999998E-4</v>
       </c>
-      <c r="Y85" s="121">
-        <f t="shared" ref="Y85:Y99" si="9">X85+($Y$83-$X$83)*Z85</f>
+      <c r="Y85" s="92">
+        <f t="shared" ref="Y85:Y99" si="11">X85+($Y$83-$X$83)*Z85</f>
         <v>2.0170588235294114E-4</v>
       </c>
       <c r="Z85">
-        <f t="shared" ref="Z85:Z99" si="10">(X85-W85)/($X$83-$W$83)</f>
+        <f t="shared" ref="Z85:Z99" si="12">(X85-W85)/($X$83-$W$83)</f>
         <v>-3.5764705882352941E-5</v>
       </c>
       <c r="AA85" s="83" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AB85" s="81">
         <v>3.0801934E-2</v>
@@ -10206,21 +10206,21 @@
       <c r="H86" s="81">
         <v>1.9361118E-3</v>
       </c>
-      <c r="I86" s="120">
+      <c r="I86" s="91">
         <v>1.5814690000000001E-3</v>
       </c>
-      <c r="J86" s="129">
+      <c r="J86" s="98">
         <v>9.77E-4</v>
       </c>
-      <c r="K86" s="125">
+      <c r="K86" s="96">
         <v>2.7099999999999997E-4</v>
       </c>
-      <c r="L86" s="121">
-        <f t="shared" si="7"/>
+      <c r="L86" s="92">
+        <f t="shared" si="9"/>
         <v>1.4641176470588232E-4</v>
       </c>
       <c r="M86">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-4.1529411764705884E-5</v>
       </c>
       <c r="N86" s="88" t="s">
@@ -10247,21 +10247,21 @@
       <c r="U86" s="81">
         <v>1.5421367E-3</v>
       </c>
-      <c r="V86" s="120">
+      <c r="V86" s="91">
         <v>1.2227608999999999E-3</v>
       </c>
-      <c r="W86" s="129">
+      <c r="W86" s="98">
         <v>7.4100000000000001E-4</v>
       </c>
-      <c r="X86" s="125">
+      <c r="X86" s="96">
         <v>1.65E-4</v>
       </c>
-      <c r="Y86" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y86" s="92">
+        <f t="shared" si="11"/>
         <v>6.335294117647058E-5</v>
       </c>
       <c r="Z86">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-3.3882352941176473E-5</v>
       </c>
       <c r="AA86" s="35"/>
@@ -10299,21 +10299,21 @@
       <c r="H87" s="81">
         <v>2.9596564999999999E-3</v>
       </c>
-      <c r="I87" s="120">
+      <c r="I87" s="91">
         <v>2.5001934000000001E-3</v>
       </c>
-      <c r="J87" s="128">
+      <c r="J87" s="97">
         <v>2.1267130000000001E-3</v>
       </c>
-      <c r="K87" s="125">
+      <c r="K87" s="96">
         <v>6.4599999999999998E-4</v>
       </c>
-      <c r="L87" s="121">
-        <f t="shared" si="7"/>
+      <c r="L87" s="92">
+        <f t="shared" si="9"/>
         <v>3.8469770588235287E-4</v>
       </c>
       <c r="M87">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-8.7100764705882374E-5</v>
       </c>
       <c r="N87" s="88" t="s">
@@ -10340,36 +10340,36 @@
       <c r="U87" s="81">
         <v>2.0807315999999999E-3</v>
       </c>
-      <c r="V87" s="120">
+      <c r="V87" s="91">
         <v>1.6750273E-3</v>
       </c>
-      <c r="W87" s="128">
+      <c r="W87" s="97">
         <v>1.469932E-3</v>
       </c>
-      <c r="X87" s="125">
+      <c r="X87" s="96">
         <v>3.9800000000000002E-4</v>
       </c>
-      <c r="Y87" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y87" s="92">
+        <f t="shared" si="11"/>
         <v>2.0883552941176474E-4</v>
       </c>
       <c r="Z87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-6.3054823529411761E-5</v>
       </c>
-      <c r="AA87" s="126" t="s">
+      <c r="AA87" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="AB87" s="115" t="s">
+      <c r="AB87" s="105" t="s">
         <v>75</v>
       </c>
-      <c r="AC87" s="116"/>
-      <c r="AD87" s="116"/>
-      <c r="AE87" s="116"/>
-      <c r="AF87" s="116"/>
-      <c r="AG87" s="116"/>
-      <c r="AH87" s="116"/>
-      <c r="AI87" s="117"/>
+      <c r="AC87" s="106"/>
+      <c r="AD87" s="106"/>
+      <c r="AE87" s="106"/>
+      <c r="AF87" s="106"/>
+      <c r="AG87" s="106"/>
+      <c r="AH87" s="106"/>
+      <c r="AI87" s="107"/>
     </row>
     <row r="88" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="74" t="s">
@@ -10396,21 +10396,21 @@
       <c r="H88" s="81">
         <v>4.4258235999999999E-3</v>
       </c>
-      <c r="I88" s="120">
+      <c r="I88" s="91">
         <v>3.7640993E-3</v>
       </c>
-      <c r="J88" s="128">
+      <c r="J88" s="97">
         <v>3.647225E-3</v>
       </c>
-      <c r="K88" s="124">
+      <c r="K88" s="95">
         <v>2.068032E-3</v>
       </c>
-      <c r="L88" s="121">
-        <f t="shared" si="7"/>
+      <c r="L88" s="92">
+        <f t="shared" si="9"/>
         <v>1.7893508823529412E-3</v>
       </c>
       <c r="M88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-9.2893705882352942E-5</v>
       </c>
       <c r="N88" s="88" t="s">
@@ -10437,47 +10437,47 @@
       <c r="U88" s="81">
         <v>2.9634518E-3</v>
       </c>
-      <c r="V88" s="120">
+      <c r="V88" s="91">
         <v>2.3815536E-3</v>
       </c>
-      <c r="W88" s="128">
+      <c r="W88" s="97">
         <v>3.4466029999999999E-3</v>
       </c>
-      <c r="X88" s="124">
+      <c r="X88" s="95">
         <v>1.022128E-3</v>
       </c>
-      <c r="Y88" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y88" s="92">
+        <f t="shared" si="11"/>
         <v>5.9427947058823534E-4</v>
       </c>
       <c r="Z88">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-1.4261617647058823E-4</v>
       </c>
-      <c r="AA88" s="127"/>
+      <c r="AA88" s="100"/>
       <c r="AB88" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC88" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="AC88" s="76" t="s">
+      <c r="AD88" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="AD88" s="76" t="s">
+      <c r="AE88" s="76" t="s">
         <v>98</v>
       </c>
-      <c r="AE88" s="76" t="s">
+      <c r="AF88" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG88" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="AF88" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="AG88" s="76" t="s">
+      <c r="AH88" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI88" s="76" t="s">
         <v>100</v>
-      </c>
-      <c r="AH88" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI88" s="76" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
@@ -10505,21 +10505,21 @@
       <c r="H89" s="81">
         <v>5.1091371999999998E-3</v>
       </c>
-      <c r="I89" s="120">
+      <c r="I89" s="91">
         <v>4.3315932999999996E-3</v>
       </c>
-      <c r="J89" s="128">
+      <c r="J89" s="97">
         <v>5.7620409999999999E-3</v>
       </c>
-      <c r="K89" s="124">
+      <c r="K89" s="95">
         <v>2.644057E-3</v>
       </c>
-      <c r="L89" s="121">
-        <f t="shared" si="7"/>
+      <c r="L89" s="92">
+        <f t="shared" si="9"/>
         <v>2.0938245294117646E-3</v>
       </c>
       <c r="M89">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-1.8341082352941175E-4</v>
       </c>
       <c r="N89" s="88" t="s">
@@ -10546,21 +10546,21 @@
       <c r="U89" s="81">
         <v>3.9385823E-3</v>
       </c>
-      <c r="V89" s="120">
+      <c r="V89" s="91">
         <v>3.1198295999999999E-3</v>
       </c>
-      <c r="W89" s="128">
+      <c r="W89" s="97">
         <v>5.689525E-3</v>
       </c>
-      <c r="X89" s="124">
+      <c r="X89" s="95">
         <v>1.4837839999999999E-3</v>
       </c>
-      <c r="Y89" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y89" s="92">
+        <f t="shared" si="11"/>
         <v>7.4159441176470582E-4</v>
       </c>
       <c r="Z89">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-2.4739652941176469E-4</v>
       </c>
       <c r="AA89" s="80">
@@ -10616,21 +10616,21 @@
       <c r="H90" s="81">
         <v>6.0814568000000001E-3</v>
       </c>
-      <c r="I90" s="120">
+      <c r="I90" s="91">
         <v>5.1669517000000002E-3</v>
       </c>
-      <c r="J90" s="128">
+      <c r="J90" s="97">
         <v>8.5842190000000006E-3</v>
       </c>
-      <c r="K90" s="124">
+      <c r="K90" s="95">
         <v>3.4039669999999999E-3</v>
       </c>
-      <c r="L90" s="121">
-        <f t="shared" si="7"/>
+      <c r="L90" s="92">
+        <f t="shared" si="9"/>
         <v>2.4898048823529411E-3</v>
       </c>
       <c r="M90">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-3.0472070588235297E-4</v>
       </c>
       <c r="N90" s="88" t="s">
@@ -10657,25 +10657,25 @@
       <c r="U90" s="81">
         <v>4.7939851999999998E-3</v>
       </c>
-      <c r="V90" s="120">
+      <c r="V90" s="91">
         <v>3.7817176000000002E-3</v>
       </c>
-      <c r="W90" s="128">
+      <c r="W90" s="97">
         <v>6.367841E-3</v>
       </c>
-      <c r="X90" s="124">
+      <c r="X90" s="95">
         <v>1.8290649999999999E-3</v>
       </c>
-      <c r="Y90" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y90" s="92">
+        <f t="shared" si="11"/>
         <v>1.0281045294117646E-3</v>
       </c>
       <c r="Z90">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-2.6698682352941175E-4</v>
       </c>
       <c r="AA90" s="83" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AB90" s="81">
         <v>2.7320634999999999E-2</v>
@@ -10727,21 +10727,21 @@
       <c r="H91" s="81">
         <v>7.5515045999999999E-3</v>
       </c>
-      <c r="I91" s="120">
+      <c r="I91" s="91">
         <v>6.4414638999999996E-3</v>
       </c>
-      <c r="J91" s="128">
+      <c r="J91" s="97">
         <v>1.0363597E-2</v>
       </c>
-      <c r="K91" s="124">
+      <c r="K91" s="95">
         <v>3.9863540000000001E-3</v>
       </c>
-      <c r="L91" s="121">
-        <f t="shared" si="7"/>
+      <c r="L91" s="92">
+        <f t="shared" si="9"/>
         <v>2.8609581764705884E-3</v>
       </c>
       <c r="M91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-3.7513194117647059E-4</v>
       </c>
       <c r="N91" s="88" t="s">
@@ -10768,21 +10768,21 @@
       <c r="U91" s="81">
         <v>5.8713664000000004E-3</v>
       </c>
-      <c r="V91" s="120">
+      <c r="V91" s="91">
         <v>4.6448573999999998E-3</v>
       </c>
-      <c r="W91" s="128">
+      <c r="W91" s="97">
         <v>6.1407370000000003E-3</v>
       </c>
-      <c r="X91" s="124">
+      <c r="X91" s="95">
         <v>1.8174109999999999E-3</v>
       </c>
-      <c r="Y91" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y91" s="92">
+        <f t="shared" si="11"/>
         <v>1.0544711176470585E-3</v>
       </c>
       <c r="Z91">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-2.5431329411764711E-4</v>
       </c>
     </row>
@@ -10811,21 +10811,21 @@
       <c r="H92" s="81">
         <v>9.3492987999999992E-3</v>
       </c>
-      <c r="I92" s="120">
+      <c r="I92" s="91">
         <v>8.0432449999999992E-3</v>
       </c>
-      <c r="J92" s="128">
+      <c r="J92" s="97">
         <v>1.1498424E-2</v>
       </c>
-      <c r="K92" s="124">
+      <c r="K92" s="95">
         <v>4.6618329999999998E-3</v>
       </c>
-      <c r="L92" s="121">
-        <f t="shared" si="7"/>
+      <c r="L92" s="92">
+        <f t="shared" si="9"/>
         <v>3.4553757647058821E-3</v>
       </c>
       <c r="M92">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-4.021524117647059E-4</v>
       </c>
       <c r="N92" s="88" t="s">
@@ -10852,21 +10852,21 @@
       <c r="U92" s="81">
         <v>7.0247197000000003E-3</v>
       </c>
-      <c r="V92" s="120">
+      <c r="V92" s="91">
         <v>5.6773359000000002E-3</v>
       </c>
-      <c r="W92" s="128">
+      <c r="W92" s="97">
         <v>5.9637040000000002E-3</v>
       </c>
-      <c r="X92" s="124">
+      <c r="X92" s="95">
         <v>2.1249369999999999E-3</v>
       </c>
-      <c r="Y92" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y92" s="92">
+        <f t="shared" si="11"/>
         <v>1.4475075294117646E-3</v>
       </c>
       <c r="Z92">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-2.2580982352941178E-4</v>
       </c>
     </row>
@@ -10895,21 +10895,21 @@
       <c r="H93" s="81">
         <v>1.1624491000000001E-2</v>
       </c>
-      <c r="I93" s="120">
+      <c r="I93" s="91">
         <v>1.0135829000000001E-2</v>
       </c>
-      <c r="J93" s="128">
+      <c r="J93" s="97">
         <v>1.4937591E-2</v>
       </c>
-      <c r="K93" s="124">
+      <c r="K93" s="95">
         <v>6.616434E-3</v>
       </c>
-      <c r="L93" s="121">
-        <f t="shared" si="7"/>
+      <c r="L93" s="92">
+        <f t="shared" si="9"/>
         <v>5.1479945294117648E-3</v>
       </c>
       <c r="M93">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-4.8947982352941168E-4</v>
       </c>
       <c r="N93" s="88" t="s">
@@ -10936,21 +10936,21 @@
       <c r="U93" s="81">
         <v>8.1201847999999993E-3</v>
       </c>
-      <c r="V93" s="120">
+      <c r="V93" s="91">
         <v>6.6691631000000001E-3</v>
       </c>
-      <c r="W93" s="128">
+      <c r="W93" s="97">
         <v>6.78533E-3</v>
       </c>
-      <c r="X93" s="124">
+      <c r="X93" s="95">
         <v>3.1711669999999999E-3</v>
       </c>
-      <c r="Y93" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y93" s="92">
+        <f t="shared" si="11"/>
         <v>2.5333735294117646E-3</v>
       </c>
       <c r="Z93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-2.1259782352941176E-4</v>
       </c>
     </row>
@@ -10979,21 +10979,21 @@
       <c r="H94" s="81">
         <v>1.5751589999999999E-2</v>
       </c>
-      <c r="I94" s="120">
+      <c r="I94" s="91">
         <v>1.4004198000000001E-2</v>
       </c>
-      <c r="J94" s="128">
+      <c r="J94" s="97">
         <v>2.0927292E-2</v>
       </c>
-      <c r="K94" s="124">
+      <c r="K94" s="95">
         <v>1.0831970999999999E-2</v>
       </c>
-      <c r="L94" s="121">
-        <f t="shared" si="7"/>
+      <c r="L94" s="92">
+        <f t="shared" si="9"/>
         <v>9.050443764705882E-3</v>
       </c>
       <c r="M94">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-5.9384241176470591E-4</v>
       </c>
       <c r="N94" s="88" t="s">
@@ -11020,21 +11020,21 @@
       <c r="U94" s="81">
         <v>1.0674833E-2</v>
       </c>
-      <c r="V94" s="120">
+      <c r="V94" s="91">
         <v>8.9763412999999993E-3</v>
       </c>
-      <c r="W94" s="128">
+      <c r="W94" s="97">
         <v>9.8414439999999995E-3</v>
       </c>
-      <c r="X94" s="124">
+      <c r="X94" s="95">
         <v>5.1947219999999997E-3</v>
       </c>
-      <c r="Y94" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y94" s="92">
+        <f t="shared" si="11"/>
         <v>4.3747122352941169E-3</v>
       </c>
       <c r="Z94">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-2.7333658823529413E-4</v>
       </c>
     </row>
@@ -11063,21 +11063,21 @@
       <c r="H95" s="81">
         <v>2.0631349E-2</v>
       </c>
-      <c r="I95" s="120">
+      <c r="I95" s="91">
         <v>1.8576009000000001E-2</v>
       </c>
-      <c r="J95" s="128">
+      <c r="J95" s="97">
         <v>2.6352477999999999E-2</v>
       </c>
-      <c r="K95" s="124">
+      <c r="K95" s="95">
         <v>1.6475909E-2</v>
       </c>
-      <c r="L95" s="121">
-        <f t="shared" si="7"/>
+      <c r="L95" s="92">
+        <f t="shared" si="9"/>
         <v>1.473298505882353E-2</v>
       </c>
       <c r="M95">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-5.8097464705882346E-4</v>
       </c>
       <c r="N95" s="88" t="s">
@@ -11104,21 +11104,21 @@
       <c r="U95" s="81">
         <v>1.4094534000000001E-2</v>
       </c>
-      <c r="V95" s="120">
+      <c r="V95" s="91">
         <v>1.2049147E-2</v>
       </c>
-      <c r="W95" s="128">
+      <c r="W95" s="97">
         <v>1.3256046E-2</v>
       </c>
-      <c r="X95" s="124">
+      <c r="X95" s="95">
         <v>8.2955149999999998E-3</v>
       </c>
-      <c r="Y95" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y95" s="92">
+        <f t="shared" si="11"/>
         <v>7.4201271764705885E-3</v>
       </c>
       <c r="Z95">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-2.917959411764706E-4</v>
       </c>
     </row>
@@ -11147,21 +11147,21 @@
       <c r="H96" s="81">
         <v>3.0365044000000001E-2</v>
       </c>
-      <c r="I96" s="120">
+      <c r="I96" s="91">
         <v>2.7759598999999999E-2</v>
       </c>
-      <c r="J96" s="128">
+      <c r="J96" s="97">
         <v>3.6052813000000003E-2</v>
       </c>
-      <c r="K96" s="124">
+      <c r="K96" s="95">
         <v>2.3964659999999999E-2</v>
       </c>
-      <c r="L96" s="121">
-        <f t="shared" si="7"/>
+      <c r="L96" s="92">
+        <f t="shared" si="9"/>
         <v>2.1831456529411764E-2</v>
       </c>
       <c r="M96">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-7.11067823529412E-4</v>
       </c>
       <c r="N96" s="84" t="s">
@@ -11188,21 +11188,21 @@
       <c r="U96" s="81">
         <v>2.1257570999999999E-2</v>
       </c>
-      <c r="V96" s="120">
+      <c r="V96" s="91">
         <v>1.8543285E-2</v>
       </c>
-      <c r="W96" s="128">
+      <c r="W96" s="97">
         <v>1.9917550999999999E-2</v>
       </c>
-      <c r="X96" s="124">
+      <c r="X96" s="95">
         <v>1.2142778999999999E-2</v>
       </c>
-      <c r="Y96" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y96" s="92">
+        <f t="shared" si="11"/>
         <v>1.0770760411764705E-2</v>
       </c>
       <c r="Z96">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-4.5733952941176466E-4</v>
       </c>
     </row>
@@ -11231,21 +11231,21 @@
       <c r="H97" s="81">
         <v>4.6165507000000001E-2</v>
       </c>
-      <c r="I97" s="120">
+      <c r="I97" s="91">
         <v>4.2779603999999999E-2</v>
       </c>
-      <c r="J97" s="128">
+      <c r="J97" s="97">
         <v>4.4857968999999998E-2</v>
       </c>
-      <c r="K97" s="124">
+      <c r="K97" s="95">
         <v>3.3032178000000002E-2</v>
       </c>
-      <c r="L97" s="121">
-        <f t="shared" si="7"/>
+      <c r="L97" s="92">
+        <f t="shared" si="9"/>
         <v>3.0945273705882355E-2</v>
       </c>
       <c r="M97">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-6.9563476470588205E-4</v>
       </c>
       <c r="N97" s="84" t="s">
@@ -11272,21 +11272,21 @@
       <c r="U97" s="81">
         <v>3.4126276999999997E-2</v>
       </c>
-      <c r="V97" s="120">
+      <c r="V97" s="91">
         <v>3.039122E-2</v>
       </c>
-      <c r="W97" s="128">
+      <c r="W97" s="97">
         <v>2.8481023000000001E-2</v>
       </c>
-      <c r="X97" s="124">
+      <c r="X97" s="95">
         <v>1.7584465000000001E-2</v>
       </c>
-      <c r="Y97" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y97" s="92">
+        <f t="shared" si="11"/>
         <v>1.5661543E-2</v>
       </c>
       <c r="Z97">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-6.4097399999999999E-4</v>
       </c>
     </row>
@@ -11315,21 +11315,21 @@
       <c r="H98" s="81">
         <v>7.3117043000000007E-2</v>
       </c>
-      <c r="I98" s="120">
+      <c r="I98" s="91">
         <v>6.8473476000000005E-2</v>
       </c>
-      <c r="J98" s="128">
+      <c r="J98" s="97">
         <v>6.6115557000000005E-2</v>
       </c>
-      <c r="K98" s="124">
+      <c r="K98" s="95">
         <v>4.3224483000000001E-2</v>
       </c>
-      <c r="L98" s="121">
-        <f t="shared" si="7"/>
+      <c r="L98" s="92">
+        <f t="shared" si="9"/>
         <v>3.918488170588235E-2</v>
       </c>
       <c r="M98">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-1.3465337647058826E-3</v>
       </c>
       <c r="N98" s="84" t="s">
@@ -11356,21 +11356,21 @@
       <c r="U98" s="81">
         <v>5.7037298E-2</v>
       </c>
-      <c r="V98" s="120">
+      <c r="V98" s="91">
         <v>5.1704121999999998E-2</v>
       </c>
-      <c r="W98" s="128">
+      <c r="W98" s="97">
         <v>4.3469642000000003E-2</v>
       </c>
-      <c r="X98" s="124">
+      <c r="X98" s="95">
         <v>2.5406643E-2</v>
       </c>
-      <c r="Y98" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y98" s="92">
+        <f t="shared" si="11"/>
         <v>2.2219054941176469E-2</v>
       </c>
       <c r="Z98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-1.0625293529411767E-3</v>
       </c>
     </row>
@@ -11399,21 +11399,21 @@
       <c r="H99" s="81">
         <v>0.11823134</v>
       </c>
-      <c r="I99" s="120">
+      <c r="I99" s="91">
         <v>0.11201527999999999</v>
       </c>
-      <c r="J99" s="128">
+      <c r="J99" s="97">
         <v>8.1959559000000001E-2</v>
       </c>
-      <c r="K99" s="124">
+      <c r="K99" s="95">
         <v>5.9431375000000002E-2</v>
       </c>
-      <c r="L99" s="121">
-        <f t="shared" si="7"/>
+      <c r="L99" s="92">
+        <f t="shared" si="9"/>
         <v>5.5455813117647058E-2</v>
       </c>
       <c r="M99">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-1.3251872941176471E-3</v>
       </c>
       <c r="N99" s="84" t="s">
@@ -11440,21 +11440,21 @@
       <c r="U99" s="81">
         <v>9.5537514000000004E-2</v>
       </c>
-      <c r="V99" s="120">
+      <c r="V99" s="91">
         <v>8.8066895000000006E-2</v>
       </c>
-      <c r="W99" s="128">
+      <c r="W99" s="97">
         <v>5.4374656E-2</v>
       </c>
-      <c r="X99" s="124">
+      <c r="X99" s="95">
         <v>3.7231258000000003E-2</v>
       </c>
-      <c r="Y99" s="121">
-        <f t="shared" si="9"/>
+      <c r="Y99" s="92">
+        <f t="shared" si="11"/>
         <v>3.420595247058824E-2</v>
       </c>
       <c r="Z99">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-1.0084351764705882E-3</v>
       </c>
     </row>
@@ -11560,7 +11560,7 @@
     </row>
     <row r="108" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B108" s="37"/>
       <c r="C108" s="37"/>
@@ -11588,7 +11588,7 @@
     </row>
     <row r="109" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B109" s="37"/>
       <c r="C109" s="37"/>
@@ -11616,7 +11616,7 @@
     </row>
     <row r="110" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B110" s="37"/>
       <c r="C110" s="37"/>
@@ -11643,25 +11643,25 @@
       <c r="X110" s="37"/>
     </row>
     <row r="111" spans="1:26" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="114" t="s">
-        <v>106</v>
-      </c>
-      <c r="B111" s="114"/>
-      <c r="C111" s="114"/>
-      <c r="D111" s="114"/>
-      <c r="E111" s="114"/>
-      <c r="F111" s="114"/>
-      <c r="G111" s="114"/>
-      <c r="H111" s="114"/>
-      <c r="I111" s="114"/>
-      <c r="J111" s="114"/>
-      <c r="K111" s="114"/>
-      <c r="L111" s="114"/>
-      <c r="M111" s="114"/>
-      <c r="N111" s="114"/>
-      <c r="O111" s="114"/>
-      <c r="P111" s="114"/>
-      <c r="Q111" s="114"/>
+      <c r="A111" s="116" t="s">
+        <v>104</v>
+      </c>
+      <c r="B111" s="116"/>
+      <c r="C111" s="116"/>
+      <c r="D111" s="116"/>
+      <c r="E111" s="116"/>
+      <c r="F111" s="116"/>
+      <c r="G111" s="116"/>
+      <c r="H111" s="116"/>
+      <c r="I111" s="116"/>
+      <c r="J111" s="116"/>
+      <c r="K111" s="116"/>
+      <c r="L111" s="116"/>
+      <c r="M111" s="116"/>
+      <c r="N111" s="116"/>
+      <c r="O111" s="116"/>
+      <c r="P111" s="116"/>
+      <c r="Q111" s="116"/>
       <c r="R111" s="37"/>
       <c r="S111" s="37"/>
       <c r="T111" s="37"/>
@@ -11671,17 +11671,17 @@
       <c r="X111" s="37"/>
     </row>
     <row r="112" spans="1:26" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="98" t="s">
+      <c r="A112" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="93" t="s">
-        <v>86</v>
-      </c>
-      <c r="C112" s="94"/>
-      <c r="D112" s="94"/>
-      <c r="E112" s="94"/>
-      <c r="F112" s="94"/>
-      <c r="G112" s="95"/>
+      <c r="B112" s="121" t="s">
+        <v>85</v>
+      </c>
+      <c r="C112" s="122"/>
+      <c r="D112" s="122"/>
+      <c r="E112" s="122"/>
+      <c r="F112" s="122"/>
+      <c r="G112" s="123"/>
       <c r="I112" s="73"/>
       <c r="J112" s="86" t="s">
         <v>27</v>
@@ -11700,7 +11700,7 @@
       </c>
     </row>
     <row r="113" spans="1:14" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="99"/>
+      <c r="A113" s="126"/>
       <c r="B113" s="32" t="s">
         <v>70</v>
       </c>
@@ -11744,7 +11744,7 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="100"/>
+      <c r="A114" s="127"/>
       <c r="B114" s="34" t="s">
         <v>63</v>
       </c>
@@ -11773,60 +11773,60 @@
         <v>0</v>
       </c>
       <c r="C115" s="10">
-        <f t="shared" ref="C115:G130" si="11">J116*1.1</f>
+        <f t="shared" ref="C115:G130" si="13">J116*1.1</f>
         <v>0</v>
       </c>
       <c r="D115" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E115" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F115" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G115" s="10">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="I115" s="107" t="s">
-        <v>105</v>
-      </c>
-      <c r="J115" s="107"/>
-      <c r="K115" s="107"/>
-      <c r="L115" s="107"/>
-      <c r="M115" s="107"/>
-      <c r="N115" s="107"/>
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I115" s="129" t="s">
+        <v>103</v>
+      </c>
+      <c r="J115" s="129"/>
+      <c r="K115" s="129"/>
+      <c r="L115" s="129"/>
+      <c r="M115" s="129"/>
+      <c r="N115" s="129"/>
     </row>
     <row r="116" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B116" s="10">
-        <f t="shared" ref="B116:B130" si="12">I117*1.1</f>
+        <f t="shared" ref="B116:B130" si="14">I117*1.1</f>
         <v>0</v>
       </c>
       <c r="C116" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D116" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E116" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F116" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G116" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I116" s="17">
@@ -11853,27 +11853,27 @@
         <v>12</v>
       </c>
       <c r="B117" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="C117" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D117" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E117" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F117" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G117" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I117" s="17">
@@ -11900,27 +11900,27 @@
         <v>13</v>
       </c>
       <c r="B118" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.15554000000000001</v>
       </c>
       <c r="C118" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.15554000000000001</v>
       </c>
       <c r="D118" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.15554000000000001</v>
       </c>
       <c r="E118" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>9.0213200000000021E-2</v>
       </c>
       <c r="F118" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>9.0213200000000021E-2</v>
       </c>
       <c r="G118" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6.3771400000000006E-2</v>
       </c>
       <c r="I118" s="17">
@@ -11947,27 +11947,27 @@
         <v>14</v>
       </c>
       <c r="B119" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.30580000000000007</v>
       </c>
       <c r="C119" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.30580000000000007</v>
       </c>
       <c r="D119" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.30580000000000007</v>
       </c>
       <c r="E119" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.17736400000000005</v>
       </c>
       <c r="F119" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.17736400000000005</v>
       </c>
       <c r="G119" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.12537800000000004</v>
       </c>
       <c r="I119" s="17">
@@ -11994,27 +11994,27 @@
         <v>15</v>
       </c>
       <c r="B120" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.31196000000000007</v>
       </c>
       <c r="C120" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.31196000000000007</v>
       </c>
       <c r="D120" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.31196000000000007</v>
       </c>
       <c r="E120" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.18093680000000004</v>
       </c>
       <c r="F120" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.18093680000000004</v>
       </c>
       <c r="G120" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.12790360000000003</v>
       </c>
       <c r="I120" s="17">
@@ -12041,27 +12041,27 @@
         <v>18</v>
       </c>
       <c r="B121" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.23232000000000003</v>
       </c>
       <c r="C121" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.23232000000000003</v>
       </c>
       <c r="D121" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.23232000000000003</v>
       </c>
       <c r="E121" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.13474560000000002</v>
       </c>
       <c r="F121" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.13474560000000002</v>
       </c>
       <c r="G121" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>9.5251200000000008E-2</v>
       </c>
       <c r="I121" s="17">
@@ -12088,27 +12088,27 @@
         <v>17</v>
       </c>
       <c r="B122" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.14828000000000002</v>
       </c>
       <c r="C122" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.14828000000000002</v>
       </c>
       <c r="D122" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.14828000000000002</v>
       </c>
       <c r="E122" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.600240000000002E-2</v>
       </c>
       <c r="F122" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.600240000000002E-2</v>
       </c>
       <c r="G122" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6.079480000000001E-2</v>
       </c>
       <c r="I122" s="17">
@@ -12135,27 +12135,27 @@
         <v>19</v>
       </c>
       <c r="B123" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>5.9620000000000013E-2</v>
       </c>
       <c r="C123" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.9620000000000013E-2</v>
       </c>
       <c r="D123" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.9620000000000013E-2</v>
       </c>
       <c r="E123" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.4579600000000009E-2</v>
       </c>
       <c r="F123" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.4579600000000009E-2</v>
       </c>
       <c r="G123" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.4444200000000003E-2</v>
       </c>
       <c r="I123" s="17">
@@ -12182,27 +12182,27 @@
         <v>20</v>
       </c>
       <c r="B124" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.9360000000000002E-2</v>
       </c>
       <c r="C124" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.9360000000000002E-2</v>
       </c>
       <c r="D124" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.9360000000000002E-2</v>
       </c>
       <c r="E124" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.1228800000000002E-2</v>
       </c>
       <c r="F124" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.1228800000000002E-2</v>
       </c>
       <c r="G124" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7.9376000000000013E-3</v>
       </c>
       <c r="I124" s="17">
@@ -12229,27 +12229,27 @@
         <v>21</v>
       </c>
       <c r="B125" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="C125" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D125" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E125" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F125" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G125" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I125" s="17">
@@ -12276,27 +12276,27 @@
         <v>22</v>
       </c>
       <c r="B126" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="C126" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D126" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E126" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F126" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G126" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I126" s="17">
@@ -12323,27 +12323,27 @@
         <v>42</v>
       </c>
       <c r="B127" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="C127" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D127" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E127" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F127" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G127" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I127" s="17">
@@ -12370,27 +12370,27 @@
         <v>43</v>
       </c>
       <c r="B128" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="C128" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D128" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E128" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F128" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G128" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I128" s="17">
@@ -12417,27 +12417,27 @@
         <v>44</v>
       </c>
       <c r="B129" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="C129" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D129" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E129" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F129" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G129" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I129" s="17">
@@ -12464,27 +12464,27 @@
         <v>45</v>
       </c>
       <c r="B130" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="C130" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D130" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E130" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F130" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G130" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I130" s="17">
@@ -12508,27 +12508,27 @@
     </row>
     <row r="131" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B131">
-        <f t="shared" ref="B131:G131" si="13">5*SUM(B118:B124)</f>
+        <f t="shared" ref="B131:G131" si="15">5*SUM(B118:B124)</f>
         <v>6.1644000000000005</v>
       </c>
       <c r="C131">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>6.1644000000000005</v>
       </c>
       <c r="D131">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>6.1644000000000005</v>
       </c>
       <c r="E131">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3.575352000000001</v>
       </c>
       <c r="F131">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3.575352000000001</v>
       </c>
       <c r="G131">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>2.5274040000000007</v>
       </c>
       <c r="I131" s="17">
@@ -12552,31 +12552,31 @@
     </row>
     <row r="132" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="133" spans="1:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="90" t="s">
+      <c r="A133" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="93" t="s">
-        <v>87</v>
-      </c>
-      <c r="C133" s="94"/>
-      <c r="D133" s="94"/>
-      <c r="E133" s="94"/>
-      <c r="F133" s="94"/>
-      <c r="G133" s="95"/>
-      <c r="I133" s="90" t="s">
+      <c r="B133" s="121" t="s">
+        <v>86</v>
+      </c>
+      <c r="C133" s="122"/>
+      <c r="D133" s="122"/>
+      <c r="E133" s="122"/>
+      <c r="F133" s="122"/>
+      <c r="G133" s="123"/>
+      <c r="I133" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="J133" s="93" t="s">
+      <c r="J133" s="121" t="s">
         <v>76</v>
       </c>
-      <c r="K133" s="94"/>
-      <c r="L133" s="94"/>
-      <c r="M133" s="94"/>
-      <c r="N133" s="94"/>
-      <c r="O133" s="95"/>
+      <c r="K133" s="122"/>
+      <c r="L133" s="122"/>
+      <c r="M133" s="122"/>
+      <c r="N133" s="122"/>
+      <c r="O133" s="123"/>
     </row>
     <row r="134" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="91"/>
+      <c r="A134" s="119"/>
       <c r="B134" s="26" t="s">
         <v>71</v>
       </c>
@@ -12595,7 +12595,7 @@
       <c r="G134" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I134" s="91"/>
+      <c r="I134" s="119"/>
       <c r="J134" s="26" t="s">
         <v>71</v>
       </c>
@@ -12616,7 +12616,7 @@
       </c>
     </row>
     <row r="135" spans="1:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="92"/>
+      <c r="A135" s="120"/>
       <c r="B135" s="40" t="s">
         <v>63</v>
       </c>
@@ -12635,7 +12635,7 @@
       <c r="G135" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I135" s="92"/>
+      <c r="I135" s="120"/>
       <c r="J135" s="40" t="s">
         <v>63</v>
       </c>
@@ -12796,23 +12796,23 @@
         <v>7.7770000000000006E-2</v>
       </c>
       <c r="C139" s="17">
-        <f t="shared" ref="C139:G139" si="14">C118*0.5</f>
+        <f t="shared" ref="C139:G139" si="16">C118*0.5</f>
         <v>7.7770000000000006E-2</v>
       </c>
       <c r="D139" s="17">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>7.7770000000000006E-2</v>
       </c>
       <c r="E139" s="17">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>4.5106600000000011E-2</v>
       </c>
       <c r="F139" s="17">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>4.5106600000000011E-2</v>
       </c>
       <c r="G139" s="17">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>3.1885700000000003E-2</v>
       </c>
       <c r="I139" s="50" t="s">
@@ -12823,23 +12823,23 @@
         <v>5.8327500000000004E-2</v>
       </c>
       <c r="K139" s="17">
-        <f t="shared" ref="K139:O145" si="15">C139*0.75</f>
+        <f t="shared" ref="K139:O145" si="17">C139*0.75</f>
         <v>5.8327500000000004E-2</v>
       </c>
       <c r="L139" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5.8327500000000004E-2</v>
       </c>
       <c r="M139" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3.3829950000000011E-2</v>
       </c>
       <c r="N139" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3.3829950000000011E-2</v>
       </c>
       <c r="O139" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2.3914275000000002E-2</v>
       </c>
     </row>
@@ -12848,54 +12848,54 @@
         <v>14</v>
       </c>
       <c r="B140" s="17">
-        <f t="shared" ref="B140:G145" si="16">B119*0.5</f>
+        <f t="shared" ref="B140:G145" si="18">B119*0.5</f>
         <v>0.15290000000000004</v>
       </c>
       <c r="C140" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.15290000000000004</v>
       </c>
       <c r="D140" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.15290000000000004</v>
       </c>
       <c r="E140" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.8682000000000025E-2</v>
       </c>
       <c r="F140" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.8682000000000025E-2</v>
       </c>
       <c r="G140" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>6.2689000000000022E-2</v>
       </c>
       <c r="I140" s="50" t="s">
         <v>14</v>
       </c>
       <c r="J140" s="17">
-        <f t="shared" ref="J140:J145" si="17">B140*0.75</f>
+        <f t="shared" ref="J140:J145" si="19">B140*0.75</f>
         <v>0.11467500000000003</v>
       </c>
       <c r="K140" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.11467500000000003</v>
       </c>
       <c r="L140" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.11467500000000003</v>
       </c>
       <c r="M140" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6.6511500000000015E-2</v>
       </c>
       <c r="N140" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6.6511500000000015E-2</v>
       </c>
       <c r="O140" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4.7016750000000017E-2</v>
       </c>
     </row>
@@ -12904,54 +12904,54 @@
         <v>15</v>
       </c>
       <c r="B141" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.15598000000000004</v>
       </c>
       <c r="C141" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.15598000000000004</v>
       </c>
       <c r="D141" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.15598000000000004</v>
       </c>
       <c r="E141" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>9.0468400000000018E-2</v>
       </c>
       <c r="F141" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>9.0468400000000018E-2</v>
       </c>
       <c r="G141" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>6.3951800000000017E-2</v>
       </c>
       <c r="I141" s="50" t="s">
         <v>15</v>
       </c>
       <c r="J141" s="17">
+        <f t="shared" si="19"/>
+        <v>0.11698500000000003</v>
+      </c>
+      <c r="K141" s="17">
         <f t="shared" si="17"/>
         <v>0.11698500000000003</v>
       </c>
-      <c r="K141" s="17">
-        <f t="shared" si="15"/>
+      <c r="L141" s="17">
+        <f t="shared" si="17"/>
         <v>0.11698500000000003</v>
       </c>
-      <c r="L141" s="17">
-        <f t="shared" si="15"/>
-        <v>0.11698500000000003</v>
-      </c>
       <c r="M141" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6.7851300000000017E-2</v>
       </c>
       <c r="N141" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>6.7851300000000017E-2</v>
       </c>
       <c r="O141" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4.7963850000000016E-2</v>
       </c>
     </row>
@@ -12960,54 +12960,54 @@
         <v>18</v>
       </c>
       <c r="B142" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.11616000000000001</v>
       </c>
       <c r="C142" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.11616000000000001</v>
       </c>
       <c r="D142" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.11616000000000001</v>
       </c>
       <c r="E142" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>6.737280000000001E-2</v>
       </c>
       <c r="F142" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>6.737280000000001E-2</v>
       </c>
       <c r="G142" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>4.7625600000000004E-2</v>
       </c>
       <c r="I142" s="50" t="s">
         <v>18</v>
       </c>
       <c r="J142" s="17">
+        <f t="shared" si="19"/>
+        <v>8.7120000000000003E-2</v>
+      </c>
+      <c r="K142" s="17">
         <f t="shared" si="17"/>
         <v>8.7120000000000003E-2</v>
       </c>
-      <c r="K142" s="17">
-        <f t="shared" si="15"/>
+      <c r="L142" s="17">
+        <f t="shared" si="17"/>
         <v>8.7120000000000003E-2</v>
       </c>
-      <c r="L142" s="17">
-        <f t="shared" si="15"/>
-        <v>8.7120000000000003E-2</v>
-      </c>
       <c r="M142" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5.0529600000000008E-2</v>
       </c>
       <c r="N142" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>5.0529600000000008E-2</v>
       </c>
       <c r="O142" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3.5719200000000007E-2</v>
       </c>
     </row>
@@ -13016,54 +13016,54 @@
         <v>17</v>
       </c>
       <c r="B143" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>7.4140000000000011E-2</v>
       </c>
       <c r="C143" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>7.4140000000000011E-2</v>
       </c>
       <c r="D143" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>7.4140000000000011E-2</v>
       </c>
       <c r="E143" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>4.300120000000001E-2</v>
       </c>
       <c r="F143" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>4.300120000000001E-2</v>
       </c>
       <c r="G143" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.0397400000000005E-2</v>
       </c>
       <c r="I143" s="50" t="s">
         <v>17</v>
       </c>
       <c r="J143" s="17">
+        <f t="shared" si="19"/>
+        <v>5.5605000000000009E-2</v>
+      </c>
+      <c r="K143" s="17">
         <f t="shared" si="17"/>
         <v>5.5605000000000009E-2</v>
       </c>
-      <c r="K143" s="17">
-        <f t="shared" si="15"/>
+      <c r="L143" s="17">
+        <f t="shared" si="17"/>
         <v>5.5605000000000009E-2</v>
       </c>
-      <c r="L143" s="17">
-        <f t="shared" si="15"/>
-        <v>5.5605000000000009E-2</v>
-      </c>
       <c r="M143" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3.2250900000000006E-2</v>
       </c>
       <c r="N143" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3.2250900000000006E-2</v>
       </c>
       <c r="O143" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2.2798050000000004E-2</v>
       </c>
     </row>
@@ -13072,54 +13072,54 @@
         <v>19</v>
       </c>
       <c r="B144" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.9810000000000007E-2</v>
       </c>
       <c r="C144" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.9810000000000007E-2</v>
       </c>
       <c r="D144" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.9810000000000007E-2</v>
       </c>
       <c r="E144" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.7289800000000004E-2</v>
       </c>
       <c r="F144" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.7289800000000004E-2</v>
       </c>
       <c r="G144" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.2222100000000001E-2</v>
       </c>
       <c r="I144" s="50" t="s">
         <v>19</v>
       </c>
       <c r="J144" s="17">
+        <f t="shared" si="19"/>
+        <v>2.2357500000000006E-2</v>
+      </c>
+      <c r="K144" s="17">
         <f t="shared" si="17"/>
         <v>2.2357500000000006E-2</v>
       </c>
-      <c r="K144" s="17">
-        <f t="shared" si="15"/>
+      <c r="L144" s="17">
+        <f t="shared" si="17"/>
         <v>2.2357500000000006E-2</v>
       </c>
-      <c r="L144" s="17">
-        <f t="shared" si="15"/>
-        <v>2.2357500000000006E-2</v>
-      </c>
       <c r="M144" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.2967350000000002E-2</v>
       </c>
       <c r="N144" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1.2967350000000002E-2</v>
       </c>
       <c r="O144" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>9.1665750000000015E-3</v>
       </c>
     </row>
@@ -13128,54 +13128,54 @@
         <v>20</v>
       </c>
       <c r="B145" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>9.6800000000000011E-3</v>
       </c>
       <c r="C145" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>9.6800000000000011E-3</v>
       </c>
       <c r="D145" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>9.6800000000000011E-3</v>
       </c>
       <c r="E145" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5.6144000000000012E-3</v>
       </c>
       <c r="F145" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5.6144000000000012E-3</v>
       </c>
       <c r="G145" s="17">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.9688000000000006E-3</v>
       </c>
       <c r="I145" s="50" t="s">
         <v>20</v>
       </c>
       <c r="J145" s="17">
+        <f t="shared" si="19"/>
+        <v>7.2600000000000008E-3</v>
+      </c>
+      <c r="K145" s="17">
         <f t="shared" si="17"/>
         <v>7.2600000000000008E-3</v>
       </c>
-      <c r="K145" s="17">
-        <f t="shared" si="15"/>
+      <c r="L145" s="17">
+        <f t="shared" si="17"/>
         <v>7.2600000000000008E-3</v>
       </c>
-      <c r="L145" s="17">
-        <f t="shared" si="15"/>
-        <v>7.2600000000000008E-3</v>
-      </c>
       <c r="M145" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4.2108000000000007E-3</v>
       </c>
       <c r="N145" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4.2108000000000007E-3</v>
       </c>
       <c r="O145" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2.9766000000000003E-3</v>
       </c>
     </row>
@@ -13445,57 +13445,57 @@
     </row>
     <row r="152" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B152">
-        <f t="shared" ref="B152:G152" si="18">5*SUM(B136:B151)</f>
+        <f t="shared" ref="B152:G152" si="20">5*SUM(B136:B151)</f>
         <v>3.0822000000000003</v>
       </c>
       <c r="C152">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>3.0822000000000003</v>
       </c>
       <c r="D152">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>3.0822000000000003</v>
       </c>
       <c r="E152">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>1.7876760000000005</v>
       </c>
       <c r="F152">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>1.7876760000000005</v>
       </c>
       <c r="G152">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>1.2637020000000003</v>
       </c>
       <c r="J152">
-        <f t="shared" ref="J152:O152" si="19">5*SUM(J136:J151)</f>
+        <f t="shared" ref="J152:O152" si="21">5*SUM(J136:J151)</f>
         <v>2.3116500000000002</v>
       </c>
       <c r="K152">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>2.3116500000000002</v>
       </c>
       <c r="L152">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>2.3116500000000002</v>
       </c>
       <c r="M152">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1.3407570000000004</v>
       </c>
       <c r="N152">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1.3407570000000004</v>
       </c>
       <c r="O152">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.94777650000000035</v>
       </c>
     </row>
     <row r="158" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B158" s="37"/>
       <c r="C158" s="37"/>
@@ -13575,22 +13575,22 @@
       <c r="W160" s="37"/>
     </row>
     <row r="161" spans="1:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="109" t="s">
-        <v>91</v>
-      </c>
-      <c r="B161" s="111" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="111"/>
-      <c r="D161" s="111"/>
-      <c r="E161" s="111" t="s">
+      <c r="A161" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="B161" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="112"/>
+      <c r="D161" s="112"/>
+      <c r="E161" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="F161" s="111"/>
-      <c r="G161" s="111"/>
+      <c r="F161" s="112"/>
+      <c r="G161" s="112"/>
     </row>
     <row r="162" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="109"/>
+      <c r="A162" s="104"/>
       <c r="B162" s="63" t="s">
         <v>3</v>
       </c>
@@ -13633,15 +13633,15 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J163">
-        <f t="shared" ref="J163:J178" si="20">B163*B54</f>
+        <f t="shared" ref="J163:J178" si="22">B163*B54</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="K163">
-        <f t="shared" ref="K163:K178" si="21">C163*C54</f>
+        <f t="shared" ref="K163:K178" si="23">C163*C54</f>
         <v>0</v>
       </c>
       <c r="L163">
-        <f t="shared" ref="L163:L178" si="22">D163*D54</f>
+        <f t="shared" ref="L163:L178" si="24">D163*D54</f>
         <v>0</v>
       </c>
     </row>
@@ -13668,15 +13668,15 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J164">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="K164">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L164">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -13703,15 +13703,15 @@
         <v>1.2</v>
       </c>
       <c r="J165">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.176E-2</v>
       </c>
       <c r="K165">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1.8E-3</v>
       </c>
       <c r="L165">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>6.0000000000000218E-3</v>
       </c>
       <c r="M165">
@@ -13746,23 +13746,23 @@
         <v>12.1863636363636</v>
       </c>
       <c r="J166">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.4223484848484847</v>
       </c>
       <c r="K166">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1.8215909090909104</v>
       </c>
       <c r="L166">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.0155303030302998</v>
       </c>
       <c r="M166">
-        <f t="shared" ref="M166:M178" si="23">SUM(J166:L166)</f>
+        <f t="shared" ref="M166:M178" si="25">SUM(J166:L166)</f>
         <v>3.2594696969696946</v>
       </c>
       <c r="N166">
-        <f t="shared" ref="N166:N178" si="24">1/M166</f>
+        <f t="shared" ref="N166:N178" si="26">1/M166</f>
         <v>0.30679837303893109</v>
       </c>
     </row>
@@ -13789,23 +13789,23 @@
         <v>13.4262295081967</v>
       </c>
       <c r="J167">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.41491596638655454</v>
       </c>
       <c r="K167">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1.6911764705882355</v>
       </c>
       <c r="L167">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.1470588235294099</v>
       </c>
       <c r="M167">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>3.2531512605041999</v>
       </c>
       <c r="N167">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.30739425250242186</v>
       </c>
     </row>
@@ -13832,23 +13832,23 @@
         <v>6.9705882352941204</v>
       </c>
       <c r="J168">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.39310344827586191</v>
       </c>
       <c r="K168">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1.0551724137931051</v>
       </c>
       <c r="L168">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.54482758620689675</v>
       </c>
       <c r="M168">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>1.9931034482758638</v>
       </c>
       <c r="N168">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.50173010380622796</v>
       </c>
     </row>
@@ -13875,23 +13875,23 @@
         <v>5.8421052631579</v>
       </c>
       <c r="J169">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.46610169491525449</v>
       </c>
       <c r="K169">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.84745762711864525</v>
       </c>
       <c r="L169">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.31355932203389858</v>
       </c>
       <c r="M169">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>1.6271186440677983</v>
       </c>
       <c r="N169">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.6145833333333327</v>
       </c>
     </row>
@@ -13918,23 +13918,23 @@
         <v>6.2222222222222197</v>
       </c>
       <c r="J170">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.59655172413793078</v>
       </c>
       <c r="K170">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.48965517241379319</v>
       </c>
       <c r="L170">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.19310344827586198</v>
       </c>
       <c r="M170">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>1.279310344827586</v>
       </c>
       <c r="N170">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.78167115902964968</v>
       </c>
     </row>
@@ -13961,23 +13961,23 @@
         <v>7.75</v>
       </c>
       <c r="J171">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.68881118881118886</v>
       </c>
       <c r="K171">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.40559440559440618</v>
       </c>
       <c r="L171">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.10839160839160839</v>
       </c>
       <c r="M171">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>1.2027972027972034</v>
       </c>
       <c r="N171">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.83139534883720889</v>
       </c>
     </row>
@@ -14004,23 +14004,23 @@
         <v>1</v>
       </c>
       <c r="J172">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.61194029850746257</v>
       </c>
       <c r="K172">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L172">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1E-3</v>
       </c>
       <c r="M172">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.95763022388059793</v>
       </c>
       <c r="N172">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -14047,23 +14047,23 @@
         <v>1</v>
       </c>
       <c r="J173">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.61194029850746257</v>
       </c>
       <c r="K173">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L173">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1E-3</v>
       </c>
       <c r="M173">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.95763022388059793</v>
       </c>
       <c r="N173">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -14090,23 +14090,23 @@
         <v>1</v>
       </c>
       <c r="J174">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.61194029850746257</v>
       </c>
       <c r="K174">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L174">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1E-3</v>
       </c>
       <c r="M174">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.95763022388059793</v>
       </c>
       <c r="N174">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -14133,23 +14133,23 @@
         <v>1</v>
       </c>
       <c r="J175">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.61194029850746257</v>
       </c>
       <c r="K175">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L175">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1E-3</v>
       </c>
       <c r="M175">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.95763022388059793</v>
       </c>
       <c r="N175">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -14176,23 +14176,23 @@
         <v>1</v>
       </c>
       <c r="J176">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.61194029850746257</v>
       </c>
       <c r="K176">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L176">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1E-3</v>
       </c>
       <c r="M176">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.95763022388059793</v>
       </c>
       <c r="N176">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -14219,23 +14219,23 @@
         <v>1</v>
       </c>
       <c r="J177">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.61194029850746257</v>
       </c>
       <c r="K177">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L177">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1E-3</v>
       </c>
       <c r="M177">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.95763022388059793</v>
       </c>
       <c r="N177">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -14266,23 +14266,23 @@
         <v>2.1889244186386922</v>
       </c>
       <c r="J178">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.61194029850746257</v>
       </c>
       <c r="K178">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.34468992537313536</v>
       </c>
       <c r="L178">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1E-3</v>
       </c>
       <c r="M178">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.95763022388059793</v>
       </c>
       <c r="N178">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0442444015057371</v>
       </c>
     </row>
@@ -14386,9 +14386,9 @@
       <c r="AB185" s="20"/>
     </row>
     <row r="186" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="112"/>
-      <c r="B186" s="112"/>
-      <c r="C186" s="112"/>
+      <c r="A186" s="113"/>
+      <c r="B186" s="113"/>
+      <c r="C186" s="113"/>
       <c r="D186" s="20"/>
       <c r="E186" s="20"/>
       <c r="F186" s="20"/>
@@ -14537,7 +14537,7 @@
     </row>
     <row r="197" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A197" s="36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B197" s="37"/>
       <c r="C197" s="37"/>
@@ -14563,39 +14563,39 @@
       <c r="W197" s="37"/>
     </row>
     <row r="198" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="101" t="s">
+      <c r="A198" s="109" t="s">
         <v>73</v>
       </c>
-      <c r="B198" s="101"/>
-      <c r="C198" s="101"/>
-      <c r="D198" s="101"/>
-      <c r="E198" s="101"/>
-      <c r="F198" s="101"/>
+      <c r="B198" s="109"/>
+      <c r="C198" s="109"/>
+      <c r="D198" s="109"/>
+      <c r="E198" s="109"/>
+      <c r="F198" s="109"/>
     </row>
     <row r="199" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="113" t="s">
+      <c r="A199" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="B199" s="113"/>
-      <c r="C199" s="113"/>
-      <c r="D199" s="113"/>
-      <c r="E199" s="113"/>
-      <c r="F199" s="113"/>
+      <c r="B199" s="114"/>
+      <c r="C199" s="114"/>
+      <c r="D199" s="114"/>
+      <c r="E199" s="114"/>
+      <c r="F199" s="114"/>
     </row>
     <row r="200" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A200" s="96" t="s">
+      <c r="A200" s="115" t="s">
         <v>46</v>
       </c>
       <c r="B200" s="43"/>
       <c r="C200" s="43"/>
-      <c r="D200" s="96" t="s">
+      <c r="D200" s="115" t="s">
         <v>51</v>
       </c>
-      <c r="E200" s="96"/>
-      <c r="F200" s="96"/>
+      <c r="E200" s="115"/>
+      <c r="F200" s="115"/>
     </row>
     <row r="201" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A201" s="96"/>
+      <c r="A201" s="115"/>
       <c r="B201" s="43"/>
       <c r="C201" s="44" t="s">
         <v>47</v>
@@ -14630,22 +14630,22 @@
         <v>0</v>
       </c>
       <c r="H202">
-        <f t="shared" ref="H202:H217" si="25">D202*B54</f>
+        <f t="shared" ref="H202:H217" si="27">D202*B54</f>
         <v>0</v>
       </c>
       <c r="I202">
-        <f t="shared" ref="I202:I217" si="26">E202*C54</f>
+        <f t="shared" ref="I202:I217" si="28">E202*C54</f>
         <v>0</v>
       </c>
       <c r="J202">
-        <f t="shared" ref="J202:J217" si="27">F202*D54</f>
+        <f t="shared" ref="J202:J217" si="29">F202*D54</f>
         <v>0</v>
       </c>
       <c r="N202" s="73" t="s">
         <v>2</v>
       </c>
       <c r="O202" s="108" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P202" s="108"/>
       <c r="Q202" s="108"/>
@@ -14666,15 +14666,15 @@
         <v>0</v>
       </c>
       <c r="H203">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="I203">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="J203">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="N203" s="45" t="s">
@@ -14708,15 +14708,15 @@
         <v>1.1232</v>
       </c>
       <c r="H204">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>3.0575999999999999</v>
       </c>
       <c r="I204">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>2.8080000000000001E-2</v>
       </c>
       <c r="J204">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>5.6160000000000203E-3</v>
       </c>
       <c r="K204">
@@ -14754,19 +14754,19 @@
         <v>5.6159999999999997</v>
       </c>
       <c r="H205">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>7.9418181818181806</v>
       </c>
       <c r="I205">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>3.814909090909091</v>
       </c>
       <c r="J205">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.46799999999999986</v>
       </c>
       <c r="K205">
-        <f t="shared" ref="K205:K217" si="28">SUM(H205:J205)</f>
+        <f t="shared" ref="K205:K217" si="30">SUM(H205:J205)</f>
         <v>12.224727272727272</v>
       </c>
       <c r="N205" s="45" t="s">
@@ -14802,34 +14802,34 @@
         <v>22.463999999999999</v>
       </c>
       <c r="H206">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>29.452100840336129</v>
       </c>
       <c r="I206">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>16.570084033613444</v>
       </c>
       <c r="J206">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>1.9191932773109244</v>
       </c>
       <c r="K206">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>47.941378151260494</v>
       </c>
       <c r="N206" s="45" t="s">
         <v>33</v>
       </c>
       <c r="O206" s="9">
-        <f t="shared" ref="O206:O218" si="29">D205/D204</f>
+        <f t="shared" ref="O206:O218" si="31">D205/D204</f>
         <v>5</v>
       </c>
       <c r="P206" s="9">
-        <f t="shared" ref="P206:P218" si="30">E205/E204</f>
+        <f t="shared" ref="P206:P218" si="32">E205/E204</f>
         <v>4.9999999999999991</v>
       </c>
       <c r="Q206" s="9">
-        <f t="shared" ref="Q206:Q218" si="31">F205/F204</f>
+        <f t="shared" ref="Q206:Q218" si="33">F205/F204</f>
         <v>5</v>
       </c>
     </row>
@@ -14851,34 +14851,34 @@
         <v>56.16</v>
       </c>
       <c r="H207">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>79.613793103448273</v>
       </c>
       <c r="I207">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>38.515862068965518</v>
       </c>
       <c r="J207">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>4.38951724137931</v>
       </c>
       <c r="K207">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>122.5191724137931</v>
       </c>
       <c r="N207" s="45" t="s">
         <v>34</v>
       </c>
       <c r="O207" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="P207" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>4</v>
       </c>
       <c r="Q207" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>4</v>
       </c>
     </row>
@@ -14890,7 +14890,7 @@
         <v>10</v>
       </c>
       <c r="C208" s="43">
-        <f t="shared" ref="C208:C217" si="32">EXP(LN(0.5)*B207/10)</f>
+        <f t="shared" ref="C208:C217" si="34">EXP(LN(0.5)*B207/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D208" s="65">
@@ -14903,19 +14903,19 @@
         <v>39.711116831436499</v>
       </c>
       <c r="H208">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>66.683764924100601</v>
       </c>
       <c r="I208">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>22.622623053690308</v>
       </c>
       <c r="J208">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>2.1313876265460268</v>
       </c>
       <c r="K208">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>91.437775604336935</v>
       </c>
       <c r="M208" s="39"/>
@@ -14923,15 +14923,15 @@
         <v>35</v>
       </c>
       <c r="O208" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>2.5</v>
       </c>
       <c r="P208" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>2.5</v>
       </c>
       <c r="Q208" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>2.5</v>
       </c>
     </row>
@@ -14943,7 +14943,7 @@
         <v>15</v>
       </c>
       <c r="C209" s="43">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.5</v>
       </c>
       <c r="D209" s="65">
@@ -14956,34 +14956,34 @@
         <v>28.08</v>
       </c>
       <c r="H209">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>59.710344827586205</v>
       </c>
       <c r="I209">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>9.5213793103448268</v>
       </c>
       <c r="J209">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.87144827586206886</v>
       </c>
       <c r="K209">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>70.103172413793089</v>
       </c>
       <c r="N209" s="45" t="s">
         <v>36</v>
       </c>
       <c r="O209" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.70710678118654491</v>
       </c>
       <c r="P209" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.70710678118654813</v>
       </c>
       <c r="Q209" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.70710678118654735</v>
       </c>
     </row>
@@ -14995,7 +14995,7 @@
         <v>20</v>
       </c>
       <c r="C210" s="43">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.35355339059327379</v>
       </c>
       <c r="D210" s="65">
@@ -15008,34 +15008,34 @@
         <v>19.855558415718299</v>
       </c>
       <c r="H210">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>45.126269126632387</v>
       </c>
       <c r="I210">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>5.5540023540470607</v>
       </c>
       <c r="J210">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.27770011770235381</v>
       </c>
       <c r="K210">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>50.957971598381803</v>
       </c>
       <c r="N210" s="45" t="s">
         <v>37</v>
       </c>
       <c r="O210" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.70710678118655024</v>
       </c>
       <c r="P210" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.70710678118654691</v>
       </c>
       <c r="Q210" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.70710678118654768</v>
       </c>
     </row>
@@ -15047,7 +15047,7 @@
         <v>25</v>
       </c>
       <c r="C211" s="43">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.25</v>
       </c>
       <c r="D211" s="65">
@@ -15060,34 +15060,34 @@
         <v>14.04</v>
       </c>
       <c r="H211">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>33.179104477611936</v>
       </c>
       <c r="I211">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>3.4691373134328458</v>
       </c>
       <c r="J211">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>1.4039999999999999E-2</v>
       </c>
       <c r="K211">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>36.662281791044784</v>
       </c>
       <c r="N211" s="45" t="s">
         <v>38</v>
       </c>
       <c r="O211" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.70710678118654735</v>
       </c>
       <c r="P211" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.70710678118654713</v>
       </c>
       <c r="Q211" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.70710678118654913</v>
       </c>
     </row>
@@ -15099,7 +15099,7 @@
         <v>30</v>
       </c>
       <c r="C212" s="43">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.17677669529663689</v>
       </c>
       <c r="D212" s="65">
@@ -15112,34 +15112,34 @@
         <v>9.92777920785913</v>
       </c>
       <c r="H212">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>23.461169769816379</v>
       </c>
       <c r="I212">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>2.4530505191956449</v>
       </c>
       <c r="J212">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>9.9277792078591304E-3</v>
       </c>
       <c r="K212">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>25.924148068219885</v>
       </c>
       <c r="N212" s="45" t="s">
         <v>39</v>
       </c>
       <c r="O212" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="P212" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q212" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.70710678118654591</v>
       </c>
     </row>
@@ -15151,7 +15151,7 @@
         <v>35</v>
       </c>
       <c r="C213" s="43">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.12500000000000003</v>
       </c>
       <c r="D213" s="65">
@@ -15164,34 +15164,34 @@
         <v>7.02</v>
       </c>
       <c r="H213">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>16.589552238805968</v>
       </c>
       <c r="I213">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>1.7345686567164229</v>
       </c>
       <c r="J213">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>7.0199999999999993E-3</v>
       </c>
       <c r="K213">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>18.331140895522392</v>
       </c>
       <c r="N213" s="45" t="s">
         <v>40</v>
       </c>
       <c r="O213" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.70710678118654868</v>
       </c>
       <c r="P213" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.70710678118654713</v>
       </c>
       <c r="Q213" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.70710678118654779</v>
       </c>
     </row>
@@ -15216,34 +15216,34 @@
         <v>4.9638896039295597</v>
       </c>
       <c r="H214">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>11.73058488490819</v>
       </c>
       <c r="I214">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>1.2265252595978238</v>
       </c>
       <c r="J214">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>4.96388960392956E-3</v>
       </c>
       <c r="K214">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>12.962074034109945</v>
       </c>
       <c r="N214" s="45" t="s">
         <v>41</v>
       </c>
       <c r="O214" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.70710678118654635</v>
       </c>
       <c r="P214" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q214" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.70710678118654724</v>
       </c>
     </row>
@@ -15255,7 +15255,7 @@
         <v>45</v>
       </c>
       <c r="C215" s="43">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>6.25E-2</v>
       </c>
       <c r="D215" s="65">
@@ -15268,34 +15268,34 @@
         <v>3.51</v>
       </c>
       <c r="H215">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>8.2947761194029841</v>
       </c>
       <c r="I215">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0.86728432835821145</v>
       </c>
       <c r="J215">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>3.5099999999999997E-3</v>
       </c>
       <c r="K215">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>9.1655704477611959</v>
       </c>
       <c r="N215" s="45" t="s">
         <v>42</v>
       </c>
       <c r="O215" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.70710678118654868</v>
       </c>
       <c r="P215" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.70710678118654779</v>
       </c>
       <c r="Q215" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.70710678118654702</v>
       </c>
     </row>
@@ -15307,7 +15307,7 @@
         <v>50</v>
       </c>
       <c r="C216" s="43">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>4.4194173824159223E-2</v>
       </c>
       <c r="D216" s="65">
@@ -15320,34 +15320,34 @@
         <v>2.4819448019647798</v>
       </c>
       <c r="H216">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>5.8652924424540869</v>
       </c>
       <c r="I216">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0.61326262979891122</v>
       </c>
       <c r="J216">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>2.48194480196478E-3</v>
       </c>
       <c r="K216">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>6.4810370170549634</v>
       </c>
       <c r="N216" s="45" t="s">
         <v>43</v>
       </c>
       <c r="O216" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.70710678118654635</v>
       </c>
       <c r="P216" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.70710678118654724</v>
       </c>
       <c r="Q216" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.70710678118654802</v>
       </c>
     </row>
@@ -15359,7 +15359,7 @@
         <v>55</v>
       </c>
       <c r="C217" s="43">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>3.125E-2</v>
       </c>
       <c r="D217" s="65">
@@ -15372,34 +15372,34 @@
         <v>1.7549999999999999</v>
       </c>
       <c r="H217">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>4.147388059701492</v>
       </c>
       <c r="I217">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0.43364216417910573</v>
       </c>
       <c r="J217">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>1.7549999999999998E-3</v>
       </c>
       <c r="K217">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>4.5827852238805979</v>
       </c>
       <c r="N217" s="45" t="s">
         <v>44</v>
       </c>
       <c r="O217" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="P217" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.70710678118654713</v>
       </c>
       <c r="Q217" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.70710678118654702</v>
       </c>
     </row>
@@ -15422,42 +15422,42 @@
         <v>45</v>
       </c>
       <c r="O218" s="9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.70710678118654735</v>
       </c>
       <c r="P218" s="9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q218" s="9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.70710678118654802</v>
       </c>
     </row>
     <row r="219" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="97" t="s">
+      <c r="A219" s="124" t="s">
         <v>75</v>
       </c>
-      <c r="B219" s="97"/>
-      <c r="C219" s="97"/>
-      <c r="D219" s="97"/>
-      <c r="E219" s="97"/>
-      <c r="F219" s="97"/>
+      <c r="B219" s="124"/>
+      <c r="C219" s="124"/>
+      <c r="D219" s="124"/>
+      <c r="E219" s="124"/>
+      <c r="F219" s="124"/>
     </row>
     <row r="220" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A220" s="110" t="s">
+      <c r="A220" s="111" t="s">
         <v>2</v>
       </c>
       <c r="B220" s="43"/>
       <c r="C220" s="43"/>
-      <c r="D220" s="96" t="s">
+      <c r="D220" s="115" t="s">
         <v>51</v>
       </c>
-      <c r="E220" s="96"/>
-      <c r="F220" s="96"/>
+      <c r="E220" s="115"/>
+      <c r="F220" s="115"/>
     </row>
     <row r="221" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A221" s="110"/>
+      <c r="A221" s="111"/>
       <c r="B221" s="43"/>
       <c r="C221" s="44" t="s">
         <v>47</v>
@@ -15491,7 +15491,7 @@
         <v>2</v>
       </c>
       <c r="O222" s="108" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P222" s="108"/>
       <c r="Q222" s="108"/>
@@ -15607,15 +15607,15 @@
         <v>33</v>
       </c>
       <c r="O226" s="9">
-        <f t="shared" ref="O226:O238" si="33">D225/D224</f>
+        <f t="shared" ref="O226:O238" si="35">D225/D224</f>
         <v>2.4</v>
       </c>
       <c r="P226" s="9">
-        <f t="shared" ref="P226:P238" si="34">E225/E224</f>
+        <f t="shared" ref="P226:P238" si="36">E225/E224</f>
         <v>2.4</v>
       </c>
       <c r="Q226" s="9">
-        <f t="shared" ref="Q226:Q238" si="35">F225/F224</f>
+        <f t="shared" ref="Q226:Q238" si="37">F225/F224</f>
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -15640,15 +15640,15 @@
         <v>34</v>
       </c>
       <c r="O227" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>4</v>
       </c>
       <c r="P227" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>4</v>
       </c>
       <c r="Q227" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
     </row>
@@ -15660,7 +15660,7 @@
         <v>10</v>
       </c>
       <c r="C228" s="43">
-        <f t="shared" ref="C228:C237" si="36">EXP(LN(0.5)*B227/10)</f>
+        <f t="shared" ref="C228:C237" si="38">EXP(LN(0.5)*B227/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D228" s="64">
@@ -15676,15 +15676,15 @@
         <v>35</v>
       </c>
       <c r="O228" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1.8750000000000002</v>
       </c>
       <c r="P228" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1.875</v>
       </c>
       <c r="Q228" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>1.8749999999999998</v>
       </c>
     </row>
@@ -15696,7 +15696,7 @@
         <v>15</v>
       </c>
       <c r="C229" s="43">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.5</v>
       </c>
       <c r="D229" s="64">
@@ -15712,15 +15712,15 @@
         <v>36</v>
       </c>
       <c r="O229" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="P229" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q229" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.70710678118654846</v>
       </c>
     </row>
@@ -15732,7 +15732,7 @@
         <v>20</v>
       </c>
       <c r="C230" s="43">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.35355339059327379</v>
       </c>
       <c r="D230" s="64">
@@ -15748,15 +15748,15 @@
         <v>37</v>
       </c>
       <c r="O230" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.70710678118654735</v>
       </c>
       <c r="P230" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.70710678118654702</v>
       </c>
       <c r="Q230" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.70710678118654657</v>
       </c>
     </row>
@@ -15768,7 +15768,7 @@
         <v>25</v>
       </c>
       <c r="C231" s="43">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.25</v>
       </c>
       <c r="D231" s="64">
@@ -15784,15 +15784,15 @@
         <v>38</v>
       </c>
       <c r="O231" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.70710678118654702</v>
       </c>
       <c r="P231" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q231" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.70710678118654646</v>
       </c>
     </row>
@@ -15804,7 +15804,7 @@
         <v>30</v>
       </c>
       <c r="C232" s="43">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.17677669529663689</v>
       </c>
       <c r="D232" s="64">
@@ -15820,15 +15820,15 @@
         <v>39</v>
       </c>
       <c r="O232" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="P232" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.70710678118654702</v>
       </c>
       <c r="Q232" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.70710678118654857</v>
       </c>
     </row>
@@ -15840,7 +15840,7 @@
         <v>35</v>
       </c>
       <c r="C233" s="43">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.12500000000000003</v>
       </c>
       <c r="D233" s="64">
@@ -15856,15 +15856,15 @@
         <v>40</v>
       </c>
       <c r="O233" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.78567420131838739</v>
       </c>
       <c r="P233" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.78567420131838561</v>
       </c>
       <c r="Q233" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.78567420131838639</v>
       </c>
     </row>
@@ -15876,7 +15876,7 @@
         <v>40</v>
       </c>
       <c r="C234" s="43">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>8.8388347648318447E-2</v>
       </c>
       <c r="D234" s="64">
@@ -15892,15 +15892,15 @@
         <v>41</v>
       </c>
       <c r="O234" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.70710678118654635</v>
       </c>
       <c r="P234" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q234" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.70710678118654724</v>
       </c>
     </row>
@@ -15912,7 +15912,7 @@
         <v>45</v>
       </c>
       <c r="C235" s="43">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>6.25E-2</v>
       </c>
       <c r="D235" s="64">
@@ -15928,15 +15928,15 @@
         <v>42</v>
       </c>
       <c r="O235" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.70710678118654868</v>
       </c>
       <c r="P235" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.70710678118654779</v>
       </c>
       <c r="Q235" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.70710678118654702</v>
       </c>
     </row>
@@ -15964,15 +15964,15 @@
         <v>43</v>
       </c>
       <c r="O236" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.70710678118654635</v>
       </c>
       <c r="P236" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.70710678118654724</v>
       </c>
       <c r="Q236" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.70710678118654802</v>
       </c>
     </row>
@@ -15984,7 +15984,7 @@
         <v>55</v>
       </c>
       <c r="C237" s="43">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>3.125E-2</v>
       </c>
       <c r="D237" s="64">
@@ -16000,15 +16000,15 @@
         <v>44</v>
       </c>
       <c r="O237" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="P237" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.70710678118654713</v>
       </c>
       <c r="Q237" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.70710678118654702</v>
       </c>
     </row>
@@ -16023,15 +16023,15 @@
         <v>45</v>
       </c>
       <c r="O238" s="9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.70710678118654735</v>
       </c>
       <c r="P238" s="9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q238" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.70710678118654802</v>
       </c>
     </row>
@@ -16088,27 +16088,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="AA87:AA88"/>
-    <mergeCell ref="N81:N83"/>
-    <mergeCell ref="B81:L82"/>
-    <mergeCell ref="AA81:AI81"/>
-    <mergeCell ref="AB82:AI82"/>
-    <mergeCell ref="AB87:AI87"/>
-    <mergeCell ref="O81:Y82"/>
-    <mergeCell ref="AA82:AA83"/>
-    <mergeCell ref="O222:Q222"/>
-    <mergeCell ref="O202:Q202"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A161:A162"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="E161:G161"/>
-    <mergeCell ref="A186:C186"/>
-    <mergeCell ref="A198:F198"/>
-    <mergeCell ref="A199:F199"/>
-    <mergeCell ref="D200:F200"/>
-    <mergeCell ref="D220:F220"/>
-    <mergeCell ref="A111:Q111"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="I133:I135"/>
     <mergeCell ref="J133:O133"/>
@@ -16125,6 +16104,27 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="I115:N115"/>
+    <mergeCell ref="O222:Q222"/>
+    <mergeCell ref="O202:Q202"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="E161:G161"/>
+    <mergeCell ref="A186:C186"/>
+    <mergeCell ref="A198:F198"/>
+    <mergeCell ref="A199:F199"/>
+    <mergeCell ref="D200:F200"/>
+    <mergeCell ref="D220:F220"/>
+    <mergeCell ref="A111:Q111"/>
+    <mergeCell ref="AA87:AA88"/>
+    <mergeCell ref="N81:N83"/>
+    <mergeCell ref="B81:L82"/>
+    <mergeCell ref="AA81:AI81"/>
+    <mergeCell ref="AB82:AI82"/>
+    <mergeCell ref="AB87:AI87"/>
+    <mergeCell ref="O81:Y82"/>
+    <mergeCell ref="AA82:AA83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Enable auto-updating & increase initial population size
Change assumption about the historical decline of the KZN
provincial share of the SA population. Increased the slope to assume a
larger initial provincial share in 1950, which is used to estimate the
KZN population size in 1950. The initial population size in 1925 is then
back-extrapolated.

Use equations rather than built-in Excel trendlines to calculate
exponential trend for KZN population changes by age from 1925-1950. This
enables auto-updating of estimated 1925 population size by gender and
age with changes to assumptions about the KZN provincial share in 1950.
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2625" windowHeight="2385" tabRatio="607"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11220" windowHeight="6495" tabRatio="607"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -2008,52 +2008,52 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>-152100.42167838168</c:v>
+                  <c:v>-232193.22062680181</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-106612.48230402569</c:v>
+                  <c:v>-159981.19086849148</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-107405.94202558786</c:v>
+                  <c:v>-130604.16798656604</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-101517.15463011744</c:v>
+                  <c:v>-116663.80924930885</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-72544.531411124772</c:v>
+                  <c:v>-105384.52275663237</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-64144.510344209695</c:v>
+                  <c:v>-95487.192629204481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-52521.552285925158</c:v>
+                  <c:v>-88295.901522314613</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-43004.6692962585</c:v>
+                  <c:v>-81236.378677701534</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-62733.386819434447</c:v>
+                  <c:v>-73180.407288058326</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-35212.241466369451</c:v>
+                  <c:v>-62269.527941188258</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-35474.307358708502</c:v>
+                  <c:v>-49094.741236225527</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-24318.165076374728</c:v>
+                  <c:v>-38060.556537016608</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-19243.353103262907</c:v>
+                  <c:v>-27479.140628878631</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-11512.902075623842</c:v>
+                  <c:v>-18576.101123217755</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-9496.9275082166223</c:v>
+                  <c:v>-12334.925672142715</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-6028.6940611282835</c:v>
+                  <c:v>-6594.7830785775623</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2180,52 +2180,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>203324.64541775131</c:v>
+                  <c:v>234484.12029553554</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>142517.32455685426</c:v>
+                  <c:v>163173.86739175185</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>124325.88693031289</c:v>
+                  <c:v>133156.32309972768</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90430.410916924244</c:v>
+                  <c:v>114321.67152989602</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>73084.441583464475</c:v>
+                  <c:v>99000.049567582799</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>61533.430640663515</c:v>
+                  <c:v>87233.488605604201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>74044.458827794922</c:v>
+                  <c:v>80038.973435362466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43647.172872749325</c:v>
+                  <c:v>71997.696512421899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>58960.6802707362</c:v>
+                  <c:v>65881.136053851194</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40119.832401277803</c:v>
+                  <c:v>56375.674465783348</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24318.165076374728</c:v>
+                  <c:v>47786.56286470851</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30874.570169486131</c:v>
+                  <c:v>38751.396319462903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25994.838038336002</c:v>
+                  <c:v>32112.4572883867</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18188.290291429978</c:v>
+                  <c:v>23809.872215759977</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11968.314355555985</c:v>
+                  <c:v>15544.560996940714</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4496.1121070609634</c:v>
+                  <c:v>7569.8454502498134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2487,7 +2487,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3183,7 +3182,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3311,7 +3309,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4000,7 +3997,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4122,7 +4118,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5608,7 +5603,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8221,8 +8215,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AI245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L103" sqref="L103"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8386,18 +8380,18 @@
         <v>6</v>
       </c>
       <c r="B6" s="54">
-        <v>152.10042167838168</v>
+        <v>232.1932206268018</v>
       </c>
       <c r="C6" s="54">
-        <v>203.3246454177513</v>
+        <v>234.48412029553555</v>
       </c>
       <c r="D6" s="51">
         <f>B6*1000</f>
-        <v>152100.42167838168</v>
+        <v>232193.22062680181</v>
       </c>
       <c r="E6" s="51">
         <f>C6*1000</f>
-        <v>203324.64541775131</v>
+        <v>234484.12029553554</v>
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="56"/>
@@ -8409,18 +8403,18 @@
         <v>9</v>
       </c>
       <c r="B7" s="54">
-        <v>106.61248230402569</v>
+        <v>159.98119086849147</v>
       </c>
       <c r="C7" s="54">
-        <v>142.51732455685425</v>
+        <v>163.17386739175186</v>
       </c>
       <c r="D7" s="51">
         <f t="shared" ref="D7:D21" si="0">B7*1000</f>
-        <v>106612.48230402569</v>
+        <v>159981.19086849148</v>
       </c>
       <c r="E7" s="51">
         <f t="shared" ref="E7:E21" si="1">C7*1000</f>
-        <v>142517.32455685426</v>
+        <v>163173.86739175185</v>
       </c>
       <c r="F7" s="56"/>
       <c r="G7" s="56"/>
@@ -8432,18 +8426,18 @@
         <v>12</v>
       </c>
       <c r="B8" s="54">
-        <v>107.40594202558786</v>
+        <v>130.60416798656604</v>
       </c>
       <c r="C8" s="54">
-        <v>124.32588693031289</v>
+        <v>133.15632309972767</v>
       </c>
       <c r="D8" s="51">
         <f t="shared" si="0"/>
-        <v>107405.94202558786</v>
+        <v>130604.16798656604</v>
       </c>
       <c r="E8" s="51">
         <f t="shared" si="1"/>
-        <v>124325.88693031289</v>
+        <v>133156.32309972768</v>
       </c>
       <c r="F8" s="56"/>
       <c r="G8" s="56"/>
@@ -8455,18 +8449,18 @@
         <v>13</v>
       </c>
       <c r="B9" s="54">
-        <v>101.51715463011743</v>
+        <v>116.66380924930885</v>
       </c>
       <c r="C9" s="54">
-        <v>90.430410916924245</v>
+        <v>114.32167152989602</v>
       </c>
       <c r="D9" s="51">
         <f t="shared" si="0"/>
-        <v>101517.15463011744</v>
+        <v>116663.80924930885</v>
       </c>
       <c r="E9" s="51">
         <f t="shared" si="1"/>
-        <v>90430.410916924244</v>
+        <v>114321.67152989602</v>
       </c>
       <c r="F9" s="56"/>
       <c r="G9" s="56"/>
@@ -8478,18 +8472,18 @@
         <v>14</v>
       </c>
       <c r="B10" s="54">
-        <v>72.544531411124765</v>
+        <v>105.38452275663238</v>
       </c>
       <c r="C10" s="54">
-        <v>73.084441583464468</v>
+        <v>99.000049567582792</v>
       </c>
       <c r="D10" s="51">
         <f t="shared" si="0"/>
-        <v>72544.531411124772</v>
+        <v>105384.52275663237</v>
       </c>
       <c r="E10" s="51">
         <f t="shared" si="1"/>
-        <v>73084.441583464475</v>
+        <v>99000.049567582799</v>
       </c>
       <c r="F10" s="56"/>
       <c r="G10" s="56"/>
@@ -8501,18 +8495,18 @@
         <v>15</v>
       </c>
       <c r="B11" s="54">
-        <v>64.144510344209692</v>
+        <v>95.487192629204486</v>
       </c>
       <c r="C11" s="54">
-        <v>61.533430640663518</v>
+        <v>87.233488605604208</v>
       </c>
       <c r="D11" s="51">
         <f t="shared" si="0"/>
-        <v>64144.510344209695</v>
+        <v>95487.192629204481</v>
       </c>
       <c r="E11" s="51">
         <f t="shared" si="1"/>
-        <v>61533.430640663515</v>
+        <v>87233.488605604201</v>
       </c>
       <c r="F11" s="56"/>
       <c r="G11" s="56"/>
@@ -8524,18 +8518,18 @@
         <v>16</v>
       </c>
       <c r="B12" s="54">
-        <v>52.521552285925161</v>
+        <v>88.295901522314608</v>
       </c>
       <c r="C12" s="54">
-        <v>74.044458827794926</v>
+        <v>80.038973435362465</v>
       </c>
       <c r="D12" s="51">
         <f t="shared" si="0"/>
-        <v>52521.552285925158</v>
+        <v>88295.901522314613</v>
       </c>
       <c r="E12" s="51">
         <f t="shared" si="1"/>
-        <v>74044.458827794922</v>
+        <v>80038.973435362466</v>
       </c>
       <c r="F12" s="56"/>
       <c r="G12" s="56"/>
@@ -8547,18 +8541,18 @@
         <v>17</v>
       </c>
       <c r="B13" s="54">
-        <v>43.004669296258498</v>
+        <v>81.236378677701538</v>
       </c>
       <c r="C13" s="54">
-        <v>43.647172872749323</v>
+        <v>71.997696512421896</v>
       </c>
       <c r="D13" s="51">
         <f t="shared" si="0"/>
-        <v>43004.6692962585</v>
+        <v>81236.378677701534</v>
       </c>
       <c r="E13" s="51">
         <f t="shared" si="1"/>
-        <v>43647.172872749325</v>
+        <v>71997.696512421899</v>
       </c>
       <c r="F13" s="56"/>
       <c r="G13" s="56"/>
@@ -8570,18 +8564,18 @@
         <v>19</v>
       </c>
       <c r="B14" s="54">
-        <v>62.73338681943445</v>
+        <v>73.180407288058333</v>
       </c>
       <c r="C14" s="54">
-        <v>58.960680270736198</v>
+        <v>65.881136053851193</v>
       </c>
       <c r="D14" s="51">
         <f t="shared" si="0"/>
-        <v>62733.386819434447</v>
+        <v>73180.407288058326</v>
       </c>
       <c r="E14" s="51">
         <f t="shared" si="1"/>
-        <v>58960.6802707362</v>
+        <v>65881.136053851194</v>
       </c>
       <c r="F14" s="56"/>
       <c r="G14" s="56"/>
@@ -8593,18 +8587,18 @@
         <v>20</v>
       </c>
       <c r="B15" s="54">
-        <v>35.212241466369449</v>
+        <v>62.269527941188258</v>
       </c>
       <c r="C15" s="54">
-        <v>40.119832401277804</v>
+        <v>56.375674465783348</v>
       </c>
       <c r="D15" s="51">
         <f t="shared" si="0"/>
-        <v>35212.241466369451</v>
+        <v>62269.527941188258</v>
       </c>
       <c r="E15" s="51">
         <f t="shared" si="1"/>
-        <v>40119.832401277803</v>
+        <v>56375.674465783348</v>
       </c>
       <c r="F15" s="56"/>
       <c r="G15" s="56"/>
@@ -8616,18 +8610,18 @@
         <v>21</v>
       </c>
       <c r="B16" s="54">
-        <v>35.474307358708501</v>
+        <v>49.094741236225531</v>
       </c>
       <c r="C16" s="54">
-        <v>24.318165076374729</v>
+        <v>47.786562864708507</v>
       </c>
       <c r="D16" s="51">
         <f t="shared" si="0"/>
-        <v>35474.307358708502</v>
+        <v>49094.741236225527</v>
       </c>
       <c r="E16" s="51">
         <f t="shared" si="1"/>
-        <v>24318.165076374728</v>
+        <v>47786.56286470851</v>
       </c>
       <c r="F16" s="56"/>
       <c r="G16" s="56"/>
@@ -8639,18 +8633,18 @@
         <v>22</v>
       </c>
       <c r="B17" s="54">
-        <v>24.318165076374729</v>
+        <v>38.060556537016609</v>
       </c>
       <c r="C17" s="54">
-        <v>30.87457016948613</v>
+        <v>38.751396319462906</v>
       </c>
       <c r="D17" s="51">
         <f t="shared" si="0"/>
-        <v>24318.165076374728</v>
+        <v>38060.556537016608</v>
       </c>
       <c r="E17" s="51">
         <f t="shared" si="1"/>
-        <v>30874.570169486131</v>
+        <v>38751.396319462903</v>
       </c>
       <c r="F17" s="56"/>
       <c r="G17" s="56"/>
@@ -8662,18 +8656,18 @@
         <v>42</v>
       </c>
       <c r="B18" s="54">
-        <v>19.243353103262908</v>
+        <v>27.479140628878632</v>
       </c>
       <c r="C18" s="54">
-        <v>25.994838038336002</v>
+        <v>32.1124572883867</v>
       </c>
       <c r="D18" s="51">
         <f t="shared" si="0"/>
-        <v>19243.353103262907</v>
+        <v>27479.140628878631</v>
       </c>
       <c r="E18" s="51">
         <f t="shared" si="1"/>
-        <v>25994.838038336002</v>
+        <v>32112.4572883867</v>
       </c>
       <c r="F18" s="56"/>
       <c r="G18" s="56"/>
@@ -8685,18 +8679,18 @@
         <v>43</v>
       </c>
       <c r="B19" s="54">
-        <v>11.512902075623842</v>
+        <v>18.576101123217754</v>
       </c>
       <c r="C19" s="54">
-        <v>18.188290291429979</v>
+        <v>23.809872215759977</v>
       </c>
       <c r="D19" s="51">
         <f t="shared" si="0"/>
-        <v>11512.902075623842</v>
+        <v>18576.101123217755</v>
       </c>
       <c r="E19" s="51">
         <f t="shared" si="1"/>
-        <v>18188.290291429978</v>
+        <v>23809.872215759977</v>
       </c>
       <c r="F19" s="56"/>
       <c r="G19" s="56"/>
@@ -8708,18 +8702,18 @@
         <v>44</v>
       </c>
       <c r="B20" s="54">
-        <v>9.496927508216622</v>
+        <v>12.334925672142715</v>
       </c>
       <c r="C20" s="54">
-        <v>11.968314355555986</v>
+        <v>15.544560996940714</v>
       </c>
       <c r="D20" s="51">
         <f t="shared" si="0"/>
-        <v>9496.9275082166223</v>
+        <v>12334.925672142715</v>
       </c>
       <c r="E20" s="51">
         <f t="shared" si="1"/>
-        <v>11968.314355555985</v>
+        <v>15544.560996940714</v>
       </c>
       <c r="F20" s="56"/>
       <c r="G20" s="56"/>
@@ -8731,18 +8725,18 @@
         <v>45</v>
       </c>
       <c r="B21" s="54">
-        <v>6.0286940611282835</v>
+        <v>6.5947830785775619</v>
       </c>
       <c r="C21" s="54">
-        <v>4.4961121070609638</v>
+        <v>7.5698454502498134</v>
       </c>
       <c r="D21" s="51">
         <f t="shared" si="0"/>
-        <v>6028.6940611282835</v>
+        <v>6594.7830785775623</v>
       </c>
       <c r="E21" s="51">
         <f t="shared" si="1"/>
-        <v>4496.1121070609634</v>
+        <v>7569.8454502498134</v>
       </c>
       <c r="F21" s="56"/>
       <c r="G21" s="56"/>
@@ -8755,23 +8749,23 @@
       </c>
       <c r="B22" s="9">
         <f>SUM(B6:B21)</f>
-        <v>903.87124144474967</v>
+        <v>1297.4365678223264</v>
       </c>
       <c r="C22" s="9">
         <f>SUM(C6:C21)</f>
-        <v>1027.8285744567727</v>
+        <v>1271.2376960930251</v>
       </c>
       <c r="D22" s="9">
         <f>SUM(D6:D21)</f>
-        <v>903871.24144474964</v>
+        <v>1297436.5678223267</v>
       </c>
       <c r="E22" s="9">
         <f>SUM(E6:E21)</f>
-        <v>1027828.5744567729</v>
+        <v>1271237.6960930256</v>
       </c>
       <c r="F22" s="57">
         <f>D22+E22</f>
-        <v>1931699.8159015225</v>
+        <v>2568674.2639153525</v>
       </c>
       <c r="G22" s="25"/>
       <c r="X22" s="13"/>
@@ -8811,11 +8805,11 @@
       </c>
       <c r="B29" s="58">
         <f>(-1)*D6</f>
-        <v>-152100.42167838168</v>
+        <v>-232193.22062680181</v>
       </c>
       <c r="C29" s="17">
         <f>E6</f>
-        <v>203324.64541775131</v>
+        <v>234484.12029553554</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -8824,11 +8818,11 @@
       </c>
       <c r="B30" s="58">
         <f t="shared" ref="B30:B44" si="2">(-1)*D7</f>
-        <v>-106612.48230402569</v>
+        <v>-159981.19086849148</v>
       </c>
       <c r="C30" s="17">
         <f t="shared" ref="C30:C44" si="3">E7</f>
-        <v>142517.32455685426</v>
+        <v>163173.86739175185</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -8837,11 +8831,11 @@
       </c>
       <c r="B31" s="58">
         <f t="shared" si="2"/>
-        <v>-107405.94202558786</v>
+        <v>-130604.16798656604</v>
       </c>
       <c r="C31" s="17">
         <f t="shared" si="3"/>
-        <v>124325.88693031289</v>
+        <v>133156.32309972768</v>
       </c>
       <c r="L31" s="8"/>
     </row>
@@ -8851,11 +8845,11 @@
       </c>
       <c r="B32" s="58">
         <f t="shared" si="2"/>
-        <v>-101517.15463011744</v>
+        <v>-116663.80924930885</v>
       </c>
       <c r="C32" s="17">
         <f t="shared" si="3"/>
-        <v>90430.410916924244</v>
+        <v>114321.67152989602</v>
       </c>
     </row>
     <row r="33" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
@@ -8864,11 +8858,11 @@
       </c>
       <c r="B33" s="58">
         <f t="shared" si="2"/>
-        <v>-72544.531411124772</v>
+        <v>-105384.52275663237</v>
       </c>
       <c r="C33" s="17">
         <f t="shared" si="3"/>
-        <v>73084.441583464475</v>
+        <v>99000.049567582799</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
@@ -8877,11 +8871,11 @@
       </c>
       <c r="B34" s="58">
         <f t="shared" si="2"/>
-        <v>-64144.510344209695</v>
+        <v>-95487.192629204481</v>
       </c>
       <c r="C34" s="17">
         <f t="shared" si="3"/>
-        <v>61533.430640663515</v>
+        <v>87233.488605604201</v>
       </c>
     </row>
     <row r="35" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
@@ -8890,11 +8884,11 @@
       </c>
       <c r="B35" s="58">
         <f t="shared" si="2"/>
-        <v>-52521.552285925158</v>
+        <v>-88295.901522314613</v>
       </c>
       <c r="C35" s="17">
         <f t="shared" si="3"/>
-        <v>74044.458827794922</v>
+        <v>80038.973435362466</v>
       </c>
     </row>
     <row r="36" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
@@ -8903,11 +8897,11 @@
       </c>
       <c r="B36" s="58">
         <f t="shared" si="2"/>
-        <v>-43004.6692962585</v>
+        <v>-81236.378677701534</v>
       </c>
       <c r="C36" s="17">
         <f t="shared" si="3"/>
-        <v>43647.172872749325</v>
+        <v>71997.696512421899</v>
       </c>
       <c r="X36" s="13"/>
       <c r="Y36" s="13"/>
@@ -8925,11 +8919,11 @@
       </c>
       <c r="B37" s="58">
         <f t="shared" si="2"/>
-        <v>-62733.386819434447</v>
+        <v>-73180.407288058326</v>
       </c>
       <c r="C37" s="17">
         <f t="shared" si="3"/>
-        <v>58960.6802707362</v>
+        <v>65881.136053851194</v>
       </c>
       <c r="X37" s="14"/>
       <c r="Y37" s="14"/>
@@ -8946,11 +8940,11 @@
       </c>
       <c r="B38" s="58">
         <f t="shared" si="2"/>
-        <v>-35212.241466369451</v>
+        <v>-62269.527941188258</v>
       </c>
       <c r="C38" s="17">
         <f t="shared" si="3"/>
-        <v>40119.832401277803</v>
+        <v>56375.674465783348</v>
       </c>
       <c r="X38" s="22"/>
       <c r="Y38" s="22"/>
@@ -8967,11 +8961,11 @@
       </c>
       <c r="B39" s="58">
         <f t="shared" si="2"/>
-        <v>-35474.307358708502</v>
+        <v>-49094.741236225527</v>
       </c>
       <c r="C39" s="17">
         <f t="shared" si="3"/>
-        <v>24318.165076374728</v>
+        <v>47786.56286470851</v>
       </c>
       <c r="X39" s="23"/>
       <c r="Y39" s="23"/>
@@ -8988,11 +8982,11 @@
       </c>
       <c r="B40" s="58">
         <f t="shared" si="2"/>
-        <v>-24318.165076374728</v>
+        <v>-38060.556537016608</v>
       </c>
       <c r="C40" s="17">
         <f t="shared" si="3"/>
-        <v>30874.570169486131</v>
+        <v>38751.396319462903</v>
       </c>
       <c r="X40" s="23"/>
       <c r="Y40" s="23"/>
@@ -9009,11 +9003,11 @@
       </c>
       <c r="B41" s="58">
         <f t="shared" si="2"/>
-        <v>-19243.353103262907</v>
+        <v>-27479.140628878631</v>
       </c>
       <c r="C41" s="17">
         <f t="shared" si="3"/>
-        <v>25994.838038336002</v>
+        <v>32112.4572883867</v>
       </c>
       <c r="X41" s="23"/>
       <c r="Y41" s="23"/>
@@ -9030,11 +9024,11 @@
       </c>
       <c r="B42" s="58">
         <f t="shared" si="2"/>
-        <v>-11512.902075623842</v>
+        <v>-18576.101123217755</v>
       </c>
       <c r="C42" s="17">
         <f t="shared" si="3"/>
-        <v>18188.290291429978</v>
+        <v>23809.872215759977</v>
       </c>
       <c r="X42" s="24"/>
       <c r="Y42" s="24"/>
@@ -9051,11 +9045,11 @@
       </c>
       <c r="B43" s="58">
         <f t="shared" si="2"/>
-        <v>-9496.9275082166223</v>
+        <v>-12334.925672142715</v>
       </c>
       <c r="C43" s="17">
         <f t="shared" si="3"/>
-        <v>11968.314355555985</v>
+        <v>15544.560996940714</v>
       </c>
       <c r="X43" s="24"/>
       <c r="Y43" s="24"/>
@@ -9072,11 +9066,11 @@
       </c>
       <c r="B44" s="58">
         <f t="shared" si="2"/>
-        <v>-6028.6940611282835</v>
+        <v>-6594.7830785775623</v>
       </c>
       <c r="C44" s="17">
         <f t="shared" si="3"/>
-        <v>4496.1121070609634</v>
+        <v>7569.8454502498134</v>
       </c>
       <c r="X44" s="24"/>
       <c r="Y44" s="24"/>

</xml_diff>

<commit_message>
Update GDB Results Tool citation
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -495,10 +495,10 @@
     </r>
   </si>
   <si>
-    <t>UN World Population Prospects 2019, File MORT/17-2: Abridged life tables, for males/females, 1950-2100; GHDx GBD Results Tool</t>
+    <t>Used UN values from 1950-1990 before the widespread HIV epidemic. Used the GHDx GBD Results Tool to subtract HIV-specific mortality from all-cause mortality after 1990. Smoothed over the trough in the 1990s and made the decline in under 5 mortality a little less severe. Extrapolated the trend between 2000 and 2017 to 2020.</t>
   </si>
   <si>
-    <t>Used UN values from 1950-1990 before the widespread HIV epidemic. Used the GHDx GBD Results Tool to subtract HIV-specific mortality from all-cause mortality after 1990. Smoothed over the trough in the 1990s and made the decline in under 5 mortality a little less severe. Extrapolated the trend between 2000 and 2017 to 2020.</t>
+    <t>UN World Population Prospects 2019, File MORT/17-2: Abridged life tables, for males/females, 1950-2100; GHDx GBD Results Tool: Global Burden of Disease Collaborative Network, Global Burden of Disease Study 2017 (GBD 2017) Results. Seattle, United States: Institute for Health Metrics and Evaluation (IHME), 2018. Available from http://ghdx.healthdata.org/gbd-results-tool. Accessed Feb 21, 2020.</t>
   </si>
 </sst>
 </file>
@@ -958,7 +958,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1365,6 +1365,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1422,7 +1431,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1646,60 +1655,6 @@
     <xf numFmtId="11" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1721,6 +1676,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1733,12 +1691,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -2487,6 +2499,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3182,6 +3195,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3309,6 +3323,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3997,6 +4012,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8215,8 +8231,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AI245"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C21"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O207" sqref="O207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8288,16 +8304,16 @@
       <c r="Y1" s="37"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -8349,14 +8365,14 @@
       <c r="A4" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="109" t="s">
+      <c r="B4" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="109" t="s">
+      <c r="C4" s="112"/>
+      <c r="D4" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="110"/>
+      <c r="E4" s="112"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -8784,10 +8800,10 @@
       <c r="A27" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="109" t="s">
+      <c r="B27" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="110"/>
+      <c r="C27" s="112"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -9202,19 +9218,19 @@
       <c r="AE51" s="24"/>
     </row>
     <row r="52" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="128" t="s">
+      <c r="A52" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="128" t="s">
+      <c r="B52" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="128"/>
-      <c r="D52" s="128"/>
-      <c r="E52" s="128" t="s">
+      <c r="C52" s="113"/>
+      <c r="D52" s="113"/>
+      <c r="E52" s="113" t="s">
         <v>57</v>
       </c>
-      <c r="F52" s="128"/>
-      <c r="G52" s="128"/>
+      <c r="F52" s="113"/>
+      <c r="G52" s="113"/>
       <c r="X52" s="22"/>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
@@ -9225,7 +9241,7 @@
       <c r="AE52" s="22"/>
     </row>
     <row r="53" spans="1:31" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="128"/>
+      <c r="A53" s="113"/>
       <c r="B53" s="33" t="s">
         <v>3</v>
       </c>
@@ -9704,7 +9720,7 @@
     </row>
     <row r="79" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="38" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B79" s="37"/>
       <c r="C79" s="37"/>
@@ -9732,7 +9748,7 @@
     </row>
     <row r="80" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B80" s="37"/>
       <c r="C80" s="37"/>
@@ -9759,91 +9775,91 @@
       <c r="X80" s="37"/>
     </row>
     <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="101" t="s">
+      <c r="A81" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="104" t="s">
+      <c r="B81" s="119" t="s">
         <v>80</v>
       </c>
-      <c r="C81" s="104"/>
-      <c r="D81" s="104"/>
-      <c r="E81" s="104"/>
-      <c r="F81" s="104"/>
-      <c r="G81" s="104"/>
-      <c r="H81" s="104"/>
-      <c r="I81" s="104"/>
-      <c r="J81" s="104"/>
-      <c r="K81" s="104"/>
-      <c r="L81" s="104"/>
-      <c r="N81" s="101" t="s">
+      <c r="C81" s="119"/>
+      <c r="D81" s="119"/>
+      <c r="E81" s="119"/>
+      <c r="F81" s="119"/>
+      <c r="G81" s="119"/>
+      <c r="H81" s="119"/>
+      <c r="I81" s="119"/>
+      <c r="J81" s="119"/>
+      <c r="K81" s="119"/>
+      <c r="L81" s="119"/>
+      <c r="N81" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="O81" s="104" t="s">
+      <c r="O81" s="119" t="s">
         <v>81</v>
       </c>
-      <c r="P81" s="104"/>
-      <c r="Q81" s="104"/>
-      <c r="R81" s="104"/>
-      <c r="S81" s="104"/>
-      <c r="T81" s="104"/>
-      <c r="U81" s="104"/>
-      <c r="V81" s="104"/>
-      <c r="W81" s="104"/>
-      <c r="X81" s="104"/>
-      <c r="Y81" s="104"/>
-      <c r="AA81" s="105" t="s">
+      <c r="P81" s="119"/>
+      <c r="Q81" s="119"/>
+      <c r="R81" s="119"/>
+      <c r="S81" s="119"/>
+      <c r="T81" s="119"/>
+      <c r="U81" s="119"/>
+      <c r="V81" s="119"/>
+      <c r="W81" s="119"/>
+      <c r="X81" s="119"/>
+      <c r="Y81" s="119"/>
+      <c r="AA81" s="127" t="s">
         <v>82</v>
       </c>
-      <c r="AB81" s="106"/>
-      <c r="AC81" s="106"/>
-      <c r="AD81" s="106"/>
-      <c r="AE81" s="106"/>
-      <c r="AF81" s="106"/>
-      <c r="AG81" s="106"/>
-      <c r="AH81" s="106"/>
-      <c r="AI81" s="107"/>
+      <c r="AB81" s="128"/>
+      <c r="AC81" s="128"/>
+      <c r="AD81" s="128"/>
+      <c r="AE81" s="128"/>
+      <c r="AF81" s="128"/>
+      <c r="AG81" s="128"/>
+      <c r="AH81" s="128"/>
+      <c r="AI81" s="129"/>
     </row>
     <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="102"/>
-      <c r="B82" s="104"/>
-      <c r="C82" s="104"/>
-      <c r="D82" s="104"/>
-      <c r="E82" s="104"/>
-      <c r="F82" s="104"/>
-      <c r="G82" s="104"/>
-      <c r="H82" s="104"/>
-      <c r="I82" s="104"/>
-      <c r="J82" s="104"/>
-      <c r="K82" s="104"/>
-      <c r="L82" s="104"/>
-      <c r="N82" s="102"/>
-      <c r="O82" s="104"/>
-      <c r="P82" s="104"/>
-      <c r="Q82" s="104"/>
-      <c r="R82" s="104"/>
-      <c r="S82" s="104"/>
-      <c r="T82" s="104"/>
-      <c r="U82" s="104"/>
-      <c r="V82" s="104"/>
-      <c r="W82" s="104"/>
-      <c r="X82" s="104"/>
-      <c r="Y82" s="104"/>
-      <c r="AA82" s="99" t="s">
+      <c r="A82" s="115"/>
+      <c r="B82" s="119"/>
+      <c r="C82" s="119"/>
+      <c r="D82" s="119"/>
+      <c r="E82" s="119"/>
+      <c r="F82" s="119"/>
+      <c r="G82" s="119"/>
+      <c r="H82" s="119"/>
+      <c r="I82" s="119"/>
+      <c r="J82" s="119"/>
+      <c r="K82" s="119"/>
+      <c r="L82" s="119"/>
+      <c r="N82" s="115"/>
+      <c r="O82" s="119"/>
+      <c r="P82" s="119"/>
+      <c r="Q82" s="119"/>
+      <c r="R82" s="119"/>
+      <c r="S82" s="119"/>
+      <c r="T82" s="119"/>
+      <c r="U82" s="119"/>
+      <c r="V82" s="119"/>
+      <c r="W82" s="119"/>
+      <c r="X82" s="119"/>
+      <c r="Y82" s="119"/>
+      <c r="AA82" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="AB82" s="105" t="s">
+      <c r="AB82" s="127" t="s">
         <v>74</v>
       </c>
-      <c r="AC82" s="106"/>
-      <c r="AD82" s="106"/>
-      <c r="AE82" s="106"/>
-      <c r="AF82" s="106"/>
-      <c r="AG82" s="106"/>
-      <c r="AH82" s="106"/>
-      <c r="AI82" s="107"/>
+      <c r="AC82" s="128"/>
+      <c r="AD82" s="128"/>
+      <c r="AE82" s="128"/>
+      <c r="AF82" s="128"/>
+      <c r="AG82" s="128"/>
+      <c r="AH82" s="128"/>
+      <c r="AI82" s="129"/>
     </row>
     <row r="83" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="103"/>
+      <c r="A83" s="116"/>
       <c r="B83" s="76" t="s">
         <v>95</v>
       </c>
@@ -9877,7 +9893,7 @@
       <c r="L83" s="89">
         <v>2020</v>
       </c>
-      <c r="N83" s="103"/>
+      <c r="N83" s="116"/>
       <c r="O83" s="76" t="s">
         <v>95</v>
       </c>
@@ -9911,7 +9927,7 @@
       <c r="Y83" s="89">
         <v>2020</v>
       </c>
-      <c r="AA83" s="100"/>
+      <c r="AA83" s="126"/>
       <c r="AB83" s="76" t="s">
         <v>95</v>
       </c>
@@ -10351,19 +10367,19 @@
         <f t="shared" si="12"/>
         <v>-6.3054823529411761E-5</v>
       </c>
-      <c r="AA87" s="99" t="s">
+      <c r="AA87" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="AB87" s="105" t="s">
+      <c r="AB87" s="127" t="s">
         <v>75</v>
       </c>
-      <c r="AC87" s="106"/>
-      <c r="AD87" s="106"/>
-      <c r="AE87" s="106"/>
-      <c r="AF87" s="106"/>
-      <c r="AG87" s="106"/>
-      <c r="AH87" s="106"/>
-      <c r="AI87" s="107"/>
+      <c r="AC87" s="128"/>
+      <c r="AD87" s="128"/>
+      <c r="AE87" s="128"/>
+      <c r="AF87" s="128"/>
+      <c r="AG87" s="128"/>
+      <c r="AH87" s="128"/>
+      <c r="AI87" s="129"/>
     </row>
     <row r="88" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="74" t="s">
@@ -10448,7 +10464,7 @@
         <f t="shared" si="12"/>
         <v>-1.4261617647058823E-4</v>
       </c>
-      <c r="AA88" s="100"/>
+      <c r="AA88" s="126"/>
       <c r="AB88" s="76" t="s">
         <v>95</v>
       </c>
@@ -11637,25 +11653,25 @@
       <c r="X110" s="37"/>
     </row>
     <row r="111" spans="1:26" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="116" t="s">
+      <c r="A111" s="124" t="s">
         <v>104</v>
       </c>
-      <c r="B111" s="116"/>
-      <c r="C111" s="116"/>
-      <c r="D111" s="116"/>
-      <c r="E111" s="116"/>
-      <c r="F111" s="116"/>
-      <c r="G111" s="116"/>
-      <c r="H111" s="116"/>
-      <c r="I111" s="116"/>
-      <c r="J111" s="116"/>
-      <c r="K111" s="116"/>
-      <c r="L111" s="116"/>
-      <c r="M111" s="116"/>
-      <c r="N111" s="116"/>
-      <c r="O111" s="116"/>
-      <c r="P111" s="116"/>
-      <c r="Q111" s="116"/>
+      <c r="B111" s="124"/>
+      <c r="C111" s="124"/>
+      <c r="D111" s="124"/>
+      <c r="E111" s="124"/>
+      <c r="F111" s="124"/>
+      <c r="G111" s="124"/>
+      <c r="H111" s="124"/>
+      <c r="I111" s="124"/>
+      <c r="J111" s="124"/>
+      <c r="K111" s="124"/>
+      <c r="L111" s="124"/>
+      <c r="M111" s="124"/>
+      <c r="N111" s="124"/>
+      <c r="O111" s="124"/>
+      <c r="P111" s="124"/>
+      <c r="Q111" s="124"/>
       <c r="R111" s="37"/>
       <c r="S111" s="37"/>
       <c r="T111" s="37"/>
@@ -11665,17 +11681,17 @@
       <c r="X111" s="37"/>
     </row>
     <row r="112" spans="1:26" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="125" t="s">
+      <c r="A112" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="121" t="s">
+      <c r="B112" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="C112" s="122"/>
-      <c r="D112" s="122"/>
-      <c r="E112" s="122"/>
-      <c r="F112" s="122"/>
-      <c r="G112" s="123"/>
+      <c r="C112" s="104"/>
+      <c r="D112" s="104"/>
+      <c r="E112" s="104"/>
+      <c r="F112" s="104"/>
+      <c r="G112" s="105"/>
       <c r="I112" s="73"/>
       <c r="J112" s="86" t="s">
         <v>27</v>
@@ -11694,7 +11710,7 @@
       </c>
     </row>
     <row r="113" spans="1:14" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="126"/>
+      <c r="A113" s="109"/>
       <c r="B113" s="32" t="s">
         <v>70</v>
       </c>
@@ -11738,7 +11754,7 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="127"/>
+      <c r="A114" s="110"/>
       <c r="B114" s="34" t="s">
         <v>63</v>
       </c>
@@ -11786,14 +11802,14 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="I115" s="129" t="s">
+      <c r="I115" s="117" t="s">
         <v>103</v>
       </c>
-      <c r="J115" s="129"/>
-      <c r="K115" s="129"/>
-      <c r="L115" s="129"/>
-      <c r="M115" s="129"/>
-      <c r="N115" s="129"/>
+      <c r="J115" s="117"/>
+      <c r="K115" s="117"/>
+      <c r="L115" s="117"/>
+      <c r="M115" s="117"/>
+      <c r="N115" s="117"/>
     </row>
     <row r="116" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
@@ -12546,31 +12562,31 @@
     </row>
     <row r="132" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="133" spans="1:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="118" t="s">
+      <c r="A133" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="121" t="s">
+      <c r="B133" s="103" t="s">
         <v>86</v>
       </c>
-      <c r="C133" s="122"/>
-      <c r="D133" s="122"/>
-      <c r="E133" s="122"/>
-      <c r="F133" s="122"/>
-      <c r="G133" s="123"/>
-      <c r="I133" s="118" t="s">
+      <c r="C133" s="104"/>
+      <c r="D133" s="104"/>
+      <c r="E133" s="104"/>
+      <c r="F133" s="104"/>
+      <c r="G133" s="105"/>
+      <c r="I133" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="J133" s="121" t="s">
+      <c r="J133" s="103" t="s">
         <v>76</v>
       </c>
-      <c r="K133" s="122"/>
-      <c r="L133" s="122"/>
-      <c r="M133" s="122"/>
-      <c r="N133" s="122"/>
-      <c r="O133" s="123"/>
+      <c r="K133" s="104"/>
+      <c r="L133" s="104"/>
+      <c r="M133" s="104"/>
+      <c r="N133" s="104"/>
+      <c r="O133" s="105"/>
     </row>
     <row r="134" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="119"/>
+      <c r="A134" s="101"/>
       <c r="B134" s="26" t="s">
         <v>71</v>
       </c>
@@ -12589,7 +12605,7 @@
       <c r="G134" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I134" s="119"/>
+      <c r="I134" s="101"/>
       <c r="J134" s="26" t="s">
         <v>71</v>
       </c>
@@ -12610,7 +12626,7 @@
       </c>
     </row>
     <row r="135" spans="1:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="120"/>
+      <c r="A135" s="102"/>
       <c r="B135" s="40" t="s">
         <v>63</v>
       </c>
@@ -12629,7 +12645,7 @@
       <c r="G135" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I135" s="120"/>
+      <c r="I135" s="102"/>
       <c r="J135" s="40" t="s">
         <v>63</v>
       </c>
@@ -13569,22 +13585,22 @@
       <c r="W160" s="37"/>
     </row>
     <row r="161" spans="1:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="104" t="s">
+      <c r="A161" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="B161" s="112" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="112"/>
-      <c r="D161" s="112"/>
-      <c r="E161" s="112" t="s">
+      <c r="B161" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="121"/>
+      <c r="D161" s="121"/>
+      <c r="E161" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="F161" s="112"/>
-      <c r="G161" s="112"/>
+      <c r="F161" s="121"/>
+      <c r="G161" s="121"/>
     </row>
     <row r="162" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="104"/>
+      <c r="A162" s="119"/>
       <c r="B162" s="63" t="s">
         <v>3</v>
       </c>
@@ -14380,9 +14396,9 @@
       <c r="AB185" s="20"/>
     </row>
     <row r="186" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="113"/>
-      <c r="B186" s="113"/>
-      <c r="C186" s="113"/>
+      <c r="A186" s="122"/>
+      <c r="B186" s="122"/>
+      <c r="C186" s="122"/>
       <c r="D186" s="20"/>
       <c r="E186" s="20"/>
       <c r="F186" s="20"/>
@@ -14557,39 +14573,39 @@
       <c r="W197" s="37"/>
     </row>
     <row r="198" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="109" t="s">
+      <c r="A198" s="111" t="s">
         <v>73</v>
       </c>
-      <c r="B198" s="109"/>
-      <c r="C198" s="109"/>
-      <c r="D198" s="109"/>
-      <c r="E198" s="109"/>
-      <c r="F198" s="109"/>
+      <c r="B198" s="111"/>
+      <c r="C198" s="111"/>
+      <c r="D198" s="111"/>
+      <c r="E198" s="111"/>
+      <c r="F198" s="111"/>
     </row>
     <row r="199" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="114" t="s">
+      <c r="A199" s="123" t="s">
         <v>74</v>
       </c>
-      <c r="B199" s="114"/>
-      <c r="C199" s="114"/>
-      <c r="D199" s="114"/>
-      <c r="E199" s="114"/>
-      <c r="F199" s="114"/>
+      <c r="B199" s="123"/>
+      <c r="C199" s="123"/>
+      <c r="D199" s="123"/>
+      <c r="E199" s="123"/>
+      <c r="F199" s="123"/>
     </row>
     <row r="200" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A200" s="115" t="s">
+      <c r="A200" s="106" t="s">
         <v>46</v>
       </c>
       <c r="B200" s="43"/>
       <c r="C200" s="43"/>
-      <c r="D200" s="115" t="s">
+      <c r="D200" s="106" t="s">
         <v>51</v>
       </c>
-      <c r="E200" s="115"/>
-      <c r="F200" s="115"/>
+      <c r="E200" s="106"/>
+      <c r="F200" s="106"/>
     </row>
     <row r="201" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A201" s="115"/>
+      <c r="A201" s="106"/>
       <c r="B201" s="43"/>
       <c r="C201" s="44" t="s">
         <v>47</v>
@@ -14603,10 +14619,6 @@
       <c r="F201" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="H201">
-        <f>(365.25/7)*2.4</f>
-        <v>125.22857142857143</v>
-      </c>
     </row>
     <row r="202" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A202" s="45" t="s">
@@ -14623,26 +14635,29 @@
       <c r="F202" s="64">
         <v>0</v>
       </c>
+      <c r="G202">
+        <v>1</v>
+      </c>
       <c r="H202">
-        <f t="shared" ref="H202:H217" si="27">D202*B54</f>
-        <v>0</v>
-      </c>
-      <c r="I202">
-        <f t="shared" ref="I202:I217" si="28">E202*C54</f>
-        <v>0</v>
-      </c>
-      <c r="J202">
-        <f t="shared" ref="J202:J217" si="29">F202*D54</f>
-        <v>0</v>
+        <f>D222*G202</f>
+        <v>0</v>
+      </c>
+      <c r="J202" t="e">
+        <f>D202/E202</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K202" t="e">
+        <f>E202/F202</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="N202" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="O202" s="108" t="s">
+      <c r="O202" s="118" t="s">
         <v>94</v>
       </c>
-      <c r="P202" s="108"/>
-      <c r="Q202" s="108"/>
+      <c r="P202" s="118"/>
+      <c r="Q202" s="118"/>
     </row>
     <row r="203" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="45" t="s">
@@ -14659,17 +14674,20 @@
       <c r="F203" s="64">
         <v>0</v>
       </c>
+      <c r="G203">
+        <v>1</v>
+      </c>
       <c r="H203">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="I203">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="J203">
-        <f t="shared" si="29"/>
-        <v>0</v>
+        <f t="shared" ref="H203:H217" si="27">D223*G203</f>
+        <v>0</v>
+      </c>
+      <c r="J203" t="e">
+        <f t="shared" ref="J203:J217" si="28">D203/E203</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K203" t="e">
+        <f t="shared" ref="K203:K217" si="29">E203/F203</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="N203" s="45" t="s">
         <v>25</v>
@@ -14701,21 +14719,21 @@
       <c r="F204" s="65">
         <v>1.1232</v>
       </c>
+      <c r="G204">
+        <f t="shared" ref="G203:G217" si="30">D204/D224</f>
+        <v>0.4</v>
+      </c>
       <c r="H204">
         <f t="shared" si="27"/>
-        <v>3.0575999999999999</v>
-      </c>
-      <c r="I204">
+        <v>3.12</v>
+      </c>
+      <c r="J204">
         <f t="shared" si="28"/>
-        <v>2.8080000000000001E-2</v>
-      </c>
-      <c r="J204">
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="K204">
         <f t="shared" si="29"/>
-        <v>5.6160000000000203E-3</v>
-      </c>
-      <c r="K204">
-        <f>SUM(H204:J204)</f>
-        <v>3.0912959999999998</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N204" s="45" t="s">
         <v>24</v>
@@ -14747,21 +14765,21 @@
       <c r="F205" s="65">
         <v>5.6159999999999997</v>
       </c>
+      <c r="G205">
+        <f t="shared" si="30"/>
+        <v>0.83333333333333337</v>
+      </c>
       <c r="H205">
         <f t="shared" si="27"/>
-        <v>7.9418181818181806</v>
-      </c>
-      <c r="I205">
+        <v>15.6</v>
+      </c>
+      <c r="J205">
         <f t="shared" si="28"/>
-        <v>3.814909090909091</v>
-      </c>
-      <c r="J205">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K205">
         <f t="shared" si="29"/>
-        <v>0.46799999999999986</v>
-      </c>
-      <c r="K205">
-        <f t="shared" ref="K205:K217" si="30">SUM(H205:J205)</f>
-        <v>12.224727272727272</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N205" s="45" t="s">
         <v>32</v>
@@ -14795,21 +14813,21 @@
       <c r="F206" s="64">
         <v>22.463999999999999</v>
       </c>
+      <c r="G206">
+        <f t="shared" si="30"/>
+        <v>0.83333333333333337</v>
+      </c>
       <c r="H206">
         <f t="shared" si="27"/>
-        <v>29.452100840336129</v>
-      </c>
-      <c r="I206">
+        <v>62.4</v>
+      </c>
+      <c r="J206">
         <f t="shared" si="28"/>
-        <v>16.570084033613444</v>
-      </c>
-      <c r="J206">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K206">
         <f t="shared" si="29"/>
-        <v>1.9191932773109244</v>
-      </c>
-      <c r="K206">
-        <f t="shared" si="30"/>
-        <v>47.941378151260494</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N206" s="45" t="s">
         <v>33</v>
@@ -14844,21 +14862,21 @@
       <c r="F207" s="65">
         <v>56.16</v>
       </c>
+      <c r="G207">
+        <f t="shared" si="30"/>
+        <v>1.1111111111111112</v>
+      </c>
       <c r="H207">
         <f t="shared" si="27"/>
-        <v>79.613793103448273</v>
-      </c>
-      <c r="I207">
+        <v>156</v>
+      </c>
+      <c r="J207">
         <f t="shared" si="28"/>
-        <v>38.515862068965518</v>
-      </c>
-      <c r="J207">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K207">
         <f t="shared" si="29"/>
-        <v>4.38951724137931</v>
-      </c>
-      <c r="K207">
-        <f t="shared" si="30"/>
-        <v>122.5191724137931</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N207" s="45" t="s">
         <v>34</v>
@@ -14896,21 +14914,21 @@
       <c r="F208" s="65">
         <v>39.711116831436499</v>
       </c>
+      <c r="G208">
+        <f t="shared" si="30"/>
+        <v>1.1111111111111065</v>
+      </c>
       <c r="H208">
         <f t="shared" si="27"/>
-        <v>66.683764924100601</v>
-      </c>
-      <c r="I208">
+        <v>110.308657865101</v>
+      </c>
+      <c r="J208">
         <f t="shared" si="28"/>
-        <v>22.622623053690308</v>
-      </c>
-      <c r="J208">
+        <v>1.666666666666659</v>
+      </c>
+      <c r="K208">
         <f t="shared" si="29"/>
-        <v>2.1313876265460268</v>
-      </c>
-      <c r="K208">
-        <f t="shared" si="30"/>
-        <v>91.437775604336935</v>
+        <v>1.6666666666666685</v>
       </c>
       <c r="M208" s="39"/>
       <c r="N208" s="45" t="s">
@@ -14949,21 +14967,21 @@
       <c r="F209" s="65">
         <v>28.08</v>
       </c>
+      <c r="G209">
+        <f t="shared" si="30"/>
+        <v>1.1111111111111112</v>
+      </c>
       <c r="H209">
         <f t="shared" si="27"/>
-        <v>59.710344827586205</v>
-      </c>
-      <c r="I209">
+        <v>78</v>
+      </c>
+      <c r="J209">
         <f t="shared" si="28"/>
-        <v>9.5213793103448268</v>
-      </c>
-      <c r="J209">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K209">
         <f t="shared" si="29"/>
-        <v>0.87144827586206886</v>
-      </c>
-      <c r="K209">
-        <f t="shared" si="30"/>
-        <v>70.103172413793089</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N209" s="45" t="s">
         <v>36</v>
@@ -15001,21 +15019,21 @@
       <c r="F210" s="65">
         <v>19.855558415718299</v>
       </c>
+      <c r="G210">
+        <f t="shared" si="30"/>
+        <v>1.1111111111111116</v>
+      </c>
       <c r="H210">
         <f t="shared" si="27"/>
-        <v>45.126269126632387</v>
-      </c>
-      <c r="I210">
+        <v>55.15432893255069</v>
+      </c>
+      <c r="J210">
         <f t="shared" si="28"/>
-        <v>5.5540023540470607</v>
-      </c>
-      <c r="J210">
+        <v>1.6666666666666676</v>
+      </c>
+      <c r="K210">
         <f t="shared" si="29"/>
-        <v>0.27770011770235381</v>
-      </c>
-      <c r="K210">
-        <f t="shared" si="30"/>
-        <v>50.957971598381803</v>
+        <v>1.6666666666666619</v>
       </c>
       <c r="N210" s="45" t="s">
         <v>37</v>
@@ -15053,21 +15071,21 @@
       <c r="F211" s="65">
         <v>14.04</v>
       </c>
+      <c r="G211">
+        <f t="shared" si="30"/>
+        <v>1.1111111111111112</v>
+      </c>
       <c r="H211">
         <f t="shared" si="27"/>
-        <v>33.179104477611936</v>
-      </c>
-      <c r="I211">
+        <v>39</v>
+      </c>
+      <c r="J211">
         <f t="shared" si="28"/>
-        <v>3.4691373134328458</v>
-      </c>
-      <c r="J211">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K211">
         <f t="shared" si="29"/>
-        <v>1.4039999999999999E-2</v>
-      </c>
-      <c r="K211">
-        <f t="shared" si="30"/>
-        <v>36.662281791044784</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N211" s="45" t="s">
         <v>38</v>
@@ -15105,21 +15123,21 @@
       <c r="F212" s="65">
         <v>9.92777920785913</v>
       </c>
+      <c r="G212">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
       <c r="H212">
         <f t="shared" si="27"/>
-        <v>23.461169769816379</v>
-      </c>
-      <c r="I212">
+        <v>27.577164466275399</v>
+      </c>
+      <c r="J212">
         <f t="shared" si="28"/>
-        <v>2.4530505191956449</v>
-      </c>
-      <c r="J212">
+        <v>1.6666666666666705</v>
+      </c>
+      <c r="K212">
         <f t="shared" si="29"/>
-        <v>9.9277792078591304E-3</v>
-      </c>
-      <c r="K212">
-        <f t="shared" si="30"/>
-        <v>25.924148068219885</v>
+        <v>1.666666666666665</v>
       </c>
       <c r="N212" s="45" t="s">
         <v>39</v>
@@ -15157,21 +15175,21 @@
       <c r="F213" s="65">
         <v>7.02</v>
       </c>
+      <c r="G213">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
       <c r="H213">
         <f t="shared" si="27"/>
-        <v>16.589552238805968</v>
-      </c>
-      <c r="I213">
+        <v>19.5</v>
+      </c>
+      <c r="J213">
         <f t="shared" si="28"/>
-        <v>1.7345686567164229</v>
-      </c>
-      <c r="J213">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K213">
         <f t="shared" si="29"/>
-        <v>7.0199999999999993E-3</v>
-      </c>
-      <c r="K213">
-        <f t="shared" si="30"/>
-        <v>18.331140895522392</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N213" s="45" t="s">
         <v>40</v>
@@ -15209,21 +15227,21 @@
       <c r="F214" s="65">
         <v>4.9638896039295597</v>
       </c>
+      <c r="G214">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
       <c r="H214">
         <f t="shared" si="27"/>
-        <v>11.73058488490819</v>
-      </c>
-      <c r="I214">
+        <v>13.788582233137699</v>
+      </c>
+      <c r="J214">
         <f t="shared" si="28"/>
-        <v>1.2265252595978238</v>
-      </c>
-      <c r="J214">
+        <v>1.6666666666666687</v>
+      </c>
+      <c r="K214">
         <f t="shared" si="29"/>
-        <v>4.96388960392956E-3</v>
-      </c>
-      <c r="K214">
-        <f t="shared" si="30"/>
-        <v>12.962074034109945</v>
+        <v>1.6666666666666687</v>
       </c>
       <c r="N214" s="45" t="s">
         <v>41</v>
@@ -15261,21 +15279,21 @@
       <c r="F215" s="65">
         <v>3.51</v>
       </c>
+      <c r="G215">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
       <c r="H215">
         <f t="shared" si="27"/>
-        <v>8.2947761194029841</v>
-      </c>
-      <c r="I215">
+        <v>9.75</v>
+      </c>
+      <c r="J215">
         <f t="shared" si="28"/>
-        <v>0.86728432835821145</v>
-      </c>
-      <c r="J215">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K215">
         <f t="shared" si="29"/>
-        <v>3.5099999999999997E-3</v>
-      </c>
-      <c r="K215">
-        <f t="shared" si="30"/>
-        <v>9.1655704477611959</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N215" s="45" t="s">
         <v>42</v>
@@ -15313,21 +15331,21 @@
       <c r="F216" s="65">
         <v>2.4819448019647798</v>
       </c>
+      <c r="G216">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
       <c r="H216">
         <f t="shared" si="27"/>
-        <v>5.8652924424540869</v>
-      </c>
-      <c r="I216">
+        <v>6.8942911165688399</v>
+      </c>
+      <c r="J216">
         <f t="shared" si="28"/>
-        <v>0.61326262979891122</v>
-      </c>
-      <c r="J216">
+        <v>1.6666666666666681</v>
+      </c>
+      <c r="K216">
         <f t="shared" si="29"/>
-        <v>2.48194480196478E-3</v>
-      </c>
-      <c r="K216">
-        <f t="shared" si="30"/>
-        <v>6.4810370170549634</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N216" s="45" t="s">
         <v>43</v>
@@ -15365,21 +15383,21 @@
       <c r="F217" s="65">
         <v>1.7549999999999999</v>
       </c>
+      <c r="G217">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
       <c r="H217">
         <f t="shared" si="27"/>
-        <v>4.147388059701492</v>
-      </c>
-      <c r="I217">
+        <v>4.875</v>
+      </c>
+      <c r="J217">
         <f t="shared" si="28"/>
-        <v>0.43364216417910573</v>
-      </c>
-      <c r="J217">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K217">
         <f t="shared" si="29"/>
-        <v>1.7549999999999998E-3</v>
-      </c>
-      <c r="K217">
-        <f t="shared" si="30"/>
-        <v>4.5827852238805979</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N217" s="45" t="s">
         <v>44</v>
@@ -15404,14 +15422,6 @@
       <c r="D218" s="48"/>
       <c r="E218" s="48"/>
       <c r="F218" s="48"/>
-      <c r="K218">
-        <f>AVERAGE(K204:K217)</f>
-        <v>36.598895066563315</v>
-      </c>
-      <c r="L218">
-        <f>K218/(365.25/7)</f>
-        <v>0.70141619566308888</v>
-      </c>
       <c r="N218" s="45" t="s">
         <v>45</v>
       </c>
@@ -15429,29 +15439,29 @@
       </c>
     </row>
     <row r="219" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="124" t="s">
+      <c r="A219" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="B219" s="124"/>
-      <c r="C219" s="124"/>
-      <c r="D219" s="124"/>
-      <c r="E219" s="124"/>
-      <c r="F219" s="124"/>
+      <c r="B219" s="107"/>
+      <c r="C219" s="107"/>
+      <c r="D219" s="107"/>
+      <c r="E219" s="107"/>
+      <c r="F219" s="107"/>
     </row>
     <row r="220" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A220" s="111" t="s">
+      <c r="A220" s="120" t="s">
         <v>2</v>
       </c>
       <c r="B220" s="43"/>
       <c r="C220" s="43"/>
-      <c r="D220" s="115" t="s">
+      <c r="D220" s="106" t="s">
         <v>51</v>
       </c>
-      <c r="E220" s="115"/>
-      <c r="F220" s="115"/>
+      <c r="E220" s="106"/>
+      <c r="F220" s="106"/>
     </row>
     <row r="221" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A221" s="111"/>
+      <c r="A221" s="120"/>
       <c r="B221" s="43"/>
       <c r="C221" s="44" t="s">
         <v>47</v>
@@ -15478,17 +15488,32 @@
       <c r="E222" s="64">
         <v>0</v>
       </c>
-      <c r="F222" s="64">
-        <v>0</v>
+      <c r="F222" s="130">
+        <v>0</v>
+      </c>
+      <c r="G222" s="131">
+        <v>1</v>
+      </c>
+      <c r="H222">
+        <f>D222*G222</f>
+        <v>0</v>
+      </c>
+      <c r="J222" t="e">
+        <f>D222/E222</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K222" t="e">
+        <f>E222/F222</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="N222" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="O222" s="108" t="s">
+      <c r="O222" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="P222" s="108"/>
-      <c r="Q222" s="108"/>
+      <c r="P222" s="118"/>
+      <c r="Q222" s="118"/>
     </row>
     <row r="223" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="45" t="s">
@@ -15502,8 +15527,23 @@
       <c r="E223" s="64">
         <v>0</v>
       </c>
-      <c r="F223" s="64">
-        <v>0</v>
+      <c r="F223" s="130">
+        <v>0</v>
+      </c>
+      <c r="G223" s="131">
+        <v>1</v>
+      </c>
+      <c r="H223">
+        <f t="shared" ref="H223:H237" si="35">D223*G223</f>
+        <v>0</v>
+      </c>
+      <c r="J223" t="e">
+        <f t="shared" ref="J223:J233" si="36">D223/E223</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K223" t="e">
+        <f t="shared" ref="K223:K233" si="37">E223/F223</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="N223" s="45" t="s">
         <v>25</v>
@@ -15535,6 +15575,21 @@
       <c r="F224" s="64">
         <v>2.8079999999999998</v>
       </c>
+      <c r="G224">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H224">
+        <f t="shared" si="35"/>
+        <v>39.779999999999994</v>
+      </c>
+      <c r="J224">
+        <f t="shared" si="36"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K224">
+        <f t="shared" si="37"/>
+        <v>1.6666666666666667</v>
+      </c>
       <c r="N224" s="45" t="s">
         <v>24</v>
       </c>
@@ -15565,6 +15620,21 @@
       <c r="F225" s="65">
         <v>6.7392000000000003</v>
       </c>
+      <c r="G225">
+        <v>4.25</v>
+      </c>
+      <c r="H225">
+        <f t="shared" si="35"/>
+        <v>79.56</v>
+      </c>
+      <c r="J225">
+        <f t="shared" si="36"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K225">
+        <f t="shared" si="37"/>
+        <v>1.6666666666666665</v>
+      </c>
       <c r="N225" s="45" t="s">
         <v>32</v>
       </c>
@@ -15597,19 +15667,34 @@
       <c r="F226" s="64">
         <v>26.956800000000001</v>
       </c>
+      <c r="G226">
+        <v>1.05</v>
+      </c>
+      <c r="H226">
+        <f t="shared" si="35"/>
+        <v>78.623999999999995</v>
+      </c>
+      <c r="J226">
+        <f t="shared" si="36"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K226">
+        <f t="shared" si="37"/>
+        <v>1.6666666666666665</v>
+      </c>
       <c r="N226" s="45" t="s">
         <v>33</v>
       </c>
       <c r="O226" s="9">
-        <f t="shared" ref="O226:O238" si="35">D225/D224</f>
+        <f t="shared" ref="O226:O238" si="38">D225/D224</f>
         <v>2.4</v>
       </c>
       <c r="P226" s="9">
-        <f t="shared" ref="P226:P238" si="36">E225/E224</f>
+        <f t="shared" ref="P226:P238" si="39">E225/E224</f>
         <v>2.4</v>
       </c>
       <c r="Q226" s="9">
-        <f t="shared" ref="Q226:Q238" si="37">F225/F224</f>
+        <f t="shared" ref="Q226:Q238" si="40">F225/F224</f>
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -15627,22 +15712,37 @@
       <c r="E227" s="64">
         <v>84.24</v>
       </c>
-      <c r="F227" s="64">
+      <c r="F227" s="130">
         <v>50.543999999999997</v>
+      </c>
+      <c r="G227" s="131">
+        <v>0.4</v>
+      </c>
+      <c r="H227">
+        <f t="shared" si="35"/>
+        <v>56.160000000000004</v>
+      </c>
+      <c r="J227">
+        <f t="shared" si="36"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K227">
+        <f t="shared" si="37"/>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N227" s="45" t="s">
         <v>34</v>
       </c>
       <c r="O227" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>4</v>
       </c>
       <c r="P227" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>4</v>
       </c>
       <c r="Q227" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>4</v>
       </c>
     </row>
@@ -15654,7 +15754,7 @@
         <v>10</v>
       </c>
       <c r="C228" s="43">
-        <f t="shared" ref="C228:C237" si="38">EXP(LN(0.5)*B227/10)</f>
+        <f t="shared" ref="C228:C237" si="41">EXP(LN(0.5)*B227/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D228" s="64">
@@ -15663,22 +15763,37 @@
       <c r="E228" s="64">
         <v>59.566675247154798</v>
       </c>
-      <c r="F228" s="64">
+      <c r="F228" s="130">
         <v>35.740005148292902</v>
+      </c>
+      <c r="G228" s="131">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H228">
+        <f t="shared" si="35"/>
+        <v>54.602785643225225</v>
+      </c>
+      <c r="J228">
+        <f t="shared" si="36"/>
+        <v>1.6666666666666663</v>
+      </c>
+      <c r="K228">
+        <f t="shared" si="37"/>
+        <v>1.6666666666666656</v>
       </c>
       <c r="N228" s="45" t="s">
         <v>35</v>
       </c>
       <c r="O228" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>1.8750000000000002</v>
       </c>
       <c r="P228" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1.875</v>
       </c>
       <c r="Q228" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>1.8749999999999998</v>
       </c>
     </row>
@@ -15690,7 +15805,7 @@
         <v>15</v>
       </c>
       <c r="C229" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>0.5</v>
       </c>
       <c r="D229" s="64">
@@ -15699,22 +15814,35 @@
       <c r="E229" s="64">
         <v>42.12</v>
       </c>
-      <c r="F229" s="64">
+      <c r="F229" s="130">
         <v>25.271999999999998</v>
+      </c>
+      <c r="G229" s="132"/>
+      <c r="H229">
+        <f>H228</f>
+        <v>54.602785643225225</v>
+      </c>
+      <c r="J229">
+        <f t="shared" si="36"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K229">
+        <f t="shared" si="37"/>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N229" s="45" t="s">
         <v>36</v>
       </c>
       <c r="O229" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="P229" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q229" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654846</v>
       </c>
     </row>
@@ -15726,7 +15854,7 @@
         <v>20</v>
       </c>
       <c r="C230" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>0.35355339059327379</v>
       </c>
       <c r="D230" s="64">
@@ -15735,22 +15863,37 @@
       <c r="E230" s="64">
         <v>29.783337623577399</v>
       </c>
-      <c r="F230" s="64">
+      <c r="F230" s="130">
         <v>17.870002574146401</v>
+      </c>
+      <c r="G230" s="131">
+        <v>1</v>
+      </c>
+      <c r="H230">
+        <f t="shared" si="35"/>
+        <v>49.638896039295602</v>
+      </c>
+      <c r="J230">
+        <f t="shared" si="36"/>
+        <v>1.6666666666666645</v>
+      </c>
+      <c r="K230">
+        <f t="shared" si="37"/>
+        <v>1.6666666666666703</v>
       </c>
       <c r="N230" s="45" t="s">
         <v>37</v>
       </c>
       <c r="O230" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.70710678118654735</v>
       </c>
       <c r="P230" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654702</v>
       </c>
       <c r="Q230" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654657</v>
       </c>
     </row>
@@ -15762,7 +15905,7 @@
         <v>25</v>
       </c>
       <c r="C231" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>0.25</v>
       </c>
       <c r="D231" s="64">
@@ -15774,19 +15917,34 @@
       <c r="F231" s="64">
         <v>12.635999999999999</v>
       </c>
+      <c r="G231">
+        <v>1.5</v>
+      </c>
+      <c r="H231">
+        <f t="shared" si="35"/>
+        <v>52.650000000000006</v>
+      </c>
+      <c r="J231">
+        <f t="shared" si="36"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K231">
+        <f t="shared" si="37"/>
+        <v>1.6666666666666667</v>
+      </c>
       <c r="N231" s="45" t="s">
         <v>38</v>
       </c>
       <c r="O231" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.70710678118654702</v>
       </c>
       <c r="P231" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q231" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654646</v>
       </c>
     </row>
@@ -15798,7 +15956,7 @@
         <v>30</v>
       </c>
       <c r="C232" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>0.17677669529663689</v>
       </c>
       <c r="D232" s="64">
@@ -15810,19 +15968,34 @@
       <c r="F232" s="64">
         <v>9.92777920785913</v>
       </c>
+      <c r="G232">
+        <v>1.5</v>
+      </c>
+      <c r="H232">
+        <f t="shared" si="35"/>
+        <v>41.365746699413094</v>
+      </c>
+      <c r="J232">
+        <f t="shared" si="36"/>
+        <v>1.6666666666666705</v>
+      </c>
+      <c r="K232">
+        <f t="shared" si="37"/>
+        <v>1.666666666666665</v>
+      </c>
       <c r="N232" s="45" t="s">
         <v>39</v>
       </c>
       <c r="O232" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="P232" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654702</v>
       </c>
       <c r="Q232" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654857</v>
       </c>
     </row>
@@ -15834,7 +16007,7 @@
         <v>35</v>
       </c>
       <c r="C233" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>0.12500000000000003</v>
       </c>
       <c r="D233" s="64">
@@ -15846,19 +16019,34 @@
       <c r="F233" s="64">
         <v>7.02</v>
       </c>
+      <c r="G233">
+        <v>2</v>
+      </c>
+      <c r="H233">
+        <f t="shared" si="35"/>
+        <v>39</v>
+      </c>
+      <c r="J233">
+        <f t="shared" si="36"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K233">
+        <f t="shared" si="37"/>
+        <v>1.6666666666666667</v>
+      </c>
       <c r="N233" s="45" t="s">
         <v>40</v>
       </c>
       <c r="O233" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.78567420131838739</v>
       </c>
       <c r="P233" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.78567420131838561</v>
       </c>
       <c r="Q233" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.78567420131838639</v>
       </c>
     </row>
@@ -15870,7 +16058,7 @@
         <v>40</v>
       </c>
       <c r="C234" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>8.8388347648318447E-2</v>
       </c>
       <c r="D234" s="64">
@@ -15882,19 +16070,34 @@
       <c r="F234" s="64">
         <v>4.9638896039295597</v>
       </c>
+      <c r="G234">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H234">
+        <f t="shared" si="35"/>
+        <v>30.334880912902939</v>
+      </c>
+      <c r="J234">
+        <f>D234/E234</f>
+        <v>1.6666666666666687</v>
+      </c>
+      <c r="K234">
+        <f>E234/F234</f>
+        <v>1.6666666666666687</v>
+      </c>
       <c r="N234" s="45" t="s">
         <v>41</v>
       </c>
       <c r="O234" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.70710678118654635</v>
       </c>
       <c r="P234" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q234" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654724</v>
       </c>
     </row>
@@ -15906,7 +16109,7 @@
         <v>45</v>
       </c>
       <c r="C235" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>6.25E-2</v>
       </c>
       <c r="D235" s="64">
@@ -15918,19 +16121,34 @@
       <c r="F235" s="64">
         <v>3.51</v>
       </c>
+      <c r="G235">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H235">
+        <f t="shared" si="35"/>
+        <v>22.424999999999997</v>
+      </c>
+      <c r="J235">
+        <f t="shared" ref="J235:J237" si="42">D235/E235</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K235">
+        <f t="shared" ref="K235:K237" si="43">E235/F235</f>
+        <v>1.6666666666666667</v>
+      </c>
       <c r="N235" s="45" t="s">
         <v>42</v>
       </c>
       <c r="O235" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.70710678118654868</v>
       </c>
       <c r="P235" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654779</v>
       </c>
       <c r="Q235" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654702</v>
       </c>
     </row>
@@ -15954,19 +16172,34 @@
       <c r="F236" s="64">
         <v>2.4819448019647798</v>
       </c>
+      <c r="G236">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H236">
+        <f t="shared" si="35"/>
+        <v>15.85686956810833</v>
+      </c>
+      <c r="J236">
+        <f t="shared" si="42"/>
+        <v>1.6666666666666681</v>
+      </c>
+      <c r="K236">
+        <f t="shared" si="43"/>
+        <v>1.6666666666666667</v>
+      </c>
       <c r="N236" s="45" t="s">
         <v>43</v>
       </c>
       <c r="O236" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.70710678118654635</v>
       </c>
       <c r="P236" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654724</v>
       </c>
       <c r="Q236" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654802</v>
       </c>
     </row>
@@ -15978,7 +16211,7 @@
         <v>55</v>
       </c>
       <c r="C237" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>3.125E-2</v>
       </c>
       <c r="D237" s="64">
@@ -15990,19 +16223,34 @@
       <c r="F237" s="64">
         <v>1.7549999999999999</v>
       </c>
+      <c r="G237">
+        <v>2.1</v>
+      </c>
+      <c r="H237">
+        <f t="shared" si="35"/>
+        <v>10.237500000000001</v>
+      </c>
+      <c r="J237">
+        <f t="shared" si="42"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="K237">
+        <f t="shared" si="43"/>
+        <v>1.6666666666666667</v>
+      </c>
       <c r="N237" s="45" t="s">
         <v>44</v>
       </c>
       <c r="O237" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="P237" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654713</v>
       </c>
       <c r="Q237" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654702</v>
       </c>
     </row>
@@ -16017,15 +16265,15 @@
         <v>45</v>
       </c>
       <c r="O238" s="9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>0.70710678118654735</v>
       </c>
       <c r="P238" s="9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q238" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654802</v>
       </c>
     </row>
@@ -16082,6 +16330,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="AA87:AA88"/>
+    <mergeCell ref="N81:N83"/>
+    <mergeCell ref="B81:L82"/>
+    <mergeCell ref="AA81:AI81"/>
+    <mergeCell ref="AB82:AI82"/>
+    <mergeCell ref="AB87:AI87"/>
+    <mergeCell ref="O81:Y82"/>
+    <mergeCell ref="AA82:AA83"/>
+    <mergeCell ref="O222:Q222"/>
+    <mergeCell ref="O202:Q202"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="E161:G161"/>
+    <mergeCell ref="A186:C186"/>
+    <mergeCell ref="A198:F198"/>
+    <mergeCell ref="A199:F199"/>
+    <mergeCell ref="D200:F200"/>
+    <mergeCell ref="D220:F220"/>
+    <mergeCell ref="A111:Q111"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="I133:I135"/>
     <mergeCell ref="J133:O133"/>
@@ -16098,27 +16367,6 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="I115:N115"/>
-    <mergeCell ref="O222:Q222"/>
-    <mergeCell ref="O202:Q202"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A161:A162"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="E161:G161"/>
-    <mergeCell ref="A186:C186"/>
-    <mergeCell ref="A198:F198"/>
-    <mergeCell ref="A199:F199"/>
-    <mergeCell ref="D200:F200"/>
-    <mergeCell ref="D220:F220"/>
-    <mergeCell ref="A111:Q111"/>
-    <mergeCell ref="AA87:AA88"/>
-    <mergeCell ref="N81:N83"/>
-    <mergeCell ref="B81:L82"/>
-    <mergeCell ref="AA81:AI81"/>
-    <mergeCell ref="AB82:AI82"/>
-    <mergeCell ref="AB87:AI87"/>
-    <mergeCell ref="O81:Y82"/>
-    <mergeCell ref="AA82:AA83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update notes about acts matrix in Excel doc
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -1431,7 +1431,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1655,6 +1655,63 @@
     <xf numFmtId="11" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1676,9 +1733,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1691,66 +1745,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -4134,6 +4136,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5619,6 +5622,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8231,8 +8235,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AI245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O207" sqref="O207"/>
+    <sheetView tabSelected="1" topLeftCell="A204" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G235" sqref="G235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8304,16 +8308,16 @@
       <c r="Y1" s="37"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="120" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -8365,14 +8369,14 @@
       <c r="A4" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="112" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="111" t="s">
+      <c r="C4" s="113"/>
+      <c r="D4" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="112"/>
+      <c r="E4" s="113"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -8800,10 +8804,10 @@
       <c r="A27" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="111" t="s">
+      <c r="B27" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="112"/>
+      <c r="C27" s="113"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -9218,19 +9222,19 @@
       <c r="AE51" s="24"/>
     </row>
     <row r="52" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="113" t="s">
+      <c r="A52" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="113" t="s">
+      <c r="B52" s="131" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="113"/>
-      <c r="D52" s="113"/>
-      <c r="E52" s="113" t="s">
+      <c r="C52" s="131"/>
+      <c r="D52" s="131"/>
+      <c r="E52" s="131" t="s">
         <v>57</v>
       </c>
-      <c r="F52" s="113"/>
-      <c r="G52" s="113"/>
+      <c r="F52" s="131"/>
+      <c r="G52" s="131"/>
       <c r="X52" s="22"/>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
@@ -9241,7 +9245,7 @@
       <c r="AE52" s="22"/>
     </row>
     <row r="53" spans="1:31" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="113"/>
+      <c r="A53" s="131"/>
       <c r="B53" s="33" t="s">
         <v>3</v>
       </c>
@@ -9775,91 +9779,91 @@
       <c r="X80" s="37"/>
     </row>
     <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="114" t="s">
+      <c r="A81" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="119" t="s">
+      <c r="B81" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="C81" s="119"/>
-      <c r="D81" s="119"/>
-      <c r="E81" s="119"/>
-      <c r="F81" s="119"/>
-      <c r="G81" s="119"/>
-      <c r="H81" s="119"/>
-      <c r="I81" s="119"/>
-      <c r="J81" s="119"/>
-      <c r="K81" s="119"/>
-      <c r="L81" s="119"/>
-      <c r="N81" s="114" t="s">
+      <c r="C81" s="107"/>
+      <c r="D81" s="107"/>
+      <c r="E81" s="107"/>
+      <c r="F81" s="107"/>
+      <c r="G81" s="107"/>
+      <c r="H81" s="107"/>
+      <c r="I81" s="107"/>
+      <c r="J81" s="107"/>
+      <c r="K81" s="107"/>
+      <c r="L81" s="107"/>
+      <c r="N81" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="O81" s="119" t="s">
+      <c r="O81" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="P81" s="119"/>
-      <c r="Q81" s="119"/>
-      <c r="R81" s="119"/>
-      <c r="S81" s="119"/>
-      <c r="T81" s="119"/>
-      <c r="U81" s="119"/>
-      <c r="V81" s="119"/>
-      <c r="W81" s="119"/>
-      <c r="X81" s="119"/>
-      <c r="Y81" s="119"/>
-      <c r="AA81" s="127" t="s">
+      <c r="P81" s="107"/>
+      <c r="Q81" s="107"/>
+      <c r="R81" s="107"/>
+      <c r="S81" s="107"/>
+      <c r="T81" s="107"/>
+      <c r="U81" s="107"/>
+      <c r="V81" s="107"/>
+      <c r="W81" s="107"/>
+      <c r="X81" s="107"/>
+      <c r="Y81" s="107"/>
+      <c r="AA81" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="AB81" s="128"/>
-      <c r="AC81" s="128"/>
-      <c r="AD81" s="128"/>
-      <c r="AE81" s="128"/>
-      <c r="AF81" s="128"/>
-      <c r="AG81" s="128"/>
-      <c r="AH81" s="128"/>
-      <c r="AI81" s="129"/>
+      <c r="AB81" s="109"/>
+      <c r="AC81" s="109"/>
+      <c r="AD81" s="109"/>
+      <c r="AE81" s="109"/>
+      <c r="AF81" s="109"/>
+      <c r="AG81" s="109"/>
+      <c r="AH81" s="109"/>
+      <c r="AI81" s="110"/>
     </row>
     <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="115"/>
-      <c r="B82" s="119"/>
-      <c r="C82" s="119"/>
-      <c r="D82" s="119"/>
-      <c r="E82" s="119"/>
-      <c r="F82" s="119"/>
-      <c r="G82" s="119"/>
-      <c r="H82" s="119"/>
-      <c r="I82" s="119"/>
-      <c r="J82" s="119"/>
-      <c r="K82" s="119"/>
-      <c r="L82" s="119"/>
-      <c r="N82" s="115"/>
-      <c r="O82" s="119"/>
-      <c r="P82" s="119"/>
-      <c r="Q82" s="119"/>
-      <c r="R82" s="119"/>
-      <c r="S82" s="119"/>
-      <c r="T82" s="119"/>
-      <c r="U82" s="119"/>
-      <c r="V82" s="119"/>
-      <c r="W82" s="119"/>
-      <c r="X82" s="119"/>
-      <c r="Y82" s="119"/>
-      <c r="AA82" s="125" t="s">
+      <c r="A82" s="105"/>
+      <c r="B82" s="107"/>
+      <c r="C82" s="107"/>
+      <c r="D82" s="107"/>
+      <c r="E82" s="107"/>
+      <c r="F82" s="107"/>
+      <c r="G82" s="107"/>
+      <c r="H82" s="107"/>
+      <c r="I82" s="107"/>
+      <c r="J82" s="107"/>
+      <c r="K82" s="107"/>
+      <c r="L82" s="107"/>
+      <c r="N82" s="105"/>
+      <c r="O82" s="107"/>
+      <c r="P82" s="107"/>
+      <c r="Q82" s="107"/>
+      <c r="R82" s="107"/>
+      <c r="S82" s="107"/>
+      <c r="T82" s="107"/>
+      <c r="U82" s="107"/>
+      <c r="V82" s="107"/>
+      <c r="W82" s="107"/>
+      <c r="X82" s="107"/>
+      <c r="Y82" s="107"/>
+      <c r="AA82" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="AB82" s="127" t="s">
+      <c r="AB82" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="AC82" s="128"/>
-      <c r="AD82" s="128"/>
-      <c r="AE82" s="128"/>
-      <c r="AF82" s="128"/>
-      <c r="AG82" s="128"/>
-      <c r="AH82" s="128"/>
-      <c r="AI82" s="129"/>
+      <c r="AC82" s="109"/>
+      <c r="AD82" s="109"/>
+      <c r="AE82" s="109"/>
+      <c r="AF82" s="109"/>
+      <c r="AG82" s="109"/>
+      <c r="AH82" s="109"/>
+      <c r="AI82" s="110"/>
     </row>
     <row r="83" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="116"/>
+      <c r="A83" s="106"/>
       <c r="B83" s="76" t="s">
         <v>95</v>
       </c>
@@ -9893,7 +9897,7 @@
       <c r="L83" s="89">
         <v>2020</v>
       </c>
-      <c r="N83" s="116"/>
+      <c r="N83" s="106"/>
       <c r="O83" s="76" t="s">
         <v>95</v>
       </c>
@@ -9927,7 +9931,7 @@
       <c r="Y83" s="89">
         <v>2020</v>
       </c>
-      <c r="AA83" s="126"/>
+      <c r="AA83" s="103"/>
       <c r="AB83" s="76" t="s">
         <v>95</v>
       </c>
@@ -10367,19 +10371,19 @@
         <f t="shared" si="12"/>
         <v>-6.3054823529411761E-5</v>
       </c>
-      <c r="AA87" s="125" t="s">
+      <c r="AA87" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="AB87" s="127" t="s">
+      <c r="AB87" s="108" t="s">
         <v>75</v>
       </c>
-      <c r="AC87" s="128"/>
-      <c r="AD87" s="128"/>
-      <c r="AE87" s="128"/>
-      <c r="AF87" s="128"/>
-      <c r="AG87" s="128"/>
-      <c r="AH87" s="128"/>
-      <c r="AI87" s="129"/>
+      <c r="AC87" s="109"/>
+      <c r="AD87" s="109"/>
+      <c r="AE87" s="109"/>
+      <c r="AF87" s="109"/>
+      <c r="AG87" s="109"/>
+      <c r="AH87" s="109"/>
+      <c r="AI87" s="110"/>
     </row>
     <row r="88" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="74" t="s">
@@ -10464,7 +10468,7 @@
         <f t="shared" si="12"/>
         <v>-1.4261617647058823E-4</v>
       </c>
-      <c r="AA88" s="126"/>
+      <c r="AA88" s="103"/>
       <c r="AB88" s="76" t="s">
         <v>95</v>
       </c>
@@ -11653,25 +11657,25 @@
       <c r="X110" s="37"/>
     </row>
     <row r="111" spans="1:26" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="124" t="s">
+      <c r="A111" s="119" t="s">
         <v>104</v>
       </c>
-      <c r="B111" s="124"/>
-      <c r="C111" s="124"/>
-      <c r="D111" s="124"/>
-      <c r="E111" s="124"/>
-      <c r="F111" s="124"/>
-      <c r="G111" s="124"/>
-      <c r="H111" s="124"/>
-      <c r="I111" s="124"/>
-      <c r="J111" s="124"/>
-      <c r="K111" s="124"/>
-      <c r="L111" s="124"/>
-      <c r="M111" s="124"/>
-      <c r="N111" s="124"/>
-      <c r="O111" s="124"/>
-      <c r="P111" s="124"/>
-      <c r="Q111" s="124"/>
+      <c r="B111" s="119"/>
+      <c r="C111" s="119"/>
+      <c r="D111" s="119"/>
+      <c r="E111" s="119"/>
+      <c r="F111" s="119"/>
+      <c r="G111" s="119"/>
+      <c r="H111" s="119"/>
+      <c r="I111" s="119"/>
+      <c r="J111" s="119"/>
+      <c r="K111" s="119"/>
+      <c r="L111" s="119"/>
+      <c r="M111" s="119"/>
+      <c r="N111" s="119"/>
+      <c r="O111" s="119"/>
+      <c r="P111" s="119"/>
+      <c r="Q111" s="119"/>
       <c r="R111" s="37"/>
       <c r="S111" s="37"/>
       <c r="T111" s="37"/>
@@ -11681,17 +11685,17 @@
       <c r="X111" s="37"/>
     </row>
     <row r="112" spans="1:26" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="108" t="s">
+      <c r="A112" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="103" t="s">
+      <c r="B112" s="124" t="s">
         <v>85</v>
       </c>
-      <c r="C112" s="104"/>
-      <c r="D112" s="104"/>
-      <c r="E112" s="104"/>
-      <c r="F112" s="104"/>
-      <c r="G112" s="105"/>
+      <c r="C112" s="125"/>
+      <c r="D112" s="125"/>
+      <c r="E112" s="125"/>
+      <c r="F112" s="125"/>
+      <c r="G112" s="126"/>
       <c r="I112" s="73"/>
       <c r="J112" s="86" t="s">
         <v>27</v>
@@ -11710,7 +11714,7 @@
       </c>
     </row>
     <row r="113" spans="1:14" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="109"/>
+      <c r="A113" s="129"/>
       <c r="B113" s="32" t="s">
         <v>70</v>
       </c>
@@ -11754,7 +11758,7 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="110"/>
+      <c r="A114" s="130"/>
       <c r="B114" s="34" t="s">
         <v>63</v>
       </c>
@@ -11802,14 +11806,14 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="I115" s="117" t="s">
+      <c r="I115" s="132" t="s">
         <v>103</v>
       </c>
-      <c r="J115" s="117"/>
-      <c r="K115" s="117"/>
-      <c r="L115" s="117"/>
-      <c r="M115" s="117"/>
-      <c r="N115" s="117"/>
+      <c r="J115" s="132"/>
+      <c r="K115" s="132"/>
+      <c r="L115" s="132"/>
+      <c r="M115" s="132"/>
+      <c r="N115" s="132"/>
     </row>
     <row r="116" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
@@ -12562,31 +12566,31 @@
     </row>
     <row r="132" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="133" spans="1:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="100" t="s">
+      <c r="A133" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="103" t="s">
+      <c r="B133" s="124" t="s">
         <v>86</v>
       </c>
-      <c r="C133" s="104"/>
-      <c r="D133" s="104"/>
-      <c r="E133" s="104"/>
-      <c r="F133" s="104"/>
-      <c r="G133" s="105"/>
-      <c r="I133" s="100" t="s">
+      <c r="C133" s="125"/>
+      <c r="D133" s="125"/>
+      <c r="E133" s="125"/>
+      <c r="F133" s="125"/>
+      <c r="G133" s="126"/>
+      <c r="I133" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="J133" s="103" t="s">
+      <c r="J133" s="124" t="s">
         <v>76</v>
       </c>
-      <c r="K133" s="104"/>
-      <c r="L133" s="104"/>
-      <c r="M133" s="104"/>
-      <c r="N133" s="104"/>
-      <c r="O133" s="105"/>
+      <c r="K133" s="125"/>
+      <c r="L133" s="125"/>
+      <c r="M133" s="125"/>
+      <c r="N133" s="125"/>
+      <c r="O133" s="126"/>
     </row>
     <row r="134" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="101"/>
+      <c r="A134" s="122"/>
       <c r="B134" s="26" t="s">
         <v>71</v>
       </c>
@@ -12605,7 +12609,7 @@
       <c r="G134" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I134" s="101"/>
+      <c r="I134" s="122"/>
       <c r="J134" s="26" t="s">
         <v>71</v>
       </c>
@@ -12626,7 +12630,7 @@
       </c>
     </row>
     <row r="135" spans="1:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="102"/>
+      <c r="A135" s="123"/>
       <c r="B135" s="40" t="s">
         <v>63</v>
       </c>
@@ -12645,7 +12649,7 @@
       <c r="G135" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I135" s="102"/>
+      <c r="I135" s="123"/>
       <c r="J135" s="40" t="s">
         <v>63</v>
       </c>
@@ -13585,22 +13589,22 @@
       <c r="W160" s="37"/>
     </row>
     <row r="161" spans="1:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="119" t="s">
+      <c r="A161" s="107" t="s">
         <v>90</v>
       </c>
-      <c r="B161" s="121" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="121"/>
-      <c r="D161" s="121"/>
-      <c r="E161" s="121" t="s">
+      <c r="B161" s="115" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="115"/>
+      <c r="D161" s="115"/>
+      <c r="E161" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="F161" s="121"/>
-      <c r="G161" s="121"/>
+      <c r="F161" s="115"/>
+      <c r="G161" s="115"/>
     </row>
     <row r="162" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="119"/>
+      <c r="A162" s="107"/>
       <c r="B162" s="63" t="s">
         <v>3</v>
       </c>
@@ -14396,9 +14400,9 @@
       <c r="AB185" s="20"/>
     </row>
     <row r="186" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="122"/>
-      <c r="B186" s="122"/>
-      <c r="C186" s="122"/>
+      <c r="A186" s="116"/>
+      <c r="B186" s="116"/>
+      <c r="C186" s="116"/>
       <c r="D186" s="20"/>
       <c r="E186" s="20"/>
       <c r="F186" s="20"/>
@@ -14573,39 +14577,39 @@
       <c r="W197" s="37"/>
     </row>
     <row r="198" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="111" t="s">
+      <c r="A198" s="112" t="s">
         <v>73</v>
       </c>
-      <c r="B198" s="111"/>
-      <c r="C198" s="111"/>
-      <c r="D198" s="111"/>
-      <c r="E198" s="111"/>
-      <c r="F198" s="111"/>
+      <c r="B198" s="112"/>
+      <c r="C198" s="112"/>
+      <c r="D198" s="112"/>
+      <c r="E198" s="112"/>
+      <c r="F198" s="112"/>
     </row>
     <row r="199" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="123" t="s">
+      <c r="A199" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="B199" s="123"/>
-      <c r="C199" s="123"/>
-      <c r="D199" s="123"/>
-      <c r="E199" s="123"/>
-      <c r="F199" s="123"/>
+      <c r="B199" s="117"/>
+      <c r="C199" s="117"/>
+      <c r="D199" s="117"/>
+      <c r="E199" s="117"/>
+      <c r="F199" s="117"/>
     </row>
     <row r="200" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A200" s="106" t="s">
+      <c r="A200" s="118" t="s">
         <v>46</v>
       </c>
       <c r="B200" s="43"/>
       <c r="C200" s="43"/>
-      <c r="D200" s="106" t="s">
+      <c r="D200" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="E200" s="106"/>
-      <c r="F200" s="106"/>
+      <c r="E200" s="118"/>
+      <c r="F200" s="118"/>
     </row>
     <row r="201" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A201" s="106"/>
+      <c r="A201" s="118"/>
       <c r="B201" s="43"/>
       <c r="C201" s="44" t="s">
         <v>47</v>
@@ -14639,7 +14643,7 @@
         <v>1</v>
       </c>
       <c r="H202">
-        <f>D222*G202</f>
+        <f>H222*G202</f>
         <v>0</v>
       </c>
       <c r="J202" t="e">
@@ -14653,11 +14657,11 @@
       <c r="N202" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="O202" s="118" t="s">
+      <c r="O202" s="111" t="s">
         <v>94</v>
       </c>
-      <c r="P202" s="118"/>
-      <c r="Q202" s="118"/>
+      <c r="P202" s="111"/>
+      <c r="Q202" s="111"/>
     </row>
     <row r="203" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="45" t="s">
@@ -14678,7 +14682,7 @@
         <v>1</v>
       </c>
       <c r="H203">
-        <f t="shared" ref="H203:H217" si="27">D223*G203</f>
+        <f t="shared" ref="H203:H217" si="27">H223*G203</f>
         <v>0</v>
       </c>
       <c r="J203" t="e">
@@ -14720,12 +14724,12 @@
         <v>1.1232</v>
       </c>
       <c r="G204">
-        <f t="shared" ref="G203:G217" si="30">D204/D224</f>
+        <f t="shared" ref="G204:G217" si="30">D204/D224</f>
         <v>0.4</v>
       </c>
       <c r="H204">
         <f t="shared" si="27"/>
-        <v>3.12</v>
+        <v>15.911999999999999</v>
       </c>
       <c r="J204">
         <f t="shared" si="28"/>
@@ -14766,12 +14770,11 @@
         <v>5.6159999999999997</v>
       </c>
       <c r="G205">
-        <f t="shared" si="30"/>
-        <v>0.83333333333333337</v>
+        <v>0.8</v>
       </c>
       <c r="H205">
         <f t="shared" si="27"/>
-        <v>15.6</v>
+        <v>63.648000000000003</v>
       </c>
       <c r="J205">
         <f t="shared" si="28"/>
@@ -14814,12 +14817,11 @@
         <v>22.463999999999999</v>
       </c>
       <c r="G206">
-        <f t="shared" si="30"/>
-        <v>0.83333333333333337</v>
+        <v>0.8</v>
       </c>
       <c r="H206">
         <f t="shared" si="27"/>
-        <v>62.4</v>
+        <v>62.8992</v>
       </c>
       <c r="J206">
         <f t="shared" si="28"/>
@@ -14863,12 +14865,11 @@
         <v>56.16</v>
       </c>
       <c r="G207">
-        <f t="shared" si="30"/>
-        <v>1.1111111111111112</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H207">
         <f t="shared" si="27"/>
-        <v>156</v>
+        <v>61.77600000000001</v>
       </c>
       <c r="J207">
         <f t="shared" si="28"/>
@@ -14915,12 +14916,11 @@
         <v>39.711116831436499</v>
       </c>
       <c r="G208">
-        <f t="shared" si="30"/>
-        <v>1.1111111111111065</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H208">
         <f t="shared" si="27"/>
-        <v>110.308657865101</v>
+        <v>60.063064207547754</v>
       </c>
       <c r="J208">
         <f t="shared" si="28"/>
@@ -14968,12 +14968,11 @@
         <v>28.08</v>
       </c>
       <c r="G209">
-        <f t="shared" si="30"/>
-        <v>1.1111111111111112</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H209">
         <f t="shared" si="27"/>
-        <v>78</v>
+        <v>60.063064207547754</v>
       </c>
       <c r="J209">
         <f t="shared" si="28"/>
@@ -15020,12 +15019,11 @@
         <v>19.855558415718299</v>
       </c>
       <c r="G210">
-        <f t="shared" si="30"/>
-        <v>1.1111111111111116</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H210">
         <f t="shared" si="27"/>
-        <v>55.15432893255069</v>
+        <v>58.97100849468319</v>
       </c>
       <c r="J210">
         <f t="shared" si="28"/>
@@ -15072,12 +15070,11 @@
         <v>14.04</v>
       </c>
       <c r="G211">
-        <f t="shared" si="30"/>
-        <v>1.1111111111111112</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H211">
         <f t="shared" si="27"/>
-        <v>39</v>
+        <v>57.915000000000013</v>
       </c>
       <c r="J211">
         <f t="shared" si="28"/>
@@ -15129,7 +15126,7 @@
       </c>
       <c r="H212">
         <f t="shared" si="27"/>
-        <v>27.577164466275399</v>
+        <v>52.650000000000006</v>
       </c>
       <c r="J212">
         <f t="shared" si="28"/>
@@ -15181,7 +15178,7 @@
       </c>
       <c r="H213">
         <f t="shared" si="27"/>
-        <v>19.5</v>
+        <v>52.650000000000006</v>
       </c>
       <c r="J213">
         <f t="shared" si="28"/>
@@ -15233,7 +15230,7 @@
       </c>
       <c r="H214">
         <f t="shared" si="27"/>
-        <v>13.788582233137699</v>
+        <v>52.650000000000006</v>
       </c>
       <c r="J214">
         <f t="shared" si="28"/>
@@ -15285,7 +15282,7 @@
       </c>
       <c r="H215">
         <f t="shared" si="27"/>
-        <v>9.75</v>
+        <v>52.650000000000006</v>
       </c>
       <c r="J215">
         <f t="shared" si="28"/>
@@ -15337,7 +15334,7 @@
       </c>
       <c r="H216">
         <f t="shared" si="27"/>
-        <v>6.8942911165688399</v>
+        <v>52.650000000000006</v>
       </c>
       <c r="J216">
         <f t="shared" si="28"/>
@@ -15389,7 +15386,7 @@
       </c>
       <c r="H217">
         <f t="shared" si="27"/>
-        <v>4.875</v>
+        <v>52.650000000000006</v>
       </c>
       <c r="J217">
         <f t="shared" si="28"/>
@@ -15439,29 +15436,30 @@
       </c>
     </row>
     <row r="219" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="107" t="s">
+      <c r="A219" s="127" t="s">
         <v>75</v>
       </c>
-      <c r="B219" s="107"/>
-      <c r="C219" s="107"/>
-      <c r="D219" s="107"/>
-      <c r="E219" s="107"/>
-      <c r="F219" s="107"/>
+      <c r="B219" s="127"/>
+      <c r="C219" s="127"/>
+      <c r="D219" s="127"/>
+      <c r="E219" s="127"/>
+      <c r="F219" s="127"/>
+      <c r="L219" s="134"/>
     </row>
     <row r="220" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A220" s="120" t="s">
+      <c r="A220" s="114" t="s">
         <v>2</v>
       </c>
       <c r="B220" s="43"/>
       <c r="C220" s="43"/>
-      <c r="D220" s="106" t="s">
+      <c r="D220" s="118" t="s">
         <v>51</v>
       </c>
-      <c r="E220" s="106"/>
-      <c r="F220" s="106"/>
+      <c r="E220" s="118"/>
+      <c r="F220" s="118"/>
     </row>
     <row r="221" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A221" s="120"/>
+      <c r="A221" s="114"/>
       <c r="B221" s="43"/>
       <c r="C221" s="44" t="s">
         <v>47</v>
@@ -15488,10 +15486,10 @@
       <c r="E222" s="64">
         <v>0</v>
       </c>
-      <c r="F222" s="130">
-        <v>0</v>
-      </c>
-      <c r="G222" s="131">
+      <c r="F222" s="99">
+        <v>0</v>
+      </c>
+      <c r="G222" s="100">
         <v>1</v>
       </c>
       <c r="H222">
@@ -15509,11 +15507,11 @@
       <c r="N222" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="O222" s="118" t="s">
+      <c r="O222" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="P222" s="118"/>
-      <c r="Q222" s="118"/>
+      <c r="P222" s="111"/>
+      <c r="Q222" s="111"/>
     </row>
     <row r="223" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="45" t="s">
@@ -15527,10 +15525,10 @@
       <c r="E223" s="64">
         <v>0</v>
       </c>
-      <c r="F223" s="130">
-        <v>0</v>
-      </c>
-      <c r="G223" s="131">
+      <c r="F223" s="99">
+        <v>0</v>
+      </c>
+      <c r="G223" s="100">
         <v>1</v>
       </c>
       <c r="H223">
@@ -15627,6 +15625,10 @@
         <f t="shared" si="35"/>
         <v>79.56</v>
       </c>
+      <c r="I225">
+        <f>H225/H224</f>
+        <v>2.0000000000000004</v>
+      </c>
       <c r="J225">
         <f t="shared" si="36"/>
         <v>1.6666666666666667</v>
@@ -15674,6 +15676,10 @@
         <f t="shared" si="35"/>
         <v>78.623999999999995</v>
       </c>
+      <c r="I226">
+        <f t="shared" ref="I226:I237" si="38">H226/H225</f>
+        <v>0.98823529411764699</v>
+      </c>
       <c r="J226">
         <f t="shared" si="36"/>
         <v>1.6666666666666667</v>
@@ -15686,15 +15692,15 @@
         <v>33</v>
       </c>
       <c r="O226" s="9">
-        <f t="shared" ref="O226:O238" si="38">D225/D224</f>
+        <f t="shared" ref="O226:O238" si="39">D225/D224</f>
         <v>2.4</v>
       </c>
       <c r="P226" s="9">
-        <f t="shared" ref="P226:P238" si="39">E225/E224</f>
+        <f t="shared" ref="P226:P238" si="40">E225/E224</f>
         <v>2.4</v>
       </c>
       <c r="Q226" s="9">
-        <f t="shared" ref="Q226:Q238" si="40">F225/F224</f>
+        <f t="shared" ref="Q226:Q238" si="41">F225/F224</f>
         <v>2.4000000000000004</v>
       </c>
     </row>
@@ -15712,16 +15718,20 @@
       <c r="E227" s="64">
         <v>84.24</v>
       </c>
-      <c r="F227" s="130">
+      <c r="F227" s="99">
         <v>50.543999999999997</v>
       </c>
-      <c r="G227" s="131">
+      <c r="G227" s="100">
         <v>0.4</v>
       </c>
       <c r="H227">
         <f t="shared" si="35"/>
         <v>56.160000000000004</v>
       </c>
+      <c r="I227">
+        <f t="shared" si="38"/>
+        <v>0.71428571428571441</v>
+      </c>
       <c r="J227">
         <f t="shared" si="36"/>
         <v>1.6666666666666667</v>
@@ -15734,15 +15744,15 @@
         <v>34</v>
       </c>
       <c r="O227" s="9">
-        <f t="shared" si="38"/>
-        <v>4</v>
-      </c>
-      <c r="P227" s="9">
         <f t="shared" si="39"/>
         <v>4</v>
       </c>
+      <c r="P227" s="9">
+        <f t="shared" si="40"/>
+        <v>4</v>
+      </c>
       <c r="Q227" s="9">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>4</v>
       </c>
     </row>
@@ -15754,7 +15764,7 @@
         <v>10</v>
       </c>
       <c r="C228" s="43">
-        <f t="shared" ref="C228:C237" si="41">EXP(LN(0.5)*B227/10)</f>
+        <f t="shared" ref="C228:C237" si="42">EXP(LN(0.5)*B227/10)</f>
         <v>0.70710678118654757</v>
       </c>
       <c r="D228" s="64">
@@ -15763,16 +15773,20 @@
       <c r="E228" s="64">
         <v>59.566675247154798</v>
       </c>
-      <c r="F228" s="130">
+      <c r="F228" s="99">
         <v>35.740005148292902</v>
       </c>
-      <c r="G228" s="131">
+      <c r="G228" s="100">
         <v>0.55000000000000004</v>
       </c>
       <c r="H228">
         <f t="shared" si="35"/>
         <v>54.602785643225225</v>
       </c>
+      <c r="I228">
+        <f t="shared" si="38"/>
+        <v>0.97227182413150326</v>
+      </c>
       <c r="J228">
         <f t="shared" si="36"/>
         <v>1.6666666666666663</v>
@@ -15785,15 +15799,15 @@
         <v>35</v>
       </c>
       <c r="O228" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>1.8750000000000002</v>
       </c>
       <c r="P228" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1.875</v>
       </c>
       <c r="Q228" s="9">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>1.8749999999999998</v>
       </c>
     </row>
@@ -15805,7 +15819,7 @@
         <v>15</v>
       </c>
       <c r="C229" s="43">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.5</v>
       </c>
       <c r="D229" s="64">
@@ -15814,14 +15828,18 @@
       <c r="E229" s="64">
         <v>42.12</v>
       </c>
-      <c r="F229" s="130">
+      <c r="F229" s="99">
         <v>25.271999999999998</v>
       </c>
-      <c r="G229" s="132"/>
+      <c r="G229" s="101"/>
       <c r="H229">
         <f>H228</f>
         <v>54.602785643225225</v>
       </c>
+      <c r="I229">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
       <c r="J229">
         <f t="shared" si="36"/>
         <v>1.6666666666666667</v>
@@ -15834,15 +15852,15 @@
         <v>36</v>
       </c>
       <c r="O229" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="P229" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q229" s="9">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0.70710678118654846</v>
       </c>
     </row>
@@ -15854,7 +15872,7 @@
         <v>20</v>
       </c>
       <c r="C230" s="43">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.35355339059327379</v>
       </c>
       <c r="D230" s="64">
@@ -15863,15 +15881,19 @@
       <c r="E230" s="64">
         <v>29.783337623577399</v>
       </c>
-      <c r="F230" s="130">
+      <c r="F230" s="99">
         <v>17.870002574146401</v>
       </c>
-      <c r="G230" s="131">
-        <v>1</v>
+      <c r="G230" s="100">
+        <v>1.08</v>
       </c>
       <c r="H230">
         <f t="shared" si="35"/>
-        <v>49.638896039295602</v>
+        <v>53.610007722439256</v>
+      </c>
+      <c r="I230">
+        <f t="shared" si="38"/>
+        <v>0.98181818181818081</v>
       </c>
       <c r="J230">
         <f t="shared" si="36"/>
@@ -15885,15 +15907,15 @@
         <v>37</v>
       </c>
       <c r="O230" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654735</v>
       </c>
       <c r="P230" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654702</v>
       </c>
       <c r="Q230" s="9">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0.70710678118654657</v>
       </c>
     </row>
@@ -15905,7 +15927,7 @@
         <v>25</v>
       </c>
       <c r="C231" s="43">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.25</v>
       </c>
       <c r="D231" s="64">
@@ -15924,6 +15946,10 @@
         <f t="shared" si="35"/>
         <v>52.650000000000006</v>
       </c>
+      <c r="I231">
+        <f t="shared" si="38"/>
+        <v>0.98209275164798338</v>
+      </c>
       <c r="J231">
         <f t="shared" si="36"/>
         <v>1.6666666666666667</v>
@@ -15936,15 +15962,15 @@
         <v>38</v>
       </c>
       <c r="O231" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654702</v>
       </c>
       <c r="P231" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q231" s="9">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0.70710678118654646</v>
       </c>
     </row>
@@ -15956,7 +15982,7 @@
         <v>30</v>
       </c>
       <c r="C232" s="43">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.17677669529663689</v>
       </c>
       <c r="D232" s="64">
@@ -15968,12 +15994,13 @@
       <c r="F232" s="64">
         <v>9.92777920785913</v>
       </c>
-      <c r="G232">
-        <v>1.5</v>
-      </c>
       <c r="H232">
-        <f t="shared" si="35"/>
-        <v>41.365746699413094</v>
+        <f>H231</f>
+        <v>52.650000000000006</v>
+      </c>
+      <c r="I232">
+        <f t="shared" si="38"/>
+        <v>1</v>
       </c>
       <c r="J232">
         <f t="shared" si="36"/>
@@ -15987,15 +16014,15 @@
         <v>39</v>
       </c>
       <c r="O232" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="P232" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654702</v>
       </c>
       <c r="Q232" s="9">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0.70710678118654857</v>
       </c>
     </row>
@@ -16007,7 +16034,7 @@
         <v>35</v>
       </c>
       <c r="C233" s="43">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.12500000000000003</v>
       </c>
       <c r="D233" s="64">
@@ -16019,12 +16046,13 @@
       <c r="F233" s="64">
         <v>7.02</v>
       </c>
-      <c r="G233">
-        <v>2</v>
-      </c>
       <c r="H233">
-        <f t="shared" si="35"/>
-        <v>39</v>
+        <f t="shared" ref="H233:H237" si="43">H232</f>
+        <v>52.650000000000006</v>
+      </c>
+      <c r="I233">
+        <f t="shared" si="38"/>
+        <v>1</v>
       </c>
       <c r="J233">
         <f t="shared" si="36"/>
@@ -16038,15 +16066,15 @@
         <v>40</v>
       </c>
       <c r="O233" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.78567420131838739</v>
       </c>
       <c r="P233" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.78567420131838561</v>
       </c>
       <c r="Q233" s="9">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0.78567420131838639</v>
       </c>
     </row>
@@ -16058,7 +16086,7 @@
         <v>40</v>
       </c>
       <c r="C234" s="43">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>8.8388347648318447E-2</v>
       </c>
       <c r="D234" s="64">
@@ -16070,12 +16098,14 @@
       <c r="F234" s="64">
         <v>4.9638896039295597</v>
       </c>
-      <c r="G234">
-        <v>2.2000000000000002</v>
-      </c>
+      <c r="G234" s="133"/>
       <c r="H234">
-        <f t="shared" si="35"/>
-        <v>30.334880912902939</v>
+        <f t="shared" si="43"/>
+        <v>52.650000000000006</v>
+      </c>
+      <c r="I234">
+        <f t="shared" si="38"/>
+        <v>1</v>
       </c>
       <c r="J234">
         <f>D234/E234</f>
@@ -16089,15 +16119,15 @@
         <v>41</v>
       </c>
       <c r="O234" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654635</v>
       </c>
       <c r="P234" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q234" s="9">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0.70710678118654724</v>
       </c>
     </row>
@@ -16109,7 +16139,7 @@
         <v>45</v>
       </c>
       <c r="C235" s="43">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>6.25E-2</v>
       </c>
       <c r="D235" s="64">
@@ -16121,34 +16151,36 @@
       <c r="F235" s="64">
         <v>3.51</v>
       </c>
-      <c r="G235">
-        <v>2.2999999999999998</v>
-      </c>
+      <c r="G235" s="133"/>
       <c r="H235">
-        <f t="shared" si="35"/>
-        <v>22.424999999999997</v>
+        <f t="shared" si="43"/>
+        <v>52.650000000000006</v>
+      </c>
+      <c r="I235">
+        <f t="shared" si="38"/>
+        <v>1</v>
       </c>
       <c r="J235">
-        <f t="shared" ref="J235:J237" si="42">D235/E235</f>
+        <f t="shared" ref="J235:J237" si="44">D235/E235</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="K235">
-        <f t="shared" ref="K235:K237" si="43">E235/F235</f>
+        <f t="shared" ref="K235:K237" si="45">E235/F235</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="N235" s="45" t="s">
         <v>42</v>
       </c>
       <c r="O235" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654868</v>
       </c>
       <c r="P235" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654779</v>
       </c>
       <c r="Q235" s="9">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0.70710678118654702</v>
       </c>
     </row>
@@ -16172,34 +16204,36 @@
       <c r="F236" s="64">
         <v>2.4819448019647798</v>
       </c>
-      <c r="G236">
-        <v>2.2999999999999998</v>
-      </c>
+      <c r="G236" s="133"/>
       <c r="H236">
-        <f t="shared" si="35"/>
-        <v>15.85686956810833</v>
+        <f t="shared" si="43"/>
+        <v>52.650000000000006</v>
+      </c>
+      <c r="I236">
+        <f t="shared" si="38"/>
+        <v>1</v>
       </c>
       <c r="J236">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>1.6666666666666681</v>
       </c>
       <c r="K236">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="N236" s="45" t="s">
         <v>43</v>
       </c>
       <c r="O236" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654635</v>
       </c>
       <c r="P236" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654724</v>
       </c>
       <c r="Q236" s="9">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0.70710678118654802</v>
       </c>
     </row>
@@ -16211,7 +16245,7 @@
         <v>55</v>
       </c>
       <c r="C237" s="43">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>3.125E-2</v>
       </c>
       <c r="D237" s="64">
@@ -16223,34 +16257,36 @@
       <c r="F237" s="64">
         <v>1.7549999999999999</v>
       </c>
-      <c r="G237">
-        <v>2.1</v>
-      </c>
+      <c r="G237" s="133"/>
       <c r="H237">
-        <f t="shared" si="35"/>
-        <v>10.237500000000001</v>
+        <f t="shared" si="43"/>
+        <v>52.650000000000006</v>
+      </c>
+      <c r="I237">
+        <f t="shared" si="38"/>
+        <v>1</v>
       </c>
       <c r="J237">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="K237">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="N237" s="45" t="s">
         <v>44</v>
       </c>
       <c r="O237" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654768</v>
       </c>
       <c r="P237" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654713</v>
       </c>
       <c r="Q237" s="9">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0.70710678118654702</v>
       </c>
     </row>
@@ -16265,15 +16301,15 @@
         <v>45</v>
       </c>
       <c r="O238" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.70710678118654735</v>
       </c>
       <c r="P238" s="9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.70710678118654802</v>
       </c>
       <c r="Q238" s="9">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0.70710678118654802</v>
       </c>
     </row>
@@ -16330,27 +16366,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="AA87:AA88"/>
-    <mergeCell ref="N81:N83"/>
-    <mergeCell ref="B81:L82"/>
-    <mergeCell ref="AA81:AI81"/>
-    <mergeCell ref="AB82:AI82"/>
-    <mergeCell ref="AB87:AI87"/>
-    <mergeCell ref="O81:Y82"/>
-    <mergeCell ref="AA82:AA83"/>
-    <mergeCell ref="O222:Q222"/>
-    <mergeCell ref="O202:Q202"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A161:A162"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="E161:G161"/>
-    <mergeCell ref="A186:C186"/>
-    <mergeCell ref="A198:F198"/>
-    <mergeCell ref="A199:F199"/>
-    <mergeCell ref="D200:F200"/>
-    <mergeCell ref="D220:F220"/>
-    <mergeCell ref="A111:Q111"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="I133:I135"/>
     <mergeCell ref="J133:O133"/>
@@ -16367,6 +16382,27 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="I115:N115"/>
+    <mergeCell ref="O222:Q222"/>
+    <mergeCell ref="O202:Q202"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="E161:G161"/>
+    <mergeCell ref="A186:C186"/>
+    <mergeCell ref="A198:F198"/>
+    <mergeCell ref="A199:F199"/>
+    <mergeCell ref="D200:F200"/>
+    <mergeCell ref="D220:F220"/>
+    <mergeCell ref="A111:Q111"/>
+    <mergeCell ref="AA87:AA88"/>
+    <mergeCell ref="N81:N83"/>
+    <mergeCell ref="B81:L82"/>
+    <mergeCell ref="AA81:AI81"/>
+    <mergeCell ref="AB82:AI82"/>
+    <mergeCell ref="AB87:AI87"/>
+    <mergeCell ref="O81:Y82"/>
+    <mergeCell ref="AA82:AA83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update sim start year in plot title
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -1682,59 +1682,11 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="37" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="2" fontId="29" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1757,6 +1709,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1769,17 +1724,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="29" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -1886,11 +1886,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>KwaZulu-Natal Population Distribution (1910)</a:t>
+              <a:t>KwaZulu-Natal Population Distribution (1925)</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2405,6 +2406,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2527,6 +2529,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3222,6 +3225,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3349,6 +3353,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4037,6 +4042,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8257,7 +8263,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BJ245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT79" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="BG89" sqref="BG89"/>
     </sheetView>
   </sheetViews>
@@ -8336,16 +8342,16 @@
       <c r="Y1" s="37"/>
     </row>
     <row r="2" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -8397,14 +8403,14 @@
       <c r="A4" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="120" t="s">
+      <c r="B4" s="124" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="120" t="s">
+      <c r="C4" s="125"/>
+      <c r="D4" s="124" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="121"/>
+      <c r="E4" s="125"/>
     </row>
     <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
@@ -8832,10 +8838,10 @@
       <c r="A27" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="120" t="s">
+      <c r="B27" s="124" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="121"/>
+      <c r="C27" s="125"/>
     </row>
     <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
@@ -9250,19 +9256,19 @@
       <c r="AE51" s="24"/>
     </row>
     <row r="52" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="139" t="s">
+      <c r="A52" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="139" t="s">
+      <c r="B52" s="126" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="139"/>
-      <c r="D52" s="139"/>
-      <c r="E52" s="139" t="s">
+      <c r="C52" s="126"/>
+      <c r="D52" s="126"/>
+      <c r="E52" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="F52" s="139"/>
-      <c r="G52" s="139"/>
+      <c r="F52" s="126"/>
+      <c r="G52" s="126"/>
       <c r="X52" s="22"/>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
@@ -9273,7 +9279,7 @@
       <c r="AE52" s="22"/>
     </row>
     <row r="53" spans="1:31" ht="15" x14ac:dyDescent="0.35">
-      <c r="A53" s="139"/>
+      <c r="A53" s="126"/>
       <c r="B53" s="33" t="s">
         <v>3</v>
       </c>
@@ -9807,123 +9813,123 @@
       <c r="X80" s="37"/>
     </row>
     <row r="81" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="110" t="s">
+      <c r="A81" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="113" t="s">
+      <c r="B81" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="C81" s="113"/>
-      <c r="D81" s="113"/>
-      <c r="E81" s="113"/>
-      <c r="F81" s="113"/>
-      <c r="G81" s="113"/>
-      <c r="H81" s="113"/>
-      <c r="I81" s="113"/>
-      <c r="J81" s="113"/>
-      <c r="K81" s="113"/>
-      <c r="L81" s="113"/>
-      <c r="N81" s="110" t="s">
+      <c r="C81" s="132"/>
+      <c r="D81" s="132"/>
+      <c r="E81" s="132"/>
+      <c r="F81" s="132"/>
+      <c r="G81" s="132"/>
+      <c r="H81" s="132"/>
+      <c r="I81" s="132"/>
+      <c r="J81" s="132"/>
+      <c r="K81" s="132"/>
+      <c r="L81" s="132"/>
+      <c r="N81" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="O81" s="113" t="s">
+      <c r="O81" s="132" t="s">
         <v>81</v>
       </c>
-      <c r="P81" s="113"/>
-      <c r="Q81" s="113"/>
-      <c r="R81" s="113"/>
-      <c r="S81" s="113"/>
-      <c r="T81" s="113"/>
-      <c r="U81" s="113"/>
-      <c r="V81" s="113"/>
-      <c r="W81" s="113"/>
-      <c r="X81" s="113"/>
-      <c r="Y81" s="113"/>
-      <c r="AA81" s="116" t="s">
+      <c r="P81" s="132"/>
+      <c r="Q81" s="132"/>
+      <c r="R81" s="132"/>
+      <c r="S81" s="132"/>
+      <c r="T81" s="132"/>
+      <c r="U81" s="132"/>
+      <c r="V81" s="132"/>
+      <c r="W81" s="132"/>
+      <c r="X81" s="132"/>
+      <c r="Y81" s="132"/>
+      <c r="AA81" s="138" t="s">
         <v>82</v>
       </c>
-      <c r="AB81" s="117"/>
-      <c r="AC81" s="117"/>
-      <c r="AD81" s="117"/>
-      <c r="AE81" s="117"/>
-      <c r="AF81" s="117"/>
-      <c r="AG81" s="117"/>
-      <c r="AH81" s="117"/>
-      <c r="AI81" s="118"/>
-      <c r="AW81" s="110" t="s">
+      <c r="AB81" s="139"/>
+      <c r="AC81" s="139"/>
+      <c r="AD81" s="139"/>
+      <c r="AE81" s="139"/>
+      <c r="AF81" s="139"/>
+      <c r="AG81" s="139"/>
+      <c r="AH81" s="139"/>
+      <c r="AI81" s="140"/>
+      <c r="AW81" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="AX81" s="113" t="s">
+      <c r="AX81" s="132" t="s">
         <v>108</v>
       </c>
-      <c r="AY81" s="113"/>
-      <c r="AZ81" s="113"/>
-      <c r="BA81" s="113"/>
-      <c r="BB81" s="113"/>
-      <c r="BD81" s="110" t="s">
+      <c r="AY81" s="132"/>
+      <c r="AZ81" s="132"/>
+      <c r="BA81" s="132"/>
+      <c r="BB81" s="132"/>
+      <c r="BD81" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="BE81" s="113" t="s">
+      <c r="BE81" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="BF81" s="113"/>
-      <c r="BG81" s="113"/>
-      <c r="BH81" s="113"/>
-      <c r="BI81" s="113"/>
+      <c r="BF81" s="132"/>
+      <c r="BG81" s="132"/>
+      <c r="BH81" s="132"/>
+      <c r="BI81" s="132"/>
     </row>
     <row r="82" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="111"/>
-      <c r="B82" s="113"/>
-      <c r="C82" s="113"/>
-      <c r="D82" s="113"/>
-      <c r="E82" s="113"/>
-      <c r="F82" s="113"/>
-      <c r="G82" s="113"/>
-      <c r="H82" s="113"/>
-      <c r="I82" s="113"/>
-      <c r="J82" s="113"/>
-      <c r="K82" s="113"/>
-      <c r="L82" s="113"/>
-      <c r="N82" s="111"/>
-      <c r="O82" s="113"/>
-      <c r="P82" s="113"/>
-      <c r="Q82" s="113"/>
-      <c r="R82" s="113"/>
-      <c r="S82" s="113"/>
-      <c r="T82" s="113"/>
-      <c r="U82" s="113"/>
-      <c r="V82" s="113"/>
-      <c r="W82" s="113"/>
-      <c r="X82" s="113"/>
-      <c r="Y82" s="113"/>
-      <c r="AA82" s="114" t="s">
+      <c r="A82" s="128"/>
+      <c r="B82" s="132"/>
+      <c r="C82" s="132"/>
+      <c r="D82" s="132"/>
+      <c r="E82" s="132"/>
+      <c r="F82" s="132"/>
+      <c r="G82" s="132"/>
+      <c r="H82" s="132"/>
+      <c r="I82" s="132"/>
+      <c r="J82" s="132"/>
+      <c r="K82" s="132"/>
+      <c r="L82" s="132"/>
+      <c r="N82" s="128"/>
+      <c r="O82" s="132"/>
+      <c r="P82" s="132"/>
+      <c r="Q82" s="132"/>
+      <c r="R82" s="132"/>
+      <c r="S82" s="132"/>
+      <c r="T82" s="132"/>
+      <c r="U82" s="132"/>
+      <c r="V82" s="132"/>
+      <c r="W82" s="132"/>
+      <c r="X82" s="132"/>
+      <c r="Y82" s="132"/>
+      <c r="AA82" s="141" t="s">
         <v>2</v>
       </c>
-      <c r="AB82" s="116" t="s">
+      <c r="AB82" s="138" t="s">
         <v>74</v>
       </c>
-      <c r="AC82" s="117"/>
-      <c r="AD82" s="117"/>
-      <c r="AE82" s="117"/>
-      <c r="AF82" s="117"/>
-      <c r="AG82" s="117"/>
-      <c r="AH82" s="117"/>
-      <c r="AI82" s="118"/>
-      <c r="AW82" s="111"/>
-      <c r="AX82" s="113"/>
-      <c r="AY82" s="113"/>
-      <c r="AZ82" s="113"/>
-      <c r="BA82" s="113"/>
-      <c r="BB82" s="113"/>
-      <c r="BD82" s="111"/>
-      <c r="BE82" s="113"/>
-      <c r="BF82" s="113"/>
-      <c r="BG82" s="113"/>
-      <c r="BH82" s="113"/>
-      <c r="BI82" s="113"/>
+      <c r="AC82" s="139"/>
+      <c r="AD82" s="139"/>
+      <c r="AE82" s="139"/>
+      <c r="AF82" s="139"/>
+      <c r="AG82" s="139"/>
+      <c r="AH82" s="139"/>
+      <c r="AI82" s="140"/>
+      <c r="AW82" s="128"/>
+      <c r="AX82" s="132"/>
+      <c r="AY82" s="132"/>
+      <c r="AZ82" s="132"/>
+      <c r="BA82" s="132"/>
+      <c r="BB82" s="132"/>
+      <c r="BD82" s="128"/>
+      <c r="BE82" s="132"/>
+      <c r="BF82" s="132"/>
+      <c r="BG82" s="132"/>
+      <c r="BH82" s="132"/>
+      <c r="BI82" s="132"/>
     </row>
     <row r="83" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="112"/>
+      <c r="A83" s="129"/>
       <c r="B83" s="76" t="s">
         <v>95</v>
       </c>
@@ -9957,7 +9963,7 @@
       <c r="L83" s="89">
         <v>2020</v>
       </c>
-      <c r="N83" s="112"/>
+      <c r="N83" s="129"/>
       <c r="O83" s="76" t="s">
         <v>95</v>
       </c>
@@ -9991,7 +9997,7 @@
       <c r="Y83" s="89">
         <v>2020</v>
       </c>
-      <c r="AA83" s="115"/>
+      <c r="AA83" s="142"/>
       <c r="AB83" s="76" t="s">
         <v>95</v>
       </c>
@@ -10016,7 +10022,7 @@
       <c r="AI83" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="AW83" s="112"/>
+      <c r="AW83" s="129"/>
       <c r="AX83" s="76" t="s">
         <v>95</v>
       </c>
@@ -10032,7 +10038,7 @@
       <c r="BB83" s="94">
         <v>2020</v>
       </c>
-      <c r="BD83" s="112"/>
+      <c r="BD83" s="129"/>
       <c r="BE83" s="76" t="s">
         <v>95</v>
       </c>
@@ -10201,10 +10207,10 @@
       <c r="BD84" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="BE84" s="141">
+      <c r="BE84" s="110">
         <v>0.16283755500000002</v>
       </c>
-      <c r="BF84" s="142">
+      <c r="BF84" s="111">
         <v>4.7441704699999997E-2</v>
       </c>
       <c r="BG84" s="106">
@@ -10601,19 +10607,19 @@
         <f t="shared" si="12"/>
         <v>-6.3054823529411761E-5</v>
       </c>
-      <c r="AA87" s="114" t="s">
+      <c r="AA87" s="141" t="s">
         <v>2</v>
       </c>
-      <c r="AB87" s="116" t="s">
+      <c r="AB87" s="138" t="s">
         <v>75</v>
       </c>
-      <c r="AC87" s="117"/>
-      <c r="AD87" s="117"/>
-      <c r="AE87" s="117"/>
-      <c r="AF87" s="117"/>
-      <c r="AG87" s="117"/>
-      <c r="AH87" s="117"/>
-      <c r="AI87" s="118"/>
+      <c r="AC87" s="139"/>
+      <c r="AD87" s="139"/>
+      <c r="AE87" s="139"/>
+      <c r="AF87" s="139"/>
+      <c r="AG87" s="139"/>
+      <c r="AH87" s="139"/>
+      <c r="AI87" s="140"/>
       <c r="AW87" s="102" t="s">
         <v>13</v>
       </c>
@@ -10744,7 +10750,7 @@
         <f t="shared" si="12"/>
         <v>-1.4261617647058823E-4</v>
       </c>
-      <c r="AA88" s="115"/>
+      <c r="AA88" s="142"/>
       <c r="AB88" s="76" t="s">
         <v>95</v>
       </c>
@@ -12485,25 +12491,25 @@
       <c r="X110" s="37"/>
     </row>
     <row r="111" spans="1:62" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="127" t="s">
+      <c r="A111" s="137" t="s">
         <v>104</v>
       </c>
-      <c r="B111" s="127"/>
-      <c r="C111" s="127"/>
-      <c r="D111" s="127"/>
-      <c r="E111" s="127"/>
-      <c r="F111" s="127"/>
-      <c r="G111" s="127"/>
-      <c r="H111" s="127"/>
-      <c r="I111" s="127"/>
-      <c r="J111" s="127"/>
-      <c r="K111" s="127"/>
-      <c r="L111" s="127"/>
-      <c r="M111" s="127"/>
-      <c r="N111" s="127"/>
-      <c r="O111" s="127"/>
-      <c r="P111" s="127"/>
-      <c r="Q111" s="127"/>
+      <c r="B111" s="137"/>
+      <c r="C111" s="137"/>
+      <c r="D111" s="137"/>
+      <c r="E111" s="137"/>
+      <c r="F111" s="137"/>
+      <c r="G111" s="137"/>
+      <c r="H111" s="137"/>
+      <c r="I111" s="137"/>
+      <c r="J111" s="137"/>
+      <c r="K111" s="137"/>
+      <c r="L111" s="137"/>
+      <c r="M111" s="137"/>
+      <c r="N111" s="137"/>
+      <c r="O111" s="137"/>
+      <c r="P111" s="137"/>
+      <c r="Q111" s="137"/>
       <c r="R111" s="37"/>
       <c r="S111" s="37"/>
       <c r="T111" s="37"/>
@@ -12513,17 +12519,17 @@
       <c r="X111" s="37"/>
     </row>
     <row r="112" spans="1:62" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="136" t="s">
+      <c r="A112" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="132" t="s">
+      <c r="B112" s="116" t="s">
         <v>85</v>
       </c>
-      <c r="C112" s="133"/>
-      <c r="D112" s="133"/>
-      <c r="E112" s="133"/>
-      <c r="F112" s="133"/>
-      <c r="G112" s="134"/>
+      <c r="C112" s="117"/>
+      <c r="D112" s="117"/>
+      <c r="E112" s="117"/>
+      <c r="F112" s="117"/>
+      <c r="G112" s="118"/>
       <c r="I112" s="73"/>
       <c r="J112" s="86" t="s">
         <v>27</v>
@@ -12542,7 +12548,7 @@
       </c>
     </row>
     <row r="113" spans="1:14" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="137"/>
+      <c r="A113" s="122"/>
       <c r="B113" s="32" t="s">
         <v>70</v>
       </c>
@@ -12586,7 +12592,7 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="138"/>
+      <c r="A114" s="123"/>
       <c r="B114" s="34" t="s">
         <v>63</v>
       </c>
@@ -12634,14 +12640,14 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="I115" s="140" t="s">
+      <c r="I115" s="130" t="s">
         <v>103</v>
       </c>
-      <c r="J115" s="140"/>
-      <c r="K115" s="140"/>
-      <c r="L115" s="140"/>
-      <c r="M115" s="140"/>
-      <c r="N115" s="140"/>
+      <c r="J115" s="130"/>
+      <c r="K115" s="130"/>
+      <c r="L115" s="130"/>
+      <c r="M115" s="130"/>
+      <c r="N115" s="130"/>
     </row>
     <row r="116" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
@@ -13394,31 +13400,31 @@
     </row>
     <row r="132" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="133" spans="1:15" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A133" s="129" t="s">
+      <c r="A133" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="132" t="s">
+      <c r="B133" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="C133" s="133"/>
-      <c r="D133" s="133"/>
-      <c r="E133" s="133"/>
-      <c r="F133" s="133"/>
-      <c r="G133" s="134"/>
-      <c r="I133" s="129" t="s">
+      <c r="C133" s="117"/>
+      <c r="D133" s="117"/>
+      <c r="E133" s="117"/>
+      <c r="F133" s="117"/>
+      <c r="G133" s="118"/>
+      <c r="I133" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="J133" s="132" t="s">
+      <c r="J133" s="116" t="s">
         <v>76</v>
       </c>
-      <c r="K133" s="133"/>
-      <c r="L133" s="133"/>
-      <c r="M133" s="133"/>
-      <c r="N133" s="133"/>
-      <c r="O133" s="134"/>
+      <c r="K133" s="117"/>
+      <c r="L133" s="117"/>
+      <c r="M133" s="117"/>
+      <c r="N133" s="117"/>
+      <c r="O133" s="118"/>
     </row>
     <row r="134" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="130"/>
+      <c r="A134" s="114"/>
       <c r="B134" s="26" t="s">
         <v>71</v>
       </c>
@@ -13437,7 +13443,7 @@
       <c r="G134" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I134" s="130"/>
+      <c r="I134" s="114"/>
       <c r="J134" s="26" t="s">
         <v>71</v>
       </c>
@@ -13458,7 +13464,7 @@
       </c>
     </row>
     <row r="135" spans="1:15" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A135" s="131"/>
+      <c r="A135" s="115"/>
       <c r="B135" s="40" t="s">
         <v>63</v>
       </c>
@@ -13477,7 +13483,7 @@
       <c r="G135" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I135" s="131"/>
+      <c r="I135" s="115"/>
       <c r="J135" s="40" t="s">
         <v>63</v>
       </c>
@@ -14417,22 +14423,22 @@
       <c r="W160" s="37"/>
     </row>
     <row r="161" spans="1:14" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="113" t="s">
+      <c r="A161" s="132" t="s">
         <v>90</v>
       </c>
-      <c r="B161" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="123"/>
-      <c r="D161" s="123"/>
-      <c r="E161" s="123" t="s">
+      <c r="B161" s="134" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="134"/>
+      <c r="D161" s="134"/>
+      <c r="E161" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="F161" s="123"/>
-      <c r="G161" s="123"/>
+      <c r="F161" s="134"/>
+      <c r="G161" s="134"/>
     </row>
     <row r="162" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A162" s="113"/>
+      <c r="A162" s="132"/>
       <c r="B162" s="63" t="s">
         <v>3</v>
       </c>
@@ -15228,9 +15234,9 @@
       <c r="AB185" s="20"/>
     </row>
     <row r="186" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A186" s="124"/>
-      <c r="B186" s="124"/>
-      <c r="C186" s="124"/>
+      <c r="A186" s="135"/>
+      <c r="B186" s="135"/>
+      <c r="C186" s="135"/>
       <c r="D186" s="20"/>
       <c r="E186" s="20"/>
       <c r="F186" s="20"/>
@@ -15405,39 +15411,39 @@
       <c r="W197" s="37"/>
     </row>
     <row r="198" spans="1:23" s="39" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A198" s="120" t="s">
+      <c r="A198" s="124" t="s">
         <v>73</v>
       </c>
-      <c r="B198" s="120"/>
-      <c r="C198" s="120"/>
-      <c r="D198" s="120"/>
-      <c r="E198" s="120"/>
-      <c r="F198" s="120"/>
+      <c r="B198" s="124"/>
+      <c r="C198" s="124"/>
+      <c r="D198" s="124"/>
+      <c r="E198" s="124"/>
+      <c r="F198" s="124"/>
     </row>
     <row r="199" spans="1:23" s="39" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A199" s="125" t="s">
+      <c r="A199" s="136" t="s">
         <v>74</v>
       </c>
-      <c r="B199" s="125"/>
-      <c r="C199" s="125"/>
-      <c r="D199" s="125"/>
-      <c r="E199" s="125"/>
-      <c r="F199" s="125"/>
+      <c r="B199" s="136"/>
+      <c r="C199" s="136"/>
+      <c r="D199" s="136"/>
+      <c r="E199" s="136"/>
+      <c r="F199" s="136"/>
     </row>
     <row r="200" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A200" s="126" t="s">
+      <c r="A200" s="119" t="s">
         <v>46</v>
       </c>
       <c r="B200" s="43"/>
       <c r="C200" s="43"/>
-      <c r="D200" s="126" t="s">
+      <c r="D200" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="E200" s="126"/>
-      <c r="F200" s="126"/>
+      <c r="E200" s="119"/>
+      <c r="F200" s="119"/>
     </row>
     <row r="201" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A201" s="126"/>
+      <c r="A201" s="119"/>
       <c r="B201" s="43"/>
       <c r="C201" s="44" t="s">
         <v>47</v>
@@ -15485,11 +15491,11 @@
       <c r="N202" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="O202" s="119" t="s">
+      <c r="O202" s="131" t="s">
         <v>94</v>
       </c>
-      <c r="P202" s="119"/>
-      <c r="Q202" s="119"/>
+      <c r="P202" s="131"/>
+      <c r="Q202" s="131"/>
     </row>
     <row r="203" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A203" s="45" t="s">
@@ -16264,30 +16270,30 @@
       </c>
     </row>
     <row r="219" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A219" s="135" t="s">
+      <c r="A219" s="120" t="s">
         <v>75</v>
       </c>
-      <c r="B219" s="135"/>
-      <c r="C219" s="135"/>
-      <c r="D219" s="135"/>
-      <c r="E219" s="135"/>
-      <c r="F219" s="135"/>
+      <c r="B219" s="120"/>
+      <c r="C219" s="120"/>
+      <c r="D219" s="120"/>
+      <c r="E219" s="120"/>
+      <c r="F219" s="120"/>
       <c r="L219" s="104"/>
     </row>
     <row r="220" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A220" s="122" t="s">
+      <c r="A220" s="133" t="s">
         <v>2</v>
       </c>
       <c r="B220" s="43"/>
       <c r="C220" s="43"/>
-      <c r="D220" s="126" t="s">
+      <c r="D220" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="E220" s="126"/>
-      <c r="F220" s="126"/>
+      <c r="E220" s="119"/>
+      <c r="F220" s="119"/>
     </row>
     <row r="221" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A221" s="122"/>
+      <c r="A221" s="133"/>
       <c r="B221" s="43"/>
       <c r="C221" s="44" t="s">
         <v>47</v>
@@ -16335,11 +16341,11 @@
       <c r="N222" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="O222" s="119" t="s">
+      <c r="O222" s="131" t="s">
         <v>93</v>
       </c>
-      <c r="P222" s="119"/>
-      <c r="Q222" s="119"/>
+      <c r="P222" s="131"/>
+      <c r="Q222" s="131"/>
     </row>
     <row r="223" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A223" s="45" t="s">
@@ -17194,6 +17200,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="AW81:AW83"/>
+    <mergeCell ref="AX81:BB82"/>
+    <mergeCell ref="BD81:BD83"/>
+    <mergeCell ref="BE81:BI82"/>
+    <mergeCell ref="AA87:AA88"/>
+    <mergeCell ref="AA81:AI81"/>
+    <mergeCell ref="AB82:AI82"/>
+    <mergeCell ref="AB87:AI87"/>
+    <mergeCell ref="O81:Y82"/>
+    <mergeCell ref="AA82:AA83"/>
+    <mergeCell ref="O222:Q222"/>
+    <mergeCell ref="O202:Q202"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="E161:G161"/>
+    <mergeCell ref="A186:C186"/>
+    <mergeCell ref="A198:F198"/>
+    <mergeCell ref="A199:F199"/>
+    <mergeCell ref="D200:F200"/>
+    <mergeCell ref="D220:F220"/>
+    <mergeCell ref="A111:Q111"/>
+    <mergeCell ref="N81:N83"/>
+    <mergeCell ref="B81:L82"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="I133:I135"/>
     <mergeCell ref="J133:O133"/>
@@ -17210,31 +17241,6 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="I115:N115"/>
-    <mergeCell ref="O222:Q222"/>
-    <mergeCell ref="O202:Q202"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A161:A162"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="E161:G161"/>
-    <mergeCell ref="A186:C186"/>
-    <mergeCell ref="A198:F198"/>
-    <mergeCell ref="A199:F199"/>
-    <mergeCell ref="D200:F200"/>
-    <mergeCell ref="D220:F220"/>
-    <mergeCell ref="A111:Q111"/>
-    <mergeCell ref="N81:N83"/>
-    <mergeCell ref="B81:L82"/>
-    <mergeCell ref="AA81:AI81"/>
-    <mergeCell ref="AB82:AI82"/>
-    <mergeCell ref="AB87:AI87"/>
-    <mergeCell ref="O81:Y82"/>
-    <mergeCell ref="AA82:AA83"/>
-    <mergeCell ref="AW81:AW83"/>
-    <mergeCell ref="AX81:BB82"/>
-    <mergeCell ref="BD81:BD83"/>
-    <mergeCell ref="BE81:BI82"/>
-    <mergeCell ref="AA87:AA88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update baseline acts values for male bias and female adjustment
Related to #73
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11220" windowHeight="6500" tabRatio="369"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11220" windowHeight="6495" tabRatio="369"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -508,7 +508,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000;\-0.00000;0"/>
     <numFmt numFmtId="165" formatCode="###;\-###;0"/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="39" x14ac:knownFonts="1">
     <font>
@@ -1671,6 +1671,19 @@
     <xf numFmtId="2" fontId="29" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="48"/>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="27" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1707,6 +1720,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1718,9 +1734,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1758,19 +1771,6 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="48"/>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="27" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1882,7 +1882,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2397,7 +2396,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2520,7 +2518,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3216,7 +3213,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3344,7 +3340,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4033,7 +4028,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8253,55 +8247,55 @@
   <dimension ref="A1:BJ245"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A193" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P213" sqref="P213"/>
+      <selection activeCell="C224" sqref="C224"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
     <col min="14" max="14" width="25" customWidth="1"/>
-    <col min="15" max="15" width="11.81640625" customWidth="1"/>
-    <col min="16" max="16" width="17.7265625" customWidth="1"/>
-    <col min="17" max="17" width="19.81640625" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.85546875" customWidth="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.81640625" customWidth="1"/>
-    <col min="21" max="21" width="15.453125" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" customWidth="1"/>
     <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.81640625" customWidth="1"/>
-    <col min="24" max="24" width="13.26953125" customWidth="1"/>
-    <col min="25" max="25" width="14.1796875" customWidth="1"/>
-    <col min="26" max="26" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.26953125" customWidth="1"/>
-    <col min="28" max="29" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" customWidth="1"/>
+    <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" customWidth="1"/>
+    <col min="28" max="29" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.1796875" customWidth="1"/>
+    <col min="32" max="32" width="14.140625" customWidth="1"/>
     <col min="33" max="34" width="12" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.81640625" customWidth="1"/>
-    <col min="49" max="49" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="54" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="58" max="60" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.85546875" customWidth="1"/>
+    <col min="49" max="49" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="54" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="60" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>103</v>
       </c>
@@ -8330,17 +8324,17 @@
       <c r="X1" s="37"/>
       <c r="Y1" s="37"/>
     </row>
-    <row r="2" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="119" t="s">
+    <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="126" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -8359,7 +8353,7 @@
       <c r="X2" s="37"/>
       <c r="Y2" s="37"/>
     </row>
-    <row r="3" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>77</v>
       </c>
@@ -8388,20 +8382,20 @@
       <c r="X3" s="37"/>
       <c r="Y3" s="37"/>
     </row>
-    <row r="4" spans="1:25" s="39" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="119" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="113"/>
-      <c r="D4" s="112" t="s">
+      <c r="C4" s="120"/>
+      <c r="D4" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="113"/>
-    </row>
-    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.35">
+      <c r="E4" s="120"/>
+    </row>
+    <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="51" t="s">
         <v>0</v>
@@ -8418,7 +8412,7 @@
       <c r="F5" s="25"/>
       <c r="G5" s="39"/>
     </row>
-    <row r="6" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -8441,7 +8435,7 @@
       <c r="H6" s="39"/>
       <c r="I6" s="39"/>
     </row>
-    <row r="7" spans="1:25" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -8464,7 +8458,7 @@
       <c r="H7" s="39"/>
       <c r="I7" s="39"/>
     </row>
-    <row r="8" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -8487,7 +8481,7 @@
       <c r="H8" s="39"/>
       <c r="I8" s="39"/>
     </row>
-    <row r="9" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -8510,7 +8504,7 @@
       <c r="H9" s="39"/>
       <c r="I9" s="39"/>
     </row>
-    <row r="10" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -8533,7 +8527,7 @@
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
     </row>
-    <row r="11" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -8556,7 +8550,7 @@
       <c r="H11" s="39"/>
       <c r="I11" s="39"/>
     </row>
-    <row r="12" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -8579,7 +8573,7 @@
       <c r="H12" s="39"/>
       <c r="I12" s="39"/>
     </row>
-    <row r="13" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -8602,7 +8596,7 @@
       <c r="H13" s="39"/>
       <c r="I13" s="39"/>
     </row>
-    <row r="14" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -8625,7 +8619,7 @@
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
     </row>
-    <row r="15" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -8648,7 +8642,7 @@
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
     </row>
-    <row r="16" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
@@ -8671,7 +8665,7 @@
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
     </row>
-    <row r="17" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -8694,7 +8688,7 @@
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>41</v>
       </c>
@@ -8717,7 +8711,7 @@
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>42</v>
       </c>
@@ -8740,7 +8734,7 @@
       <c r="H19" s="39"/>
       <c r="I19" s="39"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>43</v>
       </c>
@@ -8763,7 +8757,7 @@
       <c r="H20" s="39"/>
       <c r="I20" s="39"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>44</v>
       </c>
@@ -8786,7 +8780,7 @@
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
     </row>
-    <row r="22" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>23</v>
       </c>
@@ -8813,26 +8807,26 @@
       <c r="G22" s="25"/>
       <c r="X22" s="13"/>
     </row>
-    <row r="23" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="F26" s="31"/>
     </row>
-    <row r="27" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="112" t="s">
+      <c r="B27" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="113"/>
-    </row>
-    <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.35">
+      <c r="C27" s="120"/>
+    </row>
+    <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="33" t="s">
         <v>0</v>
@@ -8842,7 +8836,7 @@
       </c>
       <c r="F28" s="15"/>
     </row>
-    <row r="29" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>6</v>
       </c>
@@ -8855,7 +8849,7 @@
         <v>234484.12029553554</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>9</v>
       </c>
@@ -8868,7 +8862,7 @@
         <v>163173.86739175185</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>12</v>
       </c>
@@ -8882,7 +8876,7 @@
       </c>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>13</v>
       </c>
@@ -8895,7 +8889,7 @@
         <v>114321.67152989602</v>
       </c>
     </row>
-    <row r="33" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>14</v>
       </c>
@@ -8908,7 +8902,7 @@
         <v>99000.049567582799</v>
       </c>
     </row>
-    <row r="34" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>15</v>
       </c>
@@ -8921,7 +8915,7 @@
         <v>87233.488605604201</v>
       </c>
     </row>
-    <row r="35" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>16</v>
       </c>
@@ -8934,7 +8928,7 @@
         <v>80038.973435362466</v>
       </c>
     </row>
-    <row r="36" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>17</v>
       </c>
@@ -8956,7 +8950,7 @@
       <c r="AE36" s="6"/>
       <c r="AF36" s="13"/>
     </row>
-    <row r="37" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>19</v>
       </c>
@@ -8977,7 +8971,7 @@
       <c r="AD37" s="14"/>
       <c r="AE37" s="14"/>
     </row>
-    <row r="38" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>20</v>
       </c>
@@ -8998,7 +8992,7 @@
       <c r="AD38" s="22"/>
       <c r="AE38" s="22"/>
     </row>
-    <row r="39" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
@@ -9019,7 +9013,7 @@
       <c r="AD39" s="23"/>
       <c r="AE39" s="23"/>
     </row>
-    <row r="40" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>22</v>
       </c>
@@ -9040,7 +9034,7 @@
       <c r="AD40" s="23"/>
       <c r="AE40" s="23"/>
     </row>
-    <row r="41" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>41</v>
       </c>
@@ -9061,7 +9055,7 @@
       <c r="AD41" s="23"/>
       <c r="AE41" s="23"/>
     </row>
-    <row r="42" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>42</v>
       </c>
@@ -9082,7 +9076,7 @@
       <c r="AD42" s="24"/>
       <c r="AE42" s="24"/>
     </row>
-    <row r="43" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>43</v>
       </c>
@@ -9103,7 +9097,7 @@
       <c r="AD43" s="24"/>
       <c r="AE43" s="24"/>
     </row>
-    <row r="44" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>44</v>
       </c>
@@ -9124,7 +9118,7 @@
       <c r="AD44" s="24"/>
       <c r="AE44" s="24"/>
     </row>
-    <row r="45" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="X45" s="24"/>
       <c r="Y45" s="24"/>
       <c r="Z45" s="24"/>
@@ -9134,7 +9128,7 @@
       <c r="AD45" s="24"/>
       <c r="AE45" s="24"/>
     </row>
-    <row r="46" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="X46" s="24"/>
       <c r="Y46" s="24"/>
       <c r="Z46" s="24"/>
@@ -9144,7 +9138,7 @@
       <c r="AD46" s="24"/>
       <c r="AE46" s="24"/>
     </row>
-    <row r="47" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="X47" s="24"/>
       <c r="Y47" s="24"/>
       <c r="Z47" s="24"/>
@@ -9154,7 +9148,7 @@
       <c r="AD47" s="24"/>
       <c r="AE47" s="24"/>
     </row>
-    <row r="48" spans="1:32" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="X48" s="24"/>
       <c r="Y48" s="24"/>
       <c r="Z48" s="24"/>
@@ -9164,7 +9158,7 @@
       <c r="AD48" s="24"/>
       <c r="AE48" s="24"/>
     </row>
-    <row r="49" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="X49" s="24"/>
       <c r="Y49" s="24"/>
       <c r="Z49" s="24"/>
@@ -9174,7 +9168,7 @@
       <c r="AD49" s="24"/>
       <c r="AE49" s="24"/>
     </row>
-    <row r="50" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
         <v>82</v>
       </c>
@@ -9209,7 +9203,7 @@
       <c r="AD50" s="24"/>
       <c r="AE50" s="24"/>
     </row>
-    <row r="51" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="38" t="s">
         <v>56</v>
       </c>
@@ -9244,20 +9238,20 @@
       <c r="AD51" s="24"/>
       <c r="AE51" s="24"/>
     </row>
-    <row r="52" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="129" t="s">
+    <row r="52" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="129" t="s">
+      <c r="B52" s="136" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="129"/>
-      <c r="D52" s="129"/>
-      <c r="E52" s="129" t="s">
+      <c r="C52" s="136"/>
+      <c r="D52" s="136"/>
+      <c r="E52" s="136" t="s">
         <v>55</v>
       </c>
-      <c r="F52" s="129"/>
-      <c r="G52" s="129"/>
+      <c r="F52" s="136"/>
+      <c r="G52" s="136"/>
       <c r="X52" s="22"/>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
@@ -9267,8 +9261,8 @@
       <c r="AD52" s="22"/>
       <c r="AE52" s="22"/>
     </row>
-    <row r="53" spans="1:31" ht="15" x14ac:dyDescent="0.35">
-      <c r="A53" s="129"/>
+    <row r="53" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="136"/>
       <c r="B53" s="33" t="s">
         <v>3</v>
       </c>
@@ -9296,7 +9290,7 @@
       <c r="AD53" s="25"/>
       <c r="AE53" s="25"/>
     </row>
-    <row r="54" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>6</v>
       </c>
@@ -9320,7 +9314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>9</v>
       </c>
@@ -9344,7 +9338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>12</v>
       </c>
@@ -9369,7 +9363,7 @@
         <v>5.0000000000000183E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>13</v>
       </c>
@@ -9392,7 +9386,7 @@
         <v>2.4213075060532689E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>14</v>
       </c>
@@ -9415,7 +9409,7 @@
         <v>1.6393442622950817E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:31" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>15</v>
       </c>
@@ -9439,7 +9433,7 @@
       </c>
       <c r="O59" s="12"/>
     </row>
-    <row r="60" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>18</v>
       </c>
@@ -9463,7 +9457,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>17</v>
       </c>
@@ -9486,7 +9480,7 @@
         <v>1.1547344110854503E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>19</v>
       </c>
@@ -9511,7 +9505,7 @@
         <v>9.9999999999988987E-5</v>
       </c>
     </row>
-    <row r="63" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>20</v>
       </c>
@@ -9535,7 +9529,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>21</v>
       </c>
@@ -9559,7 +9553,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>22</v>
       </c>
@@ -9583,7 +9577,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
         <v>41</v>
       </c>
@@ -9607,7 +9601,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
         <v>42</v>
       </c>
@@ -9631,7 +9625,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
         <v>43</v>
       </c>
@@ -9655,7 +9649,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
         <v>44</v>
       </c>
@@ -9679,7 +9673,7 @@
         <v>1.4367816091954023E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="31" t="s">
         <v>50</v>
       </c>
@@ -9708,7 +9702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="31" t="s">
         <v>51</v>
       </c>
@@ -9717,7 +9711,7 @@
         <v>0.83084071366534329</v>
       </c>
     </row>
-    <row r="78" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="36" t="s">
         <v>57</v>
       </c>
@@ -9745,7 +9739,7 @@
       <c r="W78" s="37"/>
       <c r="X78" s="37"/>
     </row>
-    <row r="79" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="38" t="s">
         <v>105</v>
       </c>
@@ -9773,7 +9767,7 @@
       <c r="W79" s="37"/>
       <c r="X79" s="37"/>
     </row>
-    <row r="80" spans="1:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="36" t="s">
         <v>104</v>
       </c>
@@ -9801,124 +9795,124 @@
       <c r="W80" s="37"/>
       <c r="X80" s="37"/>
     </row>
-    <row r="81" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="102" t="s">
+    <row r="81" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="105" t="s">
+      <c r="B81" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="105"/>
-      <c r="D81" s="105"/>
-      <c r="E81" s="105"/>
-      <c r="F81" s="105"/>
-      <c r="G81" s="105"/>
-      <c r="H81" s="105"/>
-      <c r="I81" s="105"/>
-      <c r="J81" s="105"/>
-      <c r="K81" s="105"/>
-      <c r="L81" s="105"/>
-      <c r="N81" s="102" t="s">
+      <c r="C81" s="112"/>
+      <c r="D81" s="112"/>
+      <c r="E81" s="112"/>
+      <c r="F81" s="112"/>
+      <c r="G81" s="112"/>
+      <c r="H81" s="112"/>
+      <c r="I81" s="112"/>
+      <c r="J81" s="112"/>
+      <c r="K81" s="112"/>
+      <c r="L81" s="112"/>
+      <c r="N81" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="O81" s="105" t="s">
+      <c r="O81" s="112" t="s">
         <v>79</v>
       </c>
-      <c r="P81" s="105"/>
-      <c r="Q81" s="105"/>
-      <c r="R81" s="105"/>
-      <c r="S81" s="105"/>
-      <c r="T81" s="105"/>
-      <c r="U81" s="105"/>
-      <c r="V81" s="105"/>
-      <c r="W81" s="105"/>
-      <c r="X81" s="105"/>
-      <c r="Y81" s="105"/>
-      <c r="AA81" s="108" t="s">
+      <c r="P81" s="112"/>
+      <c r="Q81" s="112"/>
+      <c r="R81" s="112"/>
+      <c r="S81" s="112"/>
+      <c r="T81" s="112"/>
+      <c r="U81" s="112"/>
+      <c r="V81" s="112"/>
+      <c r="W81" s="112"/>
+      <c r="X81" s="112"/>
+      <c r="Y81" s="112"/>
+      <c r="AA81" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="AB81" s="109"/>
-      <c r="AC81" s="109"/>
-      <c r="AD81" s="109"/>
-      <c r="AE81" s="109"/>
-      <c r="AF81" s="109"/>
-      <c r="AG81" s="109"/>
-      <c r="AH81" s="109"/>
-      <c r="AI81" s="110"/>
-      <c r="AW81" s="102" t="s">
+      <c r="AB81" s="116"/>
+      <c r="AC81" s="116"/>
+      <c r="AD81" s="116"/>
+      <c r="AE81" s="116"/>
+      <c r="AF81" s="116"/>
+      <c r="AG81" s="116"/>
+      <c r="AH81" s="116"/>
+      <c r="AI81" s="117"/>
+      <c r="AW81" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="AX81" s="105" t="s">
+      <c r="AX81" s="112" t="s">
         <v>106</v>
       </c>
-      <c r="AY81" s="105"/>
-      <c r="AZ81" s="105"/>
-      <c r="BA81" s="105"/>
-      <c r="BB81" s="105"/>
-      <c r="BD81" s="102" t="s">
+      <c r="AY81" s="112"/>
+      <c r="AZ81" s="112"/>
+      <c r="BA81" s="112"/>
+      <c r="BB81" s="112"/>
+      <c r="BD81" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="BE81" s="105" t="s">
+      <c r="BE81" s="112" t="s">
         <v>107</v>
       </c>
-      <c r="BF81" s="105"/>
-      <c r="BG81" s="105"/>
-      <c r="BH81" s="105"/>
-      <c r="BI81" s="105"/>
-    </row>
-    <row r="82" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="103"/>
-      <c r="B82" s="105"/>
-      <c r="C82" s="105"/>
-      <c r="D82" s="105"/>
-      <c r="E82" s="105"/>
-      <c r="F82" s="105"/>
-      <c r="G82" s="105"/>
-      <c r="H82" s="105"/>
-      <c r="I82" s="105"/>
-      <c r="J82" s="105"/>
-      <c r="K82" s="105"/>
-      <c r="L82" s="105"/>
-      <c r="N82" s="103"/>
-      <c r="O82" s="105"/>
-      <c r="P82" s="105"/>
-      <c r="Q82" s="105"/>
-      <c r="R82" s="105"/>
-      <c r="S82" s="105"/>
-      <c r="T82" s="105"/>
-      <c r="U82" s="105"/>
-      <c r="V82" s="105"/>
-      <c r="W82" s="105"/>
-      <c r="X82" s="105"/>
-      <c r="Y82" s="105"/>
-      <c r="AA82" s="106" t="s">
+      <c r="BF81" s="112"/>
+      <c r="BG81" s="112"/>
+      <c r="BH81" s="112"/>
+      <c r="BI81" s="112"/>
+    </row>
+    <row r="82" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="110"/>
+      <c r="B82" s="112"/>
+      <c r="C82" s="112"/>
+      <c r="D82" s="112"/>
+      <c r="E82" s="112"/>
+      <c r="F82" s="112"/>
+      <c r="G82" s="112"/>
+      <c r="H82" s="112"/>
+      <c r="I82" s="112"/>
+      <c r="J82" s="112"/>
+      <c r="K82" s="112"/>
+      <c r="L82" s="112"/>
+      <c r="N82" s="110"/>
+      <c r="O82" s="112"/>
+      <c r="P82" s="112"/>
+      <c r="Q82" s="112"/>
+      <c r="R82" s="112"/>
+      <c r="S82" s="112"/>
+      <c r="T82" s="112"/>
+      <c r="U82" s="112"/>
+      <c r="V82" s="112"/>
+      <c r="W82" s="112"/>
+      <c r="X82" s="112"/>
+      <c r="Y82" s="112"/>
+      <c r="AA82" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="AB82" s="108" t="s">
+      <c r="AB82" s="115" t="s">
         <v>72</v>
       </c>
-      <c r="AC82" s="109"/>
-      <c r="AD82" s="109"/>
-      <c r="AE82" s="109"/>
-      <c r="AF82" s="109"/>
-      <c r="AG82" s="109"/>
-      <c r="AH82" s="109"/>
-      <c r="AI82" s="110"/>
-      <c r="AW82" s="103"/>
-      <c r="AX82" s="105"/>
-      <c r="AY82" s="105"/>
-      <c r="AZ82" s="105"/>
-      <c r="BA82" s="105"/>
-      <c r="BB82" s="105"/>
-      <c r="BD82" s="103"/>
-      <c r="BE82" s="105"/>
-      <c r="BF82" s="105"/>
-      <c r="BG82" s="105"/>
-      <c r="BH82" s="105"/>
-      <c r="BI82" s="105"/>
-    </row>
-    <row r="83" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="104"/>
+      <c r="AC82" s="116"/>
+      <c r="AD82" s="116"/>
+      <c r="AE82" s="116"/>
+      <c r="AF82" s="116"/>
+      <c r="AG82" s="116"/>
+      <c r="AH82" s="116"/>
+      <c r="AI82" s="117"/>
+      <c r="AW82" s="110"/>
+      <c r="AX82" s="112"/>
+      <c r="AY82" s="112"/>
+      <c r="AZ82" s="112"/>
+      <c r="BA82" s="112"/>
+      <c r="BB82" s="112"/>
+      <c r="BD82" s="110"/>
+      <c r="BE82" s="112"/>
+      <c r="BF82" s="112"/>
+      <c r="BG82" s="112"/>
+      <c r="BH82" s="112"/>
+      <c r="BI82" s="112"/>
+    </row>
+    <row r="83" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="111"/>
       <c r="B83" s="71" t="s">
         <v>93</v>
       </c>
@@ -9952,7 +9946,7 @@
       <c r="L83" s="84">
         <v>2020</v>
       </c>
-      <c r="N83" s="104"/>
+      <c r="N83" s="111"/>
       <c r="O83" s="71" t="s">
         <v>93</v>
       </c>
@@ -9986,7 +9980,7 @@
       <c r="Y83" s="84">
         <v>2020</v>
       </c>
-      <c r="AA83" s="107"/>
+      <c r="AA83" s="114"/>
       <c r="AB83" s="71" t="s">
         <v>93</v>
       </c>
@@ -10011,7 +10005,7 @@
       <c r="AI83" s="71" t="s">
         <v>98</v>
       </c>
-      <c r="AW83" s="104"/>
+      <c r="AW83" s="111"/>
       <c r="AX83" s="71" t="s">
         <v>93</v>
       </c>
@@ -10027,7 +10021,7 @@
       <c r="BB83" s="89">
         <v>2020</v>
       </c>
-      <c r="BD83" s="104"/>
+      <c r="BD83" s="111"/>
       <c r="BE83" s="71" t="s">
         <v>93</v>
       </c>
@@ -10044,7 +10038,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="84" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="69" t="s">
         <v>6</v>
       </c>
@@ -10217,7 +10211,7 @@
         <v>-3.6249629411764703E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="69" t="s">
         <v>9</v>
       </c>
@@ -10374,7 +10368,7 @@
         <v>-3.5941176470588238E-5</v>
       </c>
     </row>
-    <row r="86" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="69" t="s">
         <v>12</v>
       </c>
@@ -10513,7 +10507,7 @@
         <v>-3.3058823529411766E-5</v>
       </c>
     </row>
-    <row r="87" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="69" t="s">
         <v>13</v>
       </c>
@@ -10596,19 +10590,19 @@
         <f t="shared" si="12"/>
         <v>-6.3054823529411761E-5</v>
       </c>
-      <c r="AA87" s="106" t="s">
+      <c r="AA87" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="AB87" s="108" t="s">
+      <c r="AB87" s="115" t="s">
         <v>73</v>
       </c>
-      <c r="AC87" s="109"/>
-      <c r="AD87" s="109"/>
-      <c r="AE87" s="109"/>
-      <c r="AF87" s="109"/>
-      <c r="AG87" s="109"/>
-      <c r="AH87" s="109"/>
-      <c r="AI87" s="110"/>
+      <c r="AC87" s="116"/>
+      <c r="AD87" s="116"/>
+      <c r="AE87" s="116"/>
+      <c r="AF87" s="116"/>
+      <c r="AG87" s="116"/>
+      <c r="AH87" s="116"/>
+      <c r="AI87" s="117"/>
       <c r="AW87" s="94" t="s">
         <v>13</v>
       </c>
@@ -10656,7 +10650,7 @@
         <v>-6.3586647058823525E-5</v>
       </c>
     </row>
-    <row r="88" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="69" t="s">
         <v>14</v>
       </c>
@@ -10739,7 +10733,7 @@
         <f t="shared" si="12"/>
         <v>-1.4261617647058823E-4</v>
       </c>
-      <c r="AA88" s="107"/>
+      <c r="AA88" s="114"/>
       <c r="AB88" s="71" t="s">
         <v>93</v>
       </c>
@@ -10811,7 +10805,7 @@
         <v>-1.9651323529411765E-4</v>
       </c>
     </row>
-    <row r="89" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="69" t="s">
         <v>15</v>
       </c>
@@ -10968,7 +10962,7 @@
         <v>-3.4676770588235289E-4</v>
       </c>
     </row>
-    <row r="90" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="69" t="s">
         <v>18</v>
       </c>
@@ -11125,7 +11119,7 @@
         <v>-3.3813217647058825E-4</v>
       </c>
     </row>
-    <row r="91" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="83" t="s">
         <v>17</v>
       </c>
@@ -11255,7 +11249,7 @@
         <v>-3.2472470588235293E-4</v>
       </c>
     </row>
-    <row r="92" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="83" t="s">
         <v>19</v>
       </c>
@@ -11385,7 +11379,7 @@
         <v>-2.6471335294117647E-4</v>
       </c>
     </row>
-    <row r="93" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="83" t="s">
         <v>20</v>
       </c>
@@ -11515,7 +11509,7 @@
         <v>-2.45104E-4</v>
       </c>
     </row>
-    <row r="94" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="83" t="s">
         <v>21</v>
       </c>
@@ -11645,7 +11639,7 @@
         <v>-3.0227070588235294E-4</v>
       </c>
     </row>
-    <row r="95" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="83" t="s">
         <v>22</v>
       </c>
@@ -11775,7 +11769,7 @@
         <v>-3.3719570588235288E-4</v>
       </c>
     </row>
-    <row r="96" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="79" t="s">
         <v>41</v>
       </c>
@@ -11905,7 +11899,7 @@
         <v>-5.0459635294117645E-4</v>
       </c>
     </row>
-    <row r="97" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="79" t="s">
         <v>42</v>
       </c>
@@ -12035,7 +12029,7 @@
         <v>-6.8948405882352935E-4</v>
       </c>
     </row>
-    <row r="98" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="79" t="s">
         <v>43</v>
       </c>
@@ -12165,7 +12159,7 @@
         <v>-1.1042807647058824E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="79" t="s">
         <v>44</v>
       </c>
@@ -12295,23 +12289,23 @@
         <v>-1.0324471764705883E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:62" x14ac:dyDescent="0.25">
       <c r="I102" s="49"/>
       <c r="J102" s="49"/>
       <c r="K102" s="48"/>
       <c r="N102" s="70"/>
     </row>
-    <row r="103" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:62" x14ac:dyDescent="0.25">
       <c r="I103" s="49"/>
       <c r="J103" s="49"/>
       <c r="K103" s="48"/>
     </row>
-    <row r="104" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:62" x14ac:dyDescent="0.25">
       <c r="I104" s="49"/>
       <c r="J104" s="49"/>
       <c r="K104" s="48"/>
     </row>
-    <row r="105" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="36" t="s">
         <v>58</v>
       </c>
@@ -12339,7 +12333,7 @@
       <c r="W105" s="37"/>
       <c r="X105" s="37"/>
     </row>
-    <row r="106" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="38" t="s">
         <v>59</v>
       </c>
@@ -12367,7 +12361,7 @@
       <c r="W106" s="37"/>
       <c r="X106" s="37"/>
     </row>
-    <row r="107" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="38" t="s">
         <v>60</v>
       </c>
@@ -12395,7 +12389,7 @@
       <c r="W107" s="37"/>
       <c r="X107" s="37"/>
     </row>
-    <row r="108" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="38" t="s">
         <v>86</v>
       </c>
@@ -12423,7 +12417,7 @@
       <c r="W108" s="37"/>
       <c r="X108" s="37"/>
     </row>
-    <row r="109" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="38" t="s">
         <v>85</v>
       </c>
@@ -12451,7 +12445,7 @@
       <c r="W109" s="37"/>
       <c r="X109" s="37"/>
     </row>
-    <row r="110" spans="1:62" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="55" t="s">
         <v>87</v>
       </c>
@@ -12479,26 +12473,26 @@
       <c r="W110" s="37"/>
       <c r="X110" s="37"/>
     </row>
-    <row r="111" spans="1:62" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="118" t="s">
+    <row r="111" spans="1:62" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="121" t="s">
         <v>102</v>
       </c>
-      <c r="B111" s="118"/>
-      <c r="C111" s="118"/>
-      <c r="D111" s="118"/>
-      <c r="E111" s="118"/>
-      <c r="F111" s="118"/>
-      <c r="G111" s="118"/>
-      <c r="H111" s="118"/>
-      <c r="I111" s="118"/>
-      <c r="J111" s="118"/>
-      <c r="K111" s="118"/>
-      <c r="L111" s="118"/>
-      <c r="M111" s="118"/>
-      <c r="N111" s="118"/>
-      <c r="O111" s="118"/>
-      <c r="P111" s="118"/>
-      <c r="Q111" s="118"/>
+      <c r="B111" s="121"/>
+      <c r="C111" s="121"/>
+      <c r="D111" s="121"/>
+      <c r="E111" s="121"/>
+      <c r="F111" s="121"/>
+      <c r="G111" s="121"/>
+      <c r="H111" s="121"/>
+      <c r="I111" s="121"/>
+      <c r="J111" s="121"/>
+      <c r="K111" s="121"/>
+      <c r="L111" s="121"/>
+      <c r="M111" s="121"/>
+      <c r="N111" s="121"/>
+      <c r="O111" s="121"/>
+      <c r="P111" s="121"/>
+      <c r="Q111" s="121"/>
       <c r="R111" s="37"/>
       <c r="S111" s="37"/>
       <c r="T111" s="37"/>
@@ -12507,18 +12501,18 @@
       <c r="W111" s="37"/>
       <c r="X111" s="37"/>
     </row>
-    <row r="112" spans="1:62" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="126" t="s">
+    <row r="112" spans="1:62" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="123" t="s">
+      <c r="B112" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="C112" s="124"/>
-      <c r="D112" s="124"/>
-      <c r="E112" s="124"/>
-      <c r="F112" s="124"/>
-      <c r="G112" s="125"/>
+      <c r="C112" s="131"/>
+      <c r="D112" s="131"/>
+      <c r="E112" s="131"/>
+      <c r="F112" s="131"/>
+      <c r="G112" s="132"/>
       <c r="I112" s="68"/>
       <c r="J112" s="81" t="s">
         <v>27</v>
@@ -12536,8 +12530,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="127"/>
+    <row r="113" spans="1:14" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="134"/>
       <c r="B113" s="32" t="s">
         <v>68</v>
       </c>
@@ -12580,8 +12574,8 @@
         <v>0.41000000000000003</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="128"/>
+    <row r="114" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="135"/>
       <c r="B114" s="34" t="s">
         <v>61</v>
       </c>
@@ -12601,7 +12595,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>6</v>
       </c>
@@ -12629,16 +12623,16 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="I115" s="130" t="s">
+      <c r="I115" s="137" t="s">
         <v>101</v>
       </c>
-      <c r="J115" s="130"/>
-      <c r="K115" s="130"/>
-      <c r="L115" s="130"/>
-      <c r="M115" s="130"/>
-      <c r="N115" s="130"/>
-    </row>
-    <row r="116" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J115" s="137"/>
+      <c r="K115" s="137"/>
+      <c r="L115" s="137"/>
+      <c r="M115" s="137"/>
+      <c r="N115" s="137"/>
+    </row>
+    <row r="116" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>9</v>
       </c>
@@ -12685,7 +12679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>12</v>
       </c>
@@ -12732,7 +12726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>13</v>
       </c>
@@ -12779,7 +12773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>14</v>
       </c>
@@ -12826,7 +12820,7 @@
         <v>5.7974000000000005E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>15</v>
       </c>
@@ -12873,7 +12867,7 @@
         <v>0.11398000000000003</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>18</v>
       </c>
@@ -12920,7 +12914,7 @@
         <v>0.11627600000000002</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>17</v>
       </c>
@@ -12967,7 +12961,7 @@
         <v>8.6592000000000002E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>19</v>
       </c>
@@ -13014,7 +13008,7 @@
         <v>5.5268000000000005E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>20</v>
       </c>
@@ -13061,7 +13055,7 @@
         <v>2.2222000000000002E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>21</v>
       </c>
@@ -13108,7 +13102,7 @@
         <v>7.2160000000000011E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>22</v>
       </c>
@@ -13155,7 +13149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="16" t="s">
         <v>41</v>
       </c>
@@ -13202,7 +13196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="16" t="s">
         <v>42</v>
       </c>
@@ -13249,7 +13243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="16" t="s">
         <v>43</v>
       </c>
@@ -13296,7 +13290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="16" t="s">
         <v>44</v>
       </c>
@@ -13343,7 +13337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B131">
         <f t="shared" ref="B131:G131" si="19">5*SUM(B118:B124)</f>
         <v>6.1644000000000005</v>
@@ -13387,33 +13381,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="133" spans="1:15" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A133" s="120" t="s">
+    <row r="132" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="133" spans="1:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="123" t="s">
+      <c r="B133" s="130" t="s">
         <v>84</v>
       </c>
-      <c r="C133" s="124"/>
-      <c r="D133" s="124"/>
-      <c r="E133" s="124"/>
-      <c r="F133" s="124"/>
-      <c r="G133" s="125"/>
-      <c r="I133" s="120" t="s">
+      <c r="C133" s="131"/>
+      <c r="D133" s="131"/>
+      <c r="E133" s="131"/>
+      <c r="F133" s="131"/>
+      <c r="G133" s="132"/>
+      <c r="I133" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="J133" s="123" t="s">
+      <c r="J133" s="130" t="s">
         <v>74</v>
       </c>
-      <c r="K133" s="124"/>
-      <c r="L133" s="124"/>
-      <c r="M133" s="124"/>
-      <c r="N133" s="124"/>
-      <c r="O133" s="125"/>
-    </row>
-    <row r="134" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="121"/>
+      <c r="K133" s="131"/>
+      <c r="L133" s="131"/>
+      <c r="M133" s="131"/>
+      <c r="N133" s="131"/>
+      <c r="O133" s="132"/>
+    </row>
+    <row r="134" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="128"/>
       <c r="B134" s="26" t="s">
         <v>69</v>
       </c>
@@ -13432,7 +13426,7 @@
       <c r="G134" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I134" s="121"/>
+      <c r="I134" s="128"/>
       <c r="J134" s="26" t="s">
         <v>69</v>
       </c>
@@ -13452,8 +13446,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="135" spans="1:15" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A135" s="122"/>
+    <row r="135" spans="1:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="129"/>
       <c r="B135" s="40" t="s">
         <v>61</v>
       </c>
@@ -13472,7 +13466,7 @@
       <c r="G135" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="I135" s="122"/>
+      <c r="I135" s="129"/>
       <c r="J135" s="40" t="s">
         <v>61</v>
       </c>
@@ -13492,7 +13486,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>6</v>
       </c>
@@ -13536,7 +13530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>9</v>
       </c>
@@ -13580,7 +13574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>12</v>
       </c>
@@ -13624,7 +13618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>13</v>
       </c>
@@ -13680,7 +13674,7 @@
         <v>1.60703928E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>14</v>
       </c>
@@ -13736,7 +13730,7 @@
         <v>3.1595256000000009E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>15</v>
       </c>
@@ -13792,7 +13786,7 @@
         <v>3.2231707200000008E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>18</v>
       </c>
@@ -13848,7 +13842,7 @@
         <v>2.4003302399999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>17</v>
       </c>
@@ -13904,7 +13898,7 @@
         <v>1.53202896E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>19</v>
       </c>
@@ -13960,7 +13954,7 @@
         <v>6.1599383999999995E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>20</v>
       </c>
@@ -14016,7 +14010,7 @@
         <v>2.0002752000000002E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>21</v>
       </c>
@@ -14060,7 +14054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>22</v>
       </c>
@@ -14104,7 +14098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="16" t="s">
         <v>41</v>
       </c>
@@ -14148,7 +14142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="16" t="s">
         <v>42</v>
       </c>
@@ -14192,7 +14186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="16" t="s">
         <v>43</v>
       </c>
@@ -14236,7 +14230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="16" t="s">
         <v>44</v>
       </c>
@@ -14280,7 +14274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B152">
         <f t="shared" ref="B152:G152" si="34">5*SUM(B136:B151)</f>
         <v>2.2191840000000003</v>
@@ -14330,7 +14324,7 @@
         <v>0.63690580800000007</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="36" t="s">
         <v>89</v>
       </c>
@@ -14357,7 +14351,7 @@
       <c r="V158" s="37"/>
       <c r="W158" s="37"/>
     </row>
-    <row r="159" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="38" t="s">
         <v>56</v>
       </c>
@@ -14384,7 +14378,7 @@
       <c r="V159" s="37"/>
       <c r="W159" s="37"/>
     </row>
-    <row r="160" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="36" t="s">
         <v>70</v>
       </c>
@@ -14411,23 +14405,23 @@
       <c r="V160" s="37"/>
       <c r="W160" s="37"/>
     </row>
-    <row r="161" spans="1:14" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="105" t="s">
+    <row r="161" spans="1:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="B161" s="115" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="115"/>
-      <c r="D161" s="115"/>
-      <c r="E161" s="115" t="s">
+      <c r="B161" s="123" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="123"/>
+      <c r="D161" s="123"/>
+      <c r="E161" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="F161" s="115"/>
-      <c r="G161" s="115"/>
-    </row>
-    <row r="162" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A162" s="105"/>
+      <c r="F161" s="123"/>
+      <c r="G161" s="123"/>
+    </row>
+    <row r="162" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A162" s="112"/>
       <c r="B162" s="58" t="s">
         <v>3</v>
       </c>
@@ -14447,7 +14441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>6</v>
       </c>
@@ -14482,7 +14476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>9</v>
       </c>
@@ -14517,7 +14511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>12</v>
       </c>
@@ -14529,7 +14523,7 @@
         <f>D165*0.22</f>
         <v>8.8000000000000009E-2</v>
       </c>
-      <c r="D165" s="132">
+      <c r="D165" s="103">
         <v>0.4</v>
       </c>
       <c r="E165" s="57">
@@ -14540,7 +14534,7 @@
         <f>G165*0.58</f>
         <v>2.61</v>
       </c>
-      <c r="G165" s="133">
+      <c r="G165" s="104">
         <v>4.5</v>
       </c>
       <c r="J165">
@@ -14564,7 +14558,7 @@
         <v>21.53316106804478</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>13</v>
       </c>
@@ -14576,7 +14570,7 @@
         <f t="shared" ref="C166:C178" si="40">D166*0.22</f>
         <v>0.17600000000000002</v>
       </c>
-      <c r="D166" s="132">
+      <c r="D166" s="103">
         <v>0.8</v>
       </c>
       <c r="E166" s="57">
@@ -14587,7 +14581,7 @@
         <f t="shared" ref="F166:F178" si="42">G166*0.58</f>
         <v>5.22</v>
       </c>
-      <c r="G166" s="134">
+      <c r="G166" s="105">
         <v>9</v>
       </c>
       <c r="J166">
@@ -14611,7 +14605,7 @@
         <v>5.4585152838427948</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>14</v>
       </c>
@@ -14623,7 +14617,7 @@
         <f t="shared" si="40"/>
         <v>2.6839999999999997</v>
       </c>
-      <c r="D167" s="132">
+      <c r="D167" s="103">
         <v>12.2</v>
       </c>
       <c r="E167" s="57">
@@ -14634,7 +14628,7 @@
         <f t="shared" si="42"/>
         <v>15.079999999999998</v>
       </c>
-      <c r="G167" s="134">
+      <c r="G167" s="105">
         <v>26</v>
       </c>
       <c r="J167">
@@ -14658,7 +14652,7 @@
         <v>0.34921290150924544</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>15</v>
       </c>
@@ -14670,7 +14664,7 @@
         <f t="shared" si="40"/>
         <v>5.5</v>
       </c>
-      <c r="D168" s="132">
+      <c r="D168" s="103">
         <v>25</v>
       </c>
       <c r="E168" s="57">
@@ -14681,7 +14675,7 @@
         <f t="shared" si="42"/>
         <v>11.02</v>
       </c>
-      <c r="G168" s="134">
+      <c r="G168" s="105">
         <v>19</v>
       </c>
       <c r="J168">
@@ -14705,7 +14699,7 @@
         <v>0.17791411042944782</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>18</v>
       </c>
@@ -14717,7 +14711,7 @@
         <f t="shared" si="40"/>
         <v>5.5</v>
       </c>
-      <c r="D169" s="132">
+      <c r="D169" s="103">
         <v>25</v>
       </c>
       <c r="E169" s="57">
@@ -14728,7 +14722,7 @@
         <f t="shared" si="42"/>
         <v>8.1199999999999992</v>
       </c>
-      <c r="G169" s="134">
+      <c r="G169" s="105">
         <v>14</v>
       </c>
       <c r="J169">
@@ -14752,7 +14746,7 @@
         <v>0.2047426257952574</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>17</v>
       </c>
@@ -14764,7 +14758,7 @@
         <f t="shared" si="40"/>
         <v>5.5</v>
       </c>
-      <c r="D170" s="132">
+      <c r="D170" s="103">
         <v>25</v>
       </c>
       <c r="E170" s="57">
@@ -14775,7 +14769,7 @@
         <f t="shared" si="42"/>
         <v>8.1199999999999992</v>
       </c>
-      <c r="G170" s="134">
+      <c r="G170" s="105">
         <v>14</v>
       </c>
       <c r="J170">
@@ -14799,7 +14793,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>19</v>
       </c>
@@ -14811,7 +14805,7 @@
         <f t="shared" si="40"/>
         <v>5.5</v>
       </c>
-      <c r="D171" s="132">
+      <c r="D171" s="103">
         <v>25</v>
       </c>
       <c r="E171" s="57">
@@ -14822,7 +14816,7 @@
         <f t="shared" si="42"/>
         <v>8.1199999999999992</v>
       </c>
-      <c r="G171" s="134">
+      <c r="G171" s="105">
         <v>14</v>
       </c>
       <c r="J171">
@@ -14846,7 +14840,7 @@
         <v>0.28387096774193549</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>20</v>
       </c>
@@ -14858,7 +14852,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D172" s="132">
+      <c r="D172" s="103">
         <v>12</v>
       </c>
       <c r="E172" s="57">
@@ -14869,7 +14863,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G172" s="134">
+      <c r="G172" s="105">
         <v>10</v>
       </c>
       <c r="J172">
@@ -14893,7 +14887,7 @@
         <v>0.65514703063897706</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>21</v>
       </c>
@@ -14905,7 +14899,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D173" s="132">
+      <c r="D173" s="103">
         <v>12</v>
       </c>
       <c r="E173" s="57">
@@ -14916,7 +14910,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G173" s="134">
+      <c r="G173" s="105">
         <v>10</v>
       </c>
       <c r="J173">
@@ -14940,7 +14934,7 @@
         <v>0.65514703063897706</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>22</v>
       </c>
@@ -14952,7 +14946,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D174" s="132">
+      <c r="D174" s="103">
         <v>12</v>
       </c>
       <c r="E174" s="57">
@@ -14963,7 +14957,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G174" s="134">
+      <c r="G174" s="105">
         <v>10</v>
       </c>
       <c r="J174">
@@ -14987,7 +14981,7 @@
         <v>0.65514703063897706</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="16" t="s">
         <v>41</v>
       </c>
@@ -14999,7 +14993,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D175" s="132">
+      <c r="D175" s="103">
         <v>12</v>
       </c>
       <c r="E175" s="57">
@@ -15010,7 +15004,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G175" s="134">
+      <c r="G175" s="105">
         <v>10</v>
       </c>
       <c r="J175">
@@ -15034,7 +15028,7 @@
         <v>0.65514703063897706</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="16" t="s">
         <v>42</v>
       </c>
@@ -15046,7 +15040,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D176" s="132">
+      <c r="D176" s="103">
         <v>12</v>
       </c>
       <c r="E176" s="57">
@@ -15057,7 +15051,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G176" s="134">
+      <c r="G176" s="105">
         <v>10</v>
       </c>
       <c r="J176">
@@ -15081,7 +15075,7 @@
         <v>0.65514703063897706</v>
       </c>
     </row>
-    <row r="177" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="16" t="s">
         <v>43</v>
       </c>
@@ -15093,7 +15087,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D177" s="132">
+      <c r="D177" s="103">
         <v>12</v>
       </c>
       <c r="E177" s="57">
@@ -15104,7 +15098,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G177" s="134">
+      <c r="G177" s="105">
         <v>10</v>
       </c>
       <c r="J177">
@@ -15128,7 +15122,7 @@
         <v>0.65514703063897706</v>
       </c>
     </row>
-    <row r="178" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="16" t="s">
         <v>44</v>
       </c>
@@ -15140,7 +15134,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D178" s="132">
+      <c r="D178" s="103">
         <v>12</v>
       </c>
       <c r="E178" s="57">
@@ -15151,7 +15145,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G178" s="134">
+      <c r="G178" s="105">
         <v>10</v>
       </c>
       <c r="H178">
@@ -15179,14 +15173,14 @@
         <v>0.65514703063897706</v>
       </c>
     </row>
-    <row r="179" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A179" s="131"/>
+    <row r="179" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A179" s="102"/>
       <c r="N179">
         <f>AVERAGE(N165:N178)</f>
         <v>2.3459604408454511</v>
       </c>
     </row>
-    <row r="183" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A183" s="7"/>
       <c r="B183" s="20"/>
       <c r="C183" s="20"/>
@@ -15216,7 +15210,7 @@
       <c r="AA183" s="20"/>
       <c r="AB183" s="20"/>
     </row>
-    <row r="184" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A184" s="20"/>
       <c r="B184" s="20"/>
       <c r="C184" s="20"/>
@@ -15246,7 +15240,7 @@
       <c r="AA184" s="20"/>
       <c r="AB184" s="20"/>
     </row>
-    <row r="185" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185" s="62"/>
       <c r="B185" s="20"/>
       <c r="C185" s="20"/>
@@ -15276,10 +15270,10 @@
       <c r="AA185" s="20"/>
       <c r="AB185" s="20"/>
     </row>
-    <row r="186" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A186" s="116"/>
-      <c r="B186" s="116"/>
-      <c r="C186" s="116"/>
+    <row r="186" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A186" s="124"/>
+      <c r="B186" s="124"/>
+      <c r="C186" s="124"/>
       <c r="D186" s="20"/>
       <c r="E186" s="20"/>
       <c r="F186" s="20"/>
@@ -15306,7 +15300,7 @@
       <c r="AA186" s="20"/>
       <c r="AB186" s="20"/>
     </row>
-    <row r="187" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A187" s="63"/>
       <c r="B187" s="64"/>
       <c r="C187" s="64"/>
@@ -15336,7 +15330,7 @@
       <c r="AA187" s="20"/>
       <c r="AB187" s="20"/>
     </row>
-    <row r="188" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A188" s="6"/>
       <c r="B188" s="61"/>
       <c r="C188" s="61"/>
@@ -15366,7 +15360,7 @@
       <c r="AA188" s="20"/>
       <c r="AB188" s="20"/>
     </row>
-    <row r="189" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A189" s="6"/>
       <c r="B189" s="61"/>
       <c r="C189" s="61"/>
@@ -15396,7 +15390,7 @@
       <c r="AA189" s="20"/>
       <c r="AB189" s="20"/>
     </row>
-    <row r="190" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A190" s="6"/>
       <c r="B190" s="61"/>
       <c r="C190" s="61"/>
@@ -15426,7 +15420,7 @@
       <c r="AA190" s="20"/>
       <c r="AB190" s="20"/>
     </row>
-    <row r="197" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A197" s="36" t="s">
         <v>90</v>
       </c>
@@ -15453,38 +15447,38 @@
       <c r="V197" s="37"/>
       <c r="W197" s="37"/>
     </row>
-    <row r="198" spans="1:23" s="39" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A198" s="112" t="s">
+    <row r="198" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A198" s="119" t="s">
         <v>71</v>
       </c>
-      <c r="B198" s="112"/>
-      <c r="C198" s="112"/>
-      <c r="D198" s="112"/>
-      <c r="E198" s="136"/>
-      <c r="F198" s="136"/>
-    </row>
-    <row r="199" spans="1:23" s="39" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A199" s="112" t="s">
+      <c r="B198" s="119"/>
+      <c r="C198" s="119"/>
+      <c r="D198" s="119"/>
+      <c r="E198" s="107"/>
+      <c r="F198" s="107"/>
+    </row>
+    <row r="199" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A199" s="119" t="s">
         <v>72</v>
       </c>
-      <c r="B199" s="112"/>
-      <c r="C199" s="112"/>
-      <c r="D199" s="112"/>
-      <c r="E199" s="136"/>
-      <c r="F199" s="136"/>
-    </row>
-    <row r="200" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A200" s="117" t="s">
+      <c r="B199" s="119"/>
+      <c r="C199" s="119"/>
+      <c r="D199" s="119"/>
+      <c r="E199" s="107"/>
+      <c r="F199" s="107"/>
+    </row>
+    <row r="200" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A200" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="B200" s="117" t="s">
+      <c r="B200" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="C200" s="117"/>
-      <c r="D200" s="117"/>
-    </row>
-    <row r="201" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A201" s="117"/>
+      <c r="C200" s="125"/>
+      <c r="D200" s="125"/>
+    </row>
+    <row r="201" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A201" s="125"/>
       <c r="B201" s="43" t="s">
         <v>46</v>
       </c>
@@ -15495,7 +15489,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="202" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A202" s="44" t="s">
         <v>25</v>
       </c>
@@ -15504,52 +15498,52 @@
         <v>0</v>
       </c>
       <c r="C202" s="59">
-        <f>0.6*B202</f>
+        <f t="shared" ref="C202:D202" si="45">C222</f>
         <v>0</v>
       </c>
       <c r="D202" s="59">
-        <f>0.6*C202</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="F202" t="e">
-        <f>B202/C202</f>
+        <f t="shared" ref="F202:F217" si="46">B202/C202</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G202" t="e">
-        <f>C202/D202</f>
+        <f t="shared" ref="G202:G217" si="47">C202/D202</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I202" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="J202" s="111" t="s">
+      <c r="J202" s="118" t="s">
         <v>92</v>
       </c>
-      <c r="K202" s="111"/>
-      <c r="L202" s="111"/>
-    </row>
-    <row r="203" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K202" s="118"/>
+      <c r="L202" s="118"/>
+    </row>
+    <row r="203" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="44" t="s">
         <v>24</v>
       </c>
       <c r="B203" s="59">
-        <f>B223</f>
+        <f t="shared" ref="B203:D203" si="48">B223</f>
         <v>0</v>
       </c>
       <c r="C203" s="59">
-        <f t="shared" ref="C203:D217" si="45">0.6*B203</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="D203" s="59">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="F203" t="e">
-        <f>B203/C203</f>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G203" t="e">
-        <f>C203/D203</f>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I203" s="44" t="s">
@@ -15565,28 +15559,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A204" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B204" s="60">
-        <f>0.8*B224</f>
-        <v>31.84</v>
+      <c r="B204" s="59">
+        <f t="shared" ref="B204:D204" si="49">B224</f>
+        <v>35.421999999999997</v>
       </c>
       <c r="C204" s="59">
-        <f t="shared" si="45"/>
-        <v>19.103999999999999</v>
+        <f t="shared" si="49"/>
+        <v>21.253199999999996</v>
       </c>
       <c r="D204" s="59">
-        <f t="shared" si="45"/>
-        <v>11.462399999999999</v>
+        <f t="shared" si="49"/>
+        <v>12.751919999999997</v>
       </c>
       <c r="F204">
-        <f>B204/C204</f>
+        <f t="shared" si="46"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G204">
-        <f>C204/D204</f>
+        <f t="shared" si="47"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="I204" s="44" t="s">
@@ -15602,28 +15596,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B205" s="60">
-        <f t="shared" ref="B205:B206" si="46">0.8*B225</f>
-        <v>63.68</v>
+      <c r="B205" s="59">
+        <f>B225</f>
+        <v>70.843999999999994</v>
       </c>
       <c r="C205" s="59">
-        <f t="shared" si="45"/>
-        <v>38.207999999999998</v>
+        <f t="shared" ref="B205:D205" si="50">C225</f>
+        <v>42.506399999999992</v>
       </c>
       <c r="D205" s="59">
-        <f t="shared" si="45"/>
-        <v>22.924799999999998</v>
+        <f t="shared" si="50"/>
+        <v>25.503839999999993</v>
       </c>
       <c r="F205">
-        <f>B205/C205</f>
+        <f t="shared" si="46"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G205">
-        <f>C205/D205</f>
+        <f t="shared" si="47"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="I205" s="44" t="s">
@@ -15639,531 +15633,531 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A206" s="44" t="s">
         <v>33</v>
       </c>
       <c r="B206" s="60">
+        <f>B225</f>
+        <v>70.843999999999994</v>
+      </c>
+      <c r="C206" s="60">
+        <f t="shared" ref="C206:D206" si="51">C225</f>
+        <v>42.506399999999992</v>
+      </c>
+      <c r="D206" s="60">
+        <f t="shared" si="51"/>
+        <v>25.503839999999993</v>
+      </c>
+      <c r="F206">
         <f t="shared" si="46"/>
-        <v>62.879999999999995</v>
-      </c>
-      <c r="C206" s="59">
-        <f t="shared" si="45"/>
-        <v>37.727999999999994</v>
-      </c>
-      <c r="D206" s="59">
-        <f t="shared" si="45"/>
-        <v>22.636799999999997</v>
-      </c>
-      <c r="F206">
-        <f>B206/C206</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="G206">
-        <f>C206/D206</f>
-        <v>1.6666666666666665</v>
+        <f t="shared" si="47"/>
+        <v>1.6666666666666667</v>
       </c>
       <c r="I206" s="44" t="s">
         <v>32</v>
       </c>
       <c r="J206" s="9">
-        <f>B205/B204</f>
+        <f t="shared" ref="J206:J218" si="52">B205/B204</f>
         <v>2</v>
       </c>
       <c r="K206" s="9">
-        <f>C205/C204</f>
+        <f t="shared" ref="K206:K218" si="53">C205/C204</f>
         <v>2</v>
       </c>
       <c r="L206" s="9">
-        <f>D205/D204</f>
+        <f t="shared" ref="L206:L218" si="54">D205/D204</f>
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207" s="44" t="s">
         <v>34</v>
       </c>
       <c r="B207" s="60">
-        <f>1.1*B227</f>
-        <v>61.820000000000007</v>
-      </c>
-      <c r="C207" s="59">
-        <f t="shared" si="45"/>
-        <v>37.092000000000006</v>
-      </c>
-      <c r="D207" s="59">
-        <f t="shared" si="45"/>
-        <v>22.255200000000002</v>
+        <f t="shared" ref="B207:D207" si="55">B226</f>
+        <v>69.953999999999994</v>
+      </c>
+      <c r="C207" s="60">
+        <f t="shared" si="55"/>
+        <v>41.972399999999993</v>
+      </c>
+      <c r="D207" s="60">
+        <f t="shared" si="55"/>
+        <v>25.183439999999994</v>
       </c>
       <c r="F207">
-        <f>B207/C207</f>
-        <v>1.6666666666666665</v>
+        <f t="shared" si="46"/>
+        <v>1.6666666666666667</v>
       </c>
       <c r="G207">
-        <f>C207/D207</f>
+        <f t="shared" si="47"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="I207" s="44" t="s">
         <v>33</v>
       </c>
       <c r="J207" s="9">
-        <f>B206/B205</f>
-        <v>0.98743718592964813</v>
+        <f t="shared" si="52"/>
+        <v>1</v>
       </c>
       <c r="K207" s="9">
-        <f>C206/C205</f>
-        <v>0.98743718592964813</v>
+        <f t="shared" si="53"/>
+        <v>1</v>
       </c>
       <c r="L207" s="9">
-        <f>D206/D205</f>
-        <v>0.98743718592964824</v>
-      </c>
-    </row>
-    <row r="208" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A208" s="44" t="s">
         <v>35</v>
       </c>
       <c r="B208" s="60">
-        <f t="shared" ref="B208:B211" si="47">1.1*B228</f>
-        <v>60.060000000000009</v>
-      </c>
-      <c r="C208" s="59">
-        <f t="shared" si="45"/>
-        <v>36.036000000000001</v>
-      </c>
-      <c r="D208" s="59">
-        <f t="shared" si="45"/>
-        <v>21.621600000000001</v>
+        <f t="shared" ref="B208:D208" si="56">B227</f>
+        <v>56.2</v>
+      </c>
+      <c r="C208" s="60">
+        <f t="shared" si="56"/>
+        <v>33.72</v>
+      </c>
+      <c r="D208" s="60">
+        <f t="shared" si="56"/>
+        <v>20.231999999999999</v>
       </c>
       <c r="F208">
-        <f>B208/C208</f>
-        <v>1.666666666666667</v>
+        <f t="shared" si="46"/>
+        <v>1.6666666666666667</v>
       </c>
       <c r="G208">
-        <f>C208/D208</f>
+        <f t="shared" si="47"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="I208" s="44" t="s">
         <v>34</v>
       </c>
       <c r="J208" s="9">
-        <f>B207/B206</f>
-        <v>0.98314249363867701</v>
+        <f t="shared" si="52"/>
+        <v>0.98743718592964824</v>
       </c>
       <c r="K208" s="9">
-        <f>C207/C206</f>
-        <v>0.98314249363867712</v>
+        <f t="shared" si="53"/>
+        <v>0.98743718592964824</v>
       </c>
       <c r="L208" s="9">
-        <f>D207/D206</f>
-        <v>0.98314249363867701</v>
+        <f t="shared" si="54"/>
+        <v>0.98743718592964824</v>
       </c>
       <c r="M208" s="39"/>
     </row>
-    <row r="209" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="44" t="s">
         <v>36</v>
       </c>
       <c r="B209" s="60">
+        <f t="shared" ref="B209:D209" si="57">B228</f>
+        <v>54.6</v>
+      </c>
+      <c r="C209" s="60">
+        <f t="shared" si="57"/>
+        <v>32.76</v>
+      </c>
+      <c r="D209" s="60">
+        <f t="shared" si="57"/>
+        <v>19.655999999999999</v>
+      </c>
+      <c r="F209">
+        <f t="shared" si="46"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="G209">
         <f t="shared" si="47"/>
-        <v>60.060000000000009</v>
-      </c>
-      <c r="C209" s="59">
-        <f t="shared" si="45"/>
-        <v>36.036000000000001</v>
-      </c>
-      <c r="D209" s="59">
-        <f t="shared" si="45"/>
-        <v>21.621600000000001</v>
-      </c>
-      <c r="F209">
-        <f>B209/C209</f>
-        <v>1.666666666666667</v>
-      </c>
-      <c r="G209">
-        <f>C209/D209</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="I209" s="44" t="s">
         <v>35</v>
       </c>
       <c r="J209" s="9">
-        <f>B208/B207</f>
-        <v>0.97153024911032027</v>
+        <f t="shared" si="52"/>
+        <v>0.80338508162506805</v>
       </c>
       <c r="K209" s="9">
-        <f>C208/C207</f>
-        <v>0.97153024911032015</v>
+        <f t="shared" si="53"/>
+        <v>0.80338508162506805</v>
       </c>
       <c r="L209" s="9">
-        <f>D208/D207</f>
-        <v>0.97153024911032027</v>
-      </c>
-    </row>
-    <row r="210" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+        <f t="shared" si="54"/>
+        <v>0.80338508162506805</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210" s="44" t="s">
         <v>37</v>
       </c>
       <c r="B210" s="60">
+        <f t="shared" ref="B210:D210" si="58">B229</f>
+        <v>54.6</v>
+      </c>
+      <c r="C210" s="60">
+        <f t="shared" si="58"/>
+        <v>32.76</v>
+      </c>
+      <c r="D210" s="60">
+        <f t="shared" si="58"/>
+        <v>19.655999999999999</v>
+      </c>
+      <c r="F210">
+        <f t="shared" si="46"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="G210">
         <f t="shared" si="47"/>
-        <v>60.060000000000009</v>
-      </c>
-      <c r="C210" s="59">
-        <f t="shared" si="45"/>
-        <v>36.036000000000001</v>
-      </c>
-      <c r="D210" s="59">
-        <f t="shared" si="45"/>
-        <v>21.621600000000001</v>
-      </c>
-      <c r="F210">
-        <f>B210/C210</f>
-        <v>1.666666666666667</v>
-      </c>
-      <c r="G210">
-        <f>C210/D210</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="I210" s="44" t="s">
         <v>36</v>
       </c>
       <c r="J210" s="9">
-        <f>B209/B208</f>
-        <v>1</v>
+        <f t="shared" si="52"/>
+        <v>0.97153024911032027</v>
       </c>
       <c r="K210" s="9">
-        <f>C209/C208</f>
-        <v>1</v>
+        <f t="shared" si="53"/>
+        <v>0.97153024911032027</v>
       </c>
       <c r="L210" s="9">
-        <f>D209/D208</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="211" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+        <f t="shared" si="54"/>
+        <v>0.97153024911032027</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A211" s="44" t="s">
         <v>38</v>
       </c>
       <c r="B211" s="60">
+        <f t="shared" ref="B211:D211" si="59">B230</f>
+        <v>54.6</v>
+      </c>
+      <c r="C211" s="60">
+        <f t="shared" si="59"/>
+        <v>32.76</v>
+      </c>
+      <c r="D211" s="60">
+        <f t="shared" si="59"/>
+        <v>19.655999999999999</v>
+      </c>
+      <c r="F211">
+        <f t="shared" si="46"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="G211">
         <f t="shared" si="47"/>
-        <v>57.970000000000006</v>
-      </c>
-      <c r="C211" s="59">
-        <f t="shared" si="45"/>
-        <v>34.782000000000004</v>
-      </c>
-      <c r="D211" s="59">
-        <f t="shared" si="45"/>
-        <v>20.869200000000003</v>
-      </c>
-      <c r="F211">
-        <f>B211/C211</f>
         <v>1.6666666666666667</v>
-      </c>
-      <c r="G211">
-        <f>C211/D211</f>
-        <v>1.6666666666666665</v>
       </c>
       <c r="I211" s="44" t="s">
         <v>37</v>
       </c>
       <c r="J211" s="9">
-        <f>B210/B209</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="K211" s="9">
-        <f>C210/C209</f>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="L211" s="9">
-        <f>D210/D209</f>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A212" s="44" t="s">
         <v>39</v>
       </c>
       <c r="B212" s="60">
-        <f>B232</f>
+        <f t="shared" ref="B212:D212" si="60">B231</f>
         <v>52.7</v>
       </c>
-      <c r="C212" s="59">
-        <f t="shared" si="45"/>
+      <c r="C212" s="60">
+        <f t="shared" si="60"/>
         <v>31.62</v>
       </c>
-      <c r="D212" s="59">
-        <f t="shared" si="45"/>
+      <c r="D212" s="60">
+        <f t="shared" si="60"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F212">
-        <f>B212/C212</f>
+        <f t="shared" si="46"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G212">
-        <f>C212/D212</f>
+        <f t="shared" si="47"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I212" s="44" t="s">
         <v>38</v>
       </c>
       <c r="J212" s="9">
-        <f>B211/B210</f>
-        <v>0.9652014652014651</v>
+        <f t="shared" si="52"/>
+        <v>1</v>
       </c>
       <c r="K212" s="9">
-        <f>C211/C210</f>
-        <v>0.96520146520146521</v>
+        <f t="shared" si="53"/>
+        <v>1</v>
       </c>
       <c r="L212" s="9">
-        <f>D211/D210</f>
-        <v>0.96520146520146533</v>
-      </c>
-    </row>
-    <row r="213" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A213" s="44" t="s">
         <v>40</v>
       </c>
       <c r="B213" s="60">
-        <f t="shared" ref="B213:B217" si="48">B233</f>
+        <f t="shared" ref="B213:D213" si="61">B232</f>
         <v>52.7</v>
       </c>
-      <c r="C213" s="59">
-        <f t="shared" si="45"/>
+      <c r="C213" s="60">
+        <f t="shared" si="61"/>
         <v>31.62</v>
       </c>
-      <c r="D213" s="59">
-        <f t="shared" si="45"/>
+      <c r="D213" s="60">
+        <f t="shared" si="61"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F213">
-        <f>B213/C213</f>
+        <f t="shared" si="46"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G213">
-        <f>C213/D213</f>
+        <f t="shared" si="47"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I213" s="44" t="s">
         <v>39</v>
       </c>
       <c r="J213" s="9">
-        <f>B212/B211</f>
-        <v>0.90909090909090906</v>
+        <f t="shared" si="52"/>
+        <v>0.96520146520146521</v>
       </c>
       <c r="K213" s="9">
-        <f>C212/C211</f>
-        <v>0.90909090909090906</v>
+        <f t="shared" si="53"/>
+        <v>0.96520146520146533</v>
       </c>
       <c r="L213" s="9">
-        <f>D212/D211</f>
-        <v>0.90909090909090906</v>
-      </c>
-    </row>
-    <row r="214" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+        <f t="shared" si="54"/>
+        <v>0.96520146520146533</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A214" s="44" t="s">
         <v>41</v>
       </c>
       <c r="B214" s="60">
-        <f t="shared" si="48"/>
+        <f t="shared" ref="B214:D214" si="62">B233</f>
         <v>52.7</v>
       </c>
-      <c r="C214" s="59">
-        <f t="shared" si="45"/>
+      <c r="C214" s="60">
+        <f t="shared" si="62"/>
         <v>31.62</v>
       </c>
-      <c r="D214" s="59">
-        <f t="shared" si="45"/>
+      <c r="D214" s="60">
+        <f t="shared" si="62"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F214">
-        <f>B214/C214</f>
+        <f t="shared" si="46"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G214">
-        <f>C214/D214</f>
+        <f t="shared" si="47"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I214" s="44" t="s">
         <v>40</v>
       </c>
       <c r="J214" s="9">
-        <f>B213/B212</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="K214" s="9">
-        <f>C213/C212</f>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="L214" s="9">
-        <f>D213/D212</f>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A215" s="44" t="s">
         <v>42</v>
       </c>
       <c r="B215" s="60">
-        <f t="shared" si="48"/>
+        <f t="shared" ref="B215:D215" si="63">B234</f>
         <v>52.7</v>
       </c>
-      <c r="C215" s="59">
-        <f t="shared" si="45"/>
+      <c r="C215" s="60">
+        <f t="shared" si="63"/>
         <v>31.62</v>
       </c>
-      <c r="D215" s="59">
-        <f t="shared" si="45"/>
+      <c r="D215" s="60">
+        <f t="shared" si="63"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F215">
-        <f>B215/C215</f>
+        <f t="shared" si="46"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G215">
-        <f>C215/D215</f>
+        <f t="shared" si="47"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I215" s="44" t="s">
         <v>41</v>
       </c>
       <c r="J215" s="9">
-        <f>B214/B213</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="K215" s="9">
-        <f>C214/C213</f>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="L215" s="9">
-        <f>D214/D213</f>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A216" s="44" t="s">
         <v>43</v>
       </c>
       <c r="B216" s="60">
-        <f t="shared" si="48"/>
+        <f t="shared" ref="B216:D216" si="64">B235</f>
         <v>52.7</v>
       </c>
-      <c r="C216" s="59">
-        <f t="shared" si="45"/>
+      <c r="C216" s="60">
+        <f t="shared" si="64"/>
         <v>31.62</v>
       </c>
-      <c r="D216" s="59">
-        <f t="shared" si="45"/>
+      <c r="D216" s="60">
+        <f t="shared" si="64"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F216">
-        <f>B216/C216</f>
+        <f t="shared" si="46"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G216">
-        <f>C216/D216</f>
+        <f t="shared" si="47"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I216" s="44" t="s">
         <v>42</v>
       </c>
       <c r="J216" s="9">
-        <f>B215/B214</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="K216" s="9">
-        <f>C215/C214</f>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="L216" s="9">
-        <f>D215/D214</f>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A217" s="44" t="s">
         <v>44</v>
       </c>
       <c r="B217" s="60">
-        <f t="shared" si="48"/>
+        <f t="shared" ref="B217:D217" si="65">B236</f>
         <v>52.7</v>
       </c>
-      <c r="C217" s="59">
-        <f t="shared" si="45"/>
+      <c r="C217" s="60">
+        <f t="shared" si="65"/>
         <v>31.62</v>
       </c>
-      <c r="D217" s="59">
-        <f t="shared" si="45"/>
+      <c r="D217" s="60">
+        <f t="shared" si="65"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F217">
-        <f>B217/C217</f>
+        <f t="shared" si="46"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G217">
-        <f>C217/D217</f>
+        <f t="shared" si="47"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I217" s="44" t="s">
         <v>43</v>
       </c>
       <c r="J217" s="9">
-        <f>B216/B215</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="K217" s="9">
-        <f>C216/C215</f>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="L217" s="9">
-        <f>D216/D215</f>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A218" s="42"/>
       <c r="B218" s="61"/>
       <c r="C218" s="42"/>
-      <c r="D218" s="135"/>
-      <c r="E218" s="135"/>
+      <c r="D218" s="106"/>
+      <c r="E218" s="106"/>
       <c r="I218" s="44" t="s">
         <v>44</v>
       </c>
       <c r="J218" s="9">
-        <f>B217/B216</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="K218" s="9">
-        <f>C217/C216</f>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="L218" s="9">
-        <f>D217/D216</f>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A219" s="114" t="s">
+    <row r="219" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A219" s="122" t="s">
         <v>73</v>
       </c>
-      <c r="B219" s="114"/>
-      <c r="C219" s="114"/>
-      <c r="D219" s="114"/>
-      <c r="E219" s="137"/>
-    </row>
-    <row r="220" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A220" s="114" t="s">
+      <c r="B219" s="122"/>
+      <c r="C219" s="122"/>
+      <c r="D219" s="122"/>
+      <c r="E219" s="108"/>
+    </row>
+    <row r="220" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A220" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="B220" s="117" t="s">
+      <c r="B220" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="C220" s="117"/>
-      <c r="D220" s="117"/>
+      <c r="C220" s="125"/>
+      <c r="D220" s="125"/>
       <c r="E220" s="25"/>
     </row>
-    <row r="221" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A221" s="114"/>
+    <row r="221" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A221" s="122"/>
       <c r="B221" s="43" t="s">
         <v>46</v>
       </c>
@@ -16175,7 +16169,7 @@
       </c>
       <c r="E221" s="25"/>
     </row>
-    <row r="222" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A222" s="44" t="s">
         <v>25</v>
       </c>
@@ -16192,23 +16186,23 @@
       </c>
       <c r="E222" s="25"/>
       <c r="F222" t="e">
-        <f>B222/C222</f>
+        <f t="shared" ref="F222:F237" si="66">B222/C222</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G222" t="e">
-        <f>C222/D222</f>
+        <f t="shared" ref="G222:G237" si="67">C222/D222</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I222" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="J222" s="111" t="s">
+      <c r="J222" s="118" t="s">
         <v>91</v>
       </c>
-      <c r="K222" s="111"/>
-      <c r="L222" s="111"/>
-    </row>
-    <row r="223" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K222" s="118"/>
+      <c r="L222" s="118"/>
+    </row>
+    <row r="223" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="44" t="s">
         <v>24</v>
       </c>
@@ -16216,20 +16210,20 @@
         <v>0</v>
       </c>
       <c r="C223" s="59">
-        <f t="shared" ref="C223:D237" si="49">B223*0.6</f>
+        <f t="shared" ref="C223:D237" si="68">B223*0.6</f>
         <v>0</v>
       </c>
       <c r="D223" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="E223" s="25"/>
       <c r="F223" t="e">
-        <f>B223/C223</f>
+        <f t="shared" si="66"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G223" t="e">
-        <f>C223/D223</f>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I223" s="44" t="s">
@@ -16245,28 +16239,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A224" s="44" t="s">
         <v>31</v>
       </c>
       <c r="B224" s="59">
-        <v>39.799999999999997</v>
+        <f>B225/2</f>
+        <v>35.421999999999997</v>
       </c>
       <c r="C224" s="59">
-        <f t="shared" si="49"/>
-        <v>23.88</v>
+        <f t="shared" si="68"/>
+        <v>21.253199999999996</v>
       </c>
       <c r="D224" s="59">
-        <f t="shared" si="49"/>
-        <v>14.327999999999999</v>
+        <f t="shared" si="68"/>
+        <v>12.751919999999997</v>
       </c>
       <c r="E224" s="25"/>
       <c r="F224">
-        <f>B224/C224</f>
-        <v>1.6666666666666665</v>
+        <f t="shared" si="66"/>
+        <v>1.6666666666666667</v>
       </c>
       <c r="G224">
-        <f>C224/D224</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="I224" s="44" t="s">
@@ -16282,28 +16277,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A225" s="44" t="s">
         <v>32</v>
       </c>
       <c r="B225" s="60">
-        <v>79.599999999999994</v>
+        <v>70.843999999999994</v>
       </c>
       <c r="C225" s="59">
-        <f t="shared" si="49"/>
-        <v>47.76</v>
+        <f t="shared" si="68"/>
+        <v>42.506399999999992</v>
       </c>
       <c r="D225" s="59">
-        <f t="shared" si="49"/>
-        <v>28.655999999999999</v>
+        <f t="shared" si="68"/>
+        <v>25.503839999999993</v>
       </c>
       <c r="E225" s="25"/>
       <c r="F225">
-        <f>B225/C225</f>
-        <v>1.6666666666666665</v>
+        <f t="shared" si="66"/>
+        <v>1.6666666666666667</v>
       </c>
       <c r="G225">
-        <f>C225/D225</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="I225" s="44" t="s">
@@ -16319,47 +16314,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A226" s="44" t="s">
         <v>33</v>
       </c>
       <c r="B226" s="59">
-        <v>78.599999999999994</v>
+        <v>69.953999999999994</v>
       </c>
       <c r="C226" s="59">
-        <f t="shared" si="49"/>
-        <v>47.16</v>
+        <f t="shared" si="68"/>
+        <v>41.972399999999993</v>
       </c>
       <c r="D226" s="59">
-        <f t="shared" si="49"/>
-        <v>28.295999999999996</v>
+        <f t="shared" si="68"/>
+        <v>25.183439999999994</v>
       </c>
       <c r="E226" s="25"/>
       <c r="F226">
-        <f>B226/C226</f>
+        <f t="shared" si="66"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G226">
-        <f>C226/D226</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="I226" s="44" t="s">
         <v>32</v>
       </c>
       <c r="J226" s="9">
-        <f>B225/B224</f>
+        <f t="shared" ref="J226:J238" si="69">B225/B224</f>
         <v>2</v>
       </c>
       <c r="K226" s="9">
-        <f>C225/C224</f>
+        <f t="shared" ref="K226:K238" si="70">C225/C224</f>
         <v>2</v>
       </c>
       <c r="L226" s="9">
-        <f>D225/D224</f>
+        <f t="shared" ref="L226:L238" si="71">D225/D224</f>
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A227" s="44" t="s">
         <v>34</v>
       </c>
@@ -16367,39 +16362,39 @@
         <v>56.2</v>
       </c>
       <c r="C227" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>33.72</v>
       </c>
       <c r="D227" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>20.231999999999999</v>
       </c>
       <c r="E227" s="25"/>
       <c r="F227">
-        <f>B227/C227</f>
+        <f t="shared" si="66"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G227">
-        <f>C227/D227</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="I227" s="44" t="s">
         <v>33</v>
       </c>
       <c r="J227" s="9">
-        <f>B226/B225</f>
+        <f t="shared" si="69"/>
         <v>0.98743718592964824</v>
       </c>
       <c r="K227" s="9">
-        <f>C226/C225</f>
+        <f t="shared" si="70"/>
         <v>0.98743718592964824</v>
       </c>
       <c r="L227" s="9">
-        <f>D226/D225</f>
-        <v>0.98743718592964813</v>
-      </c>
-    </row>
-    <row r="228" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+        <f t="shared" si="71"/>
+        <v>0.98743718592964824</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A228" s="44" t="s">
         <v>35</v>
       </c>
@@ -16407,39 +16402,39 @@
         <v>54.6</v>
       </c>
       <c r="C228" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>32.76</v>
       </c>
       <c r="D228" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>19.655999999999999</v>
       </c>
       <c r="E228" s="25"/>
       <c r="F228">
-        <f>B228/C228</f>
+        <f t="shared" si="66"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G228">
-        <f>C228/D228</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="I228" s="44" t="s">
         <v>34</v>
       </c>
       <c r="J228" s="9">
-        <f>B227/B226</f>
-        <v>0.71501272264631055</v>
+        <f t="shared" si="69"/>
+        <v>0.80338508162506805</v>
       </c>
       <c r="K228" s="9">
-        <f>C227/C226</f>
-        <v>0.71501272264631044</v>
+        <f t="shared" si="70"/>
+        <v>0.80338508162506805</v>
       </c>
       <c r="L228" s="9">
-        <f>D227/D226</f>
-        <v>0.71501272264631055</v>
-      </c>
-    </row>
-    <row r="229" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+        <f t="shared" si="71"/>
+        <v>0.80338508162506805</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A229" s="44" t="s">
         <v>36</v>
       </c>
@@ -16447,39 +16442,39 @@
         <v>54.6</v>
       </c>
       <c r="C229" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>32.76</v>
       </c>
       <c r="D229" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>19.655999999999999</v>
       </c>
       <c r="E229" s="25"/>
       <c r="F229">
-        <f>B229/C229</f>
+        <f t="shared" si="66"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G229">
-        <f>C229/D229</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="I229" s="44" t="s">
         <v>35</v>
       </c>
       <c r="J229" s="9">
-        <f>B228/B227</f>
+        <f t="shared" si="69"/>
         <v>0.97153024911032027</v>
       </c>
       <c r="K229" s="9">
-        <f>C228/C227</f>
+        <f t="shared" si="70"/>
         <v>0.97153024911032027</v>
       </c>
       <c r="L229" s="9">
-        <f>D228/D227</f>
+        <f t="shared" si="71"/>
         <v>0.97153024911032027</v>
       </c>
     </row>
-    <row r="230" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A230" s="44" t="s">
         <v>37</v>
       </c>
@@ -16487,39 +16482,39 @@
         <v>54.6</v>
       </c>
       <c r="C230" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>32.76</v>
       </c>
       <c r="D230" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>19.655999999999999</v>
       </c>
       <c r="E230" s="25"/>
       <c r="F230">
-        <f>B230/C230</f>
+        <f t="shared" si="66"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G230">
-        <f>C230/D230</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="I230" s="44" t="s">
         <v>36</v>
       </c>
       <c r="J230" s="9">
-        <f>B229/B228</f>
+        <f t="shared" si="69"/>
         <v>1</v>
       </c>
       <c r="K230" s="9">
-        <f>C229/C228</f>
+        <f t="shared" si="70"/>
         <v>1</v>
       </c>
       <c r="L230" s="9">
-        <f>D229/D228</f>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A231" s="44" t="s">
         <v>38</v>
       </c>
@@ -16527,38 +16522,38 @@
         <v>52.7</v>
       </c>
       <c r="C231" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>31.62</v>
       </c>
       <c r="D231" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F231">
-        <f>B231/C231</f>
+        <f t="shared" si="66"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G231">
-        <f>C231/D231</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I231" s="44" t="s">
         <v>37</v>
       </c>
       <c r="J231" s="9">
-        <f>B230/B229</f>
+        <f t="shared" si="69"/>
         <v>1</v>
       </c>
       <c r="K231" s="9">
-        <f>C230/C229</f>
+        <f t="shared" si="70"/>
         <v>1</v>
       </c>
       <c r="L231" s="9">
-        <f>D230/D229</f>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="44" t="s">
         <v>39</v>
       </c>
@@ -16566,38 +16561,38 @@
         <v>52.7</v>
       </c>
       <c r="C232" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>31.62</v>
       </c>
       <c r="D232" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F232">
-        <f>B232/C232</f>
+        <f t="shared" si="66"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G232">
-        <f>C232/D232</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I232" s="44" t="s">
         <v>38</v>
       </c>
       <c r="J232" s="9">
-        <f>B231/B230</f>
+        <f t="shared" si="69"/>
         <v>0.96520146520146521</v>
       </c>
       <c r="K232" s="9">
-        <f>C231/C230</f>
+        <f t="shared" si="70"/>
         <v>0.96520146520146533</v>
       </c>
       <c r="L232" s="9">
-        <f>D231/D230</f>
+        <f t="shared" si="71"/>
         <v>0.96520146520146533</v>
       </c>
     </row>
-    <row r="233" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A233" s="44" t="s">
         <v>40</v>
       </c>
@@ -16605,38 +16600,38 @@
         <v>52.7</v>
       </c>
       <c r="C233" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>31.62</v>
       </c>
       <c r="D233" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F233">
-        <f>B233/C233</f>
+        <f t="shared" si="66"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G233">
-        <f>C233/D233</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I233" s="44" t="s">
         <v>39</v>
       </c>
       <c r="J233" s="9">
-        <f>B232/B231</f>
+        <f t="shared" si="69"/>
         <v>1</v>
       </c>
       <c r="K233" s="9">
-        <f>C232/C231</f>
+        <f t="shared" si="70"/>
         <v>1</v>
       </c>
       <c r="L233" s="9">
-        <f>D232/D231</f>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A234" s="44" t="s">
         <v>41</v>
       </c>
@@ -16644,38 +16639,38 @@
         <v>52.7</v>
       </c>
       <c r="C234" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>31.62</v>
       </c>
       <c r="D234" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F234">
-        <f>B234/C234</f>
+        <f t="shared" si="66"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G234">
-        <f>C234/D234</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I234" s="44" t="s">
         <v>40</v>
       </c>
       <c r="J234" s="9">
-        <f>B233/B232</f>
+        <f t="shared" si="69"/>
         <v>1</v>
       </c>
       <c r="K234" s="9">
-        <f>C233/C232</f>
+        <f t="shared" si="70"/>
         <v>1</v>
       </c>
       <c r="L234" s="9">
-        <f>D233/D232</f>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A235" s="44" t="s">
         <v>42</v>
       </c>
@@ -16683,38 +16678,38 @@
         <v>52.7</v>
       </c>
       <c r="C235" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>31.62</v>
       </c>
       <c r="D235" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F235">
-        <f>B235/C235</f>
+        <f t="shared" si="66"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G235">
-        <f>C235/D235</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I235" s="44" t="s">
         <v>41</v>
       </c>
       <c r="J235" s="9">
-        <f>B234/B233</f>
+        <f t="shared" si="69"/>
         <v>1</v>
       </c>
       <c r="K235" s="9">
-        <f>C234/C233</f>
+        <f t="shared" si="70"/>
         <v>1</v>
       </c>
       <c r="L235" s="9">
-        <f>D234/D233</f>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A236" s="44" t="s">
         <v>43</v>
       </c>
@@ -16722,38 +16717,38 @@
         <v>52.7</v>
       </c>
       <c r="C236" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>31.62</v>
       </c>
       <c r="D236" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F236">
-        <f>B236/C236</f>
+        <f t="shared" si="66"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G236">
-        <f>C236/D236</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I236" s="44" t="s">
         <v>42</v>
       </c>
       <c r="J236" s="9">
-        <f>B235/B234</f>
+        <f t="shared" si="69"/>
         <v>1</v>
       </c>
       <c r="K236" s="9">
-        <f>C235/C234</f>
+        <f t="shared" si="70"/>
         <v>1</v>
       </c>
       <c r="L236" s="9">
-        <f>D235/D234</f>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A237" s="44" t="s">
         <v>44</v>
       </c>
@@ -16761,38 +16756,38 @@
         <v>52.7</v>
       </c>
       <c r="C237" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>31.62</v>
       </c>
       <c r="D237" s="59">
-        <f t="shared" si="49"/>
+        <f t="shared" si="68"/>
         <v>18.972000000000001</v>
       </c>
       <c r="F237">
-        <f>B237/C237</f>
+        <f t="shared" si="66"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="G237">
-        <f>C237/D237</f>
+        <f t="shared" si="67"/>
         <v>1.6666666666666665</v>
       </c>
       <c r="I237" s="44" t="s">
         <v>43</v>
       </c>
       <c r="J237" s="9">
-        <f>B236/B235</f>
+        <f t="shared" si="69"/>
         <v>1</v>
       </c>
       <c r="K237" s="9">
-        <f>C236/C235</f>
+        <f t="shared" si="70"/>
         <v>1</v>
       </c>
       <c r="L237" s="9">
-        <f>D236/D235</f>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A238" s="35"/>
       <c r="B238" s="35"/>
       <c r="C238" s="42"/>
@@ -16803,19 +16798,19 @@
         <v>44</v>
       </c>
       <c r="J238" s="9">
-        <f>B237/B236</f>
+        <f t="shared" si="69"/>
         <v>1</v>
       </c>
       <c r="K238" s="9">
-        <f>C237/C236</f>
+        <f t="shared" si="70"/>
         <v>1</v>
       </c>
       <c r="L238" s="9">
-        <f>D237/D236</f>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A239" s="66"/>
       <c r="B239" s="20"/>
       <c r="C239" s="20"/>
@@ -16823,7 +16818,7 @@
       <c r="E239" s="67"/>
       <c r="F239" s="35"/>
     </row>
-    <row r="240" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A240" s="63"/>
       <c r="B240" s="64"/>
       <c r="C240" s="64"/>
@@ -16831,35 +16826,35 @@
       <c r="E240" s="67"/>
       <c r="F240" s="35"/>
     </row>
-    <row r="241" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A241" s="6"/>
       <c r="B241" s="61"/>
       <c r="C241" s="61"/>
       <c r="D241" s="61"/>
       <c r="E241" s="25"/>
     </row>
-    <row r="242" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A242" s="6"/>
       <c r="B242" s="61"/>
       <c r="C242" s="61"/>
       <c r="D242" s="61"/>
       <c r="E242" s="25"/>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="25"/>
       <c r="B243" s="25"/>
       <c r="C243" s="25"/>
       <c r="D243" s="25"/>
       <c r="E243" s="25"/>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="25"/>
       <c r="B244" s="25"/>
       <c r="C244" s="25"/>
       <c r="D244" s="25"/>
       <c r="E244" s="25"/>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="25"/>
       <c r="B245" s="25"/>
       <c r="C245" s="25"/>
@@ -16868,6 +16863,8 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="A219:D219"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="I133:I135"/>
     <mergeCell ref="J133:O133"/>
@@ -16883,7 +16880,14 @@
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
     <mergeCell ref="I115:N115"/>
-    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="O81:Y82"/>
+    <mergeCell ref="AA82:AA83"/>
+    <mergeCell ref="J222:L222"/>
+    <mergeCell ref="J202:L202"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A111:Q111"/>
+    <mergeCell ref="N81:N83"/>
+    <mergeCell ref="B81:L82"/>
     <mergeCell ref="A220:A221"/>
     <mergeCell ref="B161:D161"/>
     <mergeCell ref="E161:G161"/>
@@ -16892,15 +16896,6 @@
     <mergeCell ref="B220:D220"/>
     <mergeCell ref="A198:D198"/>
     <mergeCell ref="A199:D199"/>
-    <mergeCell ref="A219:D219"/>
-    <mergeCell ref="O81:Y82"/>
-    <mergeCell ref="AA82:AA83"/>
-    <mergeCell ref="J222:L222"/>
-    <mergeCell ref="J202:L202"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A111:Q111"/>
-    <mergeCell ref="N81:N83"/>
-    <mergeCell ref="B81:L82"/>
     <mergeCell ref="AW81:AW83"/>
     <mergeCell ref="AX81:BB82"/>
     <mergeCell ref="BD81:BD83"/>

</xml_diff>

<commit_message>
Update highlighting of IHME ub on bkrnd mortality
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -339,12 +339,6 @@
     <t>Statistical Release P0302 2019 Mid-year population estimates Table 5.3</t>
   </si>
   <si>
-    <t>Male Background Mortality</t>
-  </si>
-  <si>
-    <t>Female Background Mortality</t>
-  </si>
-  <si>
     <t>For the 0-4 age group, summed mortality for age 0 and ages 1-4</t>
   </si>
   <si>
@@ -489,9 +483,6 @@
     </r>
   </si>
   <si>
-    <t>Used UN values from 1950-1990 before the widespread HIV epidemic. Used the GHDx GBD Results Tool to subtract HIV-specific mortality from all-cause mortality after 1990. Smoothed over the trough in the 1990s and made the decline in under 5 mortality a little less severe. Extrapolated the trend between 2000 and 2017 to 2020.</t>
-  </si>
-  <si>
     <t>UN World Population Prospects 2019, File MORT/17-2: Abridged life tables, for males/females, 1950-2100; GHDx GBD Results Tool: Global Burden of Disease Collaborative Network, Global Burden of Disease Study 2017 (GBD 2017) Results. Seattle, United States: Institute for Health Metrics and Evaluation (IHME), 2018. Available from http://ghdx.healthdata.org/gbd-results-tool. Accessed Feb 21, 2020.</t>
   </si>
   <si>
@@ -500,17 +491,28 @@
   <si>
     <t>Female Background Mortality (upper bound)</t>
   </si>
+  <si>
+    <t>Used UN values from 1950-1990 before the widespread HIV epidemic. Used the GHDx GBD Results Tool to subtract HIV-specific mortality from all-cause mortality after 1990. Smoothed over the trough in the 1990s and made the decline in under 5 mortality a little less severe. Extrapolated the trend between 2000 and 2017 to 2020. Due to excessive population growth in the model, later switched to using the upper CI on background mortality rates, calculated from the IHME data as the upper bound on IHME all-cause mortality minus the lower bound on HIV-specific mortality (SCROLL RIGHT TO SEE VALUES).</t>
+  </si>
+  <si>
+    <t>Male Background Mortality (baseline estimate)</t>
+  </si>
+  <si>
+    <t>Female Background Mortality (baseline estimate)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.00000;\-0.00000;0"/>
     <numFmt numFmtId="165" formatCode="###;\-###;0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0000;\-0.0000;0"/>
+    <numFmt numFmtId="172" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,10 +766,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -1434,9 +1432,9 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="27">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1597,9 +1595,6 @@
     <xf numFmtId="164" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="33" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1615,9 +1610,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1628,13 +1620,6 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1647,31 +1632,16 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="29" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="37" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="29" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="48"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="48"/>
     <xf numFmtId="2" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1684,55 +1654,13 @@
     <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1756,6 +1684,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1765,11 +1696,104 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="170" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="29" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="29" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="172" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="172" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1882,6 +1906,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2396,6 +2421,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2518,6 +2544,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3213,6 +3240,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3340,6 +3368,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4028,6 +4057,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4149,6 +4179,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5634,6 +5665,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8246,8 +8278,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BJ245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C224" sqref="C224"/>
+    <sheetView tabSelected="1" topLeftCell="AF61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AS73" sqref="AS73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8288,16 +8320,21 @@
     <col min="37" max="38" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="15.85546875" customWidth="1"/>
     <col min="49" max="49" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="54" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="58" max="60" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -8325,16 +8362,16 @@
       <c r="Y1" s="37"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -8386,14 +8423,14 @@
       <c r="A4" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="120"/>
-      <c r="D4" s="119" t="s">
+      <c r="C4" s="112"/>
+      <c r="D4" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="120"/>
+      <c r="E4" s="112"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -8821,10 +8858,10 @@
       <c r="A27" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="119" t="s">
+      <c r="B27" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="120"/>
+      <c r="C27" s="112"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -9170,7 +9207,7 @@
     </row>
     <row r="50" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B50" s="37"/>
       <c r="C50" s="37"/>
@@ -9239,19 +9276,19 @@
       <c r="AE51" s="24"/>
     </row>
     <row r="52" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="136" t="s">
+      <c r="A52" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="136" t="s">
+      <c r="B52" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="136"/>
-      <c r="D52" s="136"/>
-      <c r="E52" s="136" t="s">
+      <c r="C52" s="113"/>
+      <c r="D52" s="113"/>
+      <c r="E52" s="113" t="s">
         <v>55</v>
       </c>
-      <c r="F52" s="136"/>
-      <c r="G52" s="136"/>
+      <c r="F52" s="113"/>
+      <c r="G52" s="113"/>
       <c r="X52" s="22"/>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
@@ -9262,7 +9299,7 @@
       <c r="AE52" s="22"/>
     </row>
     <row r="53" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="136"/>
+      <c r="A53" s="113"/>
       <c r="B53" s="33" t="s">
         <v>3</v>
       </c>
@@ -9741,7 +9778,7 @@
     </row>
     <row r="79" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="38" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B79" s="37"/>
       <c r="C79" s="37"/>
@@ -9767,274 +9804,274 @@
       <c r="W79" s="37"/>
       <c r="X79" s="37"/>
     </row>
-    <row r="80" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="36" t="s">
+    <row r="80" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="127" t="s">
+        <v>105</v>
+      </c>
+      <c r="B80" s="127"/>
+      <c r="C80" s="127"/>
+      <c r="D80" s="127"/>
+      <c r="E80" s="127"/>
+      <c r="F80" s="127"/>
+      <c r="G80" s="127"/>
+      <c r="H80" s="127"/>
+      <c r="I80" s="127"/>
+      <c r="J80" s="127"/>
+      <c r="K80" s="127"/>
+      <c r="L80" s="127"/>
+      <c r="M80" s="127"/>
+      <c r="N80" s="127"/>
+      <c r="O80" s="127"/>
+      <c r="P80" s="127"/>
+      <c r="Q80" s="127"/>
+      <c r="R80" s="127"/>
+      <c r="S80" s="127"/>
+      <c r="T80" s="127"/>
+      <c r="U80" s="127"/>
+      <c r="V80" s="127"/>
+      <c r="W80" s="127"/>
+      <c r="X80" s="127"/>
+    </row>
+    <row r="81" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="114" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="98" t="s">
+        <v>106</v>
+      </c>
+      <c r="C81" s="98"/>
+      <c r="D81" s="98"/>
+      <c r="E81" s="98"/>
+      <c r="F81" s="98"/>
+      <c r="G81" s="98"/>
+      <c r="H81" s="98"/>
+      <c r="I81" s="98"/>
+      <c r="J81" s="98"/>
+      <c r="K81" s="98"/>
+      <c r="L81" s="98"/>
+      <c r="N81" s="114" t="s">
+        <v>2</v>
+      </c>
+      <c r="O81" s="98" t="s">
+        <v>107</v>
+      </c>
+      <c r="P81" s="98"/>
+      <c r="Q81" s="98"/>
+      <c r="R81" s="98"/>
+      <c r="S81" s="98"/>
+      <c r="T81" s="98"/>
+      <c r="U81" s="98"/>
+      <c r="V81" s="98"/>
+      <c r="W81" s="98"/>
+      <c r="X81" s="98"/>
+      <c r="Y81" s="98"/>
+      <c r="AA81" s="124" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB81" s="125"/>
+      <c r="AC81" s="125"/>
+      <c r="AD81" s="125"/>
+      <c r="AE81" s="125"/>
+      <c r="AF81" s="125"/>
+      <c r="AG81" s="125"/>
+      <c r="AH81" s="125"/>
+      <c r="AI81" s="126"/>
+      <c r="AW81" s="114" t="s">
+        <v>2</v>
+      </c>
+      <c r="AX81" s="98" t="s">
+        <v>103</v>
+      </c>
+      <c r="AY81" s="98"/>
+      <c r="AZ81" s="98"/>
+      <c r="BA81" s="98"/>
+      <c r="BB81" s="98"/>
+      <c r="BD81" s="114" t="s">
+        <v>2</v>
+      </c>
+      <c r="BE81" s="98" t="s">
         <v>104</v>
       </c>
-      <c r="B80" s="37"/>
-      <c r="C80" s="37"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="37"/>
-      <c r="F80" s="37"/>
-      <c r="G80" s="37"/>
-      <c r="H80" s="37"/>
-      <c r="I80" s="37"/>
-      <c r="J80" s="37"/>
-      <c r="K80" s="37"/>
-      <c r="L80" s="37"/>
-      <c r="M80" s="37"/>
-      <c r="N80" s="37"/>
-      <c r="O80" s="37"/>
-      <c r="P80" s="37"/>
-      <c r="Q80" s="37"/>
-      <c r="R80" s="37"/>
-      <c r="S80" s="37"/>
-      <c r="T80" s="37"/>
-      <c r="U80" s="37"/>
-      <c r="V80" s="37"/>
-      <c r="W80" s="37"/>
-      <c r="X80" s="37"/>
-    </row>
-    <row r="81" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="109" t="s">
+      <c r="BF81" s="98"/>
+      <c r="BG81" s="98"/>
+      <c r="BH81" s="98"/>
+      <c r="BI81" s="98"/>
+    </row>
+    <row r="82" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="115"/>
+      <c r="B82" s="98"/>
+      <c r="C82" s="98"/>
+      <c r="D82" s="98"/>
+      <c r="E82" s="98"/>
+      <c r="F82" s="98"/>
+      <c r="G82" s="98"/>
+      <c r="H82" s="98"/>
+      <c r="I82" s="98"/>
+      <c r="J82" s="98"/>
+      <c r="K82" s="98"/>
+      <c r="L82" s="98"/>
+      <c r="N82" s="115"/>
+      <c r="O82" s="98"/>
+      <c r="P82" s="98"/>
+      <c r="Q82" s="98"/>
+      <c r="R82" s="98"/>
+      <c r="S82" s="98"/>
+      <c r="T82" s="98"/>
+      <c r="U82" s="98"/>
+      <c r="V82" s="98"/>
+      <c r="W82" s="98"/>
+      <c r="X82" s="98"/>
+      <c r="Y82" s="98"/>
+      <c r="AA82" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="112" t="s">
-        <v>78</v>
-      </c>
-      <c r="C81" s="112"/>
-      <c r="D81" s="112"/>
-      <c r="E81" s="112"/>
-      <c r="F81" s="112"/>
-      <c r="G81" s="112"/>
-      <c r="H81" s="112"/>
-      <c r="I81" s="112"/>
-      <c r="J81" s="112"/>
-      <c r="K81" s="112"/>
-      <c r="L81" s="112"/>
-      <c r="N81" s="109" t="s">
-        <v>2</v>
-      </c>
-      <c r="O81" s="112" t="s">
-        <v>79</v>
-      </c>
-      <c r="P81" s="112"/>
-      <c r="Q81" s="112"/>
-      <c r="R81" s="112"/>
-      <c r="S81" s="112"/>
-      <c r="T81" s="112"/>
-      <c r="U81" s="112"/>
-      <c r="V81" s="112"/>
-      <c r="W81" s="112"/>
-      <c r="X81" s="112"/>
-      <c r="Y81" s="112"/>
-      <c r="AA81" s="115" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB81" s="116"/>
-      <c r="AC81" s="116"/>
-      <c r="AD81" s="116"/>
-      <c r="AE81" s="116"/>
-      <c r="AF81" s="116"/>
-      <c r="AG81" s="116"/>
-      <c r="AH81" s="116"/>
-      <c r="AI81" s="117"/>
-      <c r="AW81" s="109" t="s">
-        <v>2</v>
-      </c>
-      <c r="AX81" s="112" t="s">
-        <v>106</v>
-      </c>
-      <c r="AY81" s="112"/>
-      <c r="AZ81" s="112"/>
-      <c r="BA81" s="112"/>
-      <c r="BB81" s="112"/>
-      <c r="BD81" s="109" t="s">
-        <v>2</v>
-      </c>
-      <c r="BE81" s="112" t="s">
-        <v>107</v>
-      </c>
-      <c r="BF81" s="112"/>
-      <c r="BG81" s="112"/>
-      <c r="BH81" s="112"/>
-      <c r="BI81" s="112"/>
-    </row>
-    <row r="82" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="110"/>
-      <c r="B82" s="112"/>
-      <c r="C82" s="112"/>
-      <c r="D82" s="112"/>
-      <c r="E82" s="112"/>
-      <c r="F82" s="112"/>
-      <c r="G82" s="112"/>
-      <c r="H82" s="112"/>
-      <c r="I82" s="112"/>
-      <c r="J82" s="112"/>
-      <c r="K82" s="112"/>
-      <c r="L82" s="112"/>
-      <c r="N82" s="110"/>
-      <c r="O82" s="112"/>
-      <c r="P82" s="112"/>
-      <c r="Q82" s="112"/>
-      <c r="R82" s="112"/>
-      <c r="S82" s="112"/>
-      <c r="T82" s="112"/>
-      <c r="U82" s="112"/>
-      <c r="V82" s="112"/>
-      <c r="W82" s="112"/>
-      <c r="X82" s="112"/>
-      <c r="Y82" s="112"/>
-      <c r="AA82" s="113" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB82" s="115" t="s">
+      <c r="AB82" s="124" t="s">
         <v>72</v>
       </c>
-      <c r="AC82" s="116"/>
-      <c r="AD82" s="116"/>
-      <c r="AE82" s="116"/>
-      <c r="AF82" s="116"/>
-      <c r="AG82" s="116"/>
-      <c r="AH82" s="116"/>
-      <c r="AI82" s="117"/>
-      <c r="AW82" s="110"/>
-      <c r="AX82" s="112"/>
-      <c r="AY82" s="112"/>
-      <c r="AZ82" s="112"/>
-      <c r="BA82" s="112"/>
-      <c r="BB82" s="112"/>
-      <c r="BD82" s="110"/>
-      <c r="BE82" s="112"/>
-      <c r="BF82" s="112"/>
-      <c r="BG82" s="112"/>
-      <c r="BH82" s="112"/>
-      <c r="BI82" s="112"/>
+      <c r="AC82" s="125"/>
+      <c r="AD82" s="125"/>
+      <c r="AE82" s="125"/>
+      <c r="AF82" s="125"/>
+      <c r="AG82" s="125"/>
+      <c r="AH82" s="125"/>
+      <c r="AI82" s="126"/>
+      <c r="AW82" s="115"/>
+      <c r="AX82" s="98"/>
+      <c r="AY82" s="98"/>
+      <c r="AZ82" s="98"/>
+      <c r="BA82" s="98"/>
+      <c r="BB82" s="98"/>
+      <c r="BD82" s="115"/>
+      <c r="BE82" s="98"/>
+      <c r="BF82" s="98"/>
+      <c r="BG82" s="98"/>
+      <c r="BH82" s="98"/>
+      <c r="BI82" s="98"/>
     </row>
     <row r="83" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="111"/>
+      <c r="A83" s="116"/>
       <c r="B83" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C83" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="D83" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="C83" s="71" t="s">
+      <c r="E83" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="D83" s="71" t="s">
+      <c r="F83" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="G83" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="E83" s="71" t="s">
+      <c r="H83" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="I83" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="F83" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="G83" s="71" t="s">
+      <c r="J83" s="83">
+        <v>2000</v>
+      </c>
+      <c r="K83" s="84">
+        <v>2017</v>
+      </c>
+      <c r="L83" s="82">
+        <v>2020</v>
+      </c>
+      <c r="N83" s="116"/>
+      <c r="O83" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="P83" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q83" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="R83" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="S83" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="T83" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="U83" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="H83" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="I83" s="71" t="s">
+      <c r="V83" s="72" t="s">
+        <v>96</v>
+      </c>
+      <c r="W83" s="131">
+        <v>2000</v>
+      </c>
+      <c r="X83" s="132">
+        <v>2017</v>
+      </c>
+      <c r="Y83" s="133">
+        <v>2020</v>
+      </c>
+      <c r="AA83" s="119"/>
+      <c r="AB83" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC83" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD83" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE83" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF83" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="J83" s="88">
+      <c r="AG83" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH83" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI83" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW83" s="116"/>
+      <c r="AX83" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="AY83" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="AZ83" s="83">
         <v>2000</v>
       </c>
-      <c r="K83" s="89">
+      <c r="BA83" s="84">
         <v>2017</v>
       </c>
-      <c r="L83" s="84">
+      <c r="BB83" s="84">
         <v>2020</v>
       </c>
-      <c r="N83" s="111"/>
-      <c r="O83" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="P83" s="71" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q83" s="71" t="s">
-        <v>95</v>
-      </c>
-      <c r="R83" s="71" t="s">
+      <c r="BD83" s="116"/>
+      <c r="BE83" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF83" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="S83" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="T83" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="U83" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="V83" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="W83" s="88">
+      <c r="BG83" s="83">
         <v>2000</v>
       </c>
-      <c r="X83" s="89">
+      <c r="BH83" s="84">
         <v>2017</v>
       </c>
-      <c r="Y83" s="84">
-        <v>2020</v>
-      </c>
-      <c r="AA83" s="114"/>
-      <c r="AB83" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC83" s="71" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD83" s="71" t="s">
-        <v>95</v>
-      </c>
-      <c r="AE83" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF83" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="AG83" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="AH83" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI83" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="AW83" s="111"/>
-      <c r="AX83" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="AY83" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="AZ83" s="88">
-        <v>2000</v>
-      </c>
-      <c r="BA83" s="89">
-        <v>2017</v>
-      </c>
-      <c r="BB83" s="89">
-        <v>2020</v>
-      </c>
-      <c r="BD83" s="111"/>
-      <c r="BE83" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="BF83" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="BG83" s="88">
-        <v>2000</v>
-      </c>
-      <c r="BH83" s="89">
-        <v>2017</v>
-      </c>
-      <c r="BI83" s="89">
+      <c r="BI83" s="84">
         <v>2020</v>
       </c>
     </row>
@@ -10042,7 +10079,7 @@
       <c r="A84" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="B84" s="74">
+      <c r="B84" s="73">
         <f t="shared" ref="B84:I84" si="7">SUM(AB84:AB85)</f>
         <v>0.19005920400000001</v>
       </c>
@@ -10070,17 +10107,17 @@
         <f t="shared" si="7"/>
         <v>7.0407469099999995E-2</v>
       </c>
-      <c r="I84" s="85">
+      <c r="I84" s="88">
         <f t="shared" si="7"/>
         <v>5.6975585300000006E-2</v>
       </c>
-      <c r="J84" s="92">
+      <c r="J84" s="128">
         <v>1.2464773E-2</v>
       </c>
-      <c r="K84" s="90">
+      <c r="K84" s="85">
         <v>5.892614E-3</v>
       </c>
-      <c r="L84" s="87">
+      <c r="L84" s="130">
         <f>K84+($L$83-$K$83)*M84</f>
         <v>4.7328212352941174E-3</v>
       </c>
@@ -10088,10 +10125,10 @@
         <f>(K84-J84)/($K$83-$J$83)</f>
         <v>-3.865975882352941E-4</v>
       </c>
-      <c r="N84" s="83" t="s">
+      <c r="N84" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="O84" s="74">
+      <c r="O84" s="73">
         <f t="shared" ref="O84:V84" si="8">SUM(AB89:AB90)</f>
         <v>0.16283755500000002</v>
       </c>
@@ -10119,17 +10156,17 @@
         <f t="shared" si="8"/>
         <v>5.96665085E-2</v>
       </c>
-      <c r="V84" s="85">
+      <c r="V84" s="88">
         <f t="shared" si="8"/>
         <v>4.7441704699999997E-2</v>
       </c>
-      <c r="W84" s="92">
+      <c r="W84" s="128">
         <v>1.0375972000000001E-2</v>
       </c>
-      <c r="X84" s="90">
+      <c r="X84" s="128">
         <v>4.9718649999999998E-3</v>
       </c>
-      <c r="Y84" s="87">
+      <c r="Y84" s="130">
         <f>X84+($Y$83-$X$83)*Z84</f>
         <v>4.0181990588235295E-3</v>
       </c>
@@ -10137,76 +10174,76 @@
         <f>(X84-W84)/($X$83-$W$83)</f>
         <v>-3.1788864705882357E-4</v>
       </c>
-      <c r="AA84" s="75">
-        <v>0</v>
-      </c>
-      <c r="AB84" s="76">
+      <c r="AA84" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB84" s="75">
         <v>0.15925727000000001</v>
       </c>
-      <c r="AC84" s="76">
+      <c r="AC84" s="75">
         <v>0.14222435</v>
       </c>
-      <c r="AD84" s="76">
+      <c r="AD84" s="75">
         <v>0.13109251</v>
       </c>
-      <c r="AE84" s="76">
+      <c r="AE84" s="75">
         <v>0.11936734</v>
       </c>
-      <c r="AF84" s="76">
+      <c r="AF84" s="75">
         <v>0.10190435</v>
       </c>
-      <c r="AG84" s="76">
+      <c r="AG84" s="75">
         <v>8.0275031999999996E-2</v>
       </c>
-      <c r="AH84" s="76">
+      <c r="AH84" s="75">
         <v>6.3396686999999993E-2</v>
       </c>
-      <c r="AI84" s="77">
+      <c r="AI84" s="76">
         <v>5.1751479000000003E-2</v>
       </c>
-      <c r="AW84" s="94" t="s">
+      <c r="AW84" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="AX84" s="73">
+      <c r="AX84" s="134">
         <v>0.19005920400000001</v>
       </c>
-      <c r="AY84" s="95">
+      <c r="AY84" s="135">
         <v>5.6975585300000006E-2</v>
       </c>
-      <c r="AZ84" s="96">
+      <c r="AZ84" s="136">
         <v>1.4393767E-2</v>
       </c>
-      <c r="BA84" s="96">
+      <c r="BA84" s="137">
         <v>6.7479519999999998E-3</v>
       </c>
-      <c r="BB84" s="97">
+      <c r="BB84" s="138">
         <f>BA84+($L$83-$K$83)*BC84</f>
         <v>5.3986905294117647E-3</v>
       </c>
-      <c r="BC84">
+      <c r="BC84" s="139">
         <f>(BA84-AZ84)/($K$83-$J$83)</f>
         <v>-4.4975382352941177E-4</v>
       </c>
-      <c r="BD84" s="94" t="s">
+      <c r="BD84" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="BE84" s="100">
+      <c r="BE84" s="142">
         <v>0.16283755500000002</v>
       </c>
-      <c r="BF84" s="101">
+      <c r="BF84" s="143">
         <v>4.7441704699999997E-2</v>
       </c>
-      <c r="BG84" s="96">
+      <c r="BG84" s="144">
         <v>1.1839005E-2</v>
       </c>
-      <c r="BH84" s="96">
+      <c r="BH84" s="145">
         <v>5.6765679999999999E-3</v>
       </c>
-      <c r="BI84" s="97">
+      <c r="BI84" s="146">
         <f>BH84+($Y$83-$X$83)*BJ84</f>
         <v>4.589079117647059E-3</v>
       </c>
-      <c r="BJ84">
+      <c r="BJ84" s="147">
         <f>(BH84-BG84)/($X$83-$W$83)</f>
         <v>-3.6249629411764703E-4</v>
       </c>
@@ -10215,37 +10252,37 @@
       <c r="A85" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B85" s="80">
+      <c r="B85" s="75">
         <v>8.6783771000000006E-3</v>
       </c>
-      <c r="C85" s="76">
+      <c r="C85" s="75">
         <v>7.2583379999999996E-3</v>
       </c>
-      <c r="D85" s="76">
+      <c r="D85" s="75">
         <v>6.3381319000000002E-3</v>
       </c>
-      <c r="E85" s="76">
+      <c r="E85" s="75">
         <v>5.4525481999999998E-3</v>
       </c>
-      <c r="F85" s="76">
+      <c r="F85" s="75">
         <v>4.5081523000000002E-3</v>
       </c>
-      <c r="G85" s="76">
+      <c r="G85" s="75">
         <v>3.6766398E-3</v>
       </c>
-      <c r="H85" s="76">
+      <c r="H85" s="75">
         <v>3.0634688E-3</v>
       </c>
-      <c r="I85" s="86">
+      <c r="I85" s="89">
         <v>2.4750038999999998E-3</v>
       </c>
-      <c r="J85" s="92">
+      <c r="J85" s="128">
         <v>1.2523619999999999E-3</v>
       </c>
-      <c r="K85" s="91">
+      <c r="K85" s="86">
         <v>4.3800000000000002E-4</v>
       </c>
-      <c r="L85" s="87">
+      <c r="L85" s="130">
         <f t="shared" ref="L85:L99" si="9">K85+($L$83-$K$83)*M85</f>
         <v>2.9428905882352948E-4</v>
       </c>
@@ -10253,40 +10290,40 @@
         <f t="shared" ref="M85:M99" si="10">(K85-J85)/($K$83-$J$83)</f>
         <v>-4.7903647058823526E-5</v>
       </c>
-      <c r="N85" s="83" t="s">
+      <c r="N85" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="O85" s="80">
+      <c r="O85" s="75">
         <v>7.4032815999999996E-3</v>
       </c>
-      <c r="P85" s="76">
+      <c r="P85" s="75">
         <v>6.0150315999999999E-3</v>
       </c>
-      <c r="Q85" s="76">
+      <c r="Q85" s="75">
         <v>5.2116343000000002E-3</v>
       </c>
-      <c r="R85" s="76">
+      <c r="R85" s="75">
         <v>4.4708409999999997E-3</v>
       </c>
-      <c r="S85" s="76">
+      <c r="S85" s="75">
         <v>3.6394486000000002E-3</v>
       </c>
-      <c r="T85" s="76">
+      <c r="T85" s="75">
         <v>2.8782094000000002E-3</v>
       </c>
-      <c r="U85" s="76">
+      <c r="U85" s="75">
         <v>2.3506893000000001E-3</v>
       </c>
-      <c r="V85" s="86">
+      <c r="V85" s="89">
         <v>1.8590649E-3</v>
       </c>
-      <c r="W85" s="93">
+      <c r="W85" s="129">
         <v>9.1699999999999995E-4</v>
       </c>
-      <c r="X85" s="91">
+      <c r="X85" s="129">
         <v>3.0899999999999998E-4</v>
       </c>
-      <c r="Y85" s="87">
+      <c r="Y85" s="130">
         <f t="shared" ref="Y85:Y99" si="11">X85+($Y$83-$X$83)*Z85</f>
         <v>2.0170588235294114E-4</v>
       </c>
@@ -10294,76 +10331,76 @@
         <f t="shared" ref="Z85:Z99" si="12">(X85-W85)/($X$83-$W$83)</f>
         <v>-3.5764705882352941E-5</v>
       </c>
-      <c r="AA85" s="78" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB85" s="76">
+      <c r="AA85" s="77" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB85" s="75">
         <v>3.0801934E-2</v>
       </c>
-      <c r="AC85" s="76">
+      <c r="AC85" s="75">
         <v>2.4799885000000001E-2</v>
       </c>
-      <c r="AD85" s="76">
+      <c r="AD85" s="75">
         <v>2.1231481E-2</v>
       </c>
-      <c r="AE85" s="76">
+      <c r="AE85" s="75">
         <v>1.7857484E-2</v>
       </c>
-      <c r="AF85" s="76">
+      <c r="AF85" s="75">
         <v>1.3771911E-2</v>
       </c>
-      <c r="AG85" s="76">
+      <c r="AG85" s="75">
         <v>9.7272777000000001E-3</v>
       </c>
-      <c r="AH85" s="76">
+      <c r="AH85" s="75">
         <v>7.0107820999999997E-3</v>
       </c>
-      <c r="AI85" s="77">
+      <c r="AI85" s="76">
         <v>5.2241062999999997E-3</v>
       </c>
-      <c r="AW85" s="94" t="s">
+      <c r="AW85" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="AX85" s="76">
+      <c r="AX85" s="140">
         <v>8.6783771000000006E-3</v>
       </c>
-      <c r="AY85" s="98">
+      <c r="AY85" s="141">
         <v>2.4750038999999998E-3</v>
       </c>
-      <c r="AZ85" s="96">
+      <c r="AZ85" s="136">
         <v>1.343999E-3</v>
       </c>
-      <c r="BA85" s="99">
+      <c r="BA85" s="137">
         <v>5.1699999999999999E-4</v>
       </c>
-      <c r="BB85" s="97">
+      <c r="BB85" s="138">
         <f t="shared" ref="BB85:BB99" si="13">BA85+($L$83-$K$83)*BC85</f>
         <v>3.7105899999999997E-4</v>
       </c>
-      <c r="BC85">
+      <c r="BC85" s="139">
         <f t="shared" ref="BC85:BC99" si="14">(BA85-AZ85)/($K$83-$J$83)</f>
         <v>-4.8647000000000004E-5</v>
       </c>
-      <c r="BD85" s="94" t="s">
+      <c r="BD85" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="BE85" s="76">
+      <c r="BE85" s="148">
         <v>7.4032815999999996E-3</v>
       </c>
-      <c r="BF85" s="98">
+      <c r="BF85" s="149">
         <v>1.8590649E-3</v>
       </c>
-      <c r="BG85" s="99">
+      <c r="BG85" s="144">
         <v>9.7599999999999998E-4</v>
       </c>
-      <c r="BH85" s="99">
+      <c r="BH85" s="145">
         <v>3.6499999999999998E-4</v>
       </c>
-      <c r="BI85" s="97">
+      <c r="BI85" s="146">
         <f t="shared" ref="BI85:BI99" si="15">BH85+($Y$83-$X$83)*BJ85</f>
         <v>2.5717647058823528E-4</v>
       </c>
-      <c r="BJ85">
+      <c r="BJ85" s="147">
         <f t="shared" ref="BJ85:BJ99" si="16">(BH85-BG85)/($X$83-$W$83)</f>
         <v>-3.5941176470588238E-5</v>
       </c>
@@ -10372,37 +10409,37 @@
       <c r="A86" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="B86" s="80">
+      <c r="B86" s="75">
         <v>4.7901753000000004E-3</v>
       </c>
-      <c r="C86" s="76">
+      <c r="C86" s="75">
         <v>4.1213899000000003E-3</v>
       </c>
-      <c r="D86" s="76">
+      <c r="D86" s="75">
         <v>3.6590022999999998E-3</v>
       </c>
-      <c r="E86" s="76">
+      <c r="E86" s="75">
         <v>3.198991E-3</v>
       </c>
-      <c r="F86" s="76">
+      <c r="F86" s="75">
         <v>2.7091355999999999E-3</v>
       </c>
-      <c r="G86" s="76">
+      <c r="G86" s="75">
         <v>2.2757054E-3</v>
       </c>
-      <c r="H86" s="76">
+      <c r="H86" s="75">
         <v>1.9361118E-3</v>
       </c>
-      <c r="I86" s="86">
+      <c r="I86" s="89">
         <v>1.5814690000000001E-3</v>
       </c>
-      <c r="J86" s="93">
+      <c r="J86" s="129">
         <v>9.77E-4</v>
       </c>
-      <c r="K86" s="91">
+      <c r="K86" s="86">
         <v>2.7099999999999997E-4</v>
       </c>
-      <c r="L86" s="87">
+      <c r="L86" s="130">
         <f t="shared" si="9"/>
         <v>1.4641176470588232E-4</v>
       </c>
@@ -10410,40 +10447,40 @@
         <f t="shared" si="10"/>
         <v>-4.1529411764705884E-5</v>
       </c>
-      <c r="N86" s="83" t="s">
+      <c r="N86" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="O86" s="80">
+      <c r="O86" s="75">
         <v>4.3711651000000002E-3</v>
       </c>
-      <c r="P86" s="76">
+      <c r="P86" s="75">
         <v>3.6299777000000002E-3</v>
       </c>
-      <c r="Q86" s="76">
+      <c r="Q86" s="75">
         <v>3.1849489999999999E-3</v>
       </c>
-      <c r="R86" s="76">
+      <c r="R86" s="75">
         <v>2.765787E-3</v>
       </c>
-      <c r="S86" s="76">
+      <c r="S86" s="75">
         <v>2.2931724000000001E-3</v>
       </c>
-      <c r="T86" s="76">
+      <c r="T86" s="75">
         <v>1.8562381000000001E-3</v>
       </c>
-      <c r="U86" s="76">
+      <c r="U86" s="75">
         <v>1.5421367E-3</v>
       </c>
-      <c r="V86" s="86">
+      <c r="V86" s="89">
         <v>1.2227608999999999E-3</v>
       </c>
-      <c r="W86" s="93">
+      <c r="W86" s="129">
         <v>7.4100000000000001E-4</v>
       </c>
-      <c r="X86" s="91">
+      <c r="X86" s="129">
         <v>1.65E-4</v>
       </c>
-      <c r="Y86" s="87">
+      <c r="Y86" s="130">
         <f t="shared" si="11"/>
         <v>6.335294117647058E-5</v>
       </c>
@@ -10460,49 +10497,49 @@
       <c r="AG86" s="35"/>
       <c r="AH86" s="35"/>
       <c r="AI86" s="35"/>
-      <c r="AW86" s="94" t="s">
+      <c r="AW86" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="AX86" s="76">
+      <c r="AX86" s="140">
         <v>4.7901753000000004E-3</v>
       </c>
-      <c r="AY86" s="98">
+      <c r="AY86" s="141">
         <v>1.5814690000000001E-3</v>
       </c>
-      <c r="AZ86" s="96">
+      <c r="AZ86" s="136">
         <v>1.006123E-3</v>
       </c>
-      <c r="BA86" s="99">
+      <c r="BA86" s="137">
         <v>3.1799999999999998E-4</v>
       </c>
-      <c r="BB86" s="97">
+      <c r="BB86" s="138">
         <f t="shared" si="13"/>
         <v>1.9656652941176466E-4</v>
       </c>
-      <c r="BC86">
+      <c r="BC86" s="139">
         <f t="shared" si="14"/>
         <v>-4.0477823529411771E-5</v>
       </c>
-      <c r="BD86" s="94" t="s">
+      <c r="BD86" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="BE86" s="76">
+      <c r="BE86" s="148">
         <v>4.3711651000000002E-3</v>
       </c>
-      <c r="BF86" s="98">
+      <c r="BF86" s="149">
         <v>1.2227608999999999E-3</v>
       </c>
-      <c r="BG86" s="99">
+      <c r="BG86" s="144">
         <v>7.5699999999999997E-4</v>
       </c>
-      <c r="BH86" s="99">
+      <c r="BH86" s="145">
         <v>1.95E-4</v>
       </c>
-      <c r="BI86" s="97">
+      <c r="BI86" s="146">
         <f t="shared" si="15"/>
         <v>9.5823529411764706E-5</v>
       </c>
-      <c r="BJ86">
+      <c r="BJ86" s="147">
         <f t="shared" si="16"/>
         <v>-3.3058823529411766E-5</v>
       </c>
@@ -10511,37 +10548,37 @@
       <c r="A87" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="B87" s="80">
+      <c r="B87" s="75">
         <v>5.9821824000000001E-3</v>
       </c>
-      <c r="C87" s="76">
+      <c r="C87" s="75">
         <v>5.3382910000000002E-3</v>
       </c>
-      <c r="D87" s="76">
+      <c r="D87" s="75">
         <v>4.8685472E-3</v>
       </c>
-      <c r="E87" s="76">
+      <c r="E87" s="75">
         <v>4.3821110000000002E-3</v>
       </c>
-      <c r="F87" s="76">
+      <c r="F87" s="75">
         <v>3.8498661E-3</v>
       </c>
-      <c r="G87" s="76">
+      <c r="G87" s="75">
         <v>3.3638228000000001E-3</v>
       </c>
-      <c r="H87" s="76">
+      <c r="H87" s="75">
         <v>2.9596564999999999E-3</v>
       </c>
-      <c r="I87" s="86">
+      <c r="I87" s="89">
         <v>2.5001934000000001E-3</v>
       </c>
-      <c r="J87" s="92">
+      <c r="J87" s="128">
         <v>2.1267130000000001E-3</v>
       </c>
-      <c r="K87" s="91">
+      <c r="K87" s="86">
         <v>6.4599999999999998E-4</v>
       </c>
-      <c r="L87" s="87">
+      <c r="L87" s="130">
         <f t="shared" si="9"/>
         <v>3.8469770588235287E-4</v>
       </c>
@@ -10549,40 +10586,40 @@
         <f t="shared" si="10"/>
         <v>-8.7100764705882374E-5</v>
       </c>
-      <c r="N87" s="83" t="s">
+      <c r="N87" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="O87" s="80">
+      <c r="O87" s="75">
         <v>4.8596317000000003E-3</v>
       </c>
-      <c r="P87" s="76">
+      <c r="P87" s="75">
         <v>4.1952435000000001E-3</v>
       </c>
-      <c r="Q87" s="76">
+      <c r="Q87" s="75">
         <v>3.7691500999999998E-3</v>
       </c>
-      <c r="R87" s="76">
+      <c r="R87" s="75">
         <v>3.3518339000000001E-3</v>
       </c>
-      <c r="S87" s="76">
+      <c r="S87" s="75">
         <v>2.8752540999999999E-3</v>
       </c>
-      <c r="T87" s="76">
+      <c r="T87" s="75">
         <v>2.4258770999999999E-3</v>
       </c>
-      <c r="U87" s="76">
+      <c r="U87" s="75">
         <v>2.0807315999999999E-3</v>
       </c>
-      <c r="V87" s="86">
+      <c r="V87" s="89">
         <v>1.6750273E-3</v>
       </c>
-      <c r="W87" s="92">
+      <c r="W87" s="128">
         <v>1.469932E-3</v>
       </c>
-      <c r="X87" s="91">
+      <c r="X87" s="129">
         <v>3.9800000000000002E-4</v>
       </c>
-      <c r="Y87" s="87">
+      <c r="Y87" s="130">
         <f t="shared" si="11"/>
         <v>2.0883552941176474E-4</v>
       </c>
@@ -10590,62 +10627,62 @@
         <f t="shared" si="12"/>
         <v>-6.3054823529411761E-5</v>
       </c>
-      <c r="AA87" s="113" t="s">
+      <c r="AA87" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="AB87" s="115" t="s">
+      <c r="AB87" s="124" t="s">
         <v>73</v>
       </c>
-      <c r="AC87" s="116"/>
-      <c r="AD87" s="116"/>
-      <c r="AE87" s="116"/>
-      <c r="AF87" s="116"/>
-      <c r="AG87" s="116"/>
-      <c r="AH87" s="116"/>
-      <c r="AI87" s="117"/>
-      <c r="AW87" s="94" t="s">
+      <c r="AC87" s="125"/>
+      <c r="AD87" s="125"/>
+      <c r="AE87" s="125"/>
+      <c r="AF87" s="125"/>
+      <c r="AG87" s="125"/>
+      <c r="AH87" s="125"/>
+      <c r="AI87" s="126"/>
+      <c r="AW87" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="AX87" s="76">
+      <c r="AX87" s="140">
         <v>5.9821824000000001E-3</v>
       </c>
-      <c r="AY87" s="98">
+      <c r="AY87" s="141">
         <v>2.5001934000000001E-3</v>
       </c>
-      <c r="AZ87" s="96">
+      <c r="AZ87" s="136">
         <v>2.2244869999999998E-3</v>
       </c>
-      <c r="BA87" s="99">
+      <c r="BA87" s="137">
         <v>9.2199999999999997E-4</v>
       </c>
-      <c r="BB87" s="97">
+      <c r="BB87" s="138">
         <f t="shared" si="13"/>
         <v>6.9214935294117648E-4</v>
       </c>
-      <c r="BC87">
+      <c r="BC87" s="139">
         <f t="shared" si="14"/>
         <v>-7.6616882352941159E-5</v>
       </c>
-      <c r="BD87" s="94" t="s">
+      <c r="BD87" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="BE87" s="76">
+      <c r="BE87" s="148">
         <v>4.8596317000000003E-3</v>
       </c>
-      <c r="BF87" s="98">
+      <c r="BF87" s="149">
         <v>1.6750273E-3</v>
       </c>
-      <c r="BG87" s="96">
+      <c r="BG87" s="144">
         <v>1.7839729999999999E-3</v>
       </c>
-      <c r="BH87" s="99">
+      <c r="BH87" s="145">
         <v>7.0299999999999996E-4</v>
       </c>
-      <c r="BI87" s="97">
+      <c r="BI87" s="146">
         <f t="shared" si="15"/>
         <v>5.1224005882352934E-4</v>
       </c>
-      <c r="BJ87">
+      <c r="BJ87" s="147">
         <f t="shared" si="16"/>
         <v>-6.3586647058823525E-5</v>
       </c>
@@ -10654,37 +10691,37 @@
       <c r="A88" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="B88" s="80">
+      <c r="B88" s="75">
         <v>8.4956649999999995E-3</v>
       </c>
-      <c r="C88" s="76">
+      <c r="C88" s="75">
         <v>7.6593564000000001E-3</v>
       </c>
-      <c r="D88" s="76">
+      <c r="D88" s="75">
         <v>7.0310347999999996E-3</v>
       </c>
-      <c r="E88" s="76">
+      <c r="E88" s="75">
         <v>6.3705656999999997E-3</v>
       </c>
-      <c r="F88" s="76">
+      <c r="F88" s="75">
         <v>5.6486914999999997E-3</v>
       </c>
-      <c r="G88" s="76">
+      <c r="G88" s="75">
         <v>4.9892453999999999E-3</v>
       </c>
-      <c r="H88" s="76">
+      <c r="H88" s="75">
         <v>4.4258235999999999E-3</v>
       </c>
-      <c r="I88" s="86">
+      <c r="I88" s="89">
         <v>3.7640993E-3</v>
       </c>
-      <c r="J88" s="92">
+      <c r="J88" s="128">
         <v>3.647225E-3</v>
       </c>
-      <c r="K88" s="90">
+      <c r="K88" s="85">
         <v>2.068032E-3</v>
       </c>
-      <c r="L88" s="87">
+      <c r="L88" s="130">
         <f t="shared" si="9"/>
         <v>1.7893508823529412E-3</v>
       </c>
@@ -10692,40 +10729,40 @@
         <f t="shared" si="10"/>
         <v>-9.2893705882352942E-5</v>
       </c>
-      <c r="N88" s="83" t="s">
+      <c r="N88" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="O88" s="80">
+      <c r="O88" s="75">
         <v>5.6320531999999998E-3</v>
       </c>
-      <c r="P88" s="76">
+      <c r="P88" s="75">
         <v>5.0807012E-3</v>
       </c>
-      <c r="Q88" s="76">
+      <c r="Q88" s="75">
         <v>4.6760279E-3</v>
       </c>
-      <c r="R88" s="76">
+      <c r="R88" s="75">
         <v>4.2537668999999998E-3</v>
       </c>
-      <c r="S88" s="76">
+      <c r="S88" s="75">
         <v>3.7813996000000002E-3</v>
       </c>
-      <c r="T88" s="76">
+      <c r="T88" s="75">
         <v>3.3430482E-3</v>
       </c>
-      <c r="U88" s="76">
+      <c r="U88" s="75">
         <v>2.9634518E-3</v>
       </c>
-      <c r="V88" s="86">
+      <c r="V88" s="89">
         <v>2.3815536E-3</v>
       </c>
-      <c r="W88" s="92">
+      <c r="W88" s="128">
         <v>3.4466029999999999E-3</v>
       </c>
-      <c r="X88" s="90">
+      <c r="X88" s="128">
         <v>1.022128E-3</v>
       </c>
-      <c r="Y88" s="87">
+      <c r="Y88" s="130">
         <f t="shared" si="11"/>
         <v>5.9427947058823534E-4</v>
       </c>
@@ -10733,74 +10770,74 @@
         <f t="shared" si="12"/>
         <v>-1.4261617647058823E-4</v>
       </c>
-      <c r="AA88" s="114"/>
+      <c r="AA88" s="119"/>
       <c r="AB88" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC88" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD88" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="AC88" s="71" t="s">
+      <c r="AE88" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="AD88" s="71" t="s">
+      <c r="AF88" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG88" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="AE88" s="71" t="s">
+      <c r="AH88" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI88" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="AF88" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="AG88" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="AH88" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI88" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="AW88" s="94" t="s">
+      <c r="AW88" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="AX88" s="76">
+      <c r="AX88" s="140">
         <v>8.4956649999999995E-3</v>
       </c>
-      <c r="AY88" s="98">
+      <c r="AY88" s="141">
         <v>3.7640993E-3</v>
       </c>
-      <c r="AZ88" s="96">
+      <c r="AZ88" s="136">
         <v>4.404697E-3</v>
       </c>
-      <c r="BA88" s="96">
+      <c r="BA88" s="137">
         <v>2.4275730000000001E-3</v>
       </c>
-      <c r="BB88" s="97">
+      <c r="BB88" s="138">
         <f t="shared" si="13"/>
         <v>2.0786687647058825E-3</v>
       </c>
-      <c r="BC88">
+      <c r="BC88" s="139">
         <f t="shared" si="14"/>
         <v>-1.1630141176470587E-4</v>
       </c>
-      <c r="BD88" s="94" t="s">
+      <c r="BD88" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="BE88" s="76">
+      <c r="BE88" s="148">
         <v>5.6320531999999998E-3</v>
       </c>
-      <c r="BF88" s="98">
+      <c r="BF88" s="149">
         <v>2.3815536E-3</v>
       </c>
-      <c r="BG88" s="96">
+      <c r="BG88" s="144">
         <v>4.9665059999999999E-3</v>
       </c>
-      <c r="BH88" s="96">
+      <c r="BH88" s="145">
         <v>1.625781E-3</v>
       </c>
-      <c r="BI88" s="97">
+      <c r="BI88" s="146">
         <f t="shared" si="15"/>
         <v>1.0362412941176471E-3</v>
       </c>
-      <c r="BJ88">
+      <c r="BJ88" s="147">
         <f t="shared" si="16"/>
         <v>-1.9651323529411765E-4</v>
       </c>
@@ -10809,37 +10846,37 @@
       <c r="A89" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="B89" s="80">
+      <c r="B89" s="75">
         <v>9.3605019000000001E-3</v>
       </c>
-      <c r="C89" s="76">
+      <c r="C89" s="75">
         <v>8.54654E-3</v>
       </c>
-      <c r="D89" s="76">
+      <c r="D89" s="75">
         <v>7.8817746000000004E-3</v>
       </c>
-      <c r="E89" s="76">
+      <c r="E89" s="75">
         <v>7.1632086000000001E-3</v>
       </c>
-      <c r="F89" s="76">
+      <c r="F89" s="75">
         <v>6.4013278999999999E-3</v>
       </c>
-      <c r="G89" s="76">
+      <c r="G89" s="75">
         <v>5.7255068999999999E-3</v>
       </c>
-      <c r="H89" s="76">
+      <c r="H89" s="75">
         <v>5.1091371999999998E-3</v>
       </c>
-      <c r="I89" s="86">
+      <c r="I89" s="89">
         <v>4.3315932999999996E-3</v>
       </c>
-      <c r="J89" s="92">
+      <c r="J89" s="128">
         <v>5.7620409999999999E-3</v>
       </c>
-      <c r="K89" s="90">
+      <c r="K89" s="85">
         <v>2.644057E-3</v>
       </c>
-      <c r="L89" s="87">
+      <c r="L89" s="130">
         <f t="shared" si="9"/>
         <v>2.0938245294117646E-3</v>
       </c>
@@ -10847,40 +10884,40 @@
         <f t="shared" si="10"/>
         <v>-1.8341082352941175E-4</v>
       </c>
-      <c r="N89" s="83" t="s">
+      <c r="N89" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="O89" s="80">
+      <c r="O89" s="75">
         <v>6.4621250999999996E-3</v>
       </c>
-      <c r="P89" s="76">
+      <c r="P89" s="75">
         <v>6.0272501000000001E-3</v>
       </c>
-      <c r="Q89" s="76">
+      <c r="Q89" s="75">
         <v>5.6386778999999998E-3</v>
       </c>
-      <c r="R89" s="76">
+      <c r="R89" s="75">
         <v>5.2031285000000002E-3</v>
       </c>
-      <c r="S89" s="76">
+      <c r="S89" s="75">
         <v>4.7424642000000001E-3</v>
       </c>
-      <c r="T89" s="76">
+      <c r="T89" s="75">
         <v>4.3432195999999999E-3</v>
       </c>
-      <c r="U89" s="76">
+      <c r="U89" s="75">
         <v>3.9385823E-3</v>
       </c>
-      <c r="V89" s="86">
+      <c r="V89" s="89">
         <v>3.1198295999999999E-3</v>
       </c>
-      <c r="W89" s="92">
+      <c r="W89" s="128">
         <v>5.689525E-3</v>
       </c>
-      <c r="X89" s="90">
+      <c r="X89" s="128">
         <v>1.4837839999999999E-3</v>
       </c>
-      <c r="Y89" s="87">
+      <c r="Y89" s="130">
         <f t="shared" si="11"/>
         <v>7.4159441176470582E-4</v>
       </c>
@@ -10888,76 +10925,76 @@
         <f t="shared" si="12"/>
         <v>-2.4739652941176469E-4</v>
       </c>
-      <c r="AA89" s="75">
-        <v>0</v>
-      </c>
-      <c r="AB89" s="76">
+      <c r="AA89" s="74">
+        <v>0</v>
+      </c>
+      <c r="AB89" s="75">
         <v>0.13551692000000001</v>
       </c>
-      <c r="AC89" s="76">
+      <c r="AC89" s="75">
         <v>0.12141488</v>
       </c>
-      <c r="AD89" s="76">
+      <c r="AD89" s="75">
         <v>0.11195296</v>
       </c>
-      <c r="AE89" s="76">
+      <c r="AE89" s="75">
         <v>0.10196945</v>
       </c>
-      <c r="AF89" s="76">
+      <c r="AF89" s="75">
         <v>8.7215784000000005E-2</v>
       </c>
-      <c r="AG89" s="76">
+      <c r="AG89" s="75">
         <v>6.8780059000000004E-2</v>
       </c>
-      <c r="AH89" s="76">
+      <c r="AH89" s="75">
         <v>5.3315596E-2</v>
       </c>
-      <c r="AI89" s="76">
+      <c r="AI89" s="75">
         <v>4.2747080999999999E-2</v>
       </c>
-      <c r="AW89" s="94" t="s">
+      <c r="AW89" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="AX89" s="76">
+      <c r="AX89" s="140">
         <v>9.3605019000000001E-3</v>
       </c>
-      <c r="AY89" s="98">
+      <c r="AY89" s="141">
         <v>4.3315932999999996E-3</v>
       </c>
-      <c r="AZ89" s="96">
+      <c r="AZ89" s="136">
         <v>7.9141460000000004E-3</v>
       </c>
-      <c r="BA89" s="96">
+      <c r="BA89" s="137">
         <v>3.7748500000000002E-3</v>
       </c>
-      <c r="BB89" s="97">
+      <c r="BB89" s="138">
         <f t="shared" si="13"/>
         <v>3.0443860000000001E-3</v>
       </c>
-      <c r="BC89">
+      <c r="BC89" s="139">
         <f t="shared" si="14"/>
         <v>-2.4348800000000004E-4</v>
       </c>
-      <c r="BD89" s="94" t="s">
+      <c r="BD89" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="BE89" s="76">
+      <c r="BE89" s="148">
         <v>6.4621250999999996E-3</v>
       </c>
-      <c r="BF89" s="98">
+      <c r="BF89" s="149">
         <v>3.1198295999999999E-3</v>
       </c>
-      <c r="BG89" s="96">
+      <c r="BG89" s="144">
         <v>8.7300439999999993E-3</v>
       </c>
-      <c r="BH89" s="96">
+      <c r="BH89" s="145">
         <v>2.8349930000000001E-3</v>
       </c>
-      <c r="BI89" s="97">
+      <c r="BI89" s="146">
         <f t="shared" si="15"/>
         <v>1.7946898823529415E-3</v>
       </c>
-      <c r="BJ89">
+      <c r="BJ89" s="147">
         <f t="shared" si="16"/>
         <v>-3.4676770588235289E-4</v>
       </c>
@@ -10966,37 +11003,37 @@
       <c r="A90" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="B90" s="80">
+      <c r="B90" s="75">
         <v>1.0468597E-2</v>
       </c>
-      <c r="C90" s="76">
+      <c r="C90" s="75">
         <v>9.6974886E-3</v>
       </c>
-      <c r="D90" s="76">
+      <c r="D90" s="75">
         <v>9.0068661000000001E-3</v>
       </c>
-      <c r="E90" s="76">
+      <c r="E90" s="75">
         <v>8.2366352999999996E-3</v>
       </c>
-      <c r="F90" s="76">
+      <c r="F90" s="75">
         <v>7.4406786000000003E-3</v>
       </c>
-      <c r="G90" s="76">
+      <c r="G90" s="75">
         <v>6.7541959E-3</v>
       </c>
-      <c r="H90" s="76">
+      <c r="H90" s="75">
         <v>6.0814568000000001E-3</v>
       </c>
-      <c r="I90" s="86">
+      <c r="I90" s="89">
         <v>5.1669517000000002E-3</v>
       </c>
-      <c r="J90" s="92">
+      <c r="J90" s="128">
         <v>8.5842190000000006E-3</v>
       </c>
-      <c r="K90" s="90">
+      <c r="K90" s="85">
         <v>3.4039669999999999E-3</v>
       </c>
-      <c r="L90" s="87">
+      <c r="L90" s="130">
         <f t="shared" si="9"/>
         <v>2.4898048823529411E-3</v>
       </c>
@@ -11004,40 +11041,40 @@
         <f t="shared" si="10"/>
         <v>-3.0472070588235297E-4</v>
       </c>
-      <c r="N90" s="83" t="s">
+      <c r="N90" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="O90" s="80">
+      <c r="O90" s="75">
         <v>7.3166155E-3</v>
       </c>
-      <c r="P90" s="76">
+      <c r="P90" s="75">
         <v>6.9341934000000001E-3</v>
       </c>
-      <c r="Q90" s="76">
+      <c r="Q90" s="75">
         <v>6.5407853E-3</v>
       </c>
-      <c r="R90" s="76">
+      <c r="R90" s="75">
         <v>6.0806221000000004E-3</v>
       </c>
-      <c r="S90" s="76">
+      <c r="S90" s="75">
         <v>5.6114275000000002E-3</v>
       </c>
-      <c r="T90" s="76">
+      <c r="T90" s="75">
         <v>5.226807E-3</v>
       </c>
-      <c r="U90" s="76">
+      <c r="U90" s="75">
         <v>4.7939851999999998E-3</v>
       </c>
-      <c r="V90" s="86">
+      <c r="V90" s="89">
         <v>3.7817176000000002E-3</v>
       </c>
-      <c r="W90" s="92">
+      <c r="W90" s="128">
         <v>6.367841E-3</v>
       </c>
-      <c r="X90" s="90">
+      <c r="X90" s="128">
         <v>1.8290649999999999E-3</v>
       </c>
-      <c r="Y90" s="87">
+      <c r="Y90" s="130">
         <f t="shared" si="11"/>
         <v>1.0281045294117646E-3</v>
       </c>
@@ -11045,115 +11082,115 @@
         <f t="shared" si="12"/>
         <v>-2.6698682352941175E-4</v>
       </c>
-      <c r="AA90" s="78" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB90" s="76">
+      <c r="AA90" s="77" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB90" s="75">
         <v>2.7320634999999999E-2</v>
       </c>
-      <c r="AC90" s="76">
+      <c r="AC90" s="75">
         <v>2.2139934E-2</v>
       </c>
-      <c r="AD90" s="76">
+      <c r="AD90" s="75">
         <v>1.9089755999999999E-2</v>
       </c>
-      <c r="AE90" s="76">
+      <c r="AE90" s="75">
         <v>1.6181286E-2</v>
       </c>
-      <c r="AF90" s="76">
+      <c r="AF90" s="75">
         <v>1.2619490000000001E-2</v>
       </c>
-      <c r="AG90" s="76">
+      <c r="AG90" s="75">
         <v>8.9390100000000007E-3</v>
       </c>
-      <c r="AH90" s="76">
+      <c r="AH90" s="75">
         <v>6.3509125E-3</v>
       </c>
-      <c r="AI90" s="76">
+      <c r="AI90" s="75">
         <v>4.6946237E-3</v>
       </c>
-      <c r="AW90" s="94" t="s">
+      <c r="AW90" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="AX90" s="76">
+      <c r="AX90" s="140">
         <v>1.0468597E-2</v>
       </c>
-      <c r="AY90" s="98">
+      <c r="AY90" s="141">
         <v>5.1669517000000002E-3</v>
       </c>
-      <c r="AZ90" s="96">
+      <c r="AZ90" s="136">
         <v>1.0961822E-2</v>
       </c>
-      <c r="BA90" s="96">
+      <c r="BA90" s="137">
         <v>5.0321869999999996E-3</v>
       </c>
-      <c r="BB90" s="97">
+      <c r="BB90" s="138">
         <f t="shared" si="13"/>
         <v>3.9857808235294109E-3</v>
       </c>
-      <c r="BC90">
+      <c r="BC90" s="139">
         <f t="shared" si="14"/>
         <v>-3.4880205882352943E-4</v>
       </c>
-      <c r="BD90" s="94" t="s">
+      <c r="BD90" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="BE90" s="76">
+      <c r="BE90" s="148">
         <v>7.3166155E-3</v>
       </c>
-      <c r="BF90" s="98">
+      <c r="BF90" s="149">
         <v>3.7817176000000002E-3</v>
       </c>
-      <c r="BG90" s="96">
+      <c r="BG90" s="144">
         <v>9.3410109999999998E-3</v>
       </c>
-      <c r="BH90" s="96">
+      <c r="BH90" s="145">
         <v>3.592764E-3</v>
       </c>
-      <c r="BI90" s="97">
+      <c r="BI90" s="146">
         <f t="shared" si="15"/>
         <v>2.5783674705882353E-3</v>
       </c>
-      <c r="BJ90">
+      <c r="BJ90" s="147">
         <f t="shared" si="16"/>
         <v>-3.3813217647058825E-4</v>
       </c>
     </row>
     <row r="91" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="83" t="s">
+      <c r="A91" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="B91" s="80">
+      <c r="B91" s="75">
         <v>1.2171936E-2</v>
       </c>
-      <c r="C91" s="76">
+      <c r="C91" s="75">
         <v>1.1441359E-2</v>
       </c>
-      <c r="D91" s="76">
+      <c r="D91" s="75">
         <v>1.0708901999999999E-2</v>
       </c>
-      <c r="E91" s="76">
+      <c r="E91" s="75">
         <v>9.8627973999999997E-3</v>
       </c>
-      <c r="F91" s="76">
+      <c r="F91" s="75">
         <v>9.0128794999999994E-3</v>
       </c>
-      <c r="G91" s="76">
+      <c r="G91" s="75">
         <v>8.3055105000000001E-3</v>
       </c>
-      <c r="H91" s="76">
+      <c r="H91" s="75">
         <v>7.5515045999999999E-3</v>
       </c>
-      <c r="I91" s="86">
+      <c r="I91" s="89">
         <v>6.4414638999999996E-3</v>
       </c>
-      <c r="J91" s="92">
+      <c r="J91" s="128">
         <v>1.0363597E-2</v>
       </c>
-      <c r="K91" s="90">
+      <c r="K91" s="85">
         <v>3.9863540000000001E-3</v>
       </c>
-      <c r="L91" s="87">
+      <c r="L91" s="130">
         <f t="shared" si="9"/>
         <v>2.8609581764705884E-3</v>
       </c>
@@ -11161,40 +11198,40 @@
         <f t="shared" si="10"/>
         <v>-3.7513194117647059E-4</v>
       </c>
-      <c r="N91" s="83" t="s">
+      <c r="N91" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="O91" s="80">
+      <c r="O91" s="75">
         <v>8.3061538000000004E-3</v>
       </c>
-      <c r="P91" s="76">
+      <c r="P91" s="75">
         <v>7.9964224999999993E-3</v>
       </c>
-      <c r="Q91" s="76">
+      <c r="Q91" s="75">
         <v>7.6115829000000003E-3</v>
       </c>
-      <c r="R91" s="76">
+      <c r="R91" s="75">
         <v>7.1389935000000003E-3</v>
       </c>
-      <c r="S91" s="76">
+      <c r="S91" s="75">
         <v>6.6758900000000003E-3</v>
       </c>
-      <c r="T91" s="76">
+      <c r="T91" s="75">
         <v>6.3230613000000001E-3</v>
       </c>
-      <c r="U91" s="76">
+      <c r="U91" s="75">
         <v>5.8713664000000004E-3</v>
       </c>
-      <c r="V91" s="86">
+      <c r="V91" s="89">
         <v>4.6448573999999998E-3</v>
       </c>
-      <c r="W91" s="92">
+      <c r="W91" s="128">
         <v>6.1407370000000003E-3</v>
       </c>
-      <c r="X91" s="90">
+      <c r="X91" s="128">
         <v>1.8174109999999999E-3</v>
       </c>
-      <c r="Y91" s="87">
+      <c r="Y91" s="130">
         <f t="shared" si="11"/>
         <v>1.0544711176470585E-3</v>
       </c>
@@ -11202,88 +11239,88 @@
         <f t="shared" si="12"/>
         <v>-2.5431329411764711E-4</v>
       </c>
-      <c r="AW91" s="94" t="s">
+      <c r="AW91" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="AX91" s="76">
+      <c r="AX91" s="140">
         <v>1.2171936E-2</v>
       </c>
-      <c r="AY91" s="98">
+      <c r="AY91" s="141">
         <v>6.4414638999999996E-3</v>
       </c>
-      <c r="AZ91" s="96">
+      <c r="AZ91" s="136">
         <v>1.3134368E-2</v>
       </c>
-      <c r="BA91" s="96">
+      <c r="BA91" s="137">
         <v>6.1751790000000003E-3</v>
       </c>
-      <c r="BB91" s="97">
+      <c r="BB91" s="138">
         <f t="shared" si="13"/>
         <v>4.947086823529412E-3</v>
       </c>
-      <c r="BC91">
+      <c r="BC91" s="139">
         <f t="shared" si="14"/>
         <v>-4.0936405882352944E-4</v>
       </c>
-      <c r="BD91" s="94" t="s">
+      <c r="BD91" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="BE91" s="76">
+      <c r="BE91" s="148">
         <v>8.3061538000000004E-3</v>
       </c>
-      <c r="BF91" s="98">
+      <c r="BF91" s="149">
         <v>4.6448573999999998E-3</v>
       </c>
-      <c r="BG91" s="96">
+      <c r="BG91" s="144">
         <v>9.4525909999999998E-3</v>
       </c>
-      <c r="BH91" s="96">
+      <c r="BH91" s="145">
         <v>3.9322710000000002E-3</v>
       </c>
-      <c r="BI91" s="97">
+      <c r="BI91" s="146">
         <f t="shared" si="15"/>
         <v>2.9580968823529415E-3</v>
       </c>
-      <c r="BJ91">
+      <c r="BJ91" s="147">
         <f t="shared" si="16"/>
         <v>-3.2472470588235293E-4</v>
       </c>
     </row>
     <row r="92" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="83" t="s">
+      <c r="A92" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="B92" s="80">
+      <c r="B92" s="75">
         <v>1.4352014999999999E-2</v>
       </c>
-      <c r="C92" s="76">
+      <c r="C92" s="75">
         <v>1.3609002E-2</v>
       </c>
-      <c r="D92" s="76">
+      <c r="D92" s="75">
         <v>1.2821048999999999E-2</v>
       </c>
-      <c r="E92" s="76">
+      <c r="E92" s="75">
         <v>1.189198E-2</v>
       </c>
-      <c r="F92" s="76">
+      <c r="F92" s="75">
         <v>1.0964043E-2</v>
       </c>
-      <c r="G92" s="76">
+      <c r="G92" s="75">
         <v>1.0199443000000001E-2</v>
       </c>
-      <c r="H92" s="76">
+      <c r="H92" s="75">
         <v>9.3492987999999992E-3</v>
       </c>
-      <c r="I92" s="86">
+      <c r="I92" s="89">
         <v>8.0432449999999992E-3</v>
       </c>
-      <c r="J92" s="92">
+      <c r="J92" s="128">
         <v>1.1498424E-2</v>
       </c>
-      <c r="K92" s="90">
+      <c r="K92" s="85">
         <v>4.6618329999999998E-3</v>
       </c>
-      <c r="L92" s="87">
+      <c r="L92" s="130">
         <f t="shared" si="9"/>
         <v>3.4553757647058821E-3</v>
       </c>
@@ -11291,40 +11328,40 @@
         <f t="shared" si="10"/>
         <v>-4.021524117647059E-4</v>
       </c>
-      <c r="N92" s="83" t="s">
+      <c r="N92" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="O92" s="80">
+      <c r="O92" s="75">
         <v>9.5504723999999992E-3</v>
       </c>
-      <c r="P92" s="76">
+      <c r="P92" s="75">
         <v>9.2426670999999992E-3</v>
       </c>
-      <c r="Q92" s="76">
+      <c r="Q92" s="75">
         <v>8.8507475000000006E-3</v>
       </c>
-      <c r="R92" s="76">
+      <c r="R92" s="75">
         <v>8.3638766999999999E-3</v>
       </c>
-      <c r="S92" s="76">
+      <c r="S92" s="75">
         <v>7.8806432000000006E-3</v>
       </c>
-      <c r="T92" s="76">
+      <c r="T92" s="75">
         <v>7.5079448999999998E-3</v>
       </c>
-      <c r="U92" s="76">
+      <c r="U92" s="75">
         <v>7.0247197000000003E-3</v>
       </c>
-      <c r="V92" s="86">
+      <c r="V92" s="89">
         <v>5.6773359000000002E-3</v>
       </c>
-      <c r="W92" s="92">
+      <c r="W92" s="128">
         <v>5.9637040000000002E-3</v>
       </c>
-      <c r="X92" s="90">
+      <c r="X92" s="128">
         <v>2.1249369999999999E-3</v>
       </c>
-      <c r="Y92" s="87">
+      <c r="Y92" s="130">
         <f t="shared" si="11"/>
         <v>1.4475075294117646E-3</v>
       </c>
@@ -11332,88 +11369,88 @@
         <f t="shared" si="12"/>
         <v>-2.2580982352941178E-4</v>
       </c>
-      <c r="AW92" s="94" t="s">
+      <c r="AW92" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="AX92" s="76">
+      <c r="AX92" s="140">
         <v>1.4352014999999999E-2</v>
       </c>
-      <c r="AY92" s="98">
+      <c r="AY92" s="141">
         <v>8.0432449999999992E-3</v>
       </c>
-      <c r="AZ92" s="96">
+      <c r="AZ92" s="136">
         <v>1.406663E-2</v>
       </c>
-      <c r="BA92" s="96">
+      <c r="BA92" s="137">
         <v>6.7918839999999998E-3</v>
       </c>
-      <c r="BB92" s="97">
+      <c r="BB92" s="138">
         <f t="shared" si="13"/>
         <v>5.508105294117647E-3</v>
       </c>
-      <c r="BC92">
+      <c r="BC92" s="139">
         <f t="shared" si="14"/>
         <v>-4.2792623529411765E-4</v>
       </c>
-      <c r="BD92" s="94" t="s">
+      <c r="BD92" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="BE92" s="76">
+      <c r="BE92" s="148">
         <v>9.5504723999999992E-3</v>
       </c>
-      <c r="BF92" s="98">
+      <c r="BF92" s="149">
         <v>5.6773359000000002E-3</v>
       </c>
-      <c r="BG92" s="96">
+      <c r="BG92" s="144">
         <v>8.6438820000000003E-3</v>
       </c>
-      <c r="BH92" s="96">
+      <c r="BH92" s="145">
         <v>4.1437549999999998E-3</v>
       </c>
-      <c r="BI92" s="97">
+      <c r="BI92" s="146">
         <f t="shared" si="15"/>
         <v>3.3496149411764704E-3</v>
       </c>
-      <c r="BJ92">
+      <c r="BJ92" s="147">
         <f t="shared" si="16"/>
         <v>-2.6471335294117647E-4</v>
       </c>
     </row>
     <row r="93" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="83" t="s">
+      <c r="A93" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B93" s="80">
+      <c r="B93" s="75">
         <v>1.6599328999999999E-2</v>
       </c>
-      <c r="C93" s="76">
+      <c r="C93" s="75">
         <v>1.5939089E-2</v>
       </c>
-      <c r="D93" s="76">
+      <c r="D93" s="75">
         <v>1.5164165E-2</v>
       </c>
-      <c r="E93" s="76">
+      <c r="E93" s="75">
         <v>1.4218463000000001E-2</v>
       </c>
-      <c r="F93" s="76">
+      <c r="F93" s="75">
         <v>1.3283338E-2</v>
       </c>
-      <c r="G93" s="76">
+      <c r="G93" s="75">
         <v>1.2527323E-2</v>
       </c>
-      <c r="H93" s="76">
+      <c r="H93" s="75">
         <v>1.1624491000000001E-2</v>
       </c>
-      <c r="I93" s="86">
+      <c r="I93" s="89">
         <v>1.0135829000000001E-2</v>
       </c>
-      <c r="J93" s="92">
+      <c r="J93" s="128">
         <v>1.4937591E-2</v>
       </c>
-      <c r="K93" s="90">
+      <c r="K93" s="85">
         <v>6.616434E-3</v>
       </c>
-      <c r="L93" s="87">
+      <c r="L93" s="130">
         <f t="shared" si="9"/>
         <v>5.1479945294117648E-3</v>
       </c>
@@ -11421,40 +11458,40 @@
         <f t="shared" si="10"/>
         <v>-4.8947982352941168E-4</v>
       </c>
-      <c r="N93" s="83" t="s">
+      <c r="N93" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="O93" s="80">
+      <c r="O93" s="75">
         <v>1.0526821E-2</v>
       </c>
-      <c r="P93" s="76">
+      <c r="P93" s="75">
         <v>1.0266169E-2</v>
       </c>
-      <c r="Q93" s="76">
+      <c r="Q93" s="75">
         <v>9.8958287999999991E-3</v>
       </c>
-      <c r="R93" s="76">
+      <c r="R93" s="75">
         <v>9.4230961000000002E-3</v>
       </c>
-      <c r="S93" s="76">
+      <c r="S93" s="75">
         <v>8.9566785000000006E-3</v>
       </c>
-      <c r="T93" s="76">
+      <c r="T93" s="75">
         <v>8.6049192E-3</v>
       </c>
-      <c r="U93" s="76">
+      <c r="U93" s="75">
         <v>8.1201847999999993E-3</v>
       </c>
-      <c r="V93" s="86">
+      <c r="V93" s="89">
         <v>6.6691631000000001E-3</v>
       </c>
-      <c r="W93" s="92">
+      <c r="W93" s="128">
         <v>6.78533E-3</v>
       </c>
-      <c r="X93" s="90">
+      <c r="X93" s="128">
         <v>3.1711669999999999E-3</v>
       </c>
-      <c r="Y93" s="87">
+      <c r="Y93" s="130">
         <f t="shared" si="11"/>
         <v>2.5333735294117646E-3</v>
       </c>
@@ -11462,88 +11499,88 @@
         <f t="shared" si="12"/>
         <v>-2.1259782352941176E-4</v>
       </c>
-      <c r="AW93" s="94" t="s">
+      <c r="AW93" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="AX93" s="76">
+      <c r="AX93" s="140">
         <v>1.6599328999999999E-2</v>
       </c>
-      <c r="AY93" s="98">
+      <c r="AY93" s="141">
         <v>1.0135829000000001E-2</v>
       </c>
-      <c r="AZ93" s="96">
+      <c r="AZ93" s="136">
         <v>1.7153776999999999E-2</v>
       </c>
-      <c r="BA93" s="96">
+      <c r="BA93" s="137">
         <v>8.8646409999999995E-3</v>
       </c>
-      <c r="BB93" s="97">
+      <c r="BB93" s="138">
         <f t="shared" si="13"/>
         <v>7.4018522941176465E-3</v>
       </c>
-      <c r="BC93">
+      <c r="BC93" s="139">
         <f t="shared" si="14"/>
         <v>-4.875962352941176E-4</v>
       </c>
-      <c r="BD93" s="94" t="s">
+      <c r="BD93" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="BE93" s="76">
+      <c r="BE93" s="148">
         <v>1.0526821E-2</v>
       </c>
-      <c r="BF93" s="98">
+      <c r="BF93" s="149">
         <v>6.6691631000000001E-3</v>
       </c>
-      <c r="BG93" s="96">
+      <c r="BG93" s="144">
         <v>9.377191E-3</v>
       </c>
-      <c r="BH93" s="96">
+      <c r="BH93" s="145">
         <v>5.2104229999999996E-3</v>
       </c>
-      <c r="BI93" s="97">
+      <c r="BI93" s="146">
         <f t="shared" si="15"/>
         <v>4.4751109999999995E-3</v>
       </c>
-      <c r="BJ93">
+      <c r="BJ93" s="147">
         <f t="shared" si="16"/>
         <v>-2.45104E-4</v>
       </c>
     </row>
     <row r="94" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="83" t="s">
+      <c r="A94" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="B94" s="80">
+      <c r="B94" s="75">
         <v>2.0610447E-2</v>
       </c>
-      <c r="C94" s="76">
+      <c r="C94" s="75">
         <v>2.0069169000000001E-2</v>
       </c>
-      <c r="D94" s="76">
+      <c r="D94" s="75">
         <v>1.9329669000000001E-2</v>
       </c>
-      <c r="E94" s="76">
+      <c r="E94" s="75">
         <v>1.8382102000000001E-2</v>
       </c>
-      <c r="F94" s="76">
+      <c r="F94" s="75">
         <v>1.7452718999999998E-2</v>
       </c>
-      <c r="G94" s="76">
+      <c r="G94" s="75">
         <v>1.6717211999999999E-2</v>
       </c>
-      <c r="H94" s="76">
+      <c r="H94" s="75">
         <v>1.5751589999999999E-2</v>
       </c>
-      <c r="I94" s="86">
+      <c r="I94" s="89">
         <v>1.4004198000000001E-2</v>
       </c>
-      <c r="J94" s="92">
+      <c r="J94" s="128">
         <v>2.0927292E-2</v>
       </c>
-      <c r="K94" s="90">
+      <c r="K94" s="85">
         <v>1.0831970999999999E-2</v>
       </c>
-      <c r="L94" s="87">
+      <c r="L94" s="130">
         <f t="shared" si="9"/>
         <v>9.050443764705882E-3</v>
       </c>
@@ -11551,40 +11588,40 @@
         <f t="shared" si="10"/>
         <v>-5.9384241176470591E-4</v>
       </c>
-      <c r="N94" s="83" t="s">
+      <c r="N94" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="O94" s="80">
+      <c r="O94" s="75">
         <v>1.3618289E-2</v>
       </c>
-      <c r="P94" s="76">
+      <c r="P94" s="75">
         <v>1.3279867000000001E-2</v>
       </c>
-      <c r="Q94" s="76">
+      <c r="Q94" s="75">
         <v>1.2843602000000001E-2</v>
       </c>
-      <c r="R94" s="76">
+      <c r="R94" s="75">
         <v>1.2293521999999999E-2</v>
       </c>
-      <c r="S94" s="76">
+      <c r="S94" s="75">
         <v>1.1726159999999999E-2</v>
       </c>
-      <c r="T94" s="76">
+      <c r="T94" s="75">
         <v>1.126797E-2</v>
       </c>
-      <c r="U94" s="76">
+      <c r="U94" s="75">
         <v>1.0674833E-2</v>
       </c>
-      <c r="V94" s="86">
+      <c r="V94" s="89">
         <v>8.9763412999999993E-3</v>
       </c>
-      <c r="W94" s="92">
+      <c r="W94" s="128">
         <v>9.8414439999999995E-3</v>
       </c>
-      <c r="X94" s="90">
+      <c r="X94" s="128">
         <v>5.1947219999999997E-3</v>
       </c>
-      <c r="Y94" s="87">
+      <c r="Y94" s="130">
         <f t="shared" si="11"/>
         <v>4.3747122352941169E-3</v>
       </c>
@@ -11592,88 +11629,88 @@
         <f t="shared" si="12"/>
         <v>-2.7333658823529413E-4</v>
       </c>
-      <c r="AW94" s="94" t="s">
+      <c r="AW94" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="AX94" s="76">
+      <c r="AX94" s="140">
         <v>2.0610447E-2</v>
       </c>
-      <c r="AY94" s="98">
+      <c r="AY94" s="141">
         <v>1.4004198000000001E-2</v>
       </c>
-      <c r="AZ94" s="96">
+      <c r="AZ94" s="136">
         <v>2.2671103000000001E-2</v>
       </c>
-      <c r="BA94" s="96">
+      <c r="BA94" s="137">
         <v>1.2617975999999999E-2</v>
       </c>
-      <c r="BB94" s="97">
+      <c r="BB94" s="138">
         <f t="shared" si="13"/>
         <v>1.0843894764705882E-2</v>
       </c>
-      <c r="BC94">
+      <c r="BC94" s="139">
         <f t="shared" si="14"/>
         <v>-5.9136041176470597E-4</v>
       </c>
-      <c r="BD94" s="94" t="s">
+      <c r="BD94" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="BE94" s="76">
+      <c r="BE94" s="148">
         <v>1.3618289E-2</v>
       </c>
-      <c r="BF94" s="98">
+      <c r="BF94" s="149">
         <v>8.9763412999999993E-3</v>
       </c>
-      <c r="BG94" s="96">
+      <c r="BG94" s="144">
         <v>1.1992486E-2</v>
       </c>
-      <c r="BH94" s="96">
+      <c r="BH94" s="145">
         <v>6.8538840000000002E-3</v>
       </c>
-      <c r="BI94" s="97">
+      <c r="BI94" s="146">
         <f t="shared" si="15"/>
         <v>5.9470718823529415E-3</v>
       </c>
-      <c r="BJ94">
+      <c r="BJ94" s="147">
         <f t="shared" si="16"/>
         <v>-3.0227070588235294E-4</v>
       </c>
     </row>
     <row r="95" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="83" t="s">
+      <c r="A95" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="B95" s="80">
+      <c r="B95" s="75">
         <v>2.5459668000000001E-2</v>
       </c>
-      <c r="C95" s="76">
+      <c r="C95" s="75">
         <v>2.5029438000000001E-2</v>
       </c>
-      <c r="D95" s="76">
+      <c r="D95" s="75">
         <v>2.4304803E-2</v>
       </c>
-      <c r="E95" s="76">
+      <c r="E95" s="75">
         <v>2.3329169E-2</v>
       </c>
-      <c r="F95" s="76">
+      <c r="F95" s="75">
         <v>2.2389999000000001E-2</v>
       </c>
-      <c r="G95" s="76">
+      <c r="G95" s="75">
         <v>2.1674624999999999E-2</v>
       </c>
-      <c r="H95" s="76">
+      <c r="H95" s="75">
         <v>2.0631349E-2</v>
       </c>
-      <c r="I95" s="86">
+      <c r="I95" s="89">
         <v>1.8576009000000001E-2</v>
       </c>
-      <c r="J95" s="92">
+      <c r="J95" s="128">
         <v>2.6352477999999999E-2</v>
       </c>
-      <c r="K95" s="90">
+      <c r="K95" s="85">
         <v>1.6475909E-2</v>
       </c>
-      <c r="L95" s="87">
+      <c r="L95" s="130">
         <f t="shared" si="9"/>
         <v>1.473298505882353E-2</v>
       </c>
@@ -11681,40 +11718,40 @@
         <f t="shared" si="10"/>
         <v>-5.8097464705882346E-4</v>
       </c>
-      <c r="N95" s="83" t="s">
+      <c r="N95" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="O95" s="80">
+      <c r="O95" s="75">
         <v>1.7990335999999999E-2</v>
       </c>
-      <c r="P95" s="76">
+      <c r="P95" s="75">
         <v>1.7498735000000001E-2</v>
       </c>
-      <c r="Q95" s="76">
+      <c r="Q95" s="75">
         <v>1.6939927E-2</v>
       </c>
-      <c r="R95" s="76">
+      <c r="R95" s="75">
         <v>1.6251709E-2</v>
       </c>
-      <c r="S95" s="76">
+      <c r="S95" s="75">
         <v>1.5508173E-2</v>
       </c>
-      <c r="T95" s="76">
+      <c r="T95" s="75">
         <v>1.4865150000000001E-2</v>
       </c>
-      <c r="U95" s="76">
+      <c r="U95" s="75">
         <v>1.4094534000000001E-2</v>
       </c>
-      <c r="V95" s="86">
+      <c r="V95" s="89">
         <v>1.2049147E-2</v>
       </c>
-      <c r="W95" s="92">
+      <c r="W95" s="128">
         <v>1.3256046E-2</v>
       </c>
-      <c r="X95" s="90">
+      <c r="X95" s="128">
         <v>8.2955149999999998E-3</v>
       </c>
-      <c r="Y95" s="87">
+      <c r="Y95" s="130">
         <f t="shared" si="11"/>
         <v>7.4201271764705885E-3</v>
       </c>
@@ -11722,88 +11759,88 @@
         <f t="shared" si="12"/>
         <v>-2.917959411764706E-4</v>
       </c>
-      <c r="AW95" s="94" t="s">
+      <c r="AW95" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="AX95" s="76">
+      <c r="AX95" s="140">
         <v>2.5459668000000001E-2</v>
       </c>
-      <c r="AY95" s="98">
+      <c r="AY95" s="141">
         <v>1.8576009000000001E-2</v>
       </c>
-      <c r="AZ95" s="96">
+      <c r="AZ95" s="136">
         <v>2.8196888E-2</v>
       </c>
-      <c r="BA95" s="96">
+      <c r="BA95" s="137">
         <v>1.7883441E-2</v>
       </c>
-      <c r="BB95" s="97">
+      <c r="BB95" s="138">
         <f t="shared" si="13"/>
         <v>1.6063420941176472E-2</v>
       </c>
-      <c r="BC95">
+      <c r="BC95" s="139">
         <f t="shared" si="14"/>
         <v>-6.0667335294117646E-4</v>
       </c>
-      <c r="BD95" s="94" t="s">
+      <c r="BD95" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="BE95" s="76">
+      <c r="BE95" s="148">
         <v>1.7990335999999999E-2</v>
       </c>
-      <c r="BF95" s="98">
+      <c r="BF95" s="149">
         <v>1.2049147E-2</v>
       </c>
-      <c r="BG95" s="96">
+      <c r="BG95" s="144">
         <v>1.5297870999999999E-2</v>
       </c>
-      <c r="BH95" s="96">
+      <c r="BH95" s="145">
         <v>9.5655440000000005E-3</v>
       </c>
-      <c r="BI95" s="97">
+      <c r="BI95" s="146">
         <f t="shared" si="15"/>
         <v>8.5539568823529422E-3</v>
       </c>
-      <c r="BJ95">
+      <c r="BJ95" s="147">
         <f t="shared" si="16"/>
         <v>-3.3719570588235288E-4</v>
       </c>
     </row>
     <row r="96" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="79" t="s">
+      <c r="A96" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="B96" s="80">
+      <c r="B96" s="75">
         <v>3.5184202999999997E-2</v>
       </c>
-      <c r="C96" s="76">
+      <c r="C96" s="75">
         <v>3.4928028999999999E-2</v>
       </c>
-      <c r="D96" s="76">
+      <c r="D96" s="75">
         <v>3.4222971999999997E-2</v>
       </c>
-      <c r="E96" s="76">
+      <c r="E96" s="75">
         <v>3.3195026000000002E-2</v>
       </c>
-      <c r="F96" s="76">
+      <c r="F96" s="75">
         <v>3.2233284000000001E-2</v>
       </c>
-      <c r="G96" s="76">
+      <c r="G96" s="75">
         <v>3.1546165000000001E-2</v>
       </c>
-      <c r="H96" s="76">
+      <c r="H96" s="75">
         <v>3.0365044000000001E-2</v>
       </c>
-      <c r="I96" s="86">
+      <c r="I96" s="89">
         <v>2.7759598999999999E-2</v>
       </c>
-      <c r="J96" s="92">
+      <c r="J96" s="128">
         <v>3.6052813000000003E-2</v>
       </c>
-      <c r="K96" s="90">
+      <c r="K96" s="85">
         <v>2.3964659999999999E-2</v>
       </c>
-      <c r="L96" s="87">
+      <c r="L96" s="130">
         <f t="shared" si="9"/>
         <v>2.1831456529411764E-2</v>
       </c>
@@ -11811,40 +11848,40 @@
         <f t="shared" si="10"/>
         <v>-7.11067823529412E-4</v>
       </c>
-      <c r="N96" s="79" t="s">
+      <c r="N96" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="O96" s="80">
+      <c r="O96" s="75">
         <v>2.7034006999999999E-2</v>
       </c>
-      <c r="P96" s="76">
+      <c r="P96" s="75">
         <v>2.6237897E-2</v>
       </c>
-      <c r="Q96" s="76">
+      <c r="Q96" s="75">
         <v>2.544223E-2</v>
       </c>
-      <c r="R96" s="76">
+      <c r="R96" s="75">
         <v>2.4488769000000001E-2</v>
       </c>
-      <c r="S96" s="76">
+      <c r="S96" s="75">
         <v>2.3397757000000002E-2</v>
       </c>
-      <c r="T96" s="76">
+      <c r="T96" s="75">
         <v>2.2381365E-2</v>
       </c>
-      <c r="U96" s="76">
+      <c r="U96" s="75">
         <v>2.1257570999999999E-2</v>
       </c>
-      <c r="V96" s="86">
+      <c r="V96" s="89">
         <v>1.8543285E-2</v>
       </c>
-      <c r="W96" s="92">
+      <c r="W96" s="128">
         <v>1.9917550999999999E-2</v>
       </c>
-      <c r="X96" s="90">
+      <c r="X96" s="128">
         <v>1.2142778999999999E-2</v>
       </c>
-      <c r="Y96" s="87">
+      <c r="Y96" s="130">
         <f t="shared" si="11"/>
         <v>1.0770760411764705E-2</v>
       </c>
@@ -11852,88 +11889,88 @@
         <f t="shared" si="12"/>
         <v>-4.5733952941176466E-4</v>
       </c>
-      <c r="AW96" s="79" t="s">
+      <c r="AW96" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="AX96" s="76">
+      <c r="AX96" s="140">
         <v>3.5184202999999997E-2</v>
       </c>
-      <c r="AY96" s="98">
+      <c r="AY96" s="141">
         <v>2.7759598999999999E-2</v>
       </c>
-      <c r="AZ96" s="96">
+      <c r="AZ96" s="136">
         <v>3.7754171000000003E-2</v>
       </c>
-      <c r="BA96" s="96">
+      <c r="BA96" s="137">
         <v>2.5185233000000001E-2</v>
       </c>
-      <c r="BB96" s="97">
+      <c r="BB96" s="138">
         <f t="shared" si="13"/>
         <v>2.296718511764706E-2</v>
       </c>
-      <c r="BC96">
+      <c r="BC96" s="139">
         <f t="shared" si="14"/>
         <v>-7.3934929411764716E-4</v>
       </c>
-      <c r="BD96" s="79" t="s">
+      <c r="BD96" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="BE96" s="76">
+      <c r="BE96" s="148">
         <v>2.7034006999999999E-2</v>
       </c>
-      <c r="BF96" s="98">
+      <c r="BF96" s="149">
         <v>1.8543285E-2</v>
       </c>
-      <c r="BG96" s="96">
+      <c r="BG96" s="144">
         <v>2.1810474999999999E-2</v>
       </c>
-      <c r="BH96" s="96">
+      <c r="BH96" s="145">
         <v>1.3232337E-2</v>
       </c>
-      <c r="BI96" s="97">
+      <c r="BI96" s="146">
         <f t="shared" si="15"/>
         <v>1.1718547941176471E-2</v>
       </c>
-      <c r="BJ96">
+      <c r="BJ96" s="147">
         <f t="shared" si="16"/>
         <v>-5.0459635294117645E-4</v>
       </c>
     </row>
     <row r="97" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="79" t="s">
+      <c r="A97" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="B97" s="80">
+      <c r="B97" s="75">
         <v>5.0578709999999999E-2</v>
       </c>
-      <c r="C97" s="76">
+      <c r="C97" s="75">
         <v>5.0650142000000002E-2</v>
       </c>
-      <c r="D97" s="76">
+      <c r="D97" s="75">
         <v>5.0024763E-2</v>
       </c>
-      <c r="E97" s="76">
+      <c r="E97" s="75">
         <v>4.8973602999999997E-2</v>
       </c>
-      <c r="F97" s="76">
+      <c r="F97" s="75">
         <v>4.8051199000000003E-2</v>
       </c>
-      <c r="G97" s="76">
+      <c r="G97" s="75">
         <v>4.7488384000000002E-2</v>
       </c>
-      <c r="H97" s="76">
+      <c r="H97" s="75">
         <v>4.6165507000000001E-2</v>
       </c>
-      <c r="I97" s="86">
+      <c r="I97" s="89">
         <v>4.2779603999999999E-2</v>
       </c>
-      <c r="J97" s="92">
+      <c r="J97" s="128">
         <v>4.4857968999999998E-2</v>
       </c>
-      <c r="K97" s="90">
+      <c r="K97" s="85">
         <v>3.3032178000000002E-2</v>
       </c>
-      <c r="L97" s="87">
+      <c r="L97" s="130">
         <f t="shared" si="9"/>
         <v>3.0945273705882355E-2</v>
       </c>
@@ -11941,40 +11978,40 @@
         <f t="shared" si="10"/>
         <v>-6.9563476470588205E-4</v>
       </c>
-      <c r="N97" s="79" t="s">
+      <c r="N97" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="O97" s="80">
+      <c r="O97" s="75">
         <v>4.1980367999999997E-2</v>
       </c>
-      <c r="P97" s="76">
+      <c r="P97" s="75">
         <v>4.0908139000000003E-2</v>
       </c>
-      <c r="Q97" s="76">
+      <c r="Q97" s="75">
         <v>3.9873039999999998E-2</v>
       </c>
-      <c r="R97" s="76">
+      <c r="R97" s="75">
         <v>3.8634623999999999E-2</v>
       </c>
-      <c r="S97" s="76">
+      <c r="S97" s="75">
         <v>3.7150282999999999E-2</v>
       </c>
-      <c r="T97" s="76">
+      <c r="T97" s="75">
         <v>3.5698045999999997E-2</v>
       </c>
-      <c r="U97" s="76">
+      <c r="U97" s="75">
         <v>3.4126276999999997E-2</v>
       </c>
-      <c r="V97" s="86">
+      <c r="V97" s="89">
         <v>3.039122E-2</v>
       </c>
-      <c r="W97" s="92">
+      <c r="W97" s="128">
         <v>2.8481023000000001E-2</v>
       </c>
-      <c r="X97" s="90">
+      <c r="X97" s="128">
         <v>1.7584465000000001E-2</v>
       </c>
-      <c r="Y97" s="87">
+      <c r="Y97" s="130">
         <f t="shared" si="11"/>
         <v>1.5661543E-2</v>
       </c>
@@ -11982,88 +12019,88 @@
         <f t="shared" si="12"/>
         <v>-6.4097399999999999E-4</v>
       </c>
-      <c r="AW97" s="79" t="s">
+      <c r="AW97" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="AX97" s="76">
+      <c r="AX97" s="140">
         <v>5.0578709999999999E-2</v>
       </c>
-      <c r="AY97" s="98">
+      <c r="AY97" s="141">
         <v>4.2779603999999999E-2</v>
       </c>
-      <c r="AZ97" s="96">
+      <c r="AZ97" s="136">
         <v>4.6622128999999998E-2</v>
       </c>
-      <c r="BA97" s="96">
+      <c r="BA97" s="137">
         <v>3.4253349000000002E-2</v>
       </c>
-      <c r="BB97" s="97">
+      <c r="BB97" s="138">
         <f t="shared" si="13"/>
         <v>3.2070623117647065E-2</v>
       </c>
-      <c r="BC97">
+      <c r="BC97" s="139">
         <f t="shared" si="14"/>
         <v>-7.2757529411764685E-4</v>
       </c>
-      <c r="BD97" s="79" t="s">
+      <c r="BD97" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="BE97" s="76">
+      <c r="BE97" s="148">
         <v>4.1980367999999997E-2</v>
       </c>
-      <c r="BF97" s="98">
+      <c r="BF97" s="149">
         <v>3.039122E-2</v>
       </c>
-      <c r="BG97" s="96">
+      <c r="BG97" s="144">
         <v>3.0280852E-2</v>
       </c>
-      <c r="BH97" s="96">
+      <c r="BH97" s="145">
         <v>1.8559623000000001E-2</v>
       </c>
-      <c r="BI97" s="97">
+      <c r="BI97" s="146">
         <f t="shared" si="15"/>
         <v>1.6491170823529411E-2</v>
       </c>
-      <c r="BJ97">
+      <c r="BJ97" s="147">
         <f t="shared" si="16"/>
         <v>-6.8948405882352935E-4</v>
       </c>
     </row>
     <row r="98" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="79" t="s">
+      <c r="A98" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="B98" s="80">
+      <c r="B98" s="75">
         <v>7.7074561999999999E-2</v>
       </c>
-      <c r="C98" s="76">
+      <c r="C98" s="75">
         <v>7.7622102999999998E-2</v>
       </c>
-      <c r="D98" s="76">
+      <c r="D98" s="75">
         <v>7.7095495999999999E-2</v>
       </c>
-      <c r="E98" s="76">
+      <c r="E98" s="75">
         <v>7.5980821000000004E-2</v>
       </c>
-      <c r="F98" s="76">
+      <c r="F98" s="75">
         <v>7.5089041999999995E-2</v>
       </c>
-      <c r="G98" s="76">
+      <c r="G98" s="75">
         <v>7.4689679999999994E-2</v>
       </c>
-      <c r="H98" s="76">
+      <c r="H98" s="75">
         <v>7.3117043000000007E-2</v>
       </c>
-      <c r="I98" s="86">
+      <c r="I98" s="89">
         <v>6.8473476000000005E-2</v>
       </c>
-      <c r="J98" s="92">
+      <c r="J98" s="128">
         <v>6.6115557000000005E-2</v>
       </c>
-      <c r="K98" s="90">
+      <c r="K98" s="85">
         <v>4.3224483000000001E-2</v>
       </c>
-      <c r="L98" s="87">
+      <c r="L98" s="130">
         <f t="shared" si="9"/>
         <v>3.918488170588235E-2</v>
       </c>
@@ -12071,40 +12108,40 @@
         <f t="shared" si="10"/>
         <v>-1.3465337647058826E-3</v>
       </c>
-      <c r="N98" s="79" t="s">
+      <c r="N98" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="O98" s="80">
+      <c r="O98" s="75">
         <v>6.7413652000000004E-2</v>
       </c>
-      <c r="P98" s="76">
+      <c r="P98" s="75">
         <v>6.6080293999999998E-2</v>
       </c>
-      <c r="Q98" s="76">
+      <c r="Q98" s="75">
         <v>6.4781100999999994E-2</v>
       </c>
-      <c r="R98" s="76">
+      <c r="R98" s="75">
         <v>6.3207541000000006E-2</v>
       </c>
-      <c r="S98" s="76">
+      <c r="S98" s="75">
         <v>6.1234920999999998E-2</v>
       </c>
-      <c r="T98" s="76">
+      <c r="T98" s="75">
         <v>5.9224530999999997E-2</v>
       </c>
-      <c r="U98" s="76">
+      <c r="U98" s="75">
         <v>5.7037298E-2</v>
       </c>
-      <c r="V98" s="86">
+      <c r="V98" s="89">
         <v>5.1704121999999998E-2</v>
       </c>
-      <c r="W98" s="92">
+      <c r="W98" s="128">
         <v>4.3469642000000003E-2</v>
       </c>
-      <c r="X98" s="90">
+      <c r="X98" s="128">
         <v>2.5406643E-2</v>
       </c>
-      <c r="Y98" s="87">
+      <c r="Y98" s="130">
         <f t="shared" si="11"/>
         <v>2.2219054941176469E-2</v>
       </c>
@@ -12112,88 +12149,88 @@
         <f t="shared" si="12"/>
         <v>-1.0625293529411767E-3</v>
       </c>
-      <c r="AW98" s="79" t="s">
+      <c r="AW98" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="AX98" s="76">
+      <c r="AX98" s="140">
         <v>7.7074561999999999E-2</v>
       </c>
-      <c r="AY98" s="98">
+      <c r="AY98" s="141">
         <v>6.8473476000000005E-2</v>
       </c>
-      <c r="AZ98" s="96">
+      <c r="AZ98" s="136">
         <v>6.7988487E-2</v>
       </c>
-      <c r="BA98" s="96">
+      <c r="BA98" s="137">
         <v>4.4629888999999999E-2</v>
       </c>
-      <c r="BB98" s="97">
+      <c r="BB98" s="138">
         <f t="shared" si="13"/>
         <v>4.0507783470588234E-2</v>
       </c>
-      <c r="BC98">
+      <c r="BC98" s="139">
         <f t="shared" si="14"/>
         <v>-1.3740351764705884E-3</v>
       </c>
-      <c r="BD98" s="79" t="s">
+      <c r="BD98" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="BE98" s="76">
+      <c r="BE98" s="148">
         <v>6.7413652000000004E-2</v>
       </c>
-      <c r="BF98" s="98">
+      <c r="BF98" s="149">
         <v>5.1704121999999998E-2</v>
       </c>
-      <c r="BG98" s="96">
+      <c r="BG98" s="144">
         <v>4.5201616E-2</v>
       </c>
-      <c r="BH98" s="96">
+      <c r="BH98" s="145">
         <v>2.6428843E-2</v>
       </c>
-      <c r="BI98" s="97">
+      <c r="BI98" s="146">
         <f t="shared" si="15"/>
         <v>2.3116000705882354E-2</v>
       </c>
-      <c r="BJ98">
+      <c r="BJ98" s="147">
         <f t="shared" si="16"/>
         <v>-1.1042807647058824E-3</v>
       </c>
     </row>
     <row r="99" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="79" t="s">
+      <c r="A99" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="B99" s="80">
+      <c r="B99" s="75">
         <v>0.11904474</v>
       </c>
-      <c r="C99" s="76">
+      <c r="C99" s="75">
         <v>0.12073808</v>
       </c>
-      <c r="D99" s="76">
+      <c r="D99" s="75">
         <v>0.1207081</v>
       </c>
-      <c r="E99" s="76">
+      <c r="E99" s="75">
         <v>0.1198779</v>
       </c>
-      <c r="F99" s="76">
+      <c r="F99" s="75">
         <v>0.11948436</v>
       </c>
-      <c r="G99" s="76">
+      <c r="G99" s="75">
         <v>0.11979376999999999</v>
       </c>
-      <c r="H99" s="76">
+      <c r="H99" s="75">
         <v>0.11823134</v>
       </c>
-      <c r="I99" s="86">
+      <c r="I99" s="89">
         <v>0.11201527999999999</v>
       </c>
-      <c r="J99" s="92">
+      <c r="J99" s="128">
         <v>8.1959559000000001E-2</v>
       </c>
-      <c r="K99" s="90">
+      <c r="K99" s="85">
         <v>5.9431375000000002E-2</v>
       </c>
-      <c r="L99" s="87">
+      <c r="L99" s="130">
         <f t="shared" si="9"/>
         <v>5.5455813117647058E-2</v>
       </c>
@@ -12201,40 +12238,40 @@
         <f t="shared" si="10"/>
         <v>-1.3251872941176471E-3</v>
       </c>
-      <c r="N99" s="79" t="s">
+      <c r="N99" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="O99" s="80">
+      <c r="O99" s="75">
         <v>0.10699243999999999</v>
       </c>
-      <c r="P99" s="76">
+      <c r="P99" s="75">
         <v>0.10582374</v>
       </c>
-      <c r="Q99" s="76">
+      <c r="Q99" s="75">
         <v>0.10450795</v>
       </c>
-      <c r="R99" s="76">
+      <c r="R99" s="75">
         <v>0.10282624999999999</v>
       </c>
-      <c r="S99" s="76">
+      <c r="S99" s="75">
         <v>0.10060334</v>
       </c>
-      <c r="T99" s="76">
+      <c r="T99" s="75">
         <v>9.8256107999999995E-2</v>
       </c>
-      <c r="U99" s="76">
+      <c r="U99" s="75">
         <v>9.5537514000000004E-2</v>
       </c>
-      <c r="V99" s="86">
+      <c r="V99" s="89">
         <v>8.8066895000000006E-2</v>
       </c>
-      <c r="W99" s="92">
+      <c r="W99" s="128">
         <v>5.4374656E-2</v>
       </c>
-      <c r="X99" s="90">
+      <c r="X99" s="128">
         <v>3.7231258000000003E-2</v>
       </c>
-      <c r="Y99" s="87">
+      <c r="Y99" s="130">
         <f t="shared" si="11"/>
         <v>3.420595247058824E-2</v>
       </c>
@@ -12242,52 +12279,57 @@
         <f t="shared" si="12"/>
         <v>-1.0084351764705882E-3</v>
       </c>
-      <c r="AW99" s="79" t="s">
+      <c r="AW99" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="AX99" s="76">
+      <c r="AX99" s="140">
         <v>0.11904474</v>
       </c>
-      <c r="AY99" s="98">
+      <c r="AY99" s="141">
         <v>0.11201527999999999</v>
       </c>
-      <c r="AZ99" s="96">
+      <c r="AZ99" s="136">
         <v>8.3893607999999995E-2</v>
       </c>
-      <c r="BA99" s="96">
+      <c r="BA99" s="137">
         <v>6.0996987000000003E-2</v>
       </c>
-      <c r="BB99" s="97">
+      <c r="BB99" s="138">
         <f t="shared" si="13"/>
         <v>5.6956406823529412E-2</v>
       </c>
-      <c r="BC99">
+      <c r="BC99" s="139">
         <f t="shared" si="14"/>
         <v>-1.346860058823529E-3</v>
       </c>
-      <c r="BD99" s="79" t="s">
+      <c r="BD99" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="BE99" s="76">
+      <c r="BE99" s="148">
         <v>0.10699243999999999</v>
       </c>
-      <c r="BF99" s="98">
+      <c r="BF99" s="149">
         <v>8.8066895000000006E-2</v>
       </c>
-      <c r="BG99" s="96">
+      <c r="BG99" s="144">
         <v>5.5908607999999999E-2</v>
       </c>
-      <c r="BH99" s="96">
+      <c r="BH99" s="145">
         <v>3.8357005999999999E-2</v>
       </c>
-      <c r="BI99" s="97">
+      <c r="BI99" s="146">
         <f t="shared" si="15"/>
         <v>3.5259664470588231E-2</v>
       </c>
-      <c r="BJ99">
+      <c r="BJ99" s="147">
         <f t="shared" si="16"/>
         <v>-1.0324471764705883E-3</v>
       </c>
+    </row>
+    <row r="100" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="I100" s="39"/>
+      <c r="J100" s="39"/>
+      <c r="L100" s="39"/>
     </row>
     <row r="102" spans="1:62" x14ac:dyDescent="0.25">
       <c r="I102" s="49"/>
@@ -12391,7 +12433,7 @@
     </row>
     <row r="108" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B108" s="37"/>
       <c r="C108" s="37"/>
@@ -12419,7 +12461,7 @@
     </row>
     <row r="109" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B109" s="37"/>
       <c r="C109" s="37"/>
@@ -12447,7 +12489,7 @@
     </row>
     <row r="110" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="55" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B110" s="37"/>
       <c r="C110" s="37"/>
@@ -12475,7 +12517,7 @@
     </row>
     <row r="111" spans="1:62" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="121" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B111" s="121"/>
       <c r="C111" s="121"/>
@@ -12502,36 +12544,36 @@
       <c r="X111" s="37"/>
     </row>
     <row r="112" spans="1:62" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="133" t="s">
+      <c r="A112" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="130" t="s">
-        <v>83</v>
-      </c>
-      <c r="C112" s="131"/>
-      <c r="D112" s="131"/>
-      <c r="E112" s="131"/>
-      <c r="F112" s="131"/>
-      <c r="G112" s="132"/>
+      <c r="B112" s="104" t="s">
+        <v>81</v>
+      </c>
+      <c r="C112" s="105"/>
+      <c r="D112" s="105"/>
+      <c r="E112" s="105"/>
+      <c r="F112" s="105"/>
+      <c r="G112" s="106"/>
       <c r="I112" s="68"/>
-      <c r="J112" s="81" t="s">
+      <c r="J112" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="K112" s="81" t="s">
+      <c r="K112" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="L112" s="81" t="s">
+      <c r="L112" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="M112" s="81" t="s">
+      <c r="M112" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="N112" s="81" t="s">
+      <c r="N112" s="79" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="113" spans="1:14" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="134"/>
+      <c r="A113" s="109"/>
       <c r="B113" s="32" t="s">
         <v>68</v>
       </c>
@@ -12550,7 +12592,7 @@
       <c r="G113" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I113" s="82" t="s">
+      <c r="I113" s="80" t="s">
         <v>26</v>
       </c>
       <c r="J113" s="65">
@@ -12575,7 +12617,7 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="135"/>
+      <c r="A114" s="110"/>
       <c r="B114" s="34" t="s">
         <v>61</v>
       </c>
@@ -12623,14 +12665,14 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="I115" s="137" t="s">
-        <v>101</v>
-      </c>
-      <c r="J115" s="137"/>
-      <c r="K115" s="137"/>
-      <c r="L115" s="137"/>
-      <c r="M115" s="137"/>
-      <c r="N115" s="137"/>
+      <c r="I115" s="117" t="s">
+        <v>99</v>
+      </c>
+      <c r="J115" s="117"/>
+      <c r="K115" s="117"/>
+      <c r="L115" s="117"/>
+      <c r="M115" s="117"/>
+      <c r="N115" s="117"/>
     </row>
     <row r="116" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
@@ -13383,31 +13425,31 @@
     </row>
     <row r="132" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="133" spans="1:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="127" t="s">
+      <c r="A133" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="130" t="s">
-        <v>84</v>
-      </c>
-      <c r="C133" s="131"/>
-      <c r="D133" s="131"/>
-      <c r="E133" s="131"/>
-      <c r="F133" s="131"/>
-      <c r="G133" s="132"/>
-      <c r="I133" s="127" t="s">
+      <c r="B133" s="104" t="s">
+        <v>82</v>
+      </c>
+      <c r="C133" s="105"/>
+      <c r="D133" s="105"/>
+      <c r="E133" s="105"/>
+      <c r="F133" s="105"/>
+      <c r="G133" s="106"/>
+      <c r="I133" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="J133" s="130" t="s">
+      <c r="J133" s="104" t="s">
         <v>74</v>
       </c>
-      <c r="K133" s="131"/>
-      <c r="L133" s="131"/>
-      <c r="M133" s="131"/>
-      <c r="N133" s="131"/>
-      <c r="O133" s="132"/>
+      <c r="K133" s="105"/>
+      <c r="L133" s="105"/>
+      <c r="M133" s="105"/>
+      <c r="N133" s="105"/>
+      <c r="O133" s="106"/>
     </row>
     <row r="134" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="128"/>
+      <c r="A134" s="102"/>
       <c r="B134" s="26" t="s">
         <v>69</v>
       </c>
@@ -13426,7 +13468,7 @@
       <c r="G134" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I134" s="128"/>
+      <c r="I134" s="102"/>
       <c r="J134" s="26" t="s">
         <v>69</v>
       </c>
@@ -13447,7 +13489,7 @@
       </c>
     </row>
     <row r="135" spans="1:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="129"/>
+      <c r="A135" s="103"/>
       <c r="B135" s="40" t="s">
         <v>61</v>
       </c>
@@ -13466,7 +13508,7 @@
       <c r="G135" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="I135" s="129"/>
+      <c r="I135" s="103"/>
       <c r="J135" s="40" t="s">
         <v>61</v>
       </c>
@@ -14326,7 +14368,7 @@
     </row>
     <row r="158" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B158" s="37"/>
       <c r="C158" s="37"/>
@@ -14406,22 +14448,22 @@
       <c r="W160" s="37"/>
     </row>
     <row r="161" spans="1:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="112" t="s">
-        <v>88</v>
-      </c>
-      <c r="B161" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="123"/>
-      <c r="D161" s="123"/>
-      <c r="E161" s="123" t="s">
+      <c r="A161" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="B161" s="122" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="122"/>
+      <c r="D161" s="122"/>
+      <c r="E161" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="F161" s="123"/>
-      <c r="G161" s="123"/>
+      <c r="F161" s="122"/>
+      <c r="G161" s="122"/>
     </row>
     <row r="162" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="112"/>
+      <c r="A162" s="98"/>
       <c r="B162" s="58" t="s">
         <v>3</v>
       </c>
@@ -14523,7 +14565,7 @@
         <f>D165*0.22</f>
         <v>8.8000000000000009E-2</v>
       </c>
-      <c r="D165" s="103">
+      <c r="D165" s="91">
         <v>0.4</v>
       </c>
       <c r="E165" s="57">
@@ -14534,7 +14576,7 @@
         <f>G165*0.58</f>
         <v>2.61</v>
       </c>
-      <c r="G165" s="104">
+      <c r="G165" s="92">
         <v>4.5</v>
       </c>
       <c r="J165">
@@ -14570,7 +14612,7 @@
         <f t="shared" ref="C166:C178" si="40">D166*0.22</f>
         <v>0.17600000000000002</v>
       </c>
-      <c r="D166" s="103">
+      <c r="D166" s="91">
         <v>0.8</v>
       </c>
       <c r="E166" s="57">
@@ -14581,7 +14623,7 @@
         <f t="shared" ref="F166:F178" si="42">G166*0.58</f>
         <v>5.22</v>
       </c>
-      <c r="G166" s="105">
+      <c r="G166" s="93">
         <v>9</v>
       </c>
       <c r="J166">
@@ -14617,7 +14659,7 @@
         <f t="shared" si="40"/>
         <v>2.6839999999999997</v>
       </c>
-      <c r="D167" s="103">
+      <c r="D167" s="91">
         <v>12.2</v>
       </c>
       <c r="E167" s="57">
@@ -14628,7 +14670,7 @@
         <f t="shared" si="42"/>
         <v>15.079999999999998</v>
       </c>
-      <c r="G167" s="105">
+      <c r="G167" s="93">
         <v>26</v>
       </c>
       <c r="J167">
@@ -14664,7 +14706,7 @@
         <f t="shared" si="40"/>
         <v>5.5</v>
       </c>
-      <c r="D168" s="103">
+      <c r="D168" s="91">
         <v>25</v>
       </c>
       <c r="E168" s="57">
@@ -14675,7 +14717,7 @@
         <f t="shared" si="42"/>
         <v>11.02</v>
       </c>
-      <c r="G168" s="105">
+      <c r="G168" s="93">
         <v>19</v>
       </c>
       <c r="J168">
@@ -14711,7 +14753,7 @@
         <f t="shared" si="40"/>
         <v>5.5</v>
       </c>
-      <c r="D169" s="103">
+      <c r="D169" s="91">
         <v>25</v>
       </c>
       <c r="E169" s="57">
@@ -14722,7 +14764,7 @@
         <f t="shared" si="42"/>
         <v>8.1199999999999992</v>
       </c>
-      <c r="G169" s="105">
+      <c r="G169" s="93">
         <v>14</v>
       </c>
       <c r="J169">
@@ -14758,7 +14800,7 @@
         <f t="shared" si="40"/>
         <v>5.5</v>
       </c>
-      <c r="D170" s="103">
+      <c r="D170" s="91">
         <v>25</v>
       </c>
       <c r="E170" s="57">
@@ -14769,7 +14811,7 @@
         <f t="shared" si="42"/>
         <v>8.1199999999999992</v>
       </c>
-      <c r="G170" s="105">
+      <c r="G170" s="93">
         <v>14</v>
       </c>
       <c r="J170">
@@ -14805,7 +14847,7 @@
         <f t="shared" si="40"/>
         <v>5.5</v>
       </c>
-      <c r="D171" s="103">
+      <c r="D171" s="91">
         <v>25</v>
       </c>
       <c r="E171" s="57">
@@ -14816,7 +14858,7 @@
         <f t="shared" si="42"/>
         <v>8.1199999999999992</v>
       </c>
-      <c r="G171" s="105">
+      <c r="G171" s="93">
         <v>14</v>
       </c>
       <c r="J171">
@@ -14852,7 +14894,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D172" s="103">
+      <c r="D172" s="91">
         <v>12</v>
       </c>
       <c r="E172" s="57">
@@ -14863,7 +14905,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G172" s="105">
+      <c r="G172" s="93">
         <v>10</v>
       </c>
       <c r="J172">
@@ -14899,7 +14941,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D173" s="103">
+      <c r="D173" s="91">
         <v>12</v>
       </c>
       <c r="E173" s="57">
@@ -14910,7 +14952,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G173" s="105">
+      <c r="G173" s="93">
         <v>10</v>
       </c>
       <c r="J173">
@@ -14946,7 +14988,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D174" s="103">
+      <c r="D174" s="91">
         <v>12</v>
       </c>
       <c r="E174" s="57">
@@ -14957,7 +14999,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G174" s="105">
+      <c r="G174" s="93">
         <v>10</v>
       </c>
       <c r="J174">
@@ -14993,7 +15035,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D175" s="103">
+      <c r="D175" s="91">
         <v>12</v>
       </c>
       <c r="E175" s="57">
@@ -15004,7 +15046,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G175" s="105">
+      <c r="G175" s="93">
         <v>10</v>
       </c>
       <c r="J175">
@@ -15040,7 +15082,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D176" s="103">
+      <c r="D176" s="91">
         <v>12</v>
       </c>
       <c r="E176" s="57">
@@ -15051,7 +15093,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G176" s="105">
+      <c r="G176" s="93">
         <v>10</v>
       </c>
       <c r="J176">
@@ -15087,7 +15129,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D177" s="103">
+      <c r="D177" s="91">
         <v>12</v>
       </c>
       <c r="E177" s="57">
@@ -15098,7 +15140,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G177" s="105">
+      <c r="G177" s="93">
         <v>10</v>
       </c>
       <c r="J177">
@@ -15134,7 +15176,7 @@
         <f t="shared" si="40"/>
         <v>2.64</v>
       </c>
-      <c r="D178" s="103">
+      <c r="D178" s="91">
         <v>12</v>
       </c>
       <c r="E178" s="57">
@@ -15145,7 +15187,7 @@
         <f t="shared" si="42"/>
         <v>5.8</v>
       </c>
-      <c r="G178" s="105">
+      <c r="G178" s="93">
         <v>10</v>
       </c>
       <c r="H178">
@@ -15174,7 +15216,7 @@
       </c>
     </row>
     <row r="179" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A179" s="102"/>
+      <c r="A179" s="90"/>
       <c r="N179">
         <f>AVERAGE(N165:N178)</f>
         <v>2.3459604408454511</v>
@@ -15271,9 +15313,9 @@
       <c r="AB185" s="20"/>
     </row>
     <row r="186" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="124"/>
-      <c r="B186" s="124"/>
-      <c r="C186" s="124"/>
+      <c r="A186" s="123"/>
+      <c r="B186" s="123"/>
+      <c r="C186" s="123"/>
       <c r="D186" s="20"/>
       <c r="E186" s="20"/>
       <c r="F186" s="20"/>
@@ -15422,7 +15464,7 @@
     </row>
     <row r="197" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A197" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B197" s="37"/>
       <c r="C197" s="37"/>
@@ -15448,37 +15490,37 @@
       <c r="W197" s="37"/>
     </row>
     <row r="198" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="119" t="s">
+      <c r="A198" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="B198" s="119"/>
-      <c r="C198" s="119"/>
-      <c r="D198" s="119"/>
-      <c r="E198" s="107"/>
-      <c r="F198" s="107"/>
+      <c r="B198" s="111"/>
+      <c r="C198" s="111"/>
+      <c r="D198" s="111"/>
+      <c r="E198" s="95"/>
+      <c r="F198" s="95"/>
     </row>
     <row r="199" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="119" t="s">
+      <c r="A199" s="111" t="s">
         <v>72</v>
       </c>
-      <c r="B199" s="119"/>
-      <c r="C199" s="119"/>
-      <c r="D199" s="119"/>
-      <c r="E199" s="107"/>
-      <c r="F199" s="107"/>
+      <c r="B199" s="111"/>
+      <c r="C199" s="111"/>
+      <c r="D199" s="111"/>
+      <c r="E199" s="95"/>
+      <c r="F199" s="95"/>
     </row>
     <row r="200" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A200" s="125" t="s">
+      <c r="A200" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="B200" s="125" t="s">
+      <c r="B200" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="C200" s="125"/>
-      <c r="D200" s="125"/>
+      <c r="C200" s="107"/>
+      <c r="D200" s="107"/>
     </row>
     <row r="201" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A201" s="125"/>
+      <c r="A201" s="107"/>
       <c r="B201" s="43" t="s">
         <v>46</v>
       </c>
@@ -15516,11 +15558,11 @@
       <c r="I202" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="J202" s="118" t="s">
-        <v>92</v>
-      </c>
-      <c r="K202" s="118"/>
-      <c r="L202" s="118"/>
+      <c r="J202" s="120" t="s">
+        <v>90</v>
+      </c>
+      <c r="K202" s="120"/>
+      <c r="L202" s="120"/>
     </row>
     <row r="203" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="44" t="s">
@@ -15605,7 +15647,7 @@
         <v>70.843999999999994</v>
       </c>
       <c r="C205" s="59">
-        <f t="shared" ref="B205:D205" si="50">C225</f>
+        <f t="shared" ref="C205:D205" si="50">C225</f>
         <v>42.506399999999992</v>
       </c>
       <c r="D205" s="59">
@@ -16118,8 +16160,8 @@
       <c r="A218" s="42"/>
       <c r="B218" s="61"/>
       <c r="C218" s="42"/>
-      <c r="D218" s="106"/>
-      <c r="E218" s="106"/>
+      <c r="D218" s="94"/>
+      <c r="E218" s="94"/>
       <c r="I218" s="44" t="s">
         <v>44</v>
       </c>
@@ -16137,27 +16179,27 @@
       </c>
     </row>
     <row r="219" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="122" t="s">
+      <c r="A219" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="B219" s="122"/>
-      <c r="C219" s="122"/>
-      <c r="D219" s="122"/>
-      <c r="E219" s="108"/>
+      <c r="B219" s="99"/>
+      <c r="C219" s="99"/>
+      <c r="D219" s="99"/>
+      <c r="E219" s="96"/>
     </row>
     <row r="220" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A220" s="122" t="s">
+      <c r="A220" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="B220" s="125" t="s">
+      <c r="B220" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="C220" s="125"/>
-      <c r="D220" s="125"/>
+      <c r="C220" s="107"/>
+      <c r="D220" s="107"/>
       <c r="E220" s="25"/>
     </row>
     <row r="221" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A221" s="122"/>
+      <c r="A221" s="99"/>
       <c r="B221" s="43" t="s">
         <v>46</v>
       </c>
@@ -16196,11 +16238,11 @@
       <c r="I222" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="J222" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="K222" s="118"/>
-      <c r="L222" s="118"/>
+      <c r="J222" s="120" t="s">
+        <v>89</v>
+      </c>
+      <c r="K222" s="120"/>
+      <c r="L222" s="120"/>
     </row>
     <row r="223" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="44" t="s">
@@ -16862,7 +16904,33 @@
       <c r="E245" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="42">
+    <mergeCell ref="AW81:AW83"/>
+    <mergeCell ref="AX81:BB82"/>
+    <mergeCell ref="BD81:BD83"/>
+    <mergeCell ref="BE81:BI82"/>
+    <mergeCell ref="AA87:AA88"/>
+    <mergeCell ref="AA81:AI81"/>
+    <mergeCell ref="AB82:AI82"/>
+    <mergeCell ref="AB87:AI87"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A111:Q111"/>
+    <mergeCell ref="N81:N83"/>
+    <mergeCell ref="B81:L82"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="E161:G161"/>
+    <mergeCell ref="A186:C186"/>
+    <mergeCell ref="B200:D200"/>
+    <mergeCell ref="B220:D220"/>
+    <mergeCell ref="A198:D198"/>
+    <mergeCell ref="A199:D199"/>
+    <mergeCell ref="A80:X80"/>
+    <mergeCell ref="I115:N115"/>
+    <mergeCell ref="O81:Y82"/>
+    <mergeCell ref="AA82:AA83"/>
+    <mergeCell ref="J222:L222"/>
+    <mergeCell ref="J202:L202"/>
     <mergeCell ref="A161:A162"/>
     <mergeCell ref="A219:D219"/>
     <mergeCell ref="A2:H2"/>
@@ -16879,31 +16947,6 @@
     <mergeCell ref="B52:D52"/>
     <mergeCell ref="E52:G52"/>
     <mergeCell ref="A81:A83"/>
-    <mergeCell ref="I115:N115"/>
-    <mergeCell ref="O81:Y82"/>
-    <mergeCell ref="AA82:AA83"/>
-    <mergeCell ref="J222:L222"/>
-    <mergeCell ref="J202:L202"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A111:Q111"/>
-    <mergeCell ref="N81:N83"/>
-    <mergeCell ref="B81:L82"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="E161:G161"/>
-    <mergeCell ref="A186:C186"/>
-    <mergeCell ref="B200:D200"/>
-    <mergeCell ref="B220:D220"/>
-    <mergeCell ref="A198:D198"/>
-    <mergeCell ref="A199:D199"/>
-    <mergeCell ref="AW81:AW83"/>
-    <mergeCell ref="AX81:BB82"/>
-    <mergeCell ref="BD81:BD83"/>
-    <mergeCell ref="BE81:BI82"/>
-    <mergeCell ref="AA87:AA88"/>
-    <mergeCell ref="AA81:AI81"/>
-    <mergeCell ref="AB82:AI82"/>
-    <mergeCell ref="AB87:AI87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update baeline fertility decline percentages in Excel
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -509,8 +509,8 @@
     <numFmt numFmtId="164" formatCode="0.00000;\-0.00000;0"/>
     <numFmt numFmtId="165" formatCode="###;\-###;0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.0000;\-0.0000;0"/>
-    <numFmt numFmtId="172" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0000;\-0.0000;0"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="38" x14ac:knownFonts="1">
     <font>
@@ -1657,10 +1657,109 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="29" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1684,9 +1783,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1696,104 +1792,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="170" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="29" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="170" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="170" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="29" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="29" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -8278,8 +8278,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BJ245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AS73" sqref="AS73"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G155" sqref="G155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8362,16 +8362,16 @@
       <c r="Y1" s="37"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="139" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="139"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -8423,14 +8423,14 @@
       <c r="A4" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="129" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="111" t="s">
+      <c r="C4" s="130"/>
+      <c r="D4" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="112"/>
+      <c r="E4" s="130"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -8858,10 +8858,10 @@
       <c r="A27" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="111" t="s">
+      <c r="B27" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="112"/>
+      <c r="C27" s="130"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -9276,19 +9276,19 @@
       <c r="AE51" s="24"/>
     </row>
     <row r="52" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="113" t="s">
+      <c r="A52" s="149" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="113" t="s">
+      <c r="B52" s="149" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="113"/>
-      <c r="D52" s="113"/>
-      <c r="E52" s="113" t="s">
+      <c r="C52" s="149"/>
+      <c r="D52" s="149"/>
+      <c r="E52" s="149" t="s">
         <v>55</v>
       </c>
-      <c r="F52" s="113"/>
-      <c r="G52" s="113"/>
+      <c r="F52" s="149"/>
+      <c r="G52" s="149"/>
       <c r="X52" s="22"/>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
@@ -9299,7 +9299,7 @@
       <c r="AE52" s="22"/>
     </row>
     <row r="53" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="113"/>
+      <c r="A53" s="149"/>
       <c r="B53" s="33" t="s">
         <v>3</v>
       </c>
@@ -9805,151 +9805,151 @@
       <c r="X79" s="37"/>
     </row>
     <row r="80" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="127" t="s">
+      <c r="A80" s="136" t="s">
         <v>105</v>
       </c>
-      <c r="B80" s="127"/>
-      <c r="C80" s="127"/>
-      <c r="D80" s="127"/>
-      <c r="E80" s="127"/>
-      <c r="F80" s="127"/>
-      <c r="G80" s="127"/>
-      <c r="H80" s="127"/>
-      <c r="I80" s="127"/>
-      <c r="J80" s="127"/>
-      <c r="K80" s="127"/>
-      <c r="L80" s="127"/>
-      <c r="M80" s="127"/>
-      <c r="N80" s="127"/>
-      <c r="O80" s="127"/>
-      <c r="P80" s="127"/>
-      <c r="Q80" s="127"/>
-      <c r="R80" s="127"/>
-      <c r="S80" s="127"/>
-      <c r="T80" s="127"/>
-      <c r="U80" s="127"/>
-      <c r="V80" s="127"/>
-      <c r="W80" s="127"/>
-      <c r="X80" s="127"/>
+      <c r="B80" s="136"/>
+      <c r="C80" s="136"/>
+      <c r="D80" s="136"/>
+      <c r="E80" s="136"/>
+      <c r="F80" s="136"/>
+      <c r="G80" s="136"/>
+      <c r="H80" s="136"/>
+      <c r="I80" s="136"/>
+      <c r="J80" s="136"/>
+      <c r="K80" s="136"/>
+      <c r="L80" s="136"/>
+      <c r="M80" s="136"/>
+      <c r="N80" s="136"/>
+      <c r="O80" s="136"/>
+      <c r="P80" s="136"/>
+      <c r="Q80" s="136"/>
+      <c r="R80" s="136"/>
+      <c r="S80" s="136"/>
+      <c r="T80" s="136"/>
+      <c r="U80" s="136"/>
+      <c r="V80" s="136"/>
+      <c r="W80" s="136"/>
+      <c r="X80" s="136"/>
     </row>
     <row r="81" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="114" t="s">
+      <c r="A81" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="98" t="s">
+      <c r="B81" s="123" t="s">
         <v>106</v>
       </c>
-      <c r="C81" s="98"/>
-      <c r="D81" s="98"/>
-      <c r="E81" s="98"/>
-      <c r="F81" s="98"/>
-      <c r="G81" s="98"/>
-      <c r="H81" s="98"/>
-      <c r="I81" s="98"/>
-      <c r="J81" s="98"/>
-      <c r="K81" s="98"/>
-      <c r="L81" s="98"/>
-      <c r="N81" s="114" t="s">
+      <c r="C81" s="123"/>
+      <c r="D81" s="123"/>
+      <c r="E81" s="123"/>
+      <c r="F81" s="123"/>
+      <c r="G81" s="123"/>
+      <c r="H81" s="123"/>
+      <c r="I81" s="123"/>
+      <c r="J81" s="123"/>
+      <c r="K81" s="123"/>
+      <c r="L81" s="123"/>
+      <c r="N81" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="O81" s="98" t="s">
+      <c r="O81" s="123" t="s">
         <v>107</v>
       </c>
-      <c r="P81" s="98"/>
-      <c r="Q81" s="98"/>
-      <c r="R81" s="98"/>
-      <c r="S81" s="98"/>
-      <c r="T81" s="98"/>
-      <c r="U81" s="98"/>
-      <c r="V81" s="98"/>
-      <c r="W81" s="98"/>
-      <c r="X81" s="98"/>
-      <c r="Y81" s="98"/>
-      <c r="AA81" s="124" t="s">
+      <c r="P81" s="123"/>
+      <c r="Q81" s="123"/>
+      <c r="R81" s="123"/>
+      <c r="S81" s="123"/>
+      <c r="T81" s="123"/>
+      <c r="U81" s="123"/>
+      <c r="V81" s="123"/>
+      <c r="W81" s="123"/>
+      <c r="X81" s="123"/>
+      <c r="Y81" s="123"/>
+      <c r="AA81" s="126" t="s">
         <v>78</v>
       </c>
-      <c r="AB81" s="125"/>
-      <c r="AC81" s="125"/>
-      <c r="AD81" s="125"/>
-      <c r="AE81" s="125"/>
-      <c r="AF81" s="125"/>
-      <c r="AG81" s="125"/>
-      <c r="AH81" s="125"/>
-      <c r="AI81" s="126"/>
-      <c r="AW81" s="114" t="s">
+      <c r="AB81" s="127"/>
+      <c r="AC81" s="127"/>
+      <c r="AD81" s="127"/>
+      <c r="AE81" s="127"/>
+      <c r="AF81" s="127"/>
+      <c r="AG81" s="127"/>
+      <c r="AH81" s="127"/>
+      <c r="AI81" s="128"/>
+      <c r="AW81" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="AX81" s="98" t="s">
+      <c r="AX81" s="123" t="s">
         <v>103</v>
       </c>
-      <c r="AY81" s="98"/>
-      <c r="AZ81" s="98"/>
-      <c r="BA81" s="98"/>
-      <c r="BB81" s="98"/>
-      <c r="BD81" s="114" t="s">
+      <c r="AY81" s="123"/>
+      <c r="AZ81" s="123"/>
+      <c r="BA81" s="123"/>
+      <c r="BB81" s="123"/>
+      <c r="BD81" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="BE81" s="98" t="s">
+      <c r="BE81" s="123" t="s">
         <v>104</v>
       </c>
-      <c r="BF81" s="98"/>
-      <c r="BG81" s="98"/>
-      <c r="BH81" s="98"/>
-      <c r="BI81" s="98"/>
+      <c r="BF81" s="123"/>
+      <c r="BG81" s="123"/>
+      <c r="BH81" s="123"/>
+      <c r="BI81" s="123"/>
     </row>
     <row r="82" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="115"/>
-      <c r="B82" s="98"/>
-      <c r="C82" s="98"/>
-      <c r="D82" s="98"/>
-      <c r="E82" s="98"/>
-      <c r="F82" s="98"/>
-      <c r="G82" s="98"/>
-      <c r="H82" s="98"/>
-      <c r="I82" s="98"/>
-      <c r="J82" s="98"/>
-      <c r="K82" s="98"/>
-      <c r="L82" s="98"/>
-      <c r="N82" s="115"/>
-      <c r="O82" s="98"/>
-      <c r="P82" s="98"/>
-      <c r="Q82" s="98"/>
-      <c r="R82" s="98"/>
-      <c r="S82" s="98"/>
-      <c r="T82" s="98"/>
-      <c r="U82" s="98"/>
-      <c r="V82" s="98"/>
-      <c r="W82" s="98"/>
-      <c r="X82" s="98"/>
-      <c r="Y82" s="98"/>
-      <c r="AA82" s="118" t="s">
+      <c r="A82" s="121"/>
+      <c r="B82" s="123"/>
+      <c r="C82" s="123"/>
+      <c r="D82" s="123"/>
+      <c r="E82" s="123"/>
+      <c r="F82" s="123"/>
+      <c r="G82" s="123"/>
+      <c r="H82" s="123"/>
+      <c r="I82" s="123"/>
+      <c r="J82" s="123"/>
+      <c r="K82" s="123"/>
+      <c r="L82" s="123"/>
+      <c r="N82" s="121"/>
+      <c r="O82" s="123"/>
+      <c r="P82" s="123"/>
+      <c r="Q82" s="123"/>
+      <c r="R82" s="123"/>
+      <c r="S82" s="123"/>
+      <c r="T82" s="123"/>
+      <c r="U82" s="123"/>
+      <c r="V82" s="123"/>
+      <c r="W82" s="123"/>
+      <c r="X82" s="123"/>
+      <c r="Y82" s="123"/>
+      <c r="AA82" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="AB82" s="124" t="s">
+      <c r="AB82" s="126" t="s">
         <v>72</v>
       </c>
-      <c r="AC82" s="125"/>
-      <c r="AD82" s="125"/>
-      <c r="AE82" s="125"/>
-      <c r="AF82" s="125"/>
-      <c r="AG82" s="125"/>
-      <c r="AH82" s="125"/>
-      <c r="AI82" s="126"/>
-      <c r="AW82" s="115"/>
-      <c r="AX82" s="98"/>
-      <c r="AY82" s="98"/>
-      <c r="AZ82" s="98"/>
-      <c r="BA82" s="98"/>
-      <c r="BB82" s="98"/>
-      <c r="BD82" s="115"/>
-      <c r="BE82" s="98"/>
-      <c r="BF82" s="98"/>
-      <c r="BG82" s="98"/>
-      <c r="BH82" s="98"/>
-      <c r="BI82" s="98"/>
+      <c r="AC82" s="127"/>
+      <c r="AD82" s="127"/>
+      <c r="AE82" s="127"/>
+      <c r="AF82" s="127"/>
+      <c r="AG82" s="127"/>
+      <c r="AH82" s="127"/>
+      <c r="AI82" s="128"/>
+      <c r="AW82" s="121"/>
+      <c r="AX82" s="123"/>
+      <c r="AY82" s="123"/>
+      <c r="AZ82" s="123"/>
+      <c r="BA82" s="123"/>
+      <c r="BB82" s="123"/>
+      <c r="BD82" s="121"/>
+      <c r="BE82" s="123"/>
+      <c r="BF82" s="123"/>
+      <c r="BG82" s="123"/>
+      <c r="BH82" s="123"/>
+      <c r="BI82" s="123"/>
     </row>
     <row r="83" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="116"/>
+      <c r="A83" s="122"/>
       <c r="B83" s="71" t="s">
         <v>91</v>
       </c>
@@ -9983,7 +9983,7 @@
       <c r="L83" s="82">
         <v>2020</v>
       </c>
-      <c r="N83" s="116"/>
+      <c r="N83" s="122"/>
       <c r="O83" s="72" t="s">
         <v>91</v>
       </c>
@@ -10008,16 +10008,16 @@
       <c r="V83" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="W83" s="131">
+      <c r="W83" s="101">
         <v>2000</v>
       </c>
-      <c r="X83" s="132">
+      <c r="X83" s="102">
         <v>2017</v>
       </c>
-      <c r="Y83" s="133">
+      <c r="Y83" s="103">
         <v>2020</v>
       </c>
-      <c r="AA83" s="119"/>
+      <c r="AA83" s="125"/>
       <c r="AB83" s="71" t="s">
         <v>91</v>
       </c>
@@ -10042,7 +10042,7 @@
       <c r="AI83" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="AW83" s="116"/>
+      <c r="AW83" s="122"/>
       <c r="AX83" s="71" t="s">
         <v>91</v>
       </c>
@@ -10058,7 +10058,7 @@
       <c r="BB83" s="84">
         <v>2020</v>
       </c>
-      <c r="BD83" s="116"/>
+      <c r="BD83" s="122"/>
       <c r="BE83" s="71" t="s">
         <v>91</v>
       </c>
@@ -10111,13 +10111,13 @@
         <f t="shared" si="7"/>
         <v>5.6975585300000006E-2</v>
       </c>
-      <c r="J84" s="128">
+      <c r="J84" s="98">
         <v>1.2464773E-2</v>
       </c>
       <c r="K84" s="85">
         <v>5.892614E-3</v>
       </c>
-      <c r="L84" s="130">
+      <c r="L84" s="100">
         <f>K84+($L$83-$K$83)*M84</f>
         <v>4.7328212352941174E-3</v>
       </c>
@@ -10160,13 +10160,13 @@
         <f t="shared" si="8"/>
         <v>4.7441704699999997E-2</v>
       </c>
-      <c r="W84" s="128">
+      <c r="W84" s="98">
         <v>1.0375972000000001E-2</v>
       </c>
-      <c r="X84" s="128">
+      <c r="X84" s="98">
         <v>4.9718649999999998E-3</v>
       </c>
-      <c r="Y84" s="130">
+      <c r="Y84" s="100">
         <f>X84+($Y$83-$X$83)*Z84</f>
         <v>4.0181990588235295E-3</v>
       </c>
@@ -10204,46 +10204,46 @@
       <c r="AW84" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="AX84" s="134">
+      <c r="AX84" s="104">
         <v>0.19005920400000001</v>
       </c>
-      <c r="AY84" s="135">
+      <c r="AY84" s="105">
         <v>5.6975585300000006E-2</v>
       </c>
-      <c r="AZ84" s="136">
+      <c r="AZ84" s="106">
         <v>1.4393767E-2</v>
       </c>
-      <c r="BA84" s="137">
+      <c r="BA84" s="107">
         <v>6.7479519999999998E-3</v>
       </c>
-      <c r="BB84" s="138">
+      <c r="BB84" s="108">
         <f>BA84+($L$83-$K$83)*BC84</f>
         <v>5.3986905294117647E-3</v>
       </c>
-      <c r="BC84" s="139">
+      <c r="BC84" s="109">
         <f>(BA84-AZ84)/($K$83-$J$83)</f>
         <v>-4.4975382352941177E-4</v>
       </c>
       <c r="BD84" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="BE84" s="142">
+      <c r="BE84" s="112">
         <v>0.16283755500000002</v>
       </c>
-      <c r="BF84" s="143">
+      <c r="BF84" s="113">
         <v>4.7441704699999997E-2</v>
       </c>
-      <c r="BG84" s="144">
+      <c r="BG84" s="114">
         <v>1.1839005E-2</v>
       </c>
-      <c r="BH84" s="145">
+      <c r="BH84" s="115">
         <v>5.6765679999999999E-3</v>
       </c>
-      <c r="BI84" s="146">
+      <c r="BI84" s="116">
         <f>BH84+($Y$83-$X$83)*BJ84</f>
         <v>4.589079117647059E-3</v>
       </c>
-      <c r="BJ84" s="147">
+      <c r="BJ84" s="117">
         <f>(BH84-BG84)/($X$83-$W$83)</f>
         <v>-3.6249629411764703E-4</v>
       </c>
@@ -10276,13 +10276,13 @@
       <c r="I85" s="89">
         <v>2.4750038999999998E-3</v>
       </c>
-      <c r="J85" s="128">
+      <c r="J85" s="98">
         <v>1.2523619999999999E-3</v>
       </c>
       <c r="K85" s="86">
         <v>4.3800000000000002E-4</v>
       </c>
-      <c r="L85" s="130">
+      <c r="L85" s="100">
         <f t="shared" ref="L85:L99" si="9">K85+($L$83-$K$83)*M85</f>
         <v>2.9428905882352948E-4</v>
       </c>
@@ -10317,13 +10317,13 @@
       <c r="V85" s="89">
         <v>1.8590649E-3</v>
       </c>
-      <c r="W85" s="129">
+      <c r="W85" s="99">
         <v>9.1699999999999995E-4</v>
       </c>
-      <c r="X85" s="129">
+      <c r="X85" s="99">
         <v>3.0899999999999998E-4</v>
       </c>
-      <c r="Y85" s="130">
+      <c r="Y85" s="100">
         <f t="shared" ref="Y85:Y99" si="11">X85+($Y$83-$X$83)*Z85</f>
         <v>2.0170588235294114E-4</v>
       </c>
@@ -10361,46 +10361,46 @@
       <c r="AW85" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="AX85" s="140">
+      <c r="AX85" s="110">
         <v>8.6783771000000006E-3</v>
       </c>
-      <c r="AY85" s="141">
+      <c r="AY85" s="111">
         <v>2.4750038999999998E-3</v>
       </c>
-      <c r="AZ85" s="136">
+      <c r="AZ85" s="106">
         <v>1.343999E-3</v>
       </c>
-      <c r="BA85" s="137">
+      <c r="BA85" s="107">
         <v>5.1699999999999999E-4</v>
       </c>
-      <c r="BB85" s="138">
+      <c r="BB85" s="108">
         <f t="shared" ref="BB85:BB99" si="13">BA85+($L$83-$K$83)*BC85</f>
         <v>3.7105899999999997E-4</v>
       </c>
-      <c r="BC85" s="139">
+      <c r="BC85" s="109">
         <f t="shared" ref="BC85:BC99" si="14">(BA85-AZ85)/($K$83-$J$83)</f>
         <v>-4.8647000000000004E-5</v>
       </c>
       <c r="BD85" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="BE85" s="148">
+      <c r="BE85" s="118">
         <v>7.4032815999999996E-3</v>
       </c>
-      <c r="BF85" s="149">
+      <c r="BF85" s="119">
         <v>1.8590649E-3</v>
       </c>
-      <c r="BG85" s="144">
+      <c r="BG85" s="114">
         <v>9.7599999999999998E-4</v>
       </c>
-      <c r="BH85" s="145">
+      <c r="BH85" s="115">
         <v>3.6499999999999998E-4</v>
       </c>
-      <c r="BI85" s="146">
+      <c r="BI85" s="116">
         <f t="shared" ref="BI85:BI99" si="15">BH85+($Y$83-$X$83)*BJ85</f>
         <v>2.5717647058823528E-4</v>
       </c>
-      <c r="BJ85" s="147">
+      <c r="BJ85" s="117">
         <f t="shared" ref="BJ85:BJ99" si="16">(BH85-BG85)/($X$83-$W$83)</f>
         <v>-3.5941176470588238E-5</v>
       </c>
@@ -10433,13 +10433,13 @@
       <c r="I86" s="89">
         <v>1.5814690000000001E-3</v>
       </c>
-      <c r="J86" s="129">
+      <c r="J86" s="99">
         <v>9.77E-4</v>
       </c>
       <c r="K86" s="86">
         <v>2.7099999999999997E-4</v>
       </c>
-      <c r="L86" s="130">
+      <c r="L86" s="100">
         <f t="shared" si="9"/>
         <v>1.4641176470588232E-4</v>
       </c>
@@ -10474,13 +10474,13 @@
       <c r="V86" s="89">
         <v>1.2227608999999999E-3</v>
       </c>
-      <c r="W86" s="129">
+      <c r="W86" s="99">
         <v>7.4100000000000001E-4</v>
       </c>
-      <c r="X86" s="129">
+      <c r="X86" s="99">
         <v>1.65E-4</v>
       </c>
-      <c r="Y86" s="130">
+      <c r="Y86" s="100">
         <f t="shared" si="11"/>
         <v>6.335294117647058E-5</v>
       </c>
@@ -10500,46 +10500,46 @@
       <c r="AW86" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="AX86" s="140">
+      <c r="AX86" s="110">
         <v>4.7901753000000004E-3</v>
       </c>
-      <c r="AY86" s="141">
+      <c r="AY86" s="111">
         <v>1.5814690000000001E-3</v>
       </c>
-      <c r="AZ86" s="136">
+      <c r="AZ86" s="106">
         <v>1.006123E-3</v>
       </c>
-      <c r="BA86" s="137">
+      <c r="BA86" s="107">
         <v>3.1799999999999998E-4</v>
       </c>
-      <c r="BB86" s="138">
+      <c r="BB86" s="108">
         <f t="shared" si="13"/>
         <v>1.9656652941176466E-4</v>
       </c>
-      <c r="BC86" s="139">
+      <c r="BC86" s="109">
         <f t="shared" si="14"/>
         <v>-4.0477823529411771E-5</v>
       </c>
       <c r="BD86" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="BE86" s="148">
+      <c r="BE86" s="118">
         <v>4.3711651000000002E-3</v>
       </c>
-      <c r="BF86" s="149">
+      <c r="BF86" s="119">
         <v>1.2227608999999999E-3</v>
       </c>
-      <c r="BG86" s="144">
+      <c r="BG86" s="114">
         <v>7.5699999999999997E-4</v>
       </c>
-      <c r="BH86" s="145">
+      <c r="BH86" s="115">
         <v>1.95E-4</v>
       </c>
-      <c r="BI86" s="146">
+      <c r="BI86" s="116">
         <f t="shared" si="15"/>
         <v>9.5823529411764706E-5</v>
       </c>
-      <c r="BJ86" s="147">
+      <c r="BJ86" s="117">
         <f t="shared" si="16"/>
         <v>-3.3058823529411766E-5</v>
       </c>
@@ -10572,13 +10572,13 @@
       <c r="I87" s="89">
         <v>2.5001934000000001E-3</v>
       </c>
-      <c r="J87" s="128">
+      <c r="J87" s="98">
         <v>2.1267130000000001E-3</v>
       </c>
       <c r="K87" s="86">
         <v>6.4599999999999998E-4</v>
       </c>
-      <c r="L87" s="130">
+      <c r="L87" s="100">
         <f t="shared" si="9"/>
         <v>3.8469770588235287E-4</v>
       </c>
@@ -10613,13 +10613,13 @@
       <c r="V87" s="89">
         <v>1.6750273E-3</v>
       </c>
-      <c r="W87" s="128">
+      <c r="W87" s="98">
         <v>1.469932E-3</v>
       </c>
-      <c r="X87" s="129">
+      <c r="X87" s="99">
         <v>3.9800000000000002E-4</v>
       </c>
-      <c r="Y87" s="130">
+      <c r="Y87" s="100">
         <f t="shared" si="11"/>
         <v>2.0883552941176474E-4</v>
       </c>
@@ -10627,62 +10627,62 @@
         <f t="shared" si="12"/>
         <v>-6.3054823529411761E-5</v>
       </c>
-      <c r="AA87" s="118" t="s">
+      <c r="AA87" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="AB87" s="124" t="s">
+      <c r="AB87" s="126" t="s">
         <v>73</v>
       </c>
-      <c r="AC87" s="125"/>
-      <c r="AD87" s="125"/>
-      <c r="AE87" s="125"/>
-      <c r="AF87" s="125"/>
-      <c r="AG87" s="125"/>
-      <c r="AH87" s="125"/>
-      <c r="AI87" s="126"/>
+      <c r="AC87" s="127"/>
+      <c r="AD87" s="127"/>
+      <c r="AE87" s="127"/>
+      <c r="AF87" s="127"/>
+      <c r="AG87" s="127"/>
+      <c r="AH87" s="127"/>
+      <c r="AI87" s="128"/>
       <c r="AW87" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="AX87" s="140">
+      <c r="AX87" s="110">
         <v>5.9821824000000001E-3</v>
       </c>
-      <c r="AY87" s="141">
+      <c r="AY87" s="111">
         <v>2.5001934000000001E-3</v>
       </c>
-      <c r="AZ87" s="136">
+      <c r="AZ87" s="106">
         <v>2.2244869999999998E-3</v>
       </c>
-      <c r="BA87" s="137">
+      <c r="BA87" s="107">
         <v>9.2199999999999997E-4</v>
       </c>
-      <c r="BB87" s="138">
+      <c r="BB87" s="108">
         <f t="shared" si="13"/>
         <v>6.9214935294117648E-4</v>
       </c>
-      <c r="BC87" s="139">
+      <c r="BC87" s="109">
         <f t="shared" si="14"/>
         <v>-7.6616882352941159E-5</v>
       </c>
       <c r="BD87" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="BE87" s="148">
+      <c r="BE87" s="118">
         <v>4.8596317000000003E-3</v>
       </c>
-      <c r="BF87" s="149">
+      <c r="BF87" s="119">
         <v>1.6750273E-3</v>
       </c>
-      <c r="BG87" s="144">
+      <c r="BG87" s="114">
         <v>1.7839729999999999E-3</v>
       </c>
-      <c r="BH87" s="145">
+      <c r="BH87" s="115">
         <v>7.0299999999999996E-4</v>
       </c>
-      <c r="BI87" s="146">
+      <c r="BI87" s="116">
         <f t="shared" si="15"/>
         <v>5.1224005882352934E-4</v>
       </c>
-      <c r="BJ87" s="147">
+      <c r="BJ87" s="117">
         <f t="shared" si="16"/>
         <v>-6.3586647058823525E-5</v>
       </c>
@@ -10715,13 +10715,13 @@
       <c r="I88" s="89">
         <v>3.7640993E-3</v>
       </c>
-      <c r="J88" s="128">
+      <c r="J88" s="98">
         <v>3.647225E-3</v>
       </c>
       <c r="K88" s="85">
         <v>2.068032E-3</v>
       </c>
-      <c r="L88" s="130">
+      <c r="L88" s="100">
         <f t="shared" si="9"/>
         <v>1.7893508823529412E-3</v>
       </c>
@@ -10756,13 +10756,13 @@
       <c r="V88" s="89">
         <v>2.3815536E-3</v>
       </c>
-      <c r="W88" s="128">
+      <c r="W88" s="98">
         <v>3.4466029999999999E-3</v>
       </c>
-      <c r="X88" s="128">
+      <c r="X88" s="98">
         <v>1.022128E-3</v>
       </c>
-      <c r="Y88" s="130">
+      <c r="Y88" s="100">
         <f t="shared" si="11"/>
         <v>5.9427947058823534E-4</v>
       </c>
@@ -10770,7 +10770,7 @@
         <f t="shared" si="12"/>
         <v>-1.4261617647058823E-4</v>
       </c>
-      <c r="AA88" s="119"/>
+      <c r="AA88" s="125"/>
       <c r="AB88" s="71" t="s">
         <v>91</v>
       </c>
@@ -10798,46 +10798,46 @@
       <c r="AW88" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="AX88" s="140">
+      <c r="AX88" s="110">
         <v>8.4956649999999995E-3</v>
       </c>
-      <c r="AY88" s="141">
+      <c r="AY88" s="111">
         <v>3.7640993E-3</v>
       </c>
-      <c r="AZ88" s="136">
+      <c r="AZ88" s="106">
         <v>4.404697E-3</v>
       </c>
-      <c r="BA88" s="137">
+      <c r="BA88" s="107">
         <v>2.4275730000000001E-3</v>
       </c>
-      <c r="BB88" s="138">
+      <c r="BB88" s="108">
         <f t="shared" si="13"/>
         <v>2.0786687647058825E-3</v>
       </c>
-      <c r="BC88" s="139">
+      <c r="BC88" s="109">
         <f t="shared" si="14"/>
         <v>-1.1630141176470587E-4</v>
       </c>
       <c r="BD88" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="BE88" s="148">
+      <c r="BE88" s="118">
         <v>5.6320531999999998E-3</v>
       </c>
-      <c r="BF88" s="149">
+      <c r="BF88" s="119">
         <v>2.3815536E-3</v>
       </c>
-      <c r="BG88" s="144">
+      <c r="BG88" s="114">
         <v>4.9665059999999999E-3</v>
       </c>
-      <c r="BH88" s="145">
+      <c r="BH88" s="115">
         <v>1.625781E-3</v>
       </c>
-      <c r="BI88" s="146">
+      <c r="BI88" s="116">
         <f t="shared" si="15"/>
         <v>1.0362412941176471E-3</v>
       </c>
-      <c r="BJ88" s="147">
+      <c r="BJ88" s="117">
         <f t="shared" si="16"/>
         <v>-1.9651323529411765E-4</v>
       </c>
@@ -10870,13 +10870,13 @@
       <c r="I89" s="89">
         <v>4.3315932999999996E-3</v>
       </c>
-      <c r="J89" s="128">
+      <c r="J89" s="98">
         <v>5.7620409999999999E-3</v>
       </c>
       <c r="K89" s="85">
         <v>2.644057E-3</v>
       </c>
-      <c r="L89" s="130">
+      <c r="L89" s="100">
         <f t="shared" si="9"/>
         <v>2.0938245294117646E-3</v>
       </c>
@@ -10911,13 +10911,13 @@
       <c r="V89" s="89">
         <v>3.1198295999999999E-3</v>
       </c>
-      <c r="W89" s="128">
+      <c r="W89" s="98">
         <v>5.689525E-3</v>
       </c>
-      <c r="X89" s="128">
+      <c r="X89" s="98">
         <v>1.4837839999999999E-3</v>
       </c>
-      <c r="Y89" s="130">
+      <c r="Y89" s="100">
         <f t="shared" si="11"/>
         <v>7.4159441176470582E-4</v>
       </c>
@@ -10955,46 +10955,46 @@
       <c r="AW89" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="AX89" s="140">
+      <c r="AX89" s="110">
         <v>9.3605019000000001E-3</v>
       </c>
-      <c r="AY89" s="141">
+      <c r="AY89" s="111">
         <v>4.3315932999999996E-3</v>
       </c>
-      <c r="AZ89" s="136">
+      <c r="AZ89" s="106">
         <v>7.9141460000000004E-3</v>
       </c>
-      <c r="BA89" s="137">
+      <c r="BA89" s="107">
         <v>3.7748500000000002E-3</v>
       </c>
-      <c r="BB89" s="138">
+      <c r="BB89" s="108">
         <f t="shared" si="13"/>
         <v>3.0443860000000001E-3</v>
       </c>
-      <c r="BC89" s="139">
+      <c r="BC89" s="109">
         <f t="shared" si="14"/>
         <v>-2.4348800000000004E-4</v>
       </c>
       <c r="BD89" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="BE89" s="148">
+      <c r="BE89" s="118">
         <v>6.4621250999999996E-3</v>
       </c>
-      <c r="BF89" s="149">
+      <c r="BF89" s="119">
         <v>3.1198295999999999E-3</v>
       </c>
-      <c r="BG89" s="144">
+      <c r="BG89" s="114">
         <v>8.7300439999999993E-3</v>
       </c>
-      <c r="BH89" s="145">
+      <c r="BH89" s="115">
         <v>2.8349930000000001E-3</v>
       </c>
-      <c r="BI89" s="146">
+      <c r="BI89" s="116">
         <f t="shared" si="15"/>
         <v>1.7946898823529415E-3</v>
       </c>
-      <c r="BJ89" s="147">
+      <c r="BJ89" s="117">
         <f t="shared" si="16"/>
         <v>-3.4676770588235289E-4</v>
       </c>
@@ -11027,13 +11027,13 @@
       <c r="I90" s="89">
         <v>5.1669517000000002E-3</v>
       </c>
-      <c r="J90" s="128">
+      <c r="J90" s="98">
         <v>8.5842190000000006E-3</v>
       </c>
       <c r="K90" s="85">
         <v>3.4039669999999999E-3</v>
       </c>
-      <c r="L90" s="130">
+      <c r="L90" s="100">
         <f t="shared" si="9"/>
         <v>2.4898048823529411E-3</v>
       </c>
@@ -11068,13 +11068,13 @@
       <c r="V90" s="89">
         <v>3.7817176000000002E-3</v>
       </c>
-      <c r="W90" s="128">
+      <c r="W90" s="98">
         <v>6.367841E-3</v>
       </c>
-      <c r="X90" s="128">
+      <c r="X90" s="98">
         <v>1.8290649999999999E-3</v>
       </c>
-      <c r="Y90" s="130">
+      <c r="Y90" s="100">
         <f t="shared" si="11"/>
         <v>1.0281045294117646E-3</v>
       </c>
@@ -11112,46 +11112,46 @@
       <c r="AW90" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="AX90" s="140">
+      <c r="AX90" s="110">
         <v>1.0468597E-2</v>
       </c>
-      <c r="AY90" s="141">
+      <c r="AY90" s="111">
         <v>5.1669517000000002E-3</v>
       </c>
-      <c r="AZ90" s="136">
+      <c r="AZ90" s="106">
         <v>1.0961822E-2</v>
       </c>
-      <c r="BA90" s="137">
+      <c r="BA90" s="107">
         <v>5.0321869999999996E-3</v>
       </c>
-      <c r="BB90" s="138">
+      <c r="BB90" s="108">
         <f t="shared" si="13"/>
         <v>3.9857808235294109E-3</v>
       </c>
-      <c r="BC90" s="139">
+      <c r="BC90" s="109">
         <f t="shared" si="14"/>
         <v>-3.4880205882352943E-4</v>
       </c>
       <c r="BD90" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="BE90" s="148">
+      <c r="BE90" s="118">
         <v>7.3166155E-3</v>
       </c>
-      <c r="BF90" s="149">
+      <c r="BF90" s="119">
         <v>3.7817176000000002E-3</v>
       </c>
-      <c r="BG90" s="144">
+      <c r="BG90" s="114">
         <v>9.3410109999999998E-3</v>
       </c>
-      <c r="BH90" s="145">
+      <c r="BH90" s="115">
         <v>3.592764E-3</v>
       </c>
-      <c r="BI90" s="146">
+      <c r="BI90" s="116">
         <f t="shared" si="15"/>
         <v>2.5783674705882353E-3</v>
       </c>
-      <c r="BJ90" s="147">
+      <c r="BJ90" s="117">
         <f t="shared" si="16"/>
         <v>-3.3813217647058825E-4</v>
       </c>
@@ -11184,13 +11184,13 @@
       <c r="I91" s="89">
         <v>6.4414638999999996E-3</v>
       </c>
-      <c r="J91" s="128">
+      <c r="J91" s="98">
         <v>1.0363597E-2</v>
       </c>
       <c r="K91" s="85">
         <v>3.9863540000000001E-3</v>
       </c>
-      <c r="L91" s="130">
+      <c r="L91" s="100">
         <f t="shared" si="9"/>
         <v>2.8609581764705884E-3</v>
       </c>
@@ -11225,13 +11225,13 @@
       <c r="V91" s="89">
         <v>4.6448573999999998E-3</v>
       </c>
-      <c r="W91" s="128">
+      <c r="W91" s="98">
         <v>6.1407370000000003E-3</v>
       </c>
-      <c r="X91" s="128">
+      <c r="X91" s="98">
         <v>1.8174109999999999E-3</v>
       </c>
-      <c r="Y91" s="130">
+      <c r="Y91" s="100">
         <f t="shared" si="11"/>
         <v>1.0544711176470585E-3</v>
       </c>
@@ -11242,46 +11242,46 @@
       <c r="AW91" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="AX91" s="140">
+      <c r="AX91" s="110">
         <v>1.2171936E-2</v>
       </c>
-      <c r="AY91" s="141">
+      <c r="AY91" s="111">
         <v>6.4414638999999996E-3</v>
       </c>
-      <c r="AZ91" s="136">
+      <c r="AZ91" s="106">
         <v>1.3134368E-2</v>
       </c>
-      <c r="BA91" s="137">
+      <c r="BA91" s="107">
         <v>6.1751790000000003E-3</v>
       </c>
-      <c r="BB91" s="138">
+      <c r="BB91" s="108">
         <f t="shared" si="13"/>
         <v>4.947086823529412E-3</v>
       </c>
-      <c r="BC91" s="139">
+      <c r="BC91" s="109">
         <f t="shared" si="14"/>
         <v>-4.0936405882352944E-4</v>
       </c>
       <c r="BD91" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="BE91" s="148">
+      <c r="BE91" s="118">
         <v>8.3061538000000004E-3</v>
       </c>
-      <c r="BF91" s="149">
+      <c r="BF91" s="119">
         <v>4.6448573999999998E-3</v>
       </c>
-      <c r="BG91" s="144">
+      <c r="BG91" s="114">
         <v>9.4525909999999998E-3</v>
       </c>
-      <c r="BH91" s="145">
+      <c r="BH91" s="115">
         <v>3.9322710000000002E-3</v>
       </c>
-      <c r="BI91" s="146">
+      <c r="BI91" s="116">
         <f t="shared" si="15"/>
         <v>2.9580968823529415E-3</v>
       </c>
-      <c r="BJ91" s="147">
+      <c r="BJ91" s="117">
         <f t="shared" si="16"/>
         <v>-3.2472470588235293E-4</v>
       </c>
@@ -11314,13 +11314,13 @@
       <c r="I92" s="89">
         <v>8.0432449999999992E-3</v>
       </c>
-      <c r="J92" s="128">
+      <c r="J92" s="98">
         <v>1.1498424E-2</v>
       </c>
       <c r="K92" s="85">
         <v>4.6618329999999998E-3</v>
       </c>
-      <c r="L92" s="130">
+      <c r="L92" s="100">
         <f t="shared" si="9"/>
         <v>3.4553757647058821E-3</v>
       </c>
@@ -11355,13 +11355,13 @@
       <c r="V92" s="89">
         <v>5.6773359000000002E-3</v>
       </c>
-      <c r="W92" s="128">
+      <c r="W92" s="98">
         <v>5.9637040000000002E-3</v>
       </c>
-      <c r="X92" s="128">
+      <c r="X92" s="98">
         <v>2.1249369999999999E-3</v>
       </c>
-      <c r="Y92" s="130">
+      <c r="Y92" s="100">
         <f t="shared" si="11"/>
         <v>1.4475075294117646E-3</v>
       </c>
@@ -11372,46 +11372,46 @@
       <c r="AW92" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="AX92" s="140">
+      <c r="AX92" s="110">
         <v>1.4352014999999999E-2</v>
       </c>
-      <c r="AY92" s="141">
+      <c r="AY92" s="111">
         <v>8.0432449999999992E-3</v>
       </c>
-      <c r="AZ92" s="136">
+      <c r="AZ92" s="106">
         <v>1.406663E-2</v>
       </c>
-      <c r="BA92" s="137">
+      <c r="BA92" s="107">
         <v>6.7918839999999998E-3</v>
       </c>
-      <c r="BB92" s="138">
+      <c r="BB92" s="108">
         <f t="shared" si="13"/>
         <v>5.508105294117647E-3</v>
       </c>
-      <c r="BC92" s="139">
+      <c r="BC92" s="109">
         <f t="shared" si="14"/>
         <v>-4.2792623529411765E-4</v>
       </c>
       <c r="BD92" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="BE92" s="148">
+      <c r="BE92" s="118">
         <v>9.5504723999999992E-3</v>
       </c>
-      <c r="BF92" s="149">
+      <c r="BF92" s="119">
         <v>5.6773359000000002E-3</v>
       </c>
-      <c r="BG92" s="144">
+      <c r="BG92" s="114">
         <v>8.6438820000000003E-3</v>
       </c>
-      <c r="BH92" s="145">
+      <c r="BH92" s="115">
         <v>4.1437549999999998E-3</v>
       </c>
-      <c r="BI92" s="146">
+      <c r="BI92" s="116">
         <f t="shared" si="15"/>
         <v>3.3496149411764704E-3</v>
       </c>
-      <c r="BJ92" s="147">
+      <c r="BJ92" s="117">
         <f t="shared" si="16"/>
         <v>-2.6471335294117647E-4</v>
       </c>
@@ -11444,13 +11444,13 @@
       <c r="I93" s="89">
         <v>1.0135829000000001E-2</v>
       </c>
-      <c r="J93" s="128">
+      <c r="J93" s="98">
         <v>1.4937591E-2</v>
       </c>
       <c r="K93" s="85">
         <v>6.616434E-3</v>
       </c>
-      <c r="L93" s="130">
+      <c r="L93" s="100">
         <f t="shared" si="9"/>
         <v>5.1479945294117648E-3</v>
       </c>
@@ -11485,13 +11485,13 @@
       <c r="V93" s="89">
         <v>6.6691631000000001E-3</v>
       </c>
-      <c r="W93" s="128">
+      <c r="W93" s="98">
         <v>6.78533E-3</v>
       </c>
-      <c r="X93" s="128">
+      <c r="X93" s="98">
         <v>3.1711669999999999E-3</v>
       </c>
-      <c r="Y93" s="130">
+      <c r="Y93" s="100">
         <f t="shared" si="11"/>
         <v>2.5333735294117646E-3</v>
       </c>
@@ -11502,46 +11502,46 @@
       <c r="AW93" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="AX93" s="140">
+      <c r="AX93" s="110">
         <v>1.6599328999999999E-2</v>
       </c>
-      <c r="AY93" s="141">
+      <c r="AY93" s="111">
         <v>1.0135829000000001E-2</v>
       </c>
-      <c r="AZ93" s="136">
+      <c r="AZ93" s="106">
         <v>1.7153776999999999E-2</v>
       </c>
-      <c r="BA93" s="137">
+      <c r="BA93" s="107">
         <v>8.8646409999999995E-3</v>
       </c>
-      <c r="BB93" s="138">
+      <c r="BB93" s="108">
         <f t="shared" si="13"/>
         <v>7.4018522941176465E-3</v>
       </c>
-      <c r="BC93" s="139">
+      <c r="BC93" s="109">
         <f t="shared" si="14"/>
         <v>-4.875962352941176E-4</v>
       </c>
       <c r="BD93" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="BE93" s="148">
+      <c r="BE93" s="118">
         <v>1.0526821E-2</v>
       </c>
-      <c r="BF93" s="149">
+      <c r="BF93" s="119">
         <v>6.6691631000000001E-3</v>
       </c>
-      <c r="BG93" s="144">
+      <c r="BG93" s="114">
         <v>9.377191E-3</v>
       </c>
-      <c r="BH93" s="145">
+      <c r="BH93" s="115">
         <v>5.2104229999999996E-3</v>
       </c>
-      <c r="BI93" s="146">
+      <c r="BI93" s="116">
         <f t="shared" si="15"/>
         <v>4.4751109999999995E-3</v>
       </c>
-      <c r="BJ93" s="147">
+      <c r="BJ93" s="117">
         <f t="shared" si="16"/>
         <v>-2.45104E-4</v>
       </c>
@@ -11574,13 +11574,13 @@
       <c r="I94" s="89">
         <v>1.4004198000000001E-2</v>
       </c>
-      <c r="J94" s="128">
+      <c r="J94" s="98">
         <v>2.0927292E-2</v>
       </c>
       <c r="K94" s="85">
         <v>1.0831970999999999E-2</v>
       </c>
-      <c r="L94" s="130">
+      <c r="L94" s="100">
         <f t="shared" si="9"/>
         <v>9.050443764705882E-3</v>
       </c>
@@ -11615,13 +11615,13 @@
       <c r="V94" s="89">
         <v>8.9763412999999993E-3</v>
       </c>
-      <c r="W94" s="128">
+      <c r="W94" s="98">
         <v>9.8414439999999995E-3</v>
       </c>
-      <c r="X94" s="128">
+      <c r="X94" s="98">
         <v>5.1947219999999997E-3</v>
       </c>
-      <c r="Y94" s="130">
+      <c r="Y94" s="100">
         <f t="shared" si="11"/>
         <v>4.3747122352941169E-3</v>
       </c>
@@ -11632,46 +11632,46 @@
       <c r="AW94" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="AX94" s="140">
+      <c r="AX94" s="110">
         <v>2.0610447E-2</v>
       </c>
-      <c r="AY94" s="141">
+      <c r="AY94" s="111">
         <v>1.4004198000000001E-2</v>
       </c>
-      <c r="AZ94" s="136">
+      <c r="AZ94" s="106">
         <v>2.2671103000000001E-2</v>
       </c>
-      <c r="BA94" s="137">
+      <c r="BA94" s="107">
         <v>1.2617975999999999E-2</v>
       </c>
-      <c r="BB94" s="138">
+      <c r="BB94" s="108">
         <f t="shared" si="13"/>
         <v>1.0843894764705882E-2</v>
       </c>
-      <c r="BC94" s="139">
+      <c r="BC94" s="109">
         <f t="shared" si="14"/>
         <v>-5.9136041176470597E-4</v>
       </c>
       <c r="BD94" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="BE94" s="148">
+      <c r="BE94" s="118">
         <v>1.3618289E-2</v>
       </c>
-      <c r="BF94" s="149">
+      <c r="BF94" s="119">
         <v>8.9763412999999993E-3</v>
       </c>
-      <c r="BG94" s="144">
+      <c r="BG94" s="114">
         <v>1.1992486E-2</v>
       </c>
-      <c r="BH94" s="145">
+      <c r="BH94" s="115">
         <v>6.8538840000000002E-3</v>
       </c>
-      <c r="BI94" s="146">
+      <c r="BI94" s="116">
         <f t="shared" si="15"/>
         <v>5.9470718823529415E-3</v>
       </c>
-      <c r="BJ94" s="147">
+      <c r="BJ94" s="117">
         <f t="shared" si="16"/>
         <v>-3.0227070588235294E-4</v>
       </c>
@@ -11704,13 +11704,13 @@
       <c r="I95" s="89">
         <v>1.8576009000000001E-2</v>
       </c>
-      <c r="J95" s="128">
+      <c r="J95" s="98">
         <v>2.6352477999999999E-2</v>
       </c>
       <c r="K95" s="85">
         <v>1.6475909E-2</v>
       </c>
-      <c r="L95" s="130">
+      <c r="L95" s="100">
         <f t="shared" si="9"/>
         <v>1.473298505882353E-2</v>
       </c>
@@ -11745,13 +11745,13 @@
       <c r="V95" s="89">
         <v>1.2049147E-2</v>
       </c>
-      <c r="W95" s="128">
+      <c r="W95" s="98">
         <v>1.3256046E-2</v>
       </c>
-      <c r="X95" s="128">
+      <c r="X95" s="98">
         <v>8.2955149999999998E-3</v>
       </c>
-      <c r="Y95" s="130">
+      <c r="Y95" s="100">
         <f t="shared" si="11"/>
         <v>7.4201271764705885E-3</v>
       </c>
@@ -11762,46 +11762,46 @@
       <c r="AW95" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="AX95" s="140">
+      <c r="AX95" s="110">
         <v>2.5459668000000001E-2</v>
       </c>
-      <c r="AY95" s="141">
+      <c r="AY95" s="111">
         <v>1.8576009000000001E-2</v>
       </c>
-      <c r="AZ95" s="136">
+      <c r="AZ95" s="106">
         <v>2.8196888E-2</v>
       </c>
-      <c r="BA95" s="137">
+      <c r="BA95" s="107">
         <v>1.7883441E-2</v>
       </c>
-      <c r="BB95" s="138">
+      <c r="BB95" s="108">
         <f t="shared" si="13"/>
         <v>1.6063420941176472E-2</v>
       </c>
-      <c r="BC95" s="139">
+      <c r="BC95" s="109">
         <f t="shared" si="14"/>
         <v>-6.0667335294117646E-4</v>
       </c>
       <c r="BD95" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="BE95" s="148">
+      <c r="BE95" s="118">
         <v>1.7990335999999999E-2</v>
       </c>
-      <c r="BF95" s="149">
+      <c r="BF95" s="119">
         <v>1.2049147E-2</v>
       </c>
-      <c r="BG95" s="144">
+      <c r="BG95" s="114">
         <v>1.5297870999999999E-2</v>
       </c>
-      <c r="BH95" s="145">
+      <c r="BH95" s="115">
         <v>9.5655440000000005E-3</v>
       </c>
-      <c r="BI95" s="146">
+      <c r="BI95" s="116">
         <f t="shared" si="15"/>
         <v>8.5539568823529422E-3</v>
       </c>
-      <c r="BJ95" s="147">
+      <c r="BJ95" s="117">
         <f t="shared" si="16"/>
         <v>-3.3719570588235288E-4</v>
       </c>
@@ -11834,13 +11834,13 @@
       <c r="I96" s="89">
         <v>2.7759598999999999E-2</v>
       </c>
-      <c r="J96" s="128">
+      <c r="J96" s="98">
         <v>3.6052813000000003E-2</v>
       </c>
       <c r="K96" s="85">
         <v>2.3964659999999999E-2</v>
       </c>
-      <c r="L96" s="130">
+      <c r="L96" s="100">
         <f t="shared" si="9"/>
         <v>2.1831456529411764E-2</v>
       </c>
@@ -11875,13 +11875,13 @@
       <c r="V96" s="89">
         <v>1.8543285E-2</v>
       </c>
-      <c r="W96" s="128">
+      <c r="W96" s="98">
         <v>1.9917550999999999E-2</v>
       </c>
-      <c r="X96" s="128">
+      <c r="X96" s="98">
         <v>1.2142778999999999E-2</v>
       </c>
-      <c r="Y96" s="130">
+      <c r="Y96" s="100">
         <f t="shared" si="11"/>
         <v>1.0770760411764705E-2</v>
       </c>
@@ -11892,46 +11892,46 @@
       <c r="AW96" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="AX96" s="140">
+      <c r="AX96" s="110">
         <v>3.5184202999999997E-2</v>
       </c>
-      <c r="AY96" s="141">
+      <c r="AY96" s="111">
         <v>2.7759598999999999E-2</v>
       </c>
-      <c r="AZ96" s="136">
+      <c r="AZ96" s="106">
         <v>3.7754171000000003E-2</v>
       </c>
-      <c r="BA96" s="137">
+      <c r="BA96" s="107">
         <v>2.5185233000000001E-2</v>
       </c>
-      <c r="BB96" s="138">
+      <c r="BB96" s="108">
         <f t="shared" si="13"/>
         <v>2.296718511764706E-2</v>
       </c>
-      <c r="BC96" s="139">
+      <c r="BC96" s="109">
         <f t="shared" si="14"/>
         <v>-7.3934929411764716E-4</v>
       </c>
       <c r="BD96" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="BE96" s="148">
+      <c r="BE96" s="118">
         <v>2.7034006999999999E-2</v>
       </c>
-      <c r="BF96" s="149">
+      <c r="BF96" s="119">
         <v>1.8543285E-2</v>
       </c>
-      <c r="BG96" s="144">
+      <c r="BG96" s="114">
         <v>2.1810474999999999E-2</v>
       </c>
-      <c r="BH96" s="145">
+      <c r="BH96" s="115">
         <v>1.3232337E-2</v>
       </c>
-      <c r="BI96" s="146">
+      <c r="BI96" s="116">
         <f t="shared" si="15"/>
         <v>1.1718547941176471E-2</v>
       </c>
-      <c r="BJ96" s="147">
+      <c r="BJ96" s="117">
         <f t="shared" si="16"/>
         <v>-5.0459635294117645E-4</v>
       </c>
@@ -11964,13 +11964,13 @@
       <c r="I97" s="89">
         <v>4.2779603999999999E-2</v>
       </c>
-      <c r="J97" s="128">
+      <c r="J97" s="98">
         <v>4.4857968999999998E-2</v>
       </c>
       <c r="K97" s="85">
         <v>3.3032178000000002E-2</v>
       </c>
-      <c r="L97" s="130">
+      <c r="L97" s="100">
         <f t="shared" si="9"/>
         <v>3.0945273705882355E-2</v>
       </c>
@@ -12005,13 +12005,13 @@
       <c r="V97" s="89">
         <v>3.039122E-2</v>
       </c>
-      <c r="W97" s="128">
+      <c r="W97" s="98">
         <v>2.8481023000000001E-2</v>
       </c>
-      <c r="X97" s="128">
+      <c r="X97" s="98">
         <v>1.7584465000000001E-2</v>
       </c>
-      <c r="Y97" s="130">
+      <c r="Y97" s="100">
         <f t="shared" si="11"/>
         <v>1.5661543E-2</v>
       </c>
@@ -12022,46 +12022,46 @@
       <c r="AW97" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="AX97" s="140">
+      <c r="AX97" s="110">
         <v>5.0578709999999999E-2</v>
       </c>
-      <c r="AY97" s="141">
+      <c r="AY97" s="111">
         <v>4.2779603999999999E-2</v>
       </c>
-      <c r="AZ97" s="136">
+      <c r="AZ97" s="106">
         <v>4.6622128999999998E-2</v>
       </c>
-      <c r="BA97" s="137">
+      <c r="BA97" s="107">
         <v>3.4253349000000002E-2</v>
       </c>
-      <c r="BB97" s="138">
+      <c r="BB97" s="108">
         <f t="shared" si="13"/>
         <v>3.2070623117647065E-2</v>
       </c>
-      <c r="BC97" s="139">
+      <c r="BC97" s="109">
         <f t="shared" si="14"/>
         <v>-7.2757529411764685E-4</v>
       </c>
       <c r="BD97" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="BE97" s="148">
+      <c r="BE97" s="118">
         <v>4.1980367999999997E-2</v>
       </c>
-      <c r="BF97" s="149">
+      <c r="BF97" s="119">
         <v>3.039122E-2</v>
       </c>
-      <c r="BG97" s="144">
+      <c r="BG97" s="114">
         <v>3.0280852E-2</v>
       </c>
-      <c r="BH97" s="145">
+      <c r="BH97" s="115">
         <v>1.8559623000000001E-2</v>
       </c>
-      <c r="BI97" s="146">
+      <c r="BI97" s="116">
         <f t="shared" si="15"/>
         <v>1.6491170823529411E-2</v>
       </c>
-      <c r="BJ97" s="147">
+      <c r="BJ97" s="117">
         <f t="shared" si="16"/>
         <v>-6.8948405882352935E-4</v>
       </c>
@@ -12094,13 +12094,13 @@
       <c r="I98" s="89">
         <v>6.8473476000000005E-2</v>
       </c>
-      <c r="J98" s="128">
+      <c r="J98" s="98">
         <v>6.6115557000000005E-2</v>
       </c>
       <c r="K98" s="85">
         <v>4.3224483000000001E-2</v>
       </c>
-      <c r="L98" s="130">
+      <c r="L98" s="100">
         <f t="shared" si="9"/>
         <v>3.918488170588235E-2</v>
       </c>
@@ -12135,13 +12135,13 @@
       <c r="V98" s="89">
         <v>5.1704121999999998E-2</v>
       </c>
-      <c r="W98" s="128">
+      <c r="W98" s="98">
         <v>4.3469642000000003E-2</v>
       </c>
-      <c r="X98" s="128">
+      <c r="X98" s="98">
         <v>2.5406643E-2</v>
       </c>
-      <c r="Y98" s="130">
+      <c r="Y98" s="100">
         <f t="shared" si="11"/>
         <v>2.2219054941176469E-2</v>
       </c>
@@ -12152,46 +12152,46 @@
       <c r="AW98" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="AX98" s="140">
+      <c r="AX98" s="110">
         <v>7.7074561999999999E-2</v>
       </c>
-      <c r="AY98" s="141">
+      <c r="AY98" s="111">
         <v>6.8473476000000005E-2</v>
       </c>
-      <c r="AZ98" s="136">
+      <c r="AZ98" s="106">
         <v>6.7988487E-2</v>
       </c>
-      <c r="BA98" s="137">
+      <c r="BA98" s="107">
         <v>4.4629888999999999E-2</v>
       </c>
-      <c r="BB98" s="138">
+      <c r="BB98" s="108">
         <f t="shared" si="13"/>
         <v>4.0507783470588234E-2</v>
       </c>
-      <c r="BC98" s="139">
+      <c r="BC98" s="109">
         <f t="shared" si="14"/>
         <v>-1.3740351764705884E-3</v>
       </c>
       <c r="BD98" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="BE98" s="148">
+      <c r="BE98" s="118">
         <v>6.7413652000000004E-2</v>
       </c>
-      <c r="BF98" s="149">
+      <c r="BF98" s="119">
         <v>5.1704121999999998E-2</v>
       </c>
-      <c r="BG98" s="144">
+      <c r="BG98" s="114">
         <v>4.5201616E-2</v>
       </c>
-      <c r="BH98" s="145">
+      <c r="BH98" s="115">
         <v>2.6428843E-2</v>
       </c>
-      <c r="BI98" s="146">
+      <c r="BI98" s="116">
         <f t="shared" si="15"/>
         <v>2.3116000705882354E-2</v>
       </c>
-      <c r="BJ98" s="147">
+      <c r="BJ98" s="117">
         <f t="shared" si="16"/>
         <v>-1.1042807647058824E-3</v>
       </c>
@@ -12224,13 +12224,13 @@
       <c r="I99" s="89">
         <v>0.11201527999999999</v>
       </c>
-      <c r="J99" s="128">
+      <c r="J99" s="98">
         <v>8.1959559000000001E-2</v>
       </c>
       <c r="K99" s="85">
         <v>5.9431375000000002E-2</v>
       </c>
-      <c r="L99" s="130">
+      <c r="L99" s="100">
         <f t="shared" si="9"/>
         <v>5.5455813117647058E-2</v>
       </c>
@@ -12265,13 +12265,13 @@
       <c r="V99" s="89">
         <v>8.8066895000000006E-2</v>
       </c>
-      <c r="W99" s="128">
+      <c r="W99" s="98">
         <v>5.4374656E-2</v>
       </c>
-      <c r="X99" s="128">
+      <c r="X99" s="98">
         <v>3.7231258000000003E-2</v>
       </c>
-      <c r="Y99" s="130">
+      <c r="Y99" s="100">
         <f t="shared" si="11"/>
         <v>3.420595247058824E-2</v>
       </c>
@@ -12282,46 +12282,46 @@
       <c r="AW99" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="AX99" s="140">
+      <c r="AX99" s="110">
         <v>0.11904474</v>
       </c>
-      <c r="AY99" s="141">
+      <c r="AY99" s="111">
         <v>0.11201527999999999</v>
       </c>
-      <c r="AZ99" s="136">
+      <c r="AZ99" s="106">
         <v>8.3893607999999995E-2</v>
       </c>
-      <c r="BA99" s="137">
+      <c r="BA99" s="107">
         <v>6.0996987000000003E-2</v>
       </c>
-      <c r="BB99" s="138">
+      <c r="BB99" s="108">
         <f t="shared" si="13"/>
         <v>5.6956406823529412E-2</v>
       </c>
-      <c r="BC99" s="139">
+      <c r="BC99" s="109">
         <f t="shared" si="14"/>
         <v>-1.346860058823529E-3</v>
       </c>
       <c r="BD99" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="BE99" s="148">
+      <c r="BE99" s="118">
         <v>0.10699243999999999</v>
       </c>
-      <c r="BF99" s="149">
+      <c r="BF99" s="119">
         <v>8.8066895000000006E-2</v>
       </c>
-      <c r="BG99" s="144">
+      <c r="BG99" s="114">
         <v>5.5908607999999999E-2</v>
       </c>
-      <c r="BH99" s="145">
+      <c r="BH99" s="115">
         <v>3.8357005999999999E-2</v>
       </c>
-      <c r="BI99" s="146">
+      <c r="BI99" s="116">
         <f t="shared" si="15"/>
         <v>3.5259664470588231E-2</v>
       </c>
-      <c r="BJ99" s="147">
+      <c r="BJ99" s="117">
         <f t="shared" si="16"/>
         <v>-1.0324471764705883E-3</v>
       </c>
@@ -12516,25 +12516,25 @@
       <c r="X110" s="37"/>
     </row>
     <row r="111" spans="1:62" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="121" t="s">
+      <c r="A111" s="131" t="s">
         <v>100</v>
       </c>
-      <c r="B111" s="121"/>
-      <c r="C111" s="121"/>
-      <c r="D111" s="121"/>
-      <c r="E111" s="121"/>
-      <c r="F111" s="121"/>
-      <c r="G111" s="121"/>
-      <c r="H111" s="121"/>
-      <c r="I111" s="121"/>
-      <c r="J111" s="121"/>
-      <c r="K111" s="121"/>
-      <c r="L111" s="121"/>
-      <c r="M111" s="121"/>
-      <c r="N111" s="121"/>
-      <c r="O111" s="121"/>
-      <c r="P111" s="121"/>
-      <c r="Q111" s="121"/>
+      <c r="B111" s="131"/>
+      <c r="C111" s="131"/>
+      <c r="D111" s="131"/>
+      <c r="E111" s="131"/>
+      <c r="F111" s="131"/>
+      <c r="G111" s="131"/>
+      <c r="H111" s="131"/>
+      <c r="I111" s="131"/>
+      <c r="J111" s="131"/>
+      <c r="K111" s="131"/>
+      <c r="L111" s="131"/>
+      <c r="M111" s="131"/>
+      <c r="N111" s="131"/>
+      <c r="O111" s="131"/>
+      <c r="P111" s="131"/>
+      <c r="Q111" s="131"/>
       <c r="R111" s="37"/>
       <c r="S111" s="37"/>
       <c r="T111" s="37"/>
@@ -12544,17 +12544,17 @@
       <c r="X111" s="37"/>
     </row>
     <row r="112" spans="1:62" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="108" t="s">
+      <c r="A112" s="146" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="104" t="s">
+      <c r="B112" s="143" t="s">
         <v>81</v>
       </c>
-      <c r="C112" s="105"/>
-      <c r="D112" s="105"/>
-      <c r="E112" s="105"/>
-      <c r="F112" s="105"/>
-      <c r="G112" s="106"/>
+      <c r="C112" s="144"/>
+      <c r="D112" s="144"/>
+      <c r="E112" s="144"/>
+      <c r="F112" s="144"/>
+      <c r="G112" s="145"/>
       <c r="I112" s="68"/>
       <c r="J112" s="79" t="s">
         <v>27</v>
@@ -12573,7 +12573,7 @@
       </c>
     </row>
     <row r="113" spans="1:14" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="109"/>
+      <c r="A113" s="147"/>
       <c r="B113" s="32" t="s">
         <v>68</v>
       </c>
@@ -12617,7 +12617,7 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="110"/>
+      <c r="A114" s="148"/>
       <c r="B114" s="34" t="s">
         <v>61</v>
       </c>
@@ -12665,14 +12665,14 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="I115" s="117" t="s">
+      <c r="I115" s="137" t="s">
         <v>99</v>
       </c>
-      <c r="J115" s="117"/>
-      <c r="K115" s="117"/>
-      <c r="L115" s="117"/>
-      <c r="M115" s="117"/>
-      <c r="N115" s="117"/>
+      <c r="J115" s="137"/>
+      <c r="K115" s="137"/>
+      <c r="L115" s="137"/>
+      <c r="M115" s="137"/>
+      <c r="N115" s="137"/>
     </row>
     <row r="116" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
@@ -13425,31 +13425,31 @@
     </row>
     <row r="132" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="133" spans="1:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="101" t="s">
+      <c r="A133" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="104" t="s">
+      <c r="B133" s="143" t="s">
         <v>82</v>
       </c>
-      <c r="C133" s="105"/>
-      <c r="D133" s="105"/>
-      <c r="E133" s="105"/>
-      <c r="F133" s="105"/>
-      <c r="G133" s="106"/>
-      <c r="I133" s="101" t="s">
+      <c r="C133" s="144"/>
+      <c r="D133" s="144"/>
+      <c r="E133" s="144"/>
+      <c r="F133" s="144"/>
+      <c r="G133" s="145"/>
+      <c r="I133" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="J133" s="104" t="s">
+      <c r="J133" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="K133" s="105"/>
-      <c r="L133" s="105"/>
-      <c r="M133" s="105"/>
-      <c r="N133" s="105"/>
-      <c r="O133" s="106"/>
+      <c r="K133" s="144"/>
+      <c r="L133" s="144"/>
+      <c r="M133" s="144"/>
+      <c r="N133" s="144"/>
+      <c r="O133" s="145"/>
     </row>
     <row r="134" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="102"/>
+      <c r="A134" s="141"/>
       <c r="B134" s="26" t="s">
         <v>69</v>
       </c>
@@ -13468,7 +13468,7 @@
       <c r="G134" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I134" s="102"/>
+      <c r="I134" s="141"/>
       <c r="J134" s="26" t="s">
         <v>69</v>
       </c>
@@ -13489,7 +13489,7 @@
       </c>
     </row>
     <row r="135" spans="1:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="103"/>
+      <c r="A135" s="142"/>
       <c r="B135" s="40" t="s">
         <v>61</v>
       </c>
@@ -13508,7 +13508,7 @@
       <c r="G135" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="I135" s="103"/>
+      <c r="I135" s="142"/>
       <c r="J135" s="40" t="s">
         <v>61</v>
       </c>
@@ -13665,55 +13665,55 @@
         <v>13</v>
       </c>
       <c r="B139" s="17">
-        <f>B118*0.36</f>
-        <v>5.59944E-2</v>
+        <f>B118*0.37</f>
+        <v>5.7549800000000005E-2</v>
       </c>
       <c r="C139" s="17">
-        <f t="shared" ref="C139:G139" si="20">C118*0.36</f>
-        <v>5.59944E-2</v>
+        <f t="shared" ref="C139:G139" si="20">C118*0.37</f>
+        <v>5.7549800000000005E-2</v>
       </c>
       <c r="D139" s="17">
         <f t="shared" si="20"/>
-        <v>5.59944E-2</v>
+        <v>5.7549800000000005E-2</v>
       </c>
       <c r="E139" s="17">
         <f t="shared" si="20"/>
-        <v>3.2476752000000005E-2</v>
+        <v>3.3378884000000004E-2</v>
       </c>
       <c r="F139" s="17">
         <f t="shared" si="20"/>
-        <v>3.2476752000000005E-2</v>
+        <v>3.3378884000000004E-2</v>
       </c>
       <c r="G139" s="17">
         <f t="shared" si="20"/>
-        <v>2.2957704000000002E-2</v>
+        <v>2.3595418000000003E-2</v>
       </c>
       <c r="I139" s="46" t="s">
         <v>13</v>
       </c>
       <c r="J139" s="17">
-        <f>B139*0.7</f>
-        <v>3.9196079999999994E-2</v>
+        <f>B139*0.75</f>
+        <v>4.3162350000000002E-2</v>
       </c>
       <c r="K139" s="17">
-        <f t="shared" ref="K139:O139" si="21">C139*0.7</f>
-        <v>3.9196079999999994E-2</v>
+        <f t="shared" ref="K139:O139" si="21">C139*0.75</f>
+        <v>4.3162350000000002E-2</v>
       </c>
       <c r="L139" s="17">
         <f t="shared" si="21"/>
-        <v>3.9196079999999994E-2</v>
+        <v>4.3162350000000002E-2</v>
       </c>
       <c r="M139" s="17">
         <f t="shared" si="21"/>
-        <v>2.2733726400000001E-2</v>
+        <v>2.5034163000000005E-2</v>
       </c>
       <c r="N139" s="17">
         <f t="shared" si="21"/>
-        <v>2.2733726400000001E-2</v>
+        <v>2.5034163000000005E-2</v>
       </c>
       <c r="O139" s="17">
         <f t="shared" si="21"/>
-        <v>1.60703928E-2</v>
+        <v>1.7696563500000002E-2</v>
       </c>
     </row>
     <row r="140" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -13721,55 +13721,55 @@
         <v>14</v>
       </c>
       <c r="B140" s="17">
-        <f t="shared" ref="B140:G140" si="22">B119*0.36</f>
-        <v>0.11008800000000002</v>
+        <f t="shared" ref="B140:G140" si="22">B119*0.37</f>
+        <v>0.11314600000000002</v>
       </c>
       <c r="C140" s="17">
         <f t="shared" si="22"/>
-        <v>0.11008800000000002</v>
+        <v>0.11314600000000002</v>
       </c>
       <c r="D140" s="17">
         <f t="shared" si="22"/>
-        <v>0.11008800000000002</v>
+        <v>0.11314600000000002</v>
       </c>
       <c r="E140" s="17">
         <f t="shared" si="22"/>
-        <v>6.3851040000000012E-2</v>
+        <v>6.5624680000000019E-2</v>
       </c>
       <c r="F140" s="17">
         <f t="shared" si="22"/>
-        <v>6.3851040000000012E-2</v>
+        <v>6.5624680000000019E-2</v>
       </c>
       <c r="G140" s="17">
         <f t="shared" si="22"/>
-        <v>4.5136080000000016E-2</v>
+        <v>4.6389860000000019E-2</v>
       </c>
       <c r="I140" s="46" t="s">
         <v>14</v>
       </c>
       <c r="J140" s="17">
-        <f t="shared" ref="J140:J145" si="23">B140*0.7</f>
-        <v>7.7061600000000008E-2</v>
+        <f t="shared" ref="J140:J145" si="23">B140*0.75</f>
+        <v>8.4859500000000018E-2</v>
       </c>
       <c r="K140" s="17">
-        <f t="shared" ref="K140:K145" si="24">C140*0.7</f>
-        <v>7.7061600000000008E-2</v>
+        <f t="shared" ref="K140:K145" si="24">C140*0.75</f>
+        <v>8.4859500000000018E-2</v>
       </c>
       <c r="L140" s="17">
-        <f t="shared" ref="L140:L145" si="25">D140*0.7</f>
-        <v>7.7061600000000008E-2</v>
+        <f t="shared" ref="L140:L145" si="25">D140*0.75</f>
+        <v>8.4859500000000018E-2</v>
       </c>
       <c r="M140" s="17">
-        <f t="shared" ref="M140:M145" si="26">E140*0.7</f>
-        <v>4.4695728000000004E-2</v>
+        <f t="shared" ref="M140:M145" si="26">E140*0.75</f>
+        <v>4.9218510000000014E-2</v>
       </c>
       <c r="N140" s="17">
-        <f t="shared" ref="N140:N145" si="27">F140*0.7</f>
-        <v>4.4695728000000004E-2</v>
+        <f t="shared" ref="N140:N145" si="27">F140*0.75</f>
+        <v>4.9218510000000014E-2</v>
       </c>
       <c r="O140" s="17">
-        <f t="shared" ref="O140:O145" si="28">G140*0.7</f>
-        <v>3.1595256000000009E-2</v>
+        <f t="shared" ref="O140:O145" si="28">G140*0.75</f>
+        <v>3.4792395000000018E-2</v>
       </c>
     </row>
     <row r="141" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -13777,55 +13777,55 @@
         <v>15</v>
       </c>
       <c r="B141" s="17">
-        <f t="shared" ref="B141:G141" si="29">B120*0.36</f>
-        <v>0.11230560000000002</v>
+        <f t="shared" ref="B141:G141" si="29">B120*0.37</f>
+        <v>0.11542520000000002</v>
       </c>
       <c r="C141" s="17">
         <f t="shared" si="29"/>
-        <v>0.11230560000000002</v>
+        <v>0.11542520000000002</v>
       </c>
       <c r="D141" s="17">
         <f t="shared" si="29"/>
-        <v>0.11230560000000002</v>
+        <v>0.11542520000000002</v>
       </c>
       <c r="E141" s="17">
         <f t="shared" si="29"/>
-        <v>6.5137248000000009E-2</v>
+        <v>6.6946616000000014E-2</v>
       </c>
       <c r="F141" s="17">
         <f t="shared" si="29"/>
-        <v>6.5137248000000009E-2</v>
+        <v>6.6946616000000014E-2</v>
       </c>
       <c r="G141" s="17">
         <f t="shared" si="29"/>
-        <v>4.6045296000000013E-2</v>
+        <v>4.7324332000000011E-2</v>
       </c>
       <c r="I141" s="46" t="s">
         <v>15</v>
       </c>
       <c r="J141" s="17">
         <f t="shared" si="23"/>
-        <v>7.8613920000000004E-2</v>
+        <v>8.6568900000000018E-2</v>
       </c>
       <c r="K141" s="17">
         <f t="shared" si="24"/>
-        <v>7.8613920000000004E-2</v>
+        <v>8.6568900000000018E-2</v>
       </c>
       <c r="L141" s="17">
         <f t="shared" si="25"/>
-        <v>7.8613920000000004E-2</v>
+        <v>8.6568900000000018E-2</v>
       </c>
       <c r="M141" s="17">
         <f t="shared" si="26"/>
-        <v>4.5596073600000002E-2</v>
+        <v>5.0209962000000011E-2</v>
       </c>
       <c r="N141" s="17">
         <f t="shared" si="27"/>
-        <v>4.5596073600000002E-2</v>
+        <v>5.0209962000000011E-2</v>
       </c>
       <c r="O141" s="17">
         <f t="shared" si="28"/>
-        <v>3.2231707200000008E-2</v>
+        <v>3.5493249000000004E-2</v>
       </c>
     </row>
     <row r="142" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -13833,55 +13833,55 @@
         <v>18</v>
       </c>
       <c r="B142" s="17">
-        <f t="shared" ref="B142:G142" si="30">B121*0.36</f>
-        <v>8.3635200000000007E-2</v>
+        <f t="shared" ref="B142:G142" si="30">B121*0.37</f>
+        <v>8.5958400000000004E-2</v>
       </c>
       <c r="C142" s="17">
         <f t="shared" si="30"/>
-        <v>8.3635200000000007E-2</v>
+        <v>8.5958400000000004E-2</v>
       </c>
       <c r="D142" s="17">
         <f t="shared" si="30"/>
-        <v>8.3635200000000007E-2</v>
+        <v>8.5958400000000004E-2</v>
       </c>
       <c r="E142" s="17">
         <f t="shared" si="30"/>
-        <v>4.8508416000000006E-2</v>
+        <v>4.9855872000000009E-2</v>
       </c>
       <c r="F142" s="17">
         <f t="shared" si="30"/>
-        <v>4.8508416000000006E-2</v>
+        <v>4.9855872000000009E-2</v>
       </c>
       <c r="G142" s="17">
         <f t="shared" si="30"/>
-        <v>3.4290432000000003E-2</v>
+        <v>3.5242944000000005E-2</v>
       </c>
       <c r="I142" s="46" t="s">
         <v>18</v>
       </c>
       <c r="J142" s="17">
         <f t="shared" si="23"/>
-        <v>5.8544640000000002E-2</v>
+        <v>6.4468800000000007E-2</v>
       </c>
       <c r="K142" s="17">
         <f t="shared" si="24"/>
-        <v>5.8544640000000002E-2</v>
+        <v>6.4468800000000007E-2</v>
       </c>
       <c r="L142" s="17">
         <f t="shared" si="25"/>
-        <v>5.8544640000000002E-2</v>
+        <v>6.4468800000000007E-2</v>
       </c>
       <c r="M142" s="17">
         <f t="shared" si="26"/>
-        <v>3.3955891200000005E-2</v>
+        <v>3.7391904000000004E-2</v>
       </c>
       <c r="N142" s="17">
         <f t="shared" si="27"/>
-        <v>3.3955891200000005E-2</v>
+        <v>3.7391904000000004E-2</v>
       </c>
       <c r="O142" s="17">
         <f t="shared" si="28"/>
-        <v>2.4003302399999999E-2</v>
+        <v>2.6432208000000006E-2</v>
       </c>
     </row>
     <row r="143" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -13889,55 +13889,55 @@
         <v>17</v>
       </c>
       <c r="B143" s="17">
-        <f t="shared" ref="B143:G143" si="31">B122*0.36</f>
-        <v>5.3380800000000006E-2</v>
+        <f t="shared" ref="B143:G143" si="31">B122*0.37</f>
+        <v>5.4863600000000005E-2</v>
       </c>
       <c r="C143" s="17">
         <f t="shared" si="31"/>
-        <v>5.3380800000000006E-2</v>
+        <v>5.4863600000000005E-2</v>
       </c>
       <c r="D143" s="17">
         <f t="shared" si="31"/>
-        <v>5.3380800000000006E-2</v>
+        <v>5.4863600000000005E-2</v>
       </c>
       <c r="E143" s="17">
         <f t="shared" si="31"/>
-        <v>3.0960864000000005E-2</v>
+        <v>3.1820888000000006E-2</v>
       </c>
       <c r="F143" s="17">
         <f t="shared" si="31"/>
-        <v>3.0960864000000005E-2</v>
+        <v>3.1820888000000006E-2</v>
       </c>
       <c r="G143" s="17">
         <f t="shared" si="31"/>
-        <v>2.1886128000000001E-2</v>
+        <v>2.2494076000000002E-2</v>
       </c>
       <c r="I143" s="46" t="s">
         <v>17</v>
       </c>
       <c r="J143" s="17">
         <f t="shared" si="23"/>
-        <v>3.736656E-2</v>
+        <v>4.1147700000000002E-2</v>
       </c>
       <c r="K143" s="17">
         <f t="shared" si="24"/>
-        <v>3.736656E-2</v>
+        <v>4.1147700000000002E-2</v>
       </c>
       <c r="L143" s="17">
         <f t="shared" si="25"/>
-        <v>3.736656E-2</v>
+        <v>4.1147700000000002E-2</v>
       </c>
       <c r="M143" s="17">
         <f t="shared" si="26"/>
-        <v>2.1672604800000002E-2</v>
+        <v>2.3865666000000004E-2</v>
       </c>
       <c r="N143" s="17">
         <f t="shared" si="27"/>
-        <v>2.1672604800000002E-2</v>
+        <v>2.3865666000000004E-2</v>
       </c>
       <c r="O143" s="17">
         <f t="shared" si="28"/>
-        <v>1.53202896E-2</v>
+        <v>1.6870557000000001E-2</v>
       </c>
     </row>
     <row r="144" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -13945,55 +13945,55 @@
         <v>19</v>
       </c>
       <c r="B144" s="17">
-        <f t="shared" ref="B144:G144" si="32">B123*0.36</f>
-        <v>2.1463200000000005E-2</v>
+        <f t="shared" ref="B144:G144" si="32">B123*0.37</f>
+        <v>2.2059400000000003E-2</v>
       </c>
       <c r="C144" s="17">
         <f t="shared" si="32"/>
-        <v>2.1463200000000005E-2</v>
+        <v>2.2059400000000003E-2</v>
       </c>
       <c r="D144" s="17">
         <f t="shared" si="32"/>
-        <v>2.1463200000000005E-2</v>
+        <v>2.2059400000000003E-2</v>
       </c>
       <c r="E144" s="17">
         <f t="shared" si="32"/>
-        <v>1.2448656000000002E-2</v>
+        <v>1.2794452000000003E-2</v>
       </c>
       <c r="F144" s="17">
         <f t="shared" si="32"/>
-        <v>1.2448656000000002E-2</v>
+        <v>1.2794452000000003E-2</v>
       </c>
       <c r="G144" s="17">
         <f t="shared" si="32"/>
-        <v>8.799912E-3</v>
+        <v>9.044354000000001E-3</v>
       </c>
       <c r="I144" s="46" t="s">
         <v>19</v>
       </c>
       <c r="J144" s="17">
         <f t="shared" si="23"/>
-        <v>1.5024240000000003E-2</v>
+        <v>1.6544550000000002E-2</v>
       </c>
       <c r="K144" s="17">
         <f t="shared" si="24"/>
-        <v>1.5024240000000003E-2</v>
+        <v>1.6544550000000002E-2</v>
       </c>
       <c r="L144" s="17">
         <f t="shared" si="25"/>
-        <v>1.5024240000000003E-2</v>
+        <v>1.6544550000000002E-2</v>
       </c>
       <c r="M144" s="17">
         <f t="shared" si="26"/>
-        <v>8.7140592000000006E-3</v>
+        <v>9.5958390000000018E-3</v>
       </c>
       <c r="N144" s="17">
         <f t="shared" si="27"/>
-        <v>8.7140592000000006E-3</v>
+        <v>9.5958390000000018E-3</v>
       </c>
       <c r="O144" s="17">
         <f t="shared" si="28"/>
-        <v>6.1599383999999995E-3</v>
+        <v>6.7832655000000007E-3</v>
       </c>
     </row>
     <row r="145" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -14001,55 +14001,55 @@
         <v>20</v>
       </c>
       <c r="B145" s="17">
-        <f t="shared" ref="B145:G145" si="33">B124*0.36</f>
-        <v>6.9696000000000003E-3</v>
+        <f t="shared" ref="B145:G145" si="33">B124*0.37</f>
+        <v>7.1632000000000006E-3</v>
       </c>
       <c r="C145" s="17">
         <f t="shared" si="33"/>
-        <v>6.9696000000000003E-3</v>
+        <v>7.1632000000000006E-3</v>
       </c>
       <c r="D145" s="17">
         <f t="shared" si="33"/>
-        <v>6.9696000000000003E-3</v>
+        <v>7.1632000000000006E-3</v>
       </c>
       <c r="E145" s="17">
         <f t="shared" si="33"/>
-        <v>4.042368000000001E-3</v>
+        <v>4.1546560000000005E-3</v>
       </c>
       <c r="F145" s="17">
         <f t="shared" si="33"/>
-        <v>4.042368000000001E-3</v>
+        <v>4.1546560000000005E-3</v>
       </c>
       <c r="G145" s="17">
         <f t="shared" si="33"/>
-        <v>2.8575360000000004E-3</v>
+        <v>2.9369120000000003E-3</v>
       </c>
       <c r="I145" s="46" t="s">
         <v>20</v>
       </c>
       <c r="J145" s="17">
         <f t="shared" si="23"/>
-        <v>4.8787199999999996E-3</v>
+        <v>5.3724000000000003E-3</v>
       </c>
       <c r="K145" s="17">
         <f t="shared" si="24"/>
-        <v>4.8787199999999996E-3</v>
+        <v>5.3724000000000003E-3</v>
       </c>
       <c r="L145" s="17">
         <f t="shared" si="25"/>
-        <v>4.8787199999999996E-3</v>
+        <v>5.3724000000000003E-3</v>
       </c>
       <c r="M145" s="17">
         <f t="shared" si="26"/>
-        <v>2.8296576000000004E-3</v>
+        <v>3.1159920000000006E-3</v>
       </c>
       <c r="N145" s="17">
         <f t="shared" si="27"/>
-        <v>2.8296576000000004E-3</v>
+        <v>3.1159920000000006E-3</v>
       </c>
       <c r="O145" s="17">
         <f t="shared" si="28"/>
-        <v>2.0002752000000002E-3</v>
+        <v>2.2026840000000003E-3</v>
       </c>
     </row>
     <row r="146" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -14319,51 +14319,51 @@
     <row r="152" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B152">
         <f t="shared" ref="B152:G152" si="34">5*SUM(B136:B151)</f>
-        <v>2.2191840000000003</v>
+        <v>2.2808280000000005</v>
       </c>
       <c r="C152">
         <f t="shared" si="34"/>
-        <v>2.2191840000000003</v>
+        <v>2.2808280000000005</v>
       </c>
       <c r="D152">
         <f t="shared" si="34"/>
-        <v>2.2191840000000003</v>
+        <v>2.2808280000000005</v>
       </c>
       <c r="E152">
         <f t="shared" si="34"/>
-        <v>1.2871267200000003</v>
+        <v>1.3228802399999999</v>
       </c>
       <c r="F152">
         <f t="shared" si="34"/>
-        <v>1.2871267200000003</v>
+        <v>1.3228802399999999</v>
       </c>
       <c r="G152">
         <f t="shared" si="34"/>
-        <v>0.90986544000000014</v>
+        <v>0.93513948000000024</v>
       </c>
       <c r="J152">
         <f t="shared" ref="J152:O152" si="35">5*SUM(J136:J151)</f>
-        <v>1.5534288000000003</v>
+        <v>1.7106210000000002</v>
       </c>
       <c r="K152">
         <f t="shared" si="35"/>
-        <v>1.5534288000000003</v>
+        <v>1.7106210000000002</v>
       </c>
       <c r="L152">
         <f t="shared" si="35"/>
-        <v>1.5534288000000003</v>
+        <v>1.7106210000000002</v>
       </c>
       <c r="M152">
         <f t="shared" si="35"/>
-        <v>0.9009887040000002</v>
+        <v>0.99216018000000017</v>
       </c>
       <c r="N152">
         <f t="shared" si="35"/>
-        <v>0.9009887040000002</v>
+        <v>0.99216018000000017</v>
       </c>
       <c r="O152">
         <f t="shared" si="35"/>
-        <v>0.63690580800000007</v>
+        <v>0.70135461000000021</v>
       </c>
     </row>
     <row r="158" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
@@ -14448,22 +14448,22 @@
       <c r="W160" s="37"/>
     </row>
     <row r="161" spans="1:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="98" t="s">
+      <c r="A161" s="123" t="s">
         <v>86</v>
       </c>
-      <c r="B161" s="122" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="122"/>
-      <c r="D161" s="122"/>
-      <c r="E161" s="122" t="s">
+      <c r="B161" s="133" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="133"/>
+      <c r="D161" s="133"/>
+      <c r="E161" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="F161" s="122"/>
-      <c r="G161" s="122"/>
+      <c r="F161" s="133"/>
+      <c r="G161" s="133"/>
     </row>
     <row r="162" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="98"/>
+      <c r="A162" s="123"/>
       <c r="B162" s="58" t="s">
         <v>3</v>
       </c>
@@ -15313,9 +15313,9 @@
       <c r="AB185" s="20"/>
     </row>
     <row r="186" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="123"/>
-      <c r="B186" s="123"/>
-      <c r="C186" s="123"/>
+      <c r="A186" s="134"/>
+      <c r="B186" s="134"/>
+      <c r="C186" s="134"/>
       <c r="D186" s="20"/>
       <c r="E186" s="20"/>
       <c r="F186" s="20"/>
@@ -15490,37 +15490,37 @@
       <c r="W197" s="37"/>
     </row>
     <row r="198" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="111" t="s">
+      <c r="A198" s="129" t="s">
         <v>71</v>
       </c>
-      <c r="B198" s="111"/>
-      <c r="C198" s="111"/>
-      <c r="D198" s="111"/>
+      <c r="B198" s="129"/>
+      <c r="C198" s="129"/>
+      <c r="D198" s="129"/>
       <c r="E198" s="95"/>
       <c r="F198" s="95"/>
     </row>
     <row r="199" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="111" t="s">
+      <c r="A199" s="129" t="s">
         <v>72</v>
       </c>
-      <c r="B199" s="111"/>
-      <c r="C199" s="111"/>
-      <c r="D199" s="111"/>
+      <c r="B199" s="129"/>
+      <c r="C199" s="129"/>
+      <c r="D199" s="129"/>
       <c r="E199" s="95"/>
       <c r="F199" s="95"/>
     </row>
     <row r="200" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A200" s="107" t="s">
+      <c r="A200" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="B200" s="107" t="s">
+      <c r="B200" s="135" t="s">
         <v>49</v>
       </c>
-      <c r="C200" s="107"/>
-      <c r="D200" s="107"/>
+      <c r="C200" s="135"/>
+      <c r="D200" s="135"/>
     </row>
     <row r="201" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A201" s="107"/>
+      <c r="A201" s="135"/>
       <c r="B201" s="43" t="s">
         <v>46</v>
       </c>
@@ -15558,11 +15558,11 @@
       <c r="I202" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="J202" s="120" t="s">
+      <c r="J202" s="138" t="s">
         <v>90</v>
       </c>
-      <c r="K202" s="120"/>
-      <c r="L202" s="120"/>
+      <c r="K202" s="138"/>
+      <c r="L202" s="138"/>
     </row>
     <row r="203" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="44" t="s">
@@ -16179,27 +16179,27 @@
       </c>
     </row>
     <row r="219" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="99" t="s">
+      <c r="A219" s="132" t="s">
         <v>73</v>
       </c>
-      <c r="B219" s="99"/>
-      <c r="C219" s="99"/>
-      <c r="D219" s="99"/>
+      <c r="B219" s="132"/>
+      <c r="C219" s="132"/>
+      <c r="D219" s="132"/>
       <c r="E219" s="96"/>
     </row>
     <row r="220" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A220" s="99" t="s">
+      <c r="A220" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="B220" s="107" t="s">
+      <c r="B220" s="135" t="s">
         <v>49</v>
       </c>
-      <c r="C220" s="107"/>
-      <c r="D220" s="107"/>
+      <c r="C220" s="135"/>
+      <c r="D220" s="135"/>
       <c r="E220" s="25"/>
     </row>
     <row r="221" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A221" s="99"/>
+      <c r="A221" s="132"/>
       <c r="B221" s="43" t="s">
         <v>46</v>
       </c>
@@ -16238,11 +16238,11 @@
       <c r="I222" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="J222" s="120" t="s">
+      <c r="J222" s="138" t="s">
         <v>89</v>
       </c>
-      <c r="K222" s="120"/>
-      <c r="L222" s="120"/>
+      <c r="K222" s="138"/>
+      <c r="L222" s="138"/>
     </row>
     <row r="223" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="44" t="s">
@@ -16905,30 +16905,7 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="AW81:AW83"/>
-    <mergeCell ref="AX81:BB82"/>
-    <mergeCell ref="BD81:BD83"/>
-    <mergeCell ref="BE81:BI82"/>
-    <mergeCell ref="AA87:AA88"/>
-    <mergeCell ref="AA81:AI81"/>
-    <mergeCell ref="AB82:AI82"/>
-    <mergeCell ref="AB87:AI87"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A111:Q111"/>
-    <mergeCell ref="N81:N83"/>
-    <mergeCell ref="B81:L82"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="E161:G161"/>
-    <mergeCell ref="A186:C186"/>
-    <mergeCell ref="B200:D200"/>
-    <mergeCell ref="B220:D220"/>
-    <mergeCell ref="A198:D198"/>
-    <mergeCell ref="A199:D199"/>
-    <mergeCell ref="A80:X80"/>
-    <mergeCell ref="I115:N115"/>
-    <mergeCell ref="O81:Y82"/>
-    <mergeCell ref="AA82:AA83"/>
+    <mergeCell ref="A81:A83"/>
     <mergeCell ref="J222:L222"/>
     <mergeCell ref="J202:L202"/>
     <mergeCell ref="A161:A162"/>
@@ -16945,8 +16922,31 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="B52:D52"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A111:Q111"/>
+    <mergeCell ref="N81:N83"/>
+    <mergeCell ref="B81:L82"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="E161:G161"/>
+    <mergeCell ref="A186:C186"/>
+    <mergeCell ref="B200:D200"/>
+    <mergeCell ref="B220:D220"/>
+    <mergeCell ref="A198:D198"/>
+    <mergeCell ref="A199:D199"/>
+    <mergeCell ref="A80:X80"/>
+    <mergeCell ref="I115:N115"/>
+    <mergeCell ref="O81:Y82"/>
     <mergeCell ref="E52:G52"/>
-    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="AW81:AW83"/>
+    <mergeCell ref="AX81:BB82"/>
+    <mergeCell ref="BD81:BD83"/>
+    <mergeCell ref="BE81:BI82"/>
+    <mergeCell ref="AA87:AA88"/>
+    <mergeCell ref="AA81:AI81"/>
+    <mergeCell ref="AB82:AI82"/>
+    <mergeCell ref="AB87:AI87"/>
+    <mergeCell ref="AA82:AA83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Excel description of partnership data
</commit_message>
<xml_diff>
--- a/Config/Population_data.xlsx
+++ b/Config/Population_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="107">
   <si>
     <t>Male</t>
   </si>
@@ -315,9 +315,6 @@
     </r>
   </si>
   <si>
-    <t>Note: No females were found to be in the high risk group for age 30-34. No males or females were found to be in the high risk groups for ages 45-79. As such, members of the high risk groups in these age groups were assumed to contribute minimally to contact patterns and were assigned one partner per year.</t>
-  </si>
-  <si>
     <t>Coital acts per partnership</t>
   </si>
   <si>
@@ -382,27 +379,6 @@
   </si>
   <si>
     <t>Partnerships per year</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Annual number of sexual partnerships by age, gender, and sexual risk. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Values are based on Africa Centre data from KwaZulu Natal, South Africa but have been adjusted.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -498,6 +474,27 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve"> Calculate backward-projected KZN population. Assume that KZN:SA proportion was decreasing from 1925-2002 according to a slightly steeper trend than that seen from 2002-2019. Assume male and female populations by age follow exponential distributions. See Population_validation Excel document for more detail.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Annual number of sexual partnerships by age, gender, and sexual risk. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Values are based on Africa Centre data from KwaZulu Natal, South Africa but have been calibrated to fit age-specific HIV and HPV prevalence data.</t>
     </r>
   </si>
 </sst>
@@ -1704,6 +1701,10 @@
     <xf numFmtId="168" fontId="8" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1713,14 +1714,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1761,11 +1777,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1773,28 +1792,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -8276,8 +8273,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BJ245"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8332,7 +8329,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -8360,16 +8357,16 @@
       <c r="Y1" s="37"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="125" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
-      <c r="H2" s="125"/>
+      <c r="A2" s="132" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="132"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
       <c r="K2" s="37"/>
@@ -8390,7 +8387,7 @@
     </row>
     <row r="3" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
@@ -8421,14 +8418,14 @@
       <c r="A4" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="136" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="137"/>
-      <c r="D4" s="136" t="s">
+      <c r="B4" s="143" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="144"/>
+      <c r="D4" s="143" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="137"/>
+      <c r="E4" s="144"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
@@ -8457,11 +8454,11 @@
       <c r="C6" s="49">
         <v>234.48412029553555</v>
       </c>
-      <c r="D6" s="149">
+      <c r="D6" s="119">
         <f>B6*1000</f>
         <v>232193.22062680181</v>
       </c>
-      <c r="E6" s="149">
+      <c r="E6" s="119">
         <f>C6*1000</f>
         <v>234484.12029553554</v>
       </c>
@@ -8480,11 +8477,11 @@
       <c r="C7" s="49">
         <v>163.17386739175186</v>
       </c>
-      <c r="D7" s="149">
+      <c r="D7" s="119">
         <f t="shared" ref="D7:D21" si="0">B7*1000</f>
         <v>159981.19086849148</v>
       </c>
-      <c r="E7" s="149">
+      <c r="E7" s="119">
         <f t="shared" ref="E7:E21" si="1">C7*1000</f>
         <v>163173.86739175185</v>
       </c>
@@ -8503,11 +8500,11 @@
       <c r="C8" s="49">
         <v>133.15632309972767</v>
       </c>
-      <c r="D8" s="149">
+      <c r="D8" s="119">
         <f t="shared" si="0"/>
         <v>130604.16798656604</v>
       </c>
-      <c r="E8" s="149">
+      <c r="E8" s="119">
         <f t="shared" si="1"/>
         <v>133156.32309972768</v>
       </c>
@@ -8526,11 +8523,11 @@
       <c r="C9" s="49">
         <v>114.32167152989602</v>
       </c>
-      <c r="D9" s="149">
+      <c r="D9" s="119">
         <f t="shared" si="0"/>
         <v>116663.80924930885</v>
       </c>
-      <c r="E9" s="149">
+      <c r="E9" s="119">
         <f t="shared" si="1"/>
         <v>114321.67152989602</v>
       </c>
@@ -8549,11 +8546,11 @@
       <c r="C10" s="49">
         <v>99.000049567582792</v>
       </c>
-      <c r="D10" s="149">
+      <c r="D10" s="119">
         <f t="shared" si="0"/>
         <v>105384.52275663237</v>
       </c>
-      <c r="E10" s="149">
+      <c r="E10" s="119">
         <f t="shared" si="1"/>
         <v>99000.049567582799</v>
       </c>
@@ -8572,11 +8569,11 @@
       <c r="C11" s="49">
         <v>87.233488605604208</v>
       </c>
-      <c r="D11" s="149">
+      <c r="D11" s="119">
         <f t="shared" si="0"/>
         <v>95487.192629204481</v>
       </c>
-      <c r="E11" s="149">
+      <c r="E11" s="119">
         <f t="shared" si="1"/>
         <v>87233.488605604201</v>
       </c>
@@ -8595,11 +8592,11 @@
       <c r="C12" s="49">
         <v>80.038973435362465</v>
       </c>
-      <c r="D12" s="149">
+      <c r="D12" s="119">
         <f t="shared" si="0"/>
         <v>88295.901522314613</v>
       </c>
-      <c r="E12" s="149">
+      <c r="E12" s="119">
         <f t="shared" si="1"/>
         <v>80038.973435362466</v>
       </c>
@@ -8618,11 +8615,11 @@
       <c r="C13" s="49">
         <v>71.997696512421896</v>
       </c>
-      <c r="D13" s="149">
+      <c r="D13" s="119">
         <f t="shared" si="0"/>
         <v>81236.378677701534</v>
       </c>
-      <c r="E13" s="149">
+      <c r="E13" s="119">
         <f t="shared" si="1"/>
         <v>71997.696512421899</v>
       </c>
@@ -8641,11 +8638,11 @@
       <c r="C14" s="49">
         <v>65.881136053851193</v>
       </c>
-      <c r="D14" s="149">
+      <c r="D14" s="119">
         <f t="shared" si="0"/>
         <v>73180.407288058326</v>
       </c>
-      <c r="E14" s="149">
+      <c r="E14" s="119">
         <f t="shared" si="1"/>
         <v>65881.136053851194</v>
       </c>
@@ -8664,11 +8661,11 @@
       <c r="C15" s="49">
         <v>56.375674465783348</v>
       </c>
-      <c r="D15" s="149">
+      <c r="D15" s="119">
         <f t="shared" si="0"/>
         <v>62269.527941188258</v>
       </c>
-      <c r="E15" s="149">
+      <c r="E15" s="119">
         <f t="shared" si="1"/>
         <v>56375.674465783348</v>
       </c>
@@ -8687,11 +8684,11 @@
       <c r="C16" s="49">
         <v>47.786562864708507</v>
       </c>
-      <c r="D16" s="149">
+      <c r="D16" s="119">
         <f t="shared" si="0"/>
         <v>49094.741236225527</v>
       </c>
-      <c r="E16" s="149">
+      <c r="E16" s="119">
         <f t="shared" si="1"/>
         <v>47786.56286470851</v>
       </c>
@@ -8710,11 +8707,11 @@
       <c r="C17" s="49">
         <v>38.751396319462906</v>
       </c>
-      <c r="D17" s="149">
+      <c r="D17" s="119">
         <f t="shared" si="0"/>
         <v>38060.556537016608</v>
       </c>
-      <c r="E17" s="149">
+      <c r="E17" s="119">
         <f t="shared" si="1"/>
         <v>38751.396319462903</v>
       </c>
@@ -8733,11 +8730,11 @@
       <c r="C18" s="49">
         <v>32.1124572883867</v>
       </c>
-      <c r="D18" s="149">
+      <c r="D18" s="119">
         <f t="shared" si="0"/>
         <v>27479.140628878631</v>
       </c>
-      <c r="E18" s="149">
+      <c r="E18" s="119">
         <f t="shared" si="1"/>
         <v>32112.4572883867</v>
       </c>
@@ -8756,11 +8753,11 @@
       <c r="C19" s="49">
         <v>23.809872215759977</v>
       </c>
-      <c r="D19" s="149">
+      <c r="D19" s="119">
         <f t="shared" si="0"/>
         <v>18576.101123217755</v>
       </c>
-      <c r="E19" s="149">
+      <c r="E19" s="119">
         <f t="shared" si="1"/>
         <v>23809.872215759977</v>
       </c>
@@ -8779,11 +8776,11 @@
       <c r="C20" s="49">
         <v>15.544560996940714</v>
       </c>
-      <c r="D20" s="149">
+      <c r="D20" s="119">
         <f t="shared" si="0"/>
         <v>12334.925672142715</v>
       </c>
-      <c r="E20" s="149">
+      <c r="E20" s="119">
         <f t="shared" si="1"/>
         <v>15544.560996940714</v>
       </c>
@@ -8802,11 +8799,11 @@
       <c r="C21" s="49">
         <v>7.5698454502498134</v>
       </c>
-      <c r="D21" s="149">
+      <c r="D21" s="119">
         <f t="shared" si="0"/>
         <v>6594.7830785775623</v>
       </c>
-      <c r="E21" s="149">
+      <c r="E21" s="119">
         <f t="shared" si="1"/>
         <v>7569.8454502498134</v>
       </c>
@@ -8856,10 +8853,10 @@
       <c r="A27" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="136" t="s">
+      <c r="B27" s="143" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="137"/>
+      <c r="C27" s="144"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
@@ -9205,7 +9202,7 @@
     </row>
     <row r="50" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B50" s="37"/>
       <c r="C50" s="37"/>
@@ -9274,19 +9271,19 @@
       <c r="AE51" s="24"/>
     </row>
     <row r="52" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="138" t="s">
+      <c r="A52" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="138" t="s">
+      <c r="B52" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="138"/>
-      <c r="D52" s="138"/>
-      <c r="E52" s="138" t="s">
+      <c r="C52" s="131"/>
+      <c r="D52" s="131"/>
+      <c r="E52" s="131" t="s">
         <v>55</v>
       </c>
-      <c r="F52" s="138"/>
-      <c r="G52" s="138"/>
+      <c r="F52" s="131"/>
+      <c r="G52" s="131"/>
       <c r="X52" s="22"/>
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
@@ -9297,7 +9294,7 @@
       <c r="AE52" s="22"/>
     </row>
     <row r="53" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="138"/>
+      <c r="A53" s="131"/>
       <c r="B53" s="33" t="s">
         <v>3</v>
       </c>
@@ -9776,7 +9773,7 @@
     </row>
     <row r="79" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B79" s="37"/>
       <c r="C79" s="37"/>
@@ -9803,174 +9800,174 @@
       <c r="X79" s="37"/>
     </row>
     <row r="80" spans="1:24" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="142" t="s">
+      <c r="A80" s="129" t="s">
+        <v>102</v>
+      </c>
+      <c r="B80" s="129"/>
+      <c r="C80" s="129"/>
+      <c r="D80" s="129"/>
+      <c r="E80" s="129"/>
+      <c r="F80" s="129"/>
+      <c r="G80" s="129"/>
+      <c r="H80" s="129"/>
+      <c r="I80" s="129"/>
+      <c r="J80" s="129"/>
+      <c r="K80" s="129"/>
+      <c r="L80" s="129"/>
+      <c r="M80" s="129"/>
+      <c r="N80" s="129"/>
+      <c r="O80" s="129"/>
+      <c r="P80" s="129"/>
+      <c r="Q80" s="129"/>
+      <c r="R80" s="129"/>
+      <c r="S80" s="129"/>
+      <c r="T80" s="129"/>
+      <c r="U80" s="129"/>
+      <c r="V80" s="129"/>
+      <c r="W80" s="129"/>
+      <c r="X80" s="129"/>
+    </row>
+    <row r="81" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="120" t="s">
+        <v>103</v>
+      </c>
+      <c r="C81" s="120"/>
+      <c r="D81" s="120"/>
+      <c r="E81" s="120"/>
+      <c r="F81" s="120"/>
+      <c r="G81" s="120"/>
+      <c r="H81" s="120"/>
+      <c r="I81" s="120"/>
+      <c r="J81" s="120"/>
+      <c r="K81" s="120"/>
+      <c r="L81" s="120"/>
+      <c r="N81" s="121" t="s">
+        <v>2</v>
+      </c>
+      <c r="O81" s="120" t="s">
         <v>104</v>
       </c>
-      <c r="B80" s="142"/>
-      <c r="C80" s="142"/>
-      <c r="D80" s="142"/>
-      <c r="E80" s="142"/>
-      <c r="F80" s="142"/>
-      <c r="G80" s="142"/>
-      <c r="H80" s="142"/>
-      <c r="I80" s="142"/>
-      <c r="J80" s="142"/>
-      <c r="K80" s="142"/>
-      <c r="L80" s="142"/>
-      <c r="M80" s="142"/>
-      <c r="N80" s="142"/>
-      <c r="O80" s="142"/>
-      <c r="P80" s="142"/>
-      <c r="Q80" s="142"/>
-      <c r="R80" s="142"/>
-      <c r="S80" s="142"/>
-      <c r="T80" s="142"/>
-      <c r="U80" s="142"/>
-      <c r="V80" s="142"/>
-      <c r="W80" s="142"/>
-      <c r="X80" s="142"/>
-    </row>
-    <row r="81" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="119" t="s">
+      <c r="P81" s="120"/>
+      <c r="Q81" s="120"/>
+      <c r="R81" s="120"/>
+      <c r="S81" s="120"/>
+      <c r="T81" s="120"/>
+      <c r="U81" s="120"/>
+      <c r="V81" s="120"/>
+      <c r="W81" s="120"/>
+      <c r="X81" s="120"/>
+      <c r="Y81" s="120"/>
+      <c r="AA81" s="126" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB81" s="127"/>
+      <c r="AC81" s="127"/>
+      <c r="AD81" s="127"/>
+      <c r="AE81" s="127"/>
+      <c r="AF81" s="127"/>
+      <c r="AG81" s="127"/>
+      <c r="AH81" s="127"/>
+      <c r="AI81" s="128"/>
+      <c r="AW81" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="123" t="s">
-        <v>105</v>
-      </c>
-      <c r="C81" s="123"/>
-      <c r="D81" s="123"/>
-      <c r="E81" s="123"/>
-      <c r="F81" s="123"/>
-      <c r="G81" s="123"/>
-      <c r="H81" s="123"/>
-      <c r="I81" s="123"/>
-      <c r="J81" s="123"/>
-      <c r="K81" s="123"/>
-      <c r="L81" s="123"/>
-      <c r="N81" s="119" t="s">
+      <c r="AX81" s="120" t="s">
+        <v>100</v>
+      </c>
+      <c r="AY81" s="120"/>
+      <c r="AZ81" s="120"/>
+      <c r="BA81" s="120"/>
+      <c r="BB81" s="120"/>
+      <c r="BD81" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="O81" s="123" t="s">
-        <v>106</v>
-      </c>
-      <c r="P81" s="123"/>
-      <c r="Q81" s="123"/>
-      <c r="R81" s="123"/>
-      <c r="S81" s="123"/>
-      <c r="T81" s="123"/>
-      <c r="U81" s="123"/>
-      <c r="V81" s="123"/>
-      <c r="W81" s="123"/>
-      <c r="X81" s="123"/>
-      <c r="Y81" s="123"/>
-      <c r="AA81" s="146" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB81" s="147"/>
-      <c r="AC81" s="147"/>
-      <c r="AD81" s="147"/>
-      <c r="AE81" s="147"/>
-      <c r="AF81" s="147"/>
-      <c r="AG81" s="147"/>
-      <c r="AH81" s="147"/>
-      <c r="AI81" s="148"/>
-      <c r="AW81" s="119" t="s">
+      <c r="BE81" s="120" t="s">
+        <v>101</v>
+      </c>
+      <c r="BF81" s="120"/>
+      <c r="BG81" s="120"/>
+      <c r="BH81" s="120"/>
+      <c r="BI81" s="120"/>
+    </row>
+    <row r="82" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="122"/>
+      <c r="B82" s="120"/>
+      <c r="C82" s="120"/>
+      <c r="D82" s="120"/>
+      <c r="E82" s="120"/>
+      <c r="F82" s="120"/>
+      <c r="G82" s="120"/>
+      <c r="H82" s="120"/>
+      <c r="I82" s="120"/>
+      <c r="J82" s="120"/>
+      <c r="K82" s="120"/>
+      <c r="L82" s="120"/>
+      <c r="N82" s="122"/>
+      <c r="O82" s="120"/>
+      <c r="P82" s="120"/>
+      <c r="Q82" s="120"/>
+      <c r="R82" s="120"/>
+      <c r="S82" s="120"/>
+      <c r="T82" s="120"/>
+      <c r="U82" s="120"/>
+      <c r="V82" s="120"/>
+      <c r="W82" s="120"/>
+      <c r="X82" s="120"/>
+      <c r="Y82" s="120"/>
+      <c r="AA82" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="AX81" s="123" t="s">
-        <v>102</v>
-      </c>
-      <c r="AY81" s="123"/>
-      <c r="AZ81" s="123"/>
-      <c r="BA81" s="123"/>
-      <c r="BB81" s="123"/>
-      <c r="BD81" s="119" t="s">
-        <v>2</v>
-      </c>
-      <c r="BE81" s="123" t="s">
-        <v>103</v>
-      </c>
-      <c r="BF81" s="123"/>
-      <c r="BG81" s="123"/>
-      <c r="BH81" s="123"/>
-      <c r="BI81" s="123"/>
-    </row>
-    <row r="82" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="120"/>
-      <c r="B82" s="123"/>
-      <c r="C82" s="123"/>
-      <c r="D82" s="123"/>
-      <c r="E82" s="123"/>
-      <c r="F82" s="123"/>
-      <c r="G82" s="123"/>
-      <c r="H82" s="123"/>
-      <c r="I82" s="123"/>
-      <c r="J82" s="123"/>
-      <c r="K82" s="123"/>
-      <c r="L82" s="123"/>
-      <c r="N82" s="120"/>
-      <c r="O82" s="123"/>
-      <c r="P82" s="123"/>
-      <c r="Q82" s="123"/>
-      <c r="R82" s="123"/>
-      <c r="S82" s="123"/>
-      <c r="T82" s="123"/>
-      <c r="U82" s="123"/>
-      <c r="V82" s="123"/>
-      <c r="W82" s="123"/>
-      <c r="X82" s="123"/>
-      <c r="Y82" s="123"/>
-      <c r="AA82" s="144" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB82" s="146" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC82" s="147"/>
-      <c r="AD82" s="147"/>
-      <c r="AE82" s="147"/>
-      <c r="AF82" s="147"/>
-      <c r="AG82" s="147"/>
-      <c r="AH82" s="147"/>
-      <c r="AI82" s="148"/>
-      <c r="AW82" s="120"/>
-      <c r="AX82" s="123"/>
-      <c r="AY82" s="123"/>
-      <c r="AZ82" s="123"/>
-      <c r="BA82" s="123"/>
-      <c r="BB82" s="123"/>
-      <c r="BD82" s="120"/>
-      <c r="BE82" s="123"/>
-      <c r="BF82" s="123"/>
-      <c r="BG82" s="123"/>
-      <c r="BH82" s="123"/>
-      <c r="BI82" s="123"/>
+      <c r="AB82" s="126" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC82" s="127"/>
+      <c r="AD82" s="127"/>
+      <c r="AE82" s="127"/>
+      <c r="AF82" s="127"/>
+      <c r="AG82" s="127"/>
+      <c r="AH82" s="127"/>
+      <c r="AI82" s="128"/>
+      <c r="AW82" s="122"/>
+      <c r="AX82" s="120"/>
+      <c r="AY82" s="120"/>
+      <c r="AZ82" s="120"/>
+      <c r="BA82" s="120"/>
+      <c r="BB82" s="120"/>
+      <c r="BD82" s="122"/>
+      <c r="BE82" s="120"/>
+      <c r="BF82" s="120"/>
+      <c r="BG82" s="120"/>
+      <c r="BH82" s="120"/>
+      <c r="BI82" s="120"/>
     </row>
     <row r="83" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="121"/>
+      <c r="A83" s="123"/>
       <c r="B83" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="C83" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="D83" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="C83" s="70" t="s">
+      <c r="E83" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="D83" s="70" t="s">
+      <c r="F83" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="G83" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="E83" s="70" t="s">
+      <c r="H83" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="I83" s="70" t="s">
         <v>94</v>
-      </c>
-      <c r="F83" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="G83" s="70" t="s">
-        <v>95</v>
-      </c>
-      <c r="H83" s="70" t="s">
-        <v>97</v>
-      </c>
-      <c r="I83" s="70" t="s">
-        <v>96</v>
       </c>
       <c r="J83" s="82">
         <v>2000</v>
@@ -9981,30 +9978,30 @@
       <c r="L83" s="81">
         <v>2020</v>
       </c>
-      <c r="N83" s="121"/>
+      <c r="N83" s="123"/>
       <c r="O83" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="P83" s="71" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q83" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="P83" s="71" t="s">
+      <c r="R83" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="Q83" s="71" t="s">
+      <c r="S83" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="T83" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="R83" s="71" t="s">
+      <c r="U83" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="V83" s="71" t="s">
         <v>94</v>
-      </c>
-      <c r="S83" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="T83" s="71" t="s">
-        <v>95</v>
-      </c>
-      <c r="U83" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="V83" s="71" t="s">
-        <v>96</v>
       </c>
       <c r="W83" s="100">
         <v>2000</v>
@@ -10015,37 +10012,37 @@
       <c r="Y83" s="102">
         <v>2020</v>
       </c>
-      <c r="AA83" s="145"/>
+      <c r="AA83" s="125"/>
       <c r="AB83" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC83" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD83" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="AC83" s="70" t="s">
+      <c r="AE83" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="AD83" s="70" t="s">
+      <c r="AF83" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="AG83" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="AE83" s="70" t="s">
+      <c r="AH83" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI83" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="AF83" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="AG83" s="70" t="s">
-        <v>95</v>
-      </c>
-      <c r="AH83" s="70" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI83" s="70" t="s">
-        <v>96</v>
-      </c>
-      <c r="AW83" s="121"/>
+      <c r="AW83" s="123"/>
       <c r="AX83" s="70" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AY83" s="70" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AZ83" s="82">
         <v>2000</v>
@@ -10056,12 +10053,12 @@
       <c r="BB83" s="83">
         <v>2020</v>
       </c>
-      <c r="BD83" s="121"/>
+      <c r="BD83" s="123"/>
       <c r="BE83" s="70" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="BF83" s="70" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="BG83" s="82">
         <v>2000</v>
@@ -10330,7 +10327,7 @@
         <v>-3.5764705882352941E-5</v>
       </c>
       <c r="AA85" s="76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AB85" s="74">
         <v>3.0801934E-2</v>
@@ -10625,19 +10622,19 @@
         <f t="shared" si="12"/>
         <v>-6.3054823529411761E-5</v>
       </c>
-      <c r="AA87" s="144" t="s">
+      <c r="AA87" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="AB87" s="146" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC87" s="147"/>
-      <c r="AD87" s="147"/>
-      <c r="AE87" s="147"/>
-      <c r="AF87" s="147"/>
-      <c r="AG87" s="147"/>
-      <c r="AH87" s="147"/>
-      <c r="AI87" s="148"/>
+      <c r="AB87" s="126" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC87" s="127"/>
+      <c r="AD87" s="127"/>
+      <c r="AE87" s="127"/>
+      <c r="AF87" s="127"/>
+      <c r="AG87" s="127"/>
+      <c r="AH87" s="127"/>
+      <c r="AI87" s="128"/>
       <c r="AW87" s="86" t="s">
         <v>13</v>
       </c>
@@ -10768,30 +10765,30 @@
         <f t="shared" si="12"/>
         <v>-1.4261617647058823E-4</v>
       </c>
-      <c r="AA88" s="145"/>
+      <c r="AA88" s="125"/>
       <c r="AB88" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC88" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD88" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="AC88" s="70" t="s">
+      <c r="AE88" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="AD88" s="70" t="s">
+      <c r="AF88" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="AG88" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="AE88" s="70" t="s">
+      <c r="AH88" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI88" s="70" t="s">
         <v>94</v>
-      </c>
-      <c r="AF88" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="AG88" s="70" t="s">
-        <v>95</v>
-      </c>
-      <c r="AH88" s="70" t="s">
-        <v>97</v>
-      </c>
-      <c r="AI88" s="70" t="s">
-        <v>96</v>
       </c>
       <c r="AW88" s="86" t="s">
         <v>14</v>
@@ -11081,7 +11078,7 @@
         <v>-2.6698682352941175E-4</v>
       </c>
       <c r="AA90" s="76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AB90" s="74">
         <v>2.7320634999999999E-2</v>
@@ -12431,7 +12428,7 @@
     </row>
     <row r="108" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B108" s="37"/>
       <c r="C108" s="37"/>
@@ -12459,7 +12456,7 @@
     </row>
     <row r="109" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B109" s="37"/>
       <c r="C109" s="37"/>
@@ -12487,7 +12484,7 @@
     </row>
     <row r="110" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B110" s="37"/>
       <c r="C110" s="37"/>
@@ -12514,25 +12511,25 @@
       <c r="X110" s="37"/>
     </row>
     <row r="111" spans="1:62" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="139" t="s">
-        <v>100</v>
-      </c>
-      <c r="B111" s="139"/>
-      <c r="C111" s="139"/>
-      <c r="D111" s="139"/>
-      <c r="E111" s="139"/>
-      <c r="F111" s="139"/>
-      <c r="G111" s="139"/>
-      <c r="H111" s="139"/>
-      <c r="I111" s="139"/>
-      <c r="J111" s="139"/>
-      <c r="K111" s="139"/>
-      <c r="L111" s="139"/>
-      <c r="M111" s="139"/>
-      <c r="N111" s="139"/>
-      <c r="O111" s="139"/>
-      <c r="P111" s="139"/>
-      <c r="Q111" s="139"/>
+      <c r="A111" s="145" t="s">
+        <v>98</v>
+      </c>
+      <c r="B111" s="145"/>
+      <c r="C111" s="145"/>
+      <c r="D111" s="145"/>
+      <c r="E111" s="145"/>
+      <c r="F111" s="145"/>
+      <c r="G111" s="145"/>
+      <c r="H111" s="145"/>
+      <c r="I111" s="145"/>
+      <c r="J111" s="145"/>
+      <c r="K111" s="145"/>
+      <c r="L111" s="145"/>
+      <c r="M111" s="145"/>
+      <c r="N111" s="145"/>
+      <c r="O111" s="145"/>
+      <c r="P111" s="145"/>
+      <c r="Q111" s="145"/>
       <c r="R111" s="37"/>
       <c r="S111" s="37"/>
       <c r="T111" s="37"/>
@@ -12542,17 +12539,17 @@
       <c r="X111" s="37"/>
     </row>
     <row r="112" spans="1:62" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="133" t="s">
+      <c r="A112" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="129" t="s">
-        <v>81</v>
-      </c>
-      <c r="C112" s="130"/>
-      <c r="D112" s="130"/>
-      <c r="E112" s="130"/>
-      <c r="F112" s="130"/>
-      <c r="G112" s="131"/>
+      <c r="B112" s="136" t="s">
+        <v>80</v>
+      </c>
+      <c r="C112" s="137"/>
+      <c r="D112" s="137"/>
+      <c r="E112" s="137"/>
+      <c r="F112" s="137"/>
+      <c r="G112" s="138"/>
       <c r="I112" s="67"/>
       <c r="J112" s="78" t="s">
         <v>27</v>
@@ -12571,7 +12568,7 @@
       </c>
     </row>
     <row r="113" spans="1:14" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="134"/>
+      <c r="A113" s="141"/>
       <c r="B113" s="32" t="s">
         <v>68</v>
       </c>
@@ -12615,7 +12612,7 @@
       </c>
     </row>
     <row r="114" spans="1:14" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="135"/>
+      <c r="A114" s="142"/>
       <c r="B114" s="34" t="s">
         <v>61</v>
       </c>
@@ -12663,14 +12660,14 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="I115" s="143" t="s">
-        <v>99</v>
-      </c>
-      <c r="J115" s="143"/>
-      <c r="K115" s="143"/>
-      <c r="L115" s="143"/>
-      <c r="M115" s="143"/>
-      <c r="N115" s="143"/>
+      <c r="I115" s="130" t="s">
+        <v>97</v>
+      </c>
+      <c r="J115" s="130"/>
+      <c r="K115" s="130"/>
+      <c r="L115" s="130"/>
+      <c r="M115" s="130"/>
+      <c r="N115" s="130"/>
     </row>
     <row r="116" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
@@ -13423,31 +13420,31 @@
     </row>
     <row r="132" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="133" spans="1:15" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="126" t="s">
+      <c r="A133" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="129" t="s">
-        <v>82</v>
-      </c>
-      <c r="C133" s="130"/>
-      <c r="D133" s="130"/>
-      <c r="E133" s="130"/>
-      <c r="F133" s="130"/>
-      <c r="G133" s="131"/>
-      <c r="I133" s="126" t="s">
+      <c r="B133" s="136" t="s">
+        <v>81</v>
+      </c>
+      <c r="C133" s="137"/>
+      <c r="D133" s="137"/>
+      <c r="E133" s="137"/>
+      <c r="F133" s="137"/>
+      <c r="G133" s="138"/>
+      <c r="I133" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="J133" s="129" t="s">
-        <v>74</v>
-      </c>
-      <c r="K133" s="130"/>
-      <c r="L133" s="130"/>
-      <c r="M133" s="130"/>
-      <c r="N133" s="130"/>
-      <c r="O133" s="131"/>
+      <c r="J133" s="136" t="s">
+        <v>73</v>
+      </c>
+      <c r="K133" s="137"/>
+      <c r="L133" s="137"/>
+      <c r="M133" s="137"/>
+      <c r="N133" s="137"/>
+      <c r="O133" s="138"/>
     </row>
     <row r="134" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="127"/>
+      <c r="A134" s="134"/>
       <c r="B134" s="26" t="s">
         <v>69</v>
       </c>
@@ -13466,7 +13463,7 @@
       <c r="G134" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I134" s="127"/>
+      <c r="I134" s="134"/>
       <c r="J134" s="26" t="s">
         <v>69</v>
       </c>
@@ -13487,7 +13484,7 @@
       </c>
     </row>
     <row r="135" spans="1:15" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="128"/>
+      <c r="A135" s="135"/>
       <c r="B135" s="40" t="s">
         <v>61</v>
       </c>
@@ -13506,7 +13503,7 @@
       <c r="G135" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="I135" s="128"/>
+      <c r="I135" s="135"/>
       <c r="J135" s="40" t="s">
         <v>61</v>
       </c>
@@ -14366,7 +14363,7 @@
     </row>
     <row r="158" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="36" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="B158" s="37"/>
       <c r="C158" s="37"/>
@@ -14392,9 +14389,7 @@
       <c r="W158" s="37"/>
     </row>
     <row r="159" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A159" s="38" t="s">
-        <v>56</v>
-      </c>
+      <c r="A159" s="38"/>
       <c r="B159" s="37"/>
       <c r="C159" s="37"/>
       <c r="D159" s="37"/>
@@ -14419,9 +14414,7 @@
       <c r="W159" s="37"/>
     </row>
     <row r="160" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="36" t="s">
-        <v>70</v>
-      </c>
+      <c r="A160" s="36"/>
       <c r="B160" s="37"/>
       <c r="C160" s="37"/>
       <c r="D160" s="37"/>
@@ -14446,22 +14439,22 @@
       <c r="W160" s="37"/>
     </row>
     <row r="161" spans="1:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="123" t="s">
-        <v>86</v>
-      </c>
-      <c r="B161" s="140" t="s">
-        <v>0</v>
-      </c>
-      <c r="C161" s="140"/>
-      <c r="D161" s="140"/>
-      <c r="E161" s="140" t="s">
+      <c r="A161" s="120" t="s">
+        <v>85</v>
+      </c>
+      <c r="B161" s="148" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="148"/>
+      <c r="D161" s="148"/>
+      <c r="E161" s="148" t="s">
         <v>1</v>
       </c>
-      <c r="F161" s="140"/>
-      <c r="G161" s="140"/>
+      <c r="F161" s="148"/>
+      <c r="G161" s="148"/>
     </row>
     <row r="162" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="123"/>
+      <c r="A162" s="120"/>
       <c r="B162" s="57" t="s">
         <v>3</v>
       </c>
@@ -15311,9 +15304,9 @@
       <c r="AB185" s="20"/>
     </row>
     <row r="186" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A186" s="141"/>
-      <c r="B186" s="141"/>
-      <c r="C186" s="141"/>
+      <c r="A186" s="149"/>
+      <c r="B186" s="149"/>
+      <c r="C186" s="149"/>
       <c r="D186" s="20"/>
       <c r="E186" s="20"/>
       <c r="F186" s="20"/>
@@ -15462,7 +15455,7 @@
     </row>
     <row r="197" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A197" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B197" s="37"/>
       <c r="C197" s="37"/>
@@ -15488,37 +15481,37 @@
       <c r="W197" s="37"/>
     </row>
     <row r="198" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="136" t="s">
-        <v>71</v>
-      </c>
-      <c r="B198" s="136"/>
-      <c r="C198" s="136"/>
-      <c r="D198" s="136"/>
+      <c r="A198" s="143" t="s">
+        <v>70</v>
+      </c>
+      <c r="B198" s="143"/>
+      <c r="C198" s="143"/>
+      <c r="D198" s="143"/>
       <c r="E198" s="94"/>
       <c r="F198" s="94"/>
     </row>
     <row r="199" spans="1:23" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="136" t="s">
-        <v>72</v>
-      </c>
-      <c r="B199" s="136"/>
-      <c r="C199" s="136"/>
-      <c r="D199" s="136"/>
+      <c r="A199" s="143" t="s">
+        <v>71</v>
+      </c>
+      <c r="B199" s="143"/>
+      <c r="C199" s="143"/>
+      <c r="D199" s="143"/>
       <c r="E199" s="94"/>
       <c r="F199" s="94"/>
     </row>
     <row r="200" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A200" s="132" t="s">
+      <c r="A200" s="139" t="s">
         <v>45</v>
       </c>
-      <c r="B200" s="132" t="s">
+      <c r="B200" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="C200" s="132"/>
-      <c r="D200" s="132"/>
+      <c r="C200" s="139"/>
+      <c r="D200" s="139"/>
     </row>
     <row r="201" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A201" s="132"/>
+      <c r="A201" s="139"/>
       <c r="B201" s="43" t="s">
         <v>46</v>
       </c>
@@ -15556,11 +15549,11 @@
       <c r="I202" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="J202" s="122" t="s">
-        <v>90</v>
-      </c>
-      <c r="K202" s="122"/>
-      <c r="L202" s="122"/>
+      <c r="J202" s="146" t="s">
+        <v>88</v>
+      </c>
+      <c r="K202" s="146"/>
+      <c r="L202" s="146"/>
     </row>
     <row r="203" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="44" t="s">
@@ -16177,27 +16170,27 @@
       </c>
     </row>
     <row r="219" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="124" t="s">
-        <v>73</v>
-      </c>
-      <c r="B219" s="124"/>
-      <c r="C219" s="124"/>
-      <c r="D219" s="124"/>
+      <c r="A219" s="147" t="s">
+        <v>72</v>
+      </c>
+      <c r="B219" s="147"/>
+      <c r="C219" s="147"/>
+      <c r="D219" s="147"/>
       <c r="E219" s="95"/>
     </row>
     <row r="220" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A220" s="124" t="s">
+      <c r="A220" s="147" t="s">
         <v>2</v>
       </c>
-      <c r="B220" s="132" t="s">
+      <c r="B220" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="C220" s="132"/>
-      <c r="D220" s="132"/>
+      <c r="C220" s="139"/>
+      <c r="D220" s="139"/>
       <c r="E220" s="25"/>
     </row>
     <row r="221" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A221" s="124"/>
+      <c r="A221" s="147"/>
       <c r="B221" s="43" t="s">
         <v>46</v>
       </c>
@@ -16236,11 +16229,11 @@
       <c r="I222" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="J222" s="122" t="s">
-        <v>89</v>
-      </c>
-      <c r="K222" s="122"/>
-      <c r="L222" s="122"/>
+      <c r="J222" s="146" t="s">
+        <v>87</v>
+      </c>
+      <c r="K222" s="146"/>
+      <c r="L222" s="146"/>
     </row>
     <row r="223" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="44" t="s">
@@ -16903,19 +16896,18 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="AX81:BB82"/>
-    <mergeCell ref="BD81:BD83"/>
-    <mergeCell ref="BE81:BI82"/>
-    <mergeCell ref="AA87:AA88"/>
-    <mergeCell ref="AA81:AI81"/>
-    <mergeCell ref="AB82:AI82"/>
-    <mergeCell ref="AB87:AI87"/>
-    <mergeCell ref="AA82:AA83"/>
-    <mergeCell ref="A80:X80"/>
-    <mergeCell ref="I115:N115"/>
-    <mergeCell ref="O81:Y82"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="AW81:AW83"/>
+    <mergeCell ref="J222:L222"/>
+    <mergeCell ref="J202:L202"/>
+    <mergeCell ref="A161:A162"/>
+    <mergeCell ref="A219:D219"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B161:D161"/>
+    <mergeCell ref="E161:G161"/>
+    <mergeCell ref="A186:C186"/>
+    <mergeCell ref="B200:D200"/>
+    <mergeCell ref="B220:D220"/>
+    <mergeCell ref="A198:D198"/>
+    <mergeCell ref="A199:D199"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="I133:I135"/>
     <mergeCell ref="J133:O133"/>
@@ -16932,19 +16924,20 @@
     <mergeCell ref="A111:Q111"/>
     <mergeCell ref="N81:N83"/>
     <mergeCell ref="B81:L82"/>
+    <mergeCell ref="A80:X80"/>
+    <mergeCell ref="I115:N115"/>
+    <mergeCell ref="O81:Y82"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="AW81:AW83"/>
     <mergeCell ref="A81:A83"/>
-    <mergeCell ref="J222:L222"/>
-    <mergeCell ref="J202:L202"/>
-    <mergeCell ref="A161:A162"/>
-    <mergeCell ref="A219:D219"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B161:D161"/>
-    <mergeCell ref="E161:G161"/>
-    <mergeCell ref="A186:C186"/>
-    <mergeCell ref="B200:D200"/>
-    <mergeCell ref="B220:D220"/>
-    <mergeCell ref="A198:D198"/>
-    <mergeCell ref="A199:D199"/>
+    <mergeCell ref="AX81:BB82"/>
+    <mergeCell ref="BD81:BD83"/>
+    <mergeCell ref="BE81:BI82"/>
+    <mergeCell ref="AA87:AA88"/>
+    <mergeCell ref="AA81:AI81"/>
+    <mergeCell ref="AB82:AI82"/>
+    <mergeCell ref="AB87:AI87"/>
+    <mergeCell ref="AA82:AA83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>